<commit_message>
Add dynamic features documentation and update Excel generation script
- Introduced DYNAMIC_FEATURES_TEST.md for testing dynamic dashboard features.
- Added IMPLEMENTATION_SUMMARY.md detailing the dynamic capabilities of the dashboard.
- Updated README.md to highlight the 100% dynamic nature of the dashboard and its features.
- Created TOP5_EXPLANATION.md to explain the new approach for displaying top 5 students.
- Enhanced generate_excel.py to insert Excel formulas for dynamic calculations of Total, Average, GPA, and Grade.
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -18,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <name val="Calibri"/>
@@ -98,13 +100,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -112,7 +121,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -225,12 +239,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$9:$A$13</f>
+              <f>'Dashboard'!$A$9:$A$15</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$9:$B$13</f>
+              <f>'Dashboard'!$B$9:$B$15</f>
             </numRef>
           </val>
         </ser>
@@ -816,19 +830,21 @@
       <c r="I2" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="J2" t="n">
-        <v>580</v>
-      </c>
-      <c r="K2" t="n">
-        <v>82.86</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="J2">
+        <f>SUM(C2:I2)</f>
+        <v/>
+      </c>
+      <c r="K2" s="4">
+        <f>ROUND(AVERAGE(C2:I2),2)</f>
+        <v/>
+      </c>
+      <c r="L2" s="5">
+        <f>IF(OR(C2&lt;33,D2&lt;33,E2&lt;33,F2&lt;33,G2&lt;33,H2&lt;33,I2&lt;33),0,MIN(5,ROUND((IF(C2&gt;=80,5,IF(C2&gt;=70,4,IF(C2&gt;=60,3.5,IF(C2&gt;=50,3,IF(C2&gt;=40,2,IF(C2&gt;=33,1,0))))))+IF(D2&gt;=80,5,IF(D2&gt;=70,4,IF(D2&gt;=60,3.5,IF(D2&gt;=50,3,IF(D2&gt;=40,2,IF(D2&gt;=33,1,0))))))+IF(E2&gt;=80,5,IF(E2&gt;=70,4,IF(E2&gt;=60,3.5,IF(E2&gt;=50,3,IF(E2&gt;=40,2,IF(E2&gt;=33,1,0))))))+IF(F2&gt;=80,5,IF(F2&gt;=70,4,IF(F2&gt;=60,3.5,IF(F2&gt;=50,3,IF(F2&gt;=40,2,IF(F2&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF(H2&gt;=80,5,IF(H2&gt;=70,4,IF(H2&gt;=60,3.5,IF(H2&gt;=50,3,IF(H2&gt;=40,2,IF(H2&gt;=33,1,0))))))+IF(I2&gt;=80,5,IF(I2&gt;=70,4,IF(I2&gt;=60,3.5,IF(I2&gt;=50,3,IF(I2&gt;=40,2,IF(I2&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M2" s="6">
+        <f>IF(L2&gt;=5,"A+",IF(L2&gt;=4,"A",IF(L2&gt;=3.5,"A-",IF(L2&gt;=3,"B",IF(L2&gt;=2,"C",IF(L2&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -861,19 +877,21 @@
       <c r="I3" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="J3" t="n">
-        <v>622</v>
-      </c>
-      <c r="K3" t="n">
-        <v>88.86</v>
-      </c>
-      <c r="L3" t="n">
-        <v>5</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J3">
+        <f>SUM(C3:I3)</f>
+        <v/>
+      </c>
+      <c r="K3" s="4">
+        <f>ROUND(AVERAGE(C3:I3),2)</f>
+        <v/>
+      </c>
+      <c r="L3" s="5">
+        <f>IF(OR(C3&lt;33,D3&lt;33,E3&lt;33,F3&lt;33,G3&lt;33,H3&lt;33,I3&lt;33),0,MIN(5,ROUND((IF(C3&gt;=80,5,IF(C3&gt;=70,4,IF(C3&gt;=60,3.5,IF(C3&gt;=50,3,IF(C3&gt;=40,2,IF(C3&gt;=33,1,0))))))+IF(D3&gt;=80,5,IF(D3&gt;=70,4,IF(D3&gt;=60,3.5,IF(D3&gt;=50,3,IF(D3&gt;=40,2,IF(D3&gt;=33,1,0))))))+IF(E3&gt;=80,5,IF(E3&gt;=70,4,IF(E3&gt;=60,3.5,IF(E3&gt;=50,3,IF(E3&gt;=40,2,IF(E3&gt;=33,1,0))))))+IF(F3&gt;=80,5,IF(F3&gt;=70,4,IF(F3&gt;=60,3.5,IF(F3&gt;=50,3,IF(F3&gt;=40,2,IF(F3&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF(H3&gt;=80,5,IF(H3&gt;=70,4,IF(H3&gt;=60,3.5,IF(H3&gt;=50,3,IF(H3&gt;=40,2,IF(H3&gt;=33,1,0))))))+IF(I3&gt;=80,5,IF(I3&gt;=70,4,IF(I3&gt;=60,3.5,IF(I3&gt;=50,3,IF(I3&gt;=40,2,IF(I3&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M3" s="6">
+        <f>IF(L3&gt;=5,"A+",IF(L3&gt;=4,"A",IF(L3&gt;=3.5,"A-",IF(L3&gt;=3,"B",IF(L3&gt;=2,"C",IF(L3&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -906,19 +924,21 @@
       <c r="I4" s="3" t="n">
         <v>69</v>
       </c>
-      <c r="J4" t="n">
-        <v>490</v>
-      </c>
-      <c r="K4" t="n">
-        <v>70</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3.79</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
+      <c r="J4">
+        <f>SUM(C4:I4)</f>
+        <v/>
+      </c>
+      <c r="K4" s="4">
+        <f>ROUND(AVERAGE(C4:I4),2)</f>
+        <v/>
+      </c>
+      <c r="L4" s="5">
+        <f>IF(OR(C4&lt;33,D4&lt;33,E4&lt;33,F4&lt;33,G4&lt;33,H4&lt;33,I4&lt;33),0,MIN(5,ROUND((IF(C4&gt;=80,5,IF(C4&gt;=70,4,IF(C4&gt;=60,3.5,IF(C4&gt;=50,3,IF(C4&gt;=40,2,IF(C4&gt;=33,1,0))))))+IF(D4&gt;=80,5,IF(D4&gt;=70,4,IF(D4&gt;=60,3.5,IF(D4&gt;=50,3,IF(D4&gt;=40,2,IF(D4&gt;=33,1,0))))))+IF(E4&gt;=80,5,IF(E4&gt;=70,4,IF(E4&gt;=60,3.5,IF(E4&gt;=50,3,IF(E4&gt;=40,2,IF(E4&gt;=33,1,0))))))+IF(F4&gt;=80,5,IF(F4&gt;=70,4,IF(F4&gt;=60,3.5,IF(F4&gt;=50,3,IF(F4&gt;=40,2,IF(F4&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF(H4&gt;=80,5,IF(H4&gt;=70,4,IF(H4&gt;=60,3.5,IF(H4&gt;=50,3,IF(H4&gt;=40,2,IF(H4&gt;=33,1,0))))))+IF(I4&gt;=80,5,IF(I4&gt;=70,4,IF(I4&gt;=60,3.5,IF(I4&gt;=50,3,IF(I4&gt;=40,2,IF(I4&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M4" s="6">
+        <f>IF(L4&gt;=5,"A+",IF(L4&gt;=4,"A",IF(L4&gt;=3.5,"A-",IF(L4&gt;=3,"B",IF(L4&gt;=2,"C",IF(L4&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -951,19 +971,21 @@
       <c r="I5" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="J5" t="n">
-        <v>658</v>
-      </c>
-      <c r="K5" t="n">
-        <v>94</v>
-      </c>
-      <c r="L5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J5">
+        <f>SUM(C5:I5)</f>
+        <v/>
+      </c>
+      <c r="K5" s="4">
+        <f>ROUND(AVERAGE(C5:I5),2)</f>
+        <v/>
+      </c>
+      <c r="L5" s="5">
+        <f>IF(OR(C5&lt;33,D5&lt;33,E5&lt;33,F5&lt;33,G5&lt;33,H5&lt;33,I5&lt;33),0,MIN(5,ROUND((IF(C5&gt;=80,5,IF(C5&gt;=70,4,IF(C5&gt;=60,3.5,IF(C5&gt;=50,3,IF(C5&gt;=40,2,IF(C5&gt;=33,1,0))))))+IF(D5&gt;=80,5,IF(D5&gt;=70,4,IF(D5&gt;=60,3.5,IF(D5&gt;=50,3,IF(D5&gt;=40,2,IF(D5&gt;=33,1,0))))))+IF(E5&gt;=80,5,IF(E5&gt;=70,4,IF(E5&gt;=60,3.5,IF(E5&gt;=50,3,IF(E5&gt;=40,2,IF(E5&gt;=33,1,0))))))+IF(F5&gt;=80,5,IF(F5&gt;=70,4,IF(F5&gt;=60,3.5,IF(F5&gt;=50,3,IF(F5&gt;=40,2,IF(F5&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF(H5&gt;=80,5,IF(H5&gt;=70,4,IF(H5&gt;=60,3.5,IF(H5&gt;=50,3,IF(H5&gt;=40,2,IF(H5&gt;=33,1,0))))))+IF(I5&gt;=80,5,IF(I5&gt;=70,4,IF(I5&gt;=60,3.5,IF(I5&gt;=50,3,IF(I5&gt;=40,2,IF(I5&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M5" s="6">
+        <f>IF(L5&gt;=5,"A+",IF(L5&gt;=4,"A",IF(L5&gt;=3.5,"A-",IF(L5&gt;=3,"B",IF(L5&gt;=2,"C",IF(L5&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -987,7 +1009,7 @@
       <c r="F6" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="7" t="n">
         <v>58</v>
       </c>
       <c r="H6" s="3" t="n">
@@ -996,19 +1018,21 @@
       <c r="I6" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="J6" t="n">
-        <v>453</v>
-      </c>
-      <c r="K6" t="n">
-        <v>64.70999999999999</v>
-      </c>
-      <c r="L6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
+      <c r="J6">
+        <f>SUM(C6:I6)</f>
+        <v/>
+      </c>
+      <c r="K6" s="4">
+        <f>ROUND(AVERAGE(C6:I6),2)</f>
+        <v/>
+      </c>
+      <c r="L6" s="5">
+        <f>IF(OR(C6&lt;33,D6&lt;33,E6&lt;33,F6&lt;33,G6&lt;33,H6&lt;33,I6&lt;33),0,MIN(5,ROUND((IF(C6&gt;=80,5,IF(C6&gt;=70,4,IF(C6&gt;=60,3.5,IF(C6&gt;=50,3,IF(C6&gt;=40,2,IF(C6&gt;=33,1,0))))))+IF(D6&gt;=80,5,IF(D6&gt;=70,4,IF(D6&gt;=60,3.5,IF(D6&gt;=50,3,IF(D6&gt;=40,2,IF(D6&gt;=33,1,0))))))+IF(E6&gt;=80,5,IF(E6&gt;=70,4,IF(E6&gt;=60,3.5,IF(E6&gt;=50,3,IF(E6&gt;=40,2,IF(E6&gt;=33,1,0))))))+IF(F6&gt;=80,5,IF(F6&gt;=70,4,IF(F6&gt;=60,3.5,IF(F6&gt;=50,3,IF(F6&gt;=40,2,IF(F6&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF(H6&gt;=80,5,IF(H6&gt;=70,4,IF(H6&gt;=60,3.5,IF(H6&gt;=50,3,IF(H6&gt;=40,2,IF(H6&gt;=33,1,0))))))+IF(I6&gt;=80,5,IF(I6&gt;=70,4,IF(I6&gt;=60,3.5,IF(I6&gt;=50,3,IF(I6&gt;=40,2,IF(I6&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M6" s="6">
+        <f>IF(L6&gt;=5,"A+",IF(L6&gt;=4,"A",IF(L6&gt;=3.5,"A-",IF(L6&gt;=3,"B",IF(L6&gt;=2,"C",IF(L6&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -1041,19 +1065,21 @@
       <c r="I7" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="J7" t="n">
-        <v>583</v>
-      </c>
-      <c r="K7" t="n">
-        <v>83.29000000000001</v>
-      </c>
-      <c r="L7" t="n">
-        <v>5</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J7">
+        <f>SUM(C7:I7)</f>
+        <v/>
+      </c>
+      <c r="K7" s="4">
+        <f>ROUND(AVERAGE(C7:I7),2)</f>
+        <v/>
+      </c>
+      <c r="L7" s="5">
+        <f>IF(OR(C7&lt;33,D7&lt;33,E7&lt;33,F7&lt;33,G7&lt;33,H7&lt;33,I7&lt;33),0,MIN(5,ROUND((IF(C7&gt;=80,5,IF(C7&gt;=70,4,IF(C7&gt;=60,3.5,IF(C7&gt;=50,3,IF(C7&gt;=40,2,IF(C7&gt;=33,1,0))))))+IF(D7&gt;=80,5,IF(D7&gt;=70,4,IF(D7&gt;=60,3.5,IF(D7&gt;=50,3,IF(D7&gt;=40,2,IF(D7&gt;=33,1,0))))))+IF(E7&gt;=80,5,IF(E7&gt;=70,4,IF(E7&gt;=60,3.5,IF(E7&gt;=50,3,IF(E7&gt;=40,2,IF(E7&gt;=33,1,0))))))+IF(F7&gt;=80,5,IF(F7&gt;=70,4,IF(F7&gt;=60,3.5,IF(F7&gt;=50,3,IF(F7&gt;=40,2,IF(F7&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF(H7&gt;=80,5,IF(H7&gt;=70,4,IF(H7&gt;=60,3.5,IF(H7&gt;=50,3,IF(H7&gt;=40,2,IF(H7&gt;=33,1,0))))))+IF(I7&gt;=80,5,IF(I7&gt;=70,4,IF(I7&gt;=60,3.5,IF(I7&gt;=50,3,IF(I7&gt;=40,2,IF(I7&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M7" s="6">
+        <f>IF(L7&gt;=5,"A+",IF(L7&gt;=4,"A",IF(L7&gt;=3.5,"A-",IF(L7&gt;=3,"B",IF(L7&gt;=2,"C",IF(L7&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -1065,40 +1091,42 @@
           <t>Jahir Ahmed</t>
         </is>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="7" t="n">
         <v>58</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="7" t="n">
         <v>52</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="7" t="n">
         <v>54</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="7" t="n">
         <v>57</v>
       </c>
-      <c r="J8" t="n">
-        <v>386</v>
-      </c>
-      <c r="K8" t="n">
-        <v>55.14</v>
-      </c>
-      <c r="L8" t="n">
-        <v>3.07</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="J8">
+        <f>SUM(C8:I8)</f>
+        <v/>
+      </c>
+      <c r="K8" s="4">
+        <f>ROUND(AVERAGE(C8:I8),2)</f>
+        <v/>
+      </c>
+      <c r="L8" s="5">
+        <f>IF(OR(C8&lt;33,D8&lt;33,E8&lt;33,F8&lt;33,G8&lt;33,H8&lt;33,I8&lt;33),0,MIN(5,ROUND((IF(C8&gt;=80,5,IF(C8&gt;=70,4,IF(C8&gt;=60,3.5,IF(C8&gt;=50,3,IF(C8&gt;=40,2,IF(C8&gt;=33,1,0))))))+IF(D8&gt;=80,5,IF(D8&gt;=70,4,IF(D8&gt;=60,3.5,IF(D8&gt;=50,3,IF(D8&gt;=40,2,IF(D8&gt;=33,1,0))))))+IF(E8&gt;=80,5,IF(E8&gt;=70,4,IF(E8&gt;=60,3.5,IF(E8&gt;=50,3,IF(E8&gt;=40,2,IF(E8&gt;=33,1,0))))))+IF(F8&gt;=80,5,IF(F8&gt;=70,4,IF(F8&gt;=60,3.5,IF(F8&gt;=50,3,IF(F8&gt;=40,2,IF(F8&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF(H8&gt;=80,5,IF(H8&gt;=70,4,IF(H8&gt;=60,3.5,IF(H8&gt;=50,3,IF(H8&gt;=40,2,IF(H8&gt;=33,1,0))))))+IF(I8&gt;=80,5,IF(I8&gt;=70,4,IF(I8&gt;=60,3.5,IF(I8&gt;=50,3,IF(I8&gt;=40,2,IF(I8&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M8" s="6">
+        <f>IF(L8&gt;=5,"A+",IF(L8&gt;=4,"A",IF(L8&gt;=3.5,"A-",IF(L8&gt;=3,"B",IF(L8&gt;=2,"C",IF(L8&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -1131,19 +1159,21 @@
       <c r="I9" s="3" t="n">
         <v>77</v>
       </c>
-      <c r="J9" t="n">
-        <v>547</v>
-      </c>
-      <c r="K9" t="n">
-        <v>78.14</v>
-      </c>
-      <c r="L9" t="n">
-        <v>4.29</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="J9">
+        <f>SUM(C9:I9)</f>
+        <v/>
+      </c>
+      <c r="K9" s="4">
+        <f>ROUND(AVERAGE(C9:I9),2)</f>
+        <v/>
+      </c>
+      <c r="L9" s="5">
+        <f>IF(OR(C9&lt;33,D9&lt;33,E9&lt;33,F9&lt;33,G9&lt;33,H9&lt;33,I9&lt;33),0,MIN(5,ROUND((IF(C9&gt;=80,5,IF(C9&gt;=70,4,IF(C9&gt;=60,3.5,IF(C9&gt;=50,3,IF(C9&gt;=40,2,IF(C9&gt;=33,1,0))))))+IF(D9&gt;=80,5,IF(D9&gt;=70,4,IF(D9&gt;=60,3.5,IF(D9&gt;=50,3,IF(D9&gt;=40,2,IF(D9&gt;=33,1,0))))))+IF(E9&gt;=80,5,IF(E9&gt;=70,4,IF(E9&gt;=60,3.5,IF(E9&gt;=50,3,IF(E9&gt;=40,2,IF(E9&gt;=33,1,0))))))+IF(F9&gt;=80,5,IF(F9&gt;=70,4,IF(F9&gt;=60,3.5,IF(F9&gt;=50,3,IF(F9&gt;=40,2,IF(F9&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF(H9&gt;=80,5,IF(H9&gt;=70,4,IF(H9&gt;=60,3.5,IF(H9&gt;=50,3,IF(H9&gt;=40,2,IF(H9&gt;=33,1,0))))))+IF(I9&gt;=80,5,IF(I9&gt;=70,4,IF(I9&gt;=60,3.5,IF(I9&gt;=50,3,IF(I9&gt;=40,2,IF(I9&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M9" s="6">
+        <f>IF(L9&gt;=5,"A+",IF(L9&gt;=4,"A",IF(L9&gt;=3.5,"A-",IF(L9&gt;=3,"B",IF(L9&gt;=2,"C",IF(L9&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -1155,40 +1185,42 @@
           <t>Tarik Hasan</t>
         </is>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="7" t="n">
         <v>48</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="7" t="n">
         <v>42</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="7" t="n">
         <v>46</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="7" t="n">
         <v>44</v>
       </c>
-      <c r="I10" s="4" t="n">
+      <c r="I10" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="J10" t="n">
-        <v>322</v>
-      </c>
-      <c r="K10" t="n">
-        <v>46</v>
-      </c>
-      <c r="L10" t="n">
-        <v>2.14</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="J10">
+        <f>SUM(C10:I10)</f>
+        <v/>
+      </c>
+      <c r="K10" s="4">
+        <f>ROUND(AVERAGE(C10:I10),2)</f>
+        <v/>
+      </c>
+      <c r="L10" s="5">
+        <f>IF(OR(C10&lt;33,D10&lt;33,E10&lt;33,F10&lt;33,G10&lt;33,H10&lt;33,I10&lt;33),0,MIN(5,ROUND((IF(C10&gt;=80,5,IF(C10&gt;=70,4,IF(C10&gt;=60,3.5,IF(C10&gt;=50,3,IF(C10&gt;=40,2,IF(C10&gt;=33,1,0))))))+IF(D10&gt;=80,5,IF(D10&gt;=70,4,IF(D10&gt;=60,3.5,IF(D10&gt;=50,3,IF(D10&gt;=40,2,IF(D10&gt;=33,1,0))))))+IF(E10&gt;=80,5,IF(E10&gt;=70,4,IF(E10&gt;=60,3.5,IF(E10&gt;=50,3,IF(E10&gt;=40,2,IF(E10&gt;=33,1,0))))))+IF(F10&gt;=80,5,IF(F10&gt;=70,4,IF(F10&gt;=60,3.5,IF(F10&gt;=50,3,IF(F10&gt;=40,2,IF(F10&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF(H10&gt;=80,5,IF(H10&gt;=70,4,IF(H10&gt;=60,3.5,IF(H10&gt;=50,3,IF(H10&gt;=40,2,IF(H10&gt;=33,1,0))))))+IF(I10&gt;=80,5,IF(I10&gt;=70,4,IF(I10&gt;=60,3.5,IF(I10&gt;=50,3,IF(I10&gt;=40,2,IF(I10&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M10" s="6">
+        <f>IF(L10&gt;=5,"A+",IF(L10&gt;=4,"A",IF(L10&gt;=3.5,"A-",IF(L10&gt;=3,"B",IF(L10&gt;=2,"C",IF(L10&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -1221,19 +1253,21 @@
       <c r="I11" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="J11" t="n">
-        <v>616</v>
-      </c>
-      <c r="K11" t="n">
-        <v>88</v>
-      </c>
-      <c r="L11" t="n">
-        <v>5</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J11">
+        <f>SUM(C11:I11)</f>
+        <v/>
+      </c>
+      <c r="K11" s="4">
+        <f>ROUND(AVERAGE(C11:I11),2)</f>
+        <v/>
+      </c>
+      <c r="L11" s="5">
+        <f>IF(OR(C11&lt;33,D11&lt;33,E11&lt;33,F11&lt;33,G11&lt;33,H11&lt;33,I11&lt;33),0,MIN(5,ROUND((IF(C11&gt;=80,5,IF(C11&gt;=70,4,IF(C11&gt;=60,3.5,IF(C11&gt;=50,3,IF(C11&gt;=40,2,IF(C11&gt;=33,1,0))))))+IF(D11&gt;=80,5,IF(D11&gt;=70,4,IF(D11&gt;=60,3.5,IF(D11&gt;=50,3,IF(D11&gt;=40,2,IF(D11&gt;=33,1,0))))))+IF(E11&gt;=80,5,IF(E11&gt;=70,4,IF(E11&gt;=60,3.5,IF(E11&gt;=50,3,IF(E11&gt;=40,2,IF(E11&gt;=33,1,0))))))+IF(F11&gt;=80,5,IF(F11&gt;=70,4,IF(F11&gt;=60,3.5,IF(F11&gt;=50,3,IF(F11&gt;=40,2,IF(F11&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF(H11&gt;=80,5,IF(H11&gt;=70,4,IF(H11&gt;=60,3.5,IF(H11&gt;=50,3,IF(H11&gt;=40,2,IF(H11&gt;=33,1,0))))))+IF(I11&gt;=80,5,IF(I11&gt;=70,4,IF(I11&gt;=60,3.5,IF(I11&gt;=50,3,IF(I11&gt;=40,2,IF(I11&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M11" s="6">
+        <f>IF(L11&gt;=5,"A+",IF(L11&gt;=4,"A",IF(L11&gt;=3.5,"A-",IF(L11&gt;=3,"B",IF(L11&gt;=2,"C",IF(L11&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -1266,19 +1300,21 @@
       <c r="I12" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="J12" t="n">
-        <v>616</v>
-      </c>
-      <c r="K12" t="n">
-        <v>88</v>
-      </c>
-      <c r="L12" t="n">
-        <v>5</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J12">
+        <f>SUM(C12:I12)</f>
+        <v/>
+      </c>
+      <c r="K12" s="4">
+        <f>ROUND(AVERAGE(C12:I12),2)</f>
+        <v/>
+      </c>
+      <c r="L12" s="5">
+        <f>IF(OR(C12&lt;33,D12&lt;33,E12&lt;33,F12&lt;33,G12&lt;33,H12&lt;33,I12&lt;33),0,MIN(5,ROUND((IF(C12&gt;=80,5,IF(C12&gt;=70,4,IF(C12&gt;=60,3.5,IF(C12&gt;=50,3,IF(C12&gt;=40,2,IF(C12&gt;=33,1,0))))))+IF(D12&gt;=80,5,IF(D12&gt;=70,4,IF(D12&gt;=60,3.5,IF(D12&gt;=50,3,IF(D12&gt;=40,2,IF(D12&gt;=33,1,0))))))+IF(E12&gt;=80,5,IF(E12&gt;=70,4,IF(E12&gt;=60,3.5,IF(E12&gt;=50,3,IF(E12&gt;=40,2,IF(E12&gt;=33,1,0))))))+IF(F12&gt;=80,5,IF(F12&gt;=70,4,IF(F12&gt;=60,3.5,IF(F12&gt;=50,3,IF(F12&gt;=40,2,IF(F12&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF(H12&gt;=80,5,IF(H12&gt;=70,4,IF(H12&gt;=60,3.5,IF(H12&gt;=50,3,IF(H12&gt;=40,2,IF(H12&gt;=33,1,0))))))+IF(I12&gt;=80,5,IF(I12&gt;=70,4,IF(I12&gt;=60,3.5,IF(I12&gt;=50,3,IF(I12&gt;=40,2,IF(I12&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M12" s="6">
+        <f>IF(L12&gt;=5,"A+",IF(L12&gt;=4,"A",IF(L12&gt;=3.5,"A-",IF(L12&gt;=3,"B",IF(L12&gt;=2,"C",IF(L12&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -1311,19 +1347,21 @@
       <c r="I13" s="3" t="n">
         <v>71</v>
       </c>
-      <c r="J13" t="n">
-        <v>483</v>
-      </c>
-      <c r="K13" t="n">
-        <v>69</v>
-      </c>
-      <c r="L13" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
+      <c r="J13">
+        <f>SUM(C13:I13)</f>
+        <v/>
+      </c>
+      <c r="K13" s="4">
+        <f>ROUND(AVERAGE(C13:I13),2)</f>
+        <v/>
+      </c>
+      <c r="L13" s="5">
+        <f>IF(OR(C13&lt;33,D13&lt;33,E13&lt;33,F13&lt;33,G13&lt;33,H13&lt;33,I13&lt;33),0,MIN(5,ROUND((IF(C13&gt;=80,5,IF(C13&gt;=70,4,IF(C13&gt;=60,3.5,IF(C13&gt;=50,3,IF(C13&gt;=40,2,IF(C13&gt;=33,1,0))))))+IF(D13&gt;=80,5,IF(D13&gt;=70,4,IF(D13&gt;=60,3.5,IF(D13&gt;=50,3,IF(D13&gt;=40,2,IF(D13&gt;=33,1,0))))))+IF(E13&gt;=80,5,IF(E13&gt;=70,4,IF(E13&gt;=60,3.5,IF(E13&gt;=50,3,IF(E13&gt;=40,2,IF(E13&gt;=33,1,0))))))+IF(F13&gt;=80,5,IF(F13&gt;=70,4,IF(F13&gt;=60,3.5,IF(F13&gt;=50,3,IF(F13&gt;=40,2,IF(F13&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF(H13&gt;=80,5,IF(H13&gt;=70,4,IF(H13&gt;=60,3.5,IF(H13&gt;=50,3,IF(H13&gt;=40,2,IF(H13&gt;=33,1,0))))))+IF(I13&gt;=80,5,IF(I13&gt;=70,4,IF(I13&gt;=60,3.5,IF(I13&gt;=50,3,IF(I13&gt;=40,2,IF(I13&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M13" s="6">
+        <f>IF(L13&gt;=5,"A+",IF(L13&gt;=4,"A",IF(L13&gt;=3.5,"A-",IF(L13&gt;=3,"B",IF(L13&gt;=2,"C",IF(L13&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -1356,19 +1394,21 @@
       <c r="I14" s="3" t="n">
         <v>77</v>
       </c>
-      <c r="J14" t="n">
-        <v>532</v>
-      </c>
-      <c r="K14" t="n">
-        <v>76</v>
-      </c>
-      <c r="L14" t="n">
-        <v>4.14</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="J14">
+        <f>SUM(C14:I14)</f>
+        <v/>
+      </c>
+      <c r="K14" s="4">
+        <f>ROUND(AVERAGE(C14:I14),2)</f>
+        <v/>
+      </c>
+      <c r="L14" s="5">
+        <f>IF(OR(C14&lt;33,D14&lt;33,E14&lt;33,F14&lt;33,G14&lt;33,H14&lt;33,I14&lt;33),0,MIN(5,ROUND((IF(C14&gt;=80,5,IF(C14&gt;=70,4,IF(C14&gt;=60,3.5,IF(C14&gt;=50,3,IF(C14&gt;=40,2,IF(C14&gt;=33,1,0))))))+IF(D14&gt;=80,5,IF(D14&gt;=70,4,IF(D14&gt;=60,3.5,IF(D14&gt;=50,3,IF(D14&gt;=40,2,IF(D14&gt;=33,1,0))))))+IF(E14&gt;=80,5,IF(E14&gt;=70,4,IF(E14&gt;=60,3.5,IF(E14&gt;=50,3,IF(E14&gt;=40,2,IF(E14&gt;=33,1,0))))))+IF(F14&gt;=80,5,IF(F14&gt;=70,4,IF(F14&gt;=60,3.5,IF(F14&gt;=50,3,IF(F14&gt;=40,2,IF(F14&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF(H14&gt;=80,5,IF(H14&gt;=70,4,IF(H14&gt;=60,3.5,IF(H14&gt;=50,3,IF(H14&gt;=40,2,IF(H14&gt;=33,1,0))))))+IF(I14&gt;=80,5,IF(I14&gt;=70,4,IF(I14&gt;=60,3.5,IF(I14&gt;=50,3,IF(I14&gt;=40,2,IF(I14&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M14" s="6">
+        <f>IF(L14&gt;=5,"A+",IF(L14&gt;=4,"A",IF(L14&gt;=3.5,"A-",IF(L14&gt;=3,"B",IF(L14&gt;=2,"C",IF(L14&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -1401,19 +1441,21 @@
       <c r="I15" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="J15" t="n">
-        <v>581</v>
-      </c>
-      <c r="K15" t="n">
-        <v>83</v>
-      </c>
-      <c r="L15" t="n">
-        <v>5</v>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J15">
+        <f>SUM(C15:I15)</f>
+        <v/>
+      </c>
+      <c r="K15" s="4">
+        <f>ROUND(AVERAGE(C15:I15),2)</f>
+        <v/>
+      </c>
+      <c r="L15" s="5">
+        <f>IF(OR(C15&lt;33,D15&lt;33,E15&lt;33,F15&lt;33,G15&lt;33,H15&lt;33,I15&lt;33),0,MIN(5,ROUND((IF(C15&gt;=80,5,IF(C15&gt;=70,4,IF(C15&gt;=60,3.5,IF(C15&gt;=50,3,IF(C15&gt;=40,2,IF(C15&gt;=33,1,0))))))+IF(D15&gt;=80,5,IF(D15&gt;=70,4,IF(D15&gt;=60,3.5,IF(D15&gt;=50,3,IF(D15&gt;=40,2,IF(D15&gt;=33,1,0))))))+IF(E15&gt;=80,5,IF(E15&gt;=70,4,IF(E15&gt;=60,3.5,IF(E15&gt;=50,3,IF(E15&gt;=40,2,IF(E15&gt;=33,1,0))))))+IF(F15&gt;=80,5,IF(F15&gt;=70,4,IF(F15&gt;=60,3.5,IF(F15&gt;=50,3,IF(F15&gt;=40,2,IF(F15&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF(H15&gt;=80,5,IF(H15&gt;=70,4,IF(H15&gt;=60,3.5,IF(H15&gt;=50,3,IF(H15&gt;=40,2,IF(H15&gt;=33,1,0))))))+IF(I15&gt;=80,5,IF(I15&gt;=70,4,IF(I15&gt;=60,3.5,IF(I15&gt;=50,3,IF(I15&gt;=40,2,IF(I15&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M15" s="6">
+        <f>IF(L15&gt;=5,"A+",IF(L15&gt;=4,"A",IF(L15&gt;=3.5,"A-",IF(L15&gt;=3,"B",IF(L15&gt;=2,"C",IF(L15&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -1425,10 +1467,10 @@
           <t>Imran Khan</t>
         </is>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="7" t="n">
         <v>58</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="7" t="n">
         <v>55</v>
       </c>
       <c r="E16" s="3" t="n">
@@ -1437,28 +1479,30 @@
       <c r="F16" s="3" t="n">
         <v>62</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="7" t="n">
         <v>54</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="7" t="n">
         <v>56</v>
       </c>
-      <c r="I16" s="4" t="n">
+      <c r="I16" s="7" t="n">
         <v>59</v>
       </c>
-      <c r="J16" t="n">
-        <v>404</v>
-      </c>
-      <c r="K16" t="n">
-        <v>57.71</v>
-      </c>
-      <c r="L16" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="J16">
+        <f>SUM(C16:I16)</f>
+        <v/>
+      </c>
+      <c r="K16" s="4">
+        <f>ROUND(AVERAGE(C16:I16),2)</f>
+        <v/>
+      </c>
+      <c r="L16" s="5">
+        <f>IF(OR(C16&lt;33,D16&lt;33,E16&lt;33,F16&lt;33,G16&lt;33,H16&lt;33,I16&lt;33),0,MIN(5,ROUND((IF(C16&gt;=80,5,IF(C16&gt;=70,4,IF(C16&gt;=60,3.5,IF(C16&gt;=50,3,IF(C16&gt;=40,2,IF(C16&gt;=33,1,0))))))+IF(D16&gt;=80,5,IF(D16&gt;=70,4,IF(D16&gt;=60,3.5,IF(D16&gt;=50,3,IF(D16&gt;=40,2,IF(D16&gt;=33,1,0))))))+IF(E16&gt;=80,5,IF(E16&gt;=70,4,IF(E16&gt;=60,3.5,IF(E16&gt;=50,3,IF(E16&gt;=40,2,IF(E16&gt;=33,1,0))))))+IF(F16&gt;=80,5,IF(F16&gt;=70,4,IF(F16&gt;=60,3.5,IF(F16&gt;=50,3,IF(F16&gt;=40,2,IF(F16&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF(H16&gt;=80,5,IF(H16&gt;=70,4,IF(H16&gt;=60,3.5,IF(H16&gt;=50,3,IF(H16&gt;=40,2,IF(H16&gt;=33,1,0))))))+IF(I16&gt;=80,5,IF(I16&gt;=70,4,IF(I16&gt;=60,3.5,IF(I16&gt;=50,3,IF(I16&gt;=40,2,IF(I16&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M16" s="6">
+        <f>IF(L16&gt;=5,"A+",IF(L16&gt;=4,"A",IF(L16&gt;=3.5,"A-",IF(L16&gt;=3,"B",IF(L16&gt;=2,"C",IF(L16&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -1491,19 +1535,21 @@
       <c r="I17" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="J17" t="n">
-        <v>612</v>
-      </c>
-      <c r="K17" t="n">
-        <v>87.43000000000001</v>
-      </c>
-      <c r="L17" t="n">
-        <v>5</v>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J17">
+        <f>SUM(C17:I17)</f>
+        <v/>
+      </c>
+      <c r="K17" s="4">
+        <f>ROUND(AVERAGE(C17:I17),2)</f>
+        <v/>
+      </c>
+      <c r="L17" s="5">
+        <f>IF(OR(C17&lt;33,D17&lt;33,E17&lt;33,F17&lt;33,G17&lt;33,H17&lt;33,I17&lt;33),0,MIN(5,ROUND((IF(C17&gt;=80,5,IF(C17&gt;=70,4,IF(C17&gt;=60,3.5,IF(C17&gt;=50,3,IF(C17&gt;=40,2,IF(C17&gt;=33,1,0))))))+IF(D17&gt;=80,5,IF(D17&gt;=70,4,IF(D17&gt;=60,3.5,IF(D17&gt;=50,3,IF(D17&gt;=40,2,IF(D17&gt;=33,1,0))))))+IF(E17&gt;=80,5,IF(E17&gt;=70,4,IF(E17&gt;=60,3.5,IF(E17&gt;=50,3,IF(E17&gt;=40,2,IF(E17&gt;=33,1,0))))))+IF(F17&gt;=80,5,IF(F17&gt;=70,4,IF(F17&gt;=60,3.5,IF(F17&gt;=50,3,IF(F17&gt;=40,2,IF(F17&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF(H17&gt;=80,5,IF(H17&gt;=70,4,IF(H17&gt;=60,3.5,IF(H17&gt;=50,3,IF(H17&gt;=40,2,IF(H17&gt;=33,1,0))))))+IF(I17&gt;=80,5,IF(I17&gt;=70,4,IF(I17&gt;=60,3.5,IF(I17&gt;=50,3,IF(I17&gt;=40,2,IF(I17&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M17" s="6">
+        <f>IF(L17&gt;=5,"A+",IF(L17&gt;=4,"A",IF(L17&gt;=3.5,"A-",IF(L17&gt;=3,"B",IF(L17&gt;=2,"C",IF(L17&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -1536,19 +1582,21 @@
       <c r="I18" s="3" t="n">
         <v>73</v>
       </c>
-      <c r="J18" t="n">
-        <v>498</v>
-      </c>
-      <c r="K18" t="n">
-        <v>71.14</v>
-      </c>
-      <c r="L18" t="n">
-        <v>3.93</v>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
+      <c r="J18">
+        <f>SUM(C18:I18)</f>
+        <v/>
+      </c>
+      <c r="K18" s="4">
+        <f>ROUND(AVERAGE(C18:I18),2)</f>
+        <v/>
+      </c>
+      <c r="L18" s="5">
+        <f>IF(OR(C18&lt;33,D18&lt;33,E18&lt;33,F18&lt;33,G18&lt;33,H18&lt;33,I18&lt;33),0,MIN(5,ROUND((IF(C18&gt;=80,5,IF(C18&gt;=70,4,IF(C18&gt;=60,3.5,IF(C18&gt;=50,3,IF(C18&gt;=40,2,IF(C18&gt;=33,1,0))))))+IF(D18&gt;=80,5,IF(D18&gt;=70,4,IF(D18&gt;=60,3.5,IF(D18&gt;=50,3,IF(D18&gt;=40,2,IF(D18&gt;=33,1,0))))))+IF(E18&gt;=80,5,IF(E18&gt;=70,4,IF(E18&gt;=60,3.5,IF(E18&gt;=50,3,IF(E18&gt;=40,2,IF(E18&gt;=33,1,0))))))+IF(F18&gt;=80,5,IF(F18&gt;=70,4,IF(F18&gt;=60,3.5,IF(F18&gt;=50,3,IF(F18&gt;=40,2,IF(F18&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF(H18&gt;=80,5,IF(H18&gt;=70,4,IF(H18&gt;=60,3.5,IF(H18&gt;=50,3,IF(H18&gt;=40,2,IF(H18&gt;=33,1,0))))))+IF(I18&gt;=80,5,IF(I18&gt;=70,4,IF(I18&gt;=60,3.5,IF(I18&gt;=50,3,IF(I18&gt;=40,2,IF(I18&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M18" s="6">
+        <f>IF(L18&gt;=5,"A+",IF(L18&gt;=4,"A",IF(L18&gt;=3.5,"A-",IF(L18&gt;=3,"B",IF(L18&gt;=2,"C",IF(L18&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -1581,19 +1629,21 @@
       <c r="I19" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="J19" t="n">
-        <v>607</v>
-      </c>
-      <c r="K19" t="n">
-        <v>86.70999999999999</v>
-      </c>
-      <c r="L19" t="n">
-        <v>5</v>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J19">
+        <f>SUM(C19:I19)</f>
+        <v/>
+      </c>
+      <c r="K19" s="4">
+        <f>ROUND(AVERAGE(C19:I19),2)</f>
+        <v/>
+      </c>
+      <c r="L19" s="5">
+        <f>IF(OR(C19&lt;33,D19&lt;33,E19&lt;33,F19&lt;33,G19&lt;33,H19&lt;33,I19&lt;33),0,MIN(5,ROUND((IF(C19&gt;=80,5,IF(C19&gt;=70,4,IF(C19&gt;=60,3.5,IF(C19&gt;=50,3,IF(C19&gt;=40,2,IF(C19&gt;=33,1,0))))))+IF(D19&gt;=80,5,IF(D19&gt;=70,4,IF(D19&gt;=60,3.5,IF(D19&gt;=50,3,IF(D19&gt;=40,2,IF(D19&gt;=33,1,0))))))+IF(E19&gt;=80,5,IF(E19&gt;=70,4,IF(E19&gt;=60,3.5,IF(E19&gt;=50,3,IF(E19&gt;=40,2,IF(E19&gt;=33,1,0))))))+IF(F19&gt;=80,5,IF(F19&gt;=70,4,IF(F19&gt;=60,3.5,IF(F19&gt;=50,3,IF(F19&gt;=40,2,IF(F19&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF(H19&gt;=80,5,IF(H19&gt;=70,4,IF(H19&gt;=60,3.5,IF(H19&gt;=50,3,IF(H19&gt;=40,2,IF(H19&gt;=33,1,0))))))+IF(I19&gt;=80,5,IF(I19&gt;=70,4,IF(I19&gt;=60,3.5,IF(I19&gt;=50,3,IF(I19&gt;=40,2,IF(I19&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M19" s="6">
+        <f>IF(L19&gt;=5,"A+",IF(L19&gt;=4,"A",IF(L19&gt;=3.5,"A-",IF(L19&gt;=3,"B",IF(L19&gt;=2,"C",IF(L19&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -1626,19 +1676,21 @@
       <c r="I20" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="J20" t="n">
-        <v>448</v>
-      </c>
-      <c r="K20" t="n">
-        <v>64</v>
-      </c>
-      <c r="L20" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
+      <c r="J20">
+        <f>SUM(C20:I20)</f>
+        <v/>
+      </c>
+      <c r="K20" s="4">
+        <f>ROUND(AVERAGE(C20:I20),2)</f>
+        <v/>
+      </c>
+      <c r="L20" s="5">
+        <f>IF(OR(C20&lt;33,D20&lt;33,E20&lt;33,F20&lt;33,G20&lt;33,H20&lt;33,I20&lt;33),0,MIN(5,ROUND((IF(C20&gt;=80,5,IF(C20&gt;=70,4,IF(C20&gt;=60,3.5,IF(C20&gt;=50,3,IF(C20&gt;=40,2,IF(C20&gt;=33,1,0))))))+IF(D20&gt;=80,5,IF(D20&gt;=70,4,IF(D20&gt;=60,3.5,IF(D20&gt;=50,3,IF(D20&gt;=40,2,IF(D20&gt;=33,1,0))))))+IF(E20&gt;=80,5,IF(E20&gt;=70,4,IF(E20&gt;=60,3.5,IF(E20&gt;=50,3,IF(E20&gt;=40,2,IF(E20&gt;=33,1,0))))))+IF(F20&gt;=80,5,IF(F20&gt;=70,4,IF(F20&gt;=60,3.5,IF(F20&gt;=50,3,IF(F20&gt;=40,2,IF(F20&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF(H20&gt;=80,5,IF(H20&gt;=70,4,IF(H20&gt;=60,3.5,IF(H20&gt;=50,3,IF(H20&gt;=40,2,IF(H20&gt;=33,1,0))))))+IF(I20&gt;=80,5,IF(I20&gt;=70,4,IF(I20&gt;=60,3.5,IF(I20&gt;=50,3,IF(I20&gt;=40,2,IF(I20&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M20" s="6">
+        <f>IF(L20&gt;=5,"A+",IF(L20&gt;=4,"A",IF(L20&gt;=3.5,"A-",IF(L20&gt;=3,"B",IF(L20&gt;=2,"C",IF(L20&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -1671,19 +1723,21 @@
       <c r="I21" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="J21" t="n">
-        <v>635</v>
-      </c>
-      <c r="K21" t="n">
-        <v>90.70999999999999</v>
-      </c>
-      <c r="L21" t="n">
-        <v>5</v>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
+      <c r="J21">
+        <f>SUM(C21:I21)</f>
+        <v/>
+      </c>
+      <c r="K21" s="4">
+        <f>ROUND(AVERAGE(C21:I21),2)</f>
+        <v/>
+      </c>
+      <c r="L21" s="5">
+        <f>IF(OR(C21&lt;33,D21&lt;33,E21&lt;33,F21&lt;33,G21&lt;33,H21&lt;33,I21&lt;33),0,MIN(5,ROUND((IF(C21&gt;=80,5,IF(C21&gt;=70,4,IF(C21&gt;=60,3.5,IF(C21&gt;=50,3,IF(C21&gt;=40,2,IF(C21&gt;=33,1,0))))))+IF(D21&gt;=80,5,IF(D21&gt;=70,4,IF(D21&gt;=60,3.5,IF(D21&gt;=50,3,IF(D21&gt;=40,2,IF(D21&gt;=33,1,0))))))+IF(E21&gt;=80,5,IF(E21&gt;=70,4,IF(E21&gt;=60,3.5,IF(E21&gt;=50,3,IF(E21&gt;=40,2,IF(E21&gt;=33,1,0))))))+IF(F21&gt;=80,5,IF(F21&gt;=70,4,IF(F21&gt;=60,3.5,IF(F21&gt;=50,3,IF(F21&gt;=40,2,IF(F21&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF(H21&gt;=80,5,IF(H21&gt;=70,4,IF(H21&gt;=60,3.5,IF(H21&gt;=50,3,IF(H21&gt;=40,2,IF(H21&gt;=33,1,0))))))+IF(I21&gt;=80,5,IF(I21&gt;=70,4,IF(I21&gt;=60,3.5,IF(I21&gt;=50,3,IF(I21&gt;=40,2,IF(I21&gt;=33,1,0)))))))/7,2)))</f>
+        <v/>
+      </c>
+      <c r="M21" s="6">
+        <f>IF(L21&gt;=5,"A+",IF(L21&gt;=4,"A",IF(L21&gt;=3.5,"A-",IF(L21&gt;=3,"B",IF(L21&gt;=2,"C",IF(L21&gt;=1,"D","F"))))))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1767,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>📊 ACADEMIC RESULTS DASHBOARD</t>
         </is>
@@ -1721,267 +1775,297 @@
     </row>
     <row r="2"/>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>SUMMARY STATISTICS</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Total Students:</t>
         </is>
       </c>
-      <c r="C5" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="C5" s="11">
+        <f>COUNTA('Data Source'!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="E5" s="10" t="inlineStr">
         <is>
           <t>Average GPA:</t>
         </is>
       </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>4.25</t>
-        </is>
-      </c>
-      <c r="H5" s="7" t="inlineStr">
+      <c r="F5" s="12">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!L:L),2), 0)</f>
+        <v/>
+      </c>
+      <c r="H5" s="10" t="inlineStr">
         <is>
           <t>Highest Total:</t>
         </is>
       </c>
-      <c r="I5" s="8" t="n">
-        <v>658</v>
-      </c>
-      <c r="K5" s="7" t="inlineStr">
+      <c r="I5" s="11">
+        <f>MAX('Data Source'!J:J)</f>
+        <v/>
+      </c>
+      <c r="K5" s="10" t="inlineStr">
         <is>
           <t>Pass Rate:</t>
         </is>
       </c>
-      <c r="L5" s="8" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
+      <c r="L5" s="13">
+        <f>IF(C5&gt;0,COUNTIF('Data Source'!L:L,"&gt;0")/C5,0)</f>
+        <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="A7" s="14" t="inlineStr">
         <is>
           <t>GRADE DISTRIBUTION</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
+      <c r="D7" s="14" t="inlineStr">
         <is>
           <t>SUBJECT-WISE AVERAGE</t>
         </is>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="G7" s="14" t="inlineStr">
         <is>
           <t>TOP 5 STUDENTS</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="15" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="15" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="15" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="15" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="10" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="15" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="B9" s="6">
+        <f>COUNTIF('Data Source'!M:M,"A+")</f>
+        <v/>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bangla</t>
+        </is>
+      </c>
+      <c r="E9" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!C:C),2),0)</f>
+        <v/>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>'Data Source'!B3</f>
+        <v/>
+      </c>
+      <c r="I9" s="5">
+        <f>'Data Source'!L3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" s="6">
+        <f>COUNTIF('Data Source'!M:M,"A")</f>
+        <v/>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E10" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!D:D),2),0)</f>
+        <v/>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <f>'Data Source'!B5</f>
+        <v/>
+      </c>
+      <c r="I10" s="5">
+        <f>'Data Source'!L5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="B11" s="6">
+        <f>COUNTIF('Data Source'!M:M,"A-")</f>
+        <v/>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+      <c r="E11" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!E:E),2),0)</f>
+        <v/>
+      </c>
+      <c r="G11" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Bangla</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>76.09999999999999</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Fatima Khan</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
+      <c r="H11">
+        <f>'Data Source'!B7</f>
+        <v/>
+      </c>
+      <c r="I11" s="5">
+        <f>'Data Source'!L7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B12" s="6">
+        <f>COUNTIF('Data Source'!M:M,"B")</f>
+        <v/>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ICT</t>
+        </is>
+      </c>
+      <c r="E12" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!F:F),2),0)</f>
+        <v/>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <f>'Data Source'!B11</f>
+        <v/>
+      </c>
+      <c r="I12" s="5">
+        <f>'Data Source'!L11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B13" s="6">
+        <f>COUNTIF('Data Source'!M:M,"C")</f>
+        <v/>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Physics</t>
+        </is>
+      </c>
+      <c r="E13" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!G:G),2),0)</f>
+        <v/>
+      </c>
+      <c r="G13" s="6" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>74.7</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Ayesha Begum</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Mathematics</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>77.3</v>
-      </c>
-      <c r="G11" t="n">
-        <v>3</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Nadia Islam</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ICT</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>79</v>
-      </c>
-      <c r="G12" t="n">
-        <v>4</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Ruhi Akter</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Physics</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>73.59999999999999</v>
-      </c>
-      <c r="G13" t="n">
-        <v>5</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Mehedi Hassan</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>5</v>
+      <c r="H13">
+        <f>'Data Source'!B12</f>
+        <v/>
+      </c>
+      <c r="I13" s="5">
+        <f>'Data Source'!L12</f>
+        <v/>
       </c>
     </row>
     <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B14" s="6">
+        <f>COUNTIF('Data Source'!M:M,"D")</f>
+        <v/>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>Chemistry</t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>75.65000000000001</v>
+      <c r="E14" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!H:H),2),0)</f>
+        <v/>
       </c>
     </row>
     <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B15" s="6">
+        <f>COUNTIF('Data Source'!M:M,"F")</f>
+        <v/>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>Biology</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>77.3</v>
+      <c r="E15" s="5">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!I:I),2),0)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GPA calculation for Quran Mazid to reflect new marking scheme and adjust related logic in Excel generation
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -72,14 +72,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0070AD47"/>
-        <bgColor rgb="0070AD47"/>
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
+        <fgColor rgb="0070AD47"/>
+        <bgColor rgb="0070AD47"/>
       </patternFill>
     </fill>
     <fill>
@@ -106,8 +106,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>143</v>
@@ -937,7 +937,7 @@
         <v>92</v>
       </c>
       <c r="N2" s="4">
-        <f>IF(C2&gt;=80,"A+",IF(C2&gt;=70,"A",IF(C2&gt;=60,"A-",IF(C2&gt;=50,"B",IF(C2&gt;=40,"C",IF(C2&gt;=33,"D","F"))))))</f>
+        <f>IF(C2/200*100&gt;=80,"A+",IF(C2/200*100&gt;=70,"A",IF(C2/200*100&gt;=60,"A-",IF(C2/200*100&gt;=50,"B",IF(C2/200*100&gt;=40,"C",IF(C2/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O2" s="4">
@@ -989,7 +989,7 @@
         <v/>
       </c>
       <c r="AA2" s="6">
-        <f>IF(OR(C2&lt;33,D2&lt;66,E2&lt;33,F2&lt;66,G2&lt;66,H2&lt;33,I2&lt;33,J2&lt;33,L2&lt;33,M2&lt;33),0,MIN(5,ROUND((IF(C2&gt;=80,5,IF(C2&gt;=70,4,IF(C2&gt;=60,3.5,IF(C2&gt;=50,3,IF(C2&gt;=40,2,IF(C2&gt;=33,1,0))))))+IF(D2/200*100&gt;=80,5,IF(D2/200*100&gt;=70,4,IF(D2/200*100&gt;=60,3.5,IF(D2/200*100&gt;=50,3,IF(D2/200*100&gt;=40,2,IF(D2/200*100&gt;=33,1,0))))))+IF(E2&gt;=80,5,IF(E2&gt;=70,4,IF(E2&gt;=60,3.5,IF(E2&gt;=50,3,IF(E2&gt;=40,2,IF(E2&gt;=33,1,0))))))+IF(F2/200*100&gt;=80,5,IF(F2/200*100&gt;=70,4,IF(F2/200*100&gt;=60,3.5,IF(F2/200*100&gt;=50,3,IF(F2/200*100&gt;=40,2,IF(F2/200*100&gt;=33,1,0))))))+IF(G2/200*100&gt;=80,5,IF(G2/200*100&gt;=70,4,IF(G2/200*100&gt;=60,3.5,IF(G2/200*100&gt;=50,3,IF(G2/200*100&gt;=40,2,IF(G2/200*100&gt;=33,1,0))))))+IF(H2&gt;=80,5,IF(H2&gt;=70,4,IF(H2&gt;=60,3.5,IF(H2&gt;=50,3,IF(H2&gt;=40,2,IF(H2&gt;=33,1,0))))))+IF(I2&gt;=80,5,IF(I2&gt;=70,4,IF(I2&gt;=60,3.5,IF(I2&gt;=50,3,IF(I2&gt;=40,2,IF(I2&gt;=33,1,0))))))+IF(J2&gt;=80,5,IF(J2&gt;=70,4,IF(J2&gt;=60,3.5,IF(J2&gt;=50,3,IF(J2&gt;=40,2,IF(J2&gt;=33,1,0)))))))/8+IF(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))&gt;=2,(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C2&lt;66,D2&lt;66,E2&lt;33,F2&lt;66,G2&lt;66,H2&lt;33,I2&lt;33,J2&lt;33,L2&lt;33,M2&lt;33),0,MIN(5,ROUND((IF(C2/200*100&gt;=80,5,IF(C2/200*100&gt;=70,4,IF(C2/200*100&gt;=60,3.5,IF(C2/200*100&gt;=50,3,IF(C2/200*100&gt;=40,2,IF(C2/200*100&gt;=33,1,0))))))+IF(D2/200*100&gt;=80,5,IF(D2/200*100&gt;=70,4,IF(D2/200*100&gt;=60,3.5,IF(D2/200*100&gt;=50,3,IF(D2/200*100&gt;=40,2,IF(D2/200*100&gt;=33,1,0))))))+IF(E2&gt;=80,5,IF(E2&gt;=70,4,IF(E2&gt;=60,3.5,IF(E2&gt;=50,3,IF(E2&gt;=40,2,IF(E2&gt;=33,1,0))))))+IF(F2/200*100&gt;=80,5,IF(F2/200*100&gt;=70,4,IF(F2/200*100&gt;=60,3.5,IF(F2/200*100&gt;=50,3,IF(F2/200*100&gt;=40,2,IF(F2/200*100&gt;=33,1,0))))))+IF(G2/200*100&gt;=80,5,IF(G2/200*100&gt;=70,4,IF(G2/200*100&gt;=60,3.5,IF(G2/200*100&gt;=50,3,IF(G2/200*100&gt;=40,2,IF(G2/200*100&gt;=33,1,0))))))+IF(H2&gt;=80,5,IF(H2&gt;=70,4,IF(H2&gt;=60,3.5,IF(H2&gt;=50,3,IF(H2&gt;=40,2,IF(H2&gt;=33,1,0))))))+IF(I2&gt;=80,5,IF(I2&gt;=70,4,IF(I2&gt;=60,3.5,IF(I2&gt;=50,3,IF(I2&gt;=40,2,IF(I2&gt;=33,1,0))))))+IF(J2&gt;=80,5,IF(J2&gt;=70,4,IF(J2&gt;=60,3.5,IF(J2&gt;=50,3,IF(J2&gt;=40,2,IF(J2&gt;=33,1,0)))))))/8+IF(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))&gt;=2,(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB2" s="4">
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>144</v>
@@ -1040,7 +1040,7 @@
         <v>80</v>
       </c>
       <c r="N3" s="4">
-        <f>IF(C3&gt;=80,"A+",IF(C3&gt;=70,"A",IF(C3&gt;=60,"A-",IF(C3&gt;=50,"B",IF(C3&gt;=40,"C",IF(C3&gt;=33,"D","F"))))))</f>
+        <f>IF(C3/200*100&gt;=80,"A+",IF(C3/200*100&gt;=70,"A",IF(C3/200*100&gt;=60,"A-",IF(C3/200*100&gt;=50,"B",IF(C3/200*100&gt;=40,"C",IF(C3/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O3" s="4">
@@ -1092,7 +1092,7 @@
         <v/>
       </c>
       <c r="AA3" s="6">
-        <f>IF(OR(C3&lt;33,D3&lt;66,E3&lt;33,F3&lt;66,G3&lt;66,H3&lt;33,I3&lt;33,J3&lt;33,L3&lt;33,M3&lt;33),0,MIN(5,ROUND((IF(C3&gt;=80,5,IF(C3&gt;=70,4,IF(C3&gt;=60,3.5,IF(C3&gt;=50,3,IF(C3&gt;=40,2,IF(C3&gt;=33,1,0))))))+IF(D3/200*100&gt;=80,5,IF(D3/200*100&gt;=70,4,IF(D3/200*100&gt;=60,3.5,IF(D3/200*100&gt;=50,3,IF(D3/200*100&gt;=40,2,IF(D3/200*100&gt;=33,1,0))))))+IF(E3&gt;=80,5,IF(E3&gt;=70,4,IF(E3&gt;=60,3.5,IF(E3&gt;=50,3,IF(E3&gt;=40,2,IF(E3&gt;=33,1,0))))))+IF(F3/200*100&gt;=80,5,IF(F3/200*100&gt;=70,4,IF(F3/200*100&gt;=60,3.5,IF(F3/200*100&gt;=50,3,IF(F3/200*100&gt;=40,2,IF(F3/200*100&gt;=33,1,0))))))+IF(G3/200*100&gt;=80,5,IF(G3/200*100&gt;=70,4,IF(G3/200*100&gt;=60,3.5,IF(G3/200*100&gt;=50,3,IF(G3/200*100&gt;=40,2,IF(G3/200*100&gt;=33,1,0))))))+IF(H3&gt;=80,5,IF(H3&gt;=70,4,IF(H3&gt;=60,3.5,IF(H3&gt;=50,3,IF(H3&gt;=40,2,IF(H3&gt;=33,1,0))))))+IF(I3&gt;=80,5,IF(I3&gt;=70,4,IF(I3&gt;=60,3.5,IF(I3&gt;=50,3,IF(I3&gt;=40,2,IF(I3&gt;=33,1,0))))))+IF(J3&gt;=80,5,IF(J3&gt;=70,4,IF(J3&gt;=60,3.5,IF(J3&gt;=50,3,IF(J3&gt;=40,2,IF(J3&gt;=33,1,0)))))))/8+IF(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))&gt;=2,(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C3&lt;66,D3&lt;66,E3&lt;33,F3&lt;66,G3&lt;66,H3&lt;33,I3&lt;33,J3&lt;33,L3&lt;33,M3&lt;33),0,MIN(5,ROUND((IF(C3/200*100&gt;=80,5,IF(C3/200*100&gt;=70,4,IF(C3/200*100&gt;=60,3.5,IF(C3/200*100&gt;=50,3,IF(C3/200*100&gt;=40,2,IF(C3/200*100&gt;=33,1,0))))))+IF(D3/200*100&gt;=80,5,IF(D3/200*100&gt;=70,4,IF(D3/200*100&gt;=60,3.5,IF(D3/200*100&gt;=50,3,IF(D3/200*100&gt;=40,2,IF(D3/200*100&gt;=33,1,0))))))+IF(E3&gt;=80,5,IF(E3&gt;=70,4,IF(E3&gt;=60,3.5,IF(E3&gt;=50,3,IF(E3&gt;=40,2,IF(E3&gt;=33,1,0))))))+IF(F3/200*100&gt;=80,5,IF(F3/200*100&gt;=70,4,IF(F3/200*100&gt;=60,3.5,IF(F3/200*100&gt;=50,3,IF(F3/200*100&gt;=40,2,IF(F3/200*100&gt;=33,1,0))))))+IF(G3/200*100&gt;=80,5,IF(G3/200*100&gt;=70,4,IF(G3/200*100&gt;=60,3.5,IF(G3/200*100&gt;=50,3,IF(G3/200*100&gt;=40,2,IF(G3/200*100&gt;=33,1,0))))))+IF(H3&gt;=80,5,IF(H3&gt;=70,4,IF(H3&gt;=60,3.5,IF(H3&gt;=50,3,IF(H3&gt;=40,2,IF(H3&gt;=33,1,0))))))+IF(I3&gt;=80,5,IF(I3&gt;=70,4,IF(I3&gt;=60,3.5,IF(I3&gt;=50,3,IF(I3&gt;=40,2,IF(I3&gt;=33,1,0))))))+IF(J3&gt;=80,5,IF(J3&gt;=70,4,IF(J3&gt;=60,3.5,IF(J3&gt;=50,3,IF(J3&gt;=40,2,IF(J3&gt;=33,1,0)))))))/8+IF(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))&gt;=2,(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB3" s="4">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>162</v>
@@ -1143,7 +1143,7 @@
         <v>83</v>
       </c>
       <c r="N4" s="4">
-        <f>IF(C4&gt;=80,"A+",IF(C4&gt;=70,"A",IF(C4&gt;=60,"A-",IF(C4&gt;=50,"B",IF(C4&gt;=40,"C",IF(C4&gt;=33,"D","F"))))))</f>
+        <f>IF(C4/200*100&gt;=80,"A+",IF(C4/200*100&gt;=70,"A",IF(C4/200*100&gt;=60,"A-",IF(C4/200*100&gt;=50,"B",IF(C4/200*100&gt;=40,"C",IF(C4/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O4" s="4">
@@ -1195,7 +1195,7 @@
         <v/>
       </c>
       <c r="AA4" s="6">
-        <f>IF(OR(C4&lt;33,D4&lt;66,E4&lt;33,F4&lt;66,G4&lt;66,H4&lt;33,I4&lt;33,J4&lt;33,L4&lt;33,M4&lt;33),0,MIN(5,ROUND((IF(C4&gt;=80,5,IF(C4&gt;=70,4,IF(C4&gt;=60,3.5,IF(C4&gt;=50,3,IF(C4&gt;=40,2,IF(C4&gt;=33,1,0))))))+IF(D4/200*100&gt;=80,5,IF(D4/200*100&gt;=70,4,IF(D4/200*100&gt;=60,3.5,IF(D4/200*100&gt;=50,3,IF(D4/200*100&gt;=40,2,IF(D4/200*100&gt;=33,1,0))))))+IF(E4&gt;=80,5,IF(E4&gt;=70,4,IF(E4&gt;=60,3.5,IF(E4&gt;=50,3,IF(E4&gt;=40,2,IF(E4&gt;=33,1,0))))))+IF(F4/200*100&gt;=80,5,IF(F4/200*100&gt;=70,4,IF(F4/200*100&gt;=60,3.5,IF(F4/200*100&gt;=50,3,IF(F4/200*100&gt;=40,2,IF(F4/200*100&gt;=33,1,0))))))+IF(G4/200*100&gt;=80,5,IF(G4/200*100&gt;=70,4,IF(G4/200*100&gt;=60,3.5,IF(G4/200*100&gt;=50,3,IF(G4/200*100&gt;=40,2,IF(G4/200*100&gt;=33,1,0))))))+IF(H4&gt;=80,5,IF(H4&gt;=70,4,IF(H4&gt;=60,3.5,IF(H4&gt;=50,3,IF(H4&gt;=40,2,IF(H4&gt;=33,1,0))))))+IF(I4&gt;=80,5,IF(I4&gt;=70,4,IF(I4&gt;=60,3.5,IF(I4&gt;=50,3,IF(I4&gt;=40,2,IF(I4&gt;=33,1,0))))))+IF(J4&gt;=80,5,IF(J4&gt;=70,4,IF(J4&gt;=60,3.5,IF(J4&gt;=50,3,IF(J4&gt;=40,2,IF(J4&gt;=33,1,0)))))))/8+IF(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))&gt;=2,(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C4&lt;66,D4&lt;66,E4&lt;33,F4&lt;66,G4&lt;66,H4&lt;33,I4&lt;33,J4&lt;33,L4&lt;33,M4&lt;33),0,MIN(5,ROUND((IF(C4/200*100&gt;=80,5,IF(C4/200*100&gt;=70,4,IF(C4/200*100&gt;=60,3.5,IF(C4/200*100&gt;=50,3,IF(C4/200*100&gt;=40,2,IF(C4/200*100&gt;=33,1,0))))))+IF(D4/200*100&gt;=80,5,IF(D4/200*100&gt;=70,4,IF(D4/200*100&gt;=60,3.5,IF(D4/200*100&gt;=50,3,IF(D4/200*100&gt;=40,2,IF(D4/200*100&gt;=33,1,0))))))+IF(E4&gt;=80,5,IF(E4&gt;=70,4,IF(E4&gt;=60,3.5,IF(E4&gt;=50,3,IF(E4&gt;=40,2,IF(E4&gt;=33,1,0))))))+IF(F4/200*100&gt;=80,5,IF(F4/200*100&gt;=70,4,IF(F4/200*100&gt;=60,3.5,IF(F4/200*100&gt;=50,3,IF(F4/200*100&gt;=40,2,IF(F4/200*100&gt;=33,1,0))))))+IF(G4/200*100&gt;=80,5,IF(G4/200*100&gt;=70,4,IF(G4/200*100&gt;=60,3.5,IF(G4/200*100&gt;=50,3,IF(G4/200*100&gt;=40,2,IF(G4/200*100&gt;=33,1,0))))))+IF(H4&gt;=80,5,IF(H4&gt;=70,4,IF(H4&gt;=60,3.5,IF(H4&gt;=50,3,IF(H4&gt;=40,2,IF(H4&gt;=33,1,0))))))+IF(I4&gt;=80,5,IF(I4&gt;=70,4,IF(I4&gt;=60,3.5,IF(I4&gt;=50,3,IF(I4&gt;=40,2,IF(I4&gt;=33,1,0))))))+IF(J4&gt;=80,5,IF(J4&gt;=70,4,IF(J4&gt;=60,3.5,IF(J4&gt;=50,3,IF(J4&gt;=40,2,IF(J4&gt;=33,1,0)))))))/8+IF(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))&gt;=2,(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB4" s="4">
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>168</v>
@@ -1246,7 +1246,7 @@
         <v>91</v>
       </c>
       <c r="N5" s="4">
-        <f>IF(C5&gt;=80,"A+",IF(C5&gt;=70,"A",IF(C5&gt;=60,"A-",IF(C5&gt;=50,"B",IF(C5&gt;=40,"C",IF(C5&gt;=33,"D","F"))))))</f>
+        <f>IF(C5/200*100&gt;=80,"A+",IF(C5/200*100&gt;=70,"A",IF(C5/200*100&gt;=60,"A-",IF(C5/200*100&gt;=50,"B",IF(C5/200*100&gt;=40,"C",IF(C5/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O5" s="4">
@@ -1298,7 +1298,7 @@
         <v/>
       </c>
       <c r="AA5" s="6">
-        <f>IF(OR(C5&lt;33,D5&lt;66,E5&lt;33,F5&lt;66,G5&lt;66,H5&lt;33,I5&lt;33,J5&lt;33,L5&lt;33,M5&lt;33),0,MIN(5,ROUND((IF(C5&gt;=80,5,IF(C5&gt;=70,4,IF(C5&gt;=60,3.5,IF(C5&gt;=50,3,IF(C5&gt;=40,2,IF(C5&gt;=33,1,0))))))+IF(D5/200*100&gt;=80,5,IF(D5/200*100&gt;=70,4,IF(D5/200*100&gt;=60,3.5,IF(D5/200*100&gt;=50,3,IF(D5/200*100&gt;=40,2,IF(D5/200*100&gt;=33,1,0))))))+IF(E5&gt;=80,5,IF(E5&gt;=70,4,IF(E5&gt;=60,3.5,IF(E5&gt;=50,3,IF(E5&gt;=40,2,IF(E5&gt;=33,1,0))))))+IF(F5/200*100&gt;=80,5,IF(F5/200*100&gt;=70,4,IF(F5/200*100&gt;=60,3.5,IF(F5/200*100&gt;=50,3,IF(F5/200*100&gt;=40,2,IF(F5/200*100&gt;=33,1,0))))))+IF(G5/200*100&gt;=80,5,IF(G5/200*100&gt;=70,4,IF(G5/200*100&gt;=60,3.5,IF(G5/200*100&gt;=50,3,IF(G5/200*100&gt;=40,2,IF(G5/200*100&gt;=33,1,0))))))+IF(H5&gt;=80,5,IF(H5&gt;=70,4,IF(H5&gt;=60,3.5,IF(H5&gt;=50,3,IF(H5&gt;=40,2,IF(H5&gt;=33,1,0))))))+IF(I5&gt;=80,5,IF(I5&gt;=70,4,IF(I5&gt;=60,3.5,IF(I5&gt;=50,3,IF(I5&gt;=40,2,IF(I5&gt;=33,1,0))))))+IF(J5&gt;=80,5,IF(J5&gt;=70,4,IF(J5&gt;=60,3.5,IF(J5&gt;=50,3,IF(J5&gt;=40,2,IF(J5&gt;=33,1,0)))))))/8+IF(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))&gt;=2,(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C5&lt;66,D5&lt;66,E5&lt;33,F5&lt;66,G5&lt;66,H5&lt;33,I5&lt;33,J5&lt;33,L5&lt;33,M5&lt;33),0,MIN(5,ROUND((IF(C5/200*100&gt;=80,5,IF(C5/200*100&gt;=70,4,IF(C5/200*100&gt;=60,3.5,IF(C5/200*100&gt;=50,3,IF(C5/200*100&gt;=40,2,IF(C5/200*100&gt;=33,1,0))))))+IF(D5/200*100&gt;=80,5,IF(D5/200*100&gt;=70,4,IF(D5/200*100&gt;=60,3.5,IF(D5/200*100&gt;=50,3,IF(D5/200*100&gt;=40,2,IF(D5/200*100&gt;=33,1,0))))))+IF(E5&gt;=80,5,IF(E5&gt;=70,4,IF(E5&gt;=60,3.5,IF(E5&gt;=50,3,IF(E5&gt;=40,2,IF(E5&gt;=33,1,0))))))+IF(F5/200*100&gt;=80,5,IF(F5/200*100&gt;=70,4,IF(F5/200*100&gt;=60,3.5,IF(F5/200*100&gt;=50,3,IF(F5/200*100&gt;=40,2,IF(F5/200*100&gt;=33,1,0))))))+IF(G5/200*100&gt;=80,5,IF(G5/200*100&gt;=70,4,IF(G5/200*100&gt;=60,3.5,IF(G5/200*100&gt;=50,3,IF(G5/200*100&gt;=40,2,IF(G5/200*100&gt;=33,1,0))))))+IF(H5&gt;=80,5,IF(H5&gt;=70,4,IF(H5&gt;=60,3.5,IF(H5&gt;=50,3,IF(H5&gt;=40,2,IF(H5&gt;=33,1,0))))))+IF(I5&gt;=80,5,IF(I5&gt;=70,4,IF(I5&gt;=60,3.5,IF(I5&gt;=50,3,IF(I5&gt;=40,2,IF(I5&gt;=33,1,0))))))+IF(J5&gt;=80,5,IF(J5&gt;=70,4,IF(J5&gt;=60,3.5,IF(J5&gt;=50,3,IF(J5&gt;=40,2,IF(J5&gt;=33,1,0)))))))/8+IF(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))&gt;=2,(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB5" s="4">
@@ -1316,7 +1316,7 @@
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>131</v>
@@ -1349,7 +1349,7 @@
         <v>94</v>
       </c>
       <c r="N6" s="4">
-        <f>IF(C6&gt;=80,"A+",IF(C6&gt;=70,"A",IF(C6&gt;=60,"A-",IF(C6&gt;=50,"B",IF(C6&gt;=40,"C",IF(C6&gt;=33,"D","F"))))))</f>
+        <f>IF(C6/200*100&gt;=80,"A+",IF(C6/200*100&gt;=70,"A",IF(C6/200*100&gt;=60,"A-",IF(C6/200*100&gt;=50,"B",IF(C6/200*100&gt;=40,"C",IF(C6/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O6" s="4">
@@ -1401,7 +1401,7 @@
         <v/>
       </c>
       <c r="AA6" s="6">
-        <f>IF(OR(C6&lt;33,D6&lt;66,E6&lt;33,F6&lt;66,G6&lt;66,H6&lt;33,I6&lt;33,J6&lt;33,L6&lt;33,M6&lt;33),0,MIN(5,ROUND((IF(C6&gt;=80,5,IF(C6&gt;=70,4,IF(C6&gt;=60,3.5,IF(C6&gt;=50,3,IF(C6&gt;=40,2,IF(C6&gt;=33,1,0))))))+IF(D6/200*100&gt;=80,5,IF(D6/200*100&gt;=70,4,IF(D6/200*100&gt;=60,3.5,IF(D6/200*100&gt;=50,3,IF(D6/200*100&gt;=40,2,IF(D6/200*100&gt;=33,1,0))))))+IF(E6&gt;=80,5,IF(E6&gt;=70,4,IF(E6&gt;=60,3.5,IF(E6&gt;=50,3,IF(E6&gt;=40,2,IF(E6&gt;=33,1,0))))))+IF(F6/200*100&gt;=80,5,IF(F6/200*100&gt;=70,4,IF(F6/200*100&gt;=60,3.5,IF(F6/200*100&gt;=50,3,IF(F6/200*100&gt;=40,2,IF(F6/200*100&gt;=33,1,0))))))+IF(G6/200*100&gt;=80,5,IF(G6/200*100&gt;=70,4,IF(G6/200*100&gt;=60,3.5,IF(G6/200*100&gt;=50,3,IF(G6/200*100&gt;=40,2,IF(G6/200*100&gt;=33,1,0))))))+IF(H6&gt;=80,5,IF(H6&gt;=70,4,IF(H6&gt;=60,3.5,IF(H6&gt;=50,3,IF(H6&gt;=40,2,IF(H6&gt;=33,1,0))))))+IF(I6&gt;=80,5,IF(I6&gt;=70,4,IF(I6&gt;=60,3.5,IF(I6&gt;=50,3,IF(I6&gt;=40,2,IF(I6&gt;=33,1,0))))))+IF(J6&gt;=80,5,IF(J6&gt;=70,4,IF(J6&gt;=60,3.5,IF(J6&gt;=50,3,IF(J6&gt;=40,2,IF(J6&gt;=33,1,0)))))))/8+IF(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))&gt;=2,(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C6&lt;66,D6&lt;66,E6&lt;33,F6&lt;66,G6&lt;66,H6&lt;33,I6&lt;33,J6&lt;33,L6&lt;33,M6&lt;33),0,MIN(5,ROUND((IF(C6/200*100&gt;=80,5,IF(C6/200*100&gt;=70,4,IF(C6/200*100&gt;=60,3.5,IF(C6/200*100&gt;=50,3,IF(C6/200*100&gt;=40,2,IF(C6/200*100&gt;=33,1,0))))))+IF(D6/200*100&gt;=80,5,IF(D6/200*100&gt;=70,4,IF(D6/200*100&gt;=60,3.5,IF(D6/200*100&gt;=50,3,IF(D6/200*100&gt;=40,2,IF(D6/200*100&gt;=33,1,0))))))+IF(E6&gt;=80,5,IF(E6&gt;=70,4,IF(E6&gt;=60,3.5,IF(E6&gt;=50,3,IF(E6&gt;=40,2,IF(E6&gt;=33,1,0))))))+IF(F6/200*100&gt;=80,5,IF(F6/200*100&gt;=70,4,IF(F6/200*100&gt;=60,3.5,IF(F6/200*100&gt;=50,3,IF(F6/200*100&gt;=40,2,IF(F6/200*100&gt;=33,1,0))))))+IF(G6/200*100&gt;=80,5,IF(G6/200*100&gt;=70,4,IF(G6/200*100&gt;=60,3.5,IF(G6/200*100&gt;=50,3,IF(G6/200*100&gt;=40,2,IF(G6/200*100&gt;=33,1,0))))))+IF(H6&gt;=80,5,IF(H6&gt;=70,4,IF(H6&gt;=60,3.5,IF(H6&gt;=50,3,IF(H6&gt;=40,2,IF(H6&gt;=33,1,0))))))+IF(I6&gt;=80,5,IF(I6&gt;=70,4,IF(I6&gt;=60,3.5,IF(I6&gt;=50,3,IF(I6&gt;=40,2,IF(I6&gt;=33,1,0))))))+IF(J6&gt;=80,5,IF(J6&gt;=70,4,IF(J6&gt;=60,3.5,IF(J6&gt;=50,3,IF(J6&gt;=40,2,IF(J6&gt;=33,1,0)))))))/8+IF(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))&gt;=2,(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB6" s="4">
@@ -1419,7 +1419,7 @@
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>165</v>
@@ -1452,7 +1452,7 @@
         <v>88</v>
       </c>
       <c r="N7" s="4">
-        <f>IF(C7&gt;=80,"A+",IF(C7&gt;=70,"A",IF(C7&gt;=60,"A-",IF(C7&gt;=50,"B",IF(C7&gt;=40,"C",IF(C7&gt;=33,"D","F"))))))</f>
+        <f>IF(C7/200*100&gt;=80,"A+",IF(C7/200*100&gt;=70,"A",IF(C7/200*100&gt;=60,"A-",IF(C7/200*100&gt;=50,"B",IF(C7/200*100&gt;=40,"C",IF(C7/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O7" s="4">
@@ -1504,7 +1504,7 @@
         <v/>
       </c>
       <c r="AA7" s="6">
-        <f>IF(OR(C7&lt;33,D7&lt;66,E7&lt;33,F7&lt;66,G7&lt;66,H7&lt;33,I7&lt;33,J7&lt;33,L7&lt;33,M7&lt;33),0,MIN(5,ROUND((IF(C7&gt;=80,5,IF(C7&gt;=70,4,IF(C7&gt;=60,3.5,IF(C7&gt;=50,3,IF(C7&gt;=40,2,IF(C7&gt;=33,1,0))))))+IF(D7/200*100&gt;=80,5,IF(D7/200*100&gt;=70,4,IF(D7/200*100&gt;=60,3.5,IF(D7/200*100&gt;=50,3,IF(D7/200*100&gt;=40,2,IF(D7/200*100&gt;=33,1,0))))))+IF(E7&gt;=80,5,IF(E7&gt;=70,4,IF(E7&gt;=60,3.5,IF(E7&gt;=50,3,IF(E7&gt;=40,2,IF(E7&gt;=33,1,0))))))+IF(F7/200*100&gt;=80,5,IF(F7/200*100&gt;=70,4,IF(F7/200*100&gt;=60,3.5,IF(F7/200*100&gt;=50,3,IF(F7/200*100&gt;=40,2,IF(F7/200*100&gt;=33,1,0))))))+IF(G7/200*100&gt;=80,5,IF(G7/200*100&gt;=70,4,IF(G7/200*100&gt;=60,3.5,IF(G7/200*100&gt;=50,3,IF(G7/200*100&gt;=40,2,IF(G7/200*100&gt;=33,1,0))))))+IF(H7&gt;=80,5,IF(H7&gt;=70,4,IF(H7&gt;=60,3.5,IF(H7&gt;=50,3,IF(H7&gt;=40,2,IF(H7&gt;=33,1,0))))))+IF(I7&gt;=80,5,IF(I7&gt;=70,4,IF(I7&gt;=60,3.5,IF(I7&gt;=50,3,IF(I7&gt;=40,2,IF(I7&gt;=33,1,0))))))+IF(J7&gt;=80,5,IF(J7&gt;=70,4,IF(J7&gt;=60,3.5,IF(J7&gt;=50,3,IF(J7&gt;=40,2,IF(J7&gt;=33,1,0)))))))/8+IF(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))&gt;=2,(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C7&lt;66,D7&lt;66,E7&lt;33,F7&lt;66,G7&lt;66,H7&lt;33,I7&lt;33,J7&lt;33,L7&lt;33,M7&lt;33),0,MIN(5,ROUND((IF(C7/200*100&gt;=80,5,IF(C7/200*100&gt;=70,4,IF(C7/200*100&gt;=60,3.5,IF(C7/200*100&gt;=50,3,IF(C7/200*100&gt;=40,2,IF(C7/200*100&gt;=33,1,0))))))+IF(D7/200*100&gt;=80,5,IF(D7/200*100&gt;=70,4,IF(D7/200*100&gt;=60,3.5,IF(D7/200*100&gt;=50,3,IF(D7/200*100&gt;=40,2,IF(D7/200*100&gt;=33,1,0))))))+IF(E7&gt;=80,5,IF(E7&gt;=70,4,IF(E7&gt;=60,3.5,IF(E7&gt;=50,3,IF(E7&gt;=40,2,IF(E7&gt;=33,1,0))))))+IF(F7/200*100&gt;=80,5,IF(F7/200*100&gt;=70,4,IF(F7/200*100&gt;=60,3.5,IF(F7/200*100&gt;=50,3,IF(F7/200*100&gt;=40,2,IF(F7/200*100&gt;=33,1,0))))))+IF(G7/200*100&gt;=80,5,IF(G7/200*100&gt;=70,4,IF(G7/200*100&gt;=60,3.5,IF(G7/200*100&gt;=50,3,IF(G7/200*100&gt;=40,2,IF(G7/200*100&gt;=33,1,0))))))+IF(H7&gt;=80,5,IF(H7&gt;=70,4,IF(H7&gt;=60,3.5,IF(H7&gt;=50,3,IF(H7&gt;=40,2,IF(H7&gt;=33,1,0))))))+IF(I7&gt;=80,5,IF(I7&gt;=70,4,IF(I7&gt;=60,3.5,IF(I7&gt;=50,3,IF(I7&gt;=40,2,IF(I7&gt;=33,1,0))))))+IF(J7&gt;=80,5,IF(J7&gt;=70,4,IF(J7&gt;=60,3.5,IF(J7&gt;=50,3,IF(J7&gt;=40,2,IF(J7&gt;=33,1,0)))))))/8+IF(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))&gt;=2,(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB7" s="4">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="C8" s="3" t="n">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>142</v>
@@ -1555,7 +1555,7 @@
         <v>81</v>
       </c>
       <c r="N8" s="4">
-        <f>IF(C8&gt;=80,"A+",IF(C8&gt;=70,"A",IF(C8&gt;=60,"A-",IF(C8&gt;=50,"B",IF(C8&gt;=40,"C",IF(C8&gt;=33,"D","F"))))))</f>
+        <f>IF(C8/200*100&gt;=80,"A+",IF(C8/200*100&gt;=70,"A",IF(C8/200*100&gt;=60,"A-",IF(C8/200*100&gt;=50,"B",IF(C8/200*100&gt;=40,"C",IF(C8/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O8" s="4">
@@ -1607,7 +1607,7 @@
         <v/>
       </c>
       <c r="AA8" s="6">
-        <f>IF(OR(C8&lt;33,D8&lt;66,E8&lt;33,F8&lt;66,G8&lt;66,H8&lt;33,I8&lt;33,J8&lt;33,L8&lt;33,M8&lt;33),0,MIN(5,ROUND((IF(C8&gt;=80,5,IF(C8&gt;=70,4,IF(C8&gt;=60,3.5,IF(C8&gt;=50,3,IF(C8&gt;=40,2,IF(C8&gt;=33,1,0))))))+IF(D8/200*100&gt;=80,5,IF(D8/200*100&gt;=70,4,IF(D8/200*100&gt;=60,3.5,IF(D8/200*100&gt;=50,3,IF(D8/200*100&gt;=40,2,IF(D8/200*100&gt;=33,1,0))))))+IF(E8&gt;=80,5,IF(E8&gt;=70,4,IF(E8&gt;=60,3.5,IF(E8&gt;=50,3,IF(E8&gt;=40,2,IF(E8&gt;=33,1,0))))))+IF(F8/200*100&gt;=80,5,IF(F8/200*100&gt;=70,4,IF(F8/200*100&gt;=60,3.5,IF(F8/200*100&gt;=50,3,IF(F8/200*100&gt;=40,2,IF(F8/200*100&gt;=33,1,0))))))+IF(G8/200*100&gt;=80,5,IF(G8/200*100&gt;=70,4,IF(G8/200*100&gt;=60,3.5,IF(G8/200*100&gt;=50,3,IF(G8/200*100&gt;=40,2,IF(G8/200*100&gt;=33,1,0))))))+IF(H8&gt;=80,5,IF(H8&gt;=70,4,IF(H8&gt;=60,3.5,IF(H8&gt;=50,3,IF(H8&gt;=40,2,IF(H8&gt;=33,1,0))))))+IF(I8&gt;=80,5,IF(I8&gt;=70,4,IF(I8&gt;=60,3.5,IF(I8&gt;=50,3,IF(I8&gt;=40,2,IF(I8&gt;=33,1,0))))))+IF(J8&gt;=80,5,IF(J8&gt;=70,4,IF(J8&gt;=60,3.5,IF(J8&gt;=50,3,IF(J8&gt;=40,2,IF(J8&gt;=33,1,0)))))))/8+IF(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))&gt;=2,(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C8&lt;66,D8&lt;66,E8&lt;33,F8&lt;66,G8&lt;66,H8&lt;33,I8&lt;33,J8&lt;33,L8&lt;33,M8&lt;33),0,MIN(5,ROUND((IF(C8/200*100&gt;=80,5,IF(C8/200*100&gt;=70,4,IF(C8/200*100&gt;=60,3.5,IF(C8/200*100&gt;=50,3,IF(C8/200*100&gt;=40,2,IF(C8/200*100&gt;=33,1,0))))))+IF(D8/200*100&gt;=80,5,IF(D8/200*100&gt;=70,4,IF(D8/200*100&gt;=60,3.5,IF(D8/200*100&gt;=50,3,IF(D8/200*100&gt;=40,2,IF(D8/200*100&gt;=33,1,0))))))+IF(E8&gt;=80,5,IF(E8&gt;=70,4,IF(E8&gt;=60,3.5,IF(E8&gt;=50,3,IF(E8&gt;=40,2,IF(E8&gt;=33,1,0))))))+IF(F8/200*100&gt;=80,5,IF(F8/200*100&gt;=70,4,IF(F8/200*100&gt;=60,3.5,IF(F8/200*100&gt;=50,3,IF(F8/200*100&gt;=40,2,IF(F8/200*100&gt;=33,1,0))))))+IF(G8/200*100&gt;=80,5,IF(G8/200*100&gt;=70,4,IF(G8/200*100&gt;=60,3.5,IF(G8/200*100&gt;=50,3,IF(G8/200*100&gt;=40,2,IF(G8/200*100&gt;=33,1,0))))))+IF(H8&gt;=80,5,IF(H8&gt;=70,4,IF(H8&gt;=60,3.5,IF(H8&gt;=50,3,IF(H8&gt;=40,2,IF(H8&gt;=33,1,0))))))+IF(I8&gt;=80,5,IF(I8&gt;=70,4,IF(I8&gt;=60,3.5,IF(I8&gt;=50,3,IF(I8&gt;=40,2,IF(I8&gt;=33,1,0))))))+IF(J8&gt;=80,5,IF(J8&gt;=70,4,IF(J8&gt;=60,3.5,IF(J8&gt;=50,3,IF(J8&gt;=40,2,IF(J8&gt;=33,1,0)))))))/8+IF(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))&gt;=2,(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB8" s="4">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>175</v>
@@ -1658,7 +1658,7 @@
         <v>92</v>
       </c>
       <c r="N9" s="4">
-        <f>IF(C9&gt;=80,"A+",IF(C9&gt;=70,"A",IF(C9&gt;=60,"A-",IF(C9&gt;=50,"B",IF(C9&gt;=40,"C",IF(C9&gt;=33,"D","F"))))))</f>
+        <f>IF(C9/200*100&gt;=80,"A+",IF(C9/200*100&gt;=70,"A",IF(C9/200*100&gt;=60,"A-",IF(C9/200*100&gt;=50,"B",IF(C9/200*100&gt;=40,"C",IF(C9/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O9" s="4">
@@ -1710,7 +1710,7 @@
         <v/>
       </c>
       <c r="AA9" s="6">
-        <f>IF(OR(C9&lt;33,D9&lt;66,E9&lt;33,F9&lt;66,G9&lt;66,H9&lt;33,I9&lt;33,J9&lt;33,L9&lt;33,M9&lt;33),0,MIN(5,ROUND((IF(C9&gt;=80,5,IF(C9&gt;=70,4,IF(C9&gt;=60,3.5,IF(C9&gt;=50,3,IF(C9&gt;=40,2,IF(C9&gt;=33,1,0))))))+IF(D9/200*100&gt;=80,5,IF(D9/200*100&gt;=70,4,IF(D9/200*100&gt;=60,3.5,IF(D9/200*100&gt;=50,3,IF(D9/200*100&gt;=40,2,IF(D9/200*100&gt;=33,1,0))))))+IF(E9&gt;=80,5,IF(E9&gt;=70,4,IF(E9&gt;=60,3.5,IF(E9&gt;=50,3,IF(E9&gt;=40,2,IF(E9&gt;=33,1,0))))))+IF(F9/200*100&gt;=80,5,IF(F9/200*100&gt;=70,4,IF(F9/200*100&gt;=60,3.5,IF(F9/200*100&gt;=50,3,IF(F9/200*100&gt;=40,2,IF(F9/200*100&gt;=33,1,0))))))+IF(G9/200*100&gt;=80,5,IF(G9/200*100&gt;=70,4,IF(G9/200*100&gt;=60,3.5,IF(G9/200*100&gt;=50,3,IF(G9/200*100&gt;=40,2,IF(G9/200*100&gt;=33,1,0))))))+IF(H9&gt;=80,5,IF(H9&gt;=70,4,IF(H9&gt;=60,3.5,IF(H9&gt;=50,3,IF(H9&gt;=40,2,IF(H9&gt;=33,1,0))))))+IF(I9&gt;=80,5,IF(I9&gt;=70,4,IF(I9&gt;=60,3.5,IF(I9&gt;=50,3,IF(I9&gt;=40,2,IF(I9&gt;=33,1,0))))))+IF(J9&gt;=80,5,IF(J9&gt;=70,4,IF(J9&gt;=60,3.5,IF(J9&gt;=50,3,IF(J9&gt;=40,2,IF(J9&gt;=33,1,0)))))))/8+IF(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))&gt;=2,(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C9&lt;66,D9&lt;66,E9&lt;33,F9&lt;66,G9&lt;66,H9&lt;33,I9&lt;33,J9&lt;33,L9&lt;33,M9&lt;33),0,MIN(5,ROUND((IF(C9/200*100&gt;=80,5,IF(C9/200*100&gt;=70,4,IF(C9/200*100&gt;=60,3.5,IF(C9/200*100&gt;=50,3,IF(C9/200*100&gt;=40,2,IF(C9/200*100&gt;=33,1,0))))))+IF(D9/200*100&gt;=80,5,IF(D9/200*100&gt;=70,4,IF(D9/200*100&gt;=60,3.5,IF(D9/200*100&gt;=50,3,IF(D9/200*100&gt;=40,2,IF(D9/200*100&gt;=33,1,0))))))+IF(E9&gt;=80,5,IF(E9&gt;=70,4,IF(E9&gt;=60,3.5,IF(E9&gt;=50,3,IF(E9&gt;=40,2,IF(E9&gt;=33,1,0))))))+IF(F9/200*100&gt;=80,5,IF(F9/200*100&gt;=70,4,IF(F9/200*100&gt;=60,3.5,IF(F9/200*100&gt;=50,3,IF(F9/200*100&gt;=40,2,IF(F9/200*100&gt;=33,1,0))))))+IF(G9/200*100&gt;=80,5,IF(G9/200*100&gt;=70,4,IF(G9/200*100&gt;=60,3.5,IF(G9/200*100&gt;=50,3,IF(G9/200*100&gt;=40,2,IF(G9/200*100&gt;=33,1,0))))))+IF(H9&gt;=80,5,IF(H9&gt;=70,4,IF(H9&gt;=60,3.5,IF(H9&gt;=50,3,IF(H9&gt;=40,2,IF(H9&gt;=33,1,0))))))+IF(I9&gt;=80,5,IF(I9&gt;=70,4,IF(I9&gt;=60,3.5,IF(I9&gt;=50,3,IF(I9&gt;=40,2,IF(I9&gt;=33,1,0))))))+IF(J9&gt;=80,5,IF(J9&gt;=70,4,IF(J9&gt;=60,3.5,IF(J9&gt;=50,3,IF(J9&gt;=40,2,IF(J9&gt;=33,1,0)))))))/8+IF(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))&gt;=2,(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB9" s="4">
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>171</v>
@@ -1761,7 +1761,7 @@
         <v>81</v>
       </c>
       <c r="N10" s="4">
-        <f>IF(C10&gt;=80,"A+",IF(C10&gt;=70,"A",IF(C10&gt;=60,"A-",IF(C10&gt;=50,"B",IF(C10&gt;=40,"C",IF(C10&gt;=33,"D","F"))))))</f>
+        <f>IF(C10/200*100&gt;=80,"A+",IF(C10/200*100&gt;=70,"A",IF(C10/200*100&gt;=60,"A-",IF(C10/200*100&gt;=50,"B",IF(C10/200*100&gt;=40,"C",IF(C10/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O10" s="4">
@@ -1813,7 +1813,7 @@
         <v/>
       </c>
       <c r="AA10" s="6">
-        <f>IF(OR(C10&lt;33,D10&lt;66,E10&lt;33,F10&lt;66,G10&lt;66,H10&lt;33,I10&lt;33,J10&lt;33,L10&lt;33,M10&lt;33),0,MIN(5,ROUND((IF(C10&gt;=80,5,IF(C10&gt;=70,4,IF(C10&gt;=60,3.5,IF(C10&gt;=50,3,IF(C10&gt;=40,2,IF(C10&gt;=33,1,0))))))+IF(D10/200*100&gt;=80,5,IF(D10/200*100&gt;=70,4,IF(D10/200*100&gt;=60,3.5,IF(D10/200*100&gt;=50,3,IF(D10/200*100&gt;=40,2,IF(D10/200*100&gt;=33,1,0))))))+IF(E10&gt;=80,5,IF(E10&gt;=70,4,IF(E10&gt;=60,3.5,IF(E10&gt;=50,3,IF(E10&gt;=40,2,IF(E10&gt;=33,1,0))))))+IF(F10/200*100&gt;=80,5,IF(F10/200*100&gt;=70,4,IF(F10/200*100&gt;=60,3.5,IF(F10/200*100&gt;=50,3,IF(F10/200*100&gt;=40,2,IF(F10/200*100&gt;=33,1,0))))))+IF(G10/200*100&gt;=80,5,IF(G10/200*100&gt;=70,4,IF(G10/200*100&gt;=60,3.5,IF(G10/200*100&gt;=50,3,IF(G10/200*100&gt;=40,2,IF(G10/200*100&gt;=33,1,0))))))+IF(H10&gt;=80,5,IF(H10&gt;=70,4,IF(H10&gt;=60,3.5,IF(H10&gt;=50,3,IF(H10&gt;=40,2,IF(H10&gt;=33,1,0))))))+IF(I10&gt;=80,5,IF(I10&gt;=70,4,IF(I10&gt;=60,3.5,IF(I10&gt;=50,3,IF(I10&gt;=40,2,IF(I10&gt;=33,1,0))))))+IF(J10&gt;=80,5,IF(J10&gt;=70,4,IF(J10&gt;=60,3.5,IF(J10&gt;=50,3,IF(J10&gt;=40,2,IF(J10&gt;=33,1,0)))))))/8+IF(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))&gt;=2,(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C10&lt;66,D10&lt;66,E10&lt;33,F10&lt;66,G10&lt;66,H10&lt;33,I10&lt;33,J10&lt;33,L10&lt;33,M10&lt;33),0,MIN(5,ROUND((IF(C10/200*100&gt;=80,5,IF(C10/200*100&gt;=70,4,IF(C10/200*100&gt;=60,3.5,IF(C10/200*100&gt;=50,3,IF(C10/200*100&gt;=40,2,IF(C10/200*100&gt;=33,1,0))))))+IF(D10/200*100&gt;=80,5,IF(D10/200*100&gt;=70,4,IF(D10/200*100&gt;=60,3.5,IF(D10/200*100&gt;=50,3,IF(D10/200*100&gt;=40,2,IF(D10/200*100&gt;=33,1,0))))))+IF(E10&gt;=80,5,IF(E10&gt;=70,4,IF(E10&gt;=60,3.5,IF(E10&gt;=50,3,IF(E10&gt;=40,2,IF(E10&gt;=33,1,0))))))+IF(F10/200*100&gt;=80,5,IF(F10/200*100&gt;=70,4,IF(F10/200*100&gt;=60,3.5,IF(F10/200*100&gt;=50,3,IF(F10/200*100&gt;=40,2,IF(F10/200*100&gt;=33,1,0))))))+IF(G10/200*100&gt;=80,5,IF(G10/200*100&gt;=70,4,IF(G10/200*100&gt;=60,3.5,IF(G10/200*100&gt;=50,3,IF(G10/200*100&gt;=40,2,IF(G10/200*100&gt;=33,1,0))))))+IF(H10&gt;=80,5,IF(H10&gt;=70,4,IF(H10&gt;=60,3.5,IF(H10&gt;=50,3,IF(H10&gt;=40,2,IF(H10&gt;=33,1,0))))))+IF(I10&gt;=80,5,IF(I10&gt;=70,4,IF(I10&gt;=60,3.5,IF(I10&gt;=50,3,IF(I10&gt;=40,2,IF(I10&gt;=33,1,0))))))+IF(J10&gt;=80,5,IF(J10&gt;=70,4,IF(J10&gt;=60,3.5,IF(J10&gt;=50,3,IF(J10&gt;=40,2,IF(J10&gt;=33,1,0)))))))/8+IF(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))&gt;=2,(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB10" s="4">
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>174</v>
@@ -1864,7 +1864,7 @@
         <v>84</v>
       </c>
       <c r="N11" s="4">
-        <f>IF(C11&gt;=80,"A+",IF(C11&gt;=70,"A",IF(C11&gt;=60,"A-",IF(C11&gt;=50,"B",IF(C11&gt;=40,"C",IF(C11&gt;=33,"D","F"))))))</f>
+        <f>IF(C11/200*100&gt;=80,"A+",IF(C11/200*100&gt;=70,"A",IF(C11/200*100&gt;=60,"A-",IF(C11/200*100&gt;=50,"B",IF(C11/200*100&gt;=40,"C",IF(C11/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O11" s="4">
@@ -1916,7 +1916,7 @@
         <v/>
       </c>
       <c r="AA11" s="6">
-        <f>IF(OR(C11&lt;33,D11&lt;66,E11&lt;33,F11&lt;66,G11&lt;66,H11&lt;33,I11&lt;33,J11&lt;33,L11&lt;33,M11&lt;33),0,MIN(5,ROUND((IF(C11&gt;=80,5,IF(C11&gt;=70,4,IF(C11&gt;=60,3.5,IF(C11&gt;=50,3,IF(C11&gt;=40,2,IF(C11&gt;=33,1,0))))))+IF(D11/200*100&gt;=80,5,IF(D11/200*100&gt;=70,4,IF(D11/200*100&gt;=60,3.5,IF(D11/200*100&gt;=50,3,IF(D11/200*100&gt;=40,2,IF(D11/200*100&gt;=33,1,0))))))+IF(E11&gt;=80,5,IF(E11&gt;=70,4,IF(E11&gt;=60,3.5,IF(E11&gt;=50,3,IF(E11&gt;=40,2,IF(E11&gt;=33,1,0))))))+IF(F11/200*100&gt;=80,5,IF(F11/200*100&gt;=70,4,IF(F11/200*100&gt;=60,3.5,IF(F11/200*100&gt;=50,3,IF(F11/200*100&gt;=40,2,IF(F11/200*100&gt;=33,1,0))))))+IF(G11/200*100&gt;=80,5,IF(G11/200*100&gt;=70,4,IF(G11/200*100&gt;=60,3.5,IF(G11/200*100&gt;=50,3,IF(G11/200*100&gt;=40,2,IF(G11/200*100&gt;=33,1,0))))))+IF(H11&gt;=80,5,IF(H11&gt;=70,4,IF(H11&gt;=60,3.5,IF(H11&gt;=50,3,IF(H11&gt;=40,2,IF(H11&gt;=33,1,0))))))+IF(I11&gt;=80,5,IF(I11&gt;=70,4,IF(I11&gt;=60,3.5,IF(I11&gt;=50,3,IF(I11&gt;=40,2,IF(I11&gt;=33,1,0))))))+IF(J11&gt;=80,5,IF(J11&gt;=70,4,IF(J11&gt;=60,3.5,IF(J11&gt;=50,3,IF(J11&gt;=40,2,IF(J11&gt;=33,1,0)))))))/8+IF(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))&gt;=2,(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C11&lt;66,D11&lt;66,E11&lt;33,F11&lt;66,G11&lt;66,H11&lt;33,I11&lt;33,J11&lt;33,L11&lt;33,M11&lt;33),0,MIN(5,ROUND((IF(C11/200*100&gt;=80,5,IF(C11/200*100&gt;=70,4,IF(C11/200*100&gt;=60,3.5,IF(C11/200*100&gt;=50,3,IF(C11/200*100&gt;=40,2,IF(C11/200*100&gt;=33,1,0))))))+IF(D11/200*100&gt;=80,5,IF(D11/200*100&gt;=70,4,IF(D11/200*100&gt;=60,3.5,IF(D11/200*100&gt;=50,3,IF(D11/200*100&gt;=40,2,IF(D11/200*100&gt;=33,1,0))))))+IF(E11&gt;=80,5,IF(E11&gt;=70,4,IF(E11&gt;=60,3.5,IF(E11&gt;=50,3,IF(E11&gt;=40,2,IF(E11&gt;=33,1,0))))))+IF(F11/200*100&gt;=80,5,IF(F11/200*100&gt;=70,4,IF(F11/200*100&gt;=60,3.5,IF(F11/200*100&gt;=50,3,IF(F11/200*100&gt;=40,2,IF(F11/200*100&gt;=33,1,0))))))+IF(G11/200*100&gt;=80,5,IF(G11/200*100&gt;=70,4,IF(G11/200*100&gt;=60,3.5,IF(G11/200*100&gt;=50,3,IF(G11/200*100&gt;=40,2,IF(G11/200*100&gt;=33,1,0))))))+IF(H11&gt;=80,5,IF(H11&gt;=70,4,IF(H11&gt;=60,3.5,IF(H11&gt;=50,3,IF(H11&gt;=40,2,IF(H11&gt;=33,1,0))))))+IF(I11&gt;=80,5,IF(I11&gt;=70,4,IF(I11&gt;=60,3.5,IF(I11&gt;=50,3,IF(I11&gt;=40,2,IF(I11&gt;=33,1,0))))))+IF(J11&gt;=80,5,IF(J11&gt;=70,4,IF(J11&gt;=60,3.5,IF(J11&gt;=50,3,IF(J11&gt;=40,2,IF(J11&gt;=33,1,0)))))))/8+IF(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))&gt;=2,(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB11" s="4">
@@ -1934,7 +1934,7 @@
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>164</v>
@@ -1967,7 +1967,7 @@
         <v>87</v>
       </c>
       <c r="N12" s="4">
-        <f>IF(C12&gt;=80,"A+",IF(C12&gt;=70,"A",IF(C12&gt;=60,"A-",IF(C12&gt;=50,"B",IF(C12&gt;=40,"C",IF(C12&gt;=33,"D","F"))))))</f>
+        <f>IF(C12/200*100&gt;=80,"A+",IF(C12/200*100&gt;=70,"A",IF(C12/200*100&gt;=60,"A-",IF(C12/200*100&gt;=50,"B",IF(C12/200*100&gt;=40,"C",IF(C12/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O12" s="4">
@@ -2019,7 +2019,7 @@
         <v/>
       </c>
       <c r="AA12" s="6">
-        <f>IF(OR(C12&lt;33,D12&lt;66,E12&lt;33,F12&lt;66,G12&lt;66,H12&lt;33,I12&lt;33,J12&lt;33,L12&lt;33,M12&lt;33),0,MIN(5,ROUND((IF(C12&gt;=80,5,IF(C12&gt;=70,4,IF(C12&gt;=60,3.5,IF(C12&gt;=50,3,IF(C12&gt;=40,2,IF(C12&gt;=33,1,0))))))+IF(D12/200*100&gt;=80,5,IF(D12/200*100&gt;=70,4,IF(D12/200*100&gt;=60,3.5,IF(D12/200*100&gt;=50,3,IF(D12/200*100&gt;=40,2,IF(D12/200*100&gt;=33,1,0))))))+IF(E12&gt;=80,5,IF(E12&gt;=70,4,IF(E12&gt;=60,3.5,IF(E12&gt;=50,3,IF(E12&gt;=40,2,IF(E12&gt;=33,1,0))))))+IF(F12/200*100&gt;=80,5,IF(F12/200*100&gt;=70,4,IF(F12/200*100&gt;=60,3.5,IF(F12/200*100&gt;=50,3,IF(F12/200*100&gt;=40,2,IF(F12/200*100&gt;=33,1,0))))))+IF(G12/200*100&gt;=80,5,IF(G12/200*100&gt;=70,4,IF(G12/200*100&gt;=60,3.5,IF(G12/200*100&gt;=50,3,IF(G12/200*100&gt;=40,2,IF(G12/200*100&gt;=33,1,0))))))+IF(H12&gt;=80,5,IF(H12&gt;=70,4,IF(H12&gt;=60,3.5,IF(H12&gt;=50,3,IF(H12&gt;=40,2,IF(H12&gt;=33,1,0))))))+IF(I12&gt;=80,5,IF(I12&gt;=70,4,IF(I12&gt;=60,3.5,IF(I12&gt;=50,3,IF(I12&gt;=40,2,IF(I12&gt;=33,1,0))))))+IF(J12&gt;=80,5,IF(J12&gt;=70,4,IF(J12&gt;=60,3.5,IF(J12&gt;=50,3,IF(J12&gt;=40,2,IF(J12&gt;=33,1,0)))))))/8+IF(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))&gt;=2,(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C12&lt;66,D12&lt;66,E12&lt;33,F12&lt;66,G12&lt;66,H12&lt;33,I12&lt;33,J12&lt;33,L12&lt;33,M12&lt;33),0,MIN(5,ROUND((IF(C12/200*100&gt;=80,5,IF(C12/200*100&gt;=70,4,IF(C12/200*100&gt;=60,3.5,IF(C12/200*100&gt;=50,3,IF(C12/200*100&gt;=40,2,IF(C12/200*100&gt;=33,1,0))))))+IF(D12/200*100&gt;=80,5,IF(D12/200*100&gt;=70,4,IF(D12/200*100&gt;=60,3.5,IF(D12/200*100&gt;=50,3,IF(D12/200*100&gt;=40,2,IF(D12/200*100&gt;=33,1,0))))))+IF(E12&gt;=80,5,IF(E12&gt;=70,4,IF(E12&gt;=60,3.5,IF(E12&gt;=50,3,IF(E12&gt;=40,2,IF(E12&gt;=33,1,0))))))+IF(F12/200*100&gt;=80,5,IF(F12/200*100&gt;=70,4,IF(F12/200*100&gt;=60,3.5,IF(F12/200*100&gt;=50,3,IF(F12/200*100&gt;=40,2,IF(F12/200*100&gt;=33,1,0))))))+IF(G12/200*100&gt;=80,5,IF(G12/200*100&gt;=70,4,IF(G12/200*100&gt;=60,3.5,IF(G12/200*100&gt;=50,3,IF(G12/200*100&gt;=40,2,IF(G12/200*100&gt;=33,1,0))))))+IF(H12&gt;=80,5,IF(H12&gt;=70,4,IF(H12&gt;=60,3.5,IF(H12&gt;=50,3,IF(H12&gt;=40,2,IF(H12&gt;=33,1,0))))))+IF(I12&gt;=80,5,IF(I12&gt;=70,4,IF(I12&gt;=60,3.5,IF(I12&gt;=50,3,IF(I12&gt;=40,2,IF(I12&gt;=33,1,0))))))+IF(J12&gt;=80,5,IF(J12&gt;=70,4,IF(J12&gt;=60,3.5,IF(J12&gt;=50,3,IF(J12&gt;=40,2,IF(J12&gt;=33,1,0)))))))/8+IF(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))&gt;=2,(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB12" s="4">
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>156</v>
@@ -2070,7 +2070,7 @@
         <v>95</v>
       </c>
       <c r="N13" s="4">
-        <f>IF(C13&gt;=80,"A+",IF(C13&gt;=70,"A",IF(C13&gt;=60,"A-",IF(C13&gt;=50,"B",IF(C13&gt;=40,"C",IF(C13&gt;=33,"D","F"))))))</f>
+        <f>IF(C13/200*100&gt;=80,"A+",IF(C13/200*100&gt;=70,"A",IF(C13/200*100&gt;=60,"A-",IF(C13/200*100&gt;=50,"B",IF(C13/200*100&gt;=40,"C",IF(C13/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O13" s="4">
@@ -2122,7 +2122,7 @@
         <v/>
       </c>
       <c r="AA13" s="6">
-        <f>IF(OR(C13&lt;33,D13&lt;66,E13&lt;33,F13&lt;66,G13&lt;66,H13&lt;33,I13&lt;33,J13&lt;33,L13&lt;33,M13&lt;33),0,MIN(5,ROUND((IF(C13&gt;=80,5,IF(C13&gt;=70,4,IF(C13&gt;=60,3.5,IF(C13&gt;=50,3,IF(C13&gt;=40,2,IF(C13&gt;=33,1,0))))))+IF(D13/200*100&gt;=80,5,IF(D13/200*100&gt;=70,4,IF(D13/200*100&gt;=60,3.5,IF(D13/200*100&gt;=50,3,IF(D13/200*100&gt;=40,2,IF(D13/200*100&gt;=33,1,0))))))+IF(E13&gt;=80,5,IF(E13&gt;=70,4,IF(E13&gt;=60,3.5,IF(E13&gt;=50,3,IF(E13&gt;=40,2,IF(E13&gt;=33,1,0))))))+IF(F13/200*100&gt;=80,5,IF(F13/200*100&gt;=70,4,IF(F13/200*100&gt;=60,3.5,IF(F13/200*100&gt;=50,3,IF(F13/200*100&gt;=40,2,IF(F13/200*100&gt;=33,1,0))))))+IF(G13/200*100&gt;=80,5,IF(G13/200*100&gt;=70,4,IF(G13/200*100&gt;=60,3.5,IF(G13/200*100&gt;=50,3,IF(G13/200*100&gt;=40,2,IF(G13/200*100&gt;=33,1,0))))))+IF(H13&gt;=80,5,IF(H13&gt;=70,4,IF(H13&gt;=60,3.5,IF(H13&gt;=50,3,IF(H13&gt;=40,2,IF(H13&gt;=33,1,0))))))+IF(I13&gt;=80,5,IF(I13&gt;=70,4,IF(I13&gt;=60,3.5,IF(I13&gt;=50,3,IF(I13&gt;=40,2,IF(I13&gt;=33,1,0))))))+IF(J13&gt;=80,5,IF(J13&gt;=70,4,IF(J13&gt;=60,3.5,IF(J13&gt;=50,3,IF(J13&gt;=40,2,IF(J13&gt;=33,1,0)))))))/8+IF(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))&gt;=2,(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C13&lt;66,D13&lt;66,E13&lt;33,F13&lt;66,G13&lt;66,H13&lt;33,I13&lt;33,J13&lt;33,L13&lt;33,M13&lt;33),0,MIN(5,ROUND((IF(C13/200*100&gt;=80,5,IF(C13/200*100&gt;=70,4,IF(C13/200*100&gt;=60,3.5,IF(C13/200*100&gt;=50,3,IF(C13/200*100&gt;=40,2,IF(C13/200*100&gt;=33,1,0))))))+IF(D13/200*100&gt;=80,5,IF(D13/200*100&gt;=70,4,IF(D13/200*100&gt;=60,3.5,IF(D13/200*100&gt;=50,3,IF(D13/200*100&gt;=40,2,IF(D13/200*100&gt;=33,1,0))))))+IF(E13&gt;=80,5,IF(E13&gt;=70,4,IF(E13&gt;=60,3.5,IF(E13&gt;=50,3,IF(E13&gt;=40,2,IF(E13&gt;=33,1,0))))))+IF(F13/200*100&gt;=80,5,IF(F13/200*100&gt;=70,4,IF(F13/200*100&gt;=60,3.5,IF(F13/200*100&gt;=50,3,IF(F13/200*100&gt;=40,2,IF(F13/200*100&gt;=33,1,0))))))+IF(G13/200*100&gt;=80,5,IF(G13/200*100&gt;=70,4,IF(G13/200*100&gt;=60,3.5,IF(G13/200*100&gt;=50,3,IF(G13/200*100&gt;=40,2,IF(G13/200*100&gt;=33,1,0))))))+IF(H13&gt;=80,5,IF(H13&gt;=70,4,IF(H13&gt;=60,3.5,IF(H13&gt;=50,3,IF(H13&gt;=40,2,IF(H13&gt;=33,1,0))))))+IF(I13&gt;=80,5,IF(I13&gt;=70,4,IF(I13&gt;=60,3.5,IF(I13&gt;=50,3,IF(I13&gt;=40,2,IF(I13&gt;=33,1,0))))))+IF(J13&gt;=80,5,IF(J13&gt;=70,4,IF(J13&gt;=60,3.5,IF(J13&gt;=50,3,IF(J13&gt;=40,2,IF(J13&gt;=33,1,0)))))))/8+IF(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))&gt;=2,(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB13" s="4">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>144</v>
@@ -2173,7 +2173,7 @@
         <v>86</v>
       </c>
       <c r="N14" s="4">
-        <f>IF(C14&gt;=80,"A+",IF(C14&gt;=70,"A",IF(C14&gt;=60,"A-",IF(C14&gt;=50,"B",IF(C14&gt;=40,"C",IF(C14&gt;=33,"D","F"))))))</f>
+        <f>IF(C14/200*100&gt;=80,"A+",IF(C14/200*100&gt;=70,"A",IF(C14/200*100&gt;=60,"A-",IF(C14/200*100&gt;=50,"B",IF(C14/200*100&gt;=40,"C",IF(C14/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O14" s="4">
@@ -2225,7 +2225,7 @@
         <v/>
       </c>
       <c r="AA14" s="6">
-        <f>IF(OR(C14&lt;33,D14&lt;66,E14&lt;33,F14&lt;66,G14&lt;66,H14&lt;33,I14&lt;33,J14&lt;33,L14&lt;33,M14&lt;33),0,MIN(5,ROUND((IF(C14&gt;=80,5,IF(C14&gt;=70,4,IF(C14&gt;=60,3.5,IF(C14&gt;=50,3,IF(C14&gt;=40,2,IF(C14&gt;=33,1,0))))))+IF(D14/200*100&gt;=80,5,IF(D14/200*100&gt;=70,4,IF(D14/200*100&gt;=60,3.5,IF(D14/200*100&gt;=50,3,IF(D14/200*100&gt;=40,2,IF(D14/200*100&gt;=33,1,0))))))+IF(E14&gt;=80,5,IF(E14&gt;=70,4,IF(E14&gt;=60,3.5,IF(E14&gt;=50,3,IF(E14&gt;=40,2,IF(E14&gt;=33,1,0))))))+IF(F14/200*100&gt;=80,5,IF(F14/200*100&gt;=70,4,IF(F14/200*100&gt;=60,3.5,IF(F14/200*100&gt;=50,3,IF(F14/200*100&gt;=40,2,IF(F14/200*100&gt;=33,1,0))))))+IF(G14/200*100&gt;=80,5,IF(G14/200*100&gt;=70,4,IF(G14/200*100&gt;=60,3.5,IF(G14/200*100&gt;=50,3,IF(G14/200*100&gt;=40,2,IF(G14/200*100&gt;=33,1,0))))))+IF(H14&gt;=80,5,IF(H14&gt;=70,4,IF(H14&gt;=60,3.5,IF(H14&gt;=50,3,IF(H14&gt;=40,2,IF(H14&gt;=33,1,0))))))+IF(I14&gt;=80,5,IF(I14&gt;=70,4,IF(I14&gt;=60,3.5,IF(I14&gt;=50,3,IF(I14&gt;=40,2,IF(I14&gt;=33,1,0))))))+IF(J14&gt;=80,5,IF(J14&gt;=70,4,IF(J14&gt;=60,3.5,IF(J14&gt;=50,3,IF(J14&gt;=40,2,IF(J14&gt;=33,1,0)))))))/8+IF(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))&gt;=2,(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C14&lt;66,D14&lt;66,E14&lt;33,F14&lt;66,G14&lt;66,H14&lt;33,I14&lt;33,J14&lt;33,L14&lt;33,M14&lt;33),0,MIN(5,ROUND((IF(C14/200*100&gt;=80,5,IF(C14/200*100&gt;=70,4,IF(C14/200*100&gt;=60,3.5,IF(C14/200*100&gt;=50,3,IF(C14/200*100&gt;=40,2,IF(C14/200*100&gt;=33,1,0))))))+IF(D14/200*100&gt;=80,5,IF(D14/200*100&gt;=70,4,IF(D14/200*100&gt;=60,3.5,IF(D14/200*100&gt;=50,3,IF(D14/200*100&gt;=40,2,IF(D14/200*100&gt;=33,1,0))))))+IF(E14&gt;=80,5,IF(E14&gt;=70,4,IF(E14&gt;=60,3.5,IF(E14&gt;=50,3,IF(E14&gt;=40,2,IF(E14&gt;=33,1,0))))))+IF(F14/200*100&gt;=80,5,IF(F14/200*100&gt;=70,4,IF(F14/200*100&gt;=60,3.5,IF(F14/200*100&gt;=50,3,IF(F14/200*100&gt;=40,2,IF(F14/200*100&gt;=33,1,0))))))+IF(G14/200*100&gt;=80,5,IF(G14/200*100&gt;=70,4,IF(G14/200*100&gt;=60,3.5,IF(G14/200*100&gt;=50,3,IF(G14/200*100&gt;=40,2,IF(G14/200*100&gt;=33,1,0))))))+IF(H14&gt;=80,5,IF(H14&gt;=70,4,IF(H14&gt;=60,3.5,IF(H14&gt;=50,3,IF(H14&gt;=40,2,IF(H14&gt;=33,1,0))))))+IF(I14&gt;=80,5,IF(I14&gt;=70,4,IF(I14&gt;=60,3.5,IF(I14&gt;=50,3,IF(I14&gt;=40,2,IF(I14&gt;=33,1,0))))))+IF(J14&gt;=80,5,IF(J14&gt;=70,4,IF(J14&gt;=60,3.5,IF(J14&gt;=50,3,IF(J14&gt;=40,2,IF(J14&gt;=33,1,0)))))))/8+IF(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))&gt;=2,(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB14" s="4">
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>158</v>
@@ -2276,7 +2276,7 @@
         <v>89</v>
       </c>
       <c r="N15" s="4">
-        <f>IF(C15&gt;=80,"A+",IF(C15&gt;=70,"A",IF(C15&gt;=60,"A-",IF(C15&gt;=50,"B",IF(C15&gt;=40,"C",IF(C15&gt;=33,"D","F"))))))</f>
+        <f>IF(C15/200*100&gt;=80,"A+",IF(C15/200*100&gt;=70,"A",IF(C15/200*100&gt;=60,"A-",IF(C15/200*100&gt;=50,"B",IF(C15/200*100&gt;=40,"C",IF(C15/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O15" s="4">
@@ -2328,7 +2328,7 @@
         <v/>
       </c>
       <c r="AA15" s="6">
-        <f>IF(OR(C15&lt;33,D15&lt;66,E15&lt;33,F15&lt;66,G15&lt;66,H15&lt;33,I15&lt;33,J15&lt;33,L15&lt;33,M15&lt;33),0,MIN(5,ROUND((IF(C15&gt;=80,5,IF(C15&gt;=70,4,IF(C15&gt;=60,3.5,IF(C15&gt;=50,3,IF(C15&gt;=40,2,IF(C15&gt;=33,1,0))))))+IF(D15/200*100&gt;=80,5,IF(D15/200*100&gt;=70,4,IF(D15/200*100&gt;=60,3.5,IF(D15/200*100&gt;=50,3,IF(D15/200*100&gt;=40,2,IF(D15/200*100&gt;=33,1,0))))))+IF(E15&gt;=80,5,IF(E15&gt;=70,4,IF(E15&gt;=60,3.5,IF(E15&gt;=50,3,IF(E15&gt;=40,2,IF(E15&gt;=33,1,0))))))+IF(F15/200*100&gt;=80,5,IF(F15/200*100&gt;=70,4,IF(F15/200*100&gt;=60,3.5,IF(F15/200*100&gt;=50,3,IF(F15/200*100&gt;=40,2,IF(F15/200*100&gt;=33,1,0))))))+IF(G15/200*100&gt;=80,5,IF(G15/200*100&gt;=70,4,IF(G15/200*100&gt;=60,3.5,IF(G15/200*100&gt;=50,3,IF(G15/200*100&gt;=40,2,IF(G15/200*100&gt;=33,1,0))))))+IF(H15&gt;=80,5,IF(H15&gt;=70,4,IF(H15&gt;=60,3.5,IF(H15&gt;=50,3,IF(H15&gt;=40,2,IF(H15&gt;=33,1,0))))))+IF(I15&gt;=80,5,IF(I15&gt;=70,4,IF(I15&gt;=60,3.5,IF(I15&gt;=50,3,IF(I15&gt;=40,2,IF(I15&gt;=33,1,0))))))+IF(J15&gt;=80,5,IF(J15&gt;=70,4,IF(J15&gt;=60,3.5,IF(J15&gt;=50,3,IF(J15&gt;=40,2,IF(J15&gt;=33,1,0)))))))/8+IF(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))&gt;=2,(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C15&lt;66,D15&lt;66,E15&lt;33,F15&lt;66,G15&lt;66,H15&lt;33,I15&lt;33,J15&lt;33,L15&lt;33,M15&lt;33),0,MIN(5,ROUND((IF(C15/200*100&gt;=80,5,IF(C15/200*100&gt;=70,4,IF(C15/200*100&gt;=60,3.5,IF(C15/200*100&gt;=50,3,IF(C15/200*100&gt;=40,2,IF(C15/200*100&gt;=33,1,0))))))+IF(D15/200*100&gt;=80,5,IF(D15/200*100&gt;=70,4,IF(D15/200*100&gt;=60,3.5,IF(D15/200*100&gt;=50,3,IF(D15/200*100&gt;=40,2,IF(D15/200*100&gt;=33,1,0))))))+IF(E15&gt;=80,5,IF(E15&gt;=70,4,IF(E15&gt;=60,3.5,IF(E15&gt;=50,3,IF(E15&gt;=40,2,IF(E15&gt;=33,1,0))))))+IF(F15/200*100&gt;=80,5,IF(F15/200*100&gt;=70,4,IF(F15/200*100&gt;=60,3.5,IF(F15/200*100&gt;=50,3,IF(F15/200*100&gt;=40,2,IF(F15/200*100&gt;=33,1,0))))))+IF(G15/200*100&gt;=80,5,IF(G15/200*100&gt;=70,4,IF(G15/200*100&gt;=60,3.5,IF(G15/200*100&gt;=50,3,IF(G15/200*100&gt;=40,2,IF(G15/200*100&gt;=33,1,0))))))+IF(H15&gt;=80,5,IF(H15&gt;=70,4,IF(H15&gt;=60,3.5,IF(H15&gt;=50,3,IF(H15&gt;=40,2,IF(H15&gt;=33,1,0))))))+IF(I15&gt;=80,5,IF(I15&gt;=70,4,IF(I15&gt;=60,3.5,IF(I15&gt;=50,3,IF(I15&gt;=40,2,IF(I15&gt;=33,1,0))))))+IF(J15&gt;=80,5,IF(J15&gt;=70,4,IF(J15&gt;=60,3.5,IF(J15&gt;=50,3,IF(J15&gt;=40,2,IF(J15&gt;=33,1,0)))))))/8+IF(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))&gt;=2,(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB15" s="4">
@@ -2346,7 +2346,7 @@
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>167</v>
@@ -2379,7 +2379,7 @@
         <v>91</v>
       </c>
       <c r="N16" s="4">
-        <f>IF(C16&gt;=80,"A+",IF(C16&gt;=70,"A",IF(C16&gt;=60,"A-",IF(C16&gt;=50,"B",IF(C16&gt;=40,"C",IF(C16&gt;=33,"D","F"))))))</f>
+        <f>IF(C16/200*100&gt;=80,"A+",IF(C16/200*100&gt;=70,"A",IF(C16/200*100&gt;=60,"A-",IF(C16/200*100&gt;=50,"B",IF(C16/200*100&gt;=40,"C",IF(C16/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O16" s="4">
@@ -2431,7 +2431,7 @@
         <v/>
       </c>
       <c r="AA16" s="6">
-        <f>IF(OR(C16&lt;33,D16&lt;66,E16&lt;33,F16&lt;66,G16&lt;66,H16&lt;33,I16&lt;33,J16&lt;33,L16&lt;33,M16&lt;33),0,MIN(5,ROUND((IF(C16&gt;=80,5,IF(C16&gt;=70,4,IF(C16&gt;=60,3.5,IF(C16&gt;=50,3,IF(C16&gt;=40,2,IF(C16&gt;=33,1,0))))))+IF(D16/200*100&gt;=80,5,IF(D16/200*100&gt;=70,4,IF(D16/200*100&gt;=60,3.5,IF(D16/200*100&gt;=50,3,IF(D16/200*100&gt;=40,2,IF(D16/200*100&gt;=33,1,0))))))+IF(E16&gt;=80,5,IF(E16&gt;=70,4,IF(E16&gt;=60,3.5,IF(E16&gt;=50,3,IF(E16&gt;=40,2,IF(E16&gt;=33,1,0))))))+IF(F16/200*100&gt;=80,5,IF(F16/200*100&gt;=70,4,IF(F16/200*100&gt;=60,3.5,IF(F16/200*100&gt;=50,3,IF(F16/200*100&gt;=40,2,IF(F16/200*100&gt;=33,1,0))))))+IF(G16/200*100&gt;=80,5,IF(G16/200*100&gt;=70,4,IF(G16/200*100&gt;=60,3.5,IF(G16/200*100&gt;=50,3,IF(G16/200*100&gt;=40,2,IF(G16/200*100&gt;=33,1,0))))))+IF(H16&gt;=80,5,IF(H16&gt;=70,4,IF(H16&gt;=60,3.5,IF(H16&gt;=50,3,IF(H16&gt;=40,2,IF(H16&gt;=33,1,0))))))+IF(I16&gt;=80,5,IF(I16&gt;=70,4,IF(I16&gt;=60,3.5,IF(I16&gt;=50,3,IF(I16&gt;=40,2,IF(I16&gt;=33,1,0))))))+IF(J16&gt;=80,5,IF(J16&gt;=70,4,IF(J16&gt;=60,3.5,IF(J16&gt;=50,3,IF(J16&gt;=40,2,IF(J16&gt;=33,1,0)))))))/8+IF(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))&gt;=2,(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C16&lt;66,D16&lt;66,E16&lt;33,F16&lt;66,G16&lt;66,H16&lt;33,I16&lt;33,J16&lt;33,L16&lt;33,M16&lt;33),0,MIN(5,ROUND((IF(C16/200*100&gt;=80,5,IF(C16/200*100&gt;=70,4,IF(C16/200*100&gt;=60,3.5,IF(C16/200*100&gt;=50,3,IF(C16/200*100&gt;=40,2,IF(C16/200*100&gt;=33,1,0))))))+IF(D16/200*100&gt;=80,5,IF(D16/200*100&gt;=70,4,IF(D16/200*100&gt;=60,3.5,IF(D16/200*100&gt;=50,3,IF(D16/200*100&gt;=40,2,IF(D16/200*100&gt;=33,1,0))))))+IF(E16&gt;=80,5,IF(E16&gt;=70,4,IF(E16&gt;=60,3.5,IF(E16&gt;=50,3,IF(E16&gt;=40,2,IF(E16&gt;=33,1,0))))))+IF(F16/200*100&gt;=80,5,IF(F16/200*100&gt;=70,4,IF(F16/200*100&gt;=60,3.5,IF(F16/200*100&gt;=50,3,IF(F16/200*100&gt;=40,2,IF(F16/200*100&gt;=33,1,0))))))+IF(G16/200*100&gt;=80,5,IF(G16/200*100&gt;=70,4,IF(G16/200*100&gt;=60,3.5,IF(G16/200*100&gt;=50,3,IF(G16/200*100&gt;=40,2,IF(G16/200*100&gt;=33,1,0))))))+IF(H16&gt;=80,5,IF(H16&gt;=70,4,IF(H16&gt;=60,3.5,IF(H16&gt;=50,3,IF(H16&gt;=40,2,IF(H16&gt;=33,1,0))))))+IF(I16&gt;=80,5,IF(I16&gt;=70,4,IF(I16&gt;=60,3.5,IF(I16&gt;=50,3,IF(I16&gt;=40,2,IF(I16&gt;=33,1,0))))))+IF(J16&gt;=80,5,IF(J16&gt;=70,4,IF(J16&gt;=60,3.5,IF(J16&gt;=50,3,IF(J16&gt;=40,2,IF(J16&gt;=33,1,0)))))))/8+IF(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))&gt;=2,(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB16" s="4">
@@ -2449,7 +2449,7 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>147</v>
@@ -2482,7 +2482,7 @@
         <v>89</v>
       </c>
       <c r="N17" s="4">
-        <f>IF(C17&gt;=80,"A+",IF(C17&gt;=70,"A",IF(C17&gt;=60,"A-",IF(C17&gt;=50,"B",IF(C17&gt;=40,"C",IF(C17&gt;=33,"D","F"))))))</f>
+        <f>IF(C17/200*100&gt;=80,"A+",IF(C17/200*100&gt;=70,"A",IF(C17/200*100&gt;=60,"A-",IF(C17/200*100&gt;=50,"B",IF(C17/200*100&gt;=40,"C",IF(C17/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O17" s="4">
@@ -2534,7 +2534,7 @@
         <v/>
       </c>
       <c r="AA17" s="6">
-        <f>IF(OR(C17&lt;33,D17&lt;66,E17&lt;33,F17&lt;66,G17&lt;66,H17&lt;33,I17&lt;33,J17&lt;33,L17&lt;33,M17&lt;33),0,MIN(5,ROUND((IF(C17&gt;=80,5,IF(C17&gt;=70,4,IF(C17&gt;=60,3.5,IF(C17&gt;=50,3,IF(C17&gt;=40,2,IF(C17&gt;=33,1,0))))))+IF(D17/200*100&gt;=80,5,IF(D17/200*100&gt;=70,4,IF(D17/200*100&gt;=60,3.5,IF(D17/200*100&gt;=50,3,IF(D17/200*100&gt;=40,2,IF(D17/200*100&gt;=33,1,0))))))+IF(E17&gt;=80,5,IF(E17&gt;=70,4,IF(E17&gt;=60,3.5,IF(E17&gt;=50,3,IF(E17&gt;=40,2,IF(E17&gt;=33,1,0))))))+IF(F17/200*100&gt;=80,5,IF(F17/200*100&gt;=70,4,IF(F17/200*100&gt;=60,3.5,IF(F17/200*100&gt;=50,3,IF(F17/200*100&gt;=40,2,IF(F17/200*100&gt;=33,1,0))))))+IF(G17/200*100&gt;=80,5,IF(G17/200*100&gt;=70,4,IF(G17/200*100&gt;=60,3.5,IF(G17/200*100&gt;=50,3,IF(G17/200*100&gt;=40,2,IF(G17/200*100&gt;=33,1,0))))))+IF(H17&gt;=80,5,IF(H17&gt;=70,4,IF(H17&gt;=60,3.5,IF(H17&gt;=50,3,IF(H17&gt;=40,2,IF(H17&gt;=33,1,0))))))+IF(I17&gt;=80,5,IF(I17&gt;=70,4,IF(I17&gt;=60,3.5,IF(I17&gt;=50,3,IF(I17&gt;=40,2,IF(I17&gt;=33,1,0))))))+IF(J17&gt;=80,5,IF(J17&gt;=70,4,IF(J17&gt;=60,3.5,IF(J17&gt;=50,3,IF(J17&gt;=40,2,IF(J17&gt;=33,1,0)))))))/8+IF(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))&gt;=2,(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C17&lt;66,D17&lt;66,E17&lt;33,F17&lt;66,G17&lt;66,H17&lt;33,I17&lt;33,J17&lt;33,L17&lt;33,M17&lt;33),0,MIN(5,ROUND((IF(C17/200*100&gt;=80,5,IF(C17/200*100&gt;=70,4,IF(C17/200*100&gt;=60,3.5,IF(C17/200*100&gt;=50,3,IF(C17/200*100&gt;=40,2,IF(C17/200*100&gt;=33,1,0))))))+IF(D17/200*100&gt;=80,5,IF(D17/200*100&gt;=70,4,IF(D17/200*100&gt;=60,3.5,IF(D17/200*100&gt;=50,3,IF(D17/200*100&gt;=40,2,IF(D17/200*100&gt;=33,1,0))))))+IF(E17&gt;=80,5,IF(E17&gt;=70,4,IF(E17&gt;=60,3.5,IF(E17&gt;=50,3,IF(E17&gt;=40,2,IF(E17&gt;=33,1,0))))))+IF(F17/200*100&gt;=80,5,IF(F17/200*100&gt;=70,4,IF(F17/200*100&gt;=60,3.5,IF(F17/200*100&gt;=50,3,IF(F17/200*100&gt;=40,2,IF(F17/200*100&gt;=33,1,0))))))+IF(G17/200*100&gt;=80,5,IF(G17/200*100&gt;=70,4,IF(G17/200*100&gt;=60,3.5,IF(G17/200*100&gt;=50,3,IF(G17/200*100&gt;=40,2,IF(G17/200*100&gt;=33,1,0))))))+IF(H17&gt;=80,5,IF(H17&gt;=70,4,IF(H17&gt;=60,3.5,IF(H17&gt;=50,3,IF(H17&gt;=40,2,IF(H17&gt;=33,1,0))))))+IF(I17&gt;=80,5,IF(I17&gt;=70,4,IF(I17&gt;=60,3.5,IF(I17&gt;=50,3,IF(I17&gt;=40,2,IF(I17&gt;=33,1,0))))))+IF(J17&gt;=80,5,IF(J17&gt;=70,4,IF(J17&gt;=60,3.5,IF(J17&gt;=50,3,IF(J17&gt;=40,2,IF(J17&gt;=33,1,0)))))))/8+IF(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))&gt;=2,(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB17" s="4">
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>181</v>
@@ -2585,7 +2585,7 @@
         <v>78</v>
       </c>
       <c r="N18" s="4">
-        <f>IF(C18&gt;=80,"A+",IF(C18&gt;=70,"A",IF(C18&gt;=60,"A-",IF(C18&gt;=50,"B",IF(C18&gt;=40,"C",IF(C18&gt;=33,"D","F"))))))</f>
+        <f>IF(C18/200*100&gt;=80,"A+",IF(C18/200*100&gt;=70,"A",IF(C18/200*100&gt;=60,"A-",IF(C18/200*100&gt;=50,"B",IF(C18/200*100&gt;=40,"C",IF(C18/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O18" s="4">
@@ -2637,7 +2637,7 @@
         <v/>
       </c>
       <c r="AA18" s="6">
-        <f>IF(OR(C18&lt;33,D18&lt;66,E18&lt;33,F18&lt;66,G18&lt;66,H18&lt;33,I18&lt;33,J18&lt;33,L18&lt;33,M18&lt;33),0,MIN(5,ROUND((IF(C18&gt;=80,5,IF(C18&gt;=70,4,IF(C18&gt;=60,3.5,IF(C18&gt;=50,3,IF(C18&gt;=40,2,IF(C18&gt;=33,1,0))))))+IF(D18/200*100&gt;=80,5,IF(D18/200*100&gt;=70,4,IF(D18/200*100&gt;=60,3.5,IF(D18/200*100&gt;=50,3,IF(D18/200*100&gt;=40,2,IF(D18/200*100&gt;=33,1,0))))))+IF(E18&gt;=80,5,IF(E18&gt;=70,4,IF(E18&gt;=60,3.5,IF(E18&gt;=50,3,IF(E18&gt;=40,2,IF(E18&gt;=33,1,0))))))+IF(F18/200*100&gt;=80,5,IF(F18/200*100&gt;=70,4,IF(F18/200*100&gt;=60,3.5,IF(F18/200*100&gt;=50,3,IF(F18/200*100&gt;=40,2,IF(F18/200*100&gt;=33,1,0))))))+IF(G18/200*100&gt;=80,5,IF(G18/200*100&gt;=70,4,IF(G18/200*100&gt;=60,3.5,IF(G18/200*100&gt;=50,3,IF(G18/200*100&gt;=40,2,IF(G18/200*100&gt;=33,1,0))))))+IF(H18&gt;=80,5,IF(H18&gt;=70,4,IF(H18&gt;=60,3.5,IF(H18&gt;=50,3,IF(H18&gt;=40,2,IF(H18&gt;=33,1,0))))))+IF(I18&gt;=80,5,IF(I18&gt;=70,4,IF(I18&gt;=60,3.5,IF(I18&gt;=50,3,IF(I18&gt;=40,2,IF(I18&gt;=33,1,0))))))+IF(J18&gt;=80,5,IF(J18&gt;=70,4,IF(J18&gt;=60,3.5,IF(J18&gt;=50,3,IF(J18&gt;=40,2,IF(J18&gt;=33,1,0)))))))/8+IF(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))&gt;=2,(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C18&lt;66,D18&lt;66,E18&lt;33,F18&lt;66,G18&lt;66,H18&lt;33,I18&lt;33,J18&lt;33,L18&lt;33,M18&lt;33),0,MIN(5,ROUND((IF(C18/200*100&gt;=80,5,IF(C18/200*100&gt;=70,4,IF(C18/200*100&gt;=60,3.5,IF(C18/200*100&gt;=50,3,IF(C18/200*100&gt;=40,2,IF(C18/200*100&gt;=33,1,0))))))+IF(D18/200*100&gt;=80,5,IF(D18/200*100&gt;=70,4,IF(D18/200*100&gt;=60,3.5,IF(D18/200*100&gt;=50,3,IF(D18/200*100&gt;=40,2,IF(D18/200*100&gt;=33,1,0))))))+IF(E18&gt;=80,5,IF(E18&gt;=70,4,IF(E18&gt;=60,3.5,IF(E18&gt;=50,3,IF(E18&gt;=40,2,IF(E18&gt;=33,1,0))))))+IF(F18/200*100&gt;=80,5,IF(F18/200*100&gt;=70,4,IF(F18/200*100&gt;=60,3.5,IF(F18/200*100&gt;=50,3,IF(F18/200*100&gt;=40,2,IF(F18/200*100&gt;=33,1,0))))))+IF(G18/200*100&gt;=80,5,IF(G18/200*100&gt;=70,4,IF(G18/200*100&gt;=60,3.5,IF(G18/200*100&gt;=50,3,IF(G18/200*100&gt;=40,2,IF(G18/200*100&gt;=33,1,0))))))+IF(H18&gt;=80,5,IF(H18&gt;=70,4,IF(H18&gt;=60,3.5,IF(H18&gt;=50,3,IF(H18&gt;=40,2,IF(H18&gt;=33,1,0))))))+IF(I18&gt;=80,5,IF(I18&gt;=70,4,IF(I18&gt;=60,3.5,IF(I18&gt;=50,3,IF(I18&gt;=40,2,IF(I18&gt;=33,1,0))))))+IF(J18&gt;=80,5,IF(J18&gt;=70,4,IF(J18&gt;=60,3.5,IF(J18&gt;=50,3,IF(J18&gt;=40,2,IF(J18&gt;=33,1,0)))))))/8+IF(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))&gt;=2,(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB18" s="4">
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>185</v>
@@ -2688,7 +2688,7 @@
         <v>82</v>
       </c>
       <c r="N19" s="4">
-        <f>IF(C19&gt;=80,"A+",IF(C19&gt;=70,"A",IF(C19&gt;=60,"A-",IF(C19&gt;=50,"B",IF(C19&gt;=40,"C",IF(C19&gt;=33,"D","F"))))))</f>
+        <f>IF(C19/200*100&gt;=80,"A+",IF(C19/200*100&gt;=70,"A",IF(C19/200*100&gt;=60,"A-",IF(C19/200*100&gt;=50,"B",IF(C19/200*100&gt;=40,"C",IF(C19/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O19" s="4">
@@ -2740,7 +2740,7 @@
         <v/>
       </c>
       <c r="AA19" s="6">
-        <f>IF(OR(C19&lt;33,D19&lt;66,E19&lt;33,F19&lt;66,G19&lt;66,H19&lt;33,I19&lt;33,J19&lt;33,L19&lt;33,M19&lt;33),0,MIN(5,ROUND((IF(C19&gt;=80,5,IF(C19&gt;=70,4,IF(C19&gt;=60,3.5,IF(C19&gt;=50,3,IF(C19&gt;=40,2,IF(C19&gt;=33,1,0))))))+IF(D19/200*100&gt;=80,5,IF(D19/200*100&gt;=70,4,IF(D19/200*100&gt;=60,3.5,IF(D19/200*100&gt;=50,3,IF(D19/200*100&gt;=40,2,IF(D19/200*100&gt;=33,1,0))))))+IF(E19&gt;=80,5,IF(E19&gt;=70,4,IF(E19&gt;=60,3.5,IF(E19&gt;=50,3,IF(E19&gt;=40,2,IF(E19&gt;=33,1,0))))))+IF(F19/200*100&gt;=80,5,IF(F19/200*100&gt;=70,4,IF(F19/200*100&gt;=60,3.5,IF(F19/200*100&gt;=50,3,IF(F19/200*100&gt;=40,2,IF(F19/200*100&gt;=33,1,0))))))+IF(G19/200*100&gt;=80,5,IF(G19/200*100&gt;=70,4,IF(G19/200*100&gt;=60,3.5,IF(G19/200*100&gt;=50,3,IF(G19/200*100&gt;=40,2,IF(G19/200*100&gt;=33,1,0))))))+IF(H19&gt;=80,5,IF(H19&gt;=70,4,IF(H19&gt;=60,3.5,IF(H19&gt;=50,3,IF(H19&gt;=40,2,IF(H19&gt;=33,1,0))))))+IF(I19&gt;=80,5,IF(I19&gt;=70,4,IF(I19&gt;=60,3.5,IF(I19&gt;=50,3,IF(I19&gt;=40,2,IF(I19&gt;=33,1,0))))))+IF(J19&gt;=80,5,IF(J19&gt;=70,4,IF(J19&gt;=60,3.5,IF(J19&gt;=50,3,IF(J19&gt;=40,2,IF(J19&gt;=33,1,0)))))))/8+IF(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))&gt;=2,(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C19&lt;66,D19&lt;66,E19&lt;33,F19&lt;66,G19&lt;66,H19&lt;33,I19&lt;33,J19&lt;33,L19&lt;33,M19&lt;33),0,MIN(5,ROUND((IF(C19/200*100&gt;=80,5,IF(C19/200*100&gt;=70,4,IF(C19/200*100&gt;=60,3.5,IF(C19/200*100&gt;=50,3,IF(C19/200*100&gt;=40,2,IF(C19/200*100&gt;=33,1,0))))))+IF(D19/200*100&gt;=80,5,IF(D19/200*100&gt;=70,4,IF(D19/200*100&gt;=60,3.5,IF(D19/200*100&gt;=50,3,IF(D19/200*100&gt;=40,2,IF(D19/200*100&gt;=33,1,0))))))+IF(E19&gt;=80,5,IF(E19&gt;=70,4,IF(E19&gt;=60,3.5,IF(E19&gt;=50,3,IF(E19&gt;=40,2,IF(E19&gt;=33,1,0))))))+IF(F19/200*100&gt;=80,5,IF(F19/200*100&gt;=70,4,IF(F19/200*100&gt;=60,3.5,IF(F19/200*100&gt;=50,3,IF(F19/200*100&gt;=40,2,IF(F19/200*100&gt;=33,1,0))))))+IF(G19/200*100&gt;=80,5,IF(G19/200*100&gt;=70,4,IF(G19/200*100&gt;=60,3.5,IF(G19/200*100&gt;=50,3,IF(G19/200*100&gt;=40,2,IF(G19/200*100&gt;=33,1,0))))))+IF(H19&gt;=80,5,IF(H19&gt;=70,4,IF(H19&gt;=60,3.5,IF(H19&gt;=50,3,IF(H19&gt;=40,2,IF(H19&gt;=33,1,0))))))+IF(I19&gt;=80,5,IF(I19&gt;=70,4,IF(I19&gt;=60,3.5,IF(I19&gt;=50,3,IF(I19&gt;=40,2,IF(I19&gt;=33,1,0))))))+IF(J19&gt;=80,5,IF(J19&gt;=70,4,IF(J19&gt;=60,3.5,IF(J19&gt;=50,3,IF(J19&gt;=40,2,IF(J19&gt;=33,1,0)))))))/8+IF(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))&gt;=2,(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB19" s="4">
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="C20" s="3" t="n">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>130</v>
@@ -2791,7 +2791,7 @@
         <v>82</v>
       </c>
       <c r="N20" s="4">
-        <f>IF(C20&gt;=80,"A+",IF(C20&gt;=70,"A",IF(C20&gt;=60,"A-",IF(C20&gt;=50,"B",IF(C20&gt;=40,"C",IF(C20&gt;=33,"D","F"))))))</f>
+        <f>IF(C20/200*100&gt;=80,"A+",IF(C20/200*100&gt;=70,"A",IF(C20/200*100&gt;=60,"A-",IF(C20/200*100&gt;=50,"B",IF(C20/200*100&gt;=40,"C",IF(C20/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O20" s="4">
@@ -2843,7 +2843,7 @@
         <v/>
       </c>
       <c r="AA20" s="6">
-        <f>IF(OR(C20&lt;33,D20&lt;66,E20&lt;33,F20&lt;66,G20&lt;66,H20&lt;33,I20&lt;33,J20&lt;33,L20&lt;33,M20&lt;33),0,MIN(5,ROUND((IF(C20&gt;=80,5,IF(C20&gt;=70,4,IF(C20&gt;=60,3.5,IF(C20&gt;=50,3,IF(C20&gt;=40,2,IF(C20&gt;=33,1,0))))))+IF(D20/200*100&gt;=80,5,IF(D20/200*100&gt;=70,4,IF(D20/200*100&gt;=60,3.5,IF(D20/200*100&gt;=50,3,IF(D20/200*100&gt;=40,2,IF(D20/200*100&gt;=33,1,0))))))+IF(E20&gt;=80,5,IF(E20&gt;=70,4,IF(E20&gt;=60,3.5,IF(E20&gt;=50,3,IF(E20&gt;=40,2,IF(E20&gt;=33,1,0))))))+IF(F20/200*100&gt;=80,5,IF(F20/200*100&gt;=70,4,IF(F20/200*100&gt;=60,3.5,IF(F20/200*100&gt;=50,3,IF(F20/200*100&gt;=40,2,IF(F20/200*100&gt;=33,1,0))))))+IF(G20/200*100&gt;=80,5,IF(G20/200*100&gt;=70,4,IF(G20/200*100&gt;=60,3.5,IF(G20/200*100&gt;=50,3,IF(G20/200*100&gt;=40,2,IF(G20/200*100&gt;=33,1,0))))))+IF(H20&gt;=80,5,IF(H20&gt;=70,4,IF(H20&gt;=60,3.5,IF(H20&gt;=50,3,IF(H20&gt;=40,2,IF(H20&gt;=33,1,0))))))+IF(I20&gt;=80,5,IF(I20&gt;=70,4,IF(I20&gt;=60,3.5,IF(I20&gt;=50,3,IF(I20&gt;=40,2,IF(I20&gt;=33,1,0))))))+IF(J20&gt;=80,5,IF(J20&gt;=70,4,IF(J20&gt;=60,3.5,IF(J20&gt;=50,3,IF(J20&gt;=40,2,IF(J20&gt;=33,1,0)))))))/8+IF(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))&gt;=2,(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C20&lt;66,D20&lt;66,E20&lt;33,F20&lt;66,G20&lt;66,H20&lt;33,I20&lt;33,J20&lt;33,L20&lt;33,M20&lt;33),0,MIN(5,ROUND((IF(C20/200*100&gt;=80,5,IF(C20/200*100&gt;=70,4,IF(C20/200*100&gt;=60,3.5,IF(C20/200*100&gt;=50,3,IF(C20/200*100&gt;=40,2,IF(C20/200*100&gt;=33,1,0))))))+IF(D20/200*100&gt;=80,5,IF(D20/200*100&gt;=70,4,IF(D20/200*100&gt;=60,3.5,IF(D20/200*100&gt;=50,3,IF(D20/200*100&gt;=40,2,IF(D20/200*100&gt;=33,1,0))))))+IF(E20&gt;=80,5,IF(E20&gt;=70,4,IF(E20&gt;=60,3.5,IF(E20&gt;=50,3,IF(E20&gt;=40,2,IF(E20&gt;=33,1,0))))))+IF(F20/200*100&gt;=80,5,IF(F20/200*100&gt;=70,4,IF(F20/200*100&gt;=60,3.5,IF(F20/200*100&gt;=50,3,IF(F20/200*100&gt;=40,2,IF(F20/200*100&gt;=33,1,0))))))+IF(G20/200*100&gt;=80,5,IF(G20/200*100&gt;=70,4,IF(G20/200*100&gt;=60,3.5,IF(G20/200*100&gt;=50,3,IF(G20/200*100&gt;=40,2,IF(G20/200*100&gt;=33,1,0))))))+IF(H20&gt;=80,5,IF(H20&gt;=70,4,IF(H20&gt;=60,3.5,IF(H20&gt;=50,3,IF(H20&gt;=40,2,IF(H20&gt;=33,1,0))))))+IF(I20&gt;=80,5,IF(I20&gt;=70,4,IF(I20&gt;=60,3.5,IF(I20&gt;=50,3,IF(I20&gt;=40,2,IF(I20&gt;=33,1,0))))))+IF(J20&gt;=80,5,IF(J20&gt;=70,4,IF(J20&gt;=60,3.5,IF(J20&gt;=50,3,IF(J20&gt;=40,2,IF(J20&gt;=33,1,0)))))))/8+IF(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))&gt;=2,(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB20" s="4">
@@ -2861,7 +2861,7 @@
         </is>
       </c>
       <c r="C21" s="3" t="n">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>178</v>
@@ -2894,7 +2894,7 @@
         <v>77</v>
       </c>
       <c r="N21" s="4">
-        <f>IF(C21&gt;=80,"A+",IF(C21&gt;=70,"A",IF(C21&gt;=60,"A-",IF(C21&gt;=50,"B",IF(C21&gt;=40,"C",IF(C21&gt;=33,"D","F"))))))</f>
+        <f>IF(C21/200*100&gt;=80,"A+",IF(C21/200*100&gt;=70,"A",IF(C21/200*100&gt;=60,"A-",IF(C21/200*100&gt;=50,"B",IF(C21/200*100&gt;=40,"C",IF(C21/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="O21" s="4">
@@ -2946,7 +2946,7 @@
         <v/>
       </c>
       <c r="AA21" s="6">
-        <f>IF(OR(C21&lt;33,D21&lt;66,E21&lt;33,F21&lt;66,G21&lt;66,H21&lt;33,I21&lt;33,J21&lt;33,L21&lt;33,M21&lt;33),0,MIN(5,ROUND((IF(C21&gt;=80,5,IF(C21&gt;=70,4,IF(C21&gt;=60,3.5,IF(C21&gt;=50,3,IF(C21&gt;=40,2,IF(C21&gt;=33,1,0))))))+IF(D21/200*100&gt;=80,5,IF(D21/200*100&gt;=70,4,IF(D21/200*100&gt;=60,3.5,IF(D21/200*100&gt;=50,3,IF(D21/200*100&gt;=40,2,IF(D21/200*100&gt;=33,1,0))))))+IF(E21&gt;=80,5,IF(E21&gt;=70,4,IF(E21&gt;=60,3.5,IF(E21&gt;=50,3,IF(E21&gt;=40,2,IF(E21&gt;=33,1,0))))))+IF(F21/200*100&gt;=80,5,IF(F21/200*100&gt;=70,4,IF(F21/200*100&gt;=60,3.5,IF(F21/200*100&gt;=50,3,IF(F21/200*100&gt;=40,2,IF(F21/200*100&gt;=33,1,0))))))+IF(G21/200*100&gt;=80,5,IF(G21/200*100&gt;=70,4,IF(G21/200*100&gt;=60,3.5,IF(G21/200*100&gt;=50,3,IF(G21/200*100&gt;=40,2,IF(G21/200*100&gt;=33,1,0))))))+IF(H21&gt;=80,5,IF(H21&gt;=70,4,IF(H21&gt;=60,3.5,IF(H21&gt;=50,3,IF(H21&gt;=40,2,IF(H21&gt;=33,1,0))))))+IF(I21&gt;=80,5,IF(I21&gt;=70,4,IF(I21&gt;=60,3.5,IF(I21&gt;=50,3,IF(I21&gt;=40,2,IF(I21&gt;=33,1,0))))))+IF(J21&gt;=80,5,IF(J21&gt;=70,4,IF(J21&gt;=60,3.5,IF(J21&gt;=50,3,IF(J21&gt;=40,2,IF(J21&gt;=33,1,0)))))))/8+IF(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))&gt;=2,(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <f>IF(OR(C21&lt;66,D21&lt;66,E21&lt;33,F21&lt;66,G21&lt;66,H21&lt;33,I21&lt;33,J21&lt;33,L21&lt;33,M21&lt;33),0,MIN(5,ROUND((IF(C21/200*100&gt;=80,5,IF(C21/200*100&gt;=70,4,IF(C21/200*100&gt;=60,3.5,IF(C21/200*100&gt;=50,3,IF(C21/200*100&gt;=40,2,IF(C21/200*100&gt;=33,1,0))))))+IF(D21/200*100&gt;=80,5,IF(D21/200*100&gt;=70,4,IF(D21/200*100&gt;=60,3.5,IF(D21/200*100&gt;=50,3,IF(D21/200*100&gt;=40,2,IF(D21/200*100&gt;=33,1,0))))))+IF(E21&gt;=80,5,IF(E21&gt;=70,4,IF(E21&gt;=60,3.5,IF(E21&gt;=50,3,IF(E21&gt;=40,2,IF(E21&gt;=33,1,0))))))+IF(F21/200*100&gt;=80,5,IF(F21/200*100&gt;=70,4,IF(F21/200*100&gt;=60,3.5,IF(F21/200*100&gt;=50,3,IF(F21/200*100&gt;=40,2,IF(F21/200*100&gt;=33,1,0))))))+IF(G21/200*100&gt;=80,5,IF(G21/200*100&gt;=70,4,IF(G21/200*100&gt;=60,3.5,IF(G21/200*100&gt;=50,3,IF(G21/200*100&gt;=40,2,IF(G21/200*100&gt;=33,1,0))))))+IF(H21&gt;=80,5,IF(H21&gt;=70,4,IF(H21&gt;=60,3.5,IF(H21&gt;=50,3,IF(H21&gt;=40,2,IF(H21&gt;=33,1,0))))))+IF(I21&gt;=80,5,IF(I21&gt;=70,4,IF(I21&gt;=60,3.5,IF(I21&gt;=50,3,IF(I21&gt;=40,2,IF(I21&gt;=33,1,0))))))+IF(J21&gt;=80,5,IF(J21&gt;=70,4,IF(J21&gt;=60,3.5,IF(J21&gt;=50,3,IF(J21&gt;=40,2,IF(J21&gt;=33,1,0)))))))/8+IF(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))&gt;=2,(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
       <c r="AB21" s="4">

</xml_diff>

<commit_message>
Add Subject Grades sheet and update GPA calculation logic in Excel generation
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Data Source" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Pivot" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Subject Grades" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Pivot" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -22,7 +23,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0&quot;%&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -56,8 +57,17 @@
       <b val="1"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -88,6 +98,18 @@
         <bgColor rgb="00FFE699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005B9BD5"/>
+        <bgColor rgb="005B9BD5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -101,18 +123,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -130,6 +152,12 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,21 +763,10 @@
     <col width="10" customWidth="1" min="11" max="11"/>
     <col width="12" customWidth="1" min="12" max="12"/>
     <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="11" customWidth="1" min="14" max="14"/>
-    <col width="11" customWidth="1" min="15" max="15"/>
-    <col width="11" customWidth="1" min="16" max="16"/>
-    <col width="11" customWidth="1" min="17" max="17"/>
-    <col width="11" customWidth="1" min="18" max="18"/>
-    <col width="11" customWidth="1" min="19" max="19"/>
-    <col width="11" customWidth="1" min="20" max="20"/>
-    <col width="10" customWidth="1" min="21" max="21"/>
-    <col width="11" customWidth="1" min="22" max="22"/>
-    <col width="11" customWidth="1" min="23" max="23"/>
-    <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="10" customWidth="1" min="25" max="25"/>
-    <col width="10" customWidth="1" min="26" max="26"/>
-    <col width="8" customWidth="1" min="27" max="27"/>
-    <col width="8" customWidth="1" min="28" max="28"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -820,75 +837,20 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Quran Grade</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Arabic Grade</t>
+          <t>Average</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Aqaid Grade</t>
+          <t>GPA</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>English Grade</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Bangla Grade</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Math Grade</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>History Grade</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>ICT Grade</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Mantiq Grade</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Career Grade</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Physical Grade</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Average</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>GPA</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Overall Grade</t>
         </is>
@@ -936,64 +898,20 @@
       <c r="M2" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="N2" s="4">
-        <f>IF(C2/200*100&gt;=80,"A+",IF(C2/200*100&gt;=70,"A",IF(C2/200*100&gt;=60,"A-",IF(C2/200*100&gt;=50,"B",IF(C2/200*100&gt;=40,"C",IF(C2/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N2">
+        <f>SUM(C2:J2)</f>
         <v/>
       </c>
       <c r="O2" s="4">
-        <f>IF(D2/200*100&gt;=80,"A+",IF(D2/200*100&gt;=70,"A",IF(D2/200*100&gt;=60,"A-",IF(D2/200*100&gt;=50,"B",IF(D2/200*100&gt;=40,"C",IF(D2/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P2" s="4">
-        <f>IF(E2&gt;=80,"A+",IF(E2&gt;=70,"A",IF(E2&gt;=60,"A-",IF(E2&gt;=50,"B",IF(E2&gt;=40,"C",IF(E2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q2" s="4">
-        <f>IF(F2/200*100&gt;=80,"A+",IF(F2/200*100&gt;=70,"A",IF(F2/200*100&gt;=60,"A-",IF(F2/200*100&gt;=50,"B",IF(F2/200*100&gt;=40,"C",IF(F2/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R2" s="4">
-        <f>IF(G2/200*100&gt;=80,"A+",IF(G2/200*100&gt;=70,"A",IF(G2/200*100&gt;=60,"A-",IF(G2/200*100&gt;=50,"B",IF(G2/200*100&gt;=40,"C",IF(G2/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S2" s="4">
-        <f>IF(H2&gt;=80,"A+",IF(H2&gt;=70,"A",IF(H2&gt;=60,"A-",IF(H2&gt;=50,"B",IF(H2&gt;=40,"C",IF(H2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T2" s="4">
-        <f>IF(I2&gt;=80,"A+",IF(I2&gt;=70,"A",IF(I2&gt;=60,"A-",IF(I2&gt;=50,"B",IF(I2&gt;=40,"C",IF(I2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U2" s="4">
-        <f>IF(J2&gt;=80,"A+",IF(J2&gt;=70,"A",IF(J2&gt;=60,"A-",IF(J2&gt;=50,"B",IF(J2&gt;=40,"C",IF(J2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V2" s="4">
-        <f>IF(K2&gt;=80,"A+",IF(K2&gt;=70,"A",IF(K2&gt;=60,"A-",IF(K2&gt;=50,"B",IF(K2&gt;=40,"C",IF(K2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W2" s="4">
-        <f>IF(L2&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X2" s="4">
-        <f>IF(M2&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y2">
-        <f>SUM(C2:J2)</f>
-        <v/>
-      </c>
-      <c r="Z2" s="5">
-        <f>ROUND(Y2/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA2" s="6">
+        <f>ROUND(N2/8,2)</f>
+        <v/>
+      </c>
+      <c r="P2" s="5">
         <f>IF(OR(C2&lt;66,D2&lt;66,E2&lt;33,F2&lt;66,G2&lt;66,H2&lt;33,I2&lt;33,J2&lt;33,L2&lt;33,M2&lt;33),0,MIN(5,ROUND((IF(C2/200*100&gt;=80,5,IF(C2/200*100&gt;=70,4,IF(C2/200*100&gt;=60,3.5,IF(C2/200*100&gt;=50,3,IF(C2/200*100&gt;=40,2,IF(C2/200*100&gt;=33,1,0))))))+IF(D2/200*100&gt;=80,5,IF(D2/200*100&gt;=70,4,IF(D2/200*100&gt;=60,3.5,IF(D2/200*100&gt;=50,3,IF(D2/200*100&gt;=40,2,IF(D2/200*100&gt;=33,1,0))))))+IF(E2&gt;=80,5,IF(E2&gt;=70,4,IF(E2&gt;=60,3.5,IF(E2&gt;=50,3,IF(E2&gt;=40,2,IF(E2&gt;=33,1,0))))))+IF(F2/200*100&gt;=80,5,IF(F2/200*100&gt;=70,4,IF(F2/200*100&gt;=60,3.5,IF(F2/200*100&gt;=50,3,IF(F2/200*100&gt;=40,2,IF(F2/200*100&gt;=33,1,0))))))+IF(G2/200*100&gt;=80,5,IF(G2/200*100&gt;=70,4,IF(G2/200*100&gt;=60,3.5,IF(G2/200*100&gt;=50,3,IF(G2/200*100&gt;=40,2,IF(G2/200*100&gt;=33,1,0))))))+IF(H2&gt;=80,5,IF(H2&gt;=70,4,IF(H2&gt;=60,3.5,IF(H2&gt;=50,3,IF(H2&gt;=40,2,IF(H2&gt;=33,1,0))))))+IF(I2&gt;=80,5,IF(I2&gt;=70,4,IF(I2&gt;=60,3.5,IF(I2&gt;=50,3,IF(I2&gt;=40,2,IF(I2&gt;=33,1,0))))))+IF(J2&gt;=80,5,IF(J2&gt;=70,4,IF(J2&gt;=60,3.5,IF(J2&gt;=50,3,IF(J2&gt;=40,2,IF(J2&gt;=33,1,0)))))))/8+IF(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))&gt;=2,(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB2" s="4">
-        <f>IF(AA2&gt;=5,"A+",IF(AA2&gt;=4,"A",IF(AA2&gt;=3.5,"A-",IF(AA2&gt;=3,"B",IF(AA2&gt;=2,"C",IF(AA2&gt;=1,"D","F"))))))</f>
+      <c r="Q2" s="6">
+        <f>IF(P2&gt;=5,"A+",IF(P2&gt;=4,"A",IF(P2&gt;=3.5,"A-",IF(P2&gt;=3,"B",IF(P2&gt;=2,"C",IF(P2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1039,64 +957,20 @@
       <c r="M3" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="N3" s="4">
-        <f>IF(C3/200*100&gt;=80,"A+",IF(C3/200*100&gt;=70,"A",IF(C3/200*100&gt;=60,"A-",IF(C3/200*100&gt;=50,"B",IF(C3/200*100&gt;=40,"C",IF(C3/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N3">
+        <f>SUM(C3:J3)</f>
         <v/>
       </c>
       <c r="O3" s="4">
-        <f>IF(D3/200*100&gt;=80,"A+",IF(D3/200*100&gt;=70,"A",IF(D3/200*100&gt;=60,"A-",IF(D3/200*100&gt;=50,"B",IF(D3/200*100&gt;=40,"C",IF(D3/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P3" s="4">
-        <f>IF(E3&gt;=80,"A+",IF(E3&gt;=70,"A",IF(E3&gt;=60,"A-",IF(E3&gt;=50,"B",IF(E3&gt;=40,"C",IF(E3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q3" s="4">
-        <f>IF(F3/200*100&gt;=80,"A+",IF(F3/200*100&gt;=70,"A",IF(F3/200*100&gt;=60,"A-",IF(F3/200*100&gt;=50,"B",IF(F3/200*100&gt;=40,"C",IF(F3/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R3" s="4">
-        <f>IF(G3/200*100&gt;=80,"A+",IF(G3/200*100&gt;=70,"A",IF(G3/200*100&gt;=60,"A-",IF(G3/200*100&gt;=50,"B",IF(G3/200*100&gt;=40,"C",IF(G3/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S3" s="4">
-        <f>IF(H3&gt;=80,"A+",IF(H3&gt;=70,"A",IF(H3&gt;=60,"A-",IF(H3&gt;=50,"B",IF(H3&gt;=40,"C",IF(H3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T3" s="4">
-        <f>IF(I3&gt;=80,"A+",IF(I3&gt;=70,"A",IF(I3&gt;=60,"A-",IF(I3&gt;=50,"B",IF(I3&gt;=40,"C",IF(I3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U3" s="4">
-        <f>IF(J3&gt;=80,"A+",IF(J3&gt;=70,"A",IF(J3&gt;=60,"A-",IF(J3&gt;=50,"B",IF(J3&gt;=40,"C",IF(J3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V3" s="4">
-        <f>IF(K3&gt;=80,"A+",IF(K3&gt;=70,"A",IF(K3&gt;=60,"A-",IF(K3&gt;=50,"B",IF(K3&gt;=40,"C",IF(K3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W3" s="4">
-        <f>IF(L3&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X3" s="4">
-        <f>IF(M3&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y3">
-        <f>SUM(C3:J3)</f>
-        <v/>
-      </c>
-      <c r="Z3" s="5">
-        <f>ROUND(Y3/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA3" s="6">
+        <f>ROUND(N3/8,2)</f>
+        <v/>
+      </c>
+      <c r="P3" s="5">
         <f>IF(OR(C3&lt;66,D3&lt;66,E3&lt;33,F3&lt;66,G3&lt;66,H3&lt;33,I3&lt;33,J3&lt;33,L3&lt;33,M3&lt;33),0,MIN(5,ROUND((IF(C3/200*100&gt;=80,5,IF(C3/200*100&gt;=70,4,IF(C3/200*100&gt;=60,3.5,IF(C3/200*100&gt;=50,3,IF(C3/200*100&gt;=40,2,IF(C3/200*100&gt;=33,1,0))))))+IF(D3/200*100&gt;=80,5,IF(D3/200*100&gt;=70,4,IF(D3/200*100&gt;=60,3.5,IF(D3/200*100&gt;=50,3,IF(D3/200*100&gt;=40,2,IF(D3/200*100&gt;=33,1,0))))))+IF(E3&gt;=80,5,IF(E3&gt;=70,4,IF(E3&gt;=60,3.5,IF(E3&gt;=50,3,IF(E3&gt;=40,2,IF(E3&gt;=33,1,0))))))+IF(F3/200*100&gt;=80,5,IF(F3/200*100&gt;=70,4,IF(F3/200*100&gt;=60,3.5,IF(F3/200*100&gt;=50,3,IF(F3/200*100&gt;=40,2,IF(F3/200*100&gt;=33,1,0))))))+IF(G3/200*100&gt;=80,5,IF(G3/200*100&gt;=70,4,IF(G3/200*100&gt;=60,3.5,IF(G3/200*100&gt;=50,3,IF(G3/200*100&gt;=40,2,IF(G3/200*100&gt;=33,1,0))))))+IF(H3&gt;=80,5,IF(H3&gt;=70,4,IF(H3&gt;=60,3.5,IF(H3&gt;=50,3,IF(H3&gt;=40,2,IF(H3&gt;=33,1,0))))))+IF(I3&gt;=80,5,IF(I3&gt;=70,4,IF(I3&gt;=60,3.5,IF(I3&gt;=50,3,IF(I3&gt;=40,2,IF(I3&gt;=33,1,0))))))+IF(J3&gt;=80,5,IF(J3&gt;=70,4,IF(J3&gt;=60,3.5,IF(J3&gt;=50,3,IF(J3&gt;=40,2,IF(J3&gt;=33,1,0)))))))/8+IF(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))&gt;=2,(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB3" s="4">
-        <f>IF(AA3&gt;=5,"A+",IF(AA3&gt;=4,"A",IF(AA3&gt;=3.5,"A-",IF(AA3&gt;=3,"B",IF(AA3&gt;=2,"C",IF(AA3&gt;=1,"D","F"))))))</f>
+      <c r="Q3" s="6">
+        <f>IF(P3&gt;=5,"A+",IF(P3&gt;=4,"A",IF(P3&gt;=3.5,"A-",IF(P3&gt;=3,"B",IF(P3&gt;=2,"C",IF(P3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1142,64 +1016,20 @@
       <c r="M4" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="N4" s="4">
-        <f>IF(C4/200*100&gt;=80,"A+",IF(C4/200*100&gt;=70,"A",IF(C4/200*100&gt;=60,"A-",IF(C4/200*100&gt;=50,"B",IF(C4/200*100&gt;=40,"C",IF(C4/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N4">
+        <f>SUM(C4:J4)</f>
         <v/>
       </c>
       <c r="O4" s="4">
-        <f>IF(D4/200*100&gt;=80,"A+",IF(D4/200*100&gt;=70,"A",IF(D4/200*100&gt;=60,"A-",IF(D4/200*100&gt;=50,"B",IF(D4/200*100&gt;=40,"C",IF(D4/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P4" s="4">
-        <f>IF(E4&gt;=80,"A+",IF(E4&gt;=70,"A",IF(E4&gt;=60,"A-",IF(E4&gt;=50,"B",IF(E4&gt;=40,"C",IF(E4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="4">
-        <f>IF(F4/200*100&gt;=80,"A+",IF(F4/200*100&gt;=70,"A",IF(F4/200*100&gt;=60,"A-",IF(F4/200*100&gt;=50,"B",IF(F4/200*100&gt;=40,"C",IF(F4/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R4" s="4">
-        <f>IF(G4/200*100&gt;=80,"A+",IF(G4/200*100&gt;=70,"A",IF(G4/200*100&gt;=60,"A-",IF(G4/200*100&gt;=50,"B",IF(G4/200*100&gt;=40,"C",IF(G4/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S4" s="4">
-        <f>IF(H4&gt;=80,"A+",IF(H4&gt;=70,"A",IF(H4&gt;=60,"A-",IF(H4&gt;=50,"B",IF(H4&gt;=40,"C",IF(H4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T4" s="4">
-        <f>IF(I4&gt;=80,"A+",IF(I4&gt;=70,"A",IF(I4&gt;=60,"A-",IF(I4&gt;=50,"B",IF(I4&gt;=40,"C",IF(I4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U4" s="4">
-        <f>IF(J4&gt;=80,"A+",IF(J4&gt;=70,"A",IF(J4&gt;=60,"A-",IF(J4&gt;=50,"B",IF(J4&gt;=40,"C",IF(J4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V4" s="4">
-        <f>IF(K4&gt;=80,"A+",IF(K4&gt;=70,"A",IF(K4&gt;=60,"A-",IF(K4&gt;=50,"B",IF(K4&gt;=40,"C",IF(K4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W4" s="4">
-        <f>IF(L4&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X4" s="4">
-        <f>IF(M4&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y4">
-        <f>SUM(C4:J4)</f>
-        <v/>
-      </c>
-      <c r="Z4" s="5">
-        <f>ROUND(Y4/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA4" s="6">
+        <f>ROUND(N4/8,2)</f>
+        <v/>
+      </c>
+      <c r="P4" s="5">
         <f>IF(OR(C4&lt;66,D4&lt;66,E4&lt;33,F4&lt;66,G4&lt;66,H4&lt;33,I4&lt;33,J4&lt;33,L4&lt;33,M4&lt;33),0,MIN(5,ROUND((IF(C4/200*100&gt;=80,5,IF(C4/200*100&gt;=70,4,IF(C4/200*100&gt;=60,3.5,IF(C4/200*100&gt;=50,3,IF(C4/200*100&gt;=40,2,IF(C4/200*100&gt;=33,1,0))))))+IF(D4/200*100&gt;=80,5,IF(D4/200*100&gt;=70,4,IF(D4/200*100&gt;=60,3.5,IF(D4/200*100&gt;=50,3,IF(D4/200*100&gt;=40,2,IF(D4/200*100&gt;=33,1,0))))))+IF(E4&gt;=80,5,IF(E4&gt;=70,4,IF(E4&gt;=60,3.5,IF(E4&gt;=50,3,IF(E4&gt;=40,2,IF(E4&gt;=33,1,0))))))+IF(F4/200*100&gt;=80,5,IF(F4/200*100&gt;=70,4,IF(F4/200*100&gt;=60,3.5,IF(F4/200*100&gt;=50,3,IF(F4/200*100&gt;=40,2,IF(F4/200*100&gt;=33,1,0))))))+IF(G4/200*100&gt;=80,5,IF(G4/200*100&gt;=70,4,IF(G4/200*100&gt;=60,3.5,IF(G4/200*100&gt;=50,3,IF(G4/200*100&gt;=40,2,IF(G4/200*100&gt;=33,1,0))))))+IF(H4&gt;=80,5,IF(H4&gt;=70,4,IF(H4&gt;=60,3.5,IF(H4&gt;=50,3,IF(H4&gt;=40,2,IF(H4&gt;=33,1,0))))))+IF(I4&gt;=80,5,IF(I4&gt;=70,4,IF(I4&gt;=60,3.5,IF(I4&gt;=50,3,IF(I4&gt;=40,2,IF(I4&gt;=33,1,0))))))+IF(J4&gt;=80,5,IF(J4&gt;=70,4,IF(J4&gt;=60,3.5,IF(J4&gt;=50,3,IF(J4&gt;=40,2,IF(J4&gt;=33,1,0)))))))/8+IF(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))&gt;=2,(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB4" s="4">
-        <f>IF(AA4&gt;=5,"A+",IF(AA4&gt;=4,"A",IF(AA4&gt;=3.5,"A-",IF(AA4&gt;=3,"B",IF(AA4&gt;=2,"C",IF(AA4&gt;=1,"D","F"))))))</f>
+      <c r="Q4" s="6">
+        <f>IF(P4&gt;=5,"A+",IF(P4&gt;=4,"A",IF(P4&gt;=3.5,"A-",IF(P4&gt;=3,"B",IF(P4&gt;=2,"C",IF(P4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1245,64 +1075,20 @@
       <c r="M5" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="N5" s="4">
-        <f>IF(C5/200*100&gt;=80,"A+",IF(C5/200*100&gt;=70,"A",IF(C5/200*100&gt;=60,"A-",IF(C5/200*100&gt;=50,"B",IF(C5/200*100&gt;=40,"C",IF(C5/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N5">
+        <f>SUM(C5:J5)</f>
         <v/>
       </c>
       <c r="O5" s="4">
-        <f>IF(D5/200*100&gt;=80,"A+",IF(D5/200*100&gt;=70,"A",IF(D5/200*100&gt;=60,"A-",IF(D5/200*100&gt;=50,"B",IF(D5/200*100&gt;=40,"C",IF(D5/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P5" s="4">
-        <f>IF(E5&gt;=80,"A+",IF(E5&gt;=70,"A",IF(E5&gt;=60,"A-",IF(E5&gt;=50,"B",IF(E5&gt;=40,"C",IF(E5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="4">
-        <f>IF(F5/200*100&gt;=80,"A+",IF(F5/200*100&gt;=70,"A",IF(F5/200*100&gt;=60,"A-",IF(F5/200*100&gt;=50,"B",IF(F5/200*100&gt;=40,"C",IF(F5/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R5" s="4">
-        <f>IF(G5/200*100&gt;=80,"A+",IF(G5/200*100&gt;=70,"A",IF(G5/200*100&gt;=60,"A-",IF(G5/200*100&gt;=50,"B",IF(G5/200*100&gt;=40,"C",IF(G5/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S5" s="4">
-        <f>IF(H5&gt;=80,"A+",IF(H5&gt;=70,"A",IF(H5&gt;=60,"A-",IF(H5&gt;=50,"B",IF(H5&gt;=40,"C",IF(H5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T5" s="4">
-        <f>IF(I5&gt;=80,"A+",IF(I5&gt;=70,"A",IF(I5&gt;=60,"A-",IF(I5&gt;=50,"B",IF(I5&gt;=40,"C",IF(I5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U5" s="4">
-        <f>IF(J5&gt;=80,"A+",IF(J5&gt;=70,"A",IF(J5&gt;=60,"A-",IF(J5&gt;=50,"B",IF(J5&gt;=40,"C",IF(J5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V5" s="4">
-        <f>IF(K5&gt;=80,"A+",IF(K5&gt;=70,"A",IF(K5&gt;=60,"A-",IF(K5&gt;=50,"B",IF(K5&gt;=40,"C",IF(K5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W5" s="4">
-        <f>IF(L5&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X5" s="4">
-        <f>IF(M5&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y5">
-        <f>SUM(C5:J5)</f>
-        <v/>
-      </c>
-      <c r="Z5" s="5">
-        <f>ROUND(Y5/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA5" s="6">
+        <f>ROUND(N5/8,2)</f>
+        <v/>
+      </c>
+      <c r="P5" s="5">
         <f>IF(OR(C5&lt;66,D5&lt;66,E5&lt;33,F5&lt;66,G5&lt;66,H5&lt;33,I5&lt;33,J5&lt;33,L5&lt;33,M5&lt;33),0,MIN(5,ROUND((IF(C5/200*100&gt;=80,5,IF(C5/200*100&gt;=70,4,IF(C5/200*100&gt;=60,3.5,IF(C5/200*100&gt;=50,3,IF(C5/200*100&gt;=40,2,IF(C5/200*100&gt;=33,1,0))))))+IF(D5/200*100&gt;=80,5,IF(D5/200*100&gt;=70,4,IF(D5/200*100&gt;=60,3.5,IF(D5/200*100&gt;=50,3,IF(D5/200*100&gt;=40,2,IF(D5/200*100&gt;=33,1,0))))))+IF(E5&gt;=80,5,IF(E5&gt;=70,4,IF(E5&gt;=60,3.5,IF(E5&gt;=50,3,IF(E5&gt;=40,2,IF(E5&gt;=33,1,0))))))+IF(F5/200*100&gt;=80,5,IF(F5/200*100&gt;=70,4,IF(F5/200*100&gt;=60,3.5,IF(F5/200*100&gt;=50,3,IF(F5/200*100&gt;=40,2,IF(F5/200*100&gt;=33,1,0))))))+IF(G5/200*100&gt;=80,5,IF(G5/200*100&gt;=70,4,IF(G5/200*100&gt;=60,3.5,IF(G5/200*100&gt;=50,3,IF(G5/200*100&gt;=40,2,IF(G5/200*100&gt;=33,1,0))))))+IF(H5&gt;=80,5,IF(H5&gt;=70,4,IF(H5&gt;=60,3.5,IF(H5&gt;=50,3,IF(H5&gt;=40,2,IF(H5&gt;=33,1,0))))))+IF(I5&gt;=80,5,IF(I5&gt;=70,4,IF(I5&gt;=60,3.5,IF(I5&gt;=50,3,IF(I5&gt;=40,2,IF(I5&gt;=33,1,0))))))+IF(J5&gt;=80,5,IF(J5&gt;=70,4,IF(J5&gt;=60,3.5,IF(J5&gt;=50,3,IF(J5&gt;=40,2,IF(J5&gt;=33,1,0)))))))/8+IF(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))&gt;=2,(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB5" s="4">
-        <f>IF(AA5&gt;=5,"A+",IF(AA5&gt;=4,"A",IF(AA5&gt;=3.5,"A-",IF(AA5&gt;=3,"B",IF(AA5&gt;=2,"C",IF(AA5&gt;=1,"D","F"))))))</f>
+      <c r="Q5" s="6">
+        <f>IF(P5&gt;=5,"A+",IF(P5&gt;=4,"A",IF(P5&gt;=3.5,"A-",IF(P5&gt;=3,"B",IF(P5&gt;=2,"C",IF(P5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1348,64 +1134,20 @@
       <c r="M6" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="N6" s="4">
-        <f>IF(C6/200*100&gt;=80,"A+",IF(C6/200*100&gt;=70,"A",IF(C6/200*100&gt;=60,"A-",IF(C6/200*100&gt;=50,"B",IF(C6/200*100&gt;=40,"C",IF(C6/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N6">
+        <f>SUM(C6:J6)</f>
         <v/>
       </c>
       <c r="O6" s="4">
-        <f>IF(D6/200*100&gt;=80,"A+",IF(D6/200*100&gt;=70,"A",IF(D6/200*100&gt;=60,"A-",IF(D6/200*100&gt;=50,"B",IF(D6/200*100&gt;=40,"C",IF(D6/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P6" s="4">
-        <f>IF(E6&gt;=80,"A+",IF(E6&gt;=70,"A",IF(E6&gt;=60,"A-",IF(E6&gt;=50,"B",IF(E6&gt;=40,"C",IF(E6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q6" s="4">
-        <f>IF(F6/200*100&gt;=80,"A+",IF(F6/200*100&gt;=70,"A",IF(F6/200*100&gt;=60,"A-",IF(F6/200*100&gt;=50,"B",IF(F6/200*100&gt;=40,"C",IF(F6/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R6" s="4">
-        <f>IF(G6/200*100&gt;=80,"A+",IF(G6/200*100&gt;=70,"A",IF(G6/200*100&gt;=60,"A-",IF(G6/200*100&gt;=50,"B",IF(G6/200*100&gt;=40,"C",IF(G6/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S6" s="4">
-        <f>IF(H6&gt;=80,"A+",IF(H6&gt;=70,"A",IF(H6&gt;=60,"A-",IF(H6&gt;=50,"B",IF(H6&gt;=40,"C",IF(H6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T6" s="4">
-        <f>IF(I6&gt;=80,"A+",IF(I6&gt;=70,"A",IF(I6&gt;=60,"A-",IF(I6&gt;=50,"B",IF(I6&gt;=40,"C",IF(I6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U6" s="4">
-        <f>IF(J6&gt;=80,"A+",IF(J6&gt;=70,"A",IF(J6&gt;=60,"A-",IF(J6&gt;=50,"B",IF(J6&gt;=40,"C",IF(J6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V6" s="4">
-        <f>IF(K6&gt;=80,"A+",IF(K6&gt;=70,"A",IF(K6&gt;=60,"A-",IF(K6&gt;=50,"B",IF(K6&gt;=40,"C",IF(K6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W6" s="4">
-        <f>IF(L6&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X6" s="4">
-        <f>IF(M6&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y6">
-        <f>SUM(C6:J6)</f>
-        <v/>
-      </c>
-      <c r="Z6" s="5">
-        <f>ROUND(Y6/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA6" s="6">
+        <f>ROUND(N6/8,2)</f>
+        <v/>
+      </c>
+      <c r="P6" s="5">
         <f>IF(OR(C6&lt;66,D6&lt;66,E6&lt;33,F6&lt;66,G6&lt;66,H6&lt;33,I6&lt;33,J6&lt;33,L6&lt;33,M6&lt;33),0,MIN(5,ROUND((IF(C6/200*100&gt;=80,5,IF(C6/200*100&gt;=70,4,IF(C6/200*100&gt;=60,3.5,IF(C6/200*100&gt;=50,3,IF(C6/200*100&gt;=40,2,IF(C6/200*100&gt;=33,1,0))))))+IF(D6/200*100&gt;=80,5,IF(D6/200*100&gt;=70,4,IF(D6/200*100&gt;=60,3.5,IF(D6/200*100&gt;=50,3,IF(D6/200*100&gt;=40,2,IF(D6/200*100&gt;=33,1,0))))))+IF(E6&gt;=80,5,IF(E6&gt;=70,4,IF(E6&gt;=60,3.5,IF(E6&gt;=50,3,IF(E6&gt;=40,2,IF(E6&gt;=33,1,0))))))+IF(F6/200*100&gt;=80,5,IF(F6/200*100&gt;=70,4,IF(F6/200*100&gt;=60,3.5,IF(F6/200*100&gt;=50,3,IF(F6/200*100&gt;=40,2,IF(F6/200*100&gt;=33,1,0))))))+IF(G6/200*100&gt;=80,5,IF(G6/200*100&gt;=70,4,IF(G6/200*100&gt;=60,3.5,IF(G6/200*100&gt;=50,3,IF(G6/200*100&gt;=40,2,IF(G6/200*100&gt;=33,1,0))))))+IF(H6&gt;=80,5,IF(H6&gt;=70,4,IF(H6&gt;=60,3.5,IF(H6&gt;=50,3,IF(H6&gt;=40,2,IF(H6&gt;=33,1,0))))))+IF(I6&gt;=80,5,IF(I6&gt;=70,4,IF(I6&gt;=60,3.5,IF(I6&gt;=50,3,IF(I6&gt;=40,2,IF(I6&gt;=33,1,0))))))+IF(J6&gt;=80,5,IF(J6&gt;=70,4,IF(J6&gt;=60,3.5,IF(J6&gt;=50,3,IF(J6&gt;=40,2,IF(J6&gt;=33,1,0)))))))/8+IF(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))&gt;=2,(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB6" s="4">
-        <f>IF(AA6&gt;=5,"A+",IF(AA6&gt;=4,"A",IF(AA6&gt;=3.5,"A-",IF(AA6&gt;=3,"B",IF(AA6&gt;=2,"C",IF(AA6&gt;=1,"D","F"))))))</f>
+      <c r="Q6" s="6">
+        <f>IF(P6&gt;=5,"A+",IF(P6&gt;=4,"A",IF(P6&gt;=3.5,"A-",IF(P6&gt;=3,"B",IF(P6&gt;=2,"C",IF(P6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1451,64 +1193,20 @@
       <c r="M7" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="N7" s="4">
-        <f>IF(C7/200*100&gt;=80,"A+",IF(C7/200*100&gt;=70,"A",IF(C7/200*100&gt;=60,"A-",IF(C7/200*100&gt;=50,"B",IF(C7/200*100&gt;=40,"C",IF(C7/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N7">
+        <f>SUM(C7:J7)</f>
         <v/>
       </c>
       <c r="O7" s="4">
-        <f>IF(D7/200*100&gt;=80,"A+",IF(D7/200*100&gt;=70,"A",IF(D7/200*100&gt;=60,"A-",IF(D7/200*100&gt;=50,"B",IF(D7/200*100&gt;=40,"C",IF(D7/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P7" s="4">
-        <f>IF(E7&gt;=80,"A+",IF(E7&gt;=70,"A",IF(E7&gt;=60,"A-",IF(E7&gt;=50,"B",IF(E7&gt;=40,"C",IF(E7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="4">
-        <f>IF(F7/200*100&gt;=80,"A+",IF(F7/200*100&gt;=70,"A",IF(F7/200*100&gt;=60,"A-",IF(F7/200*100&gt;=50,"B",IF(F7/200*100&gt;=40,"C",IF(F7/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R7" s="4">
-        <f>IF(G7/200*100&gt;=80,"A+",IF(G7/200*100&gt;=70,"A",IF(G7/200*100&gt;=60,"A-",IF(G7/200*100&gt;=50,"B",IF(G7/200*100&gt;=40,"C",IF(G7/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S7" s="4">
-        <f>IF(H7&gt;=80,"A+",IF(H7&gt;=70,"A",IF(H7&gt;=60,"A-",IF(H7&gt;=50,"B",IF(H7&gt;=40,"C",IF(H7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T7" s="4">
-        <f>IF(I7&gt;=80,"A+",IF(I7&gt;=70,"A",IF(I7&gt;=60,"A-",IF(I7&gt;=50,"B",IF(I7&gt;=40,"C",IF(I7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U7" s="4">
-        <f>IF(J7&gt;=80,"A+",IF(J7&gt;=70,"A",IF(J7&gt;=60,"A-",IF(J7&gt;=50,"B",IF(J7&gt;=40,"C",IF(J7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V7" s="4">
-        <f>IF(K7&gt;=80,"A+",IF(K7&gt;=70,"A",IF(K7&gt;=60,"A-",IF(K7&gt;=50,"B",IF(K7&gt;=40,"C",IF(K7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W7" s="4">
-        <f>IF(L7&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X7" s="4">
-        <f>IF(M7&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y7">
-        <f>SUM(C7:J7)</f>
-        <v/>
-      </c>
-      <c r="Z7" s="5">
-        <f>ROUND(Y7/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA7" s="6">
+        <f>ROUND(N7/8,2)</f>
+        <v/>
+      </c>
+      <c r="P7" s="5">
         <f>IF(OR(C7&lt;66,D7&lt;66,E7&lt;33,F7&lt;66,G7&lt;66,H7&lt;33,I7&lt;33,J7&lt;33,L7&lt;33,M7&lt;33),0,MIN(5,ROUND((IF(C7/200*100&gt;=80,5,IF(C7/200*100&gt;=70,4,IF(C7/200*100&gt;=60,3.5,IF(C7/200*100&gt;=50,3,IF(C7/200*100&gt;=40,2,IF(C7/200*100&gt;=33,1,0))))))+IF(D7/200*100&gt;=80,5,IF(D7/200*100&gt;=70,4,IF(D7/200*100&gt;=60,3.5,IF(D7/200*100&gt;=50,3,IF(D7/200*100&gt;=40,2,IF(D7/200*100&gt;=33,1,0))))))+IF(E7&gt;=80,5,IF(E7&gt;=70,4,IF(E7&gt;=60,3.5,IF(E7&gt;=50,3,IF(E7&gt;=40,2,IF(E7&gt;=33,1,0))))))+IF(F7/200*100&gt;=80,5,IF(F7/200*100&gt;=70,4,IF(F7/200*100&gt;=60,3.5,IF(F7/200*100&gt;=50,3,IF(F7/200*100&gt;=40,2,IF(F7/200*100&gt;=33,1,0))))))+IF(G7/200*100&gt;=80,5,IF(G7/200*100&gt;=70,4,IF(G7/200*100&gt;=60,3.5,IF(G7/200*100&gt;=50,3,IF(G7/200*100&gt;=40,2,IF(G7/200*100&gt;=33,1,0))))))+IF(H7&gt;=80,5,IF(H7&gt;=70,4,IF(H7&gt;=60,3.5,IF(H7&gt;=50,3,IF(H7&gt;=40,2,IF(H7&gt;=33,1,0))))))+IF(I7&gt;=80,5,IF(I7&gt;=70,4,IF(I7&gt;=60,3.5,IF(I7&gt;=50,3,IF(I7&gt;=40,2,IF(I7&gt;=33,1,0))))))+IF(J7&gt;=80,5,IF(J7&gt;=70,4,IF(J7&gt;=60,3.5,IF(J7&gt;=50,3,IF(J7&gt;=40,2,IF(J7&gt;=33,1,0)))))))/8+IF(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))&gt;=2,(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB7" s="4">
-        <f>IF(AA7&gt;=5,"A+",IF(AA7&gt;=4,"A",IF(AA7&gt;=3.5,"A-",IF(AA7&gt;=3,"B",IF(AA7&gt;=2,"C",IF(AA7&gt;=1,"D","F"))))))</f>
+      <c r="Q7" s="6">
+        <f>IF(P7&gt;=5,"A+",IF(P7&gt;=4,"A",IF(P7&gt;=3.5,"A-",IF(P7&gt;=3,"B",IF(P7&gt;=2,"C",IF(P7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1554,64 +1252,20 @@
       <c r="M8" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="N8" s="4">
-        <f>IF(C8/200*100&gt;=80,"A+",IF(C8/200*100&gt;=70,"A",IF(C8/200*100&gt;=60,"A-",IF(C8/200*100&gt;=50,"B",IF(C8/200*100&gt;=40,"C",IF(C8/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N8">
+        <f>SUM(C8:J8)</f>
         <v/>
       </c>
       <c r="O8" s="4">
-        <f>IF(D8/200*100&gt;=80,"A+",IF(D8/200*100&gt;=70,"A",IF(D8/200*100&gt;=60,"A-",IF(D8/200*100&gt;=50,"B",IF(D8/200*100&gt;=40,"C",IF(D8/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P8" s="4">
-        <f>IF(E8&gt;=80,"A+",IF(E8&gt;=70,"A",IF(E8&gt;=60,"A-",IF(E8&gt;=50,"B",IF(E8&gt;=40,"C",IF(E8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q8" s="4">
-        <f>IF(F8/200*100&gt;=80,"A+",IF(F8/200*100&gt;=70,"A",IF(F8/200*100&gt;=60,"A-",IF(F8/200*100&gt;=50,"B",IF(F8/200*100&gt;=40,"C",IF(F8/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R8" s="4">
-        <f>IF(G8/200*100&gt;=80,"A+",IF(G8/200*100&gt;=70,"A",IF(G8/200*100&gt;=60,"A-",IF(G8/200*100&gt;=50,"B",IF(G8/200*100&gt;=40,"C",IF(G8/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S8" s="4">
-        <f>IF(H8&gt;=80,"A+",IF(H8&gt;=70,"A",IF(H8&gt;=60,"A-",IF(H8&gt;=50,"B",IF(H8&gt;=40,"C",IF(H8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T8" s="4">
-        <f>IF(I8&gt;=80,"A+",IF(I8&gt;=70,"A",IF(I8&gt;=60,"A-",IF(I8&gt;=50,"B",IF(I8&gt;=40,"C",IF(I8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U8" s="4">
-        <f>IF(J8&gt;=80,"A+",IF(J8&gt;=70,"A",IF(J8&gt;=60,"A-",IF(J8&gt;=50,"B",IF(J8&gt;=40,"C",IF(J8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V8" s="4">
-        <f>IF(K8&gt;=80,"A+",IF(K8&gt;=70,"A",IF(K8&gt;=60,"A-",IF(K8&gt;=50,"B",IF(K8&gt;=40,"C",IF(K8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W8" s="4">
-        <f>IF(L8&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X8" s="4">
-        <f>IF(M8&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y8">
-        <f>SUM(C8:J8)</f>
-        <v/>
-      </c>
-      <c r="Z8" s="5">
-        <f>ROUND(Y8/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA8" s="6">
+        <f>ROUND(N8/8,2)</f>
+        <v/>
+      </c>
+      <c r="P8" s="5">
         <f>IF(OR(C8&lt;66,D8&lt;66,E8&lt;33,F8&lt;66,G8&lt;66,H8&lt;33,I8&lt;33,J8&lt;33,L8&lt;33,M8&lt;33),0,MIN(5,ROUND((IF(C8/200*100&gt;=80,5,IF(C8/200*100&gt;=70,4,IF(C8/200*100&gt;=60,3.5,IF(C8/200*100&gt;=50,3,IF(C8/200*100&gt;=40,2,IF(C8/200*100&gt;=33,1,0))))))+IF(D8/200*100&gt;=80,5,IF(D8/200*100&gt;=70,4,IF(D8/200*100&gt;=60,3.5,IF(D8/200*100&gt;=50,3,IF(D8/200*100&gt;=40,2,IF(D8/200*100&gt;=33,1,0))))))+IF(E8&gt;=80,5,IF(E8&gt;=70,4,IF(E8&gt;=60,3.5,IF(E8&gt;=50,3,IF(E8&gt;=40,2,IF(E8&gt;=33,1,0))))))+IF(F8/200*100&gt;=80,5,IF(F8/200*100&gt;=70,4,IF(F8/200*100&gt;=60,3.5,IF(F8/200*100&gt;=50,3,IF(F8/200*100&gt;=40,2,IF(F8/200*100&gt;=33,1,0))))))+IF(G8/200*100&gt;=80,5,IF(G8/200*100&gt;=70,4,IF(G8/200*100&gt;=60,3.5,IF(G8/200*100&gt;=50,3,IF(G8/200*100&gt;=40,2,IF(G8/200*100&gt;=33,1,0))))))+IF(H8&gt;=80,5,IF(H8&gt;=70,4,IF(H8&gt;=60,3.5,IF(H8&gt;=50,3,IF(H8&gt;=40,2,IF(H8&gt;=33,1,0))))))+IF(I8&gt;=80,5,IF(I8&gt;=70,4,IF(I8&gt;=60,3.5,IF(I8&gt;=50,3,IF(I8&gt;=40,2,IF(I8&gt;=33,1,0))))))+IF(J8&gt;=80,5,IF(J8&gt;=70,4,IF(J8&gt;=60,3.5,IF(J8&gt;=50,3,IF(J8&gt;=40,2,IF(J8&gt;=33,1,0)))))))/8+IF(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))&gt;=2,(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB8" s="4">
-        <f>IF(AA8&gt;=5,"A+",IF(AA8&gt;=4,"A",IF(AA8&gt;=3.5,"A-",IF(AA8&gt;=3,"B",IF(AA8&gt;=2,"C",IF(AA8&gt;=1,"D","F"))))))</f>
+      <c r="Q8" s="6">
+        <f>IF(P8&gt;=5,"A+",IF(P8&gt;=4,"A",IF(P8&gt;=3.5,"A-",IF(P8&gt;=3,"B",IF(P8&gt;=2,"C",IF(P8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1657,64 +1311,20 @@
       <c r="M9" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="N9" s="4">
-        <f>IF(C9/200*100&gt;=80,"A+",IF(C9/200*100&gt;=70,"A",IF(C9/200*100&gt;=60,"A-",IF(C9/200*100&gt;=50,"B",IF(C9/200*100&gt;=40,"C",IF(C9/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N9">
+        <f>SUM(C9:J9)</f>
         <v/>
       </c>
       <c r="O9" s="4">
-        <f>IF(D9/200*100&gt;=80,"A+",IF(D9/200*100&gt;=70,"A",IF(D9/200*100&gt;=60,"A-",IF(D9/200*100&gt;=50,"B",IF(D9/200*100&gt;=40,"C",IF(D9/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P9" s="4">
-        <f>IF(E9&gt;=80,"A+",IF(E9&gt;=70,"A",IF(E9&gt;=60,"A-",IF(E9&gt;=50,"B",IF(E9&gt;=40,"C",IF(E9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="4">
-        <f>IF(F9/200*100&gt;=80,"A+",IF(F9/200*100&gt;=70,"A",IF(F9/200*100&gt;=60,"A-",IF(F9/200*100&gt;=50,"B",IF(F9/200*100&gt;=40,"C",IF(F9/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R9" s="4">
-        <f>IF(G9/200*100&gt;=80,"A+",IF(G9/200*100&gt;=70,"A",IF(G9/200*100&gt;=60,"A-",IF(G9/200*100&gt;=50,"B",IF(G9/200*100&gt;=40,"C",IF(G9/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S9" s="4">
-        <f>IF(H9&gt;=80,"A+",IF(H9&gt;=70,"A",IF(H9&gt;=60,"A-",IF(H9&gt;=50,"B",IF(H9&gt;=40,"C",IF(H9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T9" s="4">
-        <f>IF(I9&gt;=80,"A+",IF(I9&gt;=70,"A",IF(I9&gt;=60,"A-",IF(I9&gt;=50,"B",IF(I9&gt;=40,"C",IF(I9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U9" s="4">
-        <f>IF(J9&gt;=80,"A+",IF(J9&gt;=70,"A",IF(J9&gt;=60,"A-",IF(J9&gt;=50,"B",IF(J9&gt;=40,"C",IF(J9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V9" s="4">
-        <f>IF(K9&gt;=80,"A+",IF(K9&gt;=70,"A",IF(K9&gt;=60,"A-",IF(K9&gt;=50,"B",IF(K9&gt;=40,"C",IF(K9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W9" s="4">
-        <f>IF(L9&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X9" s="4">
-        <f>IF(M9&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y9">
-        <f>SUM(C9:J9)</f>
-        <v/>
-      </c>
-      <c r="Z9" s="5">
-        <f>ROUND(Y9/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA9" s="6">
+        <f>ROUND(N9/8,2)</f>
+        <v/>
+      </c>
+      <c r="P9" s="5">
         <f>IF(OR(C9&lt;66,D9&lt;66,E9&lt;33,F9&lt;66,G9&lt;66,H9&lt;33,I9&lt;33,J9&lt;33,L9&lt;33,M9&lt;33),0,MIN(5,ROUND((IF(C9/200*100&gt;=80,5,IF(C9/200*100&gt;=70,4,IF(C9/200*100&gt;=60,3.5,IF(C9/200*100&gt;=50,3,IF(C9/200*100&gt;=40,2,IF(C9/200*100&gt;=33,1,0))))))+IF(D9/200*100&gt;=80,5,IF(D9/200*100&gt;=70,4,IF(D9/200*100&gt;=60,3.5,IF(D9/200*100&gt;=50,3,IF(D9/200*100&gt;=40,2,IF(D9/200*100&gt;=33,1,0))))))+IF(E9&gt;=80,5,IF(E9&gt;=70,4,IF(E9&gt;=60,3.5,IF(E9&gt;=50,3,IF(E9&gt;=40,2,IF(E9&gt;=33,1,0))))))+IF(F9/200*100&gt;=80,5,IF(F9/200*100&gt;=70,4,IF(F9/200*100&gt;=60,3.5,IF(F9/200*100&gt;=50,3,IF(F9/200*100&gt;=40,2,IF(F9/200*100&gt;=33,1,0))))))+IF(G9/200*100&gt;=80,5,IF(G9/200*100&gt;=70,4,IF(G9/200*100&gt;=60,3.5,IF(G9/200*100&gt;=50,3,IF(G9/200*100&gt;=40,2,IF(G9/200*100&gt;=33,1,0))))))+IF(H9&gt;=80,5,IF(H9&gt;=70,4,IF(H9&gt;=60,3.5,IF(H9&gt;=50,3,IF(H9&gt;=40,2,IF(H9&gt;=33,1,0))))))+IF(I9&gt;=80,5,IF(I9&gt;=70,4,IF(I9&gt;=60,3.5,IF(I9&gt;=50,3,IF(I9&gt;=40,2,IF(I9&gt;=33,1,0))))))+IF(J9&gt;=80,5,IF(J9&gt;=70,4,IF(J9&gt;=60,3.5,IF(J9&gt;=50,3,IF(J9&gt;=40,2,IF(J9&gt;=33,1,0)))))))/8+IF(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))&gt;=2,(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB9" s="4">
-        <f>IF(AA9&gt;=5,"A+",IF(AA9&gt;=4,"A",IF(AA9&gt;=3.5,"A-",IF(AA9&gt;=3,"B",IF(AA9&gt;=2,"C",IF(AA9&gt;=1,"D","F"))))))</f>
+      <c r="Q9" s="6">
+        <f>IF(P9&gt;=5,"A+",IF(P9&gt;=4,"A",IF(P9&gt;=3.5,"A-",IF(P9&gt;=3,"B",IF(P9&gt;=2,"C",IF(P9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1760,64 +1370,20 @@
       <c r="M10" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="N10" s="4">
-        <f>IF(C10/200*100&gt;=80,"A+",IF(C10/200*100&gt;=70,"A",IF(C10/200*100&gt;=60,"A-",IF(C10/200*100&gt;=50,"B",IF(C10/200*100&gt;=40,"C",IF(C10/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N10">
+        <f>SUM(C10:J10)</f>
         <v/>
       </c>
       <c r="O10" s="4">
-        <f>IF(D10/200*100&gt;=80,"A+",IF(D10/200*100&gt;=70,"A",IF(D10/200*100&gt;=60,"A-",IF(D10/200*100&gt;=50,"B",IF(D10/200*100&gt;=40,"C",IF(D10/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P10" s="4">
-        <f>IF(E10&gt;=80,"A+",IF(E10&gt;=70,"A",IF(E10&gt;=60,"A-",IF(E10&gt;=50,"B",IF(E10&gt;=40,"C",IF(E10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q10" s="4">
-        <f>IF(F10/200*100&gt;=80,"A+",IF(F10/200*100&gt;=70,"A",IF(F10/200*100&gt;=60,"A-",IF(F10/200*100&gt;=50,"B",IF(F10/200*100&gt;=40,"C",IF(F10/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R10" s="4">
-        <f>IF(G10/200*100&gt;=80,"A+",IF(G10/200*100&gt;=70,"A",IF(G10/200*100&gt;=60,"A-",IF(G10/200*100&gt;=50,"B",IF(G10/200*100&gt;=40,"C",IF(G10/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S10" s="4">
-        <f>IF(H10&gt;=80,"A+",IF(H10&gt;=70,"A",IF(H10&gt;=60,"A-",IF(H10&gt;=50,"B",IF(H10&gt;=40,"C",IF(H10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T10" s="4">
-        <f>IF(I10&gt;=80,"A+",IF(I10&gt;=70,"A",IF(I10&gt;=60,"A-",IF(I10&gt;=50,"B",IF(I10&gt;=40,"C",IF(I10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U10" s="4">
-        <f>IF(J10&gt;=80,"A+",IF(J10&gt;=70,"A",IF(J10&gt;=60,"A-",IF(J10&gt;=50,"B",IF(J10&gt;=40,"C",IF(J10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V10" s="4">
-        <f>IF(K10&gt;=80,"A+",IF(K10&gt;=70,"A",IF(K10&gt;=60,"A-",IF(K10&gt;=50,"B",IF(K10&gt;=40,"C",IF(K10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W10" s="4">
-        <f>IF(L10&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X10" s="4">
-        <f>IF(M10&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y10">
-        <f>SUM(C10:J10)</f>
-        <v/>
-      </c>
-      <c r="Z10" s="5">
-        <f>ROUND(Y10/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA10" s="6">
+        <f>ROUND(N10/8,2)</f>
+        <v/>
+      </c>
+      <c r="P10" s="5">
         <f>IF(OR(C10&lt;66,D10&lt;66,E10&lt;33,F10&lt;66,G10&lt;66,H10&lt;33,I10&lt;33,J10&lt;33,L10&lt;33,M10&lt;33),0,MIN(5,ROUND((IF(C10/200*100&gt;=80,5,IF(C10/200*100&gt;=70,4,IF(C10/200*100&gt;=60,3.5,IF(C10/200*100&gt;=50,3,IF(C10/200*100&gt;=40,2,IF(C10/200*100&gt;=33,1,0))))))+IF(D10/200*100&gt;=80,5,IF(D10/200*100&gt;=70,4,IF(D10/200*100&gt;=60,3.5,IF(D10/200*100&gt;=50,3,IF(D10/200*100&gt;=40,2,IF(D10/200*100&gt;=33,1,0))))))+IF(E10&gt;=80,5,IF(E10&gt;=70,4,IF(E10&gt;=60,3.5,IF(E10&gt;=50,3,IF(E10&gt;=40,2,IF(E10&gt;=33,1,0))))))+IF(F10/200*100&gt;=80,5,IF(F10/200*100&gt;=70,4,IF(F10/200*100&gt;=60,3.5,IF(F10/200*100&gt;=50,3,IF(F10/200*100&gt;=40,2,IF(F10/200*100&gt;=33,1,0))))))+IF(G10/200*100&gt;=80,5,IF(G10/200*100&gt;=70,4,IF(G10/200*100&gt;=60,3.5,IF(G10/200*100&gt;=50,3,IF(G10/200*100&gt;=40,2,IF(G10/200*100&gt;=33,1,0))))))+IF(H10&gt;=80,5,IF(H10&gt;=70,4,IF(H10&gt;=60,3.5,IF(H10&gt;=50,3,IF(H10&gt;=40,2,IF(H10&gt;=33,1,0))))))+IF(I10&gt;=80,5,IF(I10&gt;=70,4,IF(I10&gt;=60,3.5,IF(I10&gt;=50,3,IF(I10&gt;=40,2,IF(I10&gt;=33,1,0))))))+IF(J10&gt;=80,5,IF(J10&gt;=70,4,IF(J10&gt;=60,3.5,IF(J10&gt;=50,3,IF(J10&gt;=40,2,IF(J10&gt;=33,1,0)))))))/8+IF(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))&gt;=2,(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB10" s="4">
-        <f>IF(AA10&gt;=5,"A+",IF(AA10&gt;=4,"A",IF(AA10&gt;=3.5,"A-",IF(AA10&gt;=3,"B",IF(AA10&gt;=2,"C",IF(AA10&gt;=1,"D","F"))))))</f>
+      <c r="Q10" s="6">
+        <f>IF(P10&gt;=5,"A+",IF(P10&gt;=4,"A",IF(P10&gt;=3.5,"A-",IF(P10&gt;=3,"B",IF(P10&gt;=2,"C",IF(P10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1863,64 +1429,20 @@
       <c r="M11" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="N11" s="4">
-        <f>IF(C11/200*100&gt;=80,"A+",IF(C11/200*100&gt;=70,"A",IF(C11/200*100&gt;=60,"A-",IF(C11/200*100&gt;=50,"B",IF(C11/200*100&gt;=40,"C",IF(C11/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N11">
+        <f>SUM(C11:J11)</f>
         <v/>
       </c>
       <c r="O11" s="4">
-        <f>IF(D11/200*100&gt;=80,"A+",IF(D11/200*100&gt;=70,"A",IF(D11/200*100&gt;=60,"A-",IF(D11/200*100&gt;=50,"B",IF(D11/200*100&gt;=40,"C",IF(D11/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P11" s="4">
-        <f>IF(E11&gt;=80,"A+",IF(E11&gt;=70,"A",IF(E11&gt;=60,"A-",IF(E11&gt;=50,"B",IF(E11&gt;=40,"C",IF(E11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="4">
-        <f>IF(F11/200*100&gt;=80,"A+",IF(F11/200*100&gt;=70,"A",IF(F11/200*100&gt;=60,"A-",IF(F11/200*100&gt;=50,"B",IF(F11/200*100&gt;=40,"C",IF(F11/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R11" s="4">
-        <f>IF(G11/200*100&gt;=80,"A+",IF(G11/200*100&gt;=70,"A",IF(G11/200*100&gt;=60,"A-",IF(G11/200*100&gt;=50,"B",IF(G11/200*100&gt;=40,"C",IF(G11/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S11" s="4">
-        <f>IF(H11&gt;=80,"A+",IF(H11&gt;=70,"A",IF(H11&gt;=60,"A-",IF(H11&gt;=50,"B",IF(H11&gt;=40,"C",IF(H11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T11" s="4">
-        <f>IF(I11&gt;=80,"A+",IF(I11&gt;=70,"A",IF(I11&gt;=60,"A-",IF(I11&gt;=50,"B",IF(I11&gt;=40,"C",IF(I11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U11" s="4">
-        <f>IF(J11&gt;=80,"A+",IF(J11&gt;=70,"A",IF(J11&gt;=60,"A-",IF(J11&gt;=50,"B",IF(J11&gt;=40,"C",IF(J11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V11" s="4">
-        <f>IF(K11&gt;=80,"A+",IF(K11&gt;=70,"A",IF(K11&gt;=60,"A-",IF(K11&gt;=50,"B",IF(K11&gt;=40,"C",IF(K11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W11" s="4">
-        <f>IF(L11&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X11" s="4">
-        <f>IF(M11&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y11">
-        <f>SUM(C11:J11)</f>
-        <v/>
-      </c>
-      <c r="Z11" s="5">
-        <f>ROUND(Y11/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA11" s="6">
+        <f>ROUND(N11/8,2)</f>
+        <v/>
+      </c>
+      <c r="P11" s="5">
         <f>IF(OR(C11&lt;66,D11&lt;66,E11&lt;33,F11&lt;66,G11&lt;66,H11&lt;33,I11&lt;33,J11&lt;33,L11&lt;33,M11&lt;33),0,MIN(5,ROUND((IF(C11/200*100&gt;=80,5,IF(C11/200*100&gt;=70,4,IF(C11/200*100&gt;=60,3.5,IF(C11/200*100&gt;=50,3,IF(C11/200*100&gt;=40,2,IF(C11/200*100&gt;=33,1,0))))))+IF(D11/200*100&gt;=80,5,IF(D11/200*100&gt;=70,4,IF(D11/200*100&gt;=60,3.5,IF(D11/200*100&gt;=50,3,IF(D11/200*100&gt;=40,2,IF(D11/200*100&gt;=33,1,0))))))+IF(E11&gt;=80,5,IF(E11&gt;=70,4,IF(E11&gt;=60,3.5,IF(E11&gt;=50,3,IF(E11&gt;=40,2,IF(E11&gt;=33,1,0))))))+IF(F11/200*100&gt;=80,5,IF(F11/200*100&gt;=70,4,IF(F11/200*100&gt;=60,3.5,IF(F11/200*100&gt;=50,3,IF(F11/200*100&gt;=40,2,IF(F11/200*100&gt;=33,1,0))))))+IF(G11/200*100&gt;=80,5,IF(G11/200*100&gt;=70,4,IF(G11/200*100&gt;=60,3.5,IF(G11/200*100&gt;=50,3,IF(G11/200*100&gt;=40,2,IF(G11/200*100&gt;=33,1,0))))))+IF(H11&gt;=80,5,IF(H11&gt;=70,4,IF(H11&gt;=60,3.5,IF(H11&gt;=50,3,IF(H11&gt;=40,2,IF(H11&gt;=33,1,0))))))+IF(I11&gt;=80,5,IF(I11&gt;=70,4,IF(I11&gt;=60,3.5,IF(I11&gt;=50,3,IF(I11&gt;=40,2,IF(I11&gt;=33,1,0))))))+IF(J11&gt;=80,5,IF(J11&gt;=70,4,IF(J11&gt;=60,3.5,IF(J11&gt;=50,3,IF(J11&gt;=40,2,IF(J11&gt;=33,1,0)))))))/8+IF(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))&gt;=2,(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB11" s="4">
-        <f>IF(AA11&gt;=5,"A+",IF(AA11&gt;=4,"A",IF(AA11&gt;=3.5,"A-",IF(AA11&gt;=3,"B",IF(AA11&gt;=2,"C",IF(AA11&gt;=1,"D","F"))))))</f>
+      <c r="Q11" s="6">
+        <f>IF(P11&gt;=5,"A+",IF(P11&gt;=4,"A",IF(P11&gt;=3.5,"A-",IF(P11&gt;=3,"B",IF(P11&gt;=2,"C",IF(P11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1966,64 +1488,20 @@
       <c r="M12" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="N12" s="4">
-        <f>IF(C12/200*100&gt;=80,"A+",IF(C12/200*100&gt;=70,"A",IF(C12/200*100&gt;=60,"A-",IF(C12/200*100&gt;=50,"B",IF(C12/200*100&gt;=40,"C",IF(C12/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N12">
+        <f>SUM(C12:J12)</f>
         <v/>
       </c>
       <c r="O12" s="4">
-        <f>IF(D12/200*100&gt;=80,"A+",IF(D12/200*100&gt;=70,"A",IF(D12/200*100&gt;=60,"A-",IF(D12/200*100&gt;=50,"B",IF(D12/200*100&gt;=40,"C",IF(D12/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P12" s="4">
-        <f>IF(E12&gt;=80,"A+",IF(E12&gt;=70,"A",IF(E12&gt;=60,"A-",IF(E12&gt;=50,"B",IF(E12&gt;=40,"C",IF(E12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="4">
-        <f>IF(F12/200*100&gt;=80,"A+",IF(F12/200*100&gt;=70,"A",IF(F12/200*100&gt;=60,"A-",IF(F12/200*100&gt;=50,"B",IF(F12/200*100&gt;=40,"C",IF(F12/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R12" s="4">
-        <f>IF(G12/200*100&gt;=80,"A+",IF(G12/200*100&gt;=70,"A",IF(G12/200*100&gt;=60,"A-",IF(G12/200*100&gt;=50,"B",IF(G12/200*100&gt;=40,"C",IF(G12/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S12" s="4">
-        <f>IF(H12&gt;=80,"A+",IF(H12&gt;=70,"A",IF(H12&gt;=60,"A-",IF(H12&gt;=50,"B",IF(H12&gt;=40,"C",IF(H12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T12" s="4">
-        <f>IF(I12&gt;=80,"A+",IF(I12&gt;=70,"A",IF(I12&gt;=60,"A-",IF(I12&gt;=50,"B",IF(I12&gt;=40,"C",IF(I12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U12" s="4">
-        <f>IF(J12&gt;=80,"A+",IF(J12&gt;=70,"A",IF(J12&gt;=60,"A-",IF(J12&gt;=50,"B",IF(J12&gt;=40,"C",IF(J12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V12" s="4">
-        <f>IF(K12&gt;=80,"A+",IF(K12&gt;=70,"A",IF(K12&gt;=60,"A-",IF(K12&gt;=50,"B",IF(K12&gt;=40,"C",IF(K12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W12" s="4">
-        <f>IF(L12&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X12" s="4">
-        <f>IF(M12&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y12">
-        <f>SUM(C12:J12)</f>
-        <v/>
-      </c>
-      <c r="Z12" s="5">
-        <f>ROUND(Y12/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA12" s="6">
+        <f>ROUND(N12/8,2)</f>
+        <v/>
+      </c>
+      <c r="P12" s="5">
         <f>IF(OR(C12&lt;66,D12&lt;66,E12&lt;33,F12&lt;66,G12&lt;66,H12&lt;33,I12&lt;33,J12&lt;33,L12&lt;33,M12&lt;33),0,MIN(5,ROUND((IF(C12/200*100&gt;=80,5,IF(C12/200*100&gt;=70,4,IF(C12/200*100&gt;=60,3.5,IF(C12/200*100&gt;=50,3,IF(C12/200*100&gt;=40,2,IF(C12/200*100&gt;=33,1,0))))))+IF(D12/200*100&gt;=80,5,IF(D12/200*100&gt;=70,4,IF(D12/200*100&gt;=60,3.5,IF(D12/200*100&gt;=50,3,IF(D12/200*100&gt;=40,2,IF(D12/200*100&gt;=33,1,0))))))+IF(E12&gt;=80,5,IF(E12&gt;=70,4,IF(E12&gt;=60,3.5,IF(E12&gt;=50,3,IF(E12&gt;=40,2,IF(E12&gt;=33,1,0))))))+IF(F12/200*100&gt;=80,5,IF(F12/200*100&gt;=70,4,IF(F12/200*100&gt;=60,3.5,IF(F12/200*100&gt;=50,3,IF(F12/200*100&gt;=40,2,IF(F12/200*100&gt;=33,1,0))))))+IF(G12/200*100&gt;=80,5,IF(G12/200*100&gt;=70,4,IF(G12/200*100&gt;=60,3.5,IF(G12/200*100&gt;=50,3,IF(G12/200*100&gt;=40,2,IF(G12/200*100&gt;=33,1,0))))))+IF(H12&gt;=80,5,IF(H12&gt;=70,4,IF(H12&gt;=60,3.5,IF(H12&gt;=50,3,IF(H12&gt;=40,2,IF(H12&gt;=33,1,0))))))+IF(I12&gt;=80,5,IF(I12&gt;=70,4,IF(I12&gt;=60,3.5,IF(I12&gt;=50,3,IF(I12&gt;=40,2,IF(I12&gt;=33,1,0))))))+IF(J12&gt;=80,5,IF(J12&gt;=70,4,IF(J12&gt;=60,3.5,IF(J12&gt;=50,3,IF(J12&gt;=40,2,IF(J12&gt;=33,1,0)))))))/8+IF(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))&gt;=2,(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB12" s="4">
-        <f>IF(AA12&gt;=5,"A+",IF(AA12&gt;=4,"A",IF(AA12&gt;=3.5,"A-",IF(AA12&gt;=3,"B",IF(AA12&gt;=2,"C",IF(AA12&gt;=1,"D","F"))))))</f>
+      <c r="Q12" s="6">
+        <f>IF(P12&gt;=5,"A+",IF(P12&gt;=4,"A",IF(P12&gt;=3.5,"A-",IF(P12&gt;=3,"B",IF(P12&gt;=2,"C",IF(P12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2069,64 +1547,20 @@
       <c r="M13" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="N13" s="4">
-        <f>IF(C13/200*100&gt;=80,"A+",IF(C13/200*100&gt;=70,"A",IF(C13/200*100&gt;=60,"A-",IF(C13/200*100&gt;=50,"B",IF(C13/200*100&gt;=40,"C",IF(C13/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N13">
+        <f>SUM(C13:J13)</f>
         <v/>
       </c>
       <c r="O13" s="4">
-        <f>IF(D13/200*100&gt;=80,"A+",IF(D13/200*100&gt;=70,"A",IF(D13/200*100&gt;=60,"A-",IF(D13/200*100&gt;=50,"B",IF(D13/200*100&gt;=40,"C",IF(D13/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P13" s="4">
-        <f>IF(E13&gt;=80,"A+",IF(E13&gt;=70,"A",IF(E13&gt;=60,"A-",IF(E13&gt;=50,"B",IF(E13&gt;=40,"C",IF(E13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="4">
-        <f>IF(F13/200*100&gt;=80,"A+",IF(F13/200*100&gt;=70,"A",IF(F13/200*100&gt;=60,"A-",IF(F13/200*100&gt;=50,"B",IF(F13/200*100&gt;=40,"C",IF(F13/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R13" s="4">
-        <f>IF(G13/200*100&gt;=80,"A+",IF(G13/200*100&gt;=70,"A",IF(G13/200*100&gt;=60,"A-",IF(G13/200*100&gt;=50,"B",IF(G13/200*100&gt;=40,"C",IF(G13/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S13" s="4">
-        <f>IF(H13&gt;=80,"A+",IF(H13&gt;=70,"A",IF(H13&gt;=60,"A-",IF(H13&gt;=50,"B",IF(H13&gt;=40,"C",IF(H13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T13" s="4">
-        <f>IF(I13&gt;=80,"A+",IF(I13&gt;=70,"A",IF(I13&gt;=60,"A-",IF(I13&gt;=50,"B",IF(I13&gt;=40,"C",IF(I13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U13" s="4">
-        <f>IF(J13&gt;=80,"A+",IF(J13&gt;=70,"A",IF(J13&gt;=60,"A-",IF(J13&gt;=50,"B",IF(J13&gt;=40,"C",IF(J13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V13" s="4">
-        <f>IF(K13&gt;=80,"A+",IF(K13&gt;=70,"A",IF(K13&gt;=60,"A-",IF(K13&gt;=50,"B",IF(K13&gt;=40,"C",IF(K13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W13" s="4">
-        <f>IF(L13&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X13" s="4">
-        <f>IF(M13&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y13">
-        <f>SUM(C13:J13)</f>
-        <v/>
-      </c>
-      <c r="Z13" s="5">
-        <f>ROUND(Y13/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA13" s="6">
+        <f>ROUND(N13/8,2)</f>
+        <v/>
+      </c>
+      <c r="P13" s="5">
         <f>IF(OR(C13&lt;66,D13&lt;66,E13&lt;33,F13&lt;66,G13&lt;66,H13&lt;33,I13&lt;33,J13&lt;33,L13&lt;33,M13&lt;33),0,MIN(5,ROUND((IF(C13/200*100&gt;=80,5,IF(C13/200*100&gt;=70,4,IF(C13/200*100&gt;=60,3.5,IF(C13/200*100&gt;=50,3,IF(C13/200*100&gt;=40,2,IF(C13/200*100&gt;=33,1,0))))))+IF(D13/200*100&gt;=80,5,IF(D13/200*100&gt;=70,4,IF(D13/200*100&gt;=60,3.5,IF(D13/200*100&gt;=50,3,IF(D13/200*100&gt;=40,2,IF(D13/200*100&gt;=33,1,0))))))+IF(E13&gt;=80,5,IF(E13&gt;=70,4,IF(E13&gt;=60,3.5,IF(E13&gt;=50,3,IF(E13&gt;=40,2,IF(E13&gt;=33,1,0))))))+IF(F13/200*100&gt;=80,5,IF(F13/200*100&gt;=70,4,IF(F13/200*100&gt;=60,3.5,IF(F13/200*100&gt;=50,3,IF(F13/200*100&gt;=40,2,IF(F13/200*100&gt;=33,1,0))))))+IF(G13/200*100&gt;=80,5,IF(G13/200*100&gt;=70,4,IF(G13/200*100&gt;=60,3.5,IF(G13/200*100&gt;=50,3,IF(G13/200*100&gt;=40,2,IF(G13/200*100&gt;=33,1,0))))))+IF(H13&gt;=80,5,IF(H13&gt;=70,4,IF(H13&gt;=60,3.5,IF(H13&gt;=50,3,IF(H13&gt;=40,2,IF(H13&gt;=33,1,0))))))+IF(I13&gt;=80,5,IF(I13&gt;=70,4,IF(I13&gt;=60,3.5,IF(I13&gt;=50,3,IF(I13&gt;=40,2,IF(I13&gt;=33,1,0))))))+IF(J13&gt;=80,5,IF(J13&gt;=70,4,IF(J13&gt;=60,3.5,IF(J13&gt;=50,3,IF(J13&gt;=40,2,IF(J13&gt;=33,1,0)))))))/8+IF(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))&gt;=2,(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB13" s="4">
-        <f>IF(AA13&gt;=5,"A+",IF(AA13&gt;=4,"A",IF(AA13&gt;=3.5,"A-",IF(AA13&gt;=3,"B",IF(AA13&gt;=2,"C",IF(AA13&gt;=1,"D","F"))))))</f>
+      <c r="Q13" s="6">
+        <f>IF(P13&gt;=5,"A+",IF(P13&gt;=4,"A",IF(P13&gt;=3.5,"A-",IF(P13&gt;=3,"B",IF(P13&gt;=2,"C",IF(P13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2172,64 +1606,20 @@
       <c r="M14" s="2" t="n">
         <v>86</v>
       </c>
-      <c r="N14" s="4">
-        <f>IF(C14/200*100&gt;=80,"A+",IF(C14/200*100&gt;=70,"A",IF(C14/200*100&gt;=60,"A-",IF(C14/200*100&gt;=50,"B",IF(C14/200*100&gt;=40,"C",IF(C14/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N14">
+        <f>SUM(C14:J14)</f>
         <v/>
       </c>
       <c r="O14" s="4">
-        <f>IF(D14/200*100&gt;=80,"A+",IF(D14/200*100&gt;=70,"A",IF(D14/200*100&gt;=60,"A-",IF(D14/200*100&gt;=50,"B",IF(D14/200*100&gt;=40,"C",IF(D14/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P14" s="4">
-        <f>IF(E14&gt;=80,"A+",IF(E14&gt;=70,"A",IF(E14&gt;=60,"A-",IF(E14&gt;=50,"B",IF(E14&gt;=40,"C",IF(E14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="4">
-        <f>IF(F14/200*100&gt;=80,"A+",IF(F14/200*100&gt;=70,"A",IF(F14/200*100&gt;=60,"A-",IF(F14/200*100&gt;=50,"B",IF(F14/200*100&gt;=40,"C",IF(F14/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R14" s="4">
-        <f>IF(G14/200*100&gt;=80,"A+",IF(G14/200*100&gt;=70,"A",IF(G14/200*100&gt;=60,"A-",IF(G14/200*100&gt;=50,"B",IF(G14/200*100&gt;=40,"C",IF(G14/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S14" s="4">
-        <f>IF(H14&gt;=80,"A+",IF(H14&gt;=70,"A",IF(H14&gt;=60,"A-",IF(H14&gt;=50,"B",IF(H14&gt;=40,"C",IF(H14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T14" s="4">
-        <f>IF(I14&gt;=80,"A+",IF(I14&gt;=70,"A",IF(I14&gt;=60,"A-",IF(I14&gt;=50,"B",IF(I14&gt;=40,"C",IF(I14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U14" s="4">
-        <f>IF(J14&gt;=80,"A+",IF(J14&gt;=70,"A",IF(J14&gt;=60,"A-",IF(J14&gt;=50,"B",IF(J14&gt;=40,"C",IF(J14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V14" s="4">
-        <f>IF(K14&gt;=80,"A+",IF(K14&gt;=70,"A",IF(K14&gt;=60,"A-",IF(K14&gt;=50,"B",IF(K14&gt;=40,"C",IF(K14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W14" s="4">
-        <f>IF(L14&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X14" s="4">
-        <f>IF(M14&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y14">
-        <f>SUM(C14:J14)</f>
-        <v/>
-      </c>
-      <c r="Z14" s="5">
-        <f>ROUND(Y14/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA14" s="6">
+        <f>ROUND(N14/8,2)</f>
+        <v/>
+      </c>
+      <c r="P14" s="5">
         <f>IF(OR(C14&lt;66,D14&lt;66,E14&lt;33,F14&lt;66,G14&lt;66,H14&lt;33,I14&lt;33,J14&lt;33,L14&lt;33,M14&lt;33),0,MIN(5,ROUND((IF(C14/200*100&gt;=80,5,IF(C14/200*100&gt;=70,4,IF(C14/200*100&gt;=60,3.5,IF(C14/200*100&gt;=50,3,IF(C14/200*100&gt;=40,2,IF(C14/200*100&gt;=33,1,0))))))+IF(D14/200*100&gt;=80,5,IF(D14/200*100&gt;=70,4,IF(D14/200*100&gt;=60,3.5,IF(D14/200*100&gt;=50,3,IF(D14/200*100&gt;=40,2,IF(D14/200*100&gt;=33,1,0))))))+IF(E14&gt;=80,5,IF(E14&gt;=70,4,IF(E14&gt;=60,3.5,IF(E14&gt;=50,3,IF(E14&gt;=40,2,IF(E14&gt;=33,1,0))))))+IF(F14/200*100&gt;=80,5,IF(F14/200*100&gt;=70,4,IF(F14/200*100&gt;=60,3.5,IF(F14/200*100&gt;=50,3,IF(F14/200*100&gt;=40,2,IF(F14/200*100&gt;=33,1,0))))))+IF(G14/200*100&gt;=80,5,IF(G14/200*100&gt;=70,4,IF(G14/200*100&gt;=60,3.5,IF(G14/200*100&gt;=50,3,IF(G14/200*100&gt;=40,2,IF(G14/200*100&gt;=33,1,0))))))+IF(H14&gt;=80,5,IF(H14&gt;=70,4,IF(H14&gt;=60,3.5,IF(H14&gt;=50,3,IF(H14&gt;=40,2,IF(H14&gt;=33,1,0))))))+IF(I14&gt;=80,5,IF(I14&gt;=70,4,IF(I14&gt;=60,3.5,IF(I14&gt;=50,3,IF(I14&gt;=40,2,IF(I14&gt;=33,1,0))))))+IF(J14&gt;=80,5,IF(J14&gt;=70,4,IF(J14&gt;=60,3.5,IF(J14&gt;=50,3,IF(J14&gt;=40,2,IF(J14&gt;=33,1,0)))))))/8+IF(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))&gt;=2,(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB14" s="4">
-        <f>IF(AA14&gt;=5,"A+",IF(AA14&gt;=4,"A",IF(AA14&gt;=3.5,"A-",IF(AA14&gt;=3,"B",IF(AA14&gt;=2,"C",IF(AA14&gt;=1,"D","F"))))))</f>
+      <c r="Q14" s="6">
+        <f>IF(P14&gt;=5,"A+",IF(P14&gt;=4,"A",IF(P14&gt;=3.5,"A-",IF(P14&gt;=3,"B",IF(P14&gt;=2,"C",IF(P14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2275,64 +1665,20 @@
       <c r="M15" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="N15" s="4">
-        <f>IF(C15/200*100&gt;=80,"A+",IF(C15/200*100&gt;=70,"A",IF(C15/200*100&gt;=60,"A-",IF(C15/200*100&gt;=50,"B",IF(C15/200*100&gt;=40,"C",IF(C15/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N15">
+        <f>SUM(C15:J15)</f>
         <v/>
       </c>
       <c r="O15" s="4">
-        <f>IF(D15/200*100&gt;=80,"A+",IF(D15/200*100&gt;=70,"A",IF(D15/200*100&gt;=60,"A-",IF(D15/200*100&gt;=50,"B",IF(D15/200*100&gt;=40,"C",IF(D15/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P15" s="4">
-        <f>IF(E15&gt;=80,"A+",IF(E15&gt;=70,"A",IF(E15&gt;=60,"A-",IF(E15&gt;=50,"B",IF(E15&gt;=40,"C",IF(E15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="4">
-        <f>IF(F15/200*100&gt;=80,"A+",IF(F15/200*100&gt;=70,"A",IF(F15/200*100&gt;=60,"A-",IF(F15/200*100&gt;=50,"B",IF(F15/200*100&gt;=40,"C",IF(F15/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R15" s="4">
-        <f>IF(G15/200*100&gt;=80,"A+",IF(G15/200*100&gt;=70,"A",IF(G15/200*100&gt;=60,"A-",IF(G15/200*100&gt;=50,"B",IF(G15/200*100&gt;=40,"C",IF(G15/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S15" s="4">
-        <f>IF(H15&gt;=80,"A+",IF(H15&gt;=70,"A",IF(H15&gt;=60,"A-",IF(H15&gt;=50,"B",IF(H15&gt;=40,"C",IF(H15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T15" s="4">
-        <f>IF(I15&gt;=80,"A+",IF(I15&gt;=70,"A",IF(I15&gt;=60,"A-",IF(I15&gt;=50,"B",IF(I15&gt;=40,"C",IF(I15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U15" s="4">
-        <f>IF(J15&gt;=80,"A+",IF(J15&gt;=70,"A",IF(J15&gt;=60,"A-",IF(J15&gt;=50,"B",IF(J15&gt;=40,"C",IF(J15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V15" s="4">
-        <f>IF(K15&gt;=80,"A+",IF(K15&gt;=70,"A",IF(K15&gt;=60,"A-",IF(K15&gt;=50,"B",IF(K15&gt;=40,"C",IF(K15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W15" s="4">
-        <f>IF(L15&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X15" s="4">
-        <f>IF(M15&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y15">
-        <f>SUM(C15:J15)</f>
-        <v/>
-      </c>
-      <c r="Z15" s="5">
-        <f>ROUND(Y15/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA15" s="6">
+        <f>ROUND(N15/8,2)</f>
+        <v/>
+      </c>
+      <c r="P15" s="5">
         <f>IF(OR(C15&lt;66,D15&lt;66,E15&lt;33,F15&lt;66,G15&lt;66,H15&lt;33,I15&lt;33,J15&lt;33,L15&lt;33,M15&lt;33),0,MIN(5,ROUND((IF(C15/200*100&gt;=80,5,IF(C15/200*100&gt;=70,4,IF(C15/200*100&gt;=60,3.5,IF(C15/200*100&gt;=50,3,IF(C15/200*100&gt;=40,2,IF(C15/200*100&gt;=33,1,0))))))+IF(D15/200*100&gt;=80,5,IF(D15/200*100&gt;=70,4,IF(D15/200*100&gt;=60,3.5,IF(D15/200*100&gt;=50,3,IF(D15/200*100&gt;=40,2,IF(D15/200*100&gt;=33,1,0))))))+IF(E15&gt;=80,5,IF(E15&gt;=70,4,IF(E15&gt;=60,3.5,IF(E15&gt;=50,3,IF(E15&gt;=40,2,IF(E15&gt;=33,1,0))))))+IF(F15/200*100&gt;=80,5,IF(F15/200*100&gt;=70,4,IF(F15/200*100&gt;=60,3.5,IF(F15/200*100&gt;=50,3,IF(F15/200*100&gt;=40,2,IF(F15/200*100&gt;=33,1,0))))))+IF(G15/200*100&gt;=80,5,IF(G15/200*100&gt;=70,4,IF(G15/200*100&gt;=60,3.5,IF(G15/200*100&gt;=50,3,IF(G15/200*100&gt;=40,2,IF(G15/200*100&gt;=33,1,0))))))+IF(H15&gt;=80,5,IF(H15&gt;=70,4,IF(H15&gt;=60,3.5,IF(H15&gt;=50,3,IF(H15&gt;=40,2,IF(H15&gt;=33,1,0))))))+IF(I15&gt;=80,5,IF(I15&gt;=70,4,IF(I15&gt;=60,3.5,IF(I15&gt;=50,3,IF(I15&gt;=40,2,IF(I15&gt;=33,1,0))))))+IF(J15&gt;=80,5,IF(J15&gt;=70,4,IF(J15&gt;=60,3.5,IF(J15&gt;=50,3,IF(J15&gt;=40,2,IF(J15&gt;=33,1,0)))))))/8+IF(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))&gt;=2,(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB15" s="4">
-        <f>IF(AA15&gt;=5,"A+",IF(AA15&gt;=4,"A",IF(AA15&gt;=3.5,"A-",IF(AA15&gt;=3,"B",IF(AA15&gt;=2,"C",IF(AA15&gt;=1,"D","F"))))))</f>
+      <c r="Q15" s="6">
+        <f>IF(P15&gt;=5,"A+",IF(P15&gt;=4,"A",IF(P15&gt;=3.5,"A-",IF(P15&gt;=3,"B",IF(P15&gt;=2,"C",IF(P15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2378,64 +1724,20 @@
       <c r="M16" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="N16" s="4">
-        <f>IF(C16/200*100&gt;=80,"A+",IF(C16/200*100&gt;=70,"A",IF(C16/200*100&gt;=60,"A-",IF(C16/200*100&gt;=50,"B",IF(C16/200*100&gt;=40,"C",IF(C16/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N16">
+        <f>SUM(C16:J16)</f>
         <v/>
       </c>
       <c r="O16" s="4">
-        <f>IF(D16/200*100&gt;=80,"A+",IF(D16/200*100&gt;=70,"A",IF(D16/200*100&gt;=60,"A-",IF(D16/200*100&gt;=50,"B",IF(D16/200*100&gt;=40,"C",IF(D16/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P16" s="4">
-        <f>IF(E16&gt;=80,"A+",IF(E16&gt;=70,"A",IF(E16&gt;=60,"A-",IF(E16&gt;=50,"B",IF(E16&gt;=40,"C",IF(E16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="4">
-        <f>IF(F16/200*100&gt;=80,"A+",IF(F16/200*100&gt;=70,"A",IF(F16/200*100&gt;=60,"A-",IF(F16/200*100&gt;=50,"B",IF(F16/200*100&gt;=40,"C",IF(F16/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R16" s="4">
-        <f>IF(G16/200*100&gt;=80,"A+",IF(G16/200*100&gt;=70,"A",IF(G16/200*100&gt;=60,"A-",IF(G16/200*100&gt;=50,"B",IF(G16/200*100&gt;=40,"C",IF(G16/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S16" s="4">
-        <f>IF(H16&gt;=80,"A+",IF(H16&gt;=70,"A",IF(H16&gt;=60,"A-",IF(H16&gt;=50,"B",IF(H16&gt;=40,"C",IF(H16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T16" s="4">
-        <f>IF(I16&gt;=80,"A+",IF(I16&gt;=70,"A",IF(I16&gt;=60,"A-",IF(I16&gt;=50,"B",IF(I16&gt;=40,"C",IF(I16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U16" s="4">
-        <f>IF(J16&gt;=80,"A+",IF(J16&gt;=70,"A",IF(J16&gt;=60,"A-",IF(J16&gt;=50,"B",IF(J16&gt;=40,"C",IF(J16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V16" s="4">
-        <f>IF(K16&gt;=80,"A+",IF(K16&gt;=70,"A",IF(K16&gt;=60,"A-",IF(K16&gt;=50,"B",IF(K16&gt;=40,"C",IF(K16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W16" s="4">
-        <f>IF(L16&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X16" s="4">
-        <f>IF(M16&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y16">
-        <f>SUM(C16:J16)</f>
-        <v/>
-      </c>
-      <c r="Z16" s="5">
-        <f>ROUND(Y16/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA16" s="6">
+        <f>ROUND(N16/8,2)</f>
+        <v/>
+      </c>
+      <c r="P16" s="5">
         <f>IF(OR(C16&lt;66,D16&lt;66,E16&lt;33,F16&lt;66,G16&lt;66,H16&lt;33,I16&lt;33,J16&lt;33,L16&lt;33,M16&lt;33),0,MIN(5,ROUND((IF(C16/200*100&gt;=80,5,IF(C16/200*100&gt;=70,4,IF(C16/200*100&gt;=60,3.5,IF(C16/200*100&gt;=50,3,IF(C16/200*100&gt;=40,2,IF(C16/200*100&gt;=33,1,0))))))+IF(D16/200*100&gt;=80,5,IF(D16/200*100&gt;=70,4,IF(D16/200*100&gt;=60,3.5,IF(D16/200*100&gt;=50,3,IF(D16/200*100&gt;=40,2,IF(D16/200*100&gt;=33,1,0))))))+IF(E16&gt;=80,5,IF(E16&gt;=70,4,IF(E16&gt;=60,3.5,IF(E16&gt;=50,3,IF(E16&gt;=40,2,IF(E16&gt;=33,1,0))))))+IF(F16/200*100&gt;=80,5,IF(F16/200*100&gt;=70,4,IF(F16/200*100&gt;=60,3.5,IF(F16/200*100&gt;=50,3,IF(F16/200*100&gt;=40,2,IF(F16/200*100&gt;=33,1,0))))))+IF(G16/200*100&gt;=80,5,IF(G16/200*100&gt;=70,4,IF(G16/200*100&gt;=60,3.5,IF(G16/200*100&gt;=50,3,IF(G16/200*100&gt;=40,2,IF(G16/200*100&gt;=33,1,0))))))+IF(H16&gt;=80,5,IF(H16&gt;=70,4,IF(H16&gt;=60,3.5,IF(H16&gt;=50,3,IF(H16&gt;=40,2,IF(H16&gt;=33,1,0))))))+IF(I16&gt;=80,5,IF(I16&gt;=70,4,IF(I16&gt;=60,3.5,IF(I16&gt;=50,3,IF(I16&gt;=40,2,IF(I16&gt;=33,1,0))))))+IF(J16&gt;=80,5,IF(J16&gt;=70,4,IF(J16&gt;=60,3.5,IF(J16&gt;=50,3,IF(J16&gt;=40,2,IF(J16&gt;=33,1,0)))))))/8+IF(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))&gt;=2,(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB16" s="4">
-        <f>IF(AA16&gt;=5,"A+",IF(AA16&gt;=4,"A",IF(AA16&gt;=3.5,"A-",IF(AA16&gt;=3,"B",IF(AA16&gt;=2,"C",IF(AA16&gt;=1,"D","F"))))))</f>
+      <c r="Q16" s="6">
+        <f>IF(P16&gt;=5,"A+",IF(P16&gt;=4,"A",IF(P16&gt;=3.5,"A-",IF(P16&gt;=3,"B",IF(P16&gt;=2,"C",IF(P16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2481,64 +1783,20 @@
       <c r="M17" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="N17" s="4">
-        <f>IF(C17/200*100&gt;=80,"A+",IF(C17/200*100&gt;=70,"A",IF(C17/200*100&gt;=60,"A-",IF(C17/200*100&gt;=50,"B",IF(C17/200*100&gt;=40,"C",IF(C17/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N17">
+        <f>SUM(C17:J17)</f>
         <v/>
       </c>
       <c r="O17" s="4">
-        <f>IF(D17/200*100&gt;=80,"A+",IF(D17/200*100&gt;=70,"A",IF(D17/200*100&gt;=60,"A-",IF(D17/200*100&gt;=50,"B",IF(D17/200*100&gt;=40,"C",IF(D17/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P17" s="4">
-        <f>IF(E17&gt;=80,"A+",IF(E17&gt;=70,"A",IF(E17&gt;=60,"A-",IF(E17&gt;=50,"B",IF(E17&gt;=40,"C",IF(E17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="4">
-        <f>IF(F17/200*100&gt;=80,"A+",IF(F17/200*100&gt;=70,"A",IF(F17/200*100&gt;=60,"A-",IF(F17/200*100&gt;=50,"B",IF(F17/200*100&gt;=40,"C",IF(F17/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R17" s="4">
-        <f>IF(G17/200*100&gt;=80,"A+",IF(G17/200*100&gt;=70,"A",IF(G17/200*100&gt;=60,"A-",IF(G17/200*100&gt;=50,"B",IF(G17/200*100&gt;=40,"C",IF(G17/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S17" s="4">
-        <f>IF(H17&gt;=80,"A+",IF(H17&gt;=70,"A",IF(H17&gt;=60,"A-",IF(H17&gt;=50,"B",IF(H17&gt;=40,"C",IF(H17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T17" s="4">
-        <f>IF(I17&gt;=80,"A+",IF(I17&gt;=70,"A",IF(I17&gt;=60,"A-",IF(I17&gt;=50,"B",IF(I17&gt;=40,"C",IF(I17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U17" s="4">
-        <f>IF(J17&gt;=80,"A+",IF(J17&gt;=70,"A",IF(J17&gt;=60,"A-",IF(J17&gt;=50,"B",IF(J17&gt;=40,"C",IF(J17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V17" s="4">
-        <f>IF(K17&gt;=80,"A+",IF(K17&gt;=70,"A",IF(K17&gt;=60,"A-",IF(K17&gt;=50,"B",IF(K17&gt;=40,"C",IF(K17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W17" s="4">
-        <f>IF(L17&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X17" s="4">
-        <f>IF(M17&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y17">
-        <f>SUM(C17:J17)</f>
-        <v/>
-      </c>
-      <c r="Z17" s="5">
-        <f>ROUND(Y17/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA17" s="6">
+        <f>ROUND(N17/8,2)</f>
+        <v/>
+      </c>
+      <c r="P17" s="5">
         <f>IF(OR(C17&lt;66,D17&lt;66,E17&lt;33,F17&lt;66,G17&lt;66,H17&lt;33,I17&lt;33,J17&lt;33,L17&lt;33,M17&lt;33),0,MIN(5,ROUND((IF(C17/200*100&gt;=80,5,IF(C17/200*100&gt;=70,4,IF(C17/200*100&gt;=60,3.5,IF(C17/200*100&gt;=50,3,IF(C17/200*100&gt;=40,2,IF(C17/200*100&gt;=33,1,0))))))+IF(D17/200*100&gt;=80,5,IF(D17/200*100&gt;=70,4,IF(D17/200*100&gt;=60,3.5,IF(D17/200*100&gt;=50,3,IF(D17/200*100&gt;=40,2,IF(D17/200*100&gt;=33,1,0))))))+IF(E17&gt;=80,5,IF(E17&gt;=70,4,IF(E17&gt;=60,3.5,IF(E17&gt;=50,3,IF(E17&gt;=40,2,IF(E17&gt;=33,1,0))))))+IF(F17/200*100&gt;=80,5,IF(F17/200*100&gt;=70,4,IF(F17/200*100&gt;=60,3.5,IF(F17/200*100&gt;=50,3,IF(F17/200*100&gt;=40,2,IF(F17/200*100&gt;=33,1,0))))))+IF(G17/200*100&gt;=80,5,IF(G17/200*100&gt;=70,4,IF(G17/200*100&gt;=60,3.5,IF(G17/200*100&gt;=50,3,IF(G17/200*100&gt;=40,2,IF(G17/200*100&gt;=33,1,0))))))+IF(H17&gt;=80,5,IF(H17&gt;=70,4,IF(H17&gt;=60,3.5,IF(H17&gt;=50,3,IF(H17&gt;=40,2,IF(H17&gt;=33,1,0))))))+IF(I17&gt;=80,5,IF(I17&gt;=70,4,IF(I17&gt;=60,3.5,IF(I17&gt;=50,3,IF(I17&gt;=40,2,IF(I17&gt;=33,1,0))))))+IF(J17&gt;=80,5,IF(J17&gt;=70,4,IF(J17&gt;=60,3.5,IF(J17&gt;=50,3,IF(J17&gt;=40,2,IF(J17&gt;=33,1,0)))))))/8+IF(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))&gt;=2,(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB17" s="4">
-        <f>IF(AA17&gt;=5,"A+",IF(AA17&gt;=4,"A",IF(AA17&gt;=3.5,"A-",IF(AA17&gt;=3,"B",IF(AA17&gt;=2,"C",IF(AA17&gt;=1,"D","F"))))))</f>
+      <c r="Q17" s="6">
+        <f>IF(P17&gt;=5,"A+",IF(P17&gt;=4,"A",IF(P17&gt;=3.5,"A-",IF(P17&gt;=3,"B",IF(P17&gt;=2,"C",IF(P17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2584,64 +1842,20 @@
       <c r="M18" s="3" t="n">
         <v>78</v>
       </c>
-      <c r="N18" s="4">
-        <f>IF(C18/200*100&gt;=80,"A+",IF(C18/200*100&gt;=70,"A",IF(C18/200*100&gt;=60,"A-",IF(C18/200*100&gt;=50,"B",IF(C18/200*100&gt;=40,"C",IF(C18/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N18">
+        <f>SUM(C18:J18)</f>
         <v/>
       </c>
       <c r="O18" s="4">
-        <f>IF(D18/200*100&gt;=80,"A+",IF(D18/200*100&gt;=70,"A",IF(D18/200*100&gt;=60,"A-",IF(D18/200*100&gt;=50,"B",IF(D18/200*100&gt;=40,"C",IF(D18/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P18" s="4">
-        <f>IF(E18&gt;=80,"A+",IF(E18&gt;=70,"A",IF(E18&gt;=60,"A-",IF(E18&gt;=50,"B",IF(E18&gt;=40,"C",IF(E18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="4">
-        <f>IF(F18/200*100&gt;=80,"A+",IF(F18/200*100&gt;=70,"A",IF(F18/200*100&gt;=60,"A-",IF(F18/200*100&gt;=50,"B",IF(F18/200*100&gt;=40,"C",IF(F18/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R18" s="4">
-        <f>IF(G18/200*100&gt;=80,"A+",IF(G18/200*100&gt;=70,"A",IF(G18/200*100&gt;=60,"A-",IF(G18/200*100&gt;=50,"B",IF(G18/200*100&gt;=40,"C",IF(G18/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S18" s="4">
-        <f>IF(H18&gt;=80,"A+",IF(H18&gt;=70,"A",IF(H18&gt;=60,"A-",IF(H18&gt;=50,"B",IF(H18&gt;=40,"C",IF(H18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T18" s="4">
-        <f>IF(I18&gt;=80,"A+",IF(I18&gt;=70,"A",IF(I18&gt;=60,"A-",IF(I18&gt;=50,"B",IF(I18&gt;=40,"C",IF(I18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U18" s="4">
-        <f>IF(J18&gt;=80,"A+",IF(J18&gt;=70,"A",IF(J18&gt;=60,"A-",IF(J18&gt;=50,"B",IF(J18&gt;=40,"C",IF(J18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V18" s="4">
-        <f>IF(K18&gt;=80,"A+",IF(K18&gt;=70,"A",IF(K18&gt;=60,"A-",IF(K18&gt;=50,"B",IF(K18&gt;=40,"C",IF(K18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W18" s="4">
-        <f>IF(L18&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X18" s="4">
-        <f>IF(M18&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y18">
-        <f>SUM(C18:J18)</f>
-        <v/>
-      </c>
-      <c r="Z18" s="5">
-        <f>ROUND(Y18/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA18" s="6">
+        <f>ROUND(N18/8,2)</f>
+        <v/>
+      </c>
+      <c r="P18" s="5">
         <f>IF(OR(C18&lt;66,D18&lt;66,E18&lt;33,F18&lt;66,G18&lt;66,H18&lt;33,I18&lt;33,J18&lt;33,L18&lt;33,M18&lt;33),0,MIN(5,ROUND((IF(C18/200*100&gt;=80,5,IF(C18/200*100&gt;=70,4,IF(C18/200*100&gt;=60,3.5,IF(C18/200*100&gt;=50,3,IF(C18/200*100&gt;=40,2,IF(C18/200*100&gt;=33,1,0))))))+IF(D18/200*100&gt;=80,5,IF(D18/200*100&gt;=70,4,IF(D18/200*100&gt;=60,3.5,IF(D18/200*100&gt;=50,3,IF(D18/200*100&gt;=40,2,IF(D18/200*100&gt;=33,1,0))))))+IF(E18&gt;=80,5,IF(E18&gt;=70,4,IF(E18&gt;=60,3.5,IF(E18&gt;=50,3,IF(E18&gt;=40,2,IF(E18&gt;=33,1,0))))))+IF(F18/200*100&gt;=80,5,IF(F18/200*100&gt;=70,4,IF(F18/200*100&gt;=60,3.5,IF(F18/200*100&gt;=50,3,IF(F18/200*100&gt;=40,2,IF(F18/200*100&gt;=33,1,0))))))+IF(G18/200*100&gt;=80,5,IF(G18/200*100&gt;=70,4,IF(G18/200*100&gt;=60,3.5,IF(G18/200*100&gt;=50,3,IF(G18/200*100&gt;=40,2,IF(G18/200*100&gt;=33,1,0))))))+IF(H18&gt;=80,5,IF(H18&gt;=70,4,IF(H18&gt;=60,3.5,IF(H18&gt;=50,3,IF(H18&gt;=40,2,IF(H18&gt;=33,1,0))))))+IF(I18&gt;=80,5,IF(I18&gt;=70,4,IF(I18&gt;=60,3.5,IF(I18&gt;=50,3,IF(I18&gt;=40,2,IF(I18&gt;=33,1,0))))))+IF(J18&gt;=80,5,IF(J18&gt;=70,4,IF(J18&gt;=60,3.5,IF(J18&gt;=50,3,IF(J18&gt;=40,2,IF(J18&gt;=33,1,0)))))))/8+IF(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))&gt;=2,(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB18" s="4">
-        <f>IF(AA18&gt;=5,"A+",IF(AA18&gt;=4,"A",IF(AA18&gt;=3.5,"A-",IF(AA18&gt;=3,"B",IF(AA18&gt;=2,"C",IF(AA18&gt;=1,"D","F"))))))</f>
+      <c r="Q18" s="6">
+        <f>IF(P18&gt;=5,"A+",IF(P18&gt;=4,"A",IF(P18&gt;=3.5,"A-",IF(P18&gt;=3,"B",IF(P18&gt;=2,"C",IF(P18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2687,64 +1901,20 @@
       <c r="M19" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="N19" s="4">
-        <f>IF(C19/200*100&gt;=80,"A+",IF(C19/200*100&gt;=70,"A",IF(C19/200*100&gt;=60,"A-",IF(C19/200*100&gt;=50,"B",IF(C19/200*100&gt;=40,"C",IF(C19/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N19">
+        <f>SUM(C19:J19)</f>
         <v/>
       </c>
       <c r="O19" s="4">
-        <f>IF(D19/200*100&gt;=80,"A+",IF(D19/200*100&gt;=70,"A",IF(D19/200*100&gt;=60,"A-",IF(D19/200*100&gt;=50,"B",IF(D19/200*100&gt;=40,"C",IF(D19/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P19" s="4">
-        <f>IF(E19&gt;=80,"A+",IF(E19&gt;=70,"A",IF(E19&gt;=60,"A-",IF(E19&gt;=50,"B",IF(E19&gt;=40,"C",IF(E19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="4">
-        <f>IF(F19/200*100&gt;=80,"A+",IF(F19/200*100&gt;=70,"A",IF(F19/200*100&gt;=60,"A-",IF(F19/200*100&gt;=50,"B",IF(F19/200*100&gt;=40,"C",IF(F19/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R19" s="4">
-        <f>IF(G19/200*100&gt;=80,"A+",IF(G19/200*100&gt;=70,"A",IF(G19/200*100&gt;=60,"A-",IF(G19/200*100&gt;=50,"B",IF(G19/200*100&gt;=40,"C",IF(G19/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S19" s="4">
-        <f>IF(H19&gt;=80,"A+",IF(H19&gt;=70,"A",IF(H19&gt;=60,"A-",IF(H19&gt;=50,"B",IF(H19&gt;=40,"C",IF(H19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T19" s="4">
-        <f>IF(I19&gt;=80,"A+",IF(I19&gt;=70,"A",IF(I19&gt;=60,"A-",IF(I19&gt;=50,"B",IF(I19&gt;=40,"C",IF(I19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U19" s="4">
-        <f>IF(J19&gt;=80,"A+",IF(J19&gt;=70,"A",IF(J19&gt;=60,"A-",IF(J19&gt;=50,"B",IF(J19&gt;=40,"C",IF(J19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V19" s="4">
-        <f>IF(K19&gt;=80,"A+",IF(K19&gt;=70,"A",IF(K19&gt;=60,"A-",IF(K19&gt;=50,"B",IF(K19&gt;=40,"C",IF(K19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W19" s="4">
-        <f>IF(L19&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X19" s="4">
-        <f>IF(M19&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y19">
-        <f>SUM(C19:J19)</f>
-        <v/>
-      </c>
-      <c r="Z19" s="5">
-        <f>ROUND(Y19/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA19" s="6">
+        <f>ROUND(N19/8,2)</f>
+        <v/>
+      </c>
+      <c r="P19" s="5">
         <f>IF(OR(C19&lt;66,D19&lt;66,E19&lt;33,F19&lt;66,G19&lt;66,H19&lt;33,I19&lt;33,J19&lt;33,L19&lt;33,M19&lt;33),0,MIN(5,ROUND((IF(C19/200*100&gt;=80,5,IF(C19/200*100&gt;=70,4,IF(C19/200*100&gt;=60,3.5,IF(C19/200*100&gt;=50,3,IF(C19/200*100&gt;=40,2,IF(C19/200*100&gt;=33,1,0))))))+IF(D19/200*100&gt;=80,5,IF(D19/200*100&gt;=70,4,IF(D19/200*100&gt;=60,3.5,IF(D19/200*100&gt;=50,3,IF(D19/200*100&gt;=40,2,IF(D19/200*100&gt;=33,1,0))))))+IF(E19&gt;=80,5,IF(E19&gt;=70,4,IF(E19&gt;=60,3.5,IF(E19&gt;=50,3,IF(E19&gt;=40,2,IF(E19&gt;=33,1,0))))))+IF(F19/200*100&gt;=80,5,IF(F19/200*100&gt;=70,4,IF(F19/200*100&gt;=60,3.5,IF(F19/200*100&gt;=50,3,IF(F19/200*100&gt;=40,2,IF(F19/200*100&gt;=33,1,0))))))+IF(G19/200*100&gt;=80,5,IF(G19/200*100&gt;=70,4,IF(G19/200*100&gt;=60,3.5,IF(G19/200*100&gt;=50,3,IF(G19/200*100&gt;=40,2,IF(G19/200*100&gt;=33,1,0))))))+IF(H19&gt;=80,5,IF(H19&gt;=70,4,IF(H19&gt;=60,3.5,IF(H19&gt;=50,3,IF(H19&gt;=40,2,IF(H19&gt;=33,1,0))))))+IF(I19&gt;=80,5,IF(I19&gt;=70,4,IF(I19&gt;=60,3.5,IF(I19&gt;=50,3,IF(I19&gt;=40,2,IF(I19&gt;=33,1,0))))))+IF(J19&gt;=80,5,IF(J19&gt;=70,4,IF(J19&gt;=60,3.5,IF(J19&gt;=50,3,IF(J19&gt;=40,2,IF(J19&gt;=33,1,0)))))))/8+IF(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))&gt;=2,(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB19" s="4">
-        <f>IF(AA19&gt;=5,"A+",IF(AA19&gt;=4,"A",IF(AA19&gt;=3.5,"A-",IF(AA19&gt;=3,"B",IF(AA19&gt;=2,"C",IF(AA19&gt;=1,"D","F"))))))</f>
+      <c r="Q19" s="6">
+        <f>IF(P19&gt;=5,"A+",IF(P19&gt;=4,"A",IF(P19&gt;=3.5,"A-",IF(P19&gt;=3,"B",IF(P19&gt;=2,"C",IF(P19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2790,64 +1960,20 @@
       <c r="M20" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="N20" s="4">
-        <f>IF(C20/200*100&gt;=80,"A+",IF(C20/200*100&gt;=70,"A",IF(C20/200*100&gt;=60,"A-",IF(C20/200*100&gt;=50,"B",IF(C20/200*100&gt;=40,"C",IF(C20/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N20">
+        <f>SUM(C20:J20)</f>
         <v/>
       </c>
       <c r="O20" s="4">
-        <f>IF(D20/200*100&gt;=80,"A+",IF(D20/200*100&gt;=70,"A",IF(D20/200*100&gt;=60,"A-",IF(D20/200*100&gt;=50,"B",IF(D20/200*100&gt;=40,"C",IF(D20/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P20" s="4">
-        <f>IF(E20&gt;=80,"A+",IF(E20&gt;=70,"A",IF(E20&gt;=60,"A-",IF(E20&gt;=50,"B",IF(E20&gt;=40,"C",IF(E20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="4">
-        <f>IF(F20/200*100&gt;=80,"A+",IF(F20/200*100&gt;=70,"A",IF(F20/200*100&gt;=60,"A-",IF(F20/200*100&gt;=50,"B",IF(F20/200*100&gt;=40,"C",IF(F20/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R20" s="4">
-        <f>IF(G20/200*100&gt;=80,"A+",IF(G20/200*100&gt;=70,"A",IF(G20/200*100&gt;=60,"A-",IF(G20/200*100&gt;=50,"B",IF(G20/200*100&gt;=40,"C",IF(G20/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S20" s="4">
-        <f>IF(H20&gt;=80,"A+",IF(H20&gt;=70,"A",IF(H20&gt;=60,"A-",IF(H20&gt;=50,"B",IF(H20&gt;=40,"C",IF(H20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T20" s="4">
-        <f>IF(I20&gt;=80,"A+",IF(I20&gt;=70,"A",IF(I20&gt;=60,"A-",IF(I20&gt;=50,"B",IF(I20&gt;=40,"C",IF(I20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U20" s="4">
-        <f>IF(J20&gt;=80,"A+",IF(J20&gt;=70,"A",IF(J20&gt;=60,"A-",IF(J20&gt;=50,"B",IF(J20&gt;=40,"C",IF(J20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V20" s="4">
-        <f>IF(K20&gt;=80,"A+",IF(K20&gt;=70,"A",IF(K20&gt;=60,"A-",IF(K20&gt;=50,"B",IF(K20&gt;=40,"C",IF(K20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W20" s="4">
-        <f>IF(L20&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X20" s="4">
-        <f>IF(M20&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y20">
-        <f>SUM(C20:J20)</f>
-        <v/>
-      </c>
-      <c r="Z20" s="5">
-        <f>ROUND(Y20/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA20" s="6">
+        <f>ROUND(N20/8,2)</f>
+        <v/>
+      </c>
+      <c r="P20" s="5">
         <f>IF(OR(C20&lt;66,D20&lt;66,E20&lt;33,F20&lt;66,G20&lt;66,H20&lt;33,I20&lt;33,J20&lt;33,L20&lt;33,M20&lt;33),0,MIN(5,ROUND((IF(C20/200*100&gt;=80,5,IF(C20/200*100&gt;=70,4,IF(C20/200*100&gt;=60,3.5,IF(C20/200*100&gt;=50,3,IF(C20/200*100&gt;=40,2,IF(C20/200*100&gt;=33,1,0))))))+IF(D20/200*100&gt;=80,5,IF(D20/200*100&gt;=70,4,IF(D20/200*100&gt;=60,3.5,IF(D20/200*100&gt;=50,3,IF(D20/200*100&gt;=40,2,IF(D20/200*100&gt;=33,1,0))))))+IF(E20&gt;=80,5,IF(E20&gt;=70,4,IF(E20&gt;=60,3.5,IF(E20&gt;=50,3,IF(E20&gt;=40,2,IF(E20&gt;=33,1,0))))))+IF(F20/200*100&gt;=80,5,IF(F20/200*100&gt;=70,4,IF(F20/200*100&gt;=60,3.5,IF(F20/200*100&gt;=50,3,IF(F20/200*100&gt;=40,2,IF(F20/200*100&gt;=33,1,0))))))+IF(G20/200*100&gt;=80,5,IF(G20/200*100&gt;=70,4,IF(G20/200*100&gt;=60,3.5,IF(G20/200*100&gt;=50,3,IF(G20/200*100&gt;=40,2,IF(G20/200*100&gt;=33,1,0))))))+IF(H20&gt;=80,5,IF(H20&gt;=70,4,IF(H20&gt;=60,3.5,IF(H20&gt;=50,3,IF(H20&gt;=40,2,IF(H20&gt;=33,1,0))))))+IF(I20&gt;=80,5,IF(I20&gt;=70,4,IF(I20&gt;=60,3.5,IF(I20&gt;=50,3,IF(I20&gt;=40,2,IF(I20&gt;=33,1,0))))))+IF(J20&gt;=80,5,IF(J20&gt;=70,4,IF(J20&gt;=60,3.5,IF(J20&gt;=50,3,IF(J20&gt;=40,2,IF(J20&gt;=33,1,0)))))))/8+IF(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))&gt;=2,(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB20" s="4">
-        <f>IF(AA20&gt;=5,"A+",IF(AA20&gt;=4,"A",IF(AA20&gt;=3.5,"A-",IF(AA20&gt;=3,"B",IF(AA20&gt;=2,"C",IF(AA20&gt;=1,"D","F"))))))</f>
+      <c r="Q20" s="6">
+        <f>IF(P20&gt;=5,"A+",IF(P20&gt;=4,"A",IF(P20&gt;=3.5,"A-",IF(P20&gt;=3,"B",IF(P20&gt;=2,"C",IF(P20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2893,64 +2019,20 @@
       <c r="M21" s="3" t="n">
         <v>77</v>
       </c>
-      <c r="N21" s="4">
-        <f>IF(C21/200*100&gt;=80,"A+",IF(C21/200*100&gt;=70,"A",IF(C21/200*100&gt;=60,"A-",IF(C21/200*100&gt;=50,"B",IF(C21/200*100&gt;=40,"C",IF(C21/200*100&gt;=33,"D","F"))))))</f>
+      <c r="N21">
+        <f>SUM(C21:J21)</f>
         <v/>
       </c>
       <c r="O21" s="4">
-        <f>IF(D21/200*100&gt;=80,"A+",IF(D21/200*100&gt;=70,"A",IF(D21/200*100&gt;=60,"A-",IF(D21/200*100&gt;=50,"B",IF(D21/200*100&gt;=40,"C",IF(D21/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="P21" s="4">
-        <f>IF(E21&gt;=80,"A+",IF(E21&gt;=70,"A",IF(E21&gt;=60,"A-",IF(E21&gt;=50,"B",IF(E21&gt;=40,"C",IF(E21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="4">
-        <f>IF(F21/200*100&gt;=80,"A+",IF(F21/200*100&gt;=70,"A",IF(F21/200*100&gt;=60,"A-",IF(F21/200*100&gt;=50,"B",IF(F21/200*100&gt;=40,"C",IF(F21/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="R21" s="4">
-        <f>IF(G21/200*100&gt;=80,"A+",IF(G21/200*100&gt;=70,"A",IF(G21/200*100&gt;=60,"A-",IF(G21/200*100&gt;=50,"B",IF(G21/200*100&gt;=40,"C",IF(G21/200*100&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="S21" s="4">
-        <f>IF(H21&gt;=80,"A+",IF(H21&gt;=70,"A",IF(H21&gt;=60,"A-",IF(H21&gt;=50,"B",IF(H21&gt;=40,"C",IF(H21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="T21" s="4">
-        <f>IF(I21&gt;=80,"A+",IF(I21&gt;=70,"A",IF(I21&gt;=60,"A-",IF(I21&gt;=50,"B",IF(I21&gt;=40,"C",IF(I21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="U21" s="4">
-        <f>IF(J21&gt;=80,"A+",IF(J21&gt;=70,"A",IF(J21&gt;=60,"A-",IF(J21&gt;=50,"B",IF(J21&gt;=40,"C",IF(J21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="V21" s="4">
-        <f>IF(K21&gt;=80,"A+",IF(K21&gt;=70,"A",IF(K21&gt;=60,"A-",IF(K21&gt;=50,"B",IF(K21&gt;=40,"C",IF(K21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="W21" s="4">
-        <f>IF(L21&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="X21" s="4">
-        <f>IF(M21&gt;=33,"Pass","Fail")</f>
-        <v/>
-      </c>
-      <c r="Y21">
-        <f>SUM(C21:J21)</f>
-        <v/>
-      </c>
-      <c r="Z21" s="5">
-        <f>ROUND(Y21/8,2)</f>
-        <v/>
-      </c>
-      <c r="AA21" s="6">
+        <f>ROUND(N21/8,2)</f>
+        <v/>
+      </c>
+      <c r="P21" s="5">
         <f>IF(OR(C21&lt;66,D21&lt;66,E21&lt;33,F21&lt;66,G21&lt;66,H21&lt;33,I21&lt;33,J21&lt;33,L21&lt;33,M21&lt;33),0,MIN(5,ROUND((IF(C21/200*100&gt;=80,5,IF(C21/200*100&gt;=70,4,IF(C21/200*100&gt;=60,3.5,IF(C21/200*100&gt;=50,3,IF(C21/200*100&gt;=40,2,IF(C21/200*100&gt;=33,1,0))))))+IF(D21/200*100&gt;=80,5,IF(D21/200*100&gt;=70,4,IF(D21/200*100&gt;=60,3.5,IF(D21/200*100&gt;=50,3,IF(D21/200*100&gt;=40,2,IF(D21/200*100&gt;=33,1,0))))))+IF(E21&gt;=80,5,IF(E21&gt;=70,4,IF(E21&gt;=60,3.5,IF(E21&gt;=50,3,IF(E21&gt;=40,2,IF(E21&gt;=33,1,0))))))+IF(F21/200*100&gt;=80,5,IF(F21/200*100&gt;=70,4,IF(F21/200*100&gt;=60,3.5,IF(F21/200*100&gt;=50,3,IF(F21/200*100&gt;=40,2,IF(F21/200*100&gt;=33,1,0))))))+IF(G21/200*100&gt;=80,5,IF(G21/200*100&gt;=70,4,IF(G21/200*100&gt;=60,3.5,IF(G21/200*100&gt;=50,3,IF(G21/200*100&gt;=40,2,IF(G21/200*100&gt;=33,1,0))))))+IF(H21&gt;=80,5,IF(H21&gt;=70,4,IF(H21&gt;=60,3.5,IF(H21&gt;=50,3,IF(H21&gt;=40,2,IF(H21&gt;=33,1,0))))))+IF(I21&gt;=80,5,IF(I21&gt;=70,4,IF(I21&gt;=60,3.5,IF(I21&gt;=50,3,IF(I21&gt;=40,2,IF(I21&gt;=33,1,0))))))+IF(J21&gt;=80,5,IF(J21&gt;=70,4,IF(J21&gt;=60,3.5,IF(J21&gt;=50,3,IF(J21&gt;=40,2,IF(J21&gt;=33,1,0)))))))/8+IF(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))&gt;=2,(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))-2)/8,0),2)))</f>
         <v/>
       </c>
-      <c r="AB21" s="4">
-        <f>IF(AA21&gt;=5,"A+",IF(AA21&gt;=4,"A",IF(AA21&gt;=3.5,"A-",IF(AA21&gt;=3,"B",IF(AA21&gt;=2,"C",IF(AA21&gt;=1,"D","F"))))))</f>
+      <c r="Q21" s="6">
+        <f>IF(P21&gt;=5,"A+",IF(P21&gt;=4,"A",IF(P21&gt;=3.5,"A-",IF(P21&gt;=3,"B",IF(P21&gt;=2,"C",IF(P21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -3011,7 +2093,7 @@
         </is>
       </c>
       <c r="F5" s="12">
-        <f>IFERROR(ROUND(AVERAGE('Data Source'!AA:AA),2), 0)</f>
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!P:P),2), 0)</f>
         <v/>
       </c>
       <c r="H5" s="10" t="inlineStr">
@@ -3020,7 +2102,7 @@
         </is>
       </c>
       <c r="I5" s="11">
-        <f>MAX('Data Source'!Y:Y)</f>
+        <f>MAX('Data Source'!N:N)</f>
         <v/>
       </c>
       <c r="K5" s="10" t="inlineStr">
@@ -3029,7 +2111,7 @@
         </is>
       </c>
       <c r="L5" s="13">
-        <f>IF(C5&gt;0,COUNTIF('Data Source'!AA:AA,"&gt;0")/C5,0)</f>
+        <f>IF(C5&gt;0,COUNTIF('Data Source'!P:P,"&gt;0")/C5,0)</f>
         <v/>
       </c>
     </row>
@@ -3093,13 +2175,13 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="B9" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"A+")</f>
+      <c r="B9" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"A+")</f>
         <v/>
       </c>
       <c r="D9" t="inlineStr">
@@ -3107,7 +2189,7 @@
           <t>Quran Mazid</t>
         </is>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!C:C),2),0)</f>
         <v/>
       </c>
@@ -3115,26 +2197,26 @@
         <f>IFERROR(ROUND(E9/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="H9">
         <f>'Data Source'!B18</f>
         <v/>
       </c>
-      <c r="I9" s="6">
-        <f>'Data Source'!AA18</f>
+      <c r="I9" s="5">
+        <f>'Data Source'!P18</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B10" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"A")</f>
+      <c r="B10" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"A")</f>
         <v/>
       </c>
       <c r="D10" t="inlineStr">
@@ -3142,7 +2224,7 @@
           <t>Arabic (Comb.)</t>
         </is>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!D:D),2),0)</f>
         <v/>
       </c>
@@ -3150,26 +2232,26 @@
         <f>IFERROR(ROUND(E10/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H10">
         <f>'Data Source'!B17</f>
         <v/>
       </c>
-      <c r="I10" s="6">
-        <f>'Data Source'!AA17</f>
+      <c r="I10" s="5">
+        <f>'Data Source'!P17</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>A-</t>
         </is>
       </c>
-      <c r="B11" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"A-")</f>
+      <c r="B11" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"A-")</f>
         <v/>
       </c>
       <c r="D11" t="inlineStr">
@@ -3177,7 +2259,7 @@
           <t>Aqaid</t>
         </is>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!E:E),2),0)</f>
         <v/>
       </c>
@@ -3185,26 +2267,26 @@
         <f>IFERROR(ROUND(E11/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="6" t="n">
         <v>3</v>
       </c>
       <c r="H11">
         <f>'Data Source'!B8</f>
         <v/>
       </c>
-      <c r="I11" s="6">
-        <f>'Data Source'!AA8</f>
+      <c r="I11" s="5">
+        <f>'Data Source'!P8</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="B12" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"B")</f>
+      <c r="B12" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"B")</f>
         <v/>
       </c>
       <c r="D12" t="inlineStr">
@@ -3212,7 +2294,7 @@
           <t>English (Comb.)</t>
         </is>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!F:F),2),0)</f>
         <v/>
       </c>
@@ -3220,26 +2302,26 @@
         <f>IFERROR(ROUND(E12/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="6" t="n">
         <v>4</v>
       </c>
       <c r="H12">
         <f>'Data Source'!B13</f>
         <v/>
       </c>
-      <c r="I12" s="6">
-        <f>'Data Source'!AA13</f>
+      <c r="I12" s="5">
+        <f>'Data Source'!P13</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="B13" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"C")</f>
+      <c r="B13" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"C")</f>
         <v/>
       </c>
       <c r="D13" t="inlineStr">
@@ -3247,7 +2329,7 @@
           <t>Bangla (Comb.)</t>
         </is>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!G:G),2),0)</f>
         <v/>
       </c>
@@ -3255,26 +2337,26 @@
         <f>IFERROR(ROUND(E13/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="6" t="n">
         <v>5</v>
       </c>
       <c r="H13">
         <f>'Data Source'!B14</f>
         <v/>
       </c>
-      <c r="I13" s="6">
-        <f>'Data Source'!AA14</f>
+      <c r="I13" s="5">
+        <f>'Data Source'!P14</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="B14" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"D")</f>
+      <c r="B14" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"D")</f>
         <v/>
       </c>
       <c r="D14" t="inlineStr">
@@ -3282,7 +2364,7 @@
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!H:H),2),0)</f>
         <v/>
       </c>
@@ -3292,13 +2374,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="B15" s="4">
-        <f>COUNTIF('Data Source'!AB:AB,"F")</f>
+      <c r="B15" s="6">
+        <f>COUNTIF('Data Source'!Q:Q,"F")</f>
         <v/>
       </c>
       <c r="D15" t="inlineStr">
@@ -3306,7 +2388,7 @@
           <t>Islamic History</t>
         </is>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!I:I),2),0)</f>
         <v/>
       </c>
@@ -3321,7 +2403,7 @@
           <t>ICT</t>
         </is>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!J:J),2),0)</f>
         <v/>
       </c>
@@ -3336,7 +2418,7 @@
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!K:K),2),0)</f>
         <v/>
       </c>
@@ -3360,6 +2442,1369 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="17" t="inlineStr">
+        <is>
+          <t>SUBJECT-WISE GRADES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="18" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="B2" s="18" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" s="18" t="inlineStr">
+        <is>
+          <t>Quran</t>
+        </is>
+      </c>
+      <c r="D2" s="18" t="inlineStr">
+        <is>
+          <t>Arabic</t>
+        </is>
+      </c>
+      <c r="E2" s="18" t="inlineStr">
+        <is>
+          <t>Aqaid</t>
+        </is>
+      </c>
+      <c r="F2" s="18" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="G2" s="18" t="inlineStr">
+        <is>
+          <t>Bangla</t>
+        </is>
+      </c>
+      <c r="H2" s="18" t="inlineStr">
+        <is>
+          <t>Math</t>
+        </is>
+      </c>
+      <c r="I2" s="18" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="J2" s="18" t="inlineStr">
+        <is>
+          <t>ICT</t>
+        </is>
+      </c>
+      <c r="K2" s="18" t="inlineStr">
+        <is>
+          <t>Mantiq</t>
+        </is>
+      </c>
+      <c r="L2" s="18" t="inlineStr">
+        <is>
+          <t>Career</t>
+        </is>
+      </c>
+      <c r="M2" s="18" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+      <c r="N2" s="18" t="inlineStr">
+        <is>
+          <t>Overall GPA</t>
+        </is>
+      </c>
+      <c r="O2" s="18" t="inlineStr">
+        <is>
+          <t>Overall Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6">
+        <f>'Data Source'!A2</f>
+        <v/>
+      </c>
+      <c r="B3">
+        <f>'Data Source'!B2</f>
+        <v/>
+      </c>
+      <c r="C3" s="6">
+        <f>IF('Data Source'!C2/200*100&gt;=80,"A+",IF('Data Source'!C2/200*100&gt;=70,"A",IF('Data Source'!C2/200*100&gt;=60,"A-",IF('Data Source'!C2/200*100&gt;=50,"B",IF('Data Source'!C2/200*100&gt;=40,"C",IF('Data Source'!C2/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D3" s="6">
+        <f>IF('Data Source'!D2/200*100&gt;=80,"A+",IF('Data Source'!D2/200*100&gt;=70,"A",IF('Data Source'!D2/200*100&gt;=60,"A-",IF('Data Source'!D2/200*100&gt;=50,"B",IF('Data Source'!D2/200*100&gt;=40,"C",IF('Data Source'!D2/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E3" s="6">
+        <f>IF('Data Source'!E2&gt;=80,"A+",IF('Data Source'!E2&gt;=70,"A",IF('Data Source'!E2&gt;=60,"A-",IF('Data Source'!E2&gt;=50,"B",IF('Data Source'!E2&gt;=40,"C",IF('Data Source'!E2&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F3" s="6">
+        <f>IF('Data Source'!F2/200*100&gt;=80,"A+",IF('Data Source'!F2/200*100&gt;=70,"A",IF('Data Source'!F2/200*100&gt;=60,"A-",IF('Data Source'!F2/200*100&gt;=50,"B",IF('Data Source'!F2/200*100&gt;=40,"C",IF('Data Source'!F2/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G3" s="6">
+        <f>IF('Data Source'!G2/200*100&gt;=80,"A+",IF('Data Source'!G2/200*100&gt;=70,"A",IF('Data Source'!G2/200*100&gt;=60,"A-",IF('Data Source'!G2/200*100&gt;=50,"B",IF('Data Source'!G2/200*100&gt;=40,"C",IF('Data Source'!G2/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H3" s="6">
+        <f>IF('Data Source'!H2&gt;=80,"A+",IF('Data Source'!H2&gt;=70,"A",IF('Data Source'!H2&gt;=60,"A-",IF('Data Source'!H2&gt;=50,"B",IF('Data Source'!H2&gt;=40,"C",IF('Data Source'!H2&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I3" s="6">
+        <f>IF('Data Source'!I2&gt;=80,"A+",IF('Data Source'!I2&gt;=70,"A",IF('Data Source'!I2&gt;=60,"A-",IF('Data Source'!I2&gt;=50,"B",IF('Data Source'!I2&gt;=40,"C",IF('Data Source'!I2&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J3" s="6">
+        <f>IF('Data Source'!J2&gt;=80,"A+",IF('Data Source'!J2&gt;=70,"A",IF('Data Source'!J2&gt;=60,"A-",IF('Data Source'!J2&gt;=50,"B",IF('Data Source'!J2&gt;=40,"C",IF('Data Source'!J2&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K3" s="6">
+        <f>IF('Data Source'!K2&gt;=80,"A+",IF('Data Source'!K2&gt;=70,"A",IF('Data Source'!K2&gt;=60,"A-",IF('Data Source'!K2&gt;=50,"B",IF('Data Source'!K2&gt;=40,"C",IF('Data Source'!K2&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L3" s="6">
+        <f>IF('Data Source'!L2&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M3" s="6">
+        <f>IF('Data Source'!M2&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N3" s="5">
+        <f>'Data Source'!P2</f>
+        <v/>
+      </c>
+      <c r="O3" s="6">
+        <f>'Data Source'!Q2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6">
+        <f>'Data Source'!A3</f>
+        <v/>
+      </c>
+      <c r="B4">
+        <f>'Data Source'!B3</f>
+        <v/>
+      </c>
+      <c r="C4" s="6">
+        <f>IF('Data Source'!C3/200*100&gt;=80,"A+",IF('Data Source'!C3/200*100&gt;=70,"A",IF('Data Source'!C3/200*100&gt;=60,"A-",IF('Data Source'!C3/200*100&gt;=50,"B",IF('Data Source'!C3/200*100&gt;=40,"C",IF('Data Source'!C3/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D4" s="6">
+        <f>IF('Data Source'!D3/200*100&gt;=80,"A+",IF('Data Source'!D3/200*100&gt;=70,"A",IF('Data Source'!D3/200*100&gt;=60,"A-",IF('Data Source'!D3/200*100&gt;=50,"B",IF('Data Source'!D3/200*100&gt;=40,"C",IF('Data Source'!D3/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E4" s="6">
+        <f>IF('Data Source'!E3&gt;=80,"A+",IF('Data Source'!E3&gt;=70,"A",IF('Data Source'!E3&gt;=60,"A-",IF('Data Source'!E3&gt;=50,"B",IF('Data Source'!E3&gt;=40,"C",IF('Data Source'!E3&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F4" s="6">
+        <f>IF('Data Source'!F3/200*100&gt;=80,"A+",IF('Data Source'!F3/200*100&gt;=70,"A",IF('Data Source'!F3/200*100&gt;=60,"A-",IF('Data Source'!F3/200*100&gt;=50,"B",IF('Data Source'!F3/200*100&gt;=40,"C",IF('Data Source'!F3/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G4" s="6">
+        <f>IF('Data Source'!G3/200*100&gt;=80,"A+",IF('Data Source'!G3/200*100&gt;=70,"A",IF('Data Source'!G3/200*100&gt;=60,"A-",IF('Data Source'!G3/200*100&gt;=50,"B",IF('Data Source'!G3/200*100&gt;=40,"C",IF('Data Source'!G3/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H4" s="6">
+        <f>IF('Data Source'!H3&gt;=80,"A+",IF('Data Source'!H3&gt;=70,"A",IF('Data Source'!H3&gt;=60,"A-",IF('Data Source'!H3&gt;=50,"B",IF('Data Source'!H3&gt;=40,"C",IF('Data Source'!H3&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I4" s="6">
+        <f>IF('Data Source'!I3&gt;=80,"A+",IF('Data Source'!I3&gt;=70,"A",IF('Data Source'!I3&gt;=60,"A-",IF('Data Source'!I3&gt;=50,"B",IF('Data Source'!I3&gt;=40,"C",IF('Data Source'!I3&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J4" s="6">
+        <f>IF('Data Source'!J3&gt;=80,"A+",IF('Data Source'!J3&gt;=70,"A",IF('Data Source'!J3&gt;=60,"A-",IF('Data Source'!J3&gt;=50,"B",IF('Data Source'!J3&gt;=40,"C",IF('Data Source'!J3&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K4" s="6">
+        <f>IF('Data Source'!K3&gt;=80,"A+",IF('Data Source'!K3&gt;=70,"A",IF('Data Source'!K3&gt;=60,"A-",IF('Data Source'!K3&gt;=50,"B",IF('Data Source'!K3&gt;=40,"C",IF('Data Source'!K3&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L4" s="6">
+        <f>IF('Data Source'!L3&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M4" s="6">
+        <f>IF('Data Source'!M3&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N4" s="5">
+        <f>'Data Source'!P3</f>
+        <v/>
+      </c>
+      <c r="O4" s="6">
+        <f>'Data Source'!Q3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <f>'Data Source'!A4</f>
+        <v/>
+      </c>
+      <c r="B5">
+        <f>'Data Source'!B4</f>
+        <v/>
+      </c>
+      <c r="C5" s="6">
+        <f>IF('Data Source'!C4/200*100&gt;=80,"A+",IF('Data Source'!C4/200*100&gt;=70,"A",IF('Data Source'!C4/200*100&gt;=60,"A-",IF('Data Source'!C4/200*100&gt;=50,"B",IF('Data Source'!C4/200*100&gt;=40,"C",IF('Data Source'!C4/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D5" s="6">
+        <f>IF('Data Source'!D4/200*100&gt;=80,"A+",IF('Data Source'!D4/200*100&gt;=70,"A",IF('Data Source'!D4/200*100&gt;=60,"A-",IF('Data Source'!D4/200*100&gt;=50,"B",IF('Data Source'!D4/200*100&gt;=40,"C",IF('Data Source'!D4/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E5" s="6">
+        <f>IF('Data Source'!E4&gt;=80,"A+",IF('Data Source'!E4&gt;=70,"A",IF('Data Source'!E4&gt;=60,"A-",IF('Data Source'!E4&gt;=50,"B",IF('Data Source'!E4&gt;=40,"C",IF('Data Source'!E4&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F5" s="6">
+        <f>IF('Data Source'!F4/200*100&gt;=80,"A+",IF('Data Source'!F4/200*100&gt;=70,"A",IF('Data Source'!F4/200*100&gt;=60,"A-",IF('Data Source'!F4/200*100&gt;=50,"B",IF('Data Source'!F4/200*100&gt;=40,"C",IF('Data Source'!F4/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G5" s="6">
+        <f>IF('Data Source'!G4/200*100&gt;=80,"A+",IF('Data Source'!G4/200*100&gt;=70,"A",IF('Data Source'!G4/200*100&gt;=60,"A-",IF('Data Source'!G4/200*100&gt;=50,"B",IF('Data Source'!G4/200*100&gt;=40,"C",IF('Data Source'!G4/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H5" s="6">
+        <f>IF('Data Source'!H4&gt;=80,"A+",IF('Data Source'!H4&gt;=70,"A",IF('Data Source'!H4&gt;=60,"A-",IF('Data Source'!H4&gt;=50,"B",IF('Data Source'!H4&gt;=40,"C",IF('Data Source'!H4&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I5" s="6">
+        <f>IF('Data Source'!I4&gt;=80,"A+",IF('Data Source'!I4&gt;=70,"A",IF('Data Source'!I4&gt;=60,"A-",IF('Data Source'!I4&gt;=50,"B",IF('Data Source'!I4&gt;=40,"C",IF('Data Source'!I4&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J5" s="6">
+        <f>IF('Data Source'!J4&gt;=80,"A+",IF('Data Source'!J4&gt;=70,"A",IF('Data Source'!J4&gt;=60,"A-",IF('Data Source'!J4&gt;=50,"B",IF('Data Source'!J4&gt;=40,"C",IF('Data Source'!J4&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K5" s="6">
+        <f>IF('Data Source'!K4&gt;=80,"A+",IF('Data Source'!K4&gt;=70,"A",IF('Data Source'!K4&gt;=60,"A-",IF('Data Source'!K4&gt;=50,"B",IF('Data Source'!K4&gt;=40,"C",IF('Data Source'!K4&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L5" s="6">
+        <f>IF('Data Source'!L4&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M5" s="6">
+        <f>IF('Data Source'!M4&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N5" s="5">
+        <f>'Data Source'!P4</f>
+        <v/>
+      </c>
+      <c r="O5" s="6">
+        <f>'Data Source'!Q4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6">
+        <f>'Data Source'!A5</f>
+        <v/>
+      </c>
+      <c r="B6">
+        <f>'Data Source'!B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="6">
+        <f>IF('Data Source'!C5/200*100&gt;=80,"A+",IF('Data Source'!C5/200*100&gt;=70,"A",IF('Data Source'!C5/200*100&gt;=60,"A-",IF('Data Source'!C5/200*100&gt;=50,"B",IF('Data Source'!C5/200*100&gt;=40,"C",IF('Data Source'!C5/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D6" s="6">
+        <f>IF('Data Source'!D5/200*100&gt;=80,"A+",IF('Data Source'!D5/200*100&gt;=70,"A",IF('Data Source'!D5/200*100&gt;=60,"A-",IF('Data Source'!D5/200*100&gt;=50,"B",IF('Data Source'!D5/200*100&gt;=40,"C",IF('Data Source'!D5/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E6" s="6">
+        <f>IF('Data Source'!E5&gt;=80,"A+",IF('Data Source'!E5&gt;=70,"A",IF('Data Source'!E5&gt;=60,"A-",IF('Data Source'!E5&gt;=50,"B",IF('Data Source'!E5&gt;=40,"C",IF('Data Source'!E5&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F6" s="6">
+        <f>IF('Data Source'!F5/200*100&gt;=80,"A+",IF('Data Source'!F5/200*100&gt;=70,"A",IF('Data Source'!F5/200*100&gt;=60,"A-",IF('Data Source'!F5/200*100&gt;=50,"B",IF('Data Source'!F5/200*100&gt;=40,"C",IF('Data Source'!F5/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G6" s="6">
+        <f>IF('Data Source'!G5/200*100&gt;=80,"A+",IF('Data Source'!G5/200*100&gt;=70,"A",IF('Data Source'!G5/200*100&gt;=60,"A-",IF('Data Source'!G5/200*100&gt;=50,"B",IF('Data Source'!G5/200*100&gt;=40,"C",IF('Data Source'!G5/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H6" s="6">
+        <f>IF('Data Source'!H5&gt;=80,"A+",IF('Data Source'!H5&gt;=70,"A",IF('Data Source'!H5&gt;=60,"A-",IF('Data Source'!H5&gt;=50,"B",IF('Data Source'!H5&gt;=40,"C",IF('Data Source'!H5&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I6" s="6">
+        <f>IF('Data Source'!I5&gt;=80,"A+",IF('Data Source'!I5&gt;=70,"A",IF('Data Source'!I5&gt;=60,"A-",IF('Data Source'!I5&gt;=50,"B",IF('Data Source'!I5&gt;=40,"C",IF('Data Source'!I5&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J6" s="6">
+        <f>IF('Data Source'!J5&gt;=80,"A+",IF('Data Source'!J5&gt;=70,"A",IF('Data Source'!J5&gt;=60,"A-",IF('Data Source'!J5&gt;=50,"B",IF('Data Source'!J5&gt;=40,"C",IF('Data Source'!J5&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K6" s="6">
+        <f>IF('Data Source'!K5&gt;=80,"A+",IF('Data Source'!K5&gt;=70,"A",IF('Data Source'!K5&gt;=60,"A-",IF('Data Source'!K5&gt;=50,"B",IF('Data Source'!K5&gt;=40,"C",IF('Data Source'!K5&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L6" s="6">
+        <f>IF('Data Source'!L5&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M6" s="6">
+        <f>IF('Data Source'!M5&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N6" s="5">
+        <f>'Data Source'!P5</f>
+        <v/>
+      </c>
+      <c r="O6" s="6">
+        <f>'Data Source'!Q5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6">
+        <f>'Data Source'!A6</f>
+        <v/>
+      </c>
+      <c r="B7">
+        <f>'Data Source'!B6</f>
+        <v/>
+      </c>
+      <c r="C7" s="6">
+        <f>IF('Data Source'!C6/200*100&gt;=80,"A+",IF('Data Source'!C6/200*100&gt;=70,"A",IF('Data Source'!C6/200*100&gt;=60,"A-",IF('Data Source'!C6/200*100&gt;=50,"B",IF('Data Source'!C6/200*100&gt;=40,"C",IF('Data Source'!C6/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D7" s="6">
+        <f>IF('Data Source'!D6/200*100&gt;=80,"A+",IF('Data Source'!D6/200*100&gt;=70,"A",IF('Data Source'!D6/200*100&gt;=60,"A-",IF('Data Source'!D6/200*100&gt;=50,"B",IF('Data Source'!D6/200*100&gt;=40,"C",IF('Data Source'!D6/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E7" s="6">
+        <f>IF('Data Source'!E6&gt;=80,"A+",IF('Data Source'!E6&gt;=70,"A",IF('Data Source'!E6&gt;=60,"A-",IF('Data Source'!E6&gt;=50,"B",IF('Data Source'!E6&gt;=40,"C",IF('Data Source'!E6&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F7" s="6">
+        <f>IF('Data Source'!F6/200*100&gt;=80,"A+",IF('Data Source'!F6/200*100&gt;=70,"A",IF('Data Source'!F6/200*100&gt;=60,"A-",IF('Data Source'!F6/200*100&gt;=50,"B",IF('Data Source'!F6/200*100&gt;=40,"C",IF('Data Source'!F6/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G7" s="6">
+        <f>IF('Data Source'!G6/200*100&gt;=80,"A+",IF('Data Source'!G6/200*100&gt;=70,"A",IF('Data Source'!G6/200*100&gt;=60,"A-",IF('Data Source'!G6/200*100&gt;=50,"B",IF('Data Source'!G6/200*100&gt;=40,"C",IF('Data Source'!G6/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H7" s="6">
+        <f>IF('Data Source'!H6&gt;=80,"A+",IF('Data Source'!H6&gt;=70,"A",IF('Data Source'!H6&gt;=60,"A-",IF('Data Source'!H6&gt;=50,"B",IF('Data Source'!H6&gt;=40,"C",IF('Data Source'!H6&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I7" s="6">
+        <f>IF('Data Source'!I6&gt;=80,"A+",IF('Data Source'!I6&gt;=70,"A",IF('Data Source'!I6&gt;=60,"A-",IF('Data Source'!I6&gt;=50,"B",IF('Data Source'!I6&gt;=40,"C",IF('Data Source'!I6&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J7" s="6">
+        <f>IF('Data Source'!J6&gt;=80,"A+",IF('Data Source'!J6&gt;=70,"A",IF('Data Source'!J6&gt;=60,"A-",IF('Data Source'!J6&gt;=50,"B",IF('Data Source'!J6&gt;=40,"C",IF('Data Source'!J6&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K7" s="6">
+        <f>IF('Data Source'!K6&gt;=80,"A+",IF('Data Source'!K6&gt;=70,"A",IF('Data Source'!K6&gt;=60,"A-",IF('Data Source'!K6&gt;=50,"B",IF('Data Source'!K6&gt;=40,"C",IF('Data Source'!K6&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L7" s="6">
+        <f>IF('Data Source'!L6&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M7" s="6">
+        <f>IF('Data Source'!M6&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N7" s="5">
+        <f>'Data Source'!P6</f>
+        <v/>
+      </c>
+      <c r="O7" s="6">
+        <f>'Data Source'!Q6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6">
+        <f>'Data Source'!A7</f>
+        <v/>
+      </c>
+      <c r="B8">
+        <f>'Data Source'!B7</f>
+        <v/>
+      </c>
+      <c r="C8" s="6">
+        <f>IF('Data Source'!C7/200*100&gt;=80,"A+",IF('Data Source'!C7/200*100&gt;=70,"A",IF('Data Source'!C7/200*100&gt;=60,"A-",IF('Data Source'!C7/200*100&gt;=50,"B",IF('Data Source'!C7/200*100&gt;=40,"C",IF('Data Source'!C7/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D8" s="6">
+        <f>IF('Data Source'!D7/200*100&gt;=80,"A+",IF('Data Source'!D7/200*100&gt;=70,"A",IF('Data Source'!D7/200*100&gt;=60,"A-",IF('Data Source'!D7/200*100&gt;=50,"B",IF('Data Source'!D7/200*100&gt;=40,"C",IF('Data Source'!D7/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E8" s="6">
+        <f>IF('Data Source'!E7&gt;=80,"A+",IF('Data Source'!E7&gt;=70,"A",IF('Data Source'!E7&gt;=60,"A-",IF('Data Source'!E7&gt;=50,"B",IF('Data Source'!E7&gt;=40,"C",IF('Data Source'!E7&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F8" s="6">
+        <f>IF('Data Source'!F7/200*100&gt;=80,"A+",IF('Data Source'!F7/200*100&gt;=70,"A",IF('Data Source'!F7/200*100&gt;=60,"A-",IF('Data Source'!F7/200*100&gt;=50,"B",IF('Data Source'!F7/200*100&gt;=40,"C",IF('Data Source'!F7/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G8" s="6">
+        <f>IF('Data Source'!G7/200*100&gt;=80,"A+",IF('Data Source'!G7/200*100&gt;=70,"A",IF('Data Source'!G7/200*100&gt;=60,"A-",IF('Data Source'!G7/200*100&gt;=50,"B",IF('Data Source'!G7/200*100&gt;=40,"C",IF('Data Source'!G7/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H8" s="6">
+        <f>IF('Data Source'!H7&gt;=80,"A+",IF('Data Source'!H7&gt;=70,"A",IF('Data Source'!H7&gt;=60,"A-",IF('Data Source'!H7&gt;=50,"B",IF('Data Source'!H7&gt;=40,"C",IF('Data Source'!H7&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I8" s="6">
+        <f>IF('Data Source'!I7&gt;=80,"A+",IF('Data Source'!I7&gt;=70,"A",IF('Data Source'!I7&gt;=60,"A-",IF('Data Source'!I7&gt;=50,"B",IF('Data Source'!I7&gt;=40,"C",IF('Data Source'!I7&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J8" s="6">
+        <f>IF('Data Source'!J7&gt;=80,"A+",IF('Data Source'!J7&gt;=70,"A",IF('Data Source'!J7&gt;=60,"A-",IF('Data Source'!J7&gt;=50,"B",IF('Data Source'!J7&gt;=40,"C",IF('Data Source'!J7&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K8" s="6">
+        <f>IF('Data Source'!K7&gt;=80,"A+",IF('Data Source'!K7&gt;=70,"A",IF('Data Source'!K7&gt;=60,"A-",IF('Data Source'!K7&gt;=50,"B",IF('Data Source'!K7&gt;=40,"C",IF('Data Source'!K7&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L8" s="6">
+        <f>IF('Data Source'!L7&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M8" s="6">
+        <f>IF('Data Source'!M7&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N8" s="5">
+        <f>'Data Source'!P7</f>
+        <v/>
+      </c>
+      <c r="O8" s="6">
+        <f>'Data Source'!Q7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6">
+        <f>'Data Source'!A8</f>
+        <v/>
+      </c>
+      <c r="B9">
+        <f>'Data Source'!B8</f>
+        <v/>
+      </c>
+      <c r="C9" s="6">
+        <f>IF('Data Source'!C8/200*100&gt;=80,"A+",IF('Data Source'!C8/200*100&gt;=70,"A",IF('Data Source'!C8/200*100&gt;=60,"A-",IF('Data Source'!C8/200*100&gt;=50,"B",IF('Data Source'!C8/200*100&gt;=40,"C",IF('Data Source'!C8/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D9" s="6">
+        <f>IF('Data Source'!D8/200*100&gt;=80,"A+",IF('Data Source'!D8/200*100&gt;=70,"A",IF('Data Source'!D8/200*100&gt;=60,"A-",IF('Data Source'!D8/200*100&gt;=50,"B",IF('Data Source'!D8/200*100&gt;=40,"C",IF('Data Source'!D8/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E9" s="6">
+        <f>IF('Data Source'!E8&gt;=80,"A+",IF('Data Source'!E8&gt;=70,"A",IF('Data Source'!E8&gt;=60,"A-",IF('Data Source'!E8&gt;=50,"B",IF('Data Source'!E8&gt;=40,"C",IF('Data Source'!E8&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F9" s="6">
+        <f>IF('Data Source'!F8/200*100&gt;=80,"A+",IF('Data Source'!F8/200*100&gt;=70,"A",IF('Data Source'!F8/200*100&gt;=60,"A-",IF('Data Source'!F8/200*100&gt;=50,"B",IF('Data Source'!F8/200*100&gt;=40,"C",IF('Data Source'!F8/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G9" s="6">
+        <f>IF('Data Source'!G8/200*100&gt;=80,"A+",IF('Data Source'!G8/200*100&gt;=70,"A",IF('Data Source'!G8/200*100&gt;=60,"A-",IF('Data Source'!G8/200*100&gt;=50,"B",IF('Data Source'!G8/200*100&gt;=40,"C",IF('Data Source'!G8/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H9" s="6">
+        <f>IF('Data Source'!H8&gt;=80,"A+",IF('Data Source'!H8&gt;=70,"A",IF('Data Source'!H8&gt;=60,"A-",IF('Data Source'!H8&gt;=50,"B",IF('Data Source'!H8&gt;=40,"C",IF('Data Source'!H8&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I9" s="6">
+        <f>IF('Data Source'!I8&gt;=80,"A+",IF('Data Source'!I8&gt;=70,"A",IF('Data Source'!I8&gt;=60,"A-",IF('Data Source'!I8&gt;=50,"B",IF('Data Source'!I8&gt;=40,"C",IF('Data Source'!I8&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J9" s="6">
+        <f>IF('Data Source'!J8&gt;=80,"A+",IF('Data Source'!J8&gt;=70,"A",IF('Data Source'!J8&gt;=60,"A-",IF('Data Source'!J8&gt;=50,"B",IF('Data Source'!J8&gt;=40,"C",IF('Data Source'!J8&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K9" s="6">
+        <f>IF('Data Source'!K8&gt;=80,"A+",IF('Data Source'!K8&gt;=70,"A",IF('Data Source'!K8&gt;=60,"A-",IF('Data Source'!K8&gt;=50,"B",IF('Data Source'!K8&gt;=40,"C",IF('Data Source'!K8&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L9" s="6">
+        <f>IF('Data Source'!L8&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M9" s="6">
+        <f>IF('Data Source'!M8&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N9" s="5">
+        <f>'Data Source'!P8</f>
+        <v/>
+      </c>
+      <c r="O9" s="6">
+        <f>'Data Source'!Q8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6">
+        <f>'Data Source'!A9</f>
+        <v/>
+      </c>
+      <c r="B10">
+        <f>'Data Source'!B9</f>
+        <v/>
+      </c>
+      <c r="C10" s="6">
+        <f>IF('Data Source'!C9/200*100&gt;=80,"A+",IF('Data Source'!C9/200*100&gt;=70,"A",IF('Data Source'!C9/200*100&gt;=60,"A-",IF('Data Source'!C9/200*100&gt;=50,"B",IF('Data Source'!C9/200*100&gt;=40,"C",IF('Data Source'!C9/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D10" s="6">
+        <f>IF('Data Source'!D9/200*100&gt;=80,"A+",IF('Data Source'!D9/200*100&gt;=70,"A",IF('Data Source'!D9/200*100&gt;=60,"A-",IF('Data Source'!D9/200*100&gt;=50,"B",IF('Data Source'!D9/200*100&gt;=40,"C",IF('Data Source'!D9/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E10" s="6">
+        <f>IF('Data Source'!E9&gt;=80,"A+",IF('Data Source'!E9&gt;=70,"A",IF('Data Source'!E9&gt;=60,"A-",IF('Data Source'!E9&gt;=50,"B",IF('Data Source'!E9&gt;=40,"C",IF('Data Source'!E9&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F10" s="6">
+        <f>IF('Data Source'!F9/200*100&gt;=80,"A+",IF('Data Source'!F9/200*100&gt;=70,"A",IF('Data Source'!F9/200*100&gt;=60,"A-",IF('Data Source'!F9/200*100&gt;=50,"B",IF('Data Source'!F9/200*100&gt;=40,"C",IF('Data Source'!F9/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G10" s="6">
+        <f>IF('Data Source'!G9/200*100&gt;=80,"A+",IF('Data Source'!G9/200*100&gt;=70,"A",IF('Data Source'!G9/200*100&gt;=60,"A-",IF('Data Source'!G9/200*100&gt;=50,"B",IF('Data Source'!G9/200*100&gt;=40,"C",IF('Data Source'!G9/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H10" s="6">
+        <f>IF('Data Source'!H9&gt;=80,"A+",IF('Data Source'!H9&gt;=70,"A",IF('Data Source'!H9&gt;=60,"A-",IF('Data Source'!H9&gt;=50,"B",IF('Data Source'!H9&gt;=40,"C",IF('Data Source'!H9&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I10" s="6">
+        <f>IF('Data Source'!I9&gt;=80,"A+",IF('Data Source'!I9&gt;=70,"A",IF('Data Source'!I9&gt;=60,"A-",IF('Data Source'!I9&gt;=50,"B",IF('Data Source'!I9&gt;=40,"C",IF('Data Source'!I9&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J10" s="6">
+        <f>IF('Data Source'!J9&gt;=80,"A+",IF('Data Source'!J9&gt;=70,"A",IF('Data Source'!J9&gt;=60,"A-",IF('Data Source'!J9&gt;=50,"B",IF('Data Source'!J9&gt;=40,"C",IF('Data Source'!J9&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K10" s="6">
+        <f>IF('Data Source'!K9&gt;=80,"A+",IF('Data Source'!K9&gt;=70,"A",IF('Data Source'!K9&gt;=60,"A-",IF('Data Source'!K9&gt;=50,"B",IF('Data Source'!K9&gt;=40,"C",IF('Data Source'!K9&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L10" s="6">
+        <f>IF('Data Source'!L9&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M10" s="6">
+        <f>IF('Data Source'!M9&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N10" s="5">
+        <f>'Data Source'!P9</f>
+        <v/>
+      </c>
+      <c r="O10" s="6">
+        <f>'Data Source'!Q9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6">
+        <f>'Data Source'!A10</f>
+        <v/>
+      </c>
+      <c r="B11">
+        <f>'Data Source'!B10</f>
+        <v/>
+      </c>
+      <c r="C11" s="6">
+        <f>IF('Data Source'!C10/200*100&gt;=80,"A+",IF('Data Source'!C10/200*100&gt;=70,"A",IF('Data Source'!C10/200*100&gt;=60,"A-",IF('Data Source'!C10/200*100&gt;=50,"B",IF('Data Source'!C10/200*100&gt;=40,"C",IF('Data Source'!C10/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D11" s="6">
+        <f>IF('Data Source'!D10/200*100&gt;=80,"A+",IF('Data Source'!D10/200*100&gt;=70,"A",IF('Data Source'!D10/200*100&gt;=60,"A-",IF('Data Source'!D10/200*100&gt;=50,"B",IF('Data Source'!D10/200*100&gt;=40,"C",IF('Data Source'!D10/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E11" s="6">
+        <f>IF('Data Source'!E10&gt;=80,"A+",IF('Data Source'!E10&gt;=70,"A",IF('Data Source'!E10&gt;=60,"A-",IF('Data Source'!E10&gt;=50,"B",IF('Data Source'!E10&gt;=40,"C",IF('Data Source'!E10&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F11" s="6">
+        <f>IF('Data Source'!F10/200*100&gt;=80,"A+",IF('Data Source'!F10/200*100&gt;=70,"A",IF('Data Source'!F10/200*100&gt;=60,"A-",IF('Data Source'!F10/200*100&gt;=50,"B",IF('Data Source'!F10/200*100&gt;=40,"C",IF('Data Source'!F10/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G11" s="6">
+        <f>IF('Data Source'!G10/200*100&gt;=80,"A+",IF('Data Source'!G10/200*100&gt;=70,"A",IF('Data Source'!G10/200*100&gt;=60,"A-",IF('Data Source'!G10/200*100&gt;=50,"B",IF('Data Source'!G10/200*100&gt;=40,"C",IF('Data Source'!G10/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H11" s="6">
+        <f>IF('Data Source'!H10&gt;=80,"A+",IF('Data Source'!H10&gt;=70,"A",IF('Data Source'!H10&gt;=60,"A-",IF('Data Source'!H10&gt;=50,"B",IF('Data Source'!H10&gt;=40,"C",IF('Data Source'!H10&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I11" s="6">
+        <f>IF('Data Source'!I10&gt;=80,"A+",IF('Data Source'!I10&gt;=70,"A",IF('Data Source'!I10&gt;=60,"A-",IF('Data Source'!I10&gt;=50,"B",IF('Data Source'!I10&gt;=40,"C",IF('Data Source'!I10&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J11" s="6">
+        <f>IF('Data Source'!J10&gt;=80,"A+",IF('Data Source'!J10&gt;=70,"A",IF('Data Source'!J10&gt;=60,"A-",IF('Data Source'!J10&gt;=50,"B",IF('Data Source'!J10&gt;=40,"C",IF('Data Source'!J10&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K11" s="6">
+        <f>IF('Data Source'!K10&gt;=80,"A+",IF('Data Source'!K10&gt;=70,"A",IF('Data Source'!K10&gt;=60,"A-",IF('Data Source'!K10&gt;=50,"B",IF('Data Source'!K10&gt;=40,"C",IF('Data Source'!K10&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L11" s="6">
+        <f>IF('Data Source'!L10&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M11" s="6">
+        <f>IF('Data Source'!M10&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N11" s="5">
+        <f>'Data Source'!P10</f>
+        <v/>
+      </c>
+      <c r="O11" s="6">
+        <f>'Data Source'!Q10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6">
+        <f>'Data Source'!A11</f>
+        <v/>
+      </c>
+      <c r="B12">
+        <f>'Data Source'!B11</f>
+        <v/>
+      </c>
+      <c r="C12" s="6">
+        <f>IF('Data Source'!C11/200*100&gt;=80,"A+",IF('Data Source'!C11/200*100&gt;=70,"A",IF('Data Source'!C11/200*100&gt;=60,"A-",IF('Data Source'!C11/200*100&gt;=50,"B",IF('Data Source'!C11/200*100&gt;=40,"C",IF('Data Source'!C11/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D12" s="6">
+        <f>IF('Data Source'!D11/200*100&gt;=80,"A+",IF('Data Source'!D11/200*100&gt;=70,"A",IF('Data Source'!D11/200*100&gt;=60,"A-",IF('Data Source'!D11/200*100&gt;=50,"B",IF('Data Source'!D11/200*100&gt;=40,"C",IF('Data Source'!D11/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E12" s="6">
+        <f>IF('Data Source'!E11&gt;=80,"A+",IF('Data Source'!E11&gt;=70,"A",IF('Data Source'!E11&gt;=60,"A-",IF('Data Source'!E11&gt;=50,"B",IF('Data Source'!E11&gt;=40,"C",IF('Data Source'!E11&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F12" s="6">
+        <f>IF('Data Source'!F11/200*100&gt;=80,"A+",IF('Data Source'!F11/200*100&gt;=70,"A",IF('Data Source'!F11/200*100&gt;=60,"A-",IF('Data Source'!F11/200*100&gt;=50,"B",IF('Data Source'!F11/200*100&gt;=40,"C",IF('Data Source'!F11/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G12" s="6">
+        <f>IF('Data Source'!G11/200*100&gt;=80,"A+",IF('Data Source'!G11/200*100&gt;=70,"A",IF('Data Source'!G11/200*100&gt;=60,"A-",IF('Data Source'!G11/200*100&gt;=50,"B",IF('Data Source'!G11/200*100&gt;=40,"C",IF('Data Source'!G11/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H12" s="6">
+        <f>IF('Data Source'!H11&gt;=80,"A+",IF('Data Source'!H11&gt;=70,"A",IF('Data Source'!H11&gt;=60,"A-",IF('Data Source'!H11&gt;=50,"B",IF('Data Source'!H11&gt;=40,"C",IF('Data Source'!H11&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I12" s="6">
+        <f>IF('Data Source'!I11&gt;=80,"A+",IF('Data Source'!I11&gt;=70,"A",IF('Data Source'!I11&gt;=60,"A-",IF('Data Source'!I11&gt;=50,"B",IF('Data Source'!I11&gt;=40,"C",IF('Data Source'!I11&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J12" s="6">
+        <f>IF('Data Source'!J11&gt;=80,"A+",IF('Data Source'!J11&gt;=70,"A",IF('Data Source'!J11&gt;=60,"A-",IF('Data Source'!J11&gt;=50,"B",IF('Data Source'!J11&gt;=40,"C",IF('Data Source'!J11&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K12" s="6">
+        <f>IF('Data Source'!K11&gt;=80,"A+",IF('Data Source'!K11&gt;=70,"A",IF('Data Source'!K11&gt;=60,"A-",IF('Data Source'!K11&gt;=50,"B",IF('Data Source'!K11&gt;=40,"C",IF('Data Source'!K11&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L12" s="6">
+        <f>IF('Data Source'!L11&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M12" s="6">
+        <f>IF('Data Source'!M11&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N12" s="5">
+        <f>'Data Source'!P11</f>
+        <v/>
+      </c>
+      <c r="O12" s="6">
+        <f>'Data Source'!Q11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6">
+        <f>'Data Source'!A12</f>
+        <v/>
+      </c>
+      <c r="B13">
+        <f>'Data Source'!B12</f>
+        <v/>
+      </c>
+      <c r="C13" s="6">
+        <f>IF('Data Source'!C12/200*100&gt;=80,"A+",IF('Data Source'!C12/200*100&gt;=70,"A",IF('Data Source'!C12/200*100&gt;=60,"A-",IF('Data Source'!C12/200*100&gt;=50,"B",IF('Data Source'!C12/200*100&gt;=40,"C",IF('Data Source'!C12/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D13" s="6">
+        <f>IF('Data Source'!D12/200*100&gt;=80,"A+",IF('Data Source'!D12/200*100&gt;=70,"A",IF('Data Source'!D12/200*100&gt;=60,"A-",IF('Data Source'!D12/200*100&gt;=50,"B",IF('Data Source'!D12/200*100&gt;=40,"C",IF('Data Source'!D12/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E13" s="6">
+        <f>IF('Data Source'!E12&gt;=80,"A+",IF('Data Source'!E12&gt;=70,"A",IF('Data Source'!E12&gt;=60,"A-",IF('Data Source'!E12&gt;=50,"B",IF('Data Source'!E12&gt;=40,"C",IF('Data Source'!E12&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F13" s="6">
+        <f>IF('Data Source'!F12/200*100&gt;=80,"A+",IF('Data Source'!F12/200*100&gt;=70,"A",IF('Data Source'!F12/200*100&gt;=60,"A-",IF('Data Source'!F12/200*100&gt;=50,"B",IF('Data Source'!F12/200*100&gt;=40,"C",IF('Data Source'!F12/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G13" s="6">
+        <f>IF('Data Source'!G12/200*100&gt;=80,"A+",IF('Data Source'!G12/200*100&gt;=70,"A",IF('Data Source'!G12/200*100&gt;=60,"A-",IF('Data Source'!G12/200*100&gt;=50,"B",IF('Data Source'!G12/200*100&gt;=40,"C",IF('Data Source'!G12/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H13" s="6">
+        <f>IF('Data Source'!H12&gt;=80,"A+",IF('Data Source'!H12&gt;=70,"A",IF('Data Source'!H12&gt;=60,"A-",IF('Data Source'!H12&gt;=50,"B",IF('Data Source'!H12&gt;=40,"C",IF('Data Source'!H12&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I13" s="6">
+        <f>IF('Data Source'!I12&gt;=80,"A+",IF('Data Source'!I12&gt;=70,"A",IF('Data Source'!I12&gt;=60,"A-",IF('Data Source'!I12&gt;=50,"B",IF('Data Source'!I12&gt;=40,"C",IF('Data Source'!I12&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J13" s="6">
+        <f>IF('Data Source'!J12&gt;=80,"A+",IF('Data Source'!J12&gt;=70,"A",IF('Data Source'!J12&gt;=60,"A-",IF('Data Source'!J12&gt;=50,"B",IF('Data Source'!J12&gt;=40,"C",IF('Data Source'!J12&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K13" s="6">
+        <f>IF('Data Source'!K12&gt;=80,"A+",IF('Data Source'!K12&gt;=70,"A",IF('Data Source'!K12&gt;=60,"A-",IF('Data Source'!K12&gt;=50,"B",IF('Data Source'!K12&gt;=40,"C",IF('Data Source'!K12&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L13" s="6">
+        <f>IF('Data Source'!L12&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M13" s="6">
+        <f>IF('Data Source'!M12&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N13" s="5">
+        <f>'Data Source'!P12</f>
+        <v/>
+      </c>
+      <c r="O13" s="6">
+        <f>'Data Source'!Q12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6">
+        <f>'Data Source'!A13</f>
+        <v/>
+      </c>
+      <c r="B14">
+        <f>'Data Source'!B13</f>
+        <v/>
+      </c>
+      <c r="C14" s="6">
+        <f>IF('Data Source'!C13/200*100&gt;=80,"A+",IF('Data Source'!C13/200*100&gt;=70,"A",IF('Data Source'!C13/200*100&gt;=60,"A-",IF('Data Source'!C13/200*100&gt;=50,"B",IF('Data Source'!C13/200*100&gt;=40,"C",IF('Data Source'!C13/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D14" s="6">
+        <f>IF('Data Source'!D13/200*100&gt;=80,"A+",IF('Data Source'!D13/200*100&gt;=70,"A",IF('Data Source'!D13/200*100&gt;=60,"A-",IF('Data Source'!D13/200*100&gt;=50,"B",IF('Data Source'!D13/200*100&gt;=40,"C",IF('Data Source'!D13/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E14" s="6">
+        <f>IF('Data Source'!E13&gt;=80,"A+",IF('Data Source'!E13&gt;=70,"A",IF('Data Source'!E13&gt;=60,"A-",IF('Data Source'!E13&gt;=50,"B",IF('Data Source'!E13&gt;=40,"C",IF('Data Source'!E13&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F14" s="6">
+        <f>IF('Data Source'!F13/200*100&gt;=80,"A+",IF('Data Source'!F13/200*100&gt;=70,"A",IF('Data Source'!F13/200*100&gt;=60,"A-",IF('Data Source'!F13/200*100&gt;=50,"B",IF('Data Source'!F13/200*100&gt;=40,"C",IF('Data Source'!F13/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G14" s="6">
+        <f>IF('Data Source'!G13/200*100&gt;=80,"A+",IF('Data Source'!G13/200*100&gt;=70,"A",IF('Data Source'!G13/200*100&gt;=60,"A-",IF('Data Source'!G13/200*100&gt;=50,"B",IF('Data Source'!G13/200*100&gt;=40,"C",IF('Data Source'!G13/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H14" s="6">
+        <f>IF('Data Source'!H13&gt;=80,"A+",IF('Data Source'!H13&gt;=70,"A",IF('Data Source'!H13&gt;=60,"A-",IF('Data Source'!H13&gt;=50,"B",IF('Data Source'!H13&gt;=40,"C",IF('Data Source'!H13&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I14" s="6">
+        <f>IF('Data Source'!I13&gt;=80,"A+",IF('Data Source'!I13&gt;=70,"A",IF('Data Source'!I13&gt;=60,"A-",IF('Data Source'!I13&gt;=50,"B",IF('Data Source'!I13&gt;=40,"C",IF('Data Source'!I13&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J14" s="6">
+        <f>IF('Data Source'!J13&gt;=80,"A+",IF('Data Source'!J13&gt;=70,"A",IF('Data Source'!J13&gt;=60,"A-",IF('Data Source'!J13&gt;=50,"B",IF('Data Source'!J13&gt;=40,"C",IF('Data Source'!J13&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K14" s="6">
+        <f>IF('Data Source'!K13&gt;=80,"A+",IF('Data Source'!K13&gt;=70,"A",IF('Data Source'!K13&gt;=60,"A-",IF('Data Source'!K13&gt;=50,"B",IF('Data Source'!K13&gt;=40,"C",IF('Data Source'!K13&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L14" s="6">
+        <f>IF('Data Source'!L13&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M14" s="6">
+        <f>IF('Data Source'!M13&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N14" s="5">
+        <f>'Data Source'!P13</f>
+        <v/>
+      </c>
+      <c r="O14" s="6">
+        <f>'Data Source'!Q13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6">
+        <f>'Data Source'!A14</f>
+        <v/>
+      </c>
+      <c r="B15">
+        <f>'Data Source'!B14</f>
+        <v/>
+      </c>
+      <c r="C15" s="6">
+        <f>IF('Data Source'!C14/200*100&gt;=80,"A+",IF('Data Source'!C14/200*100&gt;=70,"A",IF('Data Source'!C14/200*100&gt;=60,"A-",IF('Data Source'!C14/200*100&gt;=50,"B",IF('Data Source'!C14/200*100&gt;=40,"C",IF('Data Source'!C14/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D15" s="6">
+        <f>IF('Data Source'!D14/200*100&gt;=80,"A+",IF('Data Source'!D14/200*100&gt;=70,"A",IF('Data Source'!D14/200*100&gt;=60,"A-",IF('Data Source'!D14/200*100&gt;=50,"B",IF('Data Source'!D14/200*100&gt;=40,"C",IF('Data Source'!D14/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E15" s="6">
+        <f>IF('Data Source'!E14&gt;=80,"A+",IF('Data Source'!E14&gt;=70,"A",IF('Data Source'!E14&gt;=60,"A-",IF('Data Source'!E14&gt;=50,"B",IF('Data Source'!E14&gt;=40,"C",IF('Data Source'!E14&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F15" s="6">
+        <f>IF('Data Source'!F14/200*100&gt;=80,"A+",IF('Data Source'!F14/200*100&gt;=70,"A",IF('Data Source'!F14/200*100&gt;=60,"A-",IF('Data Source'!F14/200*100&gt;=50,"B",IF('Data Source'!F14/200*100&gt;=40,"C",IF('Data Source'!F14/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G15" s="6">
+        <f>IF('Data Source'!G14/200*100&gt;=80,"A+",IF('Data Source'!G14/200*100&gt;=70,"A",IF('Data Source'!G14/200*100&gt;=60,"A-",IF('Data Source'!G14/200*100&gt;=50,"B",IF('Data Source'!G14/200*100&gt;=40,"C",IF('Data Source'!G14/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H15" s="6">
+        <f>IF('Data Source'!H14&gt;=80,"A+",IF('Data Source'!H14&gt;=70,"A",IF('Data Source'!H14&gt;=60,"A-",IF('Data Source'!H14&gt;=50,"B",IF('Data Source'!H14&gt;=40,"C",IF('Data Source'!H14&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I15" s="6">
+        <f>IF('Data Source'!I14&gt;=80,"A+",IF('Data Source'!I14&gt;=70,"A",IF('Data Source'!I14&gt;=60,"A-",IF('Data Source'!I14&gt;=50,"B",IF('Data Source'!I14&gt;=40,"C",IF('Data Source'!I14&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J15" s="6">
+        <f>IF('Data Source'!J14&gt;=80,"A+",IF('Data Source'!J14&gt;=70,"A",IF('Data Source'!J14&gt;=60,"A-",IF('Data Source'!J14&gt;=50,"B",IF('Data Source'!J14&gt;=40,"C",IF('Data Source'!J14&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K15" s="6">
+        <f>IF('Data Source'!K14&gt;=80,"A+",IF('Data Source'!K14&gt;=70,"A",IF('Data Source'!K14&gt;=60,"A-",IF('Data Source'!K14&gt;=50,"B",IF('Data Source'!K14&gt;=40,"C",IF('Data Source'!K14&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L15" s="6">
+        <f>IF('Data Source'!L14&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M15" s="6">
+        <f>IF('Data Source'!M14&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N15" s="5">
+        <f>'Data Source'!P14</f>
+        <v/>
+      </c>
+      <c r="O15" s="6">
+        <f>'Data Source'!Q14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6">
+        <f>'Data Source'!A15</f>
+        <v/>
+      </c>
+      <c r="B16">
+        <f>'Data Source'!B15</f>
+        <v/>
+      </c>
+      <c r="C16" s="6">
+        <f>IF('Data Source'!C15/200*100&gt;=80,"A+",IF('Data Source'!C15/200*100&gt;=70,"A",IF('Data Source'!C15/200*100&gt;=60,"A-",IF('Data Source'!C15/200*100&gt;=50,"B",IF('Data Source'!C15/200*100&gt;=40,"C",IF('Data Source'!C15/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D16" s="6">
+        <f>IF('Data Source'!D15/200*100&gt;=80,"A+",IF('Data Source'!D15/200*100&gt;=70,"A",IF('Data Source'!D15/200*100&gt;=60,"A-",IF('Data Source'!D15/200*100&gt;=50,"B",IF('Data Source'!D15/200*100&gt;=40,"C",IF('Data Source'!D15/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E16" s="6">
+        <f>IF('Data Source'!E15&gt;=80,"A+",IF('Data Source'!E15&gt;=70,"A",IF('Data Source'!E15&gt;=60,"A-",IF('Data Source'!E15&gt;=50,"B",IF('Data Source'!E15&gt;=40,"C",IF('Data Source'!E15&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F16" s="6">
+        <f>IF('Data Source'!F15/200*100&gt;=80,"A+",IF('Data Source'!F15/200*100&gt;=70,"A",IF('Data Source'!F15/200*100&gt;=60,"A-",IF('Data Source'!F15/200*100&gt;=50,"B",IF('Data Source'!F15/200*100&gt;=40,"C",IF('Data Source'!F15/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G16" s="6">
+        <f>IF('Data Source'!G15/200*100&gt;=80,"A+",IF('Data Source'!G15/200*100&gt;=70,"A",IF('Data Source'!G15/200*100&gt;=60,"A-",IF('Data Source'!G15/200*100&gt;=50,"B",IF('Data Source'!G15/200*100&gt;=40,"C",IF('Data Source'!G15/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H16" s="6">
+        <f>IF('Data Source'!H15&gt;=80,"A+",IF('Data Source'!H15&gt;=70,"A",IF('Data Source'!H15&gt;=60,"A-",IF('Data Source'!H15&gt;=50,"B",IF('Data Source'!H15&gt;=40,"C",IF('Data Source'!H15&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I16" s="6">
+        <f>IF('Data Source'!I15&gt;=80,"A+",IF('Data Source'!I15&gt;=70,"A",IF('Data Source'!I15&gt;=60,"A-",IF('Data Source'!I15&gt;=50,"B",IF('Data Source'!I15&gt;=40,"C",IF('Data Source'!I15&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J16" s="6">
+        <f>IF('Data Source'!J15&gt;=80,"A+",IF('Data Source'!J15&gt;=70,"A",IF('Data Source'!J15&gt;=60,"A-",IF('Data Source'!J15&gt;=50,"B",IF('Data Source'!J15&gt;=40,"C",IF('Data Source'!J15&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K16" s="6">
+        <f>IF('Data Source'!K15&gt;=80,"A+",IF('Data Source'!K15&gt;=70,"A",IF('Data Source'!K15&gt;=60,"A-",IF('Data Source'!K15&gt;=50,"B",IF('Data Source'!K15&gt;=40,"C",IF('Data Source'!K15&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L16" s="6">
+        <f>IF('Data Source'!L15&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M16" s="6">
+        <f>IF('Data Source'!M15&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N16" s="5">
+        <f>'Data Source'!P15</f>
+        <v/>
+      </c>
+      <c r="O16" s="6">
+        <f>'Data Source'!Q15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6">
+        <f>'Data Source'!A16</f>
+        <v/>
+      </c>
+      <c r="B17">
+        <f>'Data Source'!B16</f>
+        <v/>
+      </c>
+      <c r="C17" s="6">
+        <f>IF('Data Source'!C16/200*100&gt;=80,"A+",IF('Data Source'!C16/200*100&gt;=70,"A",IF('Data Source'!C16/200*100&gt;=60,"A-",IF('Data Source'!C16/200*100&gt;=50,"B",IF('Data Source'!C16/200*100&gt;=40,"C",IF('Data Source'!C16/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D17" s="6">
+        <f>IF('Data Source'!D16/200*100&gt;=80,"A+",IF('Data Source'!D16/200*100&gt;=70,"A",IF('Data Source'!D16/200*100&gt;=60,"A-",IF('Data Source'!D16/200*100&gt;=50,"B",IF('Data Source'!D16/200*100&gt;=40,"C",IF('Data Source'!D16/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E17" s="6">
+        <f>IF('Data Source'!E16&gt;=80,"A+",IF('Data Source'!E16&gt;=70,"A",IF('Data Source'!E16&gt;=60,"A-",IF('Data Source'!E16&gt;=50,"B",IF('Data Source'!E16&gt;=40,"C",IF('Data Source'!E16&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F17" s="6">
+        <f>IF('Data Source'!F16/200*100&gt;=80,"A+",IF('Data Source'!F16/200*100&gt;=70,"A",IF('Data Source'!F16/200*100&gt;=60,"A-",IF('Data Source'!F16/200*100&gt;=50,"B",IF('Data Source'!F16/200*100&gt;=40,"C",IF('Data Source'!F16/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G17" s="6">
+        <f>IF('Data Source'!G16/200*100&gt;=80,"A+",IF('Data Source'!G16/200*100&gt;=70,"A",IF('Data Source'!G16/200*100&gt;=60,"A-",IF('Data Source'!G16/200*100&gt;=50,"B",IF('Data Source'!G16/200*100&gt;=40,"C",IF('Data Source'!G16/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H17" s="6">
+        <f>IF('Data Source'!H16&gt;=80,"A+",IF('Data Source'!H16&gt;=70,"A",IF('Data Source'!H16&gt;=60,"A-",IF('Data Source'!H16&gt;=50,"B",IF('Data Source'!H16&gt;=40,"C",IF('Data Source'!H16&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I17" s="6">
+        <f>IF('Data Source'!I16&gt;=80,"A+",IF('Data Source'!I16&gt;=70,"A",IF('Data Source'!I16&gt;=60,"A-",IF('Data Source'!I16&gt;=50,"B",IF('Data Source'!I16&gt;=40,"C",IF('Data Source'!I16&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J17" s="6">
+        <f>IF('Data Source'!J16&gt;=80,"A+",IF('Data Source'!J16&gt;=70,"A",IF('Data Source'!J16&gt;=60,"A-",IF('Data Source'!J16&gt;=50,"B",IF('Data Source'!J16&gt;=40,"C",IF('Data Source'!J16&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K17" s="6">
+        <f>IF('Data Source'!K16&gt;=80,"A+",IF('Data Source'!K16&gt;=70,"A",IF('Data Source'!K16&gt;=60,"A-",IF('Data Source'!K16&gt;=50,"B",IF('Data Source'!K16&gt;=40,"C",IF('Data Source'!K16&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L17" s="6">
+        <f>IF('Data Source'!L16&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M17" s="6">
+        <f>IF('Data Source'!M16&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N17" s="5">
+        <f>'Data Source'!P16</f>
+        <v/>
+      </c>
+      <c r="O17" s="6">
+        <f>'Data Source'!Q16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6">
+        <f>'Data Source'!A17</f>
+        <v/>
+      </c>
+      <c r="B18">
+        <f>'Data Source'!B17</f>
+        <v/>
+      </c>
+      <c r="C18" s="6">
+        <f>IF('Data Source'!C17/200*100&gt;=80,"A+",IF('Data Source'!C17/200*100&gt;=70,"A",IF('Data Source'!C17/200*100&gt;=60,"A-",IF('Data Source'!C17/200*100&gt;=50,"B",IF('Data Source'!C17/200*100&gt;=40,"C",IF('Data Source'!C17/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D18" s="6">
+        <f>IF('Data Source'!D17/200*100&gt;=80,"A+",IF('Data Source'!D17/200*100&gt;=70,"A",IF('Data Source'!D17/200*100&gt;=60,"A-",IF('Data Source'!D17/200*100&gt;=50,"B",IF('Data Source'!D17/200*100&gt;=40,"C",IF('Data Source'!D17/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E18" s="6">
+        <f>IF('Data Source'!E17&gt;=80,"A+",IF('Data Source'!E17&gt;=70,"A",IF('Data Source'!E17&gt;=60,"A-",IF('Data Source'!E17&gt;=50,"B",IF('Data Source'!E17&gt;=40,"C",IF('Data Source'!E17&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F18" s="6">
+        <f>IF('Data Source'!F17/200*100&gt;=80,"A+",IF('Data Source'!F17/200*100&gt;=70,"A",IF('Data Source'!F17/200*100&gt;=60,"A-",IF('Data Source'!F17/200*100&gt;=50,"B",IF('Data Source'!F17/200*100&gt;=40,"C",IF('Data Source'!F17/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G18" s="6">
+        <f>IF('Data Source'!G17/200*100&gt;=80,"A+",IF('Data Source'!G17/200*100&gt;=70,"A",IF('Data Source'!G17/200*100&gt;=60,"A-",IF('Data Source'!G17/200*100&gt;=50,"B",IF('Data Source'!G17/200*100&gt;=40,"C",IF('Data Source'!G17/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H18" s="6">
+        <f>IF('Data Source'!H17&gt;=80,"A+",IF('Data Source'!H17&gt;=70,"A",IF('Data Source'!H17&gt;=60,"A-",IF('Data Source'!H17&gt;=50,"B",IF('Data Source'!H17&gt;=40,"C",IF('Data Source'!H17&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I18" s="6">
+        <f>IF('Data Source'!I17&gt;=80,"A+",IF('Data Source'!I17&gt;=70,"A",IF('Data Source'!I17&gt;=60,"A-",IF('Data Source'!I17&gt;=50,"B",IF('Data Source'!I17&gt;=40,"C",IF('Data Source'!I17&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J18" s="6">
+        <f>IF('Data Source'!J17&gt;=80,"A+",IF('Data Source'!J17&gt;=70,"A",IF('Data Source'!J17&gt;=60,"A-",IF('Data Source'!J17&gt;=50,"B",IF('Data Source'!J17&gt;=40,"C",IF('Data Source'!J17&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K18" s="6">
+        <f>IF('Data Source'!K17&gt;=80,"A+",IF('Data Source'!K17&gt;=70,"A",IF('Data Source'!K17&gt;=60,"A-",IF('Data Source'!K17&gt;=50,"B",IF('Data Source'!K17&gt;=40,"C",IF('Data Source'!K17&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L18" s="6">
+        <f>IF('Data Source'!L17&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M18" s="6">
+        <f>IF('Data Source'!M17&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N18" s="5">
+        <f>'Data Source'!P17</f>
+        <v/>
+      </c>
+      <c r="O18" s="6">
+        <f>'Data Source'!Q17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6">
+        <f>'Data Source'!A18</f>
+        <v/>
+      </c>
+      <c r="B19">
+        <f>'Data Source'!B18</f>
+        <v/>
+      </c>
+      <c r="C19" s="6">
+        <f>IF('Data Source'!C18/200*100&gt;=80,"A+",IF('Data Source'!C18/200*100&gt;=70,"A",IF('Data Source'!C18/200*100&gt;=60,"A-",IF('Data Source'!C18/200*100&gt;=50,"B",IF('Data Source'!C18/200*100&gt;=40,"C",IF('Data Source'!C18/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D19" s="6">
+        <f>IF('Data Source'!D18/200*100&gt;=80,"A+",IF('Data Source'!D18/200*100&gt;=70,"A",IF('Data Source'!D18/200*100&gt;=60,"A-",IF('Data Source'!D18/200*100&gt;=50,"B",IF('Data Source'!D18/200*100&gt;=40,"C",IF('Data Source'!D18/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E19" s="6">
+        <f>IF('Data Source'!E18&gt;=80,"A+",IF('Data Source'!E18&gt;=70,"A",IF('Data Source'!E18&gt;=60,"A-",IF('Data Source'!E18&gt;=50,"B",IF('Data Source'!E18&gt;=40,"C",IF('Data Source'!E18&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F19" s="6">
+        <f>IF('Data Source'!F18/200*100&gt;=80,"A+",IF('Data Source'!F18/200*100&gt;=70,"A",IF('Data Source'!F18/200*100&gt;=60,"A-",IF('Data Source'!F18/200*100&gt;=50,"B",IF('Data Source'!F18/200*100&gt;=40,"C",IF('Data Source'!F18/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G19" s="6">
+        <f>IF('Data Source'!G18/200*100&gt;=80,"A+",IF('Data Source'!G18/200*100&gt;=70,"A",IF('Data Source'!G18/200*100&gt;=60,"A-",IF('Data Source'!G18/200*100&gt;=50,"B",IF('Data Source'!G18/200*100&gt;=40,"C",IF('Data Source'!G18/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H19" s="6">
+        <f>IF('Data Source'!H18&gt;=80,"A+",IF('Data Source'!H18&gt;=70,"A",IF('Data Source'!H18&gt;=60,"A-",IF('Data Source'!H18&gt;=50,"B",IF('Data Source'!H18&gt;=40,"C",IF('Data Source'!H18&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I19" s="6">
+        <f>IF('Data Source'!I18&gt;=80,"A+",IF('Data Source'!I18&gt;=70,"A",IF('Data Source'!I18&gt;=60,"A-",IF('Data Source'!I18&gt;=50,"B",IF('Data Source'!I18&gt;=40,"C",IF('Data Source'!I18&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J19" s="6">
+        <f>IF('Data Source'!J18&gt;=80,"A+",IF('Data Source'!J18&gt;=70,"A",IF('Data Source'!J18&gt;=60,"A-",IF('Data Source'!J18&gt;=50,"B",IF('Data Source'!J18&gt;=40,"C",IF('Data Source'!J18&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K19" s="6">
+        <f>IF('Data Source'!K18&gt;=80,"A+",IF('Data Source'!K18&gt;=70,"A",IF('Data Source'!K18&gt;=60,"A-",IF('Data Source'!K18&gt;=50,"B",IF('Data Source'!K18&gt;=40,"C",IF('Data Source'!K18&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L19" s="6">
+        <f>IF('Data Source'!L18&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M19" s="6">
+        <f>IF('Data Source'!M18&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N19" s="5">
+        <f>'Data Source'!P18</f>
+        <v/>
+      </c>
+      <c r="O19" s="6">
+        <f>'Data Source'!Q18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6">
+        <f>'Data Source'!A19</f>
+        <v/>
+      </c>
+      <c r="B20">
+        <f>'Data Source'!B19</f>
+        <v/>
+      </c>
+      <c r="C20" s="6">
+        <f>IF('Data Source'!C19/200*100&gt;=80,"A+",IF('Data Source'!C19/200*100&gt;=70,"A",IF('Data Source'!C19/200*100&gt;=60,"A-",IF('Data Source'!C19/200*100&gt;=50,"B",IF('Data Source'!C19/200*100&gt;=40,"C",IF('Data Source'!C19/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D20" s="6">
+        <f>IF('Data Source'!D19/200*100&gt;=80,"A+",IF('Data Source'!D19/200*100&gt;=70,"A",IF('Data Source'!D19/200*100&gt;=60,"A-",IF('Data Source'!D19/200*100&gt;=50,"B",IF('Data Source'!D19/200*100&gt;=40,"C",IF('Data Source'!D19/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E20" s="6">
+        <f>IF('Data Source'!E19&gt;=80,"A+",IF('Data Source'!E19&gt;=70,"A",IF('Data Source'!E19&gt;=60,"A-",IF('Data Source'!E19&gt;=50,"B",IF('Data Source'!E19&gt;=40,"C",IF('Data Source'!E19&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F20" s="6">
+        <f>IF('Data Source'!F19/200*100&gt;=80,"A+",IF('Data Source'!F19/200*100&gt;=70,"A",IF('Data Source'!F19/200*100&gt;=60,"A-",IF('Data Source'!F19/200*100&gt;=50,"B",IF('Data Source'!F19/200*100&gt;=40,"C",IF('Data Source'!F19/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G20" s="6">
+        <f>IF('Data Source'!G19/200*100&gt;=80,"A+",IF('Data Source'!G19/200*100&gt;=70,"A",IF('Data Source'!G19/200*100&gt;=60,"A-",IF('Data Source'!G19/200*100&gt;=50,"B",IF('Data Source'!G19/200*100&gt;=40,"C",IF('Data Source'!G19/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H20" s="6">
+        <f>IF('Data Source'!H19&gt;=80,"A+",IF('Data Source'!H19&gt;=70,"A",IF('Data Source'!H19&gt;=60,"A-",IF('Data Source'!H19&gt;=50,"B",IF('Data Source'!H19&gt;=40,"C",IF('Data Source'!H19&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I20" s="6">
+        <f>IF('Data Source'!I19&gt;=80,"A+",IF('Data Source'!I19&gt;=70,"A",IF('Data Source'!I19&gt;=60,"A-",IF('Data Source'!I19&gt;=50,"B",IF('Data Source'!I19&gt;=40,"C",IF('Data Source'!I19&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J20" s="6">
+        <f>IF('Data Source'!J19&gt;=80,"A+",IF('Data Source'!J19&gt;=70,"A",IF('Data Source'!J19&gt;=60,"A-",IF('Data Source'!J19&gt;=50,"B",IF('Data Source'!J19&gt;=40,"C",IF('Data Source'!J19&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K20" s="6">
+        <f>IF('Data Source'!K19&gt;=80,"A+",IF('Data Source'!K19&gt;=70,"A",IF('Data Source'!K19&gt;=60,"A-",IF('Data Source'!K19&gt;=50,"B",IF('Data Source'!K19&gt;=40,"C",IF('Data Source'!K19&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L20" s="6">
+        <f>IF('Data Source'!L19&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M20" s="6">
+        <f>IF('Data Source'!M19&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N20" s="5">
+        <f>'Data Source'!P19</f>
+        <v/>
+      </c>
+      <c r="O20" s="6">
+        <f>'Data Source'!Q19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6">
+        <f>'Data Source'!A20</f>
+        <v/>
+      </c>
+      <c r="B21">
+        <f>'Data Source'!B20</f>
+        <v/>
+      </c>
+      <c r="C21" s="6">
+        <f>IF('Data Source'!C20/200*100&gt;=80,"A+",IF('Data Source'!C20/200*100&gt;=70,"A",IF('Data Source'!C20/200*100&gt;=60,"A-",IF('Data Source'!C20/200*100&gt;=50,"B",IF('Data Source'!C20/200*100&gt;=40,"C",IF('Data Source'!C20/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D21" s="6">
+        <f>IF('Data Source'!D20/200*100&gt;=80,"A+",IF('Data Source'!D20/200*100&gt;=70,"A",IF('Data Source'!D20/200*100&gt;=60,"A-",IF('Data Source'!D20/200*100&gt;=50,"B",IF('Data Source'!D20/200*100&gt;=40,"C",IF('Data Source'!D20/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E21" s="6">
+        <f>IF('Data Source'!E20&gt;=80,"A+",IF('Data Source'!E20&gt;=70,"A",IF('Data Source'!E20&gt;=60,"A-",IF('Data Source'!E20&gt;=50,"B",IF('Data Source'!E20&gt;=40,"C",IF('Data Source'!E20&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F21" s="6">
+        <f>IF('Data Source'!F20/200*100&gt;=80,"A+",IF('Data Source'!F20/200*100&gt;=70,"A",IF('Data Source'!F20/200*100&gt;=60,"A-",IF('Data Source'!F20/200*100&gt;=50,"B",IF('Data Source'!F20/200*100&gt;=40,"C",IF('Data Source'!F20/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G21" s="6">
+        <f>IF('Data Source'!G20/200*100&gt;=80,"A+",IF('Data Source'!G20/200*100&gt;=70,"A",IF('Data Source'!G20/200*100&gt;=60,"A-",IF('Data Source'!G20/200*100&gt;=50,"B",IF('Data Source'!G20/200*100&gt;=40,"C",IF('Data Source'!G20/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H21" s="6">
+        <f>IF('Data Source'!H20&gt;=80,"A+",IF('Data Source'!H20&gt;=70,"A",IF('Data Source'!H20&gt;=60,"A-",IF('Data Source'!H20&gt;=50,"B",IF('Data Source'!H20&gt;=40,"C",IF('Data Source'!H20&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I21" s="6">
+        <f>IF('Data Source'!I20&gt;=80,"A+",IF('Data Source'!I20&gt;=70,"A",IF('Data Source'!I20&gt;=60,"A-",IF('Data Source'!I20&gt;=50,"B",IF('Data Source'!I20&gt;=40,"C",IF('Data Source'!I20&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J21" s="6">
+        <f>IF('Data Source'!J20&gt;=80,"A+",IF('Data Source'!J20&gt;=70,"A",IF('Data Source'!J20&gt;=60,"A-",IF('Data Source'!J20&gt;=50,"B",IF('Data Source'!J20&gt;=40,"C",IF('Data Source'!J20&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K21" s="6">
+        <f>IF('Data Source'!K20&gt;=80,"A+",IF('Data Source'!K20&gt;=70,"A",IF('Data Source'!K20&gt;=60,"A-",IF('Data Source'!K20&gt;=50,"B",IF('Data Source'!K20&gt;=40,"C",IF('Data Source'!K20&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L21" s="6">
+        <f>IF('Data Source'!L20&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M21" s="6">
+        <f>IF('Data Source'!M20&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N21" s="5">
+        <f>'Data Source'!P20</f>
+        <v/>
+      </c>
+      <c r="O21" s="6">
+        <f>'Data Source'!Q20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6">
+        <f>'Data Source'!A21</f>
+        <v/>
+      </c>
+      <c r="B22">
+        <f>'Data Source'!B21</f>
+        <v/>
+      </c>
+      <c r="C22" s="6">
+        <f>IF('Data Source'!C21/200*100&gt;=80,"A+",IF('Data Source'!C21/200*100&gt;=70,"A",IF('Data Source'!C21/200*100&gt;=60,"A-",IF('Data Source'!C21/200*100&gt;=50,"B",IF('Data Source'!C21/200*100&gt;=40,"C",IF('Data Source'!C21/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="D22" s="6">
+        <f>IF('Data Source'!D21/200*100&gt;=80,"A+",IF('Data Source'!D21/200*100&gt;=70,"A",IF('Data Source'!D21/200*100&gt;=60,"A-",IF('Data Source'!D21/200*100&gt;=50,"B",IF('Data Source'!D21/200*100&gt;=40,"C",IF('Data Source'!D21/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="E22" s="6">
+        <f>IF('Data Source'!E21&gt;=80,"A+",IF('Data Source'!E21&gt;=70,"A",IF('Data Source'!E21&gt;=60,"A-",IF('Data Source'!E21&gt;=50,"B",IF('Data Source'!E21&gt;=40,"C",IF('Data Source'!E21&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="F22" s="6">
+        <f>IF('Data Source'!F21/200*100&gt;=80,"A+",IF('Data Source'!F21/200*100&gt;=70,"A",IF('Data Source'!F21/200*100&gt;=60,"A-",IF('Data Source'!F21/200*100&gt;=50,"B",IF('Data Source'!F21/200*100&gt;=40,"C",IF('Data Source'!F21/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="G22" s="6">
+        <f>IF('Data Source'!G21/200*100&gt;=80,"A+",IF('Data Source'!G21/200*100&gt;=70,"A",IF('Data Source'!G21/200*100&gt;=60,"A-",IF('Data Source'!G21/200*100&gt;=50,"B",IF('Data Source'!G21/200*100&gt;=40,"C",IF('Data Source'!G21/200*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="H22" s="6">
+        <f>IF('Data Source'!H21&gt;=80,"A+",IF('Data Source'!H21&gt;=70,"A",IF('Data Source'!H21&gt;=60,"A-",IF('Data Source'!H21&gt;=50,"B",IF('Data Source'!H21&gt;=40,"C",IF('Data Source'!H21&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="I22" s="6">
+        <f>IF('Data Source'!I21&gt;=80,"A+",IF('Data Source'!I21&gt;=70,"A",IF('Data Source'!I21&gt;=60,"A-",IF('Data Source'!I21&gt;=50,"B",IF('Data Source'!I21&gt;=40,"C",IF('Data Source'!I21&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="J22" s="6">
+        <f>IF('Data Source'!J21&gt;=80,"A+",IF('Data Source'!J21&gt;=70,"A",IF('Data Source'!J21&gt;=60,"A-",IF('Data Source'!J21&gt;=50,"B",IF('Data Source'!J21&gt;=40,"C",IF('Data Source'!J21&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K22" s="6">
+        <f>IF('Data Source'!K21&gt;=80,"A+",IF('Data Source'!K21&gt;=70,"A",IF('Data Source'!K21&gt;=60,"A-",IF('Data Source'!K21&gt;=50,"B",IF('Data Source'!K21&gt;=40,"C",IF('Data Source'!K21&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="L22" s="6">
+        <f>IF('Data Source'!L21&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="M22" s="6">
+        <f>IF('Data Source'!M21&gt;=33,"Pass","Fail")</f>
+        <v/>
+      </c>
+      <c r="N22" s="5">
+        <f>'Data Source'!P21</f>
+        <v/>
+      </c>
+      <c r="O22" s="6">
+        <f>'Data Source'!Q21</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Refactor Dakhil GPA calculation to accommodate new subject structure and update Excel formulas accordingly
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -128,8 +128,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -742,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,21 +752,25 @@
   <cols>
     <col width="5" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
     <col width="10" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
-    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
     <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="8" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -782,75 +786,95 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Quran_Mazid</t>
+          <t>Quran</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Arabic_Combined</t>
+          <t>Hadith</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Arabic_I</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Arabic_II</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Aqaid</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>English_Combined</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Bangla_Combined</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>English_I</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>English_II</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Bangla_I</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Bangla_II</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Islamic_History</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>ICT</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Career_Education</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Physical_Education</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Overall Grade</t>
         </is>
@@ -866,52 +890,64 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>170</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>66</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>157</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>146</v>
+        <v>89</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>64</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>84</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>64</v>
-      </c>
-      <c r="J2" s="3" t="n">
         <v>68</v>
       </c>
+      <c r="I2" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>60</v>
+      </c>
       <c r="K2" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="N2">
-        <f>SUM(C2:J2)</f>
-        <v/>
-      </c>
-      <c r="O2" s="4">
-        <f>ROUND(N2/8,2)</f>
-        <v/>
-      </c>
-      <c r="P2" s="5">
-        <f>IF(OR(C2&lt;66,D2&lt;66,E2&lt;33,F2&lt;66,G2&lt;66,H2&lt;33,I2&lt;33,J2&lt;33,L2&lt;33,M2&lt;33),0,MIN(5,ROUND((IF(C2/200*100&gt;=80,5,IF(C2/200*100&gt;=70,4,IF(C2/200*100&gt;=60,3.5,IF(C2/200*100&gt;=50,3,IF(C2/200*100&gt;=40,2,IF(C2/200*100&gt;=33,1,0))))))+IF(D2/200*100&gt;=80,5,IF(D2/200*100&gt;=70,4,IF(D2/200*100&gt;=60,3.5,IF(D2/200*100&gt;=50,3,IF(D2/200*100&gt;=40,2,IF(D2/200*100&gt;=33,1,0))))))+IF(E2&gt;=80,5,IF(E2&gt;=70,4,IF(E2&gt;=60,3.5,IF(E2&gt;=50,3,IF(E2&gt;=40,2,IF(E2&gt;=33,1,0))))))+IF(F2/200*100&gt;=80,5,IF(F2/200*100&gt;=70,4,IF(F2/200*100&gt;=60,3.5,IF(F2/200*100&gt;=50,3,IF(F2/200*100&gt;=40,2,IF(F2/200*100&gt;=33,1,0))))))+IF(G2/200*100&gt;=80,5,IF(G2/200*100&gt;=70,4,IF(G2/200*100&gt;=60,3.5,IF(G2/200*100&gt;=50,3,IF(G2/200*100&gt;=40,2,IF(G2/200*100&gt;=33,1,0))))))+IF(H2&gt;=80,5,IF(H2&gt;=70,4,IF(H2&gt;=60,3.5,IF(H2&gt;=50,3,IF(H2&gt;=40,2,IF(H2&gt;=33,1,0))))))+IF(I2&gt;=80,5,IF(I2&gt;=70,4,IF(I2&gt;=60,3.5,IF(I2&gt;=50,3,IF(I2&gt;=40,2,IF(I2&gt;=33,1,0))))))+IF(J2&gt;=80,5,IF(J2&gt;=70,4,IF(J2&gt;=60,3.5,IF(J2&gt;=50,3,IF(J2&gt;=40,2,IF(J2&gt;=33,1,0)))))))/8+IF(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))&gt;=2,(IF(K2&gt;=80,5,IF(K2&gt;=70,4,IF(K2&gt;=60,3.5,IF(K2&gt;=50,3,IF(K2&gt;=40,2,IF(K2&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q2" s="6">
-        <f>IF(P2&gt;=5,"A+",IF(P2&gt;=4,"A",IF(P2&gt;=3.5,"A-",IF(P2&gt;=3,"B",IF(P2&gt;=2,"C",IF(P2&gt;=1,"D","F"))))))</f>
+        <v>76</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="R2">
+        <f>SUM(C2:N2)</f>
+        <v/>
+      </c>
+      <c r="S2" s="4">
+        <f>ROUND(R2/12,2)</f>
+        <v/>
+      </c>
+      <c r="T2" s="5">
+        <f>IF(OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,(J2+K2)&lt;66,L2&lt;33,M2&lt;33,N2&lt;33,P2&lt;33,Q2&lt;33),0,MIN(5,ROUND((IF((C2+D2)/200*100&gt;=80,5,IF((C2+D2)/200*100&gt;=70,4,IF((C2+D2)/200*100&gt;=60,3.5,IF((C2+D2)/200*100&gt;=50,3,IF((C2+D2)/200*100&gt;=40,2,IF((C2+D2)/200*100&gt;=33,1,0))))))+IF((E2+F2)/200*100&gt;=80,5,IF((E2+F2)/200*100&gt;=70,4,IF((E2+F2)/200*100&gt;=60,3.5,IF((E2+F2)/200*100&gt;=50,3,IF((E2+F2)/200*100&gt;=40,2,IF((E2+F2)/200*100&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF((H2+I2)/200*100&gt;=80,5,IF((H2+I2)/200*100&gt;=70,4,IF((H2+I2)/200*100&gt;=60,3.5,IF((H2+I2)/200*100&gt;=50,3,IF((H2+I2)/200*100&gt;=40,2,IF((H2+I2)/200*100&gt;=33,1,0))))))+IF((J2+K2)/200*100&gt;=80,5,IF((J2+K2)/200*100&gt;=70,4,IF((J2+K2)/200*100&gt;=60,3.5,IF((J2+K2)/200*100&gt;=50,3,IF((J2+K2)/200*100&gt;=40,2,IF((J2+K2)/200*100&gt;=33,1,0))))))+IF(L2&gt;=80,5,IF(L2&gt;=70,4,IF(L2&gt;=60,3.5,IF(L2&gt;=50,3,IF(L2&gt;=40,2,IF(L2&gt;=33,1,0))))))+IF(M2&gt;=80,5,IF(M2&gt;=70,4,IF(M2&gt;=60,3.5,IF(M2&gt;=50,3,IF(M2&gt;=40,2,IF(M2&gt;=33,1,0))))))+IF(N2&gt;=80,5,IF(N2&gt;=70,4,IF(N2&gt;=60,3.5,IF(N2&gt;=50,3,IF(N2&gt;=40,2,IF(N2&gt;=33,1,0)))))))/8+IF(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))&gt;=2,(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U2" s="6">
+        <f>IF(T2&gt;=5,"A+",IF(T2&gt;=4,"A",IF(T2&gt;=3.5,"A-",IF(T2&gt;=3,"B",IF(T2&gt;=2,"C",IF(T2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -924,53 +960,65 @@
           <t>Fatima Khan</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
-        <v>137</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>144</v>
+      <c r="C3" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>156</v>
+        <v>74</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>70</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>64</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>80</v>
+        <v>86</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="N3">
-        <f>SUM(C3:J3)</f>
-        <v/>
-      </c>
-      <c r="O3" s="4">
-        <f>ROUND(N3/8,2)</f>
-        <v/>
-      </c>
-      <c r="P3" s="5">
-        <f>IF(OR(C3&lt;66,D3&lt;66,E3&lt;33,F3&lt;66,G3&lt;66,H3&lt;33,I3&lt;33,J3&lt;33,L3&lt;33,M3&lt;33),0,MIN(5,ROUND((IF(C3/200*100&gt;=80,5,IF(C3/200*100&gt;=70,4,IF(C3/200*100&gt;=60,3.5,IF(C3/200*100&gt;=50,3,IF(C3/200*100&gt;=40,2,IF(C3/200*100&gt;=33,1,0))))))+IF(D3/200*100&gt;=80,5,IF(D3/200*100&gt;=70,4,IF(D3/200*100&gt;=60,3.5,IF(D3/200*100&gt;=50,3,IF(D3/200*100&gt;=40,2,IF(D3/200*100&gt;=33,1,0))))))+IF(E3&gt;=80,5,IF(E3&gt;=70,4,IF(E3&gt;=60,3.5,IF(E3&gt;=50,3,IF(E3&gt;=40,2,IF(E3&gt;=33,1,0))))))+IF(F3/200*100&gt;=80,5,IF(F3/200*100&gt;=70,4,IF(F3/200*100&gt;=60,3.5,IF(F3/200*100&gt;=50,3,IF(F3/200*100&gt;=40,2,IF(F3/200*100&gt;=33,1,0))))))+IF(G3/200*100&gt;=80,5,IF(G3/200*100&gt;=70,4,IF(G3/200*100&gt;=60,3.5,IF(G3/200*100&gt;=50,3,IF(G3/200*100&gt;=40,2,IF(G3/200*100&gt;=33,1,0))))))+IF(H3&gt;=80,5,IF(H3&gt;=70,4,IF(H3&gt;=60,3.5,IF(H3&gt;=50,3,IF(H3&gt;=40,2,IF(H3&gt;=33,1,0))))))+IF(I3&gt;=80,5,IF(I3&gt;=70,4,IF(I3&gt;=60,3.5,IF(I3&gt;=50,3,IF(I3&gt;=40,2,IF(I3&gt;=33,1,0))))))+IF(J3&gt;=80,5,IF(J3&gt;=70,4,IF(J3&gt;=60,3.5,IF(J3&gt;=50,3,IF(J3&gt;=40,2,IF(J3&gt;=33,1,0)))))))/8+IF(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))&gt;=2,(IF(K3&gt;=80,5,IF(K3&gt;=70,4,IF(K3&gt;=60,3.5,IF(K3&gt;=50,3,IF(K3&gt;=40,2,IF(K3&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q3" s="6">
-        <f>IF(P3&gt;=5,"A+",IF(P3&gt;=4,"A",IF(P3&gt;=3.5,"A-",IF(P3&gt;=3,"B",IF(P3&gt;=2,"C",IF(P3&gt;=1,"D","F"))))))</f>
+        <v>77</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="R3">
+        <f>SUM(C3:N3)</f>
+        <v/>
+      </c>
+      <c r="S3" s="4">
+        <f>ROUND(R3/12,2)</f>
+        <v/>
+      </c>
+      <c r="T3" s="5">
+        <f>IF(OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,(J3+K3)&lt;66,L3&lt;33,M3&lt;33,N3&lt;33,P3&lt;33,Q3&lt;33),0,MIN(5,ROUND((IF((C3+D3)/200*100&gt;=80,5,IF((C3+D3)/200*100&gt;=70,4,IF((C3+D3)/200*100&gt;=60,3.5,IF((C3+D3)/200*100&gt;=50,3,IF((C3+D3)/200*100&gt;=40,2,IF((C3+D3)/200*100&gt;=33,1,0))))))+IF((E3+F3)/200*100&gt;=80,5,IF((E3+F3)/200*100&gt;=70,4,IF((E3+F3)/200*100&gt;=60,3.5,IF((E3+F3)/200*100&gt;=50,3,IF((E3+F3)/200*100&gt;=40,2,IF((E3+F3)/200*100&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF((H3+I3)/200*100&gt;=80,5,IF((H3+I3)/200*100&gt;=70,4,IF((H3+I3)/200*100&gt;=60,3.5,IF((H3+I3)/200*100&gt;=50,3,IF((H3+I3)/200*100&gt;=40,2,IF((H3+I3)/200*100&gt;=33,1,0))))))+IF((J3+K3)/200*100&gt;=80,5,IF((J3+K3)/200*100&gt;=70,4,IF((J3+K3)/200*100&gt;=60,3.5,IF((J3+K3)/200*100&gt;=50,3,IF((J3+K3)/200*100&gt;=40,2,IF((J3+K3)/200*100&gt;=33,1,0))))))+IF(L3&gt;=80,5,IF(L3&gt;=70,4,IF(L3&gt;=60,3.5,IF(L3&gt;=50,3,IF(L3&gt;=40,2,IF(L3&gt;=33,1,0))))))+IF(M3&gt;=80,5,IF(M3&gt;=70,4,IF(M3&gt;=60,3.5,IF(M3&gt;=50,3,IF(M3&gt;=40,2,IF(M3&gt;=33,1,0))))))+IF(N3&gt;=80,5,IF(N3&gt;=70,4,IF(N3&gt;=60,3.5,IF(N3&gt;=50,3,IF(N3&gt;=40,2,IF(N3&gt;=33,1,0)))))))/8+IF(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))&gt;=2,(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U3" s="6">
+        <f>IF(T3&gt;=5,"A+",IF(T3&gt;=4,"A",IF(T3&gt;=3.5,"A-",IF(T3&gt;=3,"B",IF(T3&gt;=2,"C",IF(T3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -983,53 +1031,65 @@
           <t>Karim Hassan</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
-        <v>131</v>
+      <c r="C4" s="2" t="n">
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>162</v>
-      </c>
-      <c r="E4" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="O4" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="F4" s="3" t="n">
-        <v>144</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>145</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>71</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>65</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="K4" s="2" t="n">
+      <c r="P4" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="L4" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>83</v>
-      </c>
-      <c r="N4">
-        <f>SUM(C4:J4)</f>
-        <v/>
-      </c>
-      <c r="O4" s="4">
-        <f>ROUND(N4/8,2)</f>
-        <v/>
-      </c>
-      <c r="P4" s="5">
-        <f>IF(OR(C4&lt;66,D4&lt;66,E4&lt;33,F4&lt;66,G4&lt;66,H4&lt;33,I4&lt;33,J4&lt;33,L4&lt;33,M4&lt;33),0,MIN(5,ROUND((IF(C4/200*100&gt;=80,5,IF(C4/200*100&gt;=70,4,IF(C4/200*100&gt;=60,3.5,IF(C4/200*100&gt;=50,3,IF(C4/200*100&gt;=40,2,IF(C4/200*100&gt;=33,1,0))))))+IF(D4/200*100&gt;=80,5,IF(D4/200*100&gt;=70,4,IF(D4/200*100&gt;=60,3.5,IF(D4/200*100&gt;=50,3,IF(D4/200*100&gt;=40,2,IF(D4/200*100&gt;=33,1,0))))))+IF(E4&gt;=80,5,IF(E4&gt;=70,4,IF(E4&gt;=60,3.5,IF(E4&gt;=50,3,IF(E4&gt;=40,2,IF(E4&gt;=33,1,0))))))+IF(F4/200*100&gt;=80,5,IF(F4/200*100&gt;=70,4,IF(F4/200*100&gt;=60,3.5,IF(F4/200*100&gt;=50,3,IF(F4/200*100&gt;=40,2,IF(F4/200*100&gt;=33,1,0))))))+IF(G4/200*100&gt;=80,5,IF(G4/200*100&gt;=70,4,IF(G4/200*100&gt;=60,3.5,IF(G4/200*100&gt;=50,3,IF(G4/200*100&gt;=40,2,IF(G4/200*100&gt;=33,1,0))))))+IF(H4&gt;=80,5,IF(H4&gt;=70,4,IF(H4&gt;=60,3.5,IF(H4&gt;=50,3,IF(H4&gt;=40,2,IF(H4&gt;=33,1,0))))))+IF(I4&gt;=80,5,IF(I4&gt;=70,4,IF(I4&gt;=60,3.5,IF(I4&gt;=50,3,IF(I4&gt;=40,2,IF(I4&gt;=33,1,0))))))+IF(J4&gt;=80,5,IF(J4&gt;=70,4,IF(J4&gt;=60,3.5,IF(J4&gt;=50,3,IF(J4&gt;=40,2,IF(J4&gt;=33,1,0)))))))/8+IF(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))&gt;=2,(IF(K4&gt;=80,5,IF(K4&gt;=70,4,IF(K4&gt;=60,3.5,IF(K4&gt;=50,3,IF(K4&gt;=40,2,IF(K4&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="6">
-        <f>IF(P4&gt;=5,"A+",IF(P4&gt;=4,"A",IF(P4&gt;=3.5,"A-",IF(P4&gt;=3,"B",IF(P4&gt;=2,"C",IF(P4&gt;=1,"D","F"))))))</f>
+      <c r="R4">
+        <f>SUM(C4:N4)</f>
+        <v/>
+      </c>
+      <c r="S4" s="4">
+        <f>ROUND(R4/12,2)</f>
+        <v/>
+      </c>
+      <c r="T4" s="5">
+        <f>IF(OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,(J4+K4)&lt;66,L4&lt;33,M4&lt;33,N4&lt;33,P4&lt;33,Q4&lt;33),0,MIN(5,ROUND((IF((C4+D4)/200*100&gt;=80,5,IF((C4+D4)/200*100&gt;=70,4,IF((C4+D4)/200*100&gt;=60,3.5,IF((C4+D4)/200*100&gt;=50,3,IF((C4+D4)/200*100&gt;=40,2,IF((C4+D4)/200*100&gt;=33,1,0))))))+IF((E4+F4)/200*100&gt;=80,5,IF((E4+F4)/200*100&gt;=70,4,IF((E4+F4)/200*100&gt;=60,3.5,IF((E4+F4)/200*100&gt;=50,3,IF((E4+F4)/200*100&gt;=40,2,IF((E4+F4)/200*100&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF((H4+I4)/200*100&gt;=80,5,IF((H4+I4)/200*100&gt;=70,4,IF((H4+I4)/200*100&gt;=60,3.5,IF((H4+I4)/200*100&gt;=50,3,IF((H4+I4)/200*100&gt;=40,2,IF((H4+I4)/200*100&gt;=33,1,0))))))+IF((J4+K4)/200*100&gt;=80,5,IF((J4+K4)/200*100&gt;=70,4,IF((J4+K4)/200*100&gt;=60,3.5,IF((J4+K4)/200*100&gt;=50,3,IF((J4+K4)/200*100&gt;=40,2,IF((J4+K4)/200*100&gt;=33,1,0))))))+IF(L4&gt;=80,5,IF(L4&gt;=70,4,IF(L4&gt;=60,3.5,IF(L4&gt;=50,3,IF(L4&gt;=40,2,IF(L4&gt;=33,1,0))))))+IF(M4&gt;=80,5,IF(M4&gt;=70,4,IF(M4&gt;=60,3.5,IF(M4&gt;=50,3,IF(M4&gt;=40,2,IF(M4&gt;=33,1,0))))))+IF(N4&gt;=80,5,IF(N4&gt;=70,4,IF(N4&gt;=60,3.5,IF(N4&gt;=50,3,IF(N4&gt;=40,2,IF(N4&gt;=33,1,0)))))))/8+IF(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))&gt;=2,(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U4" s="6">
+        <f>IF(T4&gt;=5,"A+",IF(T4&gt;=4,"A",IF(T4&gt;=3.5,"A-",IF(T4&gt;=3,"B",IF(T4&gt;=2,"C",IF(T4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1043,52 +1103,64 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>177</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>168</v>
-      </c>
-      <c r="E5" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="J5" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="F5" s="3" t="n">
-        <v>128</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>184</v>
-      </c>
-      <c r="H5" s="3" t="n">
+      <c r="K5" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="O5" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="K5" s="7" t="n">
-        <v>56</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>79</v>
-      </c>
-      <c r="M5" s="2" t="n">
-        <v>91</v>
-      </c>
-      <c r="N5">
-        <f>SUM(C5:J5)</f>
-        <v/>
-      </c>
-      <c r="O5" s="4">
-        <f>ROUND(N5/8,2)</f>
-        <v/>
-      </c>
-      <c r="P5" s="5">
-        <f>IF(OR(C5&lt;66,D5&lt;66,E5&lt;33,F5&lt;66,G5&lt;66,H5&lt;33,I5&lt;33,J5&lt;33,L5&lt;33,M5&lt;33),0,MIN(5,ROUND((IF(C5/200*100&gt;=80,5,IF(C5/200*100&gt;=70,4,IF(C5/200*100&gt;=60,3.5,IF(C5/200*100&gt;=50,3,IF(C5/200*100&gt;=40,2,IF(C5/200*100&gt;=33,1,0))))))+IF(D5/200*100&gt;=80,5,IF(D5/200*100&gt;=70,4,IF(D5/200*100&gt;=60,3.5,IF(D5/200*100&gt;=50,3,IF(D5/200*100&gt;=40,2,IF(D5/200*100&gt;=33,1,0))))))+IF(E5&gt;=80,5,IF(E5&gt;=70,4,IF(E5&gt;=60,3.5,IF(E5&gt;=50,3,IF(E5&gt;=40,2,IF(E5&gt;=33,1,0))))))+IF(F5/200*100&gt;=80,5,IF(F5/200*100&gt;=70,4,IF(F5/200*100&gt;=60,3.5,IF(F5/200*100&gt;=50,3,IF(F5/200*100&gt;=40,2,IF(F5/200*100&gt;=33,1,0))))))+IF(G5/200*100&gt;=80,5,IF(G5/200*100&gt;=70,4,IF(G5/200*100&gt;=60,3.5,IF(G5/200*100&gt;=50,3,IF(G5/200*100&gt;=40,2,IF(G5/200*100&gt;=33,1,0))))))+IF(H5&gt;=80,5,IF(H5&gt;=70,4,IF(H5&gt;=60,3.5,IF(H5&gt;=50,3,IF(H5&gt;=40,2,IF(H5&gt;=33,1,0))))))+IF(I5&gt;=80,5,IF(I5&gt;=70,4,IF(I5&gt;=60,3.5,IF(I5&gt;=50,3,IF(I5&gt;=40,2,IF(I5&gt;=33,1,0))))))+IF(J5&gt;=80,5,IF(J5&gt;=70,4,IF(J5&gt;=60,3.5,IF(J5&gt;=50,3,IF(J5&gt;=40,2,IF(J5&gt;=33,1,0)))))))/8+IF(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))&gt;=2,(IF(K5&gt;=80,5,IF(K5&gt;=70,4,IF(K5&gt;=60,3.5,IF(K5&gt;=50,3,IF(K5&gt;=40,2,IF(K5&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="6">
-        <f>IF(P5&gt;=5,"A+",IF(P5&gt;=4,"A",IF(P5&gt;=3.5,"A-",IF(P5&gt;=3,"B",IF(P5&gt;=2,"C",IF(P5&gt;=1,"D","F"))))))</f>
+      <c r="P5" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="R5">
+        <f>SUM(C5:N5)</f>
+        <v/>
+      </c>
+      <c r="S5" s="4">
+        <f>ROUND(R5/12,2)</f>
+        <v/>
+      </c>
+      <c r="T5" s="5">
+        <f>IF(OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,(J5+K5)&lt;66,L5&lt;33,M5&lt;33,N5&lt;33,P5&lt;33,Q5&lt;33),0,MIN(5,ROUND((IF((C5+D5)/200*100&gt;=80,5,IF((C5+D5)/200*100&gt;=70,4,IF((C5+D5)/200*100&gt;=60,3.5,IF((C5+D5)/200*100&gt;=50,3,IF((C5+D5)/200*100&gt;=40,2,IF((C5+D5)/200*100&gt;=33,1,0))))))+IF((E5+F5)/200*100&gt;=80,5,IF((E5+F5)/200*100&gt;=70,4,IF((E5+F5)/200*100&gt;=60,3.5,IF((E5+F5)/200*100&gt;=50,3,IF((E5+F5)/200*100&gt;=40,2,IF((E5+F5)/200*100&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF((H5+I5)/200*100&gt;=80,5,IF((H5+I5)/200*100&gt;=70,4,IF((H5+I5)/200*100&gt;=60,3.5,IF((H5+I5)/200*100&gt;=50,3,IF((H5+I5)/200*100&gt;=40,2,IF((H5+I5)/200*100&gt;=33,1,0))))))+IF((J5+K5)/200*100&gt;=80,5,IF((J5+K5)/200*100&gt;=70,4,IF((J5+K5)/200*100&gt;=60,3.5,IF((J5+K5)/200*100&gt;=50,3,IF((J5+K5)/200*100&gt;=40,2,IF((J5+K5)/200*100&gt;=33,1,0))))))+IF(L5&gt;=80,5,IF(L5&gt;=70,4,IF(L5&gt;=60,3.5,IF(L5&gt;=50,3,IF(L5&gt;=40,2,IF(L5&gt;=33,1,0))))))+IF(M5&gt;=80,5,IF(M5&gt;=70,4,IF(M5&gt;=60,3.5,IF(M5&gt;=50,3,IF(M5&gt;=40,2,IF(M5&gt;=33,1,0))))))+IF(N5&gt;=80,5,IF(N5&gt;=70,4,IF(N5&gt;=60,3.5,IF(N5&gt;=50,3,IF(N5&gt;=40,2,IF(N5&gt;=33,1,0)))))))/8+IF(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))&gt;=2,(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U5" s="6">
+        <f>IF(T5&gt;=5,"A+",IF(T5&gt;=4,"A",IF(T5&gt;=3.5,"A-",IF(T5&gt;=3,"B",IF(T5&gt;=2,"C",IF(T5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1101,53 +1173,65 @@
           <t>Rahim Uddin</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>147</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>131</v>
+      <c r="C6" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>69</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>125</v>
+        <v>82</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>173</v>
-      </c>
-      <c r="H6" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="H6" s="2" t="n">
+        <v>64</v>
+      </c>
       <c r="I6" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="J6" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="K6" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="O6" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q6" s="3" t="n">
         <v>89</v>
       </c>
-      <c r="K6" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="L6" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>94</v>
-      </c>
-      <c r="N6">
-        <f>SUM(C6:J6)</f>
-        <v/>
-      </c>
-      <c r="O6" s="4">
-        <f>ROUND(N6/8,2)</f>
-        <v/>
-      </c>
-      <c r="P6" s="5">
-        <f>IF(OR(C6&lt;66,D6&lt;66,E6&lt;33,F6&lt;66,G6&lt;66,H6&lt;33,I6&lt;33,J6&lt;33,L6&lt;33,M6&lt;33),0,MIN(5,ROUND((IF(C6/200*100&gt;=80,5,IF(C6/200*100&gt;=70,4,IF(C6/200*100&gt;=60,3.5,IF(C6/200*100&gt;=50,3,IF(C6/200*100&gt;=40,2,IF(C6/200*100&gt;=33,1,0))))))+IF(D6/200*100&gt;=80,5,IF(D6/200*100&gt;=70,4,IF(D6/200*100&gt;=60,3.5,IF(D6/200*100&gt;=50,3,IF(D6/200*100&gt;=40,2,IF(D6/200*100&gt;=33,1,0))))))+IF(E6&gt;=80,5,IF(E6&gt;=70,4,IF(E6&gt;=60,3.5,IF(E6&gt;=50,3,IF(E6&gt;=40,2,IF(E6&gt;=33,1,0))))))+IF(F6/200*100&gt;=80,5,IF(F6/200*100&gt;=70,4,IF(F6/200*100&gt;=60,3.5,IF(F6/200*100&gt;=50,3,IF(F6/200*100&gt;=40,2,IF(F6/200*100&gt;=33,1,0))))))+IF(G6/200*100&gt;=80,5,IF(G6/200*100&gt;=70,4,IF(G6/200*100&gt;=60,3.5,IF(G6/200*100&gt;=50,3,IF(G6/200*100&gt;=40,2,IF(G6/200*100&gt;=33,1,0))))))+IF(H6&gt;=80,5,IF(H6&gt;=70,4,IF(H6&gt;=60,3.5,IF(H6&gt;=50,3,IF(H6&gt;=40,2,IF(H6&gt;=33,1,0))))))+IF(I6&gt;=80,5,IF(I6&gt;=70,4,IF(I6&gt;=60,3.5,IF(I6&gt;=50,3,IF(I6&gt;=40,2,IF(I6&gt;=33,1,0))))))+IF(J6&gt;=80,5,IF(J6&gt;=70,4,IF(J6&gt;=60,3.5,IF(J6&gt;=50,3,IF(J6&gt;=40,2,IF(J6&gt;=33,1,0)))))))/8+IF(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))&gt;=2,(IF(K6&gt;=80,5,IF(K6&gt;=70,4,IF(K6&gt;=60,3.5,IF(K6&gt;=50,3,IF(K6&gt;=40,2,IF(K6&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q6" s="6">
-        <f>IF(P6&gt;=5,"A+",IF(P6&gt;=4,"A",IF(P6&gt;=3.5,"A-",IF(P6&gt;=3,"B",IF(P6&gt;=2,"C",IF(P6&gt;=1,"D","F"))))))</f>
+      <c r="R6">
+        <f>SUM(C6:N6)</f>
+        <v/>
+      </c>
+      <c r="S6" s="4">
+        <f>ROUND(R6/12,2)</f>
+        <v/>
+      </c>
+      <c r="T6" s="5">
+        <f>IF(OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,(J6+K6)&lt;66,L6&lt;33,M6&lt;33,N6&lt;33,P6&lt;33,Q6&lt;33),0,MIN(5,ROUND((IF((C6+D6)/200*100&gt;=80,5,IF((C6+D6)/200*100&gt;=70,4,IF((C6+D6)/200*100&gt;=60,3.5,IF((C6+D6)/200*100&gt;=50,3,IF((C6+D6)/200*100&gt;=40,2,IF((C6+D6)/200*100&gt;=33,1,0))))))+IF((E6+F6)/200*100&gt;=80,5,IF((E6+F6)/200*100&gt;=70,4,IF((E6+F6)/200*100&gt;=60,3.5,IF((E6+F6)/200*100&gt;=50,3,IF((E6+F6)/200*100&gt;=40,2,IF((E6+F6)/200*100&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF((H6+I6)/200*100&gt;=80,5,IF((H6+I6)/200*100&gt;=70,4,IF((H6+I6)/200*100&gt;=60,3.5,IF((H6+I6)/200*100&gt;=50,3,IF((H6+I6)/200*100&gt;=40,2,IF((H6+I6)/200*100&gt;=33,1,0))))))+IF((J6+K6)/200*100&gt;=80,5,IF((J6+K6)/200*100&gt;=70,4,IF((J6+K6)/200*100&gt;=60,3.5,IF((J6+K6)/200*100&gt;=50,3,IF((J6+K6)/200*100&gt;=40,2,IF((J6+K6)/200*100&gt;=33,1,0))))))+IF(L6&gt;=80,5,IF(L6&gt;=70,4,IF(L6&gt;=60,3.5,IF(L6&gt;=50,3,IF(L6&gt;=40,2,IF(L6&gt;=33,1,0))))))+IF(M6&gt;=80,5,IF(M6&gt;=70,4,IF(M6&gt;=60,3.5,IF(M6&gt;=50,3,IF(M6&gt;=40,2,IF(M6&gt;=33,1,0))))))+IF(N6&gt;=80,5,IF(N6&gt;=70,4,IF(N6&gt;=60,3.5,IF(N6&gt;=50,3,IF(N6&gt;=40,2,IF(N6&gt;=33,1,0)))))))/8+IF(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))&gt;=2,(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U6" s="6">
+        <f>IF(T6&gt;=5,"A+",IF(T6&gt;=4,"A",IF(T6&gt;=3.5,"A-",IF(T6&gt;=3,"B",IF(T6&gt;=2,"C",IF(T6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1160,53 +1244,65 @@
           <t>Nadia Islam</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>145</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>165</v>
+      <c r="C7" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>90</v>
       </c>
       <c r="E7" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="P7" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="F7" s="3" t="n">
-        <v>149</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>159</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="K7" s="3" t="n">
-        <v>69</v>
-      </c>
-      <c r="L7" s="3" t="n">
-        <v>71</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="N7">
-        <f>SUM(C7:J7)</f>
-        <v/>
-      </c>
-      <c r="O7" s="4">
-        <f>ROUND(N7/8,2)</f>
-        <v/>
-      </c>
-      <c r="P7" s="5">
-        <f>IF(OR(C7&lt;66,D7&lt;66,E7&lt;33,F7&lt;66,G7&lt;66,H7&lt;33,I7&lt;33,J7&lt;33,L7&lt;33,M7&lt;33),0,MIN(5,ROUND((IF(C7/200*100&gt;=80,5,IF(C7/200*100&gt;=70,4,IF(C7/200*100&gt;=60,3.5,IF(C7/200*100&gt;=50,3,IF(C7/200*100&gt;=40,2,IF(C7/200*100&gt;=33,1,0))))))+IF(D7/200*100&gt;=80,5,IF(D7/200*100&gt;=70,4,IF(D7/200*100&gt;=60,3.5,IF(D7/200*100&gt;=50,3,IF(D7/200*100&gt;=40,2,IF(D7/200*100&gt;=33,1,0))))))+IF(E7&gt;=80,5,IF(E7&gt;=70,4,IF(E7&gt;=60,3.5,IF(E7&gt;=50,3,IF(E7&gt;=40,2,IF(E7&gt;=33,1,0))))))+IF(F7/200*100&gt;=80,5,IF(F7/200*100&gt;=70,4,IF(F7/200*100&gt;=60,3.5,IF(F7/200*100&gt;=50,3,IF(F7/200*100&gt;=40,2,IF(F7/200*100&gt;=33,1,0))))))+IF(G7/200*100&gt;=80,5,IF(G7/200*100&gt;=70,4,IF(G7/200*100&gt;=60,3.5,IF(G7/200*100&gt;=50,3,IF(G7/200*100&gt;=40,2,IF(G7/200*100&gt;=33,1,0))))))+IF(H7&gt;=80,5,IF(H7&gt;=70,4,IF(H7&gt;=60,3.5,IF(H7&gt;=50,3,IF(H7&gt;=40,2,IF(H7&gt;=33,1,0))))))+IF(I7&gt;=80,5,IF(I7&gt;=70,4,IF(I7&gt;=60,3.5,IF(I7&gt;=50,3,IF(I7&gt;=40,2,IF(I7&gt;=33,1,0))))))+IF(J7&gt;=80,5,IF(J7&gt;=70,4,IF(J7&gt;=60,3.5,IF(J7&gt;=50,3,IF(J7&gt;=40,2,IF(J7&gt;=33,1,0)))))))/8+IF(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))&gt;=2,(IF(K7&gt;=80,5,IF(K7&gt;=70,4,IF(K7&gt;=60,3.5,IF(K7&gt;=50,3,IF(K7&gt;=40,2,IF(K7&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="6">
-        <f>IF(P7&gt;=5,"A+",IF(P7&gt;=4,"A",IF(P7&gt;=3.5,"A-",IF(P7&gt;=3,"B",IF(P7&gt;=2,"C",IF(P7&gt;=1,"D","F"))))))</f>
+      <c r="Q7" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="R7">
+        <f>SUM(C7:N7)</f>
+        <v/>
+      </c>
+      <c r="S7" s="4">
+        <f>ROUND(R7/12,2)</f>
+        <v/>
+      </c>
+      <c r="T7" s="5">
+        <f>IF(OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,(J7+K7)&lt;66,L7&lt;33,M7&lt;33,N7&lt;33,P7&lt;33,Q7&lt;33),0,MIN(5,ROUND((IF((C7+D7)/200*100&gt;=80,5,IF((C7+D7)/200*100&gt;=70,4,IF((C7+D7)/200*100&gt;=60,3.5,IF((C7+D7)/200*100&gt;=50,3,IF((C7+D7)/200*100&gt;=40,2,IF((C7+D7)/200*100&gt;=33,1,0))))))+IF((E7+F7)/200*100&gt;=80,5,IF((E7+F7)/200*100&gt;=70,4,IF((E7+F7)/200*100&gt;=60,3.5,IF((E7+F7)/200*100&gt;=50,3,IF((E7+F7)/200*100&gt;=40,2,IF((E7+F7)/200*100&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF((H7+I7)/200*100&gt;=80,5,IF((H7+I7)/200*100&gt;=70,4,IF((H7+I7)/200*100&gt;=60,3.5,IF((H7+I7)/200*100&gt;=50,3,IF((H7+I7)/200*100&gt;=40,2,IF((H7+I7)/200*100&gt;=33,1,0))))))+IF((J7+K7)/200*100&gt;=80,5,IF((J7+K7)/200*100&gt;=70,4,IF((J7+K7)/200*100&gt;=60,3.5,IF((J7+K7)/200*100&gt;=50,3,IF((J7+K7)/200*100&gt;=40,2,IF((J7+K7)/200*100&gt;=33,1,0))))))+IF(L7&gt;=80,5,IF(L7&gt;=70,4,IF(L7&gt;=60,3.5,IF(L7&gt;=50,3,IF(L7&gt;=40,2,IF(L7&gt;=33,1,0))))))+IF(M7&gt;=80,5,IF(M7&gt;=70,4,IF(M7&gt;=60,3.5,IF(M7&gt;=50,3,IF(M7&gt;=40,2,IF(M7&gt;=33,1,0))))))+IF(N7&gt;=80,5,IF(N7&gt;=70,4,IF(N7&gt;=60,3.5,IF(N7&gt;=50,3,IF(N7&gt;=40,2,IF(N7&gt;=33,1,0)))))))/8+IF(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))&gt;=2,(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U7" s="6">
+        <f>IF(T7&gt;=5,"A+",IF(T7&gt;=4,"A",IF(T7&gt;=3.5,"A-",IF(T7&gt;=3,"B",IF(T7&gt;=2,"C",IF(T7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1219,53 +1315,65 @@
           <t>Jahir Ahmed</t>
         </is>
       </c>
-      <c r="C8" s="3" t="n">
-        <v>144</v>
+      <c r="C8" s="2" t="n">
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>157</v>
+        <v>76</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>68</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="L8" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="M8" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="N8">
-        <f>SUM(C8:J8)</f>
-        <v/>
-      </c>
-      <c r="O8" s="4">
-        <f>ROUND(N8/8,2)</f>
-        <v/>
-      </c>
-      <c r="P8" s="5">
-        <f>IF(OR(C8&lt;66,D8&lt;66,E8&lt;33,F8&lt;66,G8&lt;66,H8&lt;33,I8&lt;33,J8&lt;33,L8&lt;33,M8&lt;33),0,MIN(5,ROUND((IF(C8/200*100&gt;=80,5,IF(C8/200*100&gt;=70,4,IF(C8/200*100&gt;=60,3.5,IF(C8/200*100&gt;=50,3,IF(C8/200*100&gt;=40,2,IF(C8/200*100&gt;=33,1,0))))))+IF(D8/200*100&gt;=80,5,IF(D8/200*100&gt;=70,4,IF(D8/200*100&gt;=60,3.5,IF(D8/200*100&gt;=50,3,IF(D8/200*100&gt;=40,2,IF(D8/200*100&gt;=33,1,0))))))+IF(E8&gt;=80,5,IF(E8&gt;=70,4,IF(E8&gt;=60,3.5,IF(E8&gt;=50,3,IF(E8&gt;=40,2,IF(E8&gt;=33,1,0))))))+IF(F8/200*100&gt;=80,5,IF(F8/200*100&gt;=70,4,IF(F8/200*100&gt;=60,3.5,IF(F8/200*100&gt;=50,3,IF(F8/200*100&gt;=40,2,IF(F8/200*100&gt;=33,1,0))))))+IF(G8/200*100&gt;=80,5,IF(G8/200*100&gt;=70,4,IF(G8/200*100&gt;=60,3.5,IF(G8/200*100&gt;=50,3,IF(G8/200*100&gt;=40,2,IF(G8/200*100&gt;=33,1,0))))))+IF(H8&gt;=80,5,IF(H8&gt;=70,4,IF(H8&gt;=60,3.5,IF(H8&gt;=50,3,IF(H8&gt;=40,2,IF(H8&gt;=33,1,0))))))+IF(I8&gt;=80,5,IF(I8&gt;=70,4,IF(I8&gt;=60,3.5,IF(I8&gt;=50,3,IF(I8&gt;=40,2,IF(I8&gt;=33,1,0))))))+IF(J8&gt;=80,5,IF(J8&gt;=70,4,IF(J8&gt;=60,3.5,IF(J8&gt;=50,3,IF(J8&gt;=40,2,IF(J8&gt;=33,1,0)))))))/8+IF(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))&gt;=2,(IF(K8&gt;=80,5,IF(K8&gt;=70,4,IF(K8&gt;=60,3.5,IF(K8&gt;=50,3,IF(K8&gt;=40,2,IF(K8&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q8" s="6">
-        <f>IF(P8&gt;=5,"A+",IF(P8&gt;=4,"A",IF(P8&gt;=3.5,"A-",IF(P8&gt;=3,"B",IF(P8&gt;=2,"C",IF(P8&gt;=1,"D","F"))))))</f>
+        <v>78</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="O8" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="R8">
+        <f>SUM(C8:N8)</f>
+        <v/>
+      </c>
+      <c r="S8" s="4">
+        <f>ROUND(R8/12,2)</f>
+        <v/>
+      </c>
+      <c r="T8" s="5">
+        <f>IF(OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,(J8+K8)&lt;66,L8&lt;33,M8&lt;33,N8&lt;33,P8&lt;33,Q8&lt;33),0,MIN(5,ROUND((IF((C8+D8)/200*100&gt;=80,5,IF((C8+D8)/200*100&gt;=70,4,IF((C8+D8)/200*100&gt;=60,3.5,IF((C8+D8)/200*100&gt;=50,3,IF((C8+D8)/200*100&gt;=40,2,IF((C8+D8)/200*100&gt;=33,1,0))))))+IF((E8+F8)/200*100&gt;=80,5,IF((E8+F8)/200*100&gt;=70,4,IF((E8+F8)/200*100&gt;=60,3.5,IF((E8+F8)/200*100&gt;=50,3,IF((E8+F8)/200*100&gt;=40,2,IF((E8+F8)/200*100&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF((H8+I8)/200*100&gt;=80,5,IF((H8+I8)/200*100&gt;=70,4,IF((H8+I8)/200*100&gt;=60,3.5,IF((H8+I8)/200*100&gt;=50,3,IF((H8+I8)/200*100&gt;=40,2,IF((H8+I8)/200*100&gt;=33,1,0))))))+IF((J8+K8)/200*100&gt;=80,5,IF((J8+K8)/200*100&gt;=70,4,IF((J8+K8)/200*100&gt;=60,3.5,IF((J8+K8)/200*100&gt;=50,3,IF((J8+K8)/200*100&gt;=40,2,IF((J8+K8)/200*100&gt;=33,1,0))))))+IF(L8&gt;=80,5,IF(L8&gt;=70,4,IF(L8&gt;=60,3.5,IF(L8&gt;=50,3,IF(L8&gt;=40,2,IF(L8&gt;=33,1,0))))))+IF(M8&gt;=80,5,IF(M8&gt;=70,4,IF(M8&gt;=60,3.5,IF(M8&gt;=50,3,IF(M8&gt;=40,2,IF(M8&gt;=33,1,0))))))+IF(N8&gt;=80,5,IF(N8&gt;=70,4,IF(N8&gt;=60,3.5,IF(N8&gt;=50,3,IF(N8&gt;=40,2,IF(N8&gt;=33,1,0)))))))/8+IF(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))&gt;=2,(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U8" s="6">
+        <f>IF(T8&gt;=5,"A+",IF(T8&gt;=4,"A",IF(T8&gt;=3.5,"A-",IF(T8&gt;=3,"B",IF(T8&gt;=2,"C",IF(T8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1279,52 +1387,64 @@
         </is>
       </c>
       <c r="C9" s="3" t="n">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>175</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>66</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>130</v>
+        <v>65</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>77</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>71</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>62</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="K9" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="O9" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="P9" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="L9" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="N9">
-        <f>SUM(C9:J9)</f>
-        <v/>
-      </c>
-      <c r="O9" s="4">
-        <f>ROUND(N9/8,2)</f>
-        <v/>
-      </c>
-      <c r="P9" s="5">
-        <f>IF(OR(C9&lt;66,D9&lt;66,E9&lt;33,F9&lt;66,G9&lt;66,H9&lt;33,I9&lt;33,J9&lt;33,L9&lt;33,M9&lt;33),0,MIN(5,ROUND((IF(C9/200*100&gt;=80,5,IF(C9/200*100&gt;=70,4,IF(C9/200*100&gt;=60,3.5,IF(C9/200*100&gt;=50,3,IF(C9/200*100&gt;=40,2,IF(C9/200*100&gt;=33,1,0))))))+IF(D9/200*100&gt;=80,5,IF(D9/200*100&gt;=70,4,IF(D9/200*100&gt;=60,3.5,IF(D9/200*100&gt;=50,3,IF(D9/200*100&gt;=40,2,IF(D9/200*100&gt;=33,1,0))))))+IF(E9&gt;=80,5,IF(E9&gt;=70,4,IF(E9&gt;=60,3.5,IF(E9&gt;=50,3,IF(E9&gt;=40,2,IF(E9&gt;=33,1,0))))))+IF(F9/200*100&gt;=80,5,IF(F9/200*100&gt;=70,4,IF(F9/200*100&gt;=60,3.5,IF(F9/200*100&gt;=50,3,IF(F9/200*100&gt;=40,2,IF(F9/200*100&gt;=33,1,0))))))+IF(G9/200*100&gt;=80,5,IF(G9/200*100&gt;=70,4,IF(G9/200*100&gt;=60,3.5,IF(G9/200*100&gt;=50,3,IF(G9/200*100&gt;=40,2,IF(G9/200*100&gt;=33,1,0))))))+IF(H9&gt;=80,5,IF(H9&gt;=70,4,IF(H9&gt;=60,3.5,IF(H9&gt;=50,3,IF(H9&gt;=40,2,IF(H9&gt;=33,1,0))))))+IF(I9&gt;=80,5,IF(I9&gt;=70,4,IF(I9&gt;=60,3.5,IF(I9&gt;=50,3,IF(I9&gt;=40,2,IF(I9&gt;=33,1,0))))))+IF(J9&gt;=80,5,IF(J9&gt;=70,4,IF(J9&gt;=60,3.5,IF(J9&gt;=50,3,IF(J9&gt;=40,2,IF(J9&gt;=33,1,0)))))))/8+IF(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))&gt;=2,(IF(K9&gt;=80,5,IF(K9&gt;=70,4,IF(K9&gt;=60,3.5,IF(K9&gt;=50,3,IF(K9&gt;=40,2,IF(K9&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="6">
-        <f>IF(P9&gt;=5,"A+",IF(P9&gt;=4,"A",IF(P9&gt;=3.5,"A-",IF(P9&gt;=3,"B",IF(P9&gt;=2,"C",IF(P9&gt;=1,"D","F"))))))</f>
+      <c r="Q9" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="R9">
+        <f>SUM(C9:N9)</f>
+        <v/>
+      </c>
+      <c r="S9" s="4">
+        <f>ROUND(R9/12,2)</f>
+        <v/>
+      </c>
+      <c r="T9" s="5">
+        <f>IF(OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,(J9+K9)&lt;66,L9&lt;33,M9&lt;33,N9&lt;33,P9&lt;33,Q9&lt;33),0,MIN(5,ROUND((IF((C9+D9)/200*100&gt;=80,5,IF((C9+D9)/200*100&gt;=70,4,IF((C9+D9)/200*100&gt;=60,3.5,IF((C9+D9)/200*100&gt;=50,3,IF((C9+D9)/200*100&gt;=40,2,IF((C9+D9)/200*100&gt;=33,1,0))))))+IF((E9+F9)/200*100&gt;=80,5,IF((E9+F9)/200*100&gt;=70,4,IF((E9+F9)/200*100&gt;=60,3.5,IF((E9+F9)/200*100&gt;=50,3,IF((E9+F9)/200*100&gt;=40,2,IF((E9+F9)/200*100&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF((H9+I9)/200*100&gt;=80,5,IF((H9+I9)/200*100&gt;=70,4,IF((H9+I9)/200*100&gt;=60,3.5,IF((H9+I9)/200*100&gt;=50,3,IF((H9+I9)/200*100&gt;=40,2,IF((H9+I9)/200*100&gt;=33,1,0))))))+IF((J9+K9)/200*100&gt;=80,5,IF((J9+K9)/200*100&gt;=70,4,IF((J9+K9)/200*100&gt;=60,3.5,IF((J9+K9)/200*100&gt;=50,3,IF((J9+K9)/200*100&gt;=40,2,IF((J9+K9)/200*100&gt;=33,1,0))))))+IF(L9&gt;=80,5,IF(L9&gt;=70,4,IF(L9&gt;=60,3.5,IF(L9&gt;=50,3,IF(L9&gt;=40,2,IF(L9&gt;=33,1,0))))))+IF(M9&gt;=80,5,IF(M9&gt;=70,4,IF(M9&gt;=60,3.5,IF(M9&gt;=50,3,IF(M9&gt;=40,2,IF(M9&gt;=33,1,0))))))+IF(N9&gt;=80,5,IF(N9&gt;=70,4,IF(N9&gt;=60,3.5,IF(N9&gt;=50,3,IF(N9&gt;=40,2,IF(N9&gt;=33,1,0)))))))/8+IF(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))&gt;=2,(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U9" s="6">
+        <f>IF(T9&gt;=5,"A+",IF(T9&gt;=4,"A",IF(T9&gt;=3.5,"A-",IF(T9&gt;=3,"B",IF(T9&gt;=2,"C",IF(T9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1338,52 +1458,64 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>177</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>171</v>
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>89</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>65</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>149</v>
+        <v>89</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>73</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>132</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>90</v>
       </c>
       <c r="I10" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>59</v>
+      </c>
+      <c r="M10" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="J10" s="3" t="n">
-        <v>75</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="L10" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="N10">
-        <f>SUM(C10:J10)</f>
-        <v/>
-      </c>
-      <c r="O10" s="4">
-        <f>ROUND(N10/8,2)</f>
-        <v/>
-      </c>
-      <c r="P10" s="5">
-        <f>IF(OR(C10&lt;66,D10&lt;66,E10&lt;33,F10&lt;66,G10&lt;66,H10&lt;33,I10&lt;33,J10&lt;33,L10&lt;33,M10&lt;33),0,MIN(5,ROUND((IF(C10/200*100&gt;=80,5,IF(C10/200*100&gt;=70,4,IF(C10/200*100&gt;=60,3.5,IF(C10/200*100&gt;=50,3,IF(C10/200*100&gt;=40,2,IF(C10/200*100&gt;=33,1,0))))))+IF(D10/200*100&gt;=80,5,IF(D10/200*100&gt;=70,4,IF(D10/200*100&gt;=60,3.5,IF(D10/200*100&gt;=50,3,IF(D10/200*100&gt;=40,2,IF(D10/200*100&gt;=33,1,0))))))+IF(E10&gt;=80,5,IF(E10&gt;=70,4,IF(E10&gt;=60,3.5,IF(E10&gt;=50,3,IF(E10&gt;=40,2,IF(E10&gt;=33,1,0))))))+IF(F10/200*100&gt;=80,5,IF(F10/200*100&gt;=70,4,IF(F10/200*100&gt;=60,3.5,IF(F10/200*100&gt;=50,3,IF(F10/200*100&gt;=40,2,IF(F10/200*100&gt;=33,1,0))))))+IF(G10/200*100&gt;=80,5,IF(G10/200*100&gt;=70,4,IF(G10/200*100&gt;=60,3.5,IF(G10/200*100&gt;=50,3,IF(G10/200*100&gt;=40,2,IF(G10/200*100&gt;=33,1,0))))))+IF(H10&gt;=80,5,IF(H10&gt;=70,4,IF(H10&gt;=60,3.5,IF(H10&gt;=50,3,IF(H10&gt;=40,2,IF(H10&gt;=33,1,0))))))+IF(I10&gt;=80,5,IF(I10&gt;=70,4,IF(I10&gt;=60,3.5,IF(I10&gt;=50,3,IF(I10&gt;=40,2,IF(I10&gt;=33,1,0))))))+IF(J10&gt;=80,5,IF(J10&gt;=70,4,IF(J10&gt;=60,3.5,IF(J10&gt;=50,3,IF(J10&gt;=40,2,IF(J10&gt;=33,1,0)))))))/8+IF(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))&gt;=2,(IF(K10&gt;=80,5,IF(K10&gt;=70,4,IF(K10&gt;=60,3.5,IF(K10&gt;=50,3,IF(K10&gt;=40,2,IF(K10&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q10" s="6">
-        <f>IF(P10&gt;=5,"A+",IF(P10&gt;=4,"A",IF(P10&gt;=3.5,"A-",IF(P10&gt;=3,"B",IF(P10&gt;=2,"C",IF(P10&gt;=1,"D","F"))))))</f>
+      <c r="N10" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="O10" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q10" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="R10">
+        <f>SUM(C10:N10)</f>
+        <v/>
+      </c>
+      <c r="S10" s="4">
+        <f>ROUND(R10/12,2)</f>
+        <v/>
+      </c>
+      <c r="T10" s="5">
+        <f>IF(OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,(J10+K10)&lt;66,L10&lt;33,M10&lt;33,N10&lt;33,P10&lt;33,Q10&lt;33),0,MIN(5,ROUND((IF((C10+D10)/200*100&gt;=80,5,IF((C10+D10)/200*100&gt;=70,4,IF((C10+D10)/200*100&gt;=60,3.5,IF((C10+D10)/200*100&gt;=50,3,IF((C10+D10)/200*100&gt;=40,2,IF((C10+D10)/200*100&gt;=33,1,0))))))+IF((E10+F10)/200*100&gt;=80,5,IF((E10+F10)/200*100&gt;=70,4,IF((E10+F10)/200*100&gt;=60,3.5,IF((E10+F10)/200*100&gt;=50,3,IF((E10+F10)/200*100&gt;=40,2,IF((E10+F10)/200*100&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF((H10+I10)/200*100&gt;=80,5,IF((H10+I10)/200*100&gt;=70,4,IF((H10+I10)/200*100&gt;=60,3.5,IF((H10+I10)/200*100&gt;=50,3,IF((H10+I10)/200*100&gt;=40,2,IF((H10+I10)/200*100&gt;=33,1,0))))))+IF((J10+K10)/200*100&gt;=80,5,IF((J10+K10)/200*100&gt;=70,4,IF((J10+K10)/200*100&gt;=60,3.5,IF((J10+K10)/200*100&gt;=50,3,IF((J10+K10)/200*100&gt;=40,2,IF((J10+K10)/200*100&gt;=33,1,0))))))+IF(L10&gt;=80,5,IF(L10&gt;=70,4,IF(L10&gt;=60,3.5,IF(L10&gt;=50,3,IF(L10&gt;=40,2,IF(L10&gt;=33,1,0))))))+IF(M10&gt;=80,5,IF(M10&gt;=70,4,IF(M10&gt;=60,3.5,IF(M10&gt;=50,3,IF(M10&gt;=40,2,IF(M10&gt;=33,1,0))))))+IF(N10&gt;=80,5,IF(N10&gt;=70,4,IF(N10&gt;=60,3.5,IF(N10&gt;=50,3,IF(N10&gt;=40,2,IF(N10&gt;=33,1,0)))))))/8+IF(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))&gt;=2,(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U10" s="6">
+        <f>IF(T10&gt;=5,"A+",IF(T10&gt;=4,"A",IF(T10&gt;=3.5,"A-",IF(T10&gt;=3,"B",IF(T10&gt;=2,"C",IF(T10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1397,52 +1529,64 @@
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>136</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>174</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>84</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>132</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>154</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>89</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>68</v>
-      </c>
-      <c r="K11" s="3" t="n">
-        <v>62</v>
+        <v>89</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>65</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="M11" s="2" t="n">
-        <v>84</v>
-      </c>
-      <c r="N11">
-        <f>SUM(C11:J11)</f>
-        <v/>
-      </c>
-      <c r="O11" s="4">
-        <f>ROUND(N11/8,2)</f>
-        <v/>
-      </c>
-      <c r="P11" s="5">
-        <f>IF(OR(C11&lt;66,D11&lt;66,E11&lt;33,F11&lt;66,G11&lt;66,H11&lt;33,I11&lt;33,J11&lt;33,L11&lt;33,M11&lt;33),0,MIN(5,ROUND((IF(C11/200*100&gt;=80,5,IF(C11/200*100&gt;=70,4,IF(C11/200*100&gt;=60,3.5,IF(C11/200*100&gt;=50,3,IF(C11/200*100&gt;=40,2,IF(C11/200*100&gt;=33,1,0))))))+IF(D11/200*100&gt;=80,5,IF(D11/200*100&gt;=70,4,IF(D11/200*100&gt;=60,3.5,IF(D11/200*100&gt;=50,3,IF(D11/200*100&gt;=40,2,IF(D11/200*100&gt;=33,1,0))))))+IF(E11&gt;=80,5,IF(E11&gt;=70,4,IF(E11&gt;=60,3.5,IF(E11&gt;=50,3,IF(E11&gt;=40,2,IF(E11&gt;=33,1,0))))))+IF(F11/200*100&gt;=80,5,IF(F11/200*100&gt;=70,4,IF(F11/200*100&gt;=60,3.5,IF(F11/200*100&gt;=50,3,IF(F11/200*100&gt;=40,2,IF(F11/200*100&gt;=33,1,0))))))+IF(G11/200*100&gt;=80,5,IF(G11/200*100&gt;=70,4,IF(G11/200*100&gt;=60,3.5,IF(G11/200*100&gt;=50,3,IF(G11/200*100&gt;=40,2,IF(G11/200*100&gt;=33,1,0))))))+IF(H11&gt;=80,5,IF(H11&gt;=70,4,IF(H11&gt;=60,3.5,IF(H11&gt;=50,3,IF(H11&gt;=40,2,IF(H11&gt;=33,1,0))))))+IF(I11&gt;=80,5,IF(I11&gt;=70,4,IF(I11&gt;=60,3.5,IF(I11&gt;=50,3,IF(I11&gt;=40,2,IF(I11&gt;=33,1,0))))))+IF(J11&gt;=80,5,IF(J11&gt;=70,4,IF(J11&gt;=60,3.5,IF(J11&gt;=50,3,IF(J11&gt;=40,2,IF(J11&gt;=33,1,0)))))))/8+IF(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))&gt;=2,(IF(K11&gt;=80,5,IF(K11&gt;=70,4,IF(K11&gt;=60,3.5,IF(K11&gt;=50,3,IF(K11&gt;=40,2,IF(K11&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="6">
-        <f>IF(P11&gt;=5,"A+",IF(P11&gt;=4,"A",IF(P11&gt;=3.5,"A-",IF(P11&gt;=3,"B",IF(P11&gt;=2,"C",IF(P11&gt;=1,"D","F"))))))</f>
+        <v>89</v>
+      </c>
+      <c r="M11" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="R11">
+        <f>SUM(C11:N11)</f>
+        <v/>
+      </c>
+      <c r="S11" s="4">
+        <f>ROUND(R11/12,2)</f>
+        <v/>
+      </c>
+      <c r="T11" s="5">
+        <f>IF(OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,(J11+K11)&lt;66,L11&lt;33,M11&lt;33,N11&lt;33,P11&lt;33,Q11&lt;33),0,MIN(5,ROUND((IF((C11+D11)/200*100&gt;=80,5,IF((C11+D11)/200*100&gt;=70,4,IF((C11+D11)/200*100&gt;=60,3.5,IF((C11+D11)/200*100&gt;=50,3,IF((C11+D11)/200*100&gt;=40,2,IF((C11+D11)/200*100&gt;=33,1,0))))))+IF((E11+F11)/200*100&gt;=80,5,IF((E11+F11)/200*100&gt;=70,4,IF((E11+F11)/200*100&gt;=60,3.5,IF((E11+F11)/200*100&gt;=50,3,IF((E11+F11)/200*100&gt;=40,2,IF((E11+F11)/200*100&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF((H11+I11)/200*100&gt;=80,5,IF((H11+I11)/200*100&gt;=70,4,IF((H11+I11)/200*100&gt;=60,3.5,IF((H11+I11)/200*100&gt;=50,3,IF((H11+I11)/200*100&gt;=40,2,IF((H11+I11)/200*100&gt;=33,1,0))))))+IF((J11+K11)/200*100&gt;=80,5,IF((J11+K11)/200*100&gt;=70,4,IF((J11+K11)/200*100&gt;=60,3.5,IF((J11+K11)/200*100&gt;=50,3,IF((J11+K11)/200*100&gt;=40,2,IF((J11+K11)/200*100&gt;=33,1,0))))))+IF(L11&gt;=80,5,IF(L11&gt;=70,4,IF(L11&gt;=60,3.5,IF(L11&gt;=50,3,IF(L11&gt;=40,2,IF(L11&gt;=33,1,0))))))+IF(M11&gt;=80,5,IF(M11&gt;=70,4,IF(M11&gt;=60,3.5,IF(M11&gt;=50,3,IF(M11&gt;=40,2,IF(M11&gt;=33,1,0))))))+IF(N11&gt;=80,5,IF(N11&gt;=70,4,IF(N11&gt;=60,3.5,IF(N11&gt;=50,3,IF(N11&gt;=40,2,IF(N11&gt;=33,1,0)))))))/8+IF(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))&gt;=2,(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U11" s="6">
+        <f>IF(T11&gt;=5,"A+",IF(T11&gt;=4,"A",IF(T11&gt;=3.5,"A-",IF(T11&gt;=3,"B",IF(T11&gt;=2,"C",IF(T11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1456,52 +1600,64 @@
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>173</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>164</v>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>66</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>168</v>
+        <v>70</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>85</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="I12" s="3" t="n">
-        <v>79</v>
-      </c>
-      <c r="J12" s="3" t="n">
-        <v>74</v>
-      </c>
-      <c r="K12" s="7" t="n">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>87</v>
-      </c>
-      <c r="N12">
-        <f>SUM(C12:J12)</f>
-        <v/>
-      </c>
-      <c r="O12" s="4">
-        <f>ROUND(N12/8,2)</f>
-        <v/>
-      </c>
-      <c r="P12" s="5">
-        <f>IF(OR(C12&lt;66,D12&lt;66,E12&lt;33,F12&lt;66,G12&lt;66,H12&lt;33,I12&lt;33,J12&lt;33,L12&lt;33,M12&lt;33),0,MIN(5,ROUND((IF(C12/200*100&gt;=80,5,IF(C12/200*100&gt;=70,4,IF(C12/200*100&gt;=60,3.5,IF(C12/200*100&gt;=50,3,IF(C12/200*100&gt;=40,2,IF(C12/200*100&gt;=33,1,0))))))+IF(D12/200*100&gt;=80,5,IF(D12/200*100&gt;=70,4,IF(D12/200*100&gt;=60,3.5,IF(D12/200*100&gt;=50,3,IF(D12/200*100&gt;=40,2,IF(D12/200*100&gt;=33,1,0))))))+IF(E12&gt;=80,5,IF(E12&gt;=70,4,IF(E12&gt;=60,3.5,IF(E12&gt;=50,3,IF(E12&gt;=40,2,IF(E12&gt;=33,1,0))))))+IF(F12/200*100&gt;=80,5,IF(F12/200*100&gt;=70,4,IF(F12/200*100&gt;=60,3.5,IF(F12/200*100&gt;=50,3,IF(F12/200*100&gt;=40,2,IF(F12/200*100&gt;=33,1,0))))))+IF(G12/200*100&gt;=80,5,IF(G12/200*100&gt;=70,4,IF(G12/200*100&gt;=60,3.5,IF(G12/200*100&gt;=50,3,IF(G12/200*100&gt;=40,2,IF(G12/200*100&gt;=33,1,0))))))+IF(H12&gt;=80,5,IF(H12&gt;=70,4,IF(H12&gt;=60,3.5,IF(H12&gt;=50,3,IF(H12&gt;=40,2,IF(H12&gt;=33,1,0))))))+IF(I12&gt;=80,5,IF(I12&gt;=70,4,IF(I12&gt;=60,3.5,IF(I12&gt;=50,3,IF(I12&gt;=40,2,IF(I12&gt;=33,1,0))))))+IF(J12&gt;=80,5,IF(J12&gt;=70,4,IF(J12&gt;=60,3.5,IF(J12&gt;=50,3,IF(J12&gt;=40,2,IF(J12&gt;=33,1,0)))))))/8+IF(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))&gt;=2,(IF(K12&gt;=80,5,IF(K12&gt;=70,4,IF(K12&gt;=60,3.5,IF(K12&gt;=50,3,IF(K12&gt;=40,2,IF(K12&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="6">
-        <f>IF(P12&gt;=5,"A+",IF(P12&gt;=4,"A",IF(P12&gt;=3.5,"A-",IF(P12&gt;=3,"B",IF(P12&gt;=2,"C",IF(P12&gt;=1,"D","F"))))))</f>
+        <v>63</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q12" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="R12">
+        <f>SUM(C12:N12)</f>
+        <v/>
+      </c>
+      <c r="S12" s="4">
+        <f>ROUND(R12/12,2)</f>
+        <v/>
+      </c>
+      <c r="T12" s="5">
+        <f>IF(OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,(J12+K12)&lt;66,L12&lt;33,M12&lt;33,N12&lt;33,P12&lt;33,Q12&lt;33),0,MIN(5,ROUND((IF((C12+D12)/200*100&gt;=80,5,IF((C12+D12)/200*100&gt;=70,4,IF((C12+D12)/200*100&gt;=60,3.5,IF((C12+D12)/200*100&gt;=50,3,IF((C12+D12)/200*100&gt;=40,2,IF((C12+D12)/200*100&gt;=33,1,0))))))+IF((E12+F12)/200*100&gt;=80,5,IF((E12+F12)/200*100&gt;=70,4,IF((E12+F12)/200*100&gt;=60,3.5,IF((E12+F12)/200*100&gt;=50,3,IF((E12+F12)/200*100&gt;=40,2,IF((E12+F12)/200*100&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF((H12+I12)/200*100&gt;=80,5,IF((H12+I12)/200*100&gt;=70,4,IF((H12+I12)/200*100&gt;=60,3.5,IF((H12+I12)/200*100&gt;=50,3,IF((H12+I12)/200*100&gt;=40,2,IF((H12+I12)/200*100&gt;=33,1,0))))))+IF((J12+K12)/200*100&gt;=80,5,IF((J12+K12)/200*100&gt;=70,4,IF((J12+K12)/200*100&gt;=60,3.5,IF((J12+K12)/200*100&gt;=50,3,IF((J12+K12)/200*100&gt;=40,2,IF((J12+K12)/200*100&gt;=33,1,0))))))+IF(L12&gt;=80,5,IF(L12&gt;=70,4,IF(L12&gt;=60,3.5,IF(L12&gt;=50,3,IF(L12&gt;=40,2,IF(L12&gt;=33,1,0))))))+IF(M12&gt;=80,5,IF(M12&gt;=70,4,IF(M12&gt;=60,3.5,IF(M12&gt;=50,3,IF(M12&gt;=40,2,IF(M12&gt;=33,1,0))))))+IF(N12&gt;=80,5,IF(N12&gt;=70,4,IF(N12&gt;=60,3.5,IF(N12&gt;=50,3,IF(N12&gt;=40,2,IF(N12&gt;=33,1,0)))))))/8+IF(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))&gt;=2,(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U12" s="6">
+        <f>IF(T12&gt;=5,"A+",IF(T12&gt;=4,"A",IF(T12&gt;=3.5,"A-",IF(T12&gt;=3,"B",IF(T12&gt;=2,"C",IF(T12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1515,52 +1671,64 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>177</v>
+        <v>61</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>156</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>165</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="I13" s="3" t="n">
-        <v>74</v>
-      </c>
-      <c r="J13" s="3" t="n">
-        <v>78</v>
-      </c>
-      <c r="K13" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="P13" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="L13" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="N13">
-        <f>SUM(C13:J13)</f>
-        <v/>
-      </c>
-      <c r="O13" s="4">
-        <f>ROUND(N13/8,2)</f>
-        <v/>
-      </c>
-      <c r="P13" s="5">
-        <f>IF(OR(C13&lt;66,D13&lt;66,E13&lt;33,F13&lt;66,G13&lt;66,H13&lt;33,I13&lt;33,J13&lt;33,L13&lt;33,M13&lt;33),0,MIN(5,ROUND((IF(C13/200*100&gt;=80,5,IF(C13/200*100&gt;=70,4,IF(C13/200*100&gt;=60,3.5,IF(C13/200*100&gt;=50,3,IF(C13/200*100&gt;=40,2,IF(C13/200*100&gt;=33,1,0))))))+IF(D13/200*100&gt;=80,5,IF(D13/200*100&gt;=70,4,IF(D13/200*100&gt;=60,3.5,IF(D13/200*100&gt;=50,3,IF(D13/200*100&gt;=40,2,IF(D13/200*100&gt;=33,1,0))))))+IF(E13&gt;=80,5,IF(E13&gt;=70,4,IF(E13&gt;=60,3.5,IF(E13&gt;=50,3,IF(E13&gt;=40,2,IF(E13&gt;=33,1,0))))))+IF(F13/200*100&gt;=80,5,IF(F13/200*100&gt;=70,4,IF(F13/200*100&gt;=60,3.5,IF(F13/200*100&gt;=50,3,IF(F13/200*100&gt;=40,2,IF(F13/200*100&gt;=33,1,0))))))+IF(G13/200*100&gt;=80,5,IF(G13/200*100&gt;=70,4,IF(G13/200*100&gt;=60,3.5,IF(G13/200*100&gt;=50,3,IF(G13/200*100&gt;=40,2,IF(G13/200*100&gt;=33,1,0))))))+IF(H13&gt;=80,5,IF(H13&gt;=70,4,IF(H13&gt;=60,3.5,IF(H13&gt;=50,3,IF(H13&gt;=40,2,IF(H13&gt;=33,1,0))))))+IF(I13&gt;=80,5,IF(I13&gt;=70,4,IF(I13&gt;=60,3.5,IF(I13&gt;=50,3,IF(I13&gt;=40,2,IF(I13&gt;=33,1,0))))))+IF(J13&gt;=80,5,IF(J13&gt;=70,4,IF(J13&gt;=60,3.5,IF(J13&gt;=50,3,IF(J13&gt;=40,2,IF(J13&gt;=33,1,0)))))))/8+IF(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))&gt;=2,(IF(K13&gt;=80,5,IF(K13&gt;=70,4,IF(K13&gt;=60,3.5,IF(K13&gt;=50,3,IF(K13&gt;=40,2,IF(K13&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="6">
-        <f>IF(P13&gt;=5,"A+",IF(P13&gt;=4,"A",IF(P13&gt;=3.5,"A-",IF(P13&gt;=3,"B",IF(P13&gt;=2,"C",IF(P13&gt;=1,"D","F"))))))</f>
+      <c r="Q13" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="R13">
+        <f>SUM(C13:N13)</f>
+        <v/>
+      </c>
+      <c r="S13" s="4">
+        <f>ROUND(R13/12,2)</f>
+        <v/>
+      </c>
+      <c r="T13" s="5">
+        <f>IF(OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,(J13+K13)&lt;66,L13&lt;33,M13&lt;33,N13&lt;33,P13&lt;33,Q13&lt;33),0,MIN(5,ROUND((IF((C13+D13)/200*100&gt;=80,5,IF((C13+D13)/200*100&gt;=70,4,IF((C13+D13)/200*100&gt;=60,3.5,IF((C13+D13)/200*100&gt;=50,3,IF((C13+D13)/200*100&gt;=40,2,IF((C13+D13)/200*100&gt;=33,1,0))))))+IF((E13+F13)/200*100&gt;=80,5,IF((E13+F13)/200*100&gt;=70,4,IF((E13+F13)/200*100&gt;=60,3.5,IF((E13+F13)/200*100&gt;=50,3,IF((E13+F13)/200*100&gt;=40,2,IF((E13+F13)/200*100&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF((H13+I13)/200*100&gt;=80,5,IF((H13+I13)/200*100&gt;=70,4,IF((H13+I13)/200*100&gt;=60,3.5,IF((H13+I13)/200*100&gt;=50,3,IF((H13+I13)/200*100&gt;=40,2,IF((H13+I13)/200*100&gt;=33,1,0))))))+IF((J13+K13)/200*100&gt;=80,5,IF((J13+K13)/200*100&gt;=70,4,IF((J13+K13)/200*100&gt;=60,3.5,IF((J13+K13)/200*100&gt;=50,3,IF((J13+K13)/200*100&gt;=40,2,IF((J13+K13)/200*100&gt;=33,1,0))))))+IF(L13&gt;=80,5,IF(L13&gt;=70,4,IF(L13&gt;=60,3.5,IF(L13&gt;=50,3,IF(L13&gt;=40,2,IF(L13&gt;=33,1,0))))))+IF(M13&gt;=80,5,IF(M13&gt;=70,4,IF(M13&gt;=60,3.5,IF(M13&gt;=50,3,IF(M13&gt;=40,2,IF(M13&gt;=33,1,0))))))+IF(N13&gt;=80,5,IF(N13&gt;=70,4,IF(N13&gt;=60,3.5,IF(N13&gt;=50,3,IF(N13&gt;=40,2,IF(N13&gt;=33,1,0)))))))/8+IF(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))&gt;=2,(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U13" s="6">
+        <f>IF(T13&gt;=5,"A+",IF(T13&gt;=4,"A",IF(T13&gt;=3.5,"A-",IF(T13&gt;=3,"B",IF(T13&gt;=2,"C",IF(T13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1574,52 +1742,64 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>187</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>144</v>
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="H14" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>178</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>176</v>
-      </c>
-      <c r="H14" s="3" t="n">
-        <v>78</v>
-      </c>
-      <c r="I14" s="3" t="n">
-        <v>76</v>
+      <c r="I14" s="2" t="n">
+        <v>62</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L14" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="N14" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="M14" s="2" t="n">
-        <v>86</v>
-      </c>
-      <c r="N14">
-        <f>SUM(C14:J14)</f>
-        <v/>
-      </c>
-      <c r="O14" s="4">
-        <f>ROUND(N14/8,2)</f>
-        <v/>
-      </c>
-      <c r="P14" s="5">
-        <f>IF(OR(C14&lt;66,D14&lt;66,E14&lt;33,F14&lt;66,G14&lt;66,H14&lt;33,I14&lt;33,J14&lt;33,L14&lt;33,M14&lt;33),0,MIN(5,ROUND((IF(C14/200*100&gt;=80,5,IF(C14/200*100&gt;=70,4,IF(C14/200*100&gt;=60,3.5,IF(C14/200*100&gt;=50,3,IF(C14/200*100&gt;=40,2,IF(C14/200*100&gt;=33,1,0))))))+IF(D14/200*100&gt;=80,5,IF(D14/200*100&gt;=70,4,IF(D14/200*100&gt;=60,3.5,IF(D14/200*100&gt;=50,3,IF(D14/200*100&gt;=40,2,IF(D14/200*100&gt;=33,1,0))))))+IF(E14&gt;=80,5,IF(E14&gt;=70,4,IF(E14&gt;=60,3.5,IF(E14&gt;=50,3,IF(E14&gt;=40,2,IF(E14&gt;=33,1,0))))))+IF(F14/200*100&gt;=80,5,IF(F14/200*100&gt;=70,4,IF(F14/200*100&gt;=60,3.5,IF(F14/200*100&gt;=50,3,IF(F14/200*100&gt;=40,2,IF(F14/200*100&gt;=33,1,0))))))+IF(G14/200*100&gt;=80,5,IF(G14/200*100&gt;=70,4,IF(G14/200*100&gt;=60,3.5,IF(G14/200*100&gt;=50,3,IF(G14/200*100&gt;=40,2,IF(G14/200*100&gt;=33,1,0))))))+IF(H14&gt;=80,5,IF(H14&gt;=70,4,IF(H14&gt;=60,3.5,IF(H14&gt;=50,3,IF(H14&gt;=40,2,IF(H14&gt;=33,1,0))))))+IF(I14&gt;=80,5,IF(I14&gt;=70,4,IF(I14&gt;=60,3.5,IF(I14&gt;=50,3,IF(I14&gt;=40,2,IF(I14&gt;=33,1,0))))))+IF(J14&gt;=80,5,IF(J14&gt;=70,4,IF(J14&gt;=60,3.5,IF(J14&gt;=50,3,IF(J14&gt;=40,2,IF(J14&gt;=33,1,0)))))))/8+IF(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))&gt;=2,(IF(K14&gt;=80,5,IF(K14&gt;=70,4,IF(K14&gt;=60,3.5,IF(K14&gt;=50,3,IF(K14&gt;=40,2,IF(K14&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="6">
-        <f>IF(P14&gt;=5,"A+",IF(P14&gt;=4,"A",IF(P14&gt;=3.5,"A-",IF(P14&gt;=3,"B",IF(P14&gt;=2,"C",IF(P14&gt;=1,"D","F"))))))</f>
+      <c r="O14" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="R14">
+        <f>SUM(C14:N14)</f>
+        <v/>
+      </c>
+      <c r="S14" s="4">
+        <f>ROUND(R14/12,2)</f>
+        <v/>
+      </c>
+      <c r="T14" s="5">
+        <f>IF(OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,(J14+K14)&lt;66,L14&lt;33,M14&lt;33,N14&lt;33,P14&lt;33,Q14&lt;33),0,MIN(5,ROUND((IF((C14+D14)/200*100&gt;=80,5,IF((C14+D14)/200*100&gt;=70,4,IF((C14+D14)/200*100&gt;=60,3.5,IF((C14+D14)/200*100&gt;=50,3,IF((C14+D14)/200*100&gt;=40,2,IF((C14+D14)/200*100&gt;=33,1,0))))))+IF((E14+F14)/200*100&gt;=80,5,IF((E14+F14)/200*100&gt;=70,4,IF((E14+F14)/200*100&gt;=60,3.5,IF((E14+F14)/200*100&gt;=50,3,IF((E14+F14)/200*100&gt;=40,2,IF((E14+F14)/200*100&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF((H14+I14)/200*100&gt;=80,5,IF((H14+I14)/200*100&gt;=70,4,IF((H14+I14)/200*100&gt;=60,3.5,IF((H14+I14)/200*100&gt;=50,3,IF((H14+I14)/200*100&gt;=40,2,IF((H14+I14)/200*100&gt;=33,1,0))))))+IF((J14+K14)/200*100&gt;=80,5,IF((J14+K14)/200*100&gt;=70,4,IF((J14+K14)/200*100&gt;=60,3.5,IF((J14+K14)/200*100&gt;=50,3,IF((J14+K14)/200*100&gt;=40,2,IF((J14+K14)/200*100&gt;=33,1,0))))))+IF(L14&gt;=80,5,IF(L14&gt;=70,4,IF(L14&gt;=60,3.5,IF(L14&gt;=50,3,IF(L14&gt;=40,2,IF(L14&gt;=33,1,0))))))+IF(M14&gt;=80,5,IF(M14&gt;=70,4,IF(M14&gt;=60,3.5,IF(M14&gt;=50,3,IF(M14&gt;=40,2,IF(M14&gt;=33,1,0))))))+IF(N14&gt;=80,5,IF(N14&gt;=70,4,IF(N14&gt;=60,3.5,IF(N14&gt;=50,3,IF(N14&gt;=40,2,IF(N14&gt;=33,1,0)))))))/8+IF(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))&gt;=2,(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U14" s="6">
+        <f>IF(T14&gt;=5,"A+",IF(T14&gt;=4,"A",IF(T14&gt;=3.5,"A-",IF(T14&gt;=3,"B",IF(T14&gt;=2,"C",IF(T14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1633,52 +1813,64 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>164</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>158</v>
+        <v>73</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>75</v>
       </c>
       <c r="E15" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="M15" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="O15" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="P15" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>166</v>
-      </c>
-      <c r="G15" s="3" t="n">
-        <v>159</v>
-      </c>
-      <c r="H15" s="3" t="n">
-        <v>69</v>
-      </c>
-      <c r="I15" s="3" t="n">
-        <v>68</v>
-      </c>
-      <c r="J15" s="3" t="n">
-        <v>79</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>84</v>
-      </c>
-      <c r="L15" s="2" t="n">
-        <v>94</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="N15">
-        <f>SUM(C15:J15)</f>
-        <v/>
-      </c>
-      <c r="O15" s="4">
-        <f>ROUND(N15/8,2)</f>
-        <v/>
-      </c>
-      <c r="P15" s="5">
-        <f>IF(OR(C15&lt;66,D15&lt;66,E15&lt;33,F15&lt;66,G15&lt;66,H15&lt;33,I15&lt;33,J15&lt;33,L15&lt;33,M15&lt;33),0,MIN(5,ROUND((IF(C15/200*100&gt;=80,5,IF(C15/200*100&gt;=70,4,IF(C15/200*100&gt;=60,3.5,IF(C15/200*100&gt;=50,3,IF(C15/200*100&gt;=40,2,IF(C15/200*100&gt;=33,1,0))))))+IF(D15/200*100&gt;=80,5,IF(D15/200*100&gt;=70,4,IF(D15/200*100&gt;=60,3.5,IF(D15/200*100&gt;=50,3,IF(D15/200*100&gt;=40,2,IF(D15/200*100&gt;=33,1,0))))))+IF(E15&gt;=80,5,IF(E15&gt;=70,4,IF(E15&gt;=60,3.5,IF(E15&gt;=50,3,IF(E15&gt;=40,2,IF(E15&gt;=33,1,0))))))+IF(F15/200*100&gt;=80,5,IF(F15/200*100&gt;=70,4,IF(F15/200*100&gt;=60,3.5,IF(F15/200*100&gt;=50,3,IF(F15/200*100&gt;=40,2,IF(F15/200*100&gt;=33,1,0))))))+IF(G15/200*100&gt;=80,5,IF(G15/200*100&gt;=70,4,IF(G15/200*100&gt;=60,3.5,IF(G15/200*100&gt;=50,3,IF(G15/200*100&gt;=40,2,IF(G15/200*100&gt;=33,1,0))))))+IF(H15&gt;=80,5,IF(H15&gt;=70,4,IF(H15&gt;=60,3.5,IF(H15&gt;=50,3,IF(H15&gt;=40,2,IF(H15&gt;=33,1,0))))))+IF(I15&gt;=80,5,IF(I15&gt;=70,4,IF(I15&gt;=60,3.5,IF(I15&gt;=50,3,IF(I15&gt;=40,2,IF(I15&gt;=33,1,0))))))+IF(J15&gt;=80,5,IF(J15&gt;=70,4,IF(J15&gt;=60,3.5,IF(J15&gt;=50,3,IF(J15&gt;=40,2,IF(J15&gt;=33,1,0)))))))/8+IF(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))&gt;=2,(IF(K15&gt;=80,5,IF(K15&gt;=70,4,IF(K15&gt;=60,3.5,IF(K15&gt;=50,3,IF(K15&gt;=40,2,IF(K15&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="6">
-        <f>IF(P15&gt;=5,"A+",IF(P15&gt;=4,"A",IF(P15&gt;=3.5,"A-",IF(P15&gt;=3,"B",IF(P15&gt;=2,"C",IF(P15&gt;=1,"D","F"))))))</f>
+      <c r="Q15" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="R15">
+        <f>SUM(C15:N15)</f>
+        <v/>
+      </c>
+      <c r="S15" s="4">
+        <f>ROUND(R15/12,2)</f>
+        <v/>
+      </c>
+      <c r="T15" s="5">
+        <f>IF(OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,(J15+K15)&lt;66,L15&lt;33,M15&lt;33,N15&lt;33,P15&lt;33,Q15&lt;33),0,MIN(5,ROUND((IF((C15+D15)/200*100&gt;=80,5,IF((C15+D15)/200*100&gt;=70,4,IF((C15+D15)/200*100&gt;=60,3.5,IF((C15+D15)/200*100&gt;=50,3,IF((C15+D15)/200*100&gt;=40,2,IF((C15+D15)/200*100&gt;=33,1,0))))))+IF((E15+F15)/200*100&gt;=80,5,IF((E15+F15)/200*100&gt;=70,4,IF((E15+F15)/200*100&gt;=60,3.5,IF((E15+F15)/200*100&gt;=50,3,IF((E15+F15)/200*100&gt;=40,2,IF((E15+F15)/200*100&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF((H15+I15)/200*100&gt;=80,5,IF((H15+I15)/200*100&gt;=70,4,IF((H15+I15)/200*100&gt;=60,3.5,IF((H15+I15)/200*100&gt;=50,3,IF((H15+I15)/200*100&gt;=40,2,IF((H15+I15)/200*100&gt;=33,1,0))))))+IF((J15+K15)/200*100&gt;=80,5,IF((J15+K15)/200*100&gt;=70,4,IF((J15+K15)/200*100&gt;=60,3.5,IF((J15+K15)/200*100&gt;=50,3,IF((J15+K15)/200*100&gt;=40,2,IF((J15+K15)/200*100&gt;=33,1,0))))))+IF(L15&gt;=80,5,IF(L15&gt;=70,4,IF(L15&gt;=60,3.5,IF(L15&gt;=50,3,IF(L15&gt;=40,2,IF(L15&gt;=33,1,0))))))+IF(M15&gt;=80,5,IF(M15&gt;=70,4,IF(M15&gt;=60,3.5,IF(M15&gt;=50,3,IF(M15&gt;=40,2,IF(M15&gt;=33,1,0))))))+IF(N15&gt;=80,5,IF(N15&gt;=70,4,IF(N15&gt;=60,3.5,IF(N15&gt;=50,3,IF(N15&gt;=40,2,IF(N15&gt;=33,1,0)))))))/8+IF(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))&gt;=2,(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U15" s="6">
+        <f>IF(T15&gt;=5,"A+",IF(T15&gt;=4,"A",IF(T15&gt;=3.5,"A-",IF(T15&gt;=3,"B",IF(T15&gt;=2,"C",IF(T15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1691,53 +1883,65 @@
           <t>Imran Khan</t>
         </is>
       </c>
-      <c r="C16" s="3" t="n">
-        <v>135</v>
+      <c r="C16" s="2" t="n">
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>167</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>62</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>140</v>
+        <v>73</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>76</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>63</v>
-      </c>
-      <c r="I16" s="3" t="n">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>72</v>
       </c>
       <c r="J16" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="L16" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>83</v>
-      </c>
-      <c r="L16" s="2" t="n">
-        <v>87</v>
-      </c>
       <c r="M16" s="2" t="n">
-        <v>91</v>
-      </c>
-      <c r="N16">
-        <f>SUM(C16:J16)</f>
-        <v/>
-      </c>
-      <c r="O16" s="4">
-        <f>ROUND(N16/8,2)</f>
-        <v/>
-      </c>
-      <c r="P16" s="5">
-        <f>IF(OR(C16&lt;66,D16&lt;66,E16&lt;33,F16&lt;66,G16&lt;66,H16&lt;33,I16&lt;33,J16&lt;33,L16&lt;33,M16&lt;33),0,MIN(5,ROUND((IF(C16/200*100&gt;=80,5,IF(C16/200*100&gt;=70,4,IF(C16/200*100&gt;=60,3.5,IF(C16/200*100&gt;=50,3,IF(C16/200*100&gt;=40,2,IF(C16/200*100&gt;=33,1,0))))))+IF(D16/200*100&gt;=80,5,IF(D16/200*100&gt;=70,4,IF(D16/200*100&gt;=60,3.5,IF(D16/200*100&gt;=50,3,IF(D16/200*100&gt;=40,2,IF(D16/200*100&gt;=33,1,0))))))+IF(E16&gt;=80,5,IF(E16&gt;=70,4,IF(E16&gt;=60,3.5,IF(E16&gt;=50,3,IF(E16&gt;=40,2,IF(E16&gt;=33,1,0))))))+IF(F16/200*100&gt;=80,5,IF(F16/200*100&gt;=70,4,IF(F16/200*100&gt;=60,3.5,IF(F16/200*100&gt;=50,3,IF(F16/200*100&gt;=40,2,IF(F16/200*100&gt;=33,1,0))))))+IF(G16/200*100&gt;=80,5,IF(G16/200*100&gt;=70,4,IF(G16/200*100&gt;=60,3.5,IF(G16/200*100&gt;=50,3,IF(G16/200*100&gt;=40,2,IF(G16/200*100&gt;=33,1,0))))))+IF(H16&gt;=80,5,IF(H16&gt;=70,4,IF(H16&gt;=60,3.5,IF(H16&gt;=50,3,IF(H16&gt;=40,2,IF(H16&gt;=33,1,0))))))+IF(I16&gt;=80,5,IF(I16&gt;=70,4,IF(I16&gt;=60,3.5,IF(I16&gt;=50,3,IF(I16&gt;=40,2,IF(I16&gt;=33,1,0))))))+IF(J16&gt;=80,5,IF(J16&gt;=70,4,IF(J16&gt;=60,3.5,IF(J16&gt;=50,3,IF(J16&gt;=40,2,IF(J16&gt;=33,1,0)))))))/8+IF(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))&gt;=2,(IF(K16&gt;=80,5,IF(K16&gt;=70,4,IF(K16&gt;=60,3.5,IF(K16&gt;=50,3,IF(K16&gt;=40,2,IF(K16&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="6">
-        <f>IF(P16&gt;=5,"A+",IF(P16&gt;=4,"A",IF(P16&gt;=3.5,"A-",IF(P16&gt;=3,"B",IF(P16&gt;=2,"C",IF(P16&gt;=1,"D","F"))))))</f>
+        <v>76</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="O16" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="Q16" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="R16">
+        <f>SUM(C16:N16)</f>
+        <v/>
+      </c>
+      <c r="S16" s="4">
+        <f>ROUND(R16/12,2)</f>
+        <v/>
+      </c>
+      <c r="T16" s="5">
+        <f>IF(OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,(J16+K16)&lt;66,L16&lt;33,M16&lt;33,N16&lt;33,P16&lt;33,Q16&lt;33),0,MIN(5,ROUND((IF((C16+D16)/200*100&gt;=80,5,IF((C16+D16)/200*100&gt;=70,4,IF((C16+D16)/200*100&gt;=60,3.5,IF((C16+D16)/200*100&gt;=50,3,IF((C16+D16)/200*100&gt;=40,2,IF((C16+D16)/200*100&gt;=33,1,0))))))+IF((E16+F16)/200*100&gt;=80,5,IF((E16+F16)/200*100&gt;=70,4,IF((E16+F16)/200*100&gt;=60,3.5,IF((E16+F16)/200*100&gt;=50,3,IF((E16+F16)/200*100&gt;=40,2,IF((E16+F16)/200*100&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF((H16+I16)/200*100&gt;=80,5,IF((H16+I16)/200*100&gt;=70,4,IF((H16+I16)/200*100&gt;=60,3.5,IF((H16+I16)/200*100&gt;=50,3,IF((H16+I16)/200*100&gt;=40,2,IF((H16+I16)/200*100&gt;=33,1,0))))))+IF((J16+K16)/200*100&gt;=80,5,IF((J16+K16)/200*100&gt;=70,4,IF((J16+K16)/200*100&gt;=60,3.5,IF((J16+K16)/200*100&gt;=50,3,IF((J16+K16)/200*100&gt;=40,2,IF((J16+K16)/200*100&gt;=33,1,0))))))+IF(L16&gt;=80,5,IF(L16&gt;=70,4,IF(L16&gt;=60,3.5,IF(L16&gt;=50,3,IF(L16&gt;=40,2,IF(L16&gt;=33,1,0))))))+IF(M16&gt;=80,5,IF(M16&gt;=70,4,IF(M16&gt;=60,3.5,IF(M16&gt;=50,3,IF(M16&gt;=40,2,IF(M16&gt;=33,1,0))))))+IF(N16&gt;=80,5,IF(N16&gt;=70,4,IF(N16&gt;=60,3.5,IF(N16&gt;=50,3,IF(N16&gt;=40,2,IF(N16&gt;=33,1,0)))))))/8+IF(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))&gt;=2,(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U16" s="6">
+        <f>IF(T16&gt;=5,"A+",IF(T16&gt;=4,"A",IF(T16&gt;=3.5,"A-",IF(T16&gt;=3,"B",IF(T16&gt;=2,"C",IF(T16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1750,53 +1954,65 @@
           <t>Rafia Islam</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>167</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>147</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>89</v>
+      <c r="C17" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>83</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>167</v>
+        <v>76</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="P17" s="3" t="n">
         <v>87</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <v>87</v>
-      </c>
-      <c r="J17" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="K17" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="L17" s="2" t="n">
-        <v>94</v>
-      </c>
-      <c r="M17" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="N17">
-        <f>SUM(C17:J17)</f>
-        <v/>
-      </c>
-      <c r="O17" s="4">
-        <f>ROUND(N17/8,2)</f>
-        <v/>
-      </c>
-      <c r="P17" s="5">
-        <f>IF(OR(C17&lt;66,D17&lt;66,E17&lt;33,F17&lt;66,G17&lt;66,H17&lt;33,I17&lt;33,J17&lt;33,L17&lt;33,M17&lt;33),0,MIN(5,ROUND((IF(C17/200*100&gt;=80,5,IF(C17/200*100&gt;=70,4,IF(C17/200*100&gt;=60,3.5,IF(C17/200*100&gt;=50,3,IF(C17/200*100&gt;=40,2,IF(C17/200*100&gt;=33,1,0))))))+IF(D17/200*100&gt;=80,5,IF(D17/200*100&gt;=70,4,IF(D17/200*100&gt;=60,3.5,IF(D17/200*100&gt;=50,3,IF(D17/200*100&gt;=40,2,IF(D17/200*100&gt;=33,1,0))))))+IF(E17&gt;=80,5,IF(E17&gt;=70,4,IF(E17&gt;=60,3.5,IF(E17&gt;=50,3,IF(E17&gt;=40,2,IF(E17&gt;=33,1,0))))))+IF(F17/200*100&gt;=80,5,IF(F17/200*100&gt;=70,4,IF(F17/200*100&gt;=60,3.5,IF(F17/200*100&gt;=50,3,IF(F17/200*100&gt;=40,2,IF(F17/200*100&gt;=33,1,0))))))+IF(G17/200*100&gt;=80,5,IF(G17/200*100&gt;=70,4,IF(G17/200*100&gt;=60,3.5,IF(G17/200*100&gt;=50,3,IF(G17/200*100&gt;=40,2,IF(G17/200*100&gt;=33,1,0))))))+IF(H17&gt;=80,5,IF(H17&gt;=70,4,IF(H17&gt;=60,3.5,IF(H17&gt;=50,3,IF(H17&gt;=40,2,IF(H17&gt;=33,1,0))))))+IF(I17&gt;=80,5,IF(I17&gt;=70,4,IF(I17&gt;=60,3.5,IF(I17&gt;=50,3,IF(I17&gt;=40,2,IF(I17&gt;=33,1,0))))))+IF(J17&gt;=80,5,IF(J17&gt;=70,4,IF(J17&gt;=60,3.5,IF(J17&gt;=50,3,IF(J17&gt;=40,2,IF(J17&gt;=33,1,0)))))))/8+IF(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))&gt;=2,(IF(K17&gt;=80,5,IF(K17&gt;=70,4,IF(K17&gt;=60,3.5,IF(K17&gt;=50,3,IF(K17&gt;=40,2,IF(K17&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="6">
-        <f>IF(P17&gt;=5,"A+",IF(P17&gt;=4,"A",IF(P17&gt;=3.5,"A-",IF(P17&gt;=3,"B",IF(P17&gt;=2,"C",IF(P17&gt;=1,"D","F"))))))</f>
+      <c r="Q17" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="R17">
+        <f>SUM(C17:N17)</f>
+        <v/>
+      </c>
+      <c r="S17" s="4">
+        <f>ROUND(R17/12,2)</f>
+        <v/>
+      </c>
+      <c r="T17" s="5">
+        <f>IF(OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,(J17+K17)&lt;66,L17&lt;33,M17&lt;33,N17&lt;33,P17&lt;33,Q17&lt;33),0,MIN(5,ROUND((IF((C17+D17)/200*100&gt;=80,5,IF((C17+D17)/200*100&gt;=70,4,IF((C17+D17)/200*100&gt;=60,3.5,IF((C17+D17)/200*100&gt;=50,3,IF((C17+D17)/200*100&gt;=40,2,IF((C17+D17)/200*100&gt;=33,1,0))))))+IF((E17+F17)/200*100&gt;=80,5,IF((E17+F17)/200*100&gt;=70,4,IF((E17+F17)/200*100&gt;=60,3.5,IF((E17+F17)/200*100&gt;=50,3,IF((E17+F17)/200*100&gt;=40,2,IF((E17+F17)/200*100&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF((H17+I17)/200*100&gt;=80,5,IF((H17+I17)/200*100&gt;=70,4,IF((H17+I17)/200*100&gt;=60,3.5,IF((H17+I17)/200*100&gt;=50,3,IF((H17+I17)/200*100&gt;=40,2,IF((H17+I17)/200*100&gt;=33,1,0))))))+IF((J17+K17)/200*100&gt;=80,5,IF((J17+K17)/200*100&gt;=70,4,IF((J17+K17)/200*100&gt;=60,3.5,IF((J17+K17)/200*100&gt;=50,3,IF((J17+K17)/200*100&gt;=40,2,IF((J17+K17)/200*100&gt;=33,1,0))))))+IF(L17&gt;=80,5,IF(L17&gt;=70,4,IF(L17&gt;=60,3.5,IF(L17&gt;=50,3,IF(L17&gt;=40,2,IF(L17&gt;=33,1,0))))))+IF(M17&gt;=80,5,IF(M17&gt;=70,4,IF(M17&gt;=60,3.5,IF(M17&gt;=50,3,IF(M17&gt;=40,2,IF(M17&gt;=33,1,0))))))+IF(N17&gt;=80,5,IF(N17&gt;=70,4,IF(N17&gt;=60,3.5,IF(N17&gt;=50,3,IF(N17&gt;=40,2,IF(N17&gt;=33,1,0)))))))/8+IF(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))&gt;=2,(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U17" s="6">
+        <f>IF(T17&gt;=5,"A+",IF(T17&gt;=4,"A",IF(T17&gt;=3.5,"A-",IF(T17&gt;=3,"B",IF(T17&gt;=2,"C",IF(T17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1809,53 +2025,65 @@
           <t>Shakib Rahman</t>
         </is>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>157</v>
+      <c r="C18" s="2" t="n">
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>181</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="I18" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="Q18" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="J18" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="L18" s="3" t="n">
-        <v>74</v>
-      </c>
-      <c r="M18" s="3" t="n">
-        <v>78</v>
-      </c>
-      <c r="N18">
-        <f>SUM(C18:J18)</f>
-        <v/>
-      </c>
-      <c r="O18" s="4">
-        <f>ROUND(N18/8,2)</f>
-        <v/>
-      </c>
-      <c r="P18" s="5">
-        <f>IF(OR(C18&lt;66,D18&lt;66,E18&lt;33,F18&lt;66,G18&lt;66,H18&lt;33,I18&lt;33,J18&lt;33,L18&lt;33,M18&lt;33),0,MIN(5,ROUND((IF(C18/200*100&gt;=80,5,IF(C18/200*100&gt;=70,4,IF(C18/200*100&gt;=60,3.5,IF(C18/200*100&gt;=50,3,IF(C18/200*100&gt;=40,2,IF(C18/200*100&gt;=33,1,0))))))+IF(D18/200*100&gt;=80,5,IF(D18/200*100&gt;=70,4,IF(D18/200*100&gt;=60,3.5,IF(D18/200*100&gt;=50,3,IF(D18/200*100&gt;=40,2,IF(D18/200*100&gt;=33,1,0))))))+IF(E18&gt;=80,5,IF(E18&gt;=70,4,IF(E18&gt;=60,3.5,IF(E18&gt;=50,3,IF(E18&gt;=40,2,IF(E18&gt;=33,1,0))))))+IF(F18/200*100&gt;=80,5,IF(F18/200*100&gt;=70,4,IF(F18/200*100&gt;=60,3.5,IF(F18/200*100&gt;=50,3,IF(F18/200*100&gt;=40,2,IF(F18/200*100&gt;=33,1,0))))))+IF(G18/200*100&gt;=80,5,IF(G18/200*100&gt;=70,4,IF(G18/200*100&gt;=60,3.5,IF(G18/200*100&gt;=50,3,IF(G18/200*100&gt;=40,2,IF(G18/200*100&gt;=33,1,0))))))+IF(H18&gt;=80,5,IF(H18&gt;=70,4,IF(H18&gt;=60,3.5,IF(H18&gt;=50,3,IF(H18&gt;=40,2,IF(H18&gt;=33,1,0))))))+IF(I18&gt;=80,5,IF(I18&gt;=70,4,IF(I18&gt;=60,3.5,IF(I18&gt;=50,3,IF(I18&gt;=40,2,IF(I18&gt;=33,1,0))))))+IF(J18&gt;=80,5,IF(J18&gt;=70,4,IF(J18&gt;=60,3.5,IF(J18&gt;=50,3,IF(J18&gt;=40,2,IF(J18&gt;=33,1,0)))))))/8+IF(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))&gt;=2,(IF(K18&gt;=80,5,IF(K18&gt;=70,4,IF(K18&gt;=60,3.5,IF(K18&gt;=50,3,IF(K18&gt;=40,2,IF(K18&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="6">
-        <f>IF(P18&gt;=5,"A+",IF(P18&gt;=4,"A",IF(P18&gt;=3.5,"A-",IF(P18&gt;=3,"B",IF(P18&gt;=2,"C",IF(P18&gt;=1,"D","F"))))))</f>
+      <c r="R18">
+        <f>SUM(C18:N18)</f>
+        <v/>
+      </c>
+      <c r="S18" s="4">
+        <f>ROUND(R18/12,2)</f>
+        <v/>
+      </c>
+      <c r="T18" s="5">
+        <f>IF(OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,(J18+K18)&lt;66,L18&lt;33,M18&lt;33,N18&lt;33,P18&lt;33,Q18&lt;33),0,MIN(5,ROUND((IF((C18+D18)/200*100&gt;=80,5,IF((C18+D18)/200*100&gt;=70,4,IF((C18+D18)/200*100&gt;=60,3.5,IF((C18+D18)/200*100&gt;=50,3,IF((C18+D18)/200*100&gt;=40,2,IF((C18+D18)/200*100&gt;=33,1,0))))))+IF((E18+F18)/200*100&gt;=80,5,IF((E18+F18)/200*100&gt;=70,4,IF((E18+F18)/200*100&gt;=60,3.5,IF((E18+F18)/200*100&gt;=50,3,IF((E18+F18)/200*100&gt;=40,2,IF((E18+F18)/200*100&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF((H18+I18)/200*100&gt;=80,5,IF((H18+I18)/200*100&gt;=70,4,IF((H18+I18)/200*100&gt;=60,3.5,IF((H18+I18)/200*100&gt;=50,3,IF((H18+I18)/200*100&gt;=40,2,IF((H18+I18)/200*100&gt;=33,1,0))))))+IF((J18+K18)/200*100&gt;=80,5,IF((J18+K18)/200*100&gt;=70,4,IF((J18+K18)/200*100&gt;=60,3.5,IF((J18+K18)/200*100&gt;=50,3,IF((J18+K18)/200*100&gt;=40,2,IF((J18+K18)/200*100&gt;=33,1,0))))))+IF(L18&gt;=80,5,IF(L18&gt;=70,4,IF(L18&gt;=60,3.5,IF(L18&gt;=50,3,IF(L18&gt;=40,2,IF(L18&gt;=33,1,0))))))+IF(M18&gt;=80,5,IF(M18&gt;=70,4,IF(M18&gt;=60,3.5,IF(M18&gt;=50,3,IF(M18&gt;=40,2,IF(M18&gt;=33,1,0))))))+IF(N18&gt;=80,5,IF(N18&gt;=70,4,IF(N18&gt;=60,3.5,IF(N18&gt;=50,3,IF(N18&gt;=40,2,IF(N18&gt;=33,1,0)))))))/8+IF(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))&gt;=2,(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U18" s="6">
+        <f>IF(T18&gt;=5,"A+",IF(T18&gt;=4,"A",IF(T18&gt;=3.5,"A-",IF(T18&gt;=3,"B",IF(T18&gt;=2,"C",IF(T18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1869,52 +2097,64 @@
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>132</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>185</v>
-      </c>
-      <c r="E19" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="M19" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="F19" s="3" t="n">
-        <v>146</v>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>152</v>
-      </c>
-      <c r="H19" s="3" t="n">
-        <v>60</v>
-      </c>
-      <c r="I19" s="3" t="n">
-        <v>60</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="L19" s="3" t="n">
+      <c r="N19" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="P19" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="M19" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="N19">
-        <f>SUM(C19:J19)</f>
-        <v/>
-      </c>
-      <c r="O19" s="4">
-        <f>ROUND(N19/8,2)</f>
-        <v/>
-      </c>
-      <c r="P19" s="5">
-        <f>IF(OR(C19&lt;66,D19&lt;66,E19&lt;33,F19&lt;66,G19&lt;66,H19&lt;33,I19&lt;33,J19&lt;33,L19&lt;33,M19&lt;33),0,MIN(5,ROUND((IF(C19/200*100&gt;=80,5,IF(C19/200*100&gt;=70,4,IF(C19/200*100&gt;=60,3.5,IF(C19/200*100&gt;=50,3,IF(C19/200*100&gt;=40,2,IF(C19/200*100&gt;=33,1,0))))))+IF(D19/200*100&gt;=80,5,IF(D19/200*100&gt;=70,4,IF(D19/200*100&gt;=60,3.5,IF(D19/200*100&gt;=50,3,IF(D19/200*100&gt;=40,2,IF(D19/200*100&gt;=33,1,0))))))+IF(E19&gt;=80,5,IF(E19&gt;=70,4,IF(E19&gt;=60,3.5,IF(E19&gt;=50,3,IF(E19&gt;=40,2,IF(E19&gt;=33,1,0))))))+IF(F19/200*100&gt;=80,5,IF(F19/200*100&gt;=70,4,IF(F19/200*100&gt;=60,3.5,IF(F19/200*100&gt;=50,3,IF(F19/200*100&gt;=40,2,IF(F19/200*100&gt;=33,1,0))))))+IF(G19/200*100&gt;=80,5,IF(G19/200*100&gt;=70,4,IF(G19/200*100&gt;=60,3.5,IF(G19/200*100&gt;=50,3,IF(G19/200*100&gt;=40,2,IF(G19/200*100&gt;=33,1,0))))))+IF(H19&gt;=80,5,IF(H19&gt;=70,4,IF(H19&gt;=60,3.5,IF(H19&gt;=50,3,IF(H19&gt;=40,2,IF(H19&gt;=33,1,0))))))+IF(I19&gt;=80,5,IF(I19&gt;=70,4,IF(I19&gt;=60,3.5,IF(I19&gt;=50,3,IF(I19&gt;=40,2,IF(I19&gt;=33,1,0))))))+IF(J19&gt;=80,5,IF(J19&gt;=70,4,IF(J19&gt;=60,3.5,IF(J19&gt;=50,3,IF(J19&gt;=40,2,IF(J19&gt;=33,1,0)))))))/8+IF(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))&gt;=2,(IF(K19&gt;=80,5,IF(K19&gt;=70,4,IF(K19&gt;=60,3.5,IF(K19&gt;=50,3,IF(K19&gt;=40,2,IF(K19&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="6">
-        <f>IF(P19&gt;=5,"A+",IF(P19&gt;=4,"A",IF(P19&gt;=3.5,"A-",IF(P19&gt;=3,"B",IF(P19&gt;=2,"C",IF(P19&gt;=1,"D","F"))))))</f>
+      <c r="Q19" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="R19">
+        <f>SUM(C19:N19)</f>
+        <v/>
+      </c>
+      <c r="S19" s="4">
+        <f>ROUND(R19/12,2)</f>
+        <v/>
+      </c>
+      <c r="T19" s="5">
+        <f>IF(OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,(J19+K19)&lt;66,L19&lt;33,M19&lt;33,N19&lt;33,P19&lt;33,Q19&lt;33),0,MIN(5,ROUND((IF((C19+D19)/200*100&gt;=80,5,IF((C19+D19)/200*100&gt;=70,4,IF((C19+D19)/200*100&gt;=60,3.5,IF((C19+D19)/200*100&gt;=50,3,IF((C19+D19)/200*100&gt;=40,2,IF((C19+D19)/200*100&gt;=33,1,0))))))+IF((E19+F19)/200*100&gt;=80,5,IF((E19+F19)/200*100&gt;=70,4,IF((E19+F19)/200*100&gt;=60,3.5,IF((E19+F19)/200*100&gt;=50,3,IF((E19+F19)/200*100&gt;=40,2,IF((E19+F19)/200*100&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF((H19+I19)/200*100&gt;=80,5,IF((H19+I19)/200*100&gt;=70,4,IF((H19+I19)/200*100&gt;=60,3.5,IF((H19+I19)/200*100&gt;=50,3,IF((H19+I19)/200*100&gt;=40,2,IF((H19+I19)/200*100&gt;=33,1,0))))))+IF((J19+K19)/200*100&gt;=80,5,IF((J19+K19)/200*100&gt;=70,4,IF((J19+K19)/200*100&gt;=60,3.5,IF((J19+K19)/200*100&gt;=50,3,IF((J19+K19)/200*100&gt;=40,2,IF((J19+K19)/200*100&gt;=33,1,0))))))+IF(L19&gt;=80,5,IF(L19&gt;=70,4,IF(L19&gt;=60,3.5,IF(L19&gt;=50,3,IF(L19&gt;=40,2,IF(L19&gt;=33,1,0))))))+IF(M19&gt;=80,5,IF(M19&gt;=70,4,IF(M19&gt;=60,3.5,IF(M19&gt;=50,3,IF(M19&gt;=40,2,IF(M19&gt;=33,1,0))))))+IF(N19&gt;=80,5,IF(N19&gt;=70,4,IF(N19&gt;=60,3.5,IF(N19&gt;=50,3,IF(N19&gt;=40,2,IF(N19&gt;=33,1,0)))))))/8+IF(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))&gt;=2,(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U19" s="6">
+        <f>IF(T19&gt;=5,"A+",IF(T19&gt;=4,"A",IF(T19&gt;=3.5,"A-",IF(T19&gt;=3,"B",IF(T19&gt;=2,"C",IF(T19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1927,53 +2167,65 @@
           <t>Arif Hossain</t>
         </is>
       </c>
-      <c r="C20" s="3" t="n">
-        <v>131</v>
+      <c r="C20" s="2" t="n">
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>84</v>
-      </c>
-      <c r="F20" s="3" t="n">
-        <v>154</v>
+        <v>62</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>73</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>188</v>
-      </c>
-      <c r="H20" s="7" t="n">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>87</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="L20" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="K20" s="3" t="n">
         <v>91</v>
       </c>
+      <c r="L20" s="3" t="n">
+        <v>82</v>
+      </c>
       <c r="M20" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="N20">
-        <f>SUM(C20:J20)</f>
-        <v/>
-      </c>
-      <c r="O20" s="4">
-        <f>ROUND(N20/8,2)</f>
-        <v/>
-      </c>
-      <c r="P20" s="5">
-        <f>IF(OR(C20&lt;66,D20&lt;66,E20&lt;33,F20&lt;66,G20&lt;66,H20&lt;33,I20&lt;33,J20&lt;33,L20&lt;33,M20&lt;33),0,MIN(5,ROUND((IF(C20/200*100&gt;=80,5,IF(C20/200*100&gt;=70,4,IF(C20/200*100&gt;=60,3.5,IF(C20/200*100&gt;=50,3,IF(C20/200*100&gt;=40,2,IF(C20/200*100&gt;=33,1,0))))))+IF(D20/200*100&gt;=80,5,IF(D20/200*100&gt;=70,4,IF(D20/200*100&gt;=60,3.5,IF(D20/200*100&gt;=50,3,IF(D20/200*100&gt;=40,2,IF(D20/200*100&gt;=33,1,0))))))+IF(E20&gt;=80,5,IF(E20&gt;=70,4,IF(E20&gt;=60,3.5,IF(E20&gt;=50,3,IF(E20&gt;=40,2,IF(E20&gt;=33,1,0))))))+IF(F20/200*100&gt;=80,5,IF(F20/200*100&gt;=70,4,IF(F20/200*100&gt;=60,3.5,IF(F20/200*100&gt;=50,3,IF(F20/200*100&gt;=40,2,IF(F20/200*100&gt;=33,1,0))))))+IF(G20/200*100&gt;=80,5,IF(G20/200*100&gt;=70,4,IF(G20/200*100&gt;=60,3.5,IF(G20/200*100&gt;=50,3,IF(G20/200*100&gt;=40,2,IF(G20/200*100&gt;=33,1,0))))))+IF(H20&gt;=80,5,IF(H20&gt;=70,4,IF(H20&gt;=60,3.5,IF(H20&gt;=50,3,IF(H20&gt;=40,2,IF(H20&gt;=33,1,0))))))+IF(I20&gt;=80,5,IF(I20&gt;=70,4,IF(I20&gt;=60,3.5,IF(I20&gt;=50,3,IF(I20&gt;=40,2,IF(I20&gt;=33,1,0))))))+IF(J20&gt;=80,5,IF(J20&gt;=70,4,IF(J20&gt;=60,3.5,IF(J20&gt;=50,3,IF(J20&gt;=40,2,IF(J20&gt;=33,1,0)))))))/8+IF(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))&gt;=2,(IF(K20&gt;=80,5,IF(K20&gt;=70,4,IF(K20&gt;=60,3.5,IF(K20&gt;=50,3,IF(K20&gt;=40,2,IF(K20&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="6">
-        <f>IF(P20&gt;=5,"A+",IF(P20&gt;=4,"A",IF(P20&gt;=3.5,"A-",IF(P20&gt;=3,"B",IF(P20&gt;=2,"C",IF(P20&gt;=1,"D","F"))))))</f>
+        <v>67</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="O20" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q20" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="R20">
+        <f>SUM(C20:N20)</f>
+        <v/>
+      </c>
+      <c r="S20" s="4">
+        <f>ROUND(R20/12,2)</f>
+        <v/>
+      </c>
+      <c r="T20" s="5">
+        <f>IF(OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,(J20+K20)&lt;66,L20&lt;33,M20&lt;33,N20&lt;33,P20&lt;33,Q20&lt;33),0,MIN(5,ROUND((IF((C20+D20)/200*100&gt;=80,5,IF((C20+D20)/200*100&gt;=70,4,IF((C20+D20)/200*100&gt;=60,3.5,IF((C20+D20)/200*100&gt;=50,3,IF((C20+D20)/200*100&gt;=40,2,IF((C20+D20)/200*100&gt;=33,1,0))))))+IF((E20+F20)/200*100&gt;=80,5,IF((E20+F20)/200*100&gt;=70,4,IF((E20+F20)/200*100&gt;=60,3.5,IF((E20+F20)/200*100&gt;=50,3,IF((E20+F20)/200*100&gt;=40,2,IF((E20+F20)/200*100&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF((H20+I20)/200*100&gt;=80,5,IF((H20+I20)/200*100&gt;=70,4,IF((H20+I20)/200*100&gt;=60,3.5,IF((H20+I20)/200*100&gt;=50,3,IF((H20+I20)/200*100&gt;=40,2,IF((H20+I20)/200*100&gt;=33,1,0))))))+IF((J20+K20)/200*100&gt;=80,5,IF((J20+K20)/200*100&gt;=70,4,IF((J20+K20)/200*100&gt;=60,3.5,IF((J20+K20)/200*100&gt;=50,3,IF((J20+K20)/200*100&gt;=40,2,IF((J20+K20)/200*100&gt;=33,1,0))))))+IF(L20&gt;=80,5,IF(L20&gt;=70,4,IF(L20&gt;=60,3.5,IF(L20&gt;=50,3,IF(L20&gt;=40,2,IF(L20&gt;=33,1,0))))))+IF(M20&gt;=80,5,IF(M20&gt;=70,4,IF(M20&gt;=60,3.5,IF(M20&gt;=50,3,IF(M20&gt;=40,2,IF(M20&gt;=33,1,0))))))+IF(N20&gt;=80,5,IF(N20&gt;=70,4,IF(N20&gt;=60,3.5,IF(N20&gt;=50,3,IF(N20&gt;=40,2,IF(N20&gt;=33,1,0)))))))/8+IF(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))&gt;=2,(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U20" s="6">
+        <f>IF(T20&gt;=5,"A+",IF(T20&gt;=4,"A",IF(T20&gt;=3.5,"A-",IF(T20&gt;=3,"B",IF(T20&gt;=2,"C",IF(T20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -1987,52 +2239,64 @@
         </is>
       </c>
       <c r="C21" s="3" t="n">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>178</v>
-      </c>
-      <c r="E21" s="3" t="n">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>74</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>129</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>175</v>
+        <v>87</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>80</v>
       </c>
       <c r="H21" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="M21" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="I21" s="2" t="n">
-        <v>83</v>
-      </c>
-      <c r="J21" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="K21" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="L21" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="M21" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="N21">
-        <f>SUM(C21:J21)</f>
-        <v/>
-      </c>
-      <c r="O21" s="4">
-        <f>ROUND(N21/8,2)</f>
-        <v/>
-      </c>
-      <c r="P21" s="5">
-        <f>IF(OR(C21&lt;66,D21&lt;66,E21&lt;33,F21&lt;66,G21&lt;66,H21&lt;33,I21&lt;33,J21&lt;33,L21&lt;33,M21&lt;33),0,MIN(5,ROUND((IF(C21/200*100&gt;=80,5,IF(C21/200*100&gt;=70,4,IF(C21/200*100&gt;=60,3.5,IF(C21/200*100&gt;=50,3,IF(C21/200*100&gt;=40,2,IF(C21/200*100&gt;=33,1,0))))))+IF(D21/200*100&gt;=80,5,IF(D21/200*100&gt;=70,4,IF(D21/200*100&gt;=60,3.5,IF(D21/200*100&gt;=50,3,IF(D21/200*100&gt;=40,2,IF(D21/200*100&gt;=33,1,0))))))+IF(E21&gt;=80,5,IF(E21&gt;=70,4,IF(E21&gt;=60,3.5,IF(E21&gt;=50,3,IF(E21&gt;=40,2,IF(E21&gt;=33,1,0))))))+IF(F21/200*100&gt;=80,5,IF(F21/200*100&gt;=70,4,IF(F21/200*100&gt;=60,3.5,IF(F21/200*100&gt;=50,3,IF(F21/200*100&gt;=40,2,IF(F21/200*100&gt;=33,1,0))))))+IF(G21/200*100&gt;=80,5,IF(G21/200*100&gt;=70,4,IF(G21/200*100&gt;=60,3.5,IF(G21/200*100&gt;=50,3,IF(G21/200*100&gt;=40,2,IF(G21/200*100&gt;=33,1,0))))))+IF(H21&gt;=80,5,IF(H21&gt;=70,4,IF(H21&gt;=60,3.5,IF(H21&gt;=50,3,IF(H21&gt;=40,2,IF(H21&gt;=33,1,0))))))+IF(I21&gt;=80,5,IF(I21&gt;=70,4,IF(I21&gt;=60,3.5,IF(I21&gt;=50,3,IF(I21&gt;=40,2,IF(I21&gt;=33,1,0))))))+IF(J21&gt;=80,5,IF(J21&gt;=70,4,IF(J21&gt;=60,3.5,IF(J21&gt;=50,3,IF(J21&gt;=40,2,IF(J21&gt;=33,1,0)))))))/8+IF(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))&gt;=2,(IF(K21&gt;=80,5,IF(K21&gt;=70,4,IF(K21&gt;=60,3.5,IF(K21&gt;=50,3,IF(K21&gt;=40,2,IF(K21&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="6">
-        <f>IF(P21&gt;=5,"A+",IF(P21&gt;=4,"A",IF(P21&gt;=3.5,"A-",IF(P21&gt;=3,"B",IF(P21&gt;=2,"C",IF(P21&gt;=1,"D","F"))))))</f>
+      <c r="N21" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="R21">
+        <f>SUM(C21:N21)</f>
+        <v/>
+      </c>
+      <c r="S21" s="4">
+        <f>ROUND(R21/12,2)</f>
+        <v/>
+      </c>
+      <c r="T21" s="5">
+        <f>IF(OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,(J21+K21)&lt;66,L21&lt;33,M21&lt;33,N21&lt;33,P21&lt;33,Q21&lt;33),0,MIN(5,ROUND((IF((C21+D21)/200*100&gt;=80,5,IF((C21+D21)/200*100&gt;=70,4,IF((C21+D21)/200*100&gt;=60,3.5,IF((C21+D21)/200*100&gt;=50,3,IF((C21+D21)/200*100&gt;=40,2,IF((C21+D21)/200*100&gt;=33,1,0))))))+IF((E21+F21)/200*100&gt;=80,5,IF((E21+F21)/200*100&gt;=70,4,IF((E21+F21)/200*100&gt;=60,3.5,IF((E21+F21)/200*100&gt;=50,3,IF((E21+F21)/200*100&gt;=40,2,IF((E21+F21)/200*100&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF((H21+I21)/200*100&gt;=80,5,IF((H21+I21)/200*100&gt;=70,4,IF((H21+I21)/200*100&gt;=60,3.5,IF((H21+I21)/200*100&gt;=50,3,IF((H21+I21)/200*100&gt;=40,2,IF((H21+I21)/200*100&gt;=33,1,0))))))+IF((J21+K21)/200*100&gt;=80,5,IF((J21+K21)/200*100&gt;=70,4,IF((J21+K21)/200*100&gt;=60,3.5,IF((J21+K21)/200*100&gt;=50,3,IF((J21+K21)/200*100&gt;=40,2,IF((J21+K21)/200*100&gt;=33,1,0))))))+IF(L21&gt;=80,5,IF(L21&gt;=70,4,IF(L21&gt;=60,3.5,IF(L21&gt;=50,3,IF(L21&gt;=40,2,IF(L21&gt;=33,1,0))))))+IF(M21&gt;=80,5,IF(M21&gt;=70,4,IF(M21&gt;=60,3.5,IF(M21&gt;=50,3,IF(M21&gt;=40,2,IF(M21&gt;=33,1,0))))))+IF(N21&gt;=80,5,IF(N21&gt;=70,4,IF(N21&gt;=60,3.5,IF(N21&gt;=50,3,IF(N21&gt;=40,2,IF(N21&gt;=33,1,0)))))))/8+IF(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))&gt;=2,(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U21" s="6">
+        <f>IF(T21&gt;=5,"A+",IF(T21&gt;=4,"A",IF(T21&gt;=3.5,"A-",IF(T21&gt;=3,"B",IF(T21&gt;=2,"C",IF(T21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
     </row>
@@ -2093,7 +2357,7 @@
         </is>
       </c>
       <c r="F5" s="12">
-        <f>IFERROR(ROUND(AVERAGE('Data Source'!P:P),2), 0)</f>
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!T:T),2), 0)</f>
         <v/>
       </c>
       <c r="H5" s="10" t="inlineStr">
@@ -2102,7 +2366,7 @@
         </is>
       </c>
       <c r="I5" s="11">
-        <f>MAX('Data Source'!N:N)</f>
+        <f>MAX('Data Source'!R:R)</f>
         <v/>
       </c>
       <c r="K5" s="10" t="inlineStr">
@@ -2111,7 +2375,7 @@
         </is>
       </c>
       <c r="L5" s="13">
-        <f>IF(C5&gt;0,COUNTIF('Data Source'!P:P,"&gt;0")/C5,0)</f>
+        <f>IF(C5&gt;0,COUNTIF('Data Source'!T:T,"&gt;0")/C5,0)</f>
         <v/>
       </c>
     </row>
@@ -2201,11 +2465,11 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <f>'Data Source'!B18</f>
+        <f>'Data Source'!B11</f>
         <v/>
       </c>
       <c r="I9" s="5">
-        <f>'Data Source'!P18</f>
+        <f>'Data Source'!T11</f>
         <v/>
       </c>
     </row>
@@ -2236,11 +2500,11 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <f>'Data Source'!B17</f>
+        <f>'Data Source'!B4</f>
         <v/>
       </c>
       <c r="I10" s="5">
-        <f>'Data Source'!P17</f>
+        <f>'Data Source'!T4</f>
         <v/>
       </c>
     </row>
@@ -2271,11 +2535,11 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <f>'Data Source'!B8</f>
+        <f>'Data Source'!B21</f>
         <v/>
       </c>
       <c r="I11" s="5">
-        <f>'Data Source'!P8</f>
+        <f>'Data Source'!T21</f>
         <v/>
       </c>
     </row>
@@ -2306,11 +2570,11 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <f>'Data Source'!B13</f>
+        <f>'Data Source'!B6</f>
         <v/>
       </c>
       <c r="I12" s="5">
-        <f>'Data Source'!P13</f>
+        <f>'Data Source'!T6</f>
         <v/>
       </c>
     </row>
@@ -2341,11 +2605,11 @@
         <v>5</v>
       </c>
       <c r="H13">
-        <f>'Data Source'!B14</f>
+        <f>'Data Source'!B8</f>
         <v/>
       </c>
       <c r="I13" s="5">
-        <f>'Data Source'!P14</f>
+        <f>'Data Source'!T8</f>
         <v/>
       </c>
     </row>
@@ -2487,7 +2751,7 @@
       </c>
       <c r="C2" s="18" t="inlineStr">
         <is>
-          <t>Quran</t>
+          <t>Quran+Hadith</t>
         </is>
       </c>
       <c r="D2" s="18" t="inlineStr">
@@ -2561,55 +2825,55 @@
         <v/>
       </c>
       <c r="C3" s="6">
-        <f>IF('Data Source'!C2/200*100&gt;=80,"A+",IF('Data Source'!C2/200*100&gt;=70,"A",IF('Data Source'!C2/200*100&gt;=60,"A-",IF('Data Source'!C2/200*100&gt;=50,"B",IF('Data Source'!C2/200*100&gt;=40,"C",IF('Data Source'!C2/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=80,"A+",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=70,"A",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=60,"A-",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=50,"B",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=40,"C",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D3" s="6">
-        <f>IF('Data Source'!D2/200*100&gt;=80,"A+",IF('Data Source'!D2/200*100&gt;=70,"A",IF('Data Source'!D2/200*100&gt;=60,"A-",IF('Data Source'!D2/200*100&gt;=50,"B",IF('Data Source'!D2/200*100&gt;=40,"C",IF('Data Source'!D2/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=80,"A+",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=70,"A",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=60,"A-",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=50,"B",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=40,"C",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E3" s="6">
-        <f>IF('Data Source'!E2&gt;=80,"A+",IF('Data Source'!E2&gt;=70,"A",IF('Data Source'!E2&gt;=60,"A-",IF('Data Source'!E2&gt;=50,"B",IF('Data Source'!E2&gt;=40,"C",IF('Data Source'!E2&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G2&gt;=80,"A+",IF('Data Source'!G2&gt;=70,"A",IF('Data Source'!G2&gt;=60,"A-",IF('Data Source'!G2&gt;=50,"B",IF('Data Source'!G2&gt;=40,"C",IF('Data Source'!G2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F3" s="6">
-        <f>IF('Data Source'!F2/200*100&gt;=80,"A+",IF('Data Source'!F2/200*100&gt;=70,"A",IF('Data Source'!F2/200*100&gt;=60,"A-",IF('Data Source'!F2/200*100&gt;=50,"B",IF('Data Source'!F2/200*100&gt;=40,"C",IF('Data Source'!F2/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=80,"A+",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=70,"A",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=60,"A-",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=50,"B",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=40,"C",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G3" s="6">
-        <f>IF('Data Source'!G2/200*100&gt;=80,"A+",IF('Data Source'!G2/200*100&gt;=70,"A",IF('Data Source'!G2/200*100&gt;=60,"A-",IF('Data Source'!G2/200*100&gt;=50,"B",IF('Data Source'!G2/200*100&gt;=40,"C",IF('Data Source'!G2/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=80,"A+",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=70,"A",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=60,"A-",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=50,"B",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=40,"C",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H3" s="6">
-        <f>IF('Data Source'!H2&gt;=80,"A+",IF('Data Source'!H2&gt;=70,"A",IF('Data Source'!H2&gt;=60,"A-",IF('Data Source'!H2&gt;=50,"B",IF('Data Source'!H2&gt;=40,"C",IF('Data Source'!H2&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L2&gt;=80,"A+",IF('Data Source'!L2&gt;=70,"A",IF('Data Source'!L2&gt;=60,"A-",IF('Data Source'!L2&gt;=50,"B",IF('Data Source'!L2&gt;=40,"C",IF('Data Source'!L2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I3" s="6">
-        <f>IF('Data Source'!I2&gt;=80,"A+",IF('Data Source'!I2&gt;=70,"A",IF('Data Source'!I2&gt;=60,"A-",IF('Data Source'!I2&gt;=50,"B",IF('Data Source'!I2&gt;=40,"C",IF('Data Source'!I2&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M2&gt;=80,"A+",IF('Data Source'!M2&gt;=70,"A",IF('Data Source'!M2&gt;=60,"A-",IF('Data Source'!M2&gt;=50,"B",IF('Data Source'!M2&gt;=40,"C",IF('Data Source'!M2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J3" s="6">
-        <f>IF('Data Source'!J2&gt;=80,"A+",IF('Data Source'!J2&gt;=70,"A",IF('Data Source'!J2&gt;=60,"A-",IF('Data Source'!J2&gt;=50,"B",IF('Data Source'!J2&gt;=40,"C",IF('Data Source'!J2&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N2&gt;=80,"A+",IF('Data Source'!N2&gt;=70,"A",IF('Data Source'!N2&gt;=60,"A-",IF('Data Source'!N2&gt;=50,"B",IF('Data Source'!N2&gt;=40,"C",IF('Data Source'!N2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K3" s="6">
-        <f>IF('Data Source'!K2&gt;=80,"A+",IF('Data Source'!K2&gt;=70,"A",IF('Data Source'!K2&gt;=60,"A-",IF('Data Source'!K2&gt;=50,"B",IF('Data Source'!K2&gt;=40,"C",IF('Data Source'!K2&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O2&gt;=80,"A+",IF('Data Source'!O2&gt;=70,"A",IF('Data Source'!O2&gt;=60,"A-",IF('Data Source'!O2&gt;=50,"B",IF('Data Source'!O2&gt;=40,"C",IF('Data Source'!O2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L3" s="6">
-        <f>IF('Data Source'!L2&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M3" s="6">
-        <f>IF('Data Source'!M2&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N3" s="5">
-        <f>'Data Source'!P2</f>
+        <f>'Data Source'!T2</f>
         <v/>
       </c>
       <c r="O3" s="6">
-        <f>'Data Source'!Q2</f>
+        <f>'Data Source'!U2</f>
         <v/>
       </c>
     </row>
@@ -2623,55 +2887,55 @@
         <v/>
       </c>
       <c r="C4" s="6">
-        <f>IF('Data Source'!C3/200*100&gt;=80,"A+",IF('Data Source'!C3/200*100&gt;=70,"A",IF('Data Source'!C3/200*100&gt;=60,"A-",IF('Data Source'!C3/200*100&gt;=50,"B",IF('Data Source'!C3/200*100&gt;=40,"C",IF('Data Source'!C3/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=80,"A+",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=70,"A",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=60,"A-",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=50,"B",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=40,"C",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D4" s="6">
-        <f>IF('Data Source'!D3/200*100&gt;=80,"A+",IF('Data Source'!D3/200*100&gt;=70,"A",IF('Data Source'!D3/200*100&gt;=60,"A-",IF('Data Source'!D3/200*100&gt;=50,"B",IF('Data Source'!D3/200*100&gt;=40,"C",IF('Data Source'!D3/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=80,"A+",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=70,"A",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=60,"A-",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=50,"B",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=40,"C",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E4" s="6">
-        <f>IF('Data Source'!E3&gt;=80,"A+",IF('Data Source'!E3&gt;=70,"A",IF('Data Source'!E3&gt;=60,"A-",IF('Data Source'!E3&gt;=50,"B",IF('Data Source'!E3&gt;=40,"C",IF('Data Source'!E3&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G3&gt;=80,"A+",IF('Data Source'!G3&gt;=70,"A",IF('Data Source'!G3&gt;=60,"A-",IF('Data Source'!G3&gt;=50,"B",IF('Data Source'!G3&gt;=40,"C",IF('Data Source'!G3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F4" s="6">
-        <f>IF('Data Source'!F3/200*100&gt;=80,"A+",IF('Data Source'!F3/200*100&gt;=70,"A",IF('Data Source'!F3/200*100&gt;=60,"A-",IF('Data Source'!F3/200*100&gt;=50,"B",IF('Data Source'!F3/200*100&gt;=40,"C",IF('Data Source'!F3/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=80,"A+",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=70,"A",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=60,"A-",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=50,"B",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=40,"C",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G4" s="6">
-        <f>IF('Data Source'!G3/200*100&gt;=80,"A+",IF('Data Source'!G3/200*100&gt;=70,"A",IF('Data Source'!G3/200*100&gt;=60,"A-",IF('Data Source'!G3/200*100&gt;=50,"B",IF('Data Source'!G3/200*100&gt;=40,"C",IF('Data Source'!G3/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=80,"A+",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=70,"A",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=60,"A-",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=50,"B",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=40,"C",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H4" s="6">
-        <f>IF('Data Source'!H3&gt;=80,"A+",IF('Data Source'!H3&gt;=70,"A",IF('Data Source'!H3&gt;=60,"A-",IF('Data Source'!H3&gt;=50,"B",IF('Data Source'!H3&gt;=40,"C",IF('Data Source'!H3&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L3&gt;=80,"A+",IF('Data Source'!L3&gt;=70,"A",IF('Data Source'!L3&gt;=60,"A-",IF('Data Source'!L3&gt;=50,"B",IF('Data Source'!L3&gt;=40,"C",IF('Data Source'!L3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I4" s="6">
-        <f>IF('Data Source'!I3&gt;=80,"A+",IF('Data Source'!I3&gt;=70,"A",IF('Data Source'!I3&gt;=60,"A-",IF('Data Source'!I3&gt;=50,"B",IF('Data Source'!I3&gt;=40,"C",IF('Data Source'!I3&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M3&gt;=80,"A+",IF('Data Source'!M3&gt;=70,"A",IF('Data Source'!M3&gt;=60,"A-",IF('Data Source'!M3&gt;=50,"B",IF('Data Source'!M3&gt;=40,"C",IF('Data Source'!M3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J4" s="6">
-        <f>IF('Data Source'!J3&gt;=80,"A+",IF('Data Source'!J3&gt;=70,"A",IF('Data Source'!J3&gt;=60,"A-",IF('Data Source'!J3&gt;=50,"B",IF('Data Source'!J3&gt;=40,"C",IF('Data Source'!J3&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N3&gt;=80,"A+",IF('Data Source'!N3&gt;=70,"A",IF('Data Source'!N3&gt;=60,"A-",IF('Data Source'!N3&gt;=50,"B",IF('Data Source'!N3&gt;=40,"C",IF('Data Source'!N3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K4" s="6">
-        <f>IF('Data Source'!K3&gt;=80,"A+",IF('Data Source'!K3&gt;=70,"A",IF('Data Source'!K3&gt;=60,"A-",IF('Data Source'!K3&gt;=50,"B",IF('Data Source'!K3&gt;=40,"C",IF('Data Source'!K3&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O3&gt;=80,"A+",IF('Data Source'!O3&gt;=70,"A",IF('Data Source'!O3&gt;=60,"A-",IF('Data Source'!O3&gt;=50,"B",IF('Data Source'!O3&gt;=40,"C",IF('Data Source'!O3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L4" s="6">
-        <f>IF('Data Source'!L3&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M4" s="6">
-        <f>IF('Data Source'!M3&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N4" s="5">
-        <f>'Data Source'!P3</f>
+        <f>'Data Source'!T3</f>
         <v/>
       </c>
       <c r="O4" s="6">
-        <f>'Data Source'!Q3</f>
+        <f>'Data Source'!U3</f>
         <v/>
       </c>
     </row>
@@ -2685,55 +2949,55 @@
         <v/>
       </c>
       <c r="C5" s="6">
-        <f>IF('Data Source'!C4/200*100&gt;=80,"A+",IF('Data Source'!C4/200*100&gt;=70,"A",IF('Data Source'!C4/200*100&gt;=60,"A-",IF('Data Source'!C4/200*100&gt;=50,"B",IF('Data Source'!C4/200*100&gt;=40,"C",IF('Data Source'!C4/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=80,"A+",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=70,"A",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=60,"A-",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=50,"B",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=40,"C",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D5" s="6">
-        <f>IF('Data Source'!D4/200*100&gt;=80,"A+",IF('Data Source'!D4/200*100&gt;=70,"A",IF('Data Source'!D4/200*100&gt;=60,"A-",IF('Data Source'!D4/200*100&gt;=50,"B",IF('Data Source'!D4/200*100&gt;=40,"C",IF('Data Source'!D4/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=80,"A+",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=70,"A",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=60,"A-",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=50,"B",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=40,"C",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E5" s="6">
-        <f>IF('Data Source'!E4&gt;=80,"A+",IF('Data Source'!E4&gt;=70,"A",IF('Data Source'!E4&gt;=60,"A-",IF('Data Source'!E4&gt;=50,"B",IF('Data Source'!E4&gt;=40,"C",IF('Data Source'!E4&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G4&gt;=80,"A+",IF('Data Source'!G4&gt;=70,"A",IF('Data Source'!G4&gt;=60,"A-",IF('Data Source'!G4&gt;=50,"B",IF('Data Source'!G4&gt;=40,"C",IF('Data Source'!G4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F5" s="6">
-        <f>IF('Data Source'!F4/200*100&gt;=80,"A+",IF('Data Source'!F4/200*100&gt;=70,"A",IF('Data Source'!F4/200*100&gt;=60,"A-",IF('Data Source'!F4/200*100&gt;=50,"B",IF('Data Source'!F4/200*100&gt;=40,"C",IF('Data Source'!F4/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=80,"A+",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=70,"A",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=60,"A-",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=50,"B",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=40,"C",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G5" s="6">
-        <f>IF('Data Source'!G4/200*100&gt;=80,"A+",IF('Data Source'!G4/200*100&gt;=70,"A",IF('Data Source'!G4/200*100&gt;=60,"A-",IF('Data Source'!G4/200*100&gt;=50,"B",IF('Data Source'!G4/200*100&gt;=40,"C",IF('Data Source'!G4/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=80,"A+",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=70,"A",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=60,"A-",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=50,"B",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=40,"C",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H5" s="6">
-        <f>IF('Data Source'!H4&gt;=80,"A+",IF('Data Source'!H4&gt;=70,"A",IF('Data Source'!H4&gt;=60,"A-",IF('Data Source'!H4&gt;=50,"B",IF('Data Source'!H4&gt;=40,"C",IF('Data Source'!H4&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L4&gt;=80,"A+",IF('Data Source'!L4&gt;=70,"A",IF('Data Source'!L4&gt;=60,"A-",IF('Data Source'!L4&gt;=50,"B",IF('Data Source'!L4&gt;=40,"C",IF('Data Source'!L4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I5" s="6">
-        <f>IF('Data Source'!I4&gt;=80,"A+",IF('Data Source'!I4&gt;=70,"A",IF('Data Source'!I4&gt;=60,"A-",IF('Data Source'!I4&gt;=50,"B",IF('Data Source'!I4&gt;=40,"C",IF('Data Source'!I4&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M4&gt;=80,"A+",IF('Data Source'!M4&gt;=70,"A",IF('Data Source'!M4&gt;=60,"A-",IF('Data Source'!M4&gt;=50,"B",IF('Data Source'!M4&gt;=40,"C",IF('Data Source'!M4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J5" s="6">
-        <f>IF('Data Source'!J4&gt;=80,"A+",IF('Data Source'!J4&gt;=70,"A",IF('Data Source'!J4&gt;=60,"A-",IF('Data Source'!J4&gt;=50,"B",IF('Data Source'!J4&gt;=40,"C",IF('Data Source'!J4&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N4&gt;=80,"A+",IF('Data Source'!N4&gt;=70,"A",IF('Data Source'!N4&gt;=60,"A-",IF('Data Source'!N4&gt;=50,"B",IF('Data Source'!N4&gt;=40,"C",IF('Data Source'!N4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K5" s="6">
-        <f>IF('Data Source'!K4&gt;=80,"A+",IF('Data Source'!K4&gt;=70,"A",IF('Data Source'!K4&gt;=60,"A-",IF('Data Source'!K4&gt;=50,"B",IF('Data Source'!K4&gt;=40,"C",IF('Data Source'!K4&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O4&gt;=80,"A+",IF('Data Source'!O4&gt;=70,"A",IF('Data Source'!O4&gt;=60,"A-",IF('Data Source'!O4&gt;=50,"B",IF('Data Source'!O4&gt;=40,"C",IF('Data Source'!O4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L5" s="6">
-        <f>IF('Data Source'!L4&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M5" s="6">
-        <f>IF('Data Source'!M4&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N5" s="5">
-        <f>'Data Source'!P4</f>
+        <f>'Data Source'!T4</f>
         <v/>
       </c>
       <c r="O5" s="6">
-        <f>'Data Source'!Q4</f>
+        <f>'Data Source'!U4</f>
         <v/>
       </c>
     </row>
@@ -2747,55 +3011,55 @@
         <v/>
       </c>
       <c r="C6" s="6">
-        <f>IF('Data Source'!C5/200*100&gt;=80,"A+",IF('Data Source'!C5/200*100&gt;=70,"A",IF('Data Source'!C5/200*100&gt;=60,"A-",IF('Data Source'!C5/200*100&gt;=50,"B",IF('Data Source'!C5/200*100&gt;=40,"C",IF('Data Source'!C5/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=80,"A+",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=70,"A",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=60,"A-",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=50,"B",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=40,"C",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D6" s="6">
-        <f>IF('Data Source'!D5/200*100&gt;=80,"A+",IF('Data Source'!D5/200*100&gt;=70,"A",IF('Data Source'!D5/200*100&gt;=60,"A-",IF('Data Source'!D5/200*100&gt;=50,"B",IF('Data Source'!D5/200*100&gt;=40,"C",IF('Data Source'!D5/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=80,"A+",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=70,"A",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=60,"A-",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=50,"B",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=40,"C",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E6" s="6">
-        <f>IF('Data Source'!E5&gt;=80,"A+",IF('Data Source'!E5&gt;=70,"A",IF('Data Source'!E5&gt;=60,"A-",IF('Data Source'!E5&gt;=50,"B",IF('Data Source'!E5&gt;=40,"C",IF('Data Source'!E5&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G5&gt;=80,"A+",IF('Data Source'!G5&gt;=70,"A",IF('Data Source'!G5&gt;=60,"A-",IF('Data Source'!G5&gt;=50,"B",IF('Data Source'!G5&gt;=40,"C",IF('Data Source'!G5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F6" s="6">
-        <f>IF('Data Source'!F5/200*100&gt;=80,"A+",IF('Data Source'!F5/200*100&gt;=70,"A",IF('Data Source'!F5/200*100&gt;=60,"A-",IF('Data Source'!F5/200*100&gt;=50,"B",IF('Data Source'!F5/200*100&gt;=40,"C",IF('Data Source'!F5/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=80,"A+",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=70,"A",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=60,"A-",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=50,"B",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=40,"C",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G6" s="6">
-        <f>IF('Data Source'!G5/200*100&gt;=80,"A+",IF('Data Source'!G5/200*100&gt;=70,"A",IF('Data Source'!G5/200*100&gt;=60,"A-",IF('Data Source'!G5/200*100&gt;=50,"B",IF('Data Source'!G5/200*100&gt;=40,"C",IF('Data Source'!G5/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=80,"A+",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=70,"A",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=60,"A-",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=50,"B",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=40,"C",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H6" s="6">
-        <f>IF('Data Source'!H5&gt;=80,"A+",IF('Data Source'!H5&gt;=70,"A",IF('Data Source'!H5&gt;=60,"A-",IF('Data Source'!H5&gt;=50,"B",IF('Data Source'!H5&gt;=40,"C",IF('Data Source'!H5&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L5&gt;=80,"A+",IF('Data Source'!L5&gt;=70,"A",IF('Data Source'!L5&gt;=60,"A-",IF('Data Source'!L5&gt;=50,"B",IF('Data Source'!L5&gt;=40,"C",IF('Data Source'!L5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I6" s="6">
-        <f>IF('Data Source'!I5&gt;=80,"A+",IF('Data Source'!I5&gt;=70,"A",IF('Data Source'!I5&gt;=60,"A-",IF('Data Source'!I5&gt;=50,"B",IF('Data Source'!I5&gt;=40,"C",IF('Data Source'!I5&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M5&gt;=80,"A+",IF('Data Source'!M5&gt;=70,"A",IF('Data Source'!M5&gt;=60,"A-",IF('Data Source'!M5&gt;=50,"B",IF('Data Source'!M5&gt;=40,"C",IF('Data Source'!M5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J6" s="6">
-        <f>IF('Data Source'!J5&gt;=80,"A+",IF('Data Source'!J5&gt;=70,"A",IF('Data Source'!J5&gt;=60,"A-",IF('Data Source'!J5&gt;=50,"B",IF('Data Source'!J5&gt;=40,"C",IF('Data Source'!J5&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N5&gt;=80,"A+",IF('Data Source'!N5&gt;=70,"A",IF('Data Source'!N5&gt;=60,"A-",IF('Data Source'!N5&gt;=50,"B",IF('Data Source'!N5&gt;=40,"C",IF('Data Source'!N5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K6" s="6">
-        <f>IF('Data Source'!K5&gt;=80,"A+",IF('Data Source'!K5&gt;=70,"A",IF('Data Source'!K5&gt;=60,"A-",IF('Data Source'!K5&gt;=50,"B",IF('Data Source'!K5&gt;=40,"C",IF('Data Source'!K5&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O5&gt;=80,"A+",IF('Data Source'!O5&gt;=70,"A",IF('Data Source'!O5&gt;=60,"A-",IF('Data Source'!O5&gt;=50,"B",IF('Data Source'!O5&gt;=40,"C",IF('Data Source'!O5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L6" s="6">
-        <f>IF('Data Source'!L5&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M6" s="6">
-        <f>IF('Data Source'!M5&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N6" s="5">
-        <f>'Data Source'!P5</f>
+        <f>'Data Source'!T5</f>
         <v/>
       </c>
       <c r="O6" s="6">
-        <f>'Data Source'!Q5</f>
+        <f>'Data Source'!U5</f>
         <v/>
       </c>
     </row>
@@ -2809,55 +3073,55 @@
         <v/>
       </c>
       <c r="C7" s="6">
-        <f>IF('Data Source'!C6/200*100&gt;=80,"A+",IF('Data Source'!C6/200*100&gt;=70,"A",IF('Data Source'!C6/200*100&gt;=60,"A-",IF('Data Source'!C6/200*100&gt;=50,"B",IF('Data Source'!C6/200*100&gt;=40,"C",IF('Data Source'!C6/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=80,"A+",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=70,"A",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=60,"A-",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=50,"B",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=40,"C",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D7" s="6">
-        <f>IF('Data Source'!D6/200*100&gt;=80,"A+",IF('Data Source'!D6/200*100&gt;=70,"A",IF('Data Source'!D6/200*100&gt;=60,"A-",IF('Data Source'!D6/200*100&gt;=50,"B",IF('Data Source'!D6/200*100&gt;=40,"C",IF('Data Source'!D6/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=80,"A+",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=70,"A",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=60,"A-",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=50,"B",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=40,"C",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E7" s="6">
-        <f>IF('Data Source'!E6&gt;=80,"A+",IF('Data Source'!E6&gt;=70,"A",IF('Data Source'!E6&gt;=60,"A-",IF('Data Source'!E6&gt;=50,"B",IF('Data Source'!E6&gt;=40,"C",IF('Data Source'!E6&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G6&gt;=80,"A+",IF('Data Source'!G6&gt;=70,"A",IF('Data Source'!G6&gt;=60,"A-",IF('Data Source'!G6&gt;=50,"B",IF('Data Source'!G6&gt;=40,"C",IF('Data Source'!G6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F7" s="6">
-        <f>IF('Data Source'!F6/200*100&gt;=80,"A+",IF('Data Source'!F6/200*100&gt;=70,"A",IF('Data Source'!F6/200*100&gt;=60,"A-",IF('Data Source'!F6/200*100&gt;=50,"B",IF('Data Source'!F6/200*100&gt;=40,"C",IF('Data Source'!F6/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=80,"A+",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=70,"A",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=60,"A-",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=50,"B",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=40,"C",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G7" s="6">
-        <f>IF('Data Source'!G6/200*100&gt;=80,"A+",IF('Data Source'!G6/200*100&gt;=70,"A",IF('Data Source'!G6/200*100&gt;=60,"A-",IF('Data Source'!G6/200*100&gt;=50,"B",IF('Data Source'!G6/200*100&gt;=40,"C",IF('Data Source'!G6/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=80,"A+",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=70,"A",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=60,"A-",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=50,"B",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=40,"C",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H7" s="6">
-        <f>IF('Data Source'!H6&gt;=80,"A+",IF('Data Source'!H6&gt;=70,"A",IF('Data Source'!H6&gt;=60,"A-",IF('Data Source'!H6&gt;=50,"B",IF('Data Source'!H6&gt;=40,"C",IF('Data Source'!H6&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L6&gt;=80,"A+",IF('Data Source'!L6&gt;=70,"A",IF('Data Source'!L6&gt;=60,"A-",IF('Data Source'!L6&gt;=50,"B",IF('Data Source'!L6&gt;=40,"C",IF('Data Source'!L6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I7" s="6">
-        <f>IF('Data Source'!I6&gt;=80,"A+",IF('Data Source'!I6&gt;=70,"A",IF('Data Source'!I6&gt;=60,"A-",IF('Data Source'!I6&gt;=50,"B",IF('Data Source'!I6&gt;=40,"C",IF('Data Source'!I6&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M6&gt;=80,"A+",IF('Data Source'!M6&gt;=70,"A",IF('Data Source'!M6&gt;=60,"A-",IF('Data Source'!M6&gt;=50,"B",IF('Data Source'!M6&gt;=40,"C",IF('Data Source'!M6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J7" s="6">
-        <f>IF('Data Source'!J6&gt;=80,"A+",IF('Data Source'!J6&gt;=70,"A",IF('Data Source'!J6&gt;=60,"A-",IF('Data Source'!J6&gt;=50,"B",IF('Data Source'!J6&gt;=40,"C",IF('Data Source'!J6&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N6&gt;=80,"A+",IF('Data Source'!N6&gt;=70,"A",IF('Data Source'!N6&gt;=60,"A-",IF('Data Source'!N6&gt;=50,"B",IF('Data Source'!N6&gt;=40,"C",IF('Data Source'!N6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K7" s="6">
-        <f>IF('Data Source'!K6&gt;=80,"A+",IF('Data Source'!K6&gt;=70,"A",IF('Data Source'!K6&gt;=60,"A-",IF('Data Source'!K6&gt;=50,"B",IF('Data Source'!K6&gt;=40,"C",IF('Data Source'!K6&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O6&gt;=80,"A+",IF('Data Source'!O6&gt;=70,"A",IF('Data Source'!O6&gt;=60,"A-",IF('Data Source'!O6&gt;=50,"B",IF('Data Source'!O6&gt;=40,"C",IF('Data Source'!O6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L7" s="6">
-        <f>IF('Data Source'!L6&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M7" s="6">
-        <f>IF('Data Source'!M6&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N7" s="5">
-        <f>'Data Source'!P6</f>
+        <f>'Data Source'!T6</f>
         <v/>
       </c>
       <c r="O7" s="6">
-        <f>'Data Source'!Q6</f>
+        <f>'Data Source'!U6</f>
         <v/>
       </c>
     </row>
@@ -2871,55 +3135,55 @@
         <v/>
       </c>
       <c r="C8" s="6">
-        <f>IF('Data Source'!C7/200*100&gt;=80,"A+",IF('Data Source'!C7/200*100&gt;=70,"A",IF('Data Source'!C7/200*100&gt;=60,"A-",IF('Data Source'!C7/200*100&gt;=50,"B",IF('Data Source'!C7/200*100&gt;=40,"C",IF('Data Source'!C7/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=80,"A+",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=70,"A",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=60,"A-",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=50,"B",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=40,"C",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D8" s="6">
-        <f>IF('Data Source'!D7/200*100&gt;=80,"A+",IF('Data Source'!D7/200*100&gt;=70,"A",IF('Data Source'!D7/200*100&gt;=60,"A-",IF('Data Source'!D7/200*100&gt;=50,"B",IF('Data Source'!D7/200*100&gt;=40,"C",IF('Data Source'!D7/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=80,"A+",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=70,"A",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=60,"A-",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=50,"B",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=40,"C",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E8" s="6">
-        <f>IF('Data Source'!E7&gt;=80,"A+",IF('Data Source'!E7&gt;=70,"A",IF('Data Source'!E7&gt;=60,"A-",IF('Data Source'!E7&gt;=50,"B",IF('Data Source'!E7&gt;=40,"C",IF('Data Source'!E7&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G7&gt;=80,"A+",IF('Data Source'!G7&gt;=70,"A",IF('Data Source'!G7&gt;=60,"A-",IF('Data Source'!G7&gt;=50,"B",IF('Data Source'!G7&gt;=40,"C",IF('Data Source'!G7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F8" s="6">
-        <f>IF('Data Source'!F7/200*100&gt;=80,"A+",IF('Data Source'!F7/200*100&gt;=70,"A",IF('Data Source'!F7/200*100&gt;=60,"A-",IF('Data Source'!F7/200*100&gt;=50,"B",IF('Data Source'!F7/200*100&gt;=40,"C",IF('Data Source'!F7/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=80,"A+",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=70,"A",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=60,"A-",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=50,"B",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=40,"C",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G8" s="6">
-        <f>IF('Data Source'!G7/200*100&gt;=80,"A+",IF('Data Source'!G7/200*100&gt;=70,"A",IF('Data Source'!G7/200*100&gt;=60,"A-",IF('Data Source'!G7/200*100&gt;=50,"B",IF('Data Source'!G7/200*100&gt;=40,"C",IF('Data Source'!G7/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=80,"A+",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=70,"A",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=60,"A-",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=50,"B",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=40,"C",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H8" s="6">
-        <f>IF('Data Source'!H7&gt;=80,"A+",IF('Data Source'!H7&gt;=70,"A",IF('Data Source'!H7&gt;=60,"A-",IF('Data Source'!H7&gt;=50,"B",IF('Data Source'!H7&gt;=40,"C",IF('Data Source'!H7&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L7&gt;=80,"A+",IF('Data Source'!L7&gt;=70,"A",IF('Data Source'!L7&gt;=60,"A-",IF('Data Source'!L7&gt;=50,"B",IF('Data Source'!L7&gt;=40,"C",IF('Data Source'!L7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I8" s="6">
-        <f>IF('Data Source'!I7&gt;=80,"A+",IF('Data Source'!I7&gt;=70,"A",IF('Data Source'!I7&gt;=60,"A-",IF('Data Source'!I7&gt;=50,"B",IF('Data Source'!I7&gt;=40,"C",IF('Data Source'!I7&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M7&gt;=80,"A+",IF('Data Source'!M7&gt;=70,"A",IF('Data Source'!M7&gt;=60,"A-",IF('Data Source'!M7&gt;=50,"B",IF('Data Source'!M7&gt;=40,"C",IF('Data Source'!M7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J8" s="6">
-        <f>IF('Data Source'!J7&gt;=80,"A+",IF('Data Source'!J7&gt;=70,"A",IF('Data Source'!J7&gt;=60,"A-",IF('Data Source'!J7&gt;=50,"B",IF('Data Source'!J7&gt;=40,"C",IF('Data Source'!J7&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N7&gt;=80,"A+",IF('Data Source'!N7&gt;=70,"A",IF('Data Source'!N7&gt;=60,"A-",IF('Data Source'!N7&gt;=50,"B",IF('Data Source'!N7&gt;=40,"C",IF('Data Source'!N7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K8" s="6">
-        <f>IF('Data Source'!K7&gt;=80,"A+",IF('Data Source'!K7&gt;=70,"A",IF('Data Source'!K7&gt;=60,"A-",IF('Data Source'!K7&gt;=50,"B",IF('Data Source'!K7&gt;=40,"C",IF('Data Source'!K7&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O7&gt;=80,"A+",IF('Data Source'!O7&gt;=70,"A",IF('Data Source'!O7&gt;=60,"A-",IF('Data Source'!O7&gt;=50,"B",IF('Data Source'!O7&gt;=40,"C",IF('Data Source'!O7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L8" s="6">
-        <f>IF('Data Source'!L7&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M8" s="6">
-        <f>IF('Data Source'!M7&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N8" s="5">
-        <f>'Data Source'!P7</f>
+        <f>'Data Source'!T7</f>
         <v/>
       </c>
       <c r="O8" s="6">
-        <f>'Data Source'!Q7</f>
+        <f>'Data Source'!U7</f>
         <v/>
       </c>
     </row>
@@ -2933,55 +3197,55 @@
         <v/>
       </c>
       <c r="C9" s="6">
-        <f>IF('Data Source'!C8/200*100&gt;=80,"A+",IF('Data Source'!C8/200*100&gt;=70,"A",IF('Data Source'!C8/200*100&gt;=60,"A-",IF('Data Source'!C8/200*100&gt;=50,"B",IF('Data Source'!C8/200*100&gt;=40,"C",IF('Data Source'!C8/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=80,"A+",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=70,"A",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=60,"A-",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=50,"B",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=40,"C",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D9" s="6">
-        <f>IF('Data Source'!D8/200*100&gt;=80,"A+",IF('Data Source'!D8/200*100&gt;=70,"A",IF('Data Source'!D8/200*100&gt;=60,"A-",IF('Data Source'!D8/200*100&gt;=50,"B",IF('Data Source'!D8/200*100&gt;=40,"C",IF('Data Source'!D8/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=80,"A+",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=70,"A",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=60,"A-",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=50,"B",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=40,"C",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E9" s="6">
-        <f>IF('Data Source'!E8&gt;=80,"A+",IF('Data Source'!E8&gt;=70,"A",IF('Data Source'!E8&gt;=60,"A-",IF('Data Source'!E8&gt;=50,"B",IF('Data Source'!E8&gt;=40,"C",IF('Data Source'!E8&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G8&gt;=80,"A+",IF('Data Source'!G8&gt;=70,"A",IF('Data Source'!G8&gt;=60,"A-",IF('Data Source'!G8&gt;=50,"B",IF('Data Source'!G8&gt;=40,"C",IF('Data Source'!G8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F9" s="6">
-        <f>IF('Data Source'!F8/200*100&gt;=80,"A+",IF('Data Source'!F8/200*100&gt;=70,"A",IF('Data Source'!F8/200*100&gt;=60,"A-",IF('Data Source'!F8/200*100&gt;=50,"B",IF('Data Source'!F8/200*100&gt;=40,"C",IF('Data Source'!F8/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=80,"A+",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=70,"A",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=60,"A-",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=50,"B",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=40,"C",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G9" s="6">
-        <f>IF('Data Source'!G8/200*100&gt;=80,"A+",IF('Data Source'!G8/200*100&gt;=70,"A",IF('Data Source'!G8/200*100&gt;=60,"A-",IF('Data Source'!G8/200*100&gt;=50,"B",IF('Data Source'!G8/200*100&gt;=40,"C",IF('Data Source'!G8/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=80,"A+",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=70,"A",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=60,"A-",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=50,"B",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=40,"C",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H9" s="6">
-        <f>IF('Data Source'!H8&gt;=80,"A+",IF('Data Source'!H8&gt;=70,"A",IF('Data Source'!H8&gt;=60,"A-",IF('Data Source'!H8&gt;=50,"B",IF('Data Source'!H8&gt;=40,"C",IF('Data Source'!H8&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L8&gt;=80,"A+",IF('Data Source'!L8&gt;=70,"A",IF('Data Source'!L8&gt;=60,"A-",IF('Data Source'!L8&gt;=50,"B",IF('Data Source'!L8&gt;=40,"C",IF('Data Source'!L8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I9" s="6">
-        <f>IF('Data Source'!I8&gt;=80,"A+",IF('Data Source'!I8&gt;=70,"A",IF('Data Source'!I8&gt;=60,"A-",IF('Data Source'!I8&gt;=50,"B",IF('Data Source'!I8&gt;=40,"C",IF('Data Source'!I8&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M8&gt;=80,"A+",IF('Data Source'!M8&gt;=70,"A",IF('Data Source'!M8&gt;=60,"A-",IF('Data Source'!M8&gt;=50,"B",IF('Data Source'!M8&gt;=40,"C",IF('Data Source'!M8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J9" s="6">
-        <f>IF('Data Source'!J8&gt;=80,"A+",IF('Data Source'!J8&gt;=70,"A",IF('Data Source'!J8&gt;=60,"A-",IF('Data Source'!J8&gt;=50,"B",IF('Data Source'!J8&gt;=40,"C",IF('Data Source'!J8&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N8&gt;=80,"A+",IF('Data Source'!N8&gt;=70,"A",IF('Data Source'!N8&gt;=60,"A-",IF('Data Source'!N8&gt;=50,"B",IF('Data Source'!N8&gt;=40,"C",IF('Data Source'!N8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K9" s="6">
-        <f>IF('Data Source'!K8&gt;=80,"A+",IF('Data Source'!K8&gt;=70,"A",IF('Data Source'!K8&gt;=60,"A-",IF('Data Source'!K8&gt;=50,"B",IF('Data Source'!K8&gt;=40,"C",IF('Data Source'!K8&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O8&gt;=80,"A+",IF('Data Source'!O8&gt;=70,"A",IF('Data Source'!O8&gt;=60,"A-",IF('Data Source'!O8&gt;=50,"B",IF('Data Source'!O8&gt;=40,"C",IF('Data Source'!O8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L9" s="6">
-        <f>IF('Data Source'!L8&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M9" s="6">
-        <f>IF('Data Source'!M8&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N9" s="5">
-        <f>'Data Source'!P8</f>
+        <f>'Data Source'!T8</f>
         <v/>
       </c>
       <c r="O9" s="6">
-        <f>'Data Source'!Q8</f>
+        <f>'Data Source'!U8</f>
         <v/>
       </c>
     </row>
@@ -2995,55 +3259,55 @@
         <v/>
       </c>
       <c r="C10" s="6">
-        <f>IF('Data Source'!C9/200*100&gt;=80,"A+",IF('Data Source'!C9/200*100&gt;=70,"A",IF('Data Source'!C9/200*100&gt;=60,"A-",IF('Data Source'!C9/200*100&gt;=50,"B",IF('Data Source'!C9/200*100&gt;=40,"C",IF('Data Source'!C9/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=80,"A+",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=70,"A",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=60,"A-",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=50,"B",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=40,"C",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D10" s="6">
-        <f>IF('Data Source'!D9/200*100&gt;=80,"A+",IF('Data Source'!D9/200*100&gt;=70,"A",IF('Data Source'!D9/200*100&gt;=60,"A-",IF('Data Source'!D9/200*100&gt;=50,"B",IF('Data Source'!D9/200*100&gt;=40,"C",IF('Data Source'!D9/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=80,"A+",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=70,"A",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=60,"A-",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=50,"B",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=40,"C",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E10" s="6">
-        <f>IF('Data Source'!E9&gt;=80,"A+",IF('Data Source'!E9&gt;=70,"A",IF('Data Source'!E9&gt;=60,"A-",IF('Data Source'!E9&gt;=50,"B",IF('Data Source'!E9&gt;=40,"C",IF('Data Source'!E9&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G9&gt;=80,"A+",IF('Data Source'!G9&gt;=70,"A",IF('Data Source'!G9&gt;=60,"A-",IF('Data Source'!G9&gt;=50,"B",IF('Data Source'!G9&gt;=40,"C",IF('Data Source'!G9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F10" s="6">
-        <f>IF('Data Source'!F9/200*100&gt;=80,"A+",IF('Data Source'!F9/200*100&gt;=70,"A",IF('Data Source'!F9/200*100&gt;=60,"A-",IF('Data Source'!F9/200*100&gt;=50,"B",IF('Data Source'!F9/200*100&gt;=40,"C",IF('Data Source'!F9/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=80,"A+",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=70,"A",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=60,"A-",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=50,"B",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=40,"C",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G10" s="6">
-        <f>IF('Data Source'!G9/200*100&gt;=80,"A+",IF('Data Source'!G9/200*100&gt;=70,"A",IF('Data Source'!G9/200*100&gt;=60,"A-",IF('Data Source'!G9/200*100&gt;=50,"B",IF('Data Source'!G9/200*100&gt;=40,"C",IF('Data Source'!G9/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=80,"A+",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=70,"A",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=60,"A-",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=50,"B",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=40,"C",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H10" s="6">
-        <f>IF('Data Source'!H9&gt;=80,"A+",IF('Data Source'!H9&gt;=70,"A",IF('Data Source'!H9&gt;=60,"A-",IF('Data Source'!H9&gt;=50,"B",IF('Data Source'!H9&gt;=40,"C",IF('Data Source'!H9&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L9&gt;=80,"A+",IF('Data Source'!L9&gt;=70,"A",IF('Data Source'!L9&gt;=60,"A-",IF('Data Source'!L9&gt;=50,"B",IF('Data Source'!L9&gt;=40,"C",IF('Data Source'!L9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I10" s="6">
-        <f>IF('Data Source'!I9&gt;=80,"A+",IF('Data Source'!I9&gt;=70,"A",IF('Data Source'!I9&gt;=60,"A-",IF('Data Source'!I9&gt;=50,"B",IF('Data Source'!I9&gt;=40,"C",IF('Data Source'!I9&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M9&gt;=80,"A+",IF('Data Source'!M9&gt;=70,"A",IF('Data Source'!M9&gt;=60,"A-",IF('Data Source'!M9&gt;=50,"B",IF('Data Source'!M9&gt;=40,"C",IF('Data Source'!M9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J10" s="6">
-        <f>IF('Data Source'!J9&gt;=80,"A+",IF('Data Source'!J9&gt;=70,"A",IF('Data Source'!J9&gt;=60,"A-",IF('Data Source'!J9&gt;=50,"B",IF('Data Source'!J9&gt;=40,"C",IF('Data Source'!J9&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N9&gt;=80,"A+",IF('Data Source'!N9&gt;=70,"A",IF('Data Source'!N9&gt;=60,"A-",IF('Data Source'!N9&gt;=50,"B",IF('Data Source'!N9&gt;=40,"C",IF('Data Source'!N9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K10" s="6">
-        <f>IF('Data Source'!K9&gt;=80,"A+",IF('Data Source'!K9&gt;=70,"A",IF('Data Source'!K9&gt;=60,"A-",IF('Data Source'!K9&gt;=50,"B",IF('Data Source'!K9&gt;=40,"C",IF('Data Source'!K9&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O9&gt;=80,"A+",IF('Data Source'!O9&gt;=70,"A",IF('Data Source'!O9&gt;=60,"A-",IF('Data Source'!O9&gt;=50,"B",IF('Data Source'!O9&gt;=40,"C",IF('Data Source'!O9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L10" s="6">
-        <f>IF('Data Source'!L9&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M10" s="6">
-        <f>IF('Data Source'!M9&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N10" s="5">
-        <f>'Data Source'!P9</f>
+        <f>'Data Source'!T9</f>
         <v/>
       </c>
       <c r="O10" s="6">
-        <f>'Data Source'!Q9</f>
+        <f>'Data Source'!U9</f>
         <v/>
       </c>
     </row>
@@ -3057,55 +3321,55 @@
         <v/>
       </c>
       <c r="C11" s="6">
-        <f>IF('Data Source'!C10/200*100&gt;=80,"A+",IF('Data Source'!C10/200*100&gt;=70,"A",IF('Data Source'!C10/200*100&gt;=60,"A-",IF('Data Source'!C10/200*100&gt;=50,"B",IF('Data Source'!C10/200*100&gt;=40,"C",IF('Data Source'!C10/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=80,"A+",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=70,"A",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=60,"A-",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=50,"B",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=40,"C",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D11" s="6">
-        <f>IF('Data Source'!D10/200*100&gt;=80,"A+",IF('Data Source'!D10/200*100&gt;=70,"A",IF('Data Source'!D10/200*100&gt;=60,"A-",IF('Data Source'!D10/200*100&gt;=50,"B",IF('Data Source'!D10/200*100&gt;=40,"C",IF('Data Source'!D10/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=80,"A+",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=70,"A",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=60,"A-",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=50,"B",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=40,"C",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E11" s="6">
-        <f>IF('Data Source'!E10&gt;=80,"A+",IF('Data Source'!E10&gt;=70,"A",IF('Data Source'!E10&gt;=60,"A-",IF('Data Source'!E10&gt;=50,"B",IF('Data Source'!E10&gt;=40,"C",IF('Data Source'!E10&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G10&gt;=80,"A+",IF('Data Source'!G10&gt;=70,"A",IF('Data Source'!G10&gt;=60,"A-",IF('Data Source'!G10&gt;=50,"B",IF('Data Source'!G10&gt;=40,"C",IF('Data Source'!G10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F11" s="6">
-        <f>IF('Data Source'!F10/200*100&gt;=80,"A+",IF('Data Source'!F10/200*100&gt;=70,"A",IF('Data Source'!F10/200*100&gt;=60,"A-",IF('Data Source'!F10/200*100&gt;=50,"B",IF('Data Source'!F10/200*100&gt;=40,"C",IF('Data Source'!F10/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=80,"A+",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=70,"A",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=60,"A-",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=50,"B",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=40,"C",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G11" s="6">
-        <f>IF('Data Source'!G10/200*100&gt;=80,"A+",IF('Data Source'!G10/200*100&gt;=70,"A",IF('Data Source'!G10/200*100&gt;=60,"A-",IF('Data Source'!G10/200*100&gt;=50,"B",IF('Data Source'!G10/200*100&gt;=40,"C",IF('Data Source'!G10/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=80,"A+",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=70,"A",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=60,"A-",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=50,"B",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=40,"C",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H11" s="6">
-        <f>IF('Data Source'!H10&gt;=80,"A+",IF('Data Source'!H10&gt;=70,"A",IF('Data Source'!H10&gt;=60,"A-",IF('Data Source'!H10&gt;=50,"B",IF('Data Source'!H10&gt;=40,"C",IF('Data Source'!H10&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L10&gt;=80,"A+",IF('Data Source'!L10&gt;=70,"A",IF('Data Source'!L10&gt;=60,"A-",IF('Data Source'!L10&gt;=50,"B",IF('Data Source'!L10&gt;=40,"C",IF('Data Source'!L10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I11" s="6">
-        <f>IF('Data Source'!I10&gt;=80,"A+",IF('Data Source'!I10&gt;=70,"A",IF('Data Source'!I10&gt;=60,"A-",IF('Data Source'!I10&gt;=50,"B",IF('Data Source'!I10&gt;=40,"C",IF('Data Source'!I10&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M10&gt;=80,"A+",IF('Data Source'!M10&gt;=70,"A",IF('Data Source'!M10&gt;=60,"A-",IF('Data Source'!M10&gt;=50,"B",IF('Data Source'!M10&gt;=40,"C",IF('Data Source'!M10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J11" s="6">
-        <f>IF('Data Source'!J10&gt;=80,"A+",IF('Data Source'!J10&gt;=70,"A",IF('Data Source'!J10&gt;=60,"A-",IF('Data Source'!J10&gt;=50,"B",IF('Data Source'!J10&gt;=40,"C",IF('Data Source'!J10&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N10&gt;=80,"A+",IF('Data Source'!N10&gt;=70,"A",IF('Data Source'!N10&gt;=60,"A-",IF('Data Source'!N10&gt;=50,"B",IF('Data Source'!N10&gt;=40,"C",IF('Data Source'!N10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K11" s="6">
-        <f>IF('Data Source'!K10&gt;=80,"A+",IF('Data Source'!K10&gt;=70,"A",IF('Data Source'!K10&gt;=60,"A-",IF('Data Source'!K10&gt;=50,"B",IF('Data Source'!K10&gt;=40,"C",IF('Data Source'!K10&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O10&gt;=80,"A+",IF('Data Source'!O10&gt;=70,"A",IF('Data Source'!O10&gt;=60,"A-",IF('Data Source'!O10&gt;=50,"B",IF('Data Source'!O10&gt;=40,"C",IF('Data Source'!O10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L11" s="6">
-        <f>IF('Data Source'!L10&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M11" s="6">
-        <f>IF('Data Source'!M10&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N11" s="5">
-        <f>'Data Source'!P10</f>
+        <f>'Data Source'!T10</f>
         <v/>
       </c>
       <c r="O11" s="6">
-        <f>'Data Source'!Q10</f>
+        <f>'Data Source'!U10</f>
         <v/>
       </c>
     </row>
@@ -3119,55 +3383,55 @@
         <v/>
       </c>
       <c r="C12" s="6">
-        <f>IF('Data Source'!C11/200*100&gt;=80,"A+",IF('Data Source'!C11/200*100&gt;=70,"A",IF('Data Source'!C11/200*100&gt;=60,"A-",IF('Data Source'!C11/200*100&gt;=50,"B",IF('Data Source'!C11/200*100&gt;=40,"C",IF('Data Source'!C11/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=80,"A+",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=70,"A",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=60,"A-",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=50,"B",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=40,"C",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D12" s="6">
-        <f>IF('Data Source'!D11/200*100&gt;=80,"A+",IF('Data Source'!D11/200*100&gt;=70,"A",IF('Data Source'!D11/200*100&gt;=60,"A-",IF('Data Source'!D11/200*100&gt;=50,"B",IF('Data Source'!D11/200*100&gt;=40,"C",IF('Data Source'!D11/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=80,"A+",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=70,"A",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=60,"A-",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=50,"B",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=40,"C",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E12" s="6">
-        <f>IF('Data Source'!E11&gt;=80,"A+",IF('Data Source'!E11&gt;=70,"A",IF('Data Source'!E11&gt;=60,"A-",IF('Data Source'!E11&gt;=50,"B",IF('Data Source'!E11&gt;=40,"C",IF('Data Source'!E11&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G11&gt;=80,"A+",IF('Data Source'!G11&gt;=70,"A",IF('Data Source'!G11&gt;=60,"A-",IF('Data Source'!G11&gt;=50,"B",IF('Data Source'!G11&gt;=40,"C",IF('Data Source'!G11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F12" s="6">
-        <f>IF('Data Source'!F11/200*100&gt;=80,"A+",IF('Data Source'!F11/200*100&gt;=70,"A",IF('Data Source'!F11/200*100&gt;=60,"A-",IF('Data Source'!F11/200*100&gt;=50,"B",IF('Data Source'!F11/200*100&gt;=40,"C",IF('Data Source'!F11/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=80,"A+",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=70,"A",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=60,"A-",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=50,"B",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=40,"C",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G12" s="6">
-        <f>IF('Data Source'!G11/200*100&gt;=80,"A+",IF('Data Source'!G11/200*100&gt;=70,"A",IF('Data Source'!G11/200*100&gt;=60,"A-",IF('Data Source'!G11/200*100&gt;=50,"B",IF('Data Source'!G11/200*100&gt;=40,"C",IF('Data Source'!G11/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=80,"A+",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=70,"A",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=60,"A-",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=50,"B",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=40,"C",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H12" s="6">
-        <f>IF('Data Source'!H11&gt;=80,"A+",IF('Data Source'!H11&gt;=70,"A",IF('Data Source'!H11&gt;=60,"A-",IF('Data Source'!H11&gt;=50,"B",IF('Data Source'!H11&gt;=40,"C",IF('Data Source'!H11&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L11&gt;=80,"A+",IF('Data Source'!L11&gt;=70,"A",IF('Data Source'!L11&gt;=60,"A-",IF('Data Source'!L11&gt;=50,"B",IF('Data Source'!L11&gt;=40,"C",IF('Data Source'!L11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I12" s="6">
-        <f>IF('Data Source'!I11&gt;=80,"A+",IF('Data Source'!I11&gt;=70,"A",IF('Data Source'!I11&gt;=60,"A-",IF('Data Source'!I11&gt;=50,"B",IF('Data Source'!I11&gt;=40,"C",IF('Data Source'!I11&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M11&gt;=80,"A+",IF('Data Source'!M11&gt;=70,"A",IF('Data Source'!M11&gt;=60,"A-",IF('Data Source'!M11&gt;=50,"B",IF('Data Source'!M11&gt;=40,"C",IF('Data Source'!M11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J12" s="6">
-        <f>IF('Data Source'!J11&gt;=80,"A+",IF('Data Source'!J11&gt;=70,"A",IF('Data Source'!J11&gt;=60,"A-",IF('Data Source'!J11&gt;=50,"B",IF('Data Source'!J11&gt;=40,"C",IF('Data Source'!J11&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N11&gt;=80,"A+",IF('Data Source'!N11&gt;=70,"A",IF('Data Source'!N11&gt;=60,"A-",IF('Data Source'!N11&gt;=50,"B",IF('Data Source'!N11&gt;=40,"C",IF('Data Source'!N11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K12" s="6">
-        <f>IF('Data Source'!K11&gt;=80,"A+",IF('Data Source'!K11&gt;=70,"A",IF('Data Source'!K11&gt;=60,"A-",IF('Data Source'!K11&gt;=50,"B",IF('Data Source'!K11&gt;=40,"C",IF('Data Source'!K11&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O11&gt;=80,"A+",IF('Data Source'!O11&gt;=70,"A",IF('Data Source'!O11&gt;=60,"A-",IF('Data Source'!O11&gt;=50,"B",IF('Data Source'!O11&gt;=40,"C",IF('Data Source'!O11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L12" s="6">
-        <f>IF('Data Source'!L11&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M12" s="6">
-        <f>IF('Data Source'!M11&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N12" s="5">
-        <f>'Data Source'!P11</f>
+        <f>'Data Source'!T11</f>
         <v/>
       </c>
       <c r="O12" s="6">
-        <f>'Data Source'!Q11</f>
+        <f>'Data Source'!U11</f>
         <v/>
       </c>
     </row>
@@ -3181,55 +3445,55 @@
         <v/>
       </c>
       <c r="C13" s="6">
-        <f>IF('Data Source'!C12/200*100&gt;=80,"A+",IF('Data Source'!C12/200*100&gt;=70,"A",IF('Data Source'!C12/200*100&gt;=60,"A-",IF('Data Source'!C12/200*100&gt;=50,"B",IF('Data Source'!C12/200*100&gt;=40,"C",IF('Data Source'!C12/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=80,"A+",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=70,"A",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=60,"A-",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=50,"B",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=40,"C",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D13" s="6">
-        <f>IF('Data Source'!D12/200*100&gt;=80,"A+",IF('Data Source'!D12/200*100&gt;=70,"A",IF('Data Source'!D12/200*100&gt;=60,"A-",IF('Data Source'!D12/200*100&gt;=50,"B",IF('Data Source'!D12/200*100&gt;=40,"C",IF('Data Source'!D12/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=80,"A+",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=70,"A",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=60,"A-",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=50,"B",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=40,"C",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E13" s="6">
-        <f>IF('Data Source'!E12&gt;=80,"A+",IF('Data Source'!E12&gt;=70,"A",IF('Data Source'!E12&gt;=60,"A-",IF('Data Source'!E12&gt;=50,"B",IF('Data Source'!E12&gt;=40,"C",IF('Data Source'!E12&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G12&gt;=80,"A+",IF('Data Source'!G12&gt;=70,"A",IF('Data Source'!G12&gt;=60,"A-",IF('Data Source'!G12&gt;=50,"B",IF('Data Source'!G12&gt;=40,"C",IF('Data Source'!G12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F13" s="6">
-        <f>IF('Data Source'!F12/200*100&gt;=80,"A+",IF('Data Source'!F12/200*100&gt;=70,"A",IF('Data Source'!F12/200*100&gt;=60,"A-",IF('Data Source'!F12/200*100&gt;=50,"B",IF('Data Source'!F12/200*100&gt;=40,"C",IF('Data Source'!F12/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=80,"A+",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=70,"A",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=60,"A-",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=50,"B",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=40,"C",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G13" s="6">
-        <f>IF('Data Source'!G12/200*100&gt;=80,"A+",IF('Data Source'!G12/200*100&gt;=70,"A",IF('Data Source'!G12/200*100&gt;=60,"A-",IF('Data Source'!G12/200*100&gt;=50,"B",IF('Data Source'!G12/200*100&gt;=40,"C",IF('Data Source'!G12/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=80,"A+",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=70,"A",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=60,"A-",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=50,"B",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=40,"C",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H13" s="6">
-        <f>IF('Data Source'!H12&gt;=80,"A+",IF('Data Source'!H12&gt;=70,"A",IF('Data Source'!H12&gt;=60,"A-",IF('Data Source'!H12&gt;=50,"B",IF('Data Source'!H12&gt;=40,"C",IF('Data Source'!H12&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L12&gt;=80,"A+",IF('Data Source'!L12&gt;=70,"A",IF('Data Source'!L12&gt;=60,"A-",IF('Data Source'!L12&gt;=50,"B",IF('Data Source'!L12&gt;=40,"C",IF('Data Source'!L12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I13" s="6">
-        <f>IF('Data Source'!I12&gt;=80,"A+",IF('Data Source'!I12&gt;=70,"A",IF('Data Source'!I12&gt;=60,"A-",IF('Data Source'!I12&gt;=50,"B",IF('Data Source'!I12&gt;=40,"C",IF('Data Source'!I12&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M12&gt;=80,"A+",IF('Data Source'!M12&gt;=70,"A",IF('Data Source'!M12&gt;=60,"A-",IF('Data Source'!M12&gt;=50,"B",IF('Data Source'!M12&gt;=40,"C",IF('Data Source'!M12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J13" s="6">
-        <f>IF('Data Source'!J12&gt;=80,"A+",IF('Data Source'!J12&gt;=70,"A",IF('Data Source'!J12&gt;=60,"A-",IF('Data Source'!J12&gt;=50,"B",IF('Data Source'!J12&gt;=40,"C",IF('Data Source'!J12&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N12&gt;=80,"A+",IF('Data Source'!N12&gt;=70,"A",IF('Data Source'!N12&gt;=60,"A-",IF('Data Source'!N12&gt;=50,"B",IF('Data Source'!N12&gt;=40,"C",IF('Data Source'!N12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K13" s="6">
-        <f>IF('Data Source'!K12&gt;=80,"A+",IF('Data Source'!K12&gt;=70,"A",IF('Data Source'!K12&gt;=60,"A-",IF('Data Source'!K12&gt;=50,"B",IF('Data Source'!K12&gt;=40,"C",IF('Data Source'!K12&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O12&gt;=80,"A+",IF('Data Source'!O12&gt;=70,"A",IF('Data Source'!O12&gt;=60,"A-",IF('Data Source'!O12&gt;=50,"B",IF('Data Source'!O12&gt;=40,"C",IF('Data Source'!O12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L13" s="6">
-        <f>IF('Data Source'!L12&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M13" s="6">
-        <f>IF('Data Source'!M12&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N13" s="5">
-        <f>'Data Source'!P12</f>
+        <f>'Data Source'!T12</f>
         <v/>
       </c>
       <c r="O13" s="6">
-        <f>'Data Source'!Q12</f>
+        <f>'Data Source'!U12</f>
         <v/>
       </c>
     </row>
@@ -3243,55 +3507,55 @@
         <v/>
       </c>
       <c r="C14" s="6">
-        <f>IF('Data Source'!C13/200*100&gt;=80,"A+",IF('Data Source'!C13/200*100&gt;=70,"A",IF('Data Source'!C13/200*100&gt;=60,"A-",IF('Data Source'!C13/200*100&gt;=50,"B",IF('Data Source'!C13/200*100&gt;=40,"C",IF('Data Source'!C13/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=80,"A+",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=70,"A",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=60,"A-",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=50,"B",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=40,"C",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D14" s="6">
-        <f>IF('Data Source'!D13/200*100&gt;=80,"A+",IF('Data Source'!D13/200*100&gt;=70,"A",IF('Data Source'!D13/200*100&gt;=60,"A-",IF('Data Source'!D13/200*100&gt;=50,"B",IF('Data Source'!D13/200*100&gt;=40,"C",IF('Data Source'!D13/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=80,"A+",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=70,"A",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=60,"A-",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=50,"B",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=40,"C",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E14" s="6">
-        <f>IF('Data Source'!E13&gt;=80,"A+",IF('Data Source'!E13&gt;=70,"A",IF('Data Source'!E13&gt;=60,"A-",IF('Data Source'!E13&gt;=50,"B",IF('Data Source'!E13&gt;=40,"C",IF('Data Source'!E13&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G13&gt;=80,"A+",IF('Data Source'!G13&gt;=70,"A",IF('Data Source'!G13&gt;=60,"A-",IF('Data Source'!G13&gt;=50,"B",IF('Data Source'!G13&gt;=40,"C",IF('Data Source'!G13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F14" s="6">
-        <f>IF('Data Source'!F13/200*100&gt;=80,"A+",IF('Data Source'!F13/200*100&gt;=70,"A",IF('Data Source'!F13/200*100&gt;=60,"A-",IF('Data Source'!F13/200*100&gt;=50,"B",IF('Data Source'!F13/200*100&gt;=40,"C",IF('Data Source'!F13/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=80,"A+",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=70,"A",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=60,"A-",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=50,"B",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=40,"C",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G14" s="6">
-        <f>IF('Data Source'!G13/200*100&gt;=80,"A+",IF('Data Source'!G13/200*100&gt;=70,"A",IF('Data Source'!G13/200*100&gt;=60,"A-",IF('Data Source'!G13/200*100&gt;=50,"B",IF('Data Source'!G13/200*100&gt;=40,"C",IF('Data Source'!G13/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=80,"A+",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=70,"A",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=60,"A-",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=50,"B",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=40,"C",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H14" s="6">
-        <f>IF('Data Source'!H13&gt;=80,"A+",IF('Data Source'!H13&gt;=70,"A",IF('Data Source'!H13&gt;=60,"A-",IF('Data Source'!H13&gt;=50,"B",IF('Data Source'!H13&gt;=40,"C",IF('Data Source'!H13&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L13&gt;=80,"A+",IF('Data Source'!L13&gt;=70,"A",IF('Data Source'!L13&gt;=60,"A-",IF('Data Source'!L13&gt;=50,"B",IF('Data Source'!L13&gt;=40,"C",IF('Data Source'!L13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I14" s="6">
-        <f>IF('Data Source'!I13&gt;=80,"A+",IF('Data Source'!I13&gt;=70,"A",IF('Data Source'!I13&gt;=60,"A-",IF('Data Source'!I13&gt;=50,"B",IF('Data Source'!I13&gt;=40,"C",IF('Data Source'!I13&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M13&gt;=80,"A+",IF('Data Source'!M13&gt;=70,"A",IF('Data Source'!M13&gt;=60,"A-",IF('Data Source'!M13&gt;=50,"B",IF('Data Source'!M13&gt;=40,"C",IF('Data Source'!M13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J14" s="6">
-        <f>IF('Data Source'!J13&gt;=80,"A+",IF('Data Source'!J13&gt;=70,"A",IF('Data Source'!J13&gt;=60,"A-",IF('Data Source'!J13&gt;=50,"B",IF('Data Source'!J13&gt;=40,"C",IF('Data Source'!J13&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N13&gt;=80,"A+",IF('Data Source'!N13&gt;=70,"A",IF('Data Source'!N13&gt;=60,"A-",IF('Data Source'!N13&gt;=50,"B",IF('Data Source'!N13&gt;=40,"C",IF('Data Source'!N13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K14" s="6">
-        <f>IF('Data Source'!K13&gt;=80,"A+",IF('Data Source'!K13&gt;=70,"A",IF('Data Source'!K13&gt;=60,"A-",IF('Data Source'!K13&gt;=50,"B",IF('Data Source'!K13&gt;=40,"C",IF('Data Source'!K13&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O13&gt;=80,"A+",IF('Data Source'!O13&gt;=70,"A",IF('Data Source'!O13&gt;=60,"A-",IF('Data Source'!O13&gt;=50,"B",IF('Data Source'!O13&gt;=40,"C",IF('Data Source'!O13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L14" s="6">
-        <f>IF('Data Source'!L13&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M14" s="6">
-        <f>IF('Data Source'!M13&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N14" s="5">
-        <f>'Data Source'!P13</f>
+        <f>'Data Source'!T13</f>
         <v/>
       </c>
       <c r="O14" s="6">
-        <f>'Data Source'!Q13</f>
+        <f>'Data Source'!U13</f>
         <v/>
       </c>
     </row>
@@ -3305,55 +3569,55 @@
         <v/>
       </c>
       <c r="C15" s="6">
-        <f>IF('Data Source'!C14/200*100&gt;=80,"A+",IF('Data Source'!C14/200*100&gt;=70,"A",IF('Data Source'!C14/200*100&gt;=60,"A-",IF('Data Source'!C14/200*100&gt;=50,"B",IF('Data Source'!C14/200*100&gt;=40,"C",IF('Data Source'!C14/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=80,"A+",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=70,"A",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=60,"A-",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=50,"B",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=40,"C",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D15" s="6">
-        <f>IF('Data Source'!D14/200*100&gt;=80,"A+",IF('Data Source'!D14/200*100&gt;=70,"A",IF('Data Source'!D14/200*100&gt;=60,"A-",IF('Data Source'!D14/200*100&gt;=50,"B",IF('Data Source'!D14/200*100&gt;=40,"C",IF('Data Source'!D14/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=80,"A+",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=70,"A",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=60,"A-",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=50,"B",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=40,"C",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E15" s="6">
-        <f>IF('Data Source'!E14&gt;=80,"A+",IF('Data Source'!E14&gt;=70,"A",IF('Data Source'!E14&gt;=60,"A-",IF('Data Source'!E14&gt;=50,"B",IF('Data Source'!E14&gt;=40,"C",IF('Data Source'!E14&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G14&gt;=80,"A+",IF('Data Source'!G14&gt;=70,"A",IF('Data Source'!G14&gt;=60,"A-",IF('Data Source'!G14&gt;=50,"B",IF('Data Source'!G14&gt;=40,"C",IF('Data Source'!G14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F15" s="6">
-        <f>IF('Data Source'!F14/200*100&gt;=80,"A+",IF('Data Source'!F14/200*100&gt;=70,"A",IF('Data Source'!F14/200*100&gt;=60,"A-",IF('Data Source'!F14/200*100&gt;=50,"B",IF('Data Source'!F14/200*100&gt;=40,"C",IF('Data Source'!F14/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=80,"A+",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=70,"A",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=60,"A-",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=50,"B",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=40,"C",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G15" s="6">
-        <f>IF('Data Source'!G14/200*100&gt;=80,"A+",IF('Data Source'!G14/200*100&gt;=70,"A",IF('Data Source'!G14/200*100&gt;=60,"A-",IF('Data Source'!G14/200*100&gt;=50,"B",IF('Data Source'!G14/200*100&gt;=40,"C",IF('Data Source'!G14/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=80,"A+",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=70,"A",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=60,"A-",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=50,"B",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=40,"C",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H15" s="6">
-        <f>IF('Data Source'!H14&gt;=80,"A+",IF('Data Source'!H14&gt;=70,"A",IF('Data Source'!H14&gt;=60,"A-",IF('Data Source'!H14&gt;=50,"B",IF('Data Source'!H14&gt;=40,"C",IF('Data Source'!H14&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L14&gt;=80,"A+",IF('Data Source'!L14&gt;=70,"A",IF('Data Source'!L14&gt;=60,"A-",IF('Data Source'!L14&gt;=50,"B",IF('Data Source'!L14&gt;=40,"C",IF('Data Source'!L14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I15" s="6">
-        <f>IF('Data Source'!I14&gt;=80,"A+",IF('Data Source'!I14&gt;=70,"A",IF('Data Source'!I14&gt;=60,"A-",IF('Data Source'!I14&gt;=50,"B",IF('Data Source'!I14&gt;=40,"C",IF('Data Source'!I14&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M14&gt;=80,"A+",IF('Data Source'!M14&gt;=70,"A",IF('Data Source'!M14&gt;=60,"A-",IF('Data Source'!M14&gt;=50,"B",IF('Data Source'!M14&gt;=40,"C",IF('Data Source'!M14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J15" s="6">
-        <f>IF('Data Source'!J14&gt;=80,"A+",IF('Data Source'!J14&gt;=70,"A",IF('Data Source'!J14&gt;=60,"A-",IF('Data Source'!J14&gt;=50,"B",IF('Data Source'!J14&gt;=40,"C",IF('Data Source'!J14&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N14&gt;=80,"A+",IF('Data Source'!N14&gt;=70,"A",IF('Data Source'!N14&gt;=60,"A-",IF('Data Source'!N14&gt;=50,"B",IF('Data Source'!N14&gt;=40,"C",IF('Data Source'!N14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K15" s="6">
-        <f>IF('Data Source'!K14&gt;=80,"A+",IF('Data Source'!K14&gt;=70,"A",IF('Data Source'!K14&gt;=60,"A-",IF('Data Source'!K14&gt;=50,"B",IF('Data Source'!K14&gt;=40,"C",IF('Data Source'!K14&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O14&gt;=80,"A+",IF('Data Source'!O14&gt;=70,"A",IF('Data Source'!O14&gt;=60,"A-",IF('Data Source'!O14&gt;=50,"B",IF('Data Source'!O14&gt;=40,"C",IF('Data Source'!O14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L15" s="6">
-        <f>IF('Data Source'!L14&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M15" s="6">
-        <f>IF('Data Source'!M14&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N15" s="5">
-        <f>'Data Source'!P14</f>
+        <f>'Data Source'!T14</f>
         <v/>
       </c>
       <c r="O15" s="6">
-        <f>'Data Source'!Q14</f>
+        <f>'Data Source'!U14</f>
         <v/>
       </c>
     </row>
@@ -3367,55 +3631,55 @@
         <v/>
       </c>
       <c r="C16" s="6">
-        <f>IF('Data Source'!C15/200*100&gt;=80,"A+",IF('Data Source'!C15/200*100&gt;=70,"A",IF('Data Source'!C15/200*100&gt;=60,"A-",IF('Data Source'!C15/200*100&gt;=50,"B",IF('Data Source'!C15/200*100&gt;=40,"C",IF('Data Source'!C15/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=80,"A+",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=70,"A",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=60,"A-",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=50,"B",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=40,"C",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D16" s="6">
-        <f>IF('Data Source'!D15/200*100&gt;=80,"A+",IF('Data Source'!D15/200*100&gt;=70,"A",IF('Data Source'!D15/200*100&gt;=60,"A-",IF('Data Source'!D15/200*100&gt;=50,"B",IF('Data Source'!D15/200*100&gt;=40,"C",IF('Data Source'!D15/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=80,"A+",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=70,"A",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=60,"A-",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=50,"B",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=40,"C",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E16" s="6">
-        <f>IF('Data Source'!E15&gt;=80,"A+",IF('Data Source'!E15&gt;=70,"A",IF('Data Source'!E15&gt;=60,"A-",IF('Data Source'!E15&gt;=50,"B",IF('Data Source'!E15&gt;=40,"C",IF('Data Source'!E15&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G15&gt;=80,"A+",IF('Data Source'!G15&gt;=70,"A",IF('Data Source'!G15&gt;=60,"A-",IF('Data Source'!G15&gt;=50,"B",IF('Data Source'!G15&gt;=40,"C",IF('Data Source'!G15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F16" s="6">
-        <f>IF('Data Source'!F15/200*100&gt;=80,"A+",IF('Data Source'!F15/200*100&gt;=70,"A",IF('Data Source'!F15/200*100&gt;=60,"A-",IF('Data Source'!F15/200*100&gt;=50,"B",IF('Data Source'!F15/200*100&gt;=40,"C",IF('Data Source'!F15/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=80,"A+",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=70,"A",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=60,"A-",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=50,"B",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=40,"C",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G16" s="6">
-        <f>IF('Data Source'!G15/200*100&gt;=80,"A+",IF('Data Source'!G15/200*100&gt;=70,"A",IF('Data Source'!G15/200*100&gt;=60,"A-",IF('Data Source'!G15/200*100&gt;=50,"B",IF('Data Source'!G15/200*100&gt;=40,"C",IF('Data Source'!G15/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=80,"A+",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=70,"A",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=60,"A-",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=50,"B",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=40,"C",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H16" s="6">
-        <f>IF('Data Source'!H15&gt;=80,"A+",IF('Data Source'!H15&gt;=70,"A",IF('Data Source'!H15&gt;=60,"A-",IF('Data Source'!H15&gt;=50,"B",IF('Data Source'!H15&gt;=40,"C",IF('Data Source'!H15&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L15&gt;=80,"A+",IF('Data Source'!L15&gt;=70,"A",IF('Data Source'!L15&gt;=60,"A-",IF('Data Source'!L15&gt;=50,"B",IF('Data Source'!L15&gt;=40,"C",IF('Data Source'!L15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I16" s="6">
-        <f>IF('Data Source'!I15&gt;=80,"A+",IF('Data Source'!I15&gt;=70,"A",IF('Data Source'!I15&gt;=60,"A-",IF('Data Source'!I15&gt;=50,"B",IF('Data Source'!I15&gt;=40,"C",IF('Data Source'!I15&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M15&gt;=80,"A+",IF('Data Source'!M15&gt;=70,"A",IF('Data Source'!M15&gt;=60,"A-",IF('Data Source'!M15&gt;=50,"B",IF('Data Source'!M15&gt;=40,"C",IF('Data Source'!M15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J16" s="6">
-        <f>IF('Data Source'!J15&gt;=80,"A+",IF('Data Source'!J15&gt;=70,"A",IF('Data Source'!J15&gt;=60,"A-",IF('Data Source'!J15&gt;=50,"B",IF('Data Source'!J15&gt;=40,"C",IF('Data Source'!J15&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N15&gt;=80,"A+",IF('Data Source'!N15&gt;=70,"A",IF('Data Source'!N15&gt;=60,"A-",IF('Data Source'!N15&gt;=50,"B",IF('Data Source'!N15&gt;=40,"C",IF('Data Source'!N15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K16" s="6">
-        <f>IF('Data Source'!K15&gt;=80,"A+",IF('Data Source'!K15&gt;=70,"A",IF('Data Source'!K15&gt;=60,"A-",IF('Data Source'!K15&gt;=50,"B",IF('Data Source'!K15&gt;=40,"C",IF('Data Source'!K15&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O15&gt;=80,"A+",IF('Data Source'!O15&gt;=70,"A",IF('Data Source'!O15&gt;=60,"A-",IF('Data Source'!O15&gt;=50,"B",IF('Data Source'!O15&gt;=40,"C",IF('Data Source'!O15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L16" s="6">
-        <f>IF('Data Source'!L15&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M16" s="6">
-        <f>IF('Data Source'!M15&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N16" s="5">
-        <f>'Data Source'!P15</f>
+        <f>'Data Source'!T15</f>
         <v/>
       </c>
       <c r="O16" s="6">
-        <f>'Data Source'!Q15</f>
+        <f>'Data Source'!U15</f>
         <v/>
       </c>
     </row>
@@ -3429,55 +3693,55 @@
         <v/>
       </c>
       <c r="C17" s="6">
-        <f>IF('Data Source'!C16/200*100&gt;=80,"A+",IF('Data Source'!C16/200*100&gt;=70,"A",IF('Data Source'!C16/200*100&gt;=60,"A-",IF('Data Source'!C16/200*100&gt;=50,"B",IF('Data Source'!C16/200*100&gt;=40,"C",IF('Data Source'!C16/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=80,"A+",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=70,"A",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=60,"A-",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=50,"B",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=40,"C",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D17" s="6">
-        <f>IF('Data Source'!D16/200*100&gt;=80,"A+",IF('Data Source'!D16/200*100&gt;=70,"A",IF('Data Source'!D16/200*100&gt;=60,"A-",IF('Data Source'!D16/200*100&gt;=50,"B",IF('Data Source'!D16/200*100&gt;=40,"C",IF('Data Source'!D16/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=80,"A+",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=70,"A",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=60,"A-",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=50,"B",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=40,"C",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E17" s="6">
-        <f>IF('Data Source'!E16&gt;=80,"A+",IF('Data Source'!E16&gt;=70,"A",IF('Data Source'!E16&gt;=60,"A-",IF('Data Source'!E16&gt;=50,"B",IF('Data Source'!E16&gt;=40,"C",IF('Data Source'!E16&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G16&gt;=80,"A+",IF('Data Source'!G16&gt;=70,"A",IF('Data Source'!G16&gt;=60,"A-",IF('Data Source'!G16&gt;=50,"B",IF('Data Source'!G16&gt;=40,"C",IF('Data Source'!G16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F17" s="6">
-        <f>IF('Data Source'!F16/200*100&gt;=80,"A+",IF('Data Source'!F16/200*100&gt;=70,"A",IF('Data Source'!F16/200*100&gt;=60,"A-",IF('Data Source'!F16/200*100&gt;=50,"B",IF('Data Source'!F16/200*100&gt;=40,"C",IF('Data Source'!F16/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=80,"A+",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=70,"A",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=60,"A-",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=50,"B",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=40,"C",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G17" s="6">
-        <f>IF('Data Source'!G16/200*100&gt;=80,"A+",IF('Data Source'!G16/200*100&gt;=70,"A",IF('Data Source'!G16/200*100&gt;=60,"A-",IF('Data Source'!G16/200*100&gt;=50,"B",IF('Data Source'!G16/200*100&gt;=40,"C",IF('Data Source'!G16/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=80,"A+",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=70,"A",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=60,"A-",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=50,"B",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=40,"C",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H17" s="6">
-        <f>IF('Data Source'!H16&gt;=80,"A+",IF('Data Source'!H16&gt;=70,"A",IF('Data Source'!H16&gt;=60,"A-",IF('Data Source'!H16&gt;=50,"B",IF('Data Source'!H16&gt;=40,"C",IF('Data Source'!H16&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L16&gt;=80,"A+",IF('Data Source'!L16&gt;=70,"A",IF('Data Source'!L16&gt;=60,"A-",IF('Data Source'!L16&gt;=50,"B",IF('Data Source'!L16&gt;=40,"C",IF('Data Source'!L16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I17" s="6">
-        <f>IF('Data Source'!I16&gt;=80,"A+",IF('Data Source'!I16&gt;=70,"A",IF('Data Source'!I16&gt;=60,"A-",IF('Data Source'!I16&gt;=50,"B",IF('Data Source'!I16&gt;=40,"C",IF('Data Source'!I16&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M16&gt;=80,"A+",IF('Data Source'!M16&gt;=70,"A",IF('Data Source'!M16&gt;=60,"A-",IF('Data Source'!M16&gt;=50,"B",IF('Data Source'!M16&gt;=40,"C",IF('Data Source'!M16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J17" s="6">
-        <f>IF('Data Source'!J16&gt;=80,"A+",IF('Data Source'!J16&gt;=70,"A",IF('Data Source'!J16&gt;=60,"A-",IF('Data Source'!J16&gt;=50,"B",IF('Data Source'!J16&gt;=40,"C",IF('Data Source'!J16&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N16&gt;=80,"A+",IF('Data Source'!N16&gt;=70,"A",IF('Data Source'!N16&gt;=60,"A-",IF('Data Source'!N16&gt;=50,"B",IF('Data Source'!N16&gt;=40,"C",IF('Data Source'!N16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K17" s="6">
-        <f>IF('Data Source'!K16&gt;=80,"A+",IF('Data Source'!K16&gt;=70,"A",IF('Data Source'!K16&gt;=60,"A-",IF('Data Source'!K16&gt;=50,"B",IF('Data Source'!K16&gt;=40,"C",IF('Data Source'!K16&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O16&gt;=80,"A+",IF('Data Source'!O16&gt;=70,"A",IF('Data Source'!O16&gt;=60,"A-",IF('Data Source'!O16&gt;=50,"B",IF('Data Source'!O16&gt;=40,"C",IF('Data Source'!O16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L17" s="6">
-        <f>IF('Data Source'!L16&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M17" s="6">
-        <f>IF('Data Source'!M16&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N17" s="5">
-        <f>'Data Source'!P16</f>
+        <f>'Data Source'!T16</f>
         <v/>
       </c>
       <c r="O17" s="6">
-        <f>'Data Source'!Q16</f>
+        <f>'Data Source'!U16</f>
         <v/>
       </c>
     </row>
@@ -3491,55 +3755,55 @@
         <v/>
       </c>
       <c r="C18" s="6">
-        <f>IF('Data Source'!C17/200*100&gt;=80,"A+",IF('Data Source'!C17/200*100&gt;=70,"A",IF('Data Source'!C17/200*100&gt;=60,"A-",IF('Data Source'!C17/200*100&gt;=50,"B",IF('Data Source'!C17/200*100&gt;=40,"C",IF('Data Source'!C17/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=80,"A+",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=70,"A",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=60,"A-",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=50,"B",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=40,"C",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D18" s="6">
-        <f>IF('Data Source'!D17/200*100&gt;=80,"A+",IF('Data Source'!D17/200*100&gt;=70,"A",IF('Data Source'!D17/200*100&gt;=60,"A-",IF('Data Source'!D17/200*100&gt;=50,"B",IF('Data Source'!D17/200*100&gt;=40,"C",IF('Data Source'!D17/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=80,"A+",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=70,"A",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=60,"A-",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=50,"B",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=40,"C",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E18" s="6">
-        <f>IF('Data Source'!E17&gt;=80,"A+",IF('Data Source'!E17&gt;=70,"A",IF('Data Source'!E17&gt;=60,"A-",IF('Data Source'!E17&gt;=50,"B",IF('Data Source'!E17&gt;=40,"C",IF('Data Source'!E17&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G17&gt;=80,"A+",IF('Data Source'!G17&gt;=70,"A",IF('Data Source'!G17&gt;=60,"A-",IF('Data Source'!G17&gt;=50,"B",IF('Data Source'!G17&gt;=40,"C",IF('Data Source'!G17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F18" s="6">
-        <f>IF('Data Source'!F17/200*100&gt;=80,"A+",IF('Data Source'!F17/200*100&gt;=70,"A",IF('Data Source'!F17/200*100&gt;=60,"A-",IF('Data Source'!F17/200*100&gt;=50,"B",IF('Data Source'!F17/200*100&gt;=40,"C",IF('Data Source'!F17/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=80,"A+",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=70,"A",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=60,"A-",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=50,"B",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=40,"C",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G18" s="6">
-        <f>IF('Data Source'!G17/200*100&gt;=80,"A+",IF('Data Source'!G17/200*100&gt;=70,"A",IF('Data Source'!G17/200*100&gt;=60,"A-",IF('Data Source'!G17/200*100&gt;=50,"B",IF('Data Source'!G17/200*100&gt;=40,"C",IF('Data Source'!G17/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=80,"A+",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=70,"A",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=60,"A-",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=50,"B",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=40,"C",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H18" s="6">
-        <f>IF('Data Source'!H17&gt;=80,"A+",IF('Data Source'!H17&gt;=70,"A",IF('Data Source'!H17&gt;=60,"A-",IF('Data Source'!H17&gt;=50,"B",IF('Data Source'!H17&gt;=40,"C",IF('Data Source'!H17&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L17&gt;=80,"A+",IF('Data Source'!L17&gt;=70,"A",IF('Data Source'!L17&gt;=60,"A-",IF('Data Source'!L17&gt;=50,"B",IF('Data Source'!L17&gt;=40,"C",IF('Data Source'!L17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I18" s="6">
-        <f>IF('Data Source'!I17&gt;=80,"A+",IF('Data Source'!I17&gt;=70,"A",IF('Data Source'!I17&gt;=60,"A-",IF('Data Source'!I17&gt;=50,"B",IF('Data Source'!I17&gt;=40,"C",IF('Data Source'!I17&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M17&gt;=80,"A+",IF('Data Source'!M17&gt;=70,"A",IF('Data Source'!M17&gt;=60,"A-",IF('Data Source'!M17&gt;=50,"B",IF('Data Source'!M17&gt;=40,"C",IF('Data Source'!M17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J18" s="6">
-        <f>IF('Data Source'!J17&gt;=80,"A+",IF('Data Source'!J17&gt;=70,"A",IF('Data Source'!J17&gt;=60,"A-",IF('Data Source'!J17&gt;=50,"B",IF('Data Source'!J17&gt;=40,"C",IF('Data Source'!J17&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N17&gt;=80,"A+",IF('Data Source'!N17&gt;=70,"A",IF('Data Source'!N17&gt;=60,"A-",IF('Data Source'!N17&gt;=50,"B",IF('Data Source'!N17&gt;=40,"C",IF('Data Source'!N17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K18" s="6">
-        <f>IF('Data Source'!K17&gt;=80,"A+",IF('Data Source'!K17&gt;=70,"A",IF('Data Source'!K17&gt;=60,"A-",IF('Data Source'!K17&gt;=50,"B",IF('Data Source'!K17&gt;=40,"C",IF('Data Source'!K17&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O17&gt;=80,"A+",IF('Data Source'!O17&gt;=70,"A",IF('Data Source'!O17&gt;=60,"A-",IF('Data Source'!O17&gt;=50,"B",IF('Data Source'!O17&gt;=40,"C",IF('Data Source'!O17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L18" s="6">
-        <f>IF('Data Source'!L17&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M18" s="6">
-        <f>IF('Data Source'!M17&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N18" s="5">
-        <f>'Data Source'!P17</f>
+        <f>'Data Source'!T17</f>
         <v/>
       </c>
       <c r="O18" s="6">
-        <f>'Data Source'!Q17</f>
+        <f>'Data Source'!U17</f>
         <v/>
       </c>
     </row>
@@ -3553,55 +3817,55 @@
         <v/>
       </c>
       <c r="C19" s="6">
-        <f>IF('Data Source'!C18/200*100&gt;=80,"A+",IF('Data Source'!C18/200*100&gt;=70,"A",IF('Data Source'!C18/200*100&gt;=60,"A-",IF('Data Source'!C18/200*100&gt;=50,"B",IF('Data Source'!C18/200*100&gt;=40,"C",IF('Data Source'!C18/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=80,"A+",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=70,"A",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=60,"A-",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=50,"B",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=40,"C",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D19" s="6">
-        <f>IF('Data Source'!D18/200*100&gt;=80,"A+",IF('Data Source'!D18/200*100&gt;=70,"A",IF('Data Source'!D18/200*100&gt;=60,"A-",IF('Data Source'!D18/200*100&gt;=50,"B",IF('Data Source'!D18/200*100&gt;=40,"C",IF('Data Source'!D18/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=80,"A+",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=70,"A",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=60,"A-",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=50,"B",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=40,"C",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E19" s="6">
-        <f>IF('Data Source'!E18&gt;=80,"A+",IF('Data Source'!E18&gt;=70,"A",IF('Data Source'!E18&gt;=60,"A-",IF('Data Source'!E18&gt;=50,"B",IF('Data Source'!E18&gt;=40,"C",IF('Data Source'!E18&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G18&gt;=80,"A+",IF('Data Source'!G18&gt;=70,"A",IF('Data Source'!G18&gt;=60,"A-",IF('Data Source'!G18&gt;=50,"B",IF('Data Source'!G18&gt;=40,"C",IF('Data Source'!G18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F19" s="6">
-        <f>IF('Data Source'!F18/200*100&gt;=80,"A+",IF('Data Source'!F18/200*100&gt;=70,"A",IF('Data Source'!F18/200*100&gt;=60,"A-",IF('Data Source'!F18/200*100&gt;=50,"B",IF('Data Source'!F18/200*100&gt;=40,"C",IF('Data Source'!F18/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=80,"A+",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=70,"A",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=60,"A-",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=50,"B",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=40,"C",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G19" s="6">
-        <f>IF('Data Source'!G18/200*100&gt;=80,"A+",IF('Data Source'!G18/200*100&gt;=70,"A",IF('Data Source'!G18/200*100&gt;=60,"A-",IF('Data Source'!G18/200*100&gt;=50,"B",IF('Data Source'!G18/200*100&gt;=40,"C",IF('Data Source'!G18/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=80,"A+",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=70,"A",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=60,"A-",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=50,"B",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=40,"C",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H19" s="6">
-        <f>IF('Data Source'!H18&gt;=80,"A+",IF('Data Source'!H18&gt;=70,"A",IF('Data Source'!H18&gt;=60,"A-",IF('Data Source'!H18&gt;=50,"B",IF('Data Source'!H18&gt;=40,"C",IF('Data Source'!H18&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L18&gt;=80,"A+",IF('Data Source'!L18&gt;=70,"A",IF('Data Source'!L18&gt;=60,"A-",IF('Data Source'!L18&gt;=50,"B",IF('Data Source'!L18&gt;=40,"C",IF('Data Source'!L18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I19" s="6">
-        <f>IF('Data Source'!I18&gt;=80,"A+",IF('Data Source'!I18&gt;=70,"A",IF('Data Source'!I18&gt;=60,"A-",IF('Data Source'!I18&gt;=50,"B",IF('Data Source'!I18&gt;=40,"C",IF('Data Source'!I18&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M18&gt;=80,"A+",IF('Data Source'!M18&gt;=70,"A",IF('Data Source'!M18&gt;=60,"A-",IF('Data Source'!M18&gt;=50,"B",IF('Data Source'!M18&gt;=40,"C",IF('Data Source'!M18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J19" s="6">
-        <f>IF('Data Source'!J18&gt;=80,"A+",IF('Data Source'!J18&gt;=70,"A",IF('Data Source'!J18&gt;=60,"A-",IF('Data Source'!J18&gt;=50,"B",IF('Data Source'!J18&gt;=40,"C",IF('Data Source'!J18&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N18&gt;=80,"A+",IF('Data Source'!N18&gt;=70,"A",IF('Data Source'!N18&gt;=60,"A-",IF('Data Source'!N18&gt;=50,"B",IF('Data Source'!N18&gt;=40,"C",IF('Data Source'!N18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K19" s="6">
-        <f>IF('Data Source'!K18&gt;=80,"A+",IF('Data Source'!K18&gt;=70,"A",IF('Data Source'!K18&gt;=60,"A-",IF('Data Source'!K18&gt;=50,"B",IF('Data Source'!K18&gt;=40,"C",IF('Data Source'!K18&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O18&gt;=80,"A+",IF('Data Source'!O18&gt;=70,"A",IF('Data Source'!O18&gt;=60,"A-",IF('Data Source'!O18&gt;=50,"B",IF('Data Source'!O18&gt;=40,"C",IF('Data Source'!O18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L19" s="6">
-        <f>IF('Data Source'!L18&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M19" s="6">
-        <f>IF('Data Source'!M18&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N19" s="5">
-        <f>'Data Source'!P18</f>
+        <f>'Data Source'!T18</f>
         <v/>
       </c>
       <c r="O19" s="6">
-        <f>'Data Source'!Q18</f>
+        <f>'Data Source'!U18</f>
         <v/>
       </c>
     </row>
@@ -3615,55 +3879,55 @@
         <v/>
       </c>
       <c r="C20" s="6">
-        <f>IF('Data Source'!C19/200*100&gt;=80,"A+",IF('Data Source'!C19/200*100&gt;=70,"A",IF('Data Source'!C19/200*100&gt;=60,"A-",IF('Data Source'!C19/200*100&gt;=50,"B",IF('Data Source'!C19/200*100&gt;=40,"C",IF('Data Source'!C19/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=80,"A+",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=70,"A",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=60,"A-",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=50,"B",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=40,"C",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D20" s="6">
-        <f>IF('Data Source'!D19/200*100&gt;=80,"A+",IF('Data Source'!D19/200*100&gt;=70,"A",IF('Data Source'!D19/200*100&gt;=60,"A-",IF('Data Source'!D19/200*100&gt;=50,"B",IF('Data Source'!D19/200*100&gt;=40,"C",IF('Data Source'!D19/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=80,"A+",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=70,"A",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=60,"A-",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=50,"B",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=40,"C",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E20" s="6">
-        <f>IF('Data Source'!E19&gt;=80,"A+",IF('Data Source'!E19&gt;=70,"A",IF('Data Source'!E19&gt;=60,"A-",IF('Data Source'!E19&gt;=50,"B",IF('Data Source'!E19&gt;=40,"C",IF('Data Source'!E19&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G19&gt;=80,"A+",IF('Data Source'!G19&gt;=70,"A",IF('Data Source'!G19&gt;=60,"A-",IF('Data Source'!G19&gt;=50,"B",IF('Data Source'!G19&gt;=40,"C",IF('Data Source'!G19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F20" s="6">
-        <f>IF('Data Source'!F19/200*100&gt;=80,"A+",IF('Data Source'!F19/200*100&gt;=70,"A",IF('Data Source'!F19/200*100&gt;=60,"A-",IF('Data Source'!F19/200*100&gt;=50,"B",IF('Data Source'!F19/200*100&gt;=40,"C",IF('Data Source'!F19/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=80,"A+",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=70,"A",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=60,"A-",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=50,"B",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=40,"C",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G20" s="6">
-        <f>IF('Data Source'!G19/200*100&gt;=80,"A+",IF('Data Source'!G19/200*100&gt;=70,"A",IF('Data Source'!G19/200*100&gt;=60,"A-",IF('Data Source'!G19/200*100&gt;=50,"B",IF('Data Source'!G19/200*100&gt;=40,"C",IF('Data Source'!G19/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=80,"A+",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=70,"A",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=60,"A-",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=50,"B",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=40,"C",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H20" s="6">
-        <f>IF('Data Source'!H19&gt;=80,"A+",IF('Data Source'!H19&gt;=70,"A",IF('Data Source'!H19&gt;=60,"A-",IF('Data Source'!H19&gt;=50,"B",IF('Data Source'!H19&gt;=40,"C",IF('Data Source'!H19&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L19&gt;=80,"A+",IF('Data Source'!L19&gt;=70,"A",IF('Data Source'!L19&gt;=60,"A-",IF('Data Source'!L19&gt;=50,"B",IF('Data Source'!L19&gt;=40,"C",IF('Data Source'!L19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I20" s="6">
-        <f>IF('Data Source'!I19&gt;=80,"A+",IF('Data Source'!I19&gt;=70,"A",IF('Data Source'!I19&gt;=60,"A-",IF('Data Source'!I19&gt;=50,"B",IF('Data Source'!I19&gt;=40,"C",IF('Data Source'!I19&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M19&gt;=80,"A+",IF('Data Source'!M19&gt;=70,"A",IF('Data Source'!M19&gt;=60,"A-",IF('Data Source'!M19&gt;=50,"B",IF('Data Source'!M19&gt;=40,"C",IF('Data Source'!M19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J20" s="6">
-        <f>IF('Data Source'!J19&gt;=80,"A+",IF('Data Source'!J19&gt;=70,"A",IF('Data Source'!J19&gt;=60,"A-",IF('Data Source'!J19&gt;=50,"B",IF('Data Source'!J19&gt;=40,"C",IF('Data Source'!J19&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N19&gt;=80,"A+",IF('Data Source'!N19&gt;=70,"A",IF('Data Source'!N19&gt;=60,"A-",IF('Data Source'!N19&gt;=50,"B",IF('Data Source'!N19&gt;=40,"C",IF('Data Source'!N19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K20" s="6">
-        <f>IF('Data Source'!K19&gt;=80,"A+",IF('Data Source'!K19&gt;=70,"A",IF('Data Source'!K19&gt;=60,"A-",IF('Data Source'!K19&gt;=50,"B",IF('Data Source'!K19&gt;=40,"C",IF('Data Source'!K19&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O19&gt;=80,"A+",IF('Data Source'!O19&gt;=70,"A",IF('Data Source'!O19&gt;=60,"A-",IF('Data Source'!O19&gt;=50,"B",IF('Data Source'!O19&gt;=40,"C",IF('Data Source'!O19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L20" s="6">
-        <f>IF('Data Source'!L19&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M20" s="6">
-        <f>IF('Data Source'!M19&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N20" s="5">
-        <f>'Data Source'!P19</f>
+        <f>'Data Source'!T19</f>
         <v/>
       </c>
       <c r="O20" s="6">
-        <f>'Data Source'!Q19</f>
+        <f>'Data Source'!U19</f>
         <v/>
       </c>
     </row>
@@ -3677,55 +3941,55 @@
         <v/>
       </c>
       <c r="C21" s="6">
-        <f>IF('Data Source'!C20/200*100&gt;=80,"A+",IF('Data Source'!C20/200*100&gt;=70,"A",IF('Data Source'!C20/200*100&gt;=60,"A-",IF('Data Source'!C20/200*100&gt;=50,"B",IF('Data Source'!C20/200*100&gt;=40,"C",IF('Data Source'!C20/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=80,"A+",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=70,"A",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=60,"A-",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=50,"B",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=40,"C",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D21" s="6">
-        <f>IF('Data Source'!D20/200*100&gt;=80,"A+",IF('Data Source'!D20/200*100&gt;=70,"A",IF('Data Source'!D20/200*100&gt;=60,"A-",IF('Data Source'!D20/200*100&gt;=50,"B",IF('Data Source'!D20/200*100&gt;=40,"C",IF('Data Source'!D20/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=80,"A+",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=70,"A",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=60,"A-",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=50,"B",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=40,"C",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E21" s="6">
-        <f>IF('Data Source'!E20&gt;=80,"A+",IF('Data Source'!E20&gt;=70,"A",IF('Data Source'!E20&gt;=60,"A-",IF('Data Source'!E20&gt;=50,"B",IF('Data Source'!E20&gt;=40,"C",IF('Data Source'!E20&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G20&gt;=80,"A+",IF('Data Source'!G20&gt;=70,"A",IF('Data Source'!G20&gt;=60,"A-",IF('Data Source'!G20&gt;=50,"B",IF('Data Source'!G20&gt;=40,"C",IF('Data Source'!G20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F21" s="6">
-        <f>IF('Data Source'!F20/200*100&gt;=80,"A+",IF('Data Source'!F20/200*100&gt;=70,"A",IF('Data Source'!F20/200*100&gt;=60,"A-",IF('Data Source'!F20/200*100&gt;=50,"B",IF('Data Source'!F20/200*100&gt;=40,"C",IF('Data Source'!F20/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=80,"A+",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=70,"A",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=60,"A-",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=50,"B",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=40,"C",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G21" s="6">
-        <f>IF('Data Source'!G20/200*100&gt;=80,"A+",IF('Data Source'!G20/200*100&gt;=70,"A",IF('Data Source'!G20/200*100&gt;=60,"A-",IF('Data Source'!G20/200*100&gt;=50,"B",IF('Data Source'!G20/200*100&gt;=40,"C",IF('Data Source'!G20/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=80,"A+",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=70,"A",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=60,"A-",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=50,"B",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=40,"C",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H21" s="6">
-        <f>IF('Data Source'!H20&gt;=80,"A+",IF('Data Source'!H20&gt;=70,"A",IF('Data Source'!H20&gt;=60,"A-",IF('Data Source'!H20&gt;=50,"B",IF('Data Source'!H20&gt;=40,"C",IF('Data Source'!H20&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L20&gt;=80,"A+",IF('Data Source'!L20&gt;=70,"A",IF('Data Source'!L20&gt;=60,"A-",IF('Data Source'!L20&gt;=50,"B",IF('Data Source'!L20&gt;=40,"C",IF('Data Source'!L20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I21" s="6">
-        <f>IF('Data Source'!I20&gt;=80,"A+",IF('Data Source'!I20&gt;=70,"A",IF('Data Source'!I20&gt;=60,"A-",IF('Data Source'!I20&gt;=50,"B",IF('Data Source'!I20&gt;=40,"C",IF('Data Source'!I20&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M20&gt;=80,"A+",IF('Data Source'!M20&gt;=70,"A",IF('Data Source'!M20&gt;=60,"A-",IF('Data Source'!M20&gt;=50,"B",IF('Data Source'!M20&gt;=40,"C",IF('Data Source'!M20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J21" s="6">
-        <f>IF('Data Source'!J20&gt;=80,"A+",IF('Data Source'!J20&gt;=70,"A",IF('Data Source'!J20&gt;=60,"A-",IF('Data Source'!J20&gt;=50,"B",IF('Data Source'!J20&gt;=40,"C",IF('Data Source'!J20&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N20&gt;=80,"A+",IF('Data Source'!N20&gt;=70,"A",IF('Data Source'!N20&gt;=60,"A-",IF('Data Source'!N20&gt;=50,"B",IF('Data Source'!N20&gt;=40,"C",IF('Data Source'!N20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K21" s="6">
-        <f>IF('Data Source'!K20&gt;=80,"A+",IF('Data Source'!K20&gt;=70,"A",IF('Data Source'!K20&gt;=60,"A-",IF('Data Source'!K20&gt;=50,"B",IF('Data Source'!K20&gt;=40,"C",IF('Data Source'!K20&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O20&gt;=80,"A+",IF('Data Source'!O20&gt;=70,"A",IF('Data Source'!O20&gt;=60,"A-",IF('Data Source'!O20&gt;=50,"B",IF('Data Source'!O20&gt;=40,"C",IF('Data Source'!O20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L21" s="6">
-        <f>IF('Data Source'!L20&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M21" s="6">
-        <f>IF('Data Source'!M20&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N21" s="5">
-        <f>'Data Source'!P20</f>
+        <f>'Data Source'!T20</f>
         <v/>
       </c>
       <c r="O21" s="6">
-        <f>'Data Source'!Q20</f>
+        <f>'Data Source'!U20</f>
         <v/>
       </c>
     </row>
@@ -3739,55 +4003,55 @@
         <v/>
       </c>
       <c r="C22" s="6">
-        <f>IF('Data Source'!C21/200*100&gt;=80,"A+",IF('Data Source'!C21/200*100&gt;=70,"A",IF('Data Source'!C21/200*100&gt;=60,"A-",IF('Data Source'!C21/200*100&gt;=50,"B",IF('Data Source'!C21/200*100&gt;=40,"C",IF('Data Source'!C21/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=80,"A+",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=70,"A",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=60,"A-",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=50,"B",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=40,"C",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D22" s="6">
-        <f>IF('Data Source'!D21/200*100&gt;=80,"A+",IF('Data Source'!D21/200*100&gt;=70,"A",IF('Data Source'!D21/200*100&gt;=60,"A-",IF('Data Source'!D21/200*100&gt;=50,"B",IF('Data Source'!D21/200*100&gt;=40,"C",IF('Data Source'!D21/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=80,"A+",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=70,"A",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=60,"A-",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=50,"B",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=40,"C",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E22" s="6">
-        <f>IF('Data Source'!E21&gt;=80,"A+",IF('Data Source'!E21&gt;=70,"A",IF('Data Source'!E21&gt;=60,"A-",IF('Data Source'!E21&gt;=50,"B",IF('Data Source'!E21&gt;=40,"C",IF('Data Source'!E21&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!G21&gt;=80,"A+",IF('Data Source'!G21&gt;=70,"A",IF('Data Source'!G21&gt;=60,"A-",IF('Data Source'!G21&gt;=50,"B",IF('Data Source'!G21&gt;=40,"C",IF('Data Source'!G21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F22" s="6">
-        <f>IF('Data Source'!F21/200*100&gt;=80,"A+",IF('Data Source'!F21/200*100&gt;=70,"A",IF('Data Source'!F21/200*100&gt;=60,"A-",IF('Data Source'!F21/200*100&gt;=50,"B",IF('Data Source'!F21/200*100&gt;=40,"C",IF('Data Source'!F21/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=80,"A+",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=70,"A",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=60,"A-",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=50,"B",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=40,"C",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G22" s="6">
-        <f>IF('Data Source'!G21/200*100&gt;=80,"A+",IF('Data Source'!G21/200*100&gt;=70,"A",IF('Data Source'!G21/200*100&gt;=60,"A-",IF('Data Source'!G21/200*100&gt;=50,"B",IF('Data Source'!G21/200*100&gt;=40,"C",IF('Data Source'!G21/200*100&gt;=33,"D","F"))))))</f>
+        <f>IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=80,"A+",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=70,"A",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=60,"A-",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=50,"B",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=40,"C",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H22" s="6">
-        <f>IF('Data Source'!H21&gt;=80,"A+",IF('Data Source'!H21&gt;=70,"A",IF('Data Source'!H21&gt;=60,"A-",IF('Data Source'!H21&gt;=50,"B",IF('Data Source'!H21&gt;=40,"C",IF('Data Source'!H21&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!L21&gt;=80,"A+",IF('Data Source'!L21&gt;=70,"A",IF('Data Source'!L21&gt;=60,"A-",IF('Data Source'!L21&gt;=50,"B",IF('Data Source'!L21&gt;=40,"C",IF('Data Source'!L21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I22" s="6">
-        <f>IF('Data Source'!I21&gt;=80,"A+",IF('Data Source'!I21&gt;=70,"A",IF('Data Source'!I21&gt;=60,"A-",IF('Data Source'!I21&gt;=50,"B",IF('Data Source'!I21&gt;=40,"C",IF('Data Source'!I21&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!M21&gt;=80,"A+",IF('Data Source'!M21&gt;=70,"A",IF('Data Source'!M21&gt;=60,"A-",IF('Data Source'!M21&gt;=50,"B",IF('Data Source'!M21&gt;=40,"C",IF('Data Source'!M21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J22" s="6">
-        <f>IF('Data Source'!J21&gt;=80,"A+",IF('Data Source'!J21&gt;=70,"A",IF('Data Source'!J21&gt;=60,"A-",IF('Data Source'!J21&gt;=50,"B",IF('Data Source'!J21&gt;=40,"C",IF('Data Source'!J21&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!N21&gt;=80,"A+",IF('Data Source'!N21&gt;=70,"A",IF('Data Source'!N21&gt;=60,"A-",IF('Data Source'!N21&gt;=50,"B",IF('Data Source'!N21&gt;=40,"C",IF('Data Source'!N21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K22" s="6">
-        <f>IF('Data Source'!K21&gt;=80,"A+",IF('Data Source'!K21&gt;=70,"A",IF('Data Source'!K21&gt;=60,"A-",IF('Data Source'!K21&gt;=50,"B",IF('Data Source'!K21&gt;=40,"C",IF('Data Source'!K21&gt;=33,"D","F"))))))</f>
+        <f>IF('Data Source'!O21&gt;=80,"A+",IF('Data Source'!O21&gt;=70,"A",IF('Data Source'!O21&gt;=60,"A-",IF('Data Source'!O21&gt;=50,"B",IF('Data Source'!O21&gt;=40,"C",IF('Data Source'!O21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L22" s="6">
-        <f>IF('Data Source'!L21&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!P21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="M22" s="6">
-        <f>IF('Data Source'!M21&gt;=33,"Pass","Fail")</f>
+        <f>IF('Data Source'!Q21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
       <c r="N22" s="5">
-        <f>'Data Source'!P21</f>
+        <f>'Data Source'!T21</f>
         <v/>
       </c>
       <c r="O22" s="6">
-        <f>'Data Source'!Q21</f>
+        <f>'Data Source'!U21</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ICT grading logic to reflect new marking scheme and adjust GPA calculations
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -67,7 +67,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -100,6 +100,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FC9999"/>
+        <bgColor rgb="00FC9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
       </patternFill>
@@ -123,13 +129,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -137,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -153,10 +160,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -922,31 +929,31 @@
       <c r="M2" s="3" t="n">
         <v>89</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>65</v>
+      <c r="N2" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="P2" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="Q2" s="3" t="n">
-        <v>83</v>
+      <c r="Q2" s="2" t="n">
+        <v>76</v>
       </c>
       <c r="R2">
         <f>SUM(C2:N2)</f>
         <v/>
       </c>
-      <c r="S2" s="4">
-        <f>ROUND(R2/12,2)</f>
-        <v/>
-      </c>
-      <c r="T2" s="5">
-        <f>IF(OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,(J2+K2)&lt;66,L2&lt;33,M2&lt;33,N2&lt;33,P2&lt;33,Q2&lt;33),0,MIN(5,ROUND((IF((C2+D2)/200*100&gt;=80,5,IF((C2+D2)/200*100&gt;=70,4,IF((C2+D2)/200*100&gt;=60,3.5,IF((C2+D2)/200*100&gt;=50,3,IF((C2+D2)/200*100&gt;=40,2,IF((C2+D2)/200*100&gt;=33,1,0))))))+IF((E2+F2)/200*100&gt;=80,5,IF((E2+F2)/200*100&gt;=70,4,IF((E2+F2)/200*100&gt;=60,3.5,IF((E2+F2)/200*100&gt;=50,3,IF((E2+F2)/200*100&gt;=40,2,IF((E2+F2)/200*100&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF((H2+I2)/200*100&gt;=80,5,IF((H2+I2)/200*100&gt;=70,4,IF((H2+I2)/200*100&gt;=60,3.5,IF((H2+I2)/200*100&gt;=50,3,IF((H2+I2)/200*100&gt;=40,2,IF((H2+I2)/200*100&gt;=33,1,0))))))+IF((J2+K2)/200*100&gt;=80,5,IF((J2+K2)/200*100&gt;=70,4,IF((J2+K2)/200*100&gt;=60,3.5,IF((J2+K2)/200*100&gt;=50,3,IF((J2+K2)/200*100&gt;=40,2,IF((J2+K2)/200*100&gt;=33,1,0))))))+IF(L2&gt;=80,5,IF(L2&gt;=70,4,IF(L2&gt;=60,3.5,IF(L2&gt;=50,3,IF(L2&gt;=40,2,IF(L2&gt;=33,1,0))))))+IF(M2&gt;=80,5,IF(M2&gt;=70,4,IF(M2&gt;=60,3.5,IF(M2&gt;=50,3,IF(M2&gt;=40,2,IF(M2&gt;=33,1,0))))))+IF(N2&gt;=80,5,IF(N2&gt;=70,4,IF(N2&gt;=60,3.5,IF(N2&gt;=50,3,IF(N2&gt;=40,2,IF(N2&gt;=33,1,0)))))))/8+IF(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))&gt;=2,(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U2" s="6">
+      <c r="S2" s="5">
+        <f>ROUND(R2/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T2" s="6">
+        <f>IF(OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,(J2+K2)&lt;66,L2&lt;33,M2&lt;33,N2&lt;8.25,P2&lt;33,Q2&lt;33),0,MIN(5,ROUND((IF((C2+D2)/200*100&gt;=80,5,IF((C2+D2)/200*100&gt;=70,4,IF((C2+D2)/200*100&gt;=60,3.5,IF((C2+D2)/200*100&gt;=50,3,IF((C2+D2)/200*100&gt;=40,2,IF((C2+D2)/200*100&gt;=33,1,0))))))+IF((E2+F2)/200*100&gt;=80,5,IF((E2+F2)/200*100&gt;=70,4,IF((E2+F2)/200*100&gt;=60,3.5,IF((E2+F2)/200*100&gt;=50,3,IF((E2+F2)/200*100&gt;=40,2,IF((E2+F2)/200*100&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF((H2+I2)/200*100&gt;=80,5,IF((H2+I2)/200*100&gt;=70,4,IF((H2+I2)/200*100&gt;=60,3.5,IF((H2+I2)/200*100&gt;=50,3,IF((H2+I2)/200*100&gt;=40,2,IF((H2+I2)/200*100&gt;=33,1,0))))))+IF((J2+K2)/200*100&gt;=80,5,IF((J2+K2)/200*100&gt;=70,4,IF((J2+K2)/200*100&gt;=60,3.5,IF((J2+K2)/200*100&gt;=50,3,IF((J2+K2)/200*100&gt;=40,2,IF((J2+K2)/200*100&gt;=33,1,0))))))+IF(L2&gt;=80,5,IF(L2&gt;=70,4,IF(L2&gt;=60,3.5,IF(L2&gt;=50,3,IF(L2&gt;=40,2,IF(L2&gt;=33,1,0))))))+IF(M2&gt;=80,5,IF(M2&gt;=70,4,IF(M2&gt;=60,3.5,IF(M2&gt;=50,3,IF(M2&gt;=40,2,IF(M2&gt;=33,1,0))))))+IF(N2/50*100&gt;=80,5,IF(N2/50*100&gt;=70,4,IF(N2/50*100&gt;=60,3.5,IF(N2/50*100&gt;=50,3,IF(N2/50*100&gt;=40,2,IF(N2/50*100&gt;=33,1,0)))))))/8+IF(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))&gt;=2,(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U2" s="7">
         <f>IF(T2&gt;=5,"A+",IF(T2&gt;=4,"A",IF(T2&gt;=3.5,"A-",IF(T2&gt;=3,"B",IF(T2&gt;=2,"C",IF(T2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -993,31 +1000,31 @@
       <c r="M3" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="N3" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>71</v>
+      <c r="N3" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <v>58</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>80</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="R3">
         <f>SUM(C3:N3)</f>
         <v/>
       </c>
-      <c r="S3" s="4">
-        <f>ROUND(R3/12,2)</f>
-        <v/>
-      </c>
-      <c r="T3" s="5">
-        <f>IF(OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,(J3+K3)&lt;66,L3&lt;33,M3&lt;33,N3&lt;33,P3&lt;33,Q3&lt;33),0,MIN(5,ROUND((IF((C3+D3)/200*100&gt;=80,5,IF((C3+D3)/200*100&gt;=70,4,IF((C3+D3)/200*100&gt;=60,3.5,IF((C3+D3)/200*100&gt;=50,3,IF((C3+D3)/200*100&gt;=40,2,IF((C3+D3)/200*100&gt;=33,1,0))))))+IF((E3+F3)/200*100&gt;=80,5,IF((E3+F3)/200*100&gt;=70,4,IF((E3+F3)/200*100&gt;=60,3.5,IF((E3+F3)/200*100&gt;=50,3,IF((E3+F3)/200*100&gt;=40,2,IF((E3+F3)/200*100&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF((H3+I3)/200*100&gt;=80,5,IF((H3+I3)/200*100&gt;=70,4,IF((H3+I3)/200*100&gt;=60,3.5,IF((H3+I3)/200*100&gt;=50,3,IF((H3+I3)/200*100&gt;=40,2,IF((H3+I3)/200*100&gt;=33,1,0))))))+IF((J3+K3)/200*100&gt;=80,5,IF((J3+K3)/200*100&gt;=70,4,IF((J3+K3)/200*100&gt;=60,3.5,IF((J3+K3)/200*100&gt;=50,3,IF((J3+K3)/200*100&gt;=40,2,IF((J3+K3)/200*100&gt;=33,1,0))))))+IF(L3&gt;=80,5,IF(L3&gt;=70,4,IF(L3&gt;=60,3.5,IF(L3&gt;=50,3,IF(L3&gt;=40,2,IF(L3&gt;=33,1,0))))))+IF(M3&gt;=80,5,IF(M3&gt;=70,4,IF(M3&gt;=60,3.5,IF(M3&gt;=50,3,IF(M3&gt;=40,2,IF(M3&gt;=33,1,0))))))+IF(N3&gt;=80,5,IF(N3&gt;=70,4,IF(N3&gt;=60,3.5,IF(N3&gt;=50,3,IF(N3&gt;=40,2,IF(N3&gt;=33,1,0)))))))/8+IF(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))&gt;=2,(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U3" s="6">
+      <c r="S3" s="5">
+        <f>ROUND(R3/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T3" s="6">
+        <f>IF(OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,(J3+K3)&lt;66,L3&lt;33,M3&lt;33,N3&lt;8.25,P3&lt;33,Q3&lt;33),0,MIN(5,ROUND((IF((C3+D3)/200*100&gt;=80,5,IF((C3+D3)/200*100&gt;=70,4,IF((C3+D3)/200*100&gt;=60,3.5,IF((C3+D3)/200*100&gt;=50,3,IF((C3+D3)/200*100&gt;=40,2,IF((C3+D3)/200*100&gt;=33,1,0))))))+IF((E3+F3)/200*100&gt;=80,5,IF((E3+F3)/200*100&gt;=70,4,IF((E3+F3)/200*100&gt;=60,3.5,IF((E3+F3)/200*100&gt;=50,3,IF((E3+F3)/200*100&gt;=40,2,IF((E3+F3)/200*100&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF((H3+I3)/200*100&gt;=80,5,IF((H3+I3)/200*100&gt;=70,4,IF((H3+I3)/200*100&gt;=60,3.5,IF((H3+I3)/200*100&gt;=50,3,IF((H3+I3)/200*100&gt;=40,2,IF((H3+I3)/200*100&gt;=33,1,0))))))+IF((J3+K3)/200*100&gt;=80,5,IF((J3+K3)/200*100&gt;=70,4,IF((J3+K3)/200*100&gt;=60,3.5,IF((J3+K3)/200*100&gt;=50,3,IF((J3+K3)/200*100&gt;=40,2,IF((J3+K3)/200*100&gt;=33,1,0))))))+IF(L3&gt;=80,5,IF(L3&gt;=70,4,IF(L3&gt;=60,3.5,IF(L3&gt;=50,3,IF(L3&gt;=40,2,IF(L3&gt;=33,1,0))))))+IF(M3&gt;=80,5,IF(M3&gt;=70,4,IF(M3&gt;=60,3.5,IF(M3&gt;=50,3,IF(M3&gt;=40,2,IF(M3&gt;=33,1,0))))))+IF(N3/50*100&gt;=80,5,IF(N3/50*100&gt;=70,4,IF(N3/50*100&gt;=60,3.5,IF(N3/50*100&gt;=50,3,IF(N3/50*100&gt;=40,2,IF(N3/50*100&gt;=33,1,0)))))))/8+IF(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))&gt;=2,(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U3" s="7">
         <f>IF(T3&gt;=5,"A+",IF(T3&gt;=4,"A",IF(T3&gt;=3.5,"A-",IF(T3&gt;=3,"B",IF(T3&gt;=2,"C",IF(T3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1058,37 +1065,37 @@
       <c r="K4" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="L4" s="7" t="n">
+      <c r="L4" s="4" t="n">
         <v>58</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>84</v>
       </c>
-      <c r="N4" s="3" t="n">
-        <v>83</v>
+      <c r="N4" s="4" t="n">
+        <v>48</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="R4">
         <f>SUM(C4:N4)</f>
         <v/>
       </c>
-      <c r="S4" s="4">
-        <f>ROUND(R4/12,2)</f>
-        <v/>
-      </c>
-      <c r="T4" s="5">
-        <f>IF(OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,(J4+K4)&lt;66,L4&lt;33,M4&lt;33,N4&lt;33,P4&lt;33,Q4&lt;33),0,MIN(5,ROUND((IF((C4+D4)/200*100&gt;=80,5,IF((C4+D4)/200*100&gt;=70,4,IF((C4+D4)/200*100&gt;=60,3.5,IF((C4+D4)/200*100&gt;=50,3,IF((C4+D4)/200*100&gt;=40,2,IF((C4+D4)/200*100&gt;=33,1,0))))))+IF((E4+F4)/200*100&gt;=80,5,IF((E4+F4)/200*100&gt;=70,4,IF((E4+F4)/200*100&gt;=60,3.5,IF((E4+F4)/200*100&gt;=50,3,IF((E4+F4)/200*100&gt;=40,2,IF((E4+F4)/200*100&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF((H4+I4)/200*100&gt;=80,5,IF((H4+I4)/200*100&gt;=70,4,IF((H4+I4)/200*100&gt;=60,3.5,IF((H4+I4)/200*100&gt;=50,3,IF((H4+I4)/200*100&gt;=40,2,IF((H4+I4)/200*100&gt;=33,1,0))))))+IF((J4+K4)/200*100&gt;=80,5,IF((J4+K4)/200*100&gt;=70,4,IF((J4+K4)/200*100&gt;=60,3.5,IF((J4+K4)/200*100&gt;=50,3,IF((J4+K4)/200*100&gt;=40,2,IF((J4+K4)/200*100&gt;=33,1,0))))))+IF(L4&gt;=80,5,IF(L4&gt;=70,4,IF(L4&gt;=60,3.5,IF(L4&gt;=50,3,IF(L4&gt;=40,2,IF(L4&gt;=33,1,0))))))+IF(M4&gt;=80,5,IF(M4&gt;=70,4,IF(M4&gt;=60,3.5,IF(M4&gt;=50,3,IF(M4&gt;=40,2,IF(M4&gt;=33,1,0))))))+IF(N4&gt;=80,5,IF(N4&gt;=70,4,IF(N4&gt;=60,3.5,IF(N4&gt;=50,3,IF(N4&gt;=40,2,IF(N4&gt;=33,1,0)))))))/8+IF(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))&gt;=2,(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U4" s="6">
+      <c r="S4" s="5">
+        <f>ROUND(R4/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T4" s="6">
+        <f>IF(OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,(J4+K4)&lt;66,L4&lt;33,M4&lt;33,N4&lt;8.25,P4&lt;33,Q4&lt;33),0,MIN(5,ROUND((IF((C4+D4)/200*100&gt;=80,5,IF((C4+D4)/200*100&gt;=70,4,IF((C4+D4)/200*100&gt;=60,3.5,IF((C4+D4)/200*100&gt;=50,3,IF((C4+D4)/200*100&gt;=40,2,IF((C4+D4)/200*100&gt;=33,1,0))))))+IF((E4+F4)/200*100&gt;=80,5,IF((E4+F4)/200*100&gt;=70,4,IF((E4+F4)/200*100&gt;=60,3.5,IF((E4+F4)/200*100&gt;=50,3,IF((E4+F4)/200*100&gt;=40,2,IF((E4+F4)/200*100&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF((H4+I4)/200*100&gt;=80,5,IF((H4+I4)/200*100&gt;=70,4,IF((H4+I4)/200*100&gt;=60,3.5,IF((H4+I4)/200*100&gt;=50,3,IF((H4+I4)/200*100&gt;=40,2,IF((H4+I4)/200*100&gt;=33,1,0))))))+IF((J4+K4)/200*100&gt;=80,5,IF((J4+K4)/200*100&gt;=70,4,IF((J4+K4)/200*100&gt;=60,3.5,IF((J4+K4)/200*100&gt;=50,3,IF((J4+K4)/200*100&gt;=40,2,IF((J4+K4)/200*100&gt;=33,1,0))))))+IF(L4&gt;=80,5,IF(L4&gt;=70,4,IF(L4&gt;=60,3.5,IF(L4&gt;=50,3,IF(L4&gt;=40,2,IF(L4&gt;=33,1,0))))))+IF(M4&gt;=80,5,IF(M4&gt;=70,4,IF(M4&gt;=60,3.5,IF(M4&gt;=50,3,IF(M4&gt;=40,2,IF(M4&gt;=33,1,0))))))+IF(N4/50*100&gt;=80,5,IF(N4/50*100&gt;=70,4,IF(N4/50*100&gt;=60,3.5,IF(N4/50*100&gt;=50,3,IF(N4/50*100&gt;=40,2,IF(N4/50*100&gt;=33,1,0)))))))/8+IF(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))&gt;=2,(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U4" s="7">
         <f>IF(T4&gt;=5,"A+",IF(T4&gt;=4,"A",IF(T4&gt;=3.5,"A-",IF(T4&gt;=3,"B",IF(T4&gt;=2,"C",IF(T4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1135,31 +1142,31 @@
       <c r="M5" s="3" t="n">
         <v>83</v>
       </c>
-      <c r="N5" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>90</v>
+      <c r="N5" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>73</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R5">
         <f>SUM(C5:N5)</f>
         <v/>
       </c>
-      <c r="S5" s="4">
-        <f>ROUND(R5/12,2)</f>
-        <v/>
-      </c>
-      <c r="T5" s="5">
-        <f>IF(OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,(J5+K5)&lt;66,L5&lt;33,M5&lt;33,N5&lt;33,P5&lt;33,Q5&lt;33),0,MIN(5,ROUND((IF((C5+D5)/200*100&gt;=80,5,IF((C5+D5)/200*100&gt;=70,4,IF((C5+D5)/200*100&gt;=60,3.5,IF((C5+D5)/200*100&gt;=50,3,IF((C5+D5)/200*100&gt;=40,2,IF((C5+D5)/200*100&gt;=33,1,0))))))+IF((E5+F5)/200*100&gt;=80,5,IF((E5+F5)/200*100&gt;=70,4,IF((E5+F5)/200*100&gt;=60,3.5,IF((E5+F5)/200*100&gt;=50,3,IF((E5+F5)/200*100&gt;=40,2,IF((E5+F5)/200*100&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF((H5+I5)/200*100&gt;=80,5,IF((H5+I5)/200*100&gt;=70,4,IF((H5+I5)/200*100&gt;=60,3.5,IF((H5+I5)/200*100&gt;=50,3,IF((H5+I5)/200*100&gt;=40,2,IF((H5+I5)/200*100&gt;=33,1,0))))))+IF((J5+K5)/200*100&gt;=80,5,IF((J5+K5)/200*100&gt;=70,4,IF((J5+K5)/200*100&gt;=60,3.5,IF((J5+K5)/200*100&gt;=50,3,IF((J5+K5)/200*100&gt;=40,2,IF((J5+K5)/200*100&gt;=33,1,0))))))+IF(L5&gt;=80,5,IF(L5&gt;=70,4,IF(L5&gt;=60,3.5,IF(L5&gt;=50,3,IF(L5&gt;=40,2,IF(L5&gt;=33,1,0))))))+IF(M5&gt;=80,5,IF(M5&gt;=70,4,IF(M5&gt;=60,3.5,IF(M5&gt;=50,3,IF(M5&gt;=40,2,IF(M5&gt;=33,1,0))))))+IF(N5&gt;=80,5,IF(N5&gt;=70,4,IF(N5&gt;=60,3.5,IF(N5&gt;=50,3,IF(N5&gt;=40,2,IF(N5&gt;=33,1,0)))))))/8+IF(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))&gt;=2,(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U5" s="6">
+      <c r="S5" s="5">
+        <f>ROUND(R5/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T5" s="6">
+        <f>IF(OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,(J5+K5)&lt;66,L5&lt;33,M5&lt;33,N5&lt;8.25,P5&lt;33,Q5&lt;33),0,MIN(5,ROUND((IF((C5+D5)/200*100&gt;=80,5,IF((C5+D5)/200*100&gt;=70,4,IF((C5+D5)/200*100&gt;=60,3.5,IF((C5+D5)/200*100&gt;=50,3,IF((C5+D5)/200*100&gt;=40,2,IF((C5+D5)/200*100&gt;=33,1,0))))))+IF((E5+F5)/200*100&gt;=80,5,IF((E5+F5)/200*100&gt;=70,4,IF((E5+F5)/200*100&gt;=60,3.5,IF((E5+F5)/200*100&gt;=50,3,IF((E5+F5)/200*100&gt;=40,2,IF((E5+F5)/200*100&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF((H5+I5)/200*100&gt;=80,5,IF((H5+I5)/200*100&gt;=70,4,IF((H5+I5)/200*100&gt;=60,3.5,IF((H5+I5)/200*100&gt;=50,3,IF((H5+I5)/200*100&gt;=40,2,IF((H5+I5)/200*100&gt;=33,1,0))))))+IF((J5+K5)/200*100&gt;=80,5,IF((J5+K5)/200*100&gt;=70,4,IF((J5+K5)/200*100&gt;=60,3.5,IF((J5+K5)/200*100&gt;=50,3,IF((J5+K5)/200*100&gt;=40,2,IF((J5+K5)/200*100&gt;=33,1,0))))))+IF(L5&gt;=80,5,IF(L5&gt;=70,4,IF(L5&gt;=60,3.5,IF(L5&gt;=50,3,IF(L5&gt;=40,2,IF(L5&gt;=33,1,0))))))+IF(M5&gt;=80,5,IF(M5&gt;=70,4,IF(M5&gt;=60,3.5,IF(M5&gt;=50,3,IF(M5&gt;=40,2,IF(M5&gt;=33,1,0))))))+IF(N5/50*100&gt;=80,5,IF(N5/50*100&gt;=70,4,IF(N5/50*100&gt;=60,3.5,IF(N5/50*100&gt;=50,3,IF(N5/50*100&gt;=40,2,IF(N5/50*100&gt;=33,1,0)))))))/8+IF(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))&gt;=2,(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U5" s="7">
         <f>IF(T5&gt;=5,"A+",IF(T5&gt;=4,"A",IF(T5&gt;=3.5,"A-",IF(T5&gt;=3,"B",IF(T5&gt;=2,"C",IF(T5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1206,31 +1213,31 @@
       <c r="M6" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="N6" s="2" t="n">
-        <v>72</v>
+      <c r="N6" s="8" t="n">
+        <v>37</v>
       </c>
       <c r="O6" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="P6" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="Q6" s="3" t="n">
-        <v>89</v>
+        <v>80</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>77</v>
       </c>
       <c r="R6">
         <f>SUM(C6:N6)</f>
         <v/>
       </c>
-      <c r="S6" s="4">
-        <f>ROUND(R6/12,2)</f>
-        <v/>
-      </c>
-      <c r="T6" s="5">
-        <f>IF(OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,(J6+K6)&lt;66,L6&lt;33,M6&lt;33,N6&lt;33,P6&lt;33,Q6&lt;33),0,MIN(5,ROUND((IF((C6+D6)/200*100&gt;=80,5,IF((C6+D6)/200*100&gt;=70,4,IF((C6+D6)/200*100&gt;=60,3.5,IF((C6+D6)/200*100&gt;=50,3,IF((C6+D6)/200*100&gt;=40,2,IF((C6+D6)/200*100&gt;=33,1,0))))))+IF((E6+F6)/200*100&gt;=80,5,IF((E6+F6)/200*100&gt;=70,4,IF((E6+F6)/200*100&gt;=60,3.5,IF((E6+F6)/200*100&gt;=50,3,IF((E6+F6)/200*100&gt;=40,2,IF((E6+F6)/200*100&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF((H6+I6)/200*100&gt;=80,5,IF((H6+I6)/200*100&gt;=70,4,IF((H6+I6)/200*100&gt;=60,3.5,IF((H6+I6)/200*100&gt;=50,3,IF((H6+I6)/200*100&gt;=40,2,IF((H6+I6)/200*100&gt;=33,1,0))))))+IF((J6+K6)/200*100&gt;=80,5,IF((J6+K6)/200*100&gt;=70,4,IF((J6+K6)/200*100&gt;=60,3.5,IF((J6+K6)/200*100&gt;=50,3,IF((J6+K6)/200*100&gt;=40,2,IF((J6+K6)/200*100&gt;=33,1,0))))))+IF(L6&gt;=80,5,IF(L6&gt;=70,4,IF(L6&gt;=60,3.5,IF(L6&gt;=50,3,IF(L6&gt;=40,2,IF(L6&gt;=33,1,0))))))+IF(M6&gt;=80,5,IF(M6&gt;=70,4,IF(M6&gt;=60,3.5,IF(M6&gt;=50,3,IF(M6&gt;=40,2,IF(M6&gt;=33,1,0))))))+IF(N6&gt;=80,5,IF(N6&gt;=70,4,IF(N6&gt;=60,3.5,IF(N6&gt;=50,3,IF(N6&gt;=40,2,IF(N6&gt;=33,1,0)))))))/8+IF(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))&gt;=2,(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U6" s="6">
+      <c r="S6" s="5">
+        <f>ROUND(R6/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T6" s="6">
+        <f>IF(OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,(J6+K6)&lt;66,L6&lt;33,M6&lt;33,N6&lt;8.25,P6&lt;33,Q6&lt;33),0,MIN(5,ROUND((IF((C6+D6)/200*100&gt;=80,5,IF((C6+D6)/200*100&gt;=70,4,IF((C6+D6)/200*100&gt;=60,3.5,IF((C6+D6)/200*100&gt;=50,3,IF((C6+D6)/200*100&gt;=40,2,IF((C6+D6)/200*100&gt;=33,1,0))))))+IF((E6+F6)/200*100&gt;=80,5,IF((E6+F6)/200*100&gt;=70,4,IF((E6+F6)/200*100&gt;=60,3.5,IF((E6+F6)/200*100&gt;=50,3,IF((E6+F6)/200*100&gt;=40,2,IF((E6+F6)/200*100&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF((H6+I6)/200*100&gt;=80,5,IF((H6+I6)/200*100&gt;=70,4,IF((H6+I6)/200*100&gt;=60,3.5,IF((H6+I6)/200*100&gt;=50,3,IF((H6+I6)/200*100&gt;=40,2,IF((H6+I6)/200*100&gt;=33,1,0))))))+IF((J6+K6)/200*100&gt;=80,5,IF((J6+K6)/200*100&gt;=70,4,IF((J6+K6)/200*100&gt;=60,3.5,IF((J6+K6)/200*100&gt;=50,3,IF((J6+K6)/200*100&gt;=40,2,IF((J6+K6)/200*100&gt;=33,1,0))))))+IF(L6&gt;=80,5,IF(L6&gt;=70,4,IF(L6&gt;=60,3.5,IF(L6&gt;=50,3,IF(L6&gt;=40,2,IF(L6&gt;=33,1,0))))))+IF(M6&gt;=80,5,IF(M6&gt;=70,4,IF(M6&gt;=60,3.5,IF(M6&gt;=50,3,IF(M6&gt;=40,2,IF(M6&gt;=33,1,0))))))+IF(N6/50*100&gt;=80,5,IF(N6/50*100&gt;=70,4,IF(N6/50*100&gt;=60,3.5,IF(N6/50*100&gt;=50,3,IF(N6/50*100&gt;=40,2,IF(N6/50*100&gt;=33,1,0)))))))/8+IF(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))&gt;=2,(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U6" s="7">
         <f>IF(T6&gt;=5,"A+",IF(T6&gt;=4,"A",IF(T6&gt;=3.5,"A-",IF(T6&gt;=3,"B",IF(T6&gt;=2,"C",IF(T6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1277,31 +1284,31 @@
       <c r="M7" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="N7" s="3" t="n">
-        <v>83</v>
-      </c>
-      <c r="O7" s="7" t="n">
-        <v>58</v>
+      <c r="N7" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>65</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="R7">
         <f>SUM(C7:N7)</f>
         <v/>
       </c>
-      <c r="S7" s="4">
-        <f>ROUND(R7/12,2)</f>
-        <v/>
-      </c>
-      <c r="T7" s="5">
-        <f>IF(OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,(J7+K7)&lt;66,L7&lt;33,M7&lt;33,N7&lt;33,P7&lt;33,Q7&lt;33),0,MIN(5,ROUND((IF((C7+D7)/200*100&gt;=80,5,IF((C7+D7)/200*100&gt;=70,4,IF((C7+D7)/200*100&gt;=60,3.5,IF((C7+D7)/200*100&gt;=50,3,IF((C7+D7)/200*100&gt;=40,2,IF((C7+D7)/200*100&gt;=33,1,0))))))+IF((E7+F7)/200*100&gt;=80,5,IF((E7+F7)/200*100&gt;=70,4,IF((E7+F7)/200*100&gt;=60,3.5,IF((E7+F7)/200*100&gt;=50,3,IF((E7+F7)/200*100&gt;=40,2,IF((E7+F7)/200*100&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF((H7+I7)/200*100&gt;=80,5,IF((H7+I7)/200*100&gt;=70,4,IF((H7+I7)/200*100&gt;=60,3.5,IF((H7+I7)/200*100&gt;=50,3,IF((H7+I7)/200*100&gt;=40,2,IF((H7+I7)/200*100&gt;=33,1,0))))))+IF((J7+K7)/200*100&gt;=80,5,IF((J7+K7)/200*100&gt;=70,4,IF((J7+K7)/200*100&gt;=60,3.5,IF((J7+K7)/200*100&gt;=50,3,IF((J7+K7)/200*100&gt;=40,2,IF((J7+K7)/200*100&gt;=33,1,0))))))+IF(L7&gt;=80,5,IF(L7&gt;=70,4,IF(L7&gt;=60,3.5,IF(L7&gt;=50,3,IF(L7&gt;=40,2,IF(L7&gt;=33,1,0))))))+IF(M7&gt;=80,5,IF(M7&gt;=70,4,IF(M7&gt;=60,3.5,IF(M7&gt;=50,3,IF(M7&gt;=40,2,IF(M7&gt;=33,1,0))))))+IF(N7&gt;=80,5,IF(N7&gt;=70,4,IF(N7&gt;=60,3.5,IF(N7&gt;=50,3,IF(N7&gt;=40,2,IF(N7&gt;=33,1,0)))))))/8+IF(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))&gt;=2,(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U7" s="6">
+      <c r="S7" s="5">
+        <f>ROUND(R7/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T7" s="6">
+        <f>IF(OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,(J7+K7)&lt;66,L7&lt;33,M7&lt;33,N7&lt;8.25,P7&lt;33,Q7&lt;33),0,MIN(5,ROUND((IF((C7+D7)/200*100&gt;=80,5,IF((C7+D7)/200*100&gt;=70,4,IF((C7+D7)/200*100&gt;=60,3.5,IF((C7+D7)/200*100&gt;=50,3,IF((C7+D7)/200*100&gt;=40,2,IF((C7+D7)/200*100&gt;=33,1,0))))))+IF((E7+F7)/200*100&gt;=80,5,IF((E7+F7)/200*100&gt;=70,4,IF((E7+F7)/200*100&gt;=60,3.5,IF((E7+F7)/200*100&gt;=50,3,IF((E7+F7)/200*100&gt;=40,2,IF((E7+F7)/200*100&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF((H7+I7)/200*100&gt;=80,5,IF((H7+I7)/200*100&gt;=70,4,IF((H7+I7)/200*100&gt;=60,3.5,IF((H7+I7)/200*100&gt;=50,3,IF((H7+I7)/200*100&gt;=40,2,IF((H7+I7)/200*100&gt;=33,1,0))))))+IF((J7+K7)/200*100&gt;=80,5,IF((J7+K7)/200*100&gt;=70,4,IF((J7+K7)/200*100&gt;=60,3.5,IF((J7+K7)/200*100&gt;=50,3,IF((J7+K7)/200*100&gt;=40,2,IF((J7+K7)/200*100&gt;=33,1,0))))))+IF(L7&gt;=80,5,IF(L7&gt;=70,4,IF(L7&gt;=60,3.5,IF(L7&gt;=50,3,IF(L7&gt;=40,2,IF(L7&gt;=33,1,0))))))+IF(M7&gt;=80,5,IF(M7&gt;=70,4,IF(M7&gt;=60,3.5,IF(M7&gt;=50,3,IF(M7&gt;=40,2,IF(M7&gt;=33,1,0))))))+IF(N7/50*100&gt;=80,5,IF(N7/50*100&gt;=70,4,IF(N7/50*100&gt;=60,3.5,IF(N7/50*100&gt;=50,3,IF(N7/50*100&gt;=40,2,IF(N7/50*100&gt;=33,1,0)))))))/8+IF(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))&gt;=2,(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U7" s="7">
         <f>IF(T7&gt;=5,"A+",IF(T7&gt;=4,"A",IF(T7&gt;=3.5,"A-",IF(T7&gt;=3,"B",IF(T7&gt;=2,"C",IF(T7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1348,31 +1355,31 @@
       <c r="M8" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="N8" s="2" t="n">
-        <v>72</v>
+      <c r="N8" s="8" t="n">
+        <v>37</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>71</v>
-      </c>
-      <c r="Q8" s="2" t="n">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="Q8" s="3" t="n">
+        <v>80</v>
       </c>
       <c r="R8">
         <f>SUM(C8:N8)</f>
         <v/>
       </c>
-      <c r="S8" s="4">
-        <f>ROUND(R8/12,2)</f>
-        <v/>
-      </c>
-      <c r="T8" s="5">
-        <f>IF(OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,(J8+K8)&lt;66,L8&lt;33,M8&lt;33,N8&lt;33,P8&lt;33,Q8&lt;33),0,MIN(5,ROUND((IF((C8+D8)/200*100&gt;=80,5,IF((C8+D8)/200*100&gt;=70,4,IF((C8+D8)/200*100&gt;=60,3.5,IF((C8+D8)/200*100&gt;=50,3,IF((C8+D8)/200*100&gt;=40,2,IF((C8+D8)/200*100&gt;=33,1,0))))))+IF((E8+F8)/200*100&gt;=80,5,IF((E8+F8)/200*100&gt;=70,4,IF((E8+F8)/200*100&gt;=60,3.5,IF((E8+F8)/200*100&gt;=50,3,IF((E8+F8)/200*100&gt;=40,2,IF((E8+F8)/200*100&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF((H8+I8)/200*100&gt;=80,5,IF((H8+I8)/200*100&gt;=70,4,IF((H8+I8)/200*100&gt;=60,3.5,IF((H8+I8)/200*100&gt;=50,3,IF((H8+I8)/200*100&gt;=40,2,IF((H8+I8)/200*100&gt;=33,1,0))))))+IF((J8+K8)/200*100&gt;=80,5,IF((J8+K8)/200*100&gt;=70,4,IF((J8+K8)/200*100&gt;=60,3.5,IF((J8+K8)/200*100&gt;=50,3,IF((J8+K8)/200*100&gt;=40,2,IF((J8+K8)/200*100&gt;=33,1,0))))))+IF(L8&gt;=80,5,IF(L8&gt;=70,4,IF(L8&gt;=60,3.5,IF(L8&gt;=50,3,IF(L8&gt;=40,2,IF(L8&gt;=33,1,0))))))+IF(M8&gt;=80,5,IF(M8&gt;=70,4,IF(M8&gt;=60,3.5,IF(M8&gt;=50,3,IF(M8&gt;=40,2,IF(M8&gt;=33,1,0))))))+IF(N8&gt;=80,5,IF(N8&gt;=70,4,IF(N8&gt;=60,3.5,IF(N8&gt;=50,3,IF(N8&gt;=40,2,IF(N8&gt;=33,1,0)))))))/8+IF(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))&gt;=2,(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U8" s="6">
+      <c r="S8" s="5">
+        <f>ROUND(R8/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T8" s="6">
+        <f>IF(OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,(J8+K8)&lt;66,L8&lt;33,M8&lt;33,N8&lt;8.25,P8&lt;33,Q8&lt;33),0,MIN(5,ROUND((IF((C8+D8)/200*100&gt;=80,5,IF((C8+D8)/200*100&gt;=70,4,IF((C8+D8)/200*100&gt;=60,3.5,IF((C8+D8)/200*100&gt;=50,3,IF((C8+D8)/200*100&gt;=40,2,IF((C8+D8)/200*100&gt;=33,1,0))))))+IF((E8+F8)/200*100&gt;=80,5,IF((E8+F8)/200*100&gt;=70,4,IF((E8+F8)/200*100&gt;=60,3.5,IF((E8+F8)/200*100&gt;=50,3,IF((E8+F8)/200*100&gt;=40,2,IF((E8+F8)/200*100&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF((H8+I8)/200*100&gt;=80,5,IF((H8+I8)/200*100&gt;=70,4,IF((H8+I8)/200*100&gt;=60,3.5,IF((H8+I8)/200*100&gt;=50,3,IF((H8+I8)/200*100&gt;=40,2,IF((H8+I8)/200*100&gt;=33,1,0))))))+IF((J8+K8)/200*100&gt;=80,5,IF((J8+K8)/200*100&gt;=70,4,IF((J8+K8)/200*100&gt;=60,3.5,IF((J8+K8)/200*100&gt;=50,3,IF((J8+K8)/200*100&gt;=40,2,IF((J8+K8)/200*100&gt;=33,1,0))))))+IF(L8&gt;=80,5,IF(L8&gt;=70,4,IF(L8&gt;=60,3.5,IF(L8&gt;=50,3,IF(L8&gt;=40,2,IF(L8&gt;=33,1,0))))))+IF(M8&gt;=80,5,IF(M8&gt;=70,4,IF(M8&gt;=60,3.5,IF(M8&gt;=50,3,IF(M8&gt;=40,2,IF(M8&gt;=33,1,0))))))+IF(N8/50*100&gt;=80,5,IF(N8/50*100&gt;=70,4,IF(N8/50*100&gt;=60,3.5,IF(N8/50*100&gt;=50,3,IF(N8/50*100&gt;=40,2,IF(N8/50*100&gt;=33,1,0)))))))/8+IF(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))&gt;=2,(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U8" s="7">
         <f>IF(T8&gt;=5,"A+",IF(T8&gt;=4,"A",IF(T8&gt;=3.5,"A-",IF(T8&gt;=3,"B",IF(T8&gt;=2,"C",IF(T8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1419,31 +1426,31 @@
       <c r="M9" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="N9" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="O9" s="3" t="n">
-        <v>86</v>
+      <c r="N9" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>76</v>
       </c>
       <c r="P9" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="Q9" s="2" t="n">
-        <v>76</v>
+        <v>87</v>
+      </c>
+      <c r="Q9" s="3" t="n">
+        <v>88</v>
       </c>
       <c r="R9">
         <f>SUM(C9:N9)</f>
         <v/>
       </c>
-      <c r="S9" s="4">
-        <f>ROUND(R9/12,2)</f>
-        <v/>
-      </c>
-      <c r="T9" s="5">
-        <f>IF(OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,(J9+K9)&lt;66,L9&lt;33,M9&lt;33,N9&lt;33,P9&lt;33,Q9&lt;33),0,MIN(5,ROUND((IF((C9+D9)/200*100&gt;=80,5,IF((C9+D9)/200*100&gt;=70,4,IF((C9+D9)/200*100&gt;=60,3.5,IF((C9+D9)/200*100&gt;=50,3,IF((C9+D9)/200*100&gt;=40,2,IF((C9+D9)/200*100&gt;=33,1,0))))))+IF((E9+F9)/200*100&gt;=80,5,IF((E9+F9)/200*100&gt;=70,4,IF((E9+F9)/200*100&gt;=60,3.5,IF((E9+F9)/200*100&gt;=50,3,IF((E9+F9)/200*100&gt;=40,2,IF((E9+F9)/200*100&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF((H9+I9)/200*100&gt;=80,5,IF((H9+I9)/200*100&gt;=70,4,IF((H9+I9)/200*100&gt;=60,3.5,IF((H9+I9)/200*100&gt;=50,3,IF((H9+I9)/200*100&gt;=40,2,IF((H9+I9)/200*100&gt;=33,1,0))))))+IF((J9+K9)/200*100&gt;=80,5,IF((J9+K9)/200*100&gt;=70,4,IF((J9+K9)/200*100&gt;=60,3.5,IF((J9+K9)/200*100&gt;=50,3,IF((J9+K9)/200*100&gt;=40,2,IF((J9+K9)/200*100&gt;=33,1,0))))))+IF(L9&gt;=80,5,IF(L9&gt;=70,4,IF(L9&gt;=60,3.5,IF(L9&gt;=50,3,IF(L9&gt;=40,2,IF(L9&gt;=33,1,0))))))+IF(M9&gt;=80,5,IF(M9&gt;=70,4,IF(M9&gt;=60,3.5,IF(M9&gt;=50,3,IF(M9&gt;=40,2,IF(M9&gt;=33,1,0))))))+IF(N9&gt;=80,5,IF(N9&gt;=70,4,IF(N9&gt;=60,3.5,IF(N9&gt;=50,3,IF(N9&gt;=40,2,IF(N9&gt;=33,1,0)))))))/8+IF(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))&gt;=2,(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U9" s="6">
+      <c r="S9" s="5">
+        <f>ROUND(R9/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T9" s="6">
+        <f>IF(OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,(J9+K9)&lt;66,L9&lt;33,M9&lt;33,N9&lt;8.25,P9&lt;33,Q9&lt;33),0,MIN(5,ROUND((IF((C9+D9)/200*100&gt;=80,5,IF((C9+D9)/200*100&gt;=70,4,IF((C9+D9)/200*100&gt;=60,3.5,IF((C9+D9)/200*100&gt;=50,3,IF((C9+D9)/200*100&gt;=40,2,IF((C9+D9)/200*100&gt;=33,1,0))))))+IF((E9+F9)/200*100&gt;=80,5,IF((E9+F9)/200*100&gt;=70,4,IF((E9+F9)/200*100&gt;=60,3.5,IF((E9+F9)/200*100&gt;=50,3,IF((E9+F9)/200*100&gt;=40,2,IF((E9+F9)/200*100&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF((H9+I9)/200*100&gt;=80,5,IF((H9+I9)/200*100&gt;=70,4,IF((H9+I9)/200*100&gt;=60,3.5,IF((H9+I9)/200*100&gt;=50,3,IF((H9+I9)/200*100&gt;=40,2,IF((H9+I9)/200*100&gt;=33,1,0))))))+IF((J9+K9)/200*100&gt;=80,5,IF((J9+K9)/200*100&gt;=70,4,IF((J9+K9)/200*100&gt;=60,3.5,IF((J9+K9)/200*100&gt;=50,3,IF((J9+K9)/200*100&gt;=40,2,IF((J9+K9)/200*100&gt;=33,1,0))))))+IF(L9&gt;=80,5,IF(L9&gt;=70,4,IF(L9&gt;=60,3.5,IF(L9&gt;=50,3,IF(L9&gt;=40,2,IF(L9&gt;=33,1,0))))))+IF(M9&gt;=80,5,IF(M9&gt;=70,4,IF(M9&gt;=60,3.5,IF(M9&gt;=50,3,IF(M9&gt;=40,2,IF(M9&gt;=33,1,0))))))+IF(N9/50*100&gt;=80,5,IF(N9/50*100&gt;=70,4,IF(N9/50*100&gt;=60,3.5,IF(N9/50*100&gt;=50,3,IF(N9/50*100&gt;=40,2,IF(N9/50*100&gt;=33,1,0)))))))/8+IF(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))&gt;=2,(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U9" s="7">
         <f>IF(T9&gt;=5,"A+",IF(T9&gt;=4,"A",IF(T9&gt;=3.5,"A-",IF(T9&gt;=3,"B",IF(T9&gt;=2,"C",IF(T9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1484,37 +1491,37 @@
       <c r="K10" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="L10" s="7" t="n">
+      <c r="L10" s="4" t="n">
         <v>59</v>
       </c>
       <c r="M10" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="N10" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="O10" s="3" t="n">
-        <v>80</v>
+      <c r="N10" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>62</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="R10">
         <f>SUM(C10:N10)</f>
         <v/>
       </c>
-      <c r="S10" s="4">
-        <f>ROUND(R10/12,2)</f>
-        <v/>
-      </c>
-      <c r="T10" s="5">
-        <f>IF(OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,(J10+K10)&lt;66,L10&lt;33,M10&lt;33,N10&lt;33,P10&lt;33,Q10&lt;33),0,MIN(5,ROUND((IF((C10+D10)/200*100&gt;=80,5,IF((C10+D10)/200*100&gt;=70,4,IF((C10+D10)/200*100&gt;=60,3.5,IF((C10+D10)/200*100&gt;=50,3,IF((C10+D10)/200*100&gt;=40,2,IF((C10+D10)/200*100&gt;=33,1,0))))))+IF((E10+F10)/200*100&gt;=80,5,IF((E10+F10)/200*100&gt;=70,4,IF((E10+F10)/200*100&gt;=60,3.5,IF((E10+F10)/200*100&gt;=50,3,IF((E10+F10)/200*100&gt;=40,2,IF((E10+F10)/200*100&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF((H10+I10)/200*100&gt;=80,5,IF((H10+I10)/200*100&gt;=70,4,IF((H10+I10)/200*100&gt;=60,3.5,IF((H10+I10)/200*100&gt;=50,3,IF((H10+I10)/200*100&gt;=40,2,IF((H10+I10)/200*100&gt;=33,1,0))))))+IF((J10+K10)/200*100&gt;=80,5,IF((J10+K10)/200*100&gt;=70,4,IF((J10+K10)/200*100&gt;=60,3.5,IF((J10+K10)/200*100&gt;=50,3,IF((J10+K10)/200*100&gt;=40,2,IF((J10+K10)/200*100&gt;=33,1,0))))))+IF(L10&gt;=80,5,IF(L10&gt;=70,4,IF(L10&gt;=60,3.5,IF(L10&gt;=50,3,IF(L10&gt;=40,2,IF(L10&gt;=33,1,0))))))+IF(M10&gt;=80,5,IF(M10&gt;=70,4,IF(M10&gt;=60,3.5,IF(M10&gt;=50,3,IF(M10&gt;=40,2,IF(M10&gt;=33,1,0))))))+IF(N10&gt;=80,5,IF(N10&gt;=70,4,IF(N10&gt;=60,3.5,IF(N10&gt;=50,3,IF(N10&gt;=40,2,IF(N10&gt;=33,1,0)))))))/8+IF(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))&gt;=2,(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U10" s="6">
+      <c r="S10" s="5">
+        <f>ROUND(R10/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T10" s="6">
+        <f>IF(OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,(J10+K10)&lt;66,L10&lt;33,M10&lt;33,N10&lt;8.25,P10&lt;33,Q10&lt;33),0,MIN(5,ROUND((IF((C10+D10)/200*100&gt;=80,5,IF((C10+D10)/200*100&gt;=70,4,IF((C10+D10)/200*100&gt;=60,3.5,IF((C10+D10)/200*100&gt;=50,3,IF((C10+D10)/200*100&gt;=40,2,IF((C10+D10)/200*100&gt;=33,1,0))))))+IF((E10+F10)/200*100&gt;=80,5,IF((E10+F10)/200*100&gt;=70,4,IF((E10+F10)/200*100&gt;=60,3.5,IF((E10+F10)/200*100&gt;=50,3,IF((E10+F10)/200*100&gt;=40,2,IF((E10+F10)/200*100&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF((H10+I10)/200*100&gt;=80,5,IF((H10+I10)/200*100&gt;=70,4,IF((H10+I10)/200*100&gt;=60,3.5,IF((H10+I10)/200*100&gt;=50,3,IF((H10+I10)/200*100&gt;=40,2,IF((H10+I10)/200*100&gt;=33,1,0))))))+IF((J10+K10)/200*100&gt;=80,5,IF((J10+K10)/200*100&gt;=70,4,IF((J10+K10)/200*100&gt;=60,3.5,IF((J10+K10)/200*100&gt;=50,3,IF((J10+K10)/200*100&gt;=40,2,IF((J10+K10)/200*100&gt;=33,1,0))))))+IF(L10&gt;=80,5,IF(L10&gt;=70,4,IF(L10&gt;=60,3.5,IF(L10&gt;=50,3,IF(L10&gt;=40,2,IF(L10&gt;=33,1,0))))))+IF(M10&gt;=80,5,IF(M10&gt;=70,4,IF(M10&gt;=60,3.5,IF(M10&gt;=50,3,IF(M10&gt;=40,2,IF(M10&gt;=33,1,0))))))+IF(N10/50*100&gt;=80,5,IF(N10/50*100&gt;=70,4,IF(N10/50*100&gt;=60,3.5,IF(N10/50*100&gt;=50,3,IF(N10/50*100&gt;=40,2,IF(N10/50*100&gt;=33,1,0)))))))/8+IF(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))&gt;=2,(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U10" s="7">
         <f>IF(T10&gt;=5,"A+",IF(T10&gt;=4,"A",IF(T10&gt;=3.5,"A-",IF(T10&gt;=3,"B",IF(T10&gt;=2,"C",IF(T10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1561,31 +1568,31 @@
       <c r="M11" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="N11" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="P11" s="3" t="n">
-        <v>80</v>
+      <c r="N11" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="O11" s="4" t="n">
+        <v>56</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>74</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R11">
         <f>SUM(C11:N11)</f>
         <v/>
       </c>
-      <c r="S11" s="4">
-        <f>ROUND(R11/12,2)</f>
-        <v/>
-      </c>
-      <c r="T11" s="5">
-        <f>IF(OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,(J11+K11)&lt;66,L11&lt;33,M11&lt;33,N11&lt;33,P11&lt;33,Q11&lt;33),0,MIN(5,ROUND((IF((C11+D11)/200*100&gt;=80,5,IF((C11+D11)/200*100&gt;=70,4,IF((C11+D11)/200*100&gt;=60,3.5,IF((C11+D11)/200*100&gt;=50,3,IF((C11+D11)/200*100&gt;=40,2,IF((C11+D11)/200*100&gt;=33,1,0))))))+IF((E11+F11)/200*100&gt;=80,5,IF((E11+F11)/200*100&gt;=70,4,IF((E11+F11)/200*100&gt;=60,3.5,IF((E11+F11)/200*100&gt;=50,3,IF((E11+F11)/200*100&gt;=40,2,IF((E11+F11)/200*100&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF((H11+I11)/200*100&gt;=80,5,IF((H11+I11)/200*100&gt;=70,4,IF((H11+I11)/200*100&gt;=60,3.5,IF((H11+I11)/200*100&gt;=50,3,IF((H11+I11)/200*100&gt;=40,2,IF((H11+I11)/200*100&gt;=33,1,0))))))+IF((J11+K11)/200*100&gt;=80,5,IF((J11+K11)/200*100&gt;=70,4,IF((J11+K11)/200*100&gt;=60,3.5,IF((J11+K11)/200*100&gt;=50,3,IF((J11+K11)/200*100&gt;=40,2,IF((J11+K11)/200*100&gt;=33,1,0))))))+IF(L11&gt;=80,5,IF(L11&gt;=70,4,IF(L11&gt;=60,3.5,IF(L11&gt;=50,3,IF(L11&gt;=40,2,IF(L11&gt;=33,1,0))))))+IF(M11&gt;=80,5,IF(M11&gt;=70,4,IF(M11&gt;=60,3.5,IF(M11&gt;=50,3,IF(M11&gt;=40,2,IF(M11&gt;=33,1,0))))))+IF(N11&gt;=80,5,IF(N11&gt;=70,4,IF(N11&gt;=60,3.5,IF(N11&gt;=50,3,IF(N11&gt;=40,2,IF(N11&gt;=33,1,0)))))))/8+IF(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))&gt;=2,(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U11" s="6">
+      <c r="S11" s="5">
+        <f>ROUND(R11/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T11" s="6">
+        <f>IF(OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,(J11+K11)&lt;66,L11&lt;33,M11&lt;33,N11&lt;8.25,P11&lt;33,Q11&lt;33),0,MIN(5,ROUND((IF((C11+D11)/200*100&gt;=80,5,IF((C11+D11)/200*100&gt;=70,4,IF((C11+D11)/200*100&gt;=60,3.5,IF((C11+D11)/200*100&gt;=50,3,IF((C11+D11)/200*100&gt;=40,2,IF((C11+D11)/200*100&gt;=33,1,0))))))+IF((E11+F11)/200*100&gt;=80,5,IF((E11+F11)/200*100&gt;=70,4,IF((E11+F11)/200*100&gt;=60,3.5,IF((E11+F11)/200*100&gt;=50,3,IF((E11+F11)/200*100&gt;=40,2,IF((E11+F11)/200*100&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF((H11+I11)/200*100&gt;=80,5,IF((H11+I11)/200*100&gt;=70,4,IF((H11+I11)/200*100&gt;=60,3.5,IF((H11+I11)/200*100&gt;=50,3,IF((H11+I11)/200*100&gt;=40,2,IF((H11+I11)/200*100&gt;=33,1,0))))))+IF((J11+K11)/200*100&gt;=80,5,IF((J11+K11)/200*100&gt;=70,4,IF((J11+K11)/200*100&gt;=60,3.5,IF((J11+K11)/200*100&gt;=50,3,IF((J11+K11)/200*100&gt;=40,2,IF((J11+K11)/200*100&gt;=33,1,0))))))+IF(L11&gt;=80,5,IF(L11&gt;=70,4,IF(L11&gt;=60,3.5,IF(L11&gt;=50,3,IF(L11&gt;=40,2,IF(L11&gt;=33,1,0))))))+IF(M11&gt;=80,5,IF(M11&gt;=70,4,IF(M11&gt;=60,3.5,IF(M11&gt;=50,3,IF(M11&gt;=40,2,IF(M11&gt;=33,1,0))))))+IF(N11/50*100&gt;=80,5,IF(N11/50*100&gt;=70,4,IF(N11/50*100&gt;=60,3.5,IF(N11/50*100&gt;=50,3,IF(N11/50*100&gt;=40,2,IF(N11/50*100&gt;=33,1,0)))))))/8+IF(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))&gt;=2,(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U11" s="7">
         <f>IF(T11&gt;=5,"A+",IF(T11&gt;=4,"A",IF(T11&gt;=3.5,"A-",IF(T11&gt;=3,"B",IF(T11&gt;=2,"C",IF(T11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1632,31 +1639,31 @@
       <c r="M12" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="N12" s="3" t="n">
-        <v>85</v>
-      </c>
-      <c r="O12" s="3" t="n">
-        <v>80</v>
+      <c r="N12" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="O12" s="4" t="n">
+        <v>56</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="Q12" s="2" t="n">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>81</v>
       </c>
       <c r="R12">
         <f>SUM(C12:N12)</f>
         <v/>
       </c>
-      <c r="S12" s="4">
-        <f>ROUND(R12/12,2)</f>
-        <v/>
-      </c>
-      <c r="T12" s="5">
-        <f>IF(OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,(J12+K12)&lt;66,L12&lt;33,M12&lt;33,N12&lt;33,P12&lt;33,Q12&lt;33),0,MIN(5,ROUND((IF((C12+D12)/200*100&gt;=80,5,IF((C12+D12)/200*100&gt;=70,4,IF((C12+D12)/200*100&gt;=60,3.5,IF((C12+D12)/200*100&gt;=50,3,IF((C12+D12)/200*100&gt;=40,2,IF((C12+D12)/200*100&gt;=33,1,0))))))+IF((E12+F12)/200*100&gt;=80,5,IF((E12+F12)/200*100&gt;=70,4,IF((E12+F12)/200*100&gt;=60,3.5,IF((E12+F12)/200*100&gt;=50,3,IF((E12+F12)/200*100&gt;=40,2,IF((E12+F12)/200*100&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF((H12+I12)/200*100&gt;=80,5,IF((H12+I12)/200*100&gt;=70,4,IF((H12+I12)/200*100&gt;=60,3.5,IF((H12+I12)/200*100&gt;=50,3,IF((H12+I12)/200*100&gt;=40,2,IF((H12+I12)/200*100&gt;=33,1,0))))))+IF((J12+K12)/200*100&gt;=80,5,IF((J12+K12)/200*100&gt;=70,4,IF((J12+K12)/200*100&gt;=60,3.5,IF((J12+K12)/200*100&gt;=50,3,IF((J12+K12)/200*100&gt;=40,2,IF((J12+K12)/200*100&gt;=33,1,0))))))+IF(L12&gt;=80,5,IF(L12&gt;=70,4,IF(L12&gt;=60,3.5,IF(L12&gt;=50,3,IF(L12&gt;=40,2,IF(L12&gt;=33,1,0))))))+IF(M12&gt;=80,5,IF(M12&gt;=70,4,IF(M12&gt;=60,3.5,IF(M12&gt;=50,3,IF(M12&gt;=40,2,IF(M12&gt;=33,1,0))))))+IF(N12&gt;=80,5,IF(N12&gt;=70,4,IF(N12&gt;=60,3.5,IF(N12&gt;=50,3,IF(N12&gt;=40,2,IF(N12&gt;=33,1,0)))))))/8+IF(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))&gt;=2,(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U12" s="6">
+      <c r="S12" s="5">
+        <f>ROUND(R12/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T12" s="6">
+        <f>IF(OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,(J12+K12)&lt;66,L12&lt;33,M12&lt;33,N12&lt;8.25,P12&lt;33,Q12&lt;33),0,MIN(5,ROUND((IF((C12+D12)/200*100&gt;=80,5,IF((C12+D12)/200*100&gt;=70,4,IF((C12+D12)/200*100&gt;=60,3.5,IF((C12+D12)/200*100&gt;=50,3,IF((C12+D12)/200*100&gt;=40,2,IF((C12+D12)/200*100&gt;=33,1,0))))))+IF((E12+F12)/200*100&gt;=80,5,IF((E12+F12)/200*100&gt;=70,4,IF((E12+F12)/200*100&gt;=60,3.5,IF((E12+F12)/200*100&gt;=50,3,IF((E12+F12)/200*100&gt;=40,2,IF((E12+F12)/200*100&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF((H12+I12)/200*100&gt;=80,5,IF((H12+I12)/200*100&gt;=70,4,IF((H12+I12)/200*100&gt;=60,3.5,IF((H12+I12)/200*100&gt;=50,3,IF((H12+I12)/200*100&gt;=40,2,IF((H12+I12)/200*100&gt;=33,1,0))))))+IF((J12+K12)/200*100&gt;=80,5,IF((J12+K12)/200*100&gt;=70,4,IF((J12+K12)/200*100&gt;=60,3.5,IF((J12+K12)/200*100&gt;=50,3,IF((J12+K12)/200*100&gt;=40,2,IF((J12+K12)/200*100&gt;=33,1,0))))))+IF(L12&gt;=80,5,IF(L12&gt;=70,4,IF(L12&gt;=60,3.5,IF(L12&gt;=50,3,IF(L12&gt;=40,2,IF(L12&gt;=33,1,0))))))+IF(M12&gt;=80,5,IF(M12&gt;=70,4,IF(M12&gt;=60,3.5,IF(M12&gt;=50,3,IF(M12&gt;=40,2,IF(M12&gt;=33,1,0))))))+IF(N12/50*100&gt;=80,5,IF(N12/50*100&gt;=70,4,IF(N12/50*100&gt;=60,3.5,IF(N12/50*100&gt;=50,3,IF(N12/50*100&gt;=40,2,IF(N12/50*100&gt;=33,1,0)))))))/8+IF(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))&gt;=2,(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U12" s="7">
         <f>IF(T12&gt;=5,"A+",IF(T12&gt;=4,"A",IF(T12&gt;=3.5,"A-",IF(T12&gt;=3,"B",IF(T12&gt;=2,"C",IF(T12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1703,31 +1710,31 @@
       <c r="M13" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="N13" s="2" t="n">
-        <v>66</v>
+      <c r="N13" s="8" t="n">
+        <v>32</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="Q13" s="2" t="n">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>87</v>
       </c>
       <c r="R13">
         <f>SUM(C13:N13)</f>
         <v/>
       </c>
-      <c r="S13" s="4">
-        <f>ROUND(R13/12,2)</f>
-        <v/>
-      </c>
-      <c r="T13" s="5">
-        <f>IF(OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,(J13+K13)&lt;66,L13&lt;33,M13&lt;33,N13&lt;33,P13&lt;33,Q13&lt;33),0,MIN(5,ROUND((IF((C13+D13)/200*100&gt;=80,5,IF((C13+D13)/200*100&gt;=70,4,IF((C13+D13)/200*100&gt;=60,3.5,IF((C13+D13)/200*100&gt;=50,3,IF((C13+D13)/200*100&gt;=40,2,IF((C13+D13)/200*100&gt;=33,1,0))))))+IF((E13+F13)/200*100&gt;=80,5,IF((E13+F13)/200*100&gt;=70,4,IF((E13+F13)/200*100&gt;=60,3.5,IF((E13+F13)/200*100&gt;=50,3,IF((E13+F13)/200*100&gt;=40,2,IF((E13+F13)/200*100&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF((H13+I13)/200*100&gt;=80,5,IF((H13+I13)/200*100&gt;=70,4,IF((H13+I13)/200*100&gt;=60,3.5,IF((H13+I13)/200*100&gt;=50,3,IF((H13+I13)/200*100&gt;=40,2,IF((H13+I13)/200*100&gt;=33,1,0))))))+IF((J13+K13)/200*100&gt;=80,5,IF((J13+K13)/200*100&gt;=70,4,IF((J13+K13)/200*100&gt;=60,3.5,IF((J13+K13)/200*100&gt;=50,3,IF((J13+K13)/200*100&gt;=40,2,IF((J13+K13)/200*100&gt;=33,1,0))))))+IF(L13&gt;=80,5,IF(L13&gt;=70,4,IF(L13&gt;=60,3.5,IF(L13&gt;=50,3,IF(L13&gt;=40,2,IF(L13&gt;=33,1,0))))))+IF(M13&gt;=80,5,IF(M13&gt;=70,4,IF(M13&gt;=60,3.5,IF(M13&gt;=50,3,IF(M13&gt;=40,2,IF(M13&gt;=33,1,0))))))+IF(N13&gt;=80,5,IF(N13&gt;=70,4,IF(N13&gt;=60,3.5,IF(N13&gt;=50,3,IF(N13&gt;=40,2,IF(N13&gt;=33,1,0)))))))/8+IF(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))&gt;=2,(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U13" s="6">
+      <c r="S13" s="5">
+        <f>ROUND(R13/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T13" s="6">
+        <f>IF(OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,(J13+K13)&lt;66,L13&lt;33,M13&lt;33,N13&lt;8.25,P13&lt;33,Q13&lt;33),0,MIN(5,ROUND((IF((C13+D13)/200*100&gt;=80,5,IF((C13+D13)/200*100&gt;=70,4,IF((C13+D13)/200*100&gt;=60,3.5,IF((C13+D13)/200*100&gt;=50,3,IF((C13+D13)/200*100&gt;=40,2,IF((C13+D13)/200*100&gt;=33,1,0))))))+IF((E13+F13)/200*100&gt;=80,5,IF((E13+F13)/200*100&gt;=70,4,IF((E13+F13)/200*100&gt;=60,3.5,IF((E13+F13)/200*100&gt;=50,3,IF((E13+F13)/200*100&gt;=40,2,IF((E13+F13)/200*100&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF((H13+I13)/200*100&gt;=80,5,IF((H13+I13)/200*100&gt;=70,4,IF((H13+I13)/200*100&gt;=60,3.5,IF((H13+I13)/200*100&gt;=50,3,IF((H13+I13)/200*100&gt;=40,2,IF((H13+I13)/200*100&gt;=33,1,0))))))+IF((J13+K13)/200*100&gt;=80,5,IF((J13+K13)/200*100&gt;=70,4,IF((J13+K13)/200*100&gt;=60,3.5,IF((J13+K13)/200*100&gt;=50,3,IF((J13+K13)/200*100&gt;=40,2,IF((J13+K13)/200*100&gt;=33,1,0))))))+IF(L13&gt;=80,5,IF(L13&gt;=70,4,IF(L13&gt;=60,3.5,IF(L13&gt;=50,3,IF(L13&gt;=40,2,IF(L13&gt;=33,1,0))))))+IF(M13&gt;=80,5,IF(M13&gt;=70,4,IF(M13&gt;=60,3.5,IF(M13&gt;=50,3,IF(M13&gt;=40,2,IF(M13&gt;=33,1,0))))))+IF(N13/50*100&gt;=80,5,IF(N13/50*100&gt;=70,4,IF(N13/50*100&gt;=60,3.5,IF(N13/50*100&gt;=50,3,IF(N13/50*100&gt;=40,2,IF(N13/50*100&gt;=33,1,0)))))))/8+IF(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))&gt;=2,(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U13" s="7">
         <f>IF(T13&gt;=5,"A+",IF(T13&gt;=4,"A",IF(T13&gt;=3.5,"A-",IF(T13&gt;=3,"B",IF(T13&gt;=2,"C",IF(T13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1774,31 +1781,31 @@
       <c r="M14" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="N14" s="8" t="n">
+        <v>31</v>
+      </c>
+      <c r="O14" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="O14" s="2" t="n">
-        <v>62</v>
-      </c>
       <c r="P14" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="Q14" s="3" t="n">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>76</v>
       </c>
       <c r="R14">
         <f>SUM(C14:N14)</f>
         <v/>
       </c>
-      <c r="S14" s="4">
-        <f>ROUND(R14/12,2)</f>
-        <v/>
-      </c>
-      <c r="T14" s="5">
-        <f>IF(OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,(J14+K14)&lt;66,L14&lt;33,M14&lt;33,N14&lt;33,P14&lt;33,Q14&lt;33),0,MIN(5,ROUND((IF((C14+D14)/200*100&gt;=80,5,IF((C14+D14)/200*100&gt;=70,4,IF((C14+D14)/200*100&gt;=60,3.5,IF((C14+D14)/200*100&gt;=50,3,IF((C14+D14)/200*100&gt;=40,2,IF((C14+D14)/200*100&gt;=33,1,0))))))+IF((E14+F14)/200*100&gt;=80,5,IF((E14+F14)/200*100&gt;=70,4,IF((E14+F14)/200*100&gt;=60,3.5,IF((E14+F14)/200*100&gt;=50,3,IF((E14+F14)/200*100&gt;=40,2,IF((E14+F14)/200*100&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF((H14+I14)/200*100&gt;=80,5,IF((H14+I14)/200*100&gt;=70,4,IF((H14+I14)/200*100&gt;=60,3.5,IF((H14+I14)/200*100&gt;=50,3,IF((H14+I14)/200*100&gt;=40,2,IF((H14+I14)/200*100&gt;=33,1,0))))))+IF((J14+K14)/200*100&gt;=80,5,IF((J14+K14)/200*100&gt;=70,4,IF((J14+K14)/200*100&gt;=60,3.5,IF((J14+K14)/200*100&gt;=50,3,IF((J14+K14)/200*100&gt;=40,2,IF((J14+K14)/200*100&gt;=33,1,0))))))+IF(L14&gt;=80,5,IF(L14&gt;=70,4,IF(L14&gt;=60,3.5,IF(L14&gt;=50,3,IF(L14&gt;=40,2,IF(L14&gt;=33,1,0))))))+IF(M14&gt;=80,5,IF(M14&gt;=70,4,IF(M14&gt;=60,3.5,IF(M14&gt;=50,3,IF(M14&gt;=40,2,IF(M14&gt;=33,1,0))))))+IF(N14&gt;=80,5,IF(N14&gt;=70,4,IF(N14&gt;=60,3.5,IF(N14&gt;=50,3,IF(N14&gt;=40,2,IF(N14&gt;=33,1,0)))))))/8+IF(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))&gt;=2,(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U14" s="6">
+      <c r="S14" s="5">
+        <f>ROUND(R14/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T14" s="6">
+        <f>IF(OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,(J14+K14)&lt;66,L14&lt;33,M14&lt;33,N14&lt;8.25,P14&lt;33,Q14&lt;33),0,MIN(5,ROUND((IF((C14+D14)/200*100&gt;=80,5,IF((C14+D14)/200*100&gt;=70,4,IF((C14+D14)/200*100&gt;=60,3.5,IF((C14+D14)/200*100&gt;=50,3,IF((C14+D14)/200*100&gt;=40,2,IF((C14+D14)/200*100&gt;=33,1,0))))))+IF((E14+F14)/200*100&gt;=80,5,IF((E14+F14)/200*100&gt;=70,4,IF((E14+F14)/200*100&gt;=60,3.5,IF((E14+F14)/200*100&gt;=50,3,IF((E14+F14)/200*100&gt;=40,2,IF((E14+F14)/200*100&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF((H14+I14)/200*100&gt;=80,5,IF((H14+I14)/200*100&gt;=70,4,IF((H14+I14)/200*100&gt;=60,3.5,IF((H14+I14)/200*100&gt;=50,3,IF((H14+I14)/200*100&gt;=40,2,IF((H14+I14)/200*100&gt;=33,1,0))))))+IF((J14+K14)/200*100&gt;=80,5,IF((J14+K14)/200*100&gt;=70,4,IF((J14+K14)/200*100&gt;=60,3.5,IF((J14+K14)/200*100&gt;=50,3,IF((J14+K14)/200*100&gt;=40,2,IF((J14+K14)/200*100&gt;=33,1,0))))))+IF(L14&gt;=80,5,IF(L14&gt;=70,4,IF(L14&gt;=60,3.5,IF(L14&gt;=50,3,IF(L14&gt;=40,2,IF(L14&gt;=33,1,0))))))+IF(M14&gt;=80,5,IF(M14&gt;=70,4,IF(M14&gt;=60,3.5,IF(M14&gt;=50,3,IF(M14&gt;=40,2,IF(M14&gt;=33,1,0))))))+IF(N14/50*100&gt;=80,5,IF(N14/50*100&gt;=70,4,IF(N14/50*100&gt;=60,3.5,IF(N14/50*100&gt;=50,3,IF(N14/50*100&gt;=40,2,IF(N14/50*100&gt;=33,1,0)))))))/8+IF(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))&gt;=2,(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U14" s="7">
         <f>IF(T14&gt;=5,"A+",IF(T14&gt;=4,"A",IF(T14&gt;=3.5,"A-",IF(T14&gt;=3,"B",IF(T14&gt;=2,"C",IF(T14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1845,14 +1852,14 @@
       <c r="M15" s="3" t="n">
         <v>88</v>
       </c>
-      <c r="N15" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="O15" s="7" t="n">
-        <v>56</v>
-      </c>
-      <c r="P15" s="2" t="n">
-        <v>76</v>
+      <c r="N15" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="Q15" s="3" t="n">
         <v>80</v>
@@ -1861,15 +1868,15 @@
         <f>SUM(C15:N15)</f>
         <v/>
       </c>
-      <c r="S15" s="4">
-        <f>ROUND(R15/12,2)</f>
-        <v/>
-      </c>
-      <c r="T15" s="5">
-        <f>IF(OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,(J15+K15)&lt;66,L15&lt;33,M15&lt;33,N15&lt;33,P15&lt;33,Q15&lt;33),0,MIN(5,ROUND((IF((C15+D15)/200*100&gt;=80,5,IF((C15+D15)/200*100&gt;=70,4,IF((C15+D15)/200*100&gt;=60,3.5,IF((C15+D15)/200*100&gt;=50,3,IF((C15+D15)/200*100&gt;=40,2,IF((C15+D15)/200*100&gt;=33,1,0))))))+IF((E15+F15)/200*100&gt;=80,5,IF((E15+F15)/200*100&gt;=70,4,IF((E15+F15)/200*100&gt;=60,3.5,IF((E15+F15)/200*100&gt;=50,3,IF((E15+F15)/200*100&gt;=40,2,IF((E15+F15)/200*100&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF((H15+I15)/200*100&gt;=80,5,IF((H15+I15)/200*100&gt;=70,4,IF((H15+I15)/200*100&gt;=60,3.5,IF((H15+I15)/200*100&gt;=50,3,IF((H15+I15)/200*100&gt;=40,2,IF((H15+I15)/200*100&gt;=33,1,0))))))+IF((J15+K15)/200*100&gt;=80,5,IF((J15+K15)/200*100&gt;=70,4,IF((J15+K15)/200*100&gt;=60,3.5,IF((J15+K15)/200*100&gt;=50,3,IF((J15+K15)/200*100&gt;=40,2,IF((J15+K15)/200*100&gt;=33,1,0))))))+IF(L15&gt;=80,5,IF(L15&gt;=70,4,IF(L15&gt;=60,3.5,IF(L15&gt;=50,3,IF(L15&gt;=40,2,IF(L15&gt;=33,1,0))))))+IF(M15&gt;=80,5,IF(M15&gt;=70,4,IF(M15&gt;=60,3.5,IF(M15&gt;=50,3,IF(M15&gt;=40,2,IF(M15&gt;=33,1,0))))))+IF(N15&gt;=80,5,IF(N15&gt;=70,4,IF(N15&gt;=60,3.5,IF(N15&gt;=50,3,IF(N15&gt;=40,2,IF(N15&gt;=33,1,0)))))))/8+IF(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))&gt;=2,(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U15" s="6">
+      <c r="S15" s="5">
+        <f>ROUND(R15/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T15" s="6">
+        <f>IF(OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,(J15+K15)&lt;66,L15&lt;33,M15&lt;33,N15&lt;8.25,P15&lt;33,Q15&lt;33),0,MIN(5,ROUND((IF((C15+D15)/200*100&gt;=80,5,IF((C15+D15)/200*100&gt;=70,4,IF((C15+D15)/200*100&gt;=60,3.5,IF((C15+D15)/200*100&gt;=50,3,IF((C15+D15)/200*100&gt;=40,2,IF((C15+D15)/200*100&gt;=33,1,0))))))+IF((E15+F15)/200*100&gt;=80,5,IF((E15+F15)/200*100&gt;=70,4,IF((E15+F15)/200*100&gt;=60,3.5,IF((E15+F15)/200*100&gt;=50,3,IF((E15+F15)/200*100&gt;=40,2,IF((E15+F15)/200*100&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF((H15+I15)/200*100&gt;=80,5,IF((H15+I15)/200*100&gt;=70,4,IF((H15+I15)/200*100&gt;=60,3.5,IF((H15+I15)/200*100&gt;=50,3,IF((H15+I15)/200*100&gt;=40,2,IF((H15+I15)/200*100&gt;=33,1,0))))))+IF((J15+K15)/200*100&gt;=80,5,IF((J15+K15)/200*100&gt;=70,4,IF((J15+K15)/200*100&gt;=60,3.5,IF((J15+K15)/200*100&gt;=50,3,IF((J15+K15)/200*100&gt;=40,2,IF((J15+K15)/200*100&gt;=33,1,0))))))+IF(L15&gt;=80,5,IF(L15&gt;=70,4,IF(L15&gt;=60,3.5,IF(L15&gt;=50,3,IF(L15&gt;=40,2,IF(L15&gt;=33,1,0))))))+IF(M15&gt;=80,5,IF(M15&gt;=70,4,IF(M15&gt;=60,3.5,IF(M15&gt;=50,3,IF(M15&gt;=40,2,IF(M15&gt;=33,1,0))))))+IF(N15/50*100&gt;=80,5,IF(N15/50*100&gt;=70,4,IF(N15/50*100&gt;=60,3.5,IF(N15/50*100&gt;=50,3,IF(N15/50*100&gt;=40,2,IF(N15/50*100&gt;=33,1,0)))))))/8+IF(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))&gt;=2,(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U15" s="7">
         <f>IF(T15&gt;=5,"A+",IF(T15&gt;=4,"A",IF(T15&gt;=3.5,"A-",IF(T15&gt;=3,"B",IF(T15&gt;=2,"C",IF(T15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1916,31 +1923,31 @@
       <c r="M16" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="N16" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="O16" s="7" t="n">
-        <v>56</v>
+      <c r="N16" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>76</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R16">
         <f>SUM(C16:N16)</f>
         <v/>
       </c>
-      <c r="S16" s="4">
-        <f>ROUND(R16/12,2)</f>
-        <v/>
-      </c>
-      <c r="T16" s="5">
-        <f>IF(OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,(J16+K16)&lt;66,L16&lt;33,M16&lt;33,N16&lt;33,P16&lt;33,Q16&lt;33),0,MIN(5,ROUND((IF((C16+D16)/200*100&gt;=80,5,IF((C16+D16)/200*100&gt;=70,4,IF((C16+D16)/200*100&gt;=60,3.5,IF((C16+D16)/200*100&gt;=50,3,IF((C16+D16)/200*100&gt;=40,2,IF((C16+D16)/200*100&gt;=33,1,0))))))+IF((E16+F16)/200*100&gt;=80,5,IF((E16+F16)/200*100&gt;=70,4,IF((E16+F16)/200*100&gt;=60,3.5,IF((E16+F16)/200*100&gt;=50,3,IF((E16+F16)/200*100&gt;=40,2,IF((E16+F16)/200*100&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF((H16+I16)/200*100&gt;=80,5,IF((H16+I16)/200*100&gt;=70,4,IF((H16+I16)/200*100&gt;=60,3.5,IF((H16+I16)/200*100&gt;=50,3,IF((H16+I16)/200*100&gt;=40,2,IF((H16+I16)/200*100&gt;=33,1,0))))))+IF((J16+K16)/200*100&gt;=80,5,IF((J16+K16)/200*100&gt;=70,4,IF((J16+K16)/200*100&gt;=60,3.5,IF((J16+K16)/200*100&gt;=50,3,IF((J16+K16)/200*100&gt;=40,2,IF((J16+K16)/200*100&gt;=33,1,0))))))+IF(L16&gt;=80,5,IF(L16&gt;=70,4,IF(L16&gt;=60,3.5,IF(L16&gt;=50,3,IF(L16&gt;=40,2,IF(L16&gt;=33,1,0))))))+IF(M16&gt;=80,5,IF(M16&gt;=70,4,IF(M16&gt;=60,3.5,IF(M16&gt;=50,3,IF(M16&gt;=40,2,IF(M16&gt;=33,1,0))))))+IF(N16&gt;=80,5,IF(N16&gt;=70,4,IF(N16&gt;=60,3.5,IF(N16&gt;=50,3,IF(N16&gt;=40,2,IF(N16&gt;=33,1,0)))))))/8+IF(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))&gt;=2,(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U16" s="6">
+      <c r="S16" s="5">
+        <f>ROUND(R16/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T16" s="6">
+        <f>IF(OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,(J16+K16)&lt;66,L16&lt;33,M16&lt;33,N16&lt;8.25,P16&lt;33,Q16&lt;33),0,MIN(5,ROUND((IF((C16+D16)/200*100&gt;=80,5,IF((C16+D16)/200*100&gt;=70,4,IF((C16+D16)/200*100&gt;=60,3.5,IF((C16+D16)/200*100&gt;=50,3,IF((C16+D16)/200*100&gt;=40,2,IF((C16+D16)/200*100&gt;=33,1,0))))))+IF((E16+F16)/200*100&gt;=80,5,IF((E16+F16)/200*100&gt;=70,4,IF((E16+F16)/200*100&gt;=60,3.5,IF((E16+F16)/200*100&gt;=50,3,IF((E16+F16)/200*100&gt;=40,2,IF((E16+F16)/200*100&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF((H16+I16)/200*100&gt;=80,5,IF((H16+I16)/200*100&gt;=70,4,IF((H16+I16)/200*100&gt;=60,3.5,IF((H16+I16)/200*100&gt;=50,3,IF((H16+I16)/200*100&gt;=40,2,IF((H16+I16)/200*100&gt;=33,1,0))))))+IF((J16+K16)/200*100&gt;=80,5,IF((J16+K16)/200*100&gt;=70,4,IF((J16+K16)/200*100&gt;=60,3.5,IF((J16+K16)/200*100&gt;=50,3,IF((J16+K16)/200*100&gt;=40,2,IF((J16+K16)/200*100&gt;=33,1,0))))))+IF(L16&gt;=80,5,IF(L16&gt;=70,4,IF(L16&gt;=60,3.5,IF(L16&gt;=50,3,IF(L16&gt;=40,2,IF(L16&gt;=33,1,0))))))+IF(M16&gt;=80,5,IF(M16&gt;=70,4,IF(M16&gt;=60,3.5,IF(M16&gt;=50,3,IF(M16&gt;=40,2,IF(M16&gt;=33,1,0))))))+IF(N16/50*100&gt;=80,5,IF(N16/50*100&gt;=70,4,IF(N16/50*100&gt;=60,3.5,IF(N16/50*100&gt;=50,3,IF(N16/50*100&gt;=40,2,IF(N16/50*100&gt;=33,1,0)))))))/8+IF(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))&gt;=2,(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U16" s="7">
         <f>IF(T16&gt;=5,"A+",IF(T16&gt;=4,"A",IF(T16&gt;=3.5,"A-",IF(T16&gt;=3,"B",IF(T16&gt;=2,"C",IF(T16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1987,31 +1994,31 @@
       <c r="M17" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="N17" s="2" t="n">
-        <v>66</v>
+      <c r="N17" s="4" t="n">
+        <v>46</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="P17" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="Q17" s="3" t="n">
-        <v>90</v>
+        <v>79</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="Q17" s="2" t="n">
+        <v>75</v>
       </c>
       <c r="R17">
         <f>SUM(C17:N17)</f>
         <v/>
       </c>
-      <c r="S17" s="4">
-        <f>ROUND(R17/12,2)</f>
-        <v/>
-      </c>
-      <c r="T17" s="5">
-        <f>IF(OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,(J17+K17)&lt;66,L17&lt;33,M17&lt;33,N17&lt;33,P17&lt;33,Q17&lt;33),0,MIN(5,ROUND((IF((C17+D17)/200*100&gt;=80,5,IF((C17+D17)/200*100&gt;=70,4,IF((C17+D17)/200*100&gt;=60,3.5,IF((C17+D17)/200*100&gt;=50,3,IF((C17+D17)/200*100&gt;=40,2,IF((C17+D17)/200*100&gt;=33,1,0))))))+IF((E17+F17)/200*100&gt;=80,5,IF((E17+F17)/200*100&gt;=70,4,IF((E17+F17)/200*100&gt;=60,3.5,IF((E17+F17)/200*100&gt;=50,3,IF((E17+F17)/200*100&gt;=40,2,IF((E17+F17)/200*100&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF((H17+I17)/200*100&gt;=80,5,IF((H17+I17)/200*100&gt;=70,4,IF((H17+I17)/200*100&gt;=60,3.5,IF((H17+I17)/200*100&gt;=50,3,IF((H17+I17)/200*100&gt;=40,2,IF((H17+I17)/200*100&gt;=33,1,0))))))+IF((J17+K17)/200*100&gt;=80,5,IF((J17+K17)/200*100&gt;=70,4,IF((J17+K17)/200*100&gt;=60,3.5,IF((J17+K17)/200*100&gt;=50,3,IF((J17+K17)/200*100&gt;=40,2,IF((J17+K17)/200*100&gt;=33,1,0))))))+IF(L17&gt;=80,5,IF(L17&gt;=70,4,IF(L17&gt;=60,3.5,IF(L17&gt;=50,3,IF(L17&gt;=40,2,IF(L17&gt;=33,1,0))))))+IF(M17&gt;=80,5,IF(M17&gt;=70,4,IF(M17&gt;=60,3.5,IF(M17&gt;=50,3,IF(M17&gt;=40,2,IF(M17&gt;=33,1,0))))))+IF(N17&gt;=80,5,IF(N17&gt;=70,4,IF(N17&gt;=60,3.5,IF(N17&gt;=50,3,IF(N17&gt;=40,2,IF(N17&gt;=33,1,0)))))))/8+IF(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))&gt;=2,(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U17" s="6">
+      <c r="S17" s="5">
+        <f>ROUND(R17/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T17" s="6">
+        <f>IF(OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,(J17+K17)&lt;66,L17&lt;33,M17&lt;33,N17&lt;8.25,P17&lt;33,Q17&lt;33),0,MIN(5,ROUND((IF((C17+D17)/200*100&gt;=80,5,IF((C17+D17)/200*100&gt;=70,4,IF((C17+D17)/200*100&gt;=60,3.5,IF((C17+D17)/200*100&gt;=50,3,IF((C17+D17)/200*100&gt;=40,2,IF((C17+D17)/200*100&gt;=33,1,0))))))+IF((E17+F17)/200*100&gt;=80,5,IF((E17+F17)/200*100&gt;=70,4,IF((E17+F17)/200*100&gt;=60,3.5,IF((E17+F17)/200*100&gt;=50,3,IF((E17+F17)/200*100&gt;=40,2,IF((E17+F17)/200*100&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF((H17+I17)/200*100&gt;=80,5,IF((H17+I17)/200*100&gt;=70,4,IF((H17+I17)/200*100&gt;=60,3.5,IF((H17+I17)/200*100&gt;=50,3,IF((H17+I17)/200*100&gt;=40,2,IF((H17+I17)/200*100&gt;=33,1,0))))))+IF((J17+K17)/200*100&gt;=80,5,IF((J17+K17)/200*100&gt;=70,4,IF((J17+K17)/200*100&gt;=60,3.5,IF((J17+K17)/200*100&gt;=50,3,IF((J17+K17)/200*100&gt;=40,2,IF((J17+K17)/200*100&gt;=33,1,0))))))+IF(L17&gt;=80,5,IF(L17&gt;=70,4,IF(L17&gt;=60,3.5,IF(L17&gt;=50,3,IF(L17&gt;=40,2,IF(L17&gt;=33,1,0))))))+IF(M17&gt;=80,5,IF(M17&gt;=70,4,IF(M17&gt;=60,3.5,IF(M17&gt;=50,3,IF(M17&gt;=40,2,IF(M17&gt;=33,1,0))))))+IF(N17/50*100&gt;=80,5,IF(N17/50*100&gt;=70,4,IF(N17/50*100&gt;=60,3.5,IF(N17/50*100&gt;=50,3,IF(N17/50*100&gt;=40,2,IF(N17/50*100&gt;=33,1,0)))))))/8+IF(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))&gt;=2,(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U17" s="7">
         <f>IF(T17&gt;=5,"A+",IF(T17&gt;=4,"A",IF(T17&gt;=3.5,"A-",IF(T17&gt;=3,"B",IF(T17&gt;=2,"C",IF(T17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2058,31 +2065,31 @@
       <c r="M18" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="N18" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="O18" s="2" t="n">
-        <v>72</v>
+      <c r="N18" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="O18" s="4" t="n">
+        <v>53</v>
       </c>
       <c r="P18" s="3" t="n">
         <v>84</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R18">
         <f>SUM(C18:N18)</f>
         <v/>
       </c>
-      <c r="S18" s="4">
-        <f>ROUND(R18/12,2)</f>
-        <v/>
-      </c>
-      <c r="T18" s="5">
-        <f>IF(OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,(J18+K18)&lt;66,L18&lt;33,M18&lt;33,N18&lt;33,P18&lt;33,Q18&lt;33),0,MIN(5,ROUND((IF((C18+D18)/200*100&gt;=80,5,IF((C18+D18)/200*100&gt;=70,4,IF((C18+D18)/200*100&gt;=60,3.5,IF((C18+D18)/200*100&gt;=50,3,IF((C18+D18)/200*100&gt;=40,2,IF((C18+D18)/200*100&gt;=33,1,0))))))+IF((E18+F18)/200*100&gt;=80,5,IF((E18+F18)/200*100&gt;=70,4,IF((E18+F18)/200*100&gt;=60,3.5,IF((E18+F18)/200*100&gt;=50,3,IF((E18+F18)/200*100&gt;=40,2,IF((E18+F18)/200*100&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF((H18+I18)/200*100&gt;=80,5,IF((H18+I18)/200*100&gt;=70,4,IF((H18+I18)/200*100&gt;=60,3.5,IF((H18+I18)/200*100&gt;=50,3,IF((H18+I18)/200*100&gt;=40,2,IF((H18+I18)/200*100&gt;=33,1,0))))))+IF((J18+K18)/200*100&gt;=80,5,IF((J18+K18)/200*100&gt;=70,4,IF((J18+K18)/200*100&gt;=60,3.5,IF((J18+K18)/200*100&gt;=50,3,IF((J18+K18)/200*100&gt;=40,2,IF((J18+K18)/200*100&gt;=33,1,0))))))+IF(L18&gt;=80,5,IF(L18&gt;=70,4,IF(L18&gt;=60,3.5,IF(L18&gt;=50,3,IF(L18&gt;=40,2,IF(L18&gt;=33,1,0))))))+IF(M18&gt;=80,5,IF(M18&gt;=70,4,IF(M18&gt;=60,3.5,IF(M18&gt;=50,3,IF(M18&gt;=40,2,IF(M18&gt;=33,1,0))))))+IF(N18&gt;=80,5,IF(N18&gt;=70,4,IF(N18&gt;=60,3.5,IF(N18&gt;=50,3,IF(N18&gt;=40,2,IF(N18&gt;=33,1,0)))))))/8+IF(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))&gt;=2,(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U18" s="6">
+      <c r="S18" s="5">
+        <f>ROUND(R18/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T18" s="6">
+        <f>IF(OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,(J18+K18)&lt;66,L18&lt;33,M18&lt;33,N18&lt;8.25,P18&lt;33,Q18&lt;33),0,MIN(5,ROUND((IF((C18+D18)/200*100&gt;=80,5,IF((C18+D18)/200*100&gt;=70,4,IF((C18+D18)/200*100&gt;=60,3.5,IF((C18+D18)/200*100&gt;=50,3,IF((C18+D18)/200*100&gt;=40,2,IF((C18+D18)/200*100&gt;=33,1,0))))))+IF((E18+F18)/200*100&gt;=80,5,IF((E18+F18)/200*100&gt;=70,4,IF((E18+F18)/200*100&gt;=60,3.5,IF((E18+F18)/200*100&gt;=50,3,IF((E18+F18)/200*100&gt;=40,2,IF((E18+F18)/200*100&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF((H18+I18)/200*100&gt;=80,5,IF((H18+I18)/200*100&gt;=70,4,IF((H18+I18)/200*100&gt;=60,3.5,IF((H18+I18)/200*100&gt;=50,3,IF((H18+I18)/200*100&gt;=40,2,IF((H18+I18)/200*100&gt;=33,1,0))))))+IF((J18+K18)/200*100&gt;=80,5,IF((J18+K18)/200*100&gt;=70,4,IF((J18+K18)/200*100&gt;=60,3.5,IF((J18+K18)/200*100&gt;=50,3,IF((J18+K18)/200*100&gt;=40,2,IF((J18+K18)/200*100&gt;=33,1,0))))))+IF(L18&gt;=80,5,IF(L18&gt;=70,4,IF(L18&gt;=60,3.5,IF(L18&gt;=50,3,IF(L18&gt;=40,2,IF(L18&gt;=33,1,0))))))+IF(M18&gt;=80,5,IF(M18&gt;=70,4,IF(M18&gt;=60,3.5,IF(M18&gt;=50,3,IF(M18&gt;=40,2,IF(M18&gt;=33,1,0))))))+IF(N18/50*100&gt;=80,5,IF(N18/50*100&gt;=70,4,IF(N18/50*100&gt;=60,3.5,IF(N18/50*100&gt;=50,3,IF(N18/50*100&gt;=40,2,IF(N18/50*100&gt;=33,1,0)))))))/8+IF(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))&gt;=2,(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U18" s="7">
         <f>IF(T18&gt;=5,"A+",IF(T18&gt;=4,"A",IF(T18&gt;=3.5,"A-",IF(T18&gt;=3,"B",IF(T18&gt;=2,"C",IF(T18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2129,31 +2136,31 @@
       <c r="M19" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="N19" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="O19" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="P19" s="2" t="n">
-        <v>74</v>
+      <c r="N19" s="8" t="n">
+        <v>38</v>
+      </c>
+      <c r="O19" s="4" t="n">
+        <v>56</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="R19">
         <f>SUM(C19:N19)</f>
         <v/>
       </c>
-      <c r="S19" s="4">
-        <f>ROUND(R19/12,2)</f>
-        <v/>
-      </c>
-      <c r="T19" s="5">
-        <f>IF(OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,(J19+K19)&lt;66,L19&lt;33,M19&lt;33,N19&lt;33,P19&lt;33,Q19&lt;33),0,MIN(5,ROUND((IF((C19+D19)/200*100&gt;=80,5,IF((C19+D19)/200*100&gt;=70,4,IF((C19+D19)/200*100&gt;=60,3.5,IF((C19+D19)/200*100&gt;=50,3,IF((C19+D19)/200*100&gt;=40,2,IF((C19+D19)/200*100&gt;=33,1,0))))))+IF((E19+F19)/200*100&gt;=80,5,IF((E19+F19)/200*100&gt;=70,4,IF((E19+F19)/200*100&gt;=60,3.5,IF((E19+F19)/200*100&gt;=50,3,IF((E19+F19)/200*100&gt;=40,2,IF((E19+F19)/200*100&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF((H19+I19)/200*100&gt;=80,5,IF((H19+I19)/200*100&gt;=70,4,IF((H19+I19)/200*100&gt;=60,3.5,IF((H19+I19)/200*100&gt;=50,3,IF((H19+I19)/200*100&gt;=40,2,IF((H19+I19)/200*100&gt;=33,1,0))))))+IF((J19+K19)/200*100&gt;=80,5,IF((J19+K19)/200*100&gt;=70,4,IF((J19+K19)/200*100&gt;=60,3.5,IF((J19+K19)/200*100&gt;=50,3,IF((J19+K19)/200*100&gt;=40,2,IF((J19+K19)/200*100&gt;=33,1,0))))))+IF(L19&gt;=80,5,IF(L19&gt;=70,4,IF(L19&gt;=60,3.5,IF(L19&gt;=50,3,IF(L19&gt;=40,2,IF(L19&gt;=33,1,0))))))+IF(M19&gt;=80,5,IF(M19&gt;=70,4,IF(M19&gt;=60,3.5,IF(M19&gt;=50,3,IF(M19&gt;=40,2,IF(M19&gt;=33,1,0))))))+IF(N19&gt;=80,5,IF(N19&gt;=70,4,IF(N19&gt;=60,3.5,IF(N19&gt;=50,3,IF(N19&gt;=40,2,IF(N19&gt;=33,1,0)))))))/8+IF(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))&gt;=2,(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U19" s="6">
+      <c r="S19" s="5">
+        <f>ROUND(R19/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T19" s="6">
+        <f>IF(OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,(J19+K19)&lt;66,L19&lt;33,M19&lt;33,N19&lt;8.25,P19&lt;33,Q19&lt;33),0,MIN(5,ROUND((IF((C19+D19)/200*100&gt;=80,5,IF((C19+D19)/200*100&gt;=70,4,IF((C19+D19)/200*100&gt;=60,3.5,IF((C19+D19)/200*100&gt;=50,3,IF((C19+D19)/200*100&gt;=40,2,IF((C19+D19)/200*100&gt;=33,1,0))))))+IF((E19+F19)/200*100&gt;=80,5,IF((E19+F19)/200*100&gt;=70,4,IF((E19+F19)/200*100&gt;=60,3.5,IF((E19+F19)/200*100&gt;=50,3,IF((E19+F19)/200*100&gt;=40,2,IF((E19+F19)/200*100&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF((H19+I19)/200*100&gt;=80,5,IF((H19+I19)/200*100&gt;=70,4,IF((H19+I19)/200*100&gt;=60,3.5,IF((H19+I19)/200*100&gt;=50,3,IF((H19+I19)/200*100&gt;=40,2,IF((H19+I19)/200*100&gt;=33,1,0))))))+IF((J19+K19)/200*100&gt;=80,5,IF((J19+K19)/200*100&gt;=70,4,IF((J19+K19)/200*100&gt;=60,3.5,IF((J19+K19)/200*100&gt;=50,3,IF((J19+K19)/200*100&gt;=40,2,IF((J19+K19)/200*100&gt;=33,1,0))))))+IF(L19&gt;=80,5,IF(L19&gt;=70,4,IF(L19&gt;=60,3.5,IF(L19&gt;=50,3,IF(L19&gt;=40,2,IF(L19&gt;=33,1,0))))))+IF(M19&gt;=80,5,IF(M19&gt;=70,4,IF(M19&gt;=60,3.5,IF(M19&gt;=50,3,IF(M19&gt;=40,2,IF(M19&gt;=33,1,0))))))+IF(N19/50*100&gt;=80,5,IF(N19/50*100&gt;=70,4,IF(N19/50*100&gt;=60,3.5,IF(N19/50*100&gt;=50,3,IF(N19/50*100&gt;=40,2,IF(N19/50*100&gt;=33,1,0)))))))/8+IF(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))&gt;=2,(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U19" s="7">
         <f>IF(T19&gt;=5,"A+",IF(T19&gt;=4,"A",IF(T19&gt;=3.5,"A-",IF(T19&gt;=3,"B",IF(T19&gt;=2,"C",IF(T19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2200,31 +2207,31 @@
       <c r="M20" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="N20" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="O20" s="2" t="n">
-        <v>76</v>
+      <c r="N20" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="O20" s="4" t="n">
+        <v>53</v>
       </c>
       <c r="P20" s="3" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R20">
         <f>SUM(C20:N20)</f>
         <v/>
       </c>
-      <c r="S20" s="4">
-        <f>ROUND(R20/12,2)</f>
-        <v/>
-      </c>
-      <c r="T20" s="5">
-        <f>IF(OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,(J20+K20)&lt;66,L20&lt;33,M20&lt;33,N20&lt;33,P20&lt;33,Q20&lt;33),0,MIN(5,ROUND((IF((C20+D20)/200*100&gt;=80,5,IF((C20+D20)/200*100&gt;=70,4,IF((C20+D20)/200*100&gt;=60,3.5,IF((C20+D20)/200*100&gt;=50,3,IF((C20+D20)/200*100&gt;=40,2,IF((C20+D20)/200*100&gt;=33,1,0))))))+IF((E20+F20)/200*100&gt;=80,5,IF((E20+F20)/200*100&gt;=70,4,IF((E20+F20)/200*100&gt;=60,3.5,IF((E20+F20)/200*100&gt;=50,3,IF((E20+F20)/200*100&gt;=40,2,IF((E20+F20)/200*100&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF((H20+I20)/200*100&gt;=80,5,IF((H20+I20)/200*100&gt;=70,4,IF((H20+I20)/200*100&gt;=60,3.5,IF((H20+I20)/200*100&gt;=50,3,IF((H20+I20)/200*100&gt;=40,2,IF((H20+I20)/200*100&gt;=33,1,0))))))+IF((J20+K20)/200*100&gt;=80,5,IF((J20+K20)/200*100&gt;=70,4,IF((J20+K20)/200*100&gt;=60,3.5,IF((J20+K20)/200*100&gt;=50,3,IF((J20+K20)/200*100&gt;=40,2,IF((J20+K20)/200*100&gt;=33,1,0))))))+IF(L20&gt;=80,5,IF(L20&gt;=70,4,IF(L20&gt;=60,3.5,IF(L20&gt;=50,3,IF(L20&gt;=40,2,IF(L20&gt;=33,1,0))))))+IF(M20&gt;=80,5,IF(M20&gt;=70,4,IF(M20&gt;=60,3.5,IF(M20&gt;=50,3,IF(M20&gt;=40,2,IF(M20&gt;=33,1,0))))))+IF(N20&gt;=80,5,IF(N20&gt;=70,4,IF(N20&gt;=60,3.5,IF(N20&gt;=50,3,IF(N20&gt;=40,2,IF(N20&gt;=33,1,0)))))))/8+IF(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))&gt;=2,(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U20" s="6">
+      <c r="S20" s="5">
+        <f>ROUND(R20/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T20" s="6">
+        <f>IF(OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,(J20+K20)&lt;66,L20&lt;33,M20&lt;33,N20&lt;8.25,P20&lt;33,Q20&lt;33),0,MIN(5,ROUND((IF((C20+D20)/200*100&gt;=80,5,IF((C20+D20)/200*100&gt;=70,4,IF((C20+D20)/200*100&gt;=60,3.5,IF((C20+D20)/200*100&gt;=50,3,IF((C20+D20)/200*100&gt;=40,2,IF((C20+D20)/200*100&gt;=33,1,0))))))+IF((E20+F20)/200*100&gt;=80,5,IF((E20+F20)/200*100&gt;=70,4,IF((E20+F20)/200*100&gt;=60,3.5,IF((E20+F20)/200*100&gt;=50,3,IF((E20+F20)/200*100&gt;=40,2,IF((E20+F20)/200*100&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF((H20+I20)/200*100&gt;=80,5,IF((H20+I20)/200*100&gt;=70,4,IF((H20+I20)/200*100&gt;=60,3.5,IF((H20+I20)/200*100&gt;=50,3,IF((H20+I20)/200*100&gt;=40,2,IF((H20+I20)/200*100&gt;=33,1,0))))))+IF((J20+K20)/200*100&gt;=80,5,IF((J20+K20)/200*100&gt;=70,4,IF((J20+K20)/200*100&gt;=60,3.5,IF((J20+K20)/200*100&gt;=50,3,IF((J20+K20)/200*100&gt;=40,2,IF((J20+K20)/200*100&gt;=33,1,0))))))+IF(L20&gt;=80,5,IF(L20&gt;=70,4,IF(L20&gt;=60,3.5,IF(L20&gt;=50,3,IF(L20&gt;=40,2,IF(L20&gt;=33,1,0))))))+IF(M20&gt;=80,5,IF(M20&gt;=70,4,IF(M20&gt;=60,3.5,IF(M20&gt;=50,3,IF(M20&gt;=40,2,IF(M20&gt;=33,1,0))))))+IF(N20/50*100&gt;=80,5,IF(N20/50*100&gt;=70,4,IF(N20/50*100&gt;=60,3.5,IF(N20/50*100&gt;=50,3,IF(N20/50*100&gt;=40,2,IF(N20/50*100&gt;=33,1,0)))))))/8+IF(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))&gt;=2,(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U20" s="7">
         <f>IF(T20&gt;=5,"A+",IF(T20&gt;=4,"A",IF(T20&gt;=3.5,"A-",IF(T20&gt;=3,"B",IF(T20&gt;=2,"C",IF(T20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2271,31 +2278,31 @@
       <c r="M21" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="N21" s="3" t="n">
-        <v>81</v>
+      <c r="N21" s="8" t="n">
+        <v>36</v>
       </c>
       <c r="O21" s="2" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P21" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q21" s="2" t="n">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="Q21" s="3" t="n">
+        <v>84</v>
       </c>
       <c r="R21">
         <f>SUM(C21:N21)</f>
         <v/>
       </c>
-      <c r="S21" s="4">
-        <f>ROUND(R21/12,2)</f>
-        <v/>
-      </c>
-      <c r="T21" s="5">
-        <f>IF(OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,(J21+K21)&lt;66,L21&lt;33,M21&lt;33,N21&lt;33,P21&lt;33,Q21&lt;33),0,MIN(5,ROUND((IF((C21+D21)/200*100&gt;=80,5,IF((C21+D21)/200*100&gt;=70,4,IF((C21+D21)/200*100&gt;=60,3.5,IF((C21+D21)/200*100&gt;=50,3,IF((C21+D21)/200*100&gt;=40,2,IF((C21+D21)/200*100&gt;=33,1,0))))))+IF((E21+F21)/200*100&gt;=80,5,IF((E21+F21)/200*100&gt;=70,4,IF((E21+F21)/200*100&gt;=60,3.5,IF((E21+F21)/200*100&gt;=50,3,IF((E21+F21)/200*100&gt;=40,2,IF((E21+F21)/200*100&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF((H21+I21)/200*100&gt;=80,5,IF((H21+I21)/200*100&gt;=70,4,IF((H21+I21)/200*100&gt;=60,3.5,IF((H21+I21)/200*100&gt;=50,3,IF((H21+I21)/200*100&gt;=40,2,IF((H21+I21)/200*100&gt;=33,1,0))))))+IF((J21+K21)/200*100&gt;=80,5,IF((J21+K21)/200*100&gt;=70,4,IF((J21+K21)/200*100&gt;=60,3.5,IF((J21+K21)/200*100&gt;=50,3,IF((J21+K21)/200*100&gt;=40,2,IF((J21+K21)/200*100&gt;=33,1,0))))))+IF(L21&gt;=80,5,IF(L21&gt;=70,4,IF(L21&gt;=60,3.5,IF(L21&gt;=50,3,IF(L21&gt;=40,2,IF(L21&gt;=33,1,0))))))+IF(M21&gt;=80,5,IF(M21&gt;=70,4,IF(M21&gt;=60,3.5,IF(M21&gt;=50,3,IF(M21&gt;=40,2,IF(M21&gt;=33,1,0))))))+IF(N21&gt;=80,5,IF(N21&gt;=70,4,IF(N21&gt;=60,3.5,IF(N21&gt;=50,3,IF(N21&gt;=40,2,IF(N21&gt;=33,1,0)))))))/8+IF(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))&gt;=2,(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U21" s="6">
+      <c r="S21" s="5">
+        <f>ROUND(R21/11.5,2)</f>
+        <v/>
+      </c>
+      <c r="T21" s="6">
+        <f>IF(OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,(J21+K21)&lt;66,L21&lt;33,M21&lt;33,N21&lt;8.25,P21&lt;33,Q21&lt;33),0,MIN(5,ROUND((IF((C21+D21)/200*100&gt;=80,5,IF((C21+D21)/200*100&gt;=70,4,IF((C21+D21)/200*100&gt;=60,3.5,IF((C21+D21)/200*100&gt;=50,3,IF((C21+D21)/200*100&gt;=40,2,IF((C21+D21)/200*100&gt;=33,1,0))))))+IF((E21+F21)/200*100&gt;=80,5,IF((E21+F21)/200*100&gt;=70,4,IF((E21+F21)/200*100&gt;=60,3.5,IF((E21+F21)/200*100&gt;=50,3,IF((E21+F21)/200*100&gt;=40,2,IF((E21+F21)/200*100&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF((H21+I21)/200*100&gt;=80,5,IF((H21+I21)/200*100&gt;=70,4,IF((H21+I21)/200*100&gt;=60,3.5,IF((H21+I21)/200*100&gt;=50,3,IF((H21+I21)/200*100&gt;=40,2,IF((H21+I21)/200*100&gt;=33,1,0))))))+IF((J21+K21)/200*100&gt;=80,5,IF((J21+K21)/200*100&gt;=70,4,IF((J21+K21)/200*100&gt;=60,3.5,IF((J21+K21)/200*100&gt;=50,3,IF((J21+K21)/200*100&gt;=40,2,IF((J21+K21)/200*100&gt;=33,1,0))))))+IF(L21&gt;=80,5,IF(L21&gt;=70,4,IF(L21&gt;=60,3.5,IF(L21&gt;=50,3,IF(L21&gt;=40,2,IF(L21&gt;=33,1,0))))))+IF(M21&gt;=80,5,IF(M21&gt;=70,4,IF(M21&gt;=60,3.5,IF(M21&gt;=50,3,IF(M21&gt;=40,2,IF(M21&gt;=33,1,0))))))+IF(N21/50*100&gt;=80,5,IF(N21/50*100&gt;=70,4,IF(N21/50*100&gt;=60,3.5,IF(N21/50*100&gt;=50,3,IF(N21/50*100&gt;=40,2,IF(N21/50*100&gt;=33,1,0)))))))/8+IF(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))&gt;=2,(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U21" s="7">
         <f>IF(T21&gt;=5,"A+",IF(T21&gt;=4,"A",IF(T21&gt;=3.5,"A-",IF(T21&gt;=3,"B",IF(T21&gt;=2,"C",IF(T21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2327,7 +2334,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>📊 ACADEMIC RESULTS DASHBOARD</t>
         </is>
@@ -2335,116 +2342,116 @@
     </row>
     <row r="2"/>
     <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>SUMMARY STATISTICS</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="10" t="inlineStr">
+      <c r="B5" s="11" t="inlineStr">
         <is>
           <t>Total Students:</t>
         </is>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="12">
         <f>COUNTA('Data Source'!B:B)-1</f>
         <v/>
       </c>
-      <c r="E5" s="10" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>Average GPA:</t>
         </is>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="13">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!T:T),2), 0)</f>
         <v/>
       </c>
-      <c r="H5" s="10" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>Highest Total:</t>
         </is>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="12">
         <f>MAX('Data Source'!R:R)</f>
         <v/>
       </c>
-      <c r="K5" s="10" t="inlineStr">
+      <c r="K5" s="11" t="inlineStr">
         <is>
           <t>Pass Rate:</t>
         </is>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="14">
         <f>IF(C5&gt;0,COUNTIF('Data Source'!T:T,"&gt;0")/C5,0)</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="inlineStr">
+      <c r="A7" s="15" t="inlineStr">
         <is>
           <t>GRADE DISTRIBUTION</t>
         </is>
       </c>
-      <c r="D7" s="14" t="inlineStr">
+      <c r="D7" s="15" t="inlineStr">
         <is>
           <t>SUBJECT-WISE AVERAGE</t>
         </is>
       </c>
-      <c r="G7" s="14" t="inlineStr">
+      <c r="G7" s="15" t="inlineStr">
         <is>
           <t>TOP 5 STUDENTS</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="inlineStr">
+      <c r="A8" s="16" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
       </c>
-      <c r="B8" s="15" t="inlineStr">
+      <c r="B8" s="16" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="11" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="E8" s="15" t="inlineStr">
+      <c r="E8" s="16" t="inlineStr">
         <is>
           <t>Avg</t>
         </is>
       </c>
-      <c r="F8" s="15" t="inlineStr">
+      <c r="F8" s="16" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="G8" s="15" t="inlineStr">
+      <c r="G8" s="16" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
-      <c r="H8" s="10" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="I8" s="15" t="inlineStr">
+      <c r="I8" s="16" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"A+")</f>
         <v/>
       </c>
@@ -2453,33 +2460,33 @@
           <t>Quran Mazid</t>
         </is>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!C:C),2),0)</f>
         <v/>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="17">
         <f>IFERROR(ROUND(E9/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H9">
-        <f>'Data Source'!B11</f>
-        <v/>
-      </c>
-      <c r="I9" s="5">
-        <f>'Data Source'!T11</f>
+        <f>'Data Source'!B4</f>
+        <v/>
+      </c>
+      <c r="I9" s="6">
+        <f>'Data Source'!T4</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"A")</f>
         <v/>
       </c>
@@ -2488,33 +2495,33 @@
           <t>Arabic (Comb.)</t>
         </is>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!D:D),2),0)</f>
         <v/>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="17">
         <f>IFERROR(ROUND(E10/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="7" t="n">
         <v>2</v>
       </c>
       <c r="H10">
-        <f>'Data Source'!B4</f>
-        <v/>
-      </c>
-      <c r="I10" s="5">
-        <f>'Data Source'!T4</f>
+        <f>'Data Source'!B5</f>
+        <v/>
+      </c>
+      <c r="I10" s="6">
+        <f>'Data Source'!T5</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>A-</t>
         </is>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"A-")</f>
         <v/>
       </c>
@@ -2523,33 +2530,33 @@
           <t>Aqaid</t>
         </is>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!E:E),2),0)</f>
         <v/>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="17">
         <f>IFERROR(ROUND(E11/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="7" t="n">
         <v>3</v>
       </c>
       <c r="H11">
-        <f>'Data Source'!B21</f>
-        <v/>
-      </c>
-      <c r="I11" s="5">
-        <f>'Data Source'!T21</f>
+        <f>'Data Source'!B15</f>
+        <v/>
+      </c>
+      <c r="I11" s="6">
+        <f>'Data Source'!T15</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"B")</f>
         <v/>
       </c>
@@ -2558,68 +2565,68 @@
           <t>English (Comb.)</t>
         </is>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!F:F),2),0)</f>
         <v/>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="17">
         <f>IFERROR(ROUND(E12/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G12" s="6" t="n">
+      <c r="G12" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H12">
+        <f>'Data Source'!B17</f>
+        <v/>
+      </c>
+      <c r="I12" s="6">
+        <f>'Data Source'!T17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B13" s="7">
+        <f>COUNTIF('Data Source'!Q:Q,"C")</f>
+        <v/>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bangla (Comb.)</t>
+        </is>
+      </c>
+      <c r="E13" s="6">
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!G:G),2),0)</f>
+        <v/>
+      </c>
+      <c r="F13" s="17">
+        <f>IFERROR(ROUND(E13/200*100,1),0)</f>
+        <v/>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13">
         <f>'Data Source'!B6</f>
         <v/>
       </c>
-      <c r="I12" s="5">
+      <c r="I13" s="6">
         <f>'Data Source'!T6</f>
         <v/>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="B13" s="6">
-        <f>COUNTIF('Data Source'!Q:Q,"C")</f>
-        <v/>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Bangla (Comb.)</t>
-        </is>
-      </c>
-      <c r="E13" s="5">
-        <f>IFERROR(ROUND(AVERAGE('Data Source'!G:G),2),0)</f>
-        <v/>
-      </c>
-      <c r="F13" s="16">
-        <f>IFERROR(ROUND(E13/200*100,1),0)</f>
-        <v/>
-      </c>
-      <c r="G13" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <f>'Data Source'!B8</f>
-        <v/>
-      </c>
-      <c r="I13" s="5">
-        <f>'Data Source'!T8</f>
-        <v/>
-      </c>
-    </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"D")</f>
         <v/>
       </c>
@@ -2628,22 +2635,22 @@
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!H:H),2),0)</f>
         <v/>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="17">
         <f>IFERROR(ROUND(E14/100*100,1),0)</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="inlineStr">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="7">
         <f>COUNTIF('Data Source'!Q:Q,"F")</f>
         <v/>
       </c>
@@ -2652,11 +2659,11 @@
           <t>Islamic History</t>
         </is>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!I:I),2),0)</f>
         <v/>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="17">
         <f>IFERROR(ROUND(E15/100*100,1),0)</f>
         <v/>
       </c>
@@ -2667,11 +2674,11 @@
           <t>ICT</t>
         </is>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!J:J),2),0)</f>
         <v/>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="17">
         <f>IFERROR(ROUND(E16/100*100,1),0)</f>
         <v/>
       </c>
@@ -2682,11 +2689,11 @@
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!K:K),2),0)</f>
         <v/>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="17">
         <f>IFERROR(ROUND(E17/100*100,1),0)</f>
         <v/>
       </c>
@@ -2732,91 +2739,91 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="17" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>SUBJECT-WISE GRADES</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="18" t="inlineStr">
+      <c r="A2" s="19" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="B2" s="18" t="inlineStr">
+      <c r="B2" s="19" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C2" s="18" t="inlineStr">
+      <c r="C2" s="19" t="inlineStr">
         <is>
           <t>Quran+Hadith</t>
         </is>
       </c>
-      <c r="D2" s="18" t="inlineStr">
+      <c r="D2" s="19" t="inlineStr">
         <is>
           <t>Arabic</t>
         </is>
       </c>
-      <c r="E2" s="18" t="inlineStr">
+      <c r="E2" s="19" t="inlineStr">
         <is>
           <t>Aqaid</t>
         </is>
       </c>
-      <c r="F2" s="18" t="inlineStr">
+      <c r="F2" s="19" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="G2" s="18" t="inlineStr">
+      <c r="G2" s="19" t="inlineStr">
         <is>
           <t>Bangla</t>
         </is>
       </c>
-      <c r="H2" s="18" t="inlineStr">
+      <c r="H2" s="19" t="inlineStr">
         <is>
           <t>Math</t>
         </is>
       </c>
-      <c r="I2" s="18" t="inlineStr">
+      <c r="I2" s="19" t="inlineStr">
         <is>
           <t>History</t>
         </is>
       </c>
-      <c r="J2" s="18" t="inlineStr">
+      <c r="J2" s="19" t="inlineStr">
         <is>
           <t>ICT</t>
         </is>
       </c>
-      <c r="K2" s="18" t="inlineStr">
+      <c r="K2" s="19" t="inlineStr">
         <is>
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="L2" s="18" t="inlineStr">
+      <c r="L2" s="19" t="inlineStr">
         <is>
           <t>Career</t>
         </is>
       </c>
-      <c r="M2" s="18" t="inlineStr">
+      <c r="M2" s="19" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
-      <c r="N2" s="18" t="inlineStr">
+      <c r="N2" s="19" t="inlineStr">
         <is>
           <t>Overall GPA</t>
         </is>
       </c>
-      <c r="O2" s="18" t="inlineStr">
+      <c r="O2" s="19" t="inlineStr">
         <is>
           <t>Overall Grade</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <f>'Data Source'!A2</f>
         <v/>
       </c>
@@ -2824,61 +2831,61 @@
         <f>'Data Source'!B2</f>
         <v/>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <f>IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=80,"A+",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=70,"A",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=60,"A-",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=50,"B",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=40,"C",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <f>IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=80,"A+",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=70,"A",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=60,"A-",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=50,"B",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=40,"C",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <f>IF('Data Source'!G2&gt;=80,"A+",IF('Data Source'!G2&gt;=70,"A",IF('Data Source'!G2&gt;=60,"A-",IF('Data Source'!G2&gt;=50,"B",IF('Data Source'!G2&gt;=40,"C",IF('Data Source'!G2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <f>IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=80,"A+",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=70,"A",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=60,"A-",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=50,"B",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=40,"C",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <f>IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=80,"A+",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=70,"A",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=60,"A-",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=50,"B",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=40,"C",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <f>IF('Data Source'!L2&gt;=80,"A+",IF('Data Source'!L2&gt;=70,"A",IF('Data Source'!L2&gt;=60,"A-",IF('Data Source'!L2&gt;=50,"B",IF('Data Source'!L2&gt;=40,"C",IF('Data Source'!L2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="7">
         <f>IF('Data Source'!M2&gt;=80,"A+",IF('Data Source'!M2&gt;=70,"A",IF('Data Source'!M2&gt;=60,"A-",IF('Data Source'!M2&gt;=50,"B",IF('Data Source'!M2&gt;=40,"C",IF('Data Source'!M2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J3" s="6">
-        <f>IF('Data Source'!N2&gt;=80,"A+",IF('Data Source'!N2&gt;=70,"A",IF('Data Source'!N2&gt;=60,"A-",IF('Data Source'!N2&gt;=50,"B",IF('Data Source'!N2&gt;=40,"C",IF('Data Source'!N2&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K3" s="6">
+      <c r="J3" s="7">
+        <f>IF('Data Source'!N2/50*100&gt;=80,"A+",IF('Data Source'!N2/50*100&gt;=70,"A",IF('Data Source'!N2/50*100&gt;=60,"A-",IF('Data Source'!N2/50*100&gt;=50,"B",IF('Data Source'!N2/50*100&gt;=40,"C",IF('Data Source'!N2/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K3" s="7">
         <f>IF('Data Source'!O2&gt;=80,"A+",IF('Data Source'!O2&gt;=70,"A",IF('Data Source'!O2&gt;=60,"A-",IF('Data Source'!O2&gt;=50,"B",IF('Data Source'!O2&gt;=40,"C",IF('Data Source'!O2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <f>IF('Data Source'!P2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="7">
         <f>IF('Data Source'!Q2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="6">
         <f>'Data Source'!T2</f>
         <v/>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="7">
         <f>'Data Source'!U2</f>
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <f>'Data Source'!A3</f>
         <v/>
       </c>
@@ -2886,61 +2893,61 @@
         <f>'Data Source'!B3</f>
         <v/>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <f>IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=80,"A+",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=70,"A",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=60,"A-",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=50,"B",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=40,"C",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <f>IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=80,"A+",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=70,"A",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=60,"A-",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=50,"B",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=40,"C",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <f>IF('Data Source'!G3&gt;=80,"A+",IF('Data Source'!G3&gt;=70,"A",IF('Data Source'!G3&gt;=60,"A-",IF('Data Source'!G3&gt;=50,"B",IF('Data Source'!G3&gt;=40,"C",IF('Data Source'!G3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <f>IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=80,"A+",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=70,"A",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=60,"A-",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=50,"B",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=40,"C",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <f>IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=80,"A+",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=70,"A",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=60,"A-",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=50,"B",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=40,"C",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <f>IF('Data Source'!L3&gt;=80,"A+",IF('Data Source'!L3&gt;=70,"A",IF('Data Source'!L3&gt;=60,"A-",IF('Data Source'!L3&gt;=50,"B",IF('Data Source'!L3&gt;=40,"C",IF('Data Source'!L3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="7">
         <f>IF('Data Source'!M3&gt;=80,"A+",IF('Data Source'!M3&gt;=70,"A",IF('Data Source'!M3&gt;=60,"A-",IF('Data Source'!M3&gt;=50,"B",IF('Data Source'!M3&gt;=40,"C",IF('Data Source'!M3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J4" s="6">
-        <f>IF('Data Source'!N3&gt;=80,"A+",IF('Data Source'!N3&gt;=70,"A",IF('Data Source'!N3&gt;=60,"A-",IF('Data Source'!N3&gt;=50,"B",IF('Data Source'!N3&gt;=40,"C",IF('Data Source'!N3&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K4" s="6">
+      <c r="J4" s="7">
+        <f>IF('Data Source'!N3/50*100&gt;=80,"A+",IF('Data Source'!N3/50*100&gt;=70,"A",IF('Data Source'!N3/50*100&gt;=60,"A-",IF('Data Source'!N3/50*100&gt;=50,"B",IF('Data Source'!N3/50*100&gt;=40,"C",IF('Data Source'!N3/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K4" s="7">
         <f>IF('Data Source'!O3&gt;=80,"A+",IF('Data Source'!O3&gt;=70,"A",IF('Data Source'!O3&gt;=60,"A-",IF('Data Source'!O3&gt;=50,"B",IF('Data Source'!O3&gt;=40,"C",IF('Data Source'!O3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="7">
         <f>IF('Data Source'!P3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="7">
         <f>IF('Data Source'!Q3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="6">
         <f>'Data Source'!T3</f>
         <v/>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="7">
         <f>'Data Source'!U3</f>
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <f>'Data Source'!A4</f>
         <v/>
       </c>
@@ -2948,61 +2955,61 @@
         <f>'Data Source'!B4</f>
         <v/>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <f>IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=80,"A+",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=70,"A",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=60,"A-",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=50,"B",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=40,"C",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <f>IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=80,"A+",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=70,"A",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=60,"A-",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=50,"B",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=40,"C",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <f>IF('Data Source'!G4&gt;=80,"A+",IF('Data Source'!G4&gt;=70,"A",IF('Data Source'!G4&gt;=60,"A-",IF('Data Source'!G4&gt;=50,"B",IF('Data Source'!G4&gt;=40,"C",IF('Data Source'!G4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <f>IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=80,"A+",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=70,"A",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=60,"A-",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=50,"B",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=40,"C",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <f>IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=80,"A+",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=70,"A",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=60,"A-",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=50,"B",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=40,"C",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7">
         <f>IF('Data Source'!L4&gt;=80,"A+",IF('Data Source'!L4&gt;=70,"A",IF('Data Source'!L4&gt;=60,"A-",IF('Data Source'!L4&gt;=50,"B",IF('Data Source'!L4&gt;=40,"C",IF('Data Source'!L4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="7">
         <f>IF('Data Source'!M4&gt;=80,"A+",IF('Data Source'!M4&gt;=70,"A",IF('Data Source'!M4&gt;=60,"A-",IF('Data Source'!M4&gt;=50,"B",IF('Data Source'!M4&gt;=40,"C",IF('Data Source'!M4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J5" s="6">
-        <f>IF('Data Source'!N4&gt;=80,"A+",IF('Data Source'!N4&gt;=70,"A",IF('Data Source'!N4&gt;=60,"A-",IF('Data Source'!N4&gt;=50,"B",IF('Data Source'!N4&gt;=40,"C",IF('Data Source'!N4&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K5" s="6">
+      <c r="J5" s="7">
+        <f>IF('Data Source'!N4/50*100&gt;=80,"A+",IF('Data Source'!N4/50*100&gt;=70,"A",IF('Data Source'!N4/50*100&gt;=60,"A-",IF('Data Source'!N4/50*100&gt;=50,"B",IF('Data Source'!N4/50*100&gt;=40,"C",IF('Data Source'!N4/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K5" s="7">
         <f>IF('Data Source'!O4&gt;=80,"A+",IF('Data Source'!O4&gt;=70,"A",IF('Data Source'!O4&gt;=60,"A-",IF('Data Source'!O4&gt;=50,"B",IF('Data Source'!O4&gt;=40,"C",IF('Data Source'!O4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="7">
         <f>IF('Data Source'!P4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="7">
         <f>IF('Data Source'!Q4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="6">
         <f>'Data Source'!T4</f>
         <v/>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="7">
         <f>'Data Source'!U4</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <f>'Data Source'!A5</f>
         <v/>
       </c>
@@ -3010,61 +3017,61 @@
         <f>'Data Source'!B5</f>
         <v/>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <f>IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=80,"A+",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=70,"A",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=60,"A-",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=50,"B",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=40,"C",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <f>IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=80,"A+",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=70,"A",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=60,"A-",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=50,"B",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=40,"C",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <f>IF('Data Source'!G5&gt;=80,"A+",IF('Data Source'!G5&gt;=70,"A",IF('Data Source'!G5&gt;=60,"A-",IF('Data Source'!G5&gt;=50,"B",IF('Data Source'!G5&gt;=40,"C",IF('Data Source'!G5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <f>IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=80,"A+",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=70,"A",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=60,"A-",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=50,"B",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=40,"C",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <f>IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=80,"A+",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=70,"A",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=60,"A-",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=50,"B",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=40,"C",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="7">
         <f>IF('Data Source'!L5&gt;=80,"A+",IF('Data Source'!L5&gt;=70,"A",IF('Data Source'!L5&gt;=60,"A-",IF('Data Source'!L5&gt;=50,"B",IF('Data Source'!L5&gt;=40,"C",IF('Data Source'!L5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="7">
         <f>IF('Data Source'!M5&gt;=80,"A+",IF('Data Source'!M5&gt;=70,"A",IF('Data Source'!M5&gt;=60,"A-",IF('Data Source'!M5&gt;=50,"B",IF('Data Source'!M5&gt;=40,"C",IF('Data Source'!M5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J6" s="6">
-        <f>IF('Data Source'!N5&gt;=80,"A+",IF('Data Source'!N5&gt;=70,"A",IF('Data Source'!N5&gt;=60,"A-",IF('Data Source'!N5&gt;=50,"B",IF('Data Source'!N5&gt;=40,"C",IF('Data Source'!N5&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K6" s="6">
+      <c r="J6" s="7">
+        <f>IF('Data Source'!N5/50*100&gt;=80,"A+",IF('Data Source'!N5/50*100&gt;=70,"A",IF('Data Source'!N5/50*100&gt;=60,"A-",IF('Data Source'!N5/50*100&gt;=50,"B",IF('Data Source'!N5/50*100&gt;=40,"C",IF('Data Source'!N5/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K6" s="7">
         <f>IF('Data Source'!O5&gt;=80,"A+",IF('Data Source'!O5&gt;=70,"A",IF('Data Source'!O5&gt;=60,"A-",IF('Data Source'!O5&gt;=50,"B",IF('Data Source'!O5&gt;=40,"C",IF('Data Source'!O5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="7">
         <f>IF('Data Source'!P5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <f>IF('Data Source'!Q5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="6">
         <f>'Data Source'!T5</f>
         <v/>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="7">
         <f>'Data Source'!U5</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <f>'Data Source'!A6</f>
         <v/>
       </c>
@@ -3072,61 +3079,61 @@
         <f>'Data Source'!B6</f>
         <v/>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <f>IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=80,"A+",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=70,"A",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=60,"A-",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=50,"B",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=40,"C",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <f>IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=80,"A+",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=70,"A",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=60,"A-",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=50,"B",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=40,"C",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <f>IF('Data Source'!G6&gt;=80,"A+",IF('Data Source'!G6&gt;=70,"A",IF('Data Source'!G6&gt;=60,"A-",IF('Data Source'!G6&gt;=50,"B",IF('Data Source'!G6&gt;=40,"C",IF('Data Source'!G6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <f>IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=80,"A+",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=70,"A",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=60,"A-",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=50,"B",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=40,"C",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <f>IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=80,"A+",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=70,"A",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=60,"A-",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=50,"B",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=40,"C",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="7">
         <f>IF('Data Source'!L6&gt;=80,"A+",IF('Data Source'!L6&gt;=70,"A",IF('Data Source'!L6&gt;=60,"A-",IF('Data Source'!L6&gt;=50,"B",IF('Data Source'!L6&gt;=40,"C",IF('Data Source'!L6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="7">
         <f>IF('Data Source'!M6&gt;=80,"A+",IF('Data Source'!M6&gt;=70,"A",IF('Data Source'!M6&gt;=60,"A-",IF('Data Source'!M6&gt;=50,"B",IF('Data Source'!M6&gt;=40,"C",IF('Data Source'!M6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J7" s="6">
-        <f>IF('Data Source'!N6&gt;=80,"A+",IF('Data Source'!N6&gt;=70,"A",IF('Data Source'!N6&gt;=60,"A-",IF('Data Source'!N6&gt;=50,"B",IF('Data Source'!N6&gt;=40,"C",IF('Data Source'!N6&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K7" s="6">
+      <c r="J7" s="7">
+        <f>IF('Data Source'!N6/50*100&gt;=80,"A+",IF('Data Source'!N6/50*100&gt;=70,"A",IF('Data Source'!N6/50*100&gt;=60,"A-",IF('Data Source'!N6/50*100&gt;=50,"B",IF('Data Source'!N6/50*100&gt;=40,"C",IF('Data Source'!N6/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K7" s="7">
         <f>IF('Data Source'!O6&gt;=80,"A+",IF('Data Source'!O6&gt;=70,"A",IF('Data Source'!O6&gt;=60,"A-",IF('Data Source'!O6&gt;=50,"B",IF('Data Source'!O6&gt;=40,"C",IF('Data Source'!O6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="7">
         <f>IF('Data Source'!P6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="7">
         <f>IF('Data Source'!Q6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="6">
         <f>'Data Source'!T6</f>
         <v/>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="7">
         <f>'Data Source'!U6</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <f>'Data Source'!A7</f>
         <v/>
       </c>
@@ -3134,61 +3141,61 @@
         <f>'Data Source'!B7</f>
         <v/>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <f>IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=80,"A+",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=70,"A",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=60,"A-",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=50,"B",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=40,"C",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <f>IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=80,"A+",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=70,"A",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=60,"A-",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=50,"B",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=40,"C",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <f>IF('Data Source'!G7&gt;=80,"A+",IF('Data Source'!G7&gt;=70,"A",IF('Data Source'!G7&gt;=60,"A-",IF('Data Source'!G7&gt;=50,"B",IF('Data Source'!G7&gt;=40,"C",IF('Data Source'!G7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <f>IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=80,"A+",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=70,"A",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=60,"A-",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=50,"B",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=40,"C",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <f>IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=80,"A+",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=70,"A",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=60,"A-",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=50,"B",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=40,"C",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="7">
         <f>IF('Data Source'!L7&gt;=80,"A+",IF('Data Source'!L7&gt;=70,"A",IF('Data Source'!L7&gt;=60,"A-",IF('Data Source'!L7&gt;=50,"B",IF('Data Source'!L7&gt;=40,"C",IF('Data Source'!L7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="7">
         <f>IF('Data Source'!M7&gt;=80,"A+",IF('Data Source'!M7&gt;=70,"A",IF('Data Source'!M7&gt;=60,"A-",IF('Data Source'!M7&gt;=50,"B",IF('Data Source'!M7&gt;=40,"C",IF('Data Source'!M7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J8" s="6">
-        <f>IF('Data Source'!N7&gt;=80,"A+",IF('Data Source'!N7&gt;=70,"A",IF('Data Source'!N7&gt;=60,"A-",IF('Data Source'!N7&gt;=50,"B",IF('Data Source'!N7&gt;=40,"C",IF('Data Source'!N7&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K8" s="6">
+      <c r="J8" s="7">
+        <f>IF('Data Source'!N7/50*100&gt;=80,"A+",IF('Data Source'!N7/50*100&gt;=70,"A",IF('Data Source'!N7/50*100&gt;=60,"A-",IF('Data Source'!N7/50*100&gt;=50,"B",IF('Data Source'!N7/50*100&gt;=40,"C",IF('Data Source'!N7/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K8" s="7">
         <f>IF('Data Source'!O7&gt;=80,"A+",IF('Data Source'!O7&gt;=70,"A",IF('Data Source'!O7&gt;=60,"A-",IF('Data Source'!O7&gt;=50,"B",IF('Data Source'!O7&gt;=40,"C",IF('Data Source'!O7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="7">
         <f>IF('Data Source'!P7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="7">
         <f>IF('Data Source'!Q7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="6">
         <f>'Data Source'!T7</f>
         <v/>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="7">
         <f>'Data Source'!U7</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <f>'Data Source'!A8</f>
         <v/>
       </c>
@@ -3196,61 +3203,61 @@
         <f>'Data Source'!B8</f>
         <v/>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <f>IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=80,"A+",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=70,"A",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=60,"A-",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=50,"B",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=40,"C",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <f>IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=80,"A+",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=70,"A",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=60,"A-",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=50,"B",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=40,"C",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <f>IF('Data Source'!G8&gt;=80,"A+",IF('Data Source'!G8&gt;=70,"A",IF('Data Source'!G8&gt;=60,"A-",IF('Data Source'!G8&gt;=50,"B",IF('Data Source'!G8&gt;=40,"C",IF('Data Source'!G8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <f>IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=80,"A+",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=70,"A",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=60,"A-",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=50,"B",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=40,"C",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="7">
         <f>IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=80,"A+",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=70,"A",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=60,"A-",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=50,"B",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=40,"C",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="7">
         <f>IF('Data Source'!L8&gt;=80,"A+",IF('Data Source'!L8&gt;=70,"A",IF('Data Source'!L8&gt;=60,"A-",IF('Data Source'!L8&gt;=50,"B",IF('Data Source'!L8&gt;=40,"C",IF('Data Source'!L8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="7">
         <f>IF('Data Source'!M8&gt;=80,"A+",IF('Data Source'!M8&gt;=70,"A",IF('Data Source'!M8&gt;=60,"A-",IF('Data Source'!M8&gt;=50,"B",IF('Data Source'!M8&gt;=40,"C",IF('Data Source'!M8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J9" s="6">
-        <f>IF('Data Source'!N8&gt;=80,"A+",IF('Data Source'!N8&gt;=70,"A",IF('Data Source'!N8&gt;=60,"A-",IF('Data Source'!N8&gt;=50,"B",IF('Data Source'!N8&gt;=40,"C",IF('Data Source'!N8&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K9" s="6">
+      <c r="J9" s="7">
+        <f>IF('Data Source'!N8/50*100&gt;=80,"A+",IF('Data Source'!N8/50*100&gt;=70,"A",IF('Data Source'!N8/50*100&gt;=60,"A-",IF('Data Source'!N8/50*100&gt;=50,"B",IF('Data Source'!N8/50*100&gt;=40,"C",IF('Data Source'!N8/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K9" s="7">
         <f>IF('Data Source'!O8&gt;=80,"A+",IF('Data Source'!O8&gt;=70,"A",IF('Data Source'!O8&gt;=60,"A-",IF('Data Source'!O8&gt;=50,"B",IF('Data Source'!O8&gt;=40,"C",IF('Data Source'!O8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="7">
         <f>IF('Data Source'!P8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="7">
         <f>IF('Data Source'!Q8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="6">
         <f>'Data Source'!T8</f>
         <v/>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="7">
         <f>'Data Source'!U8</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <f>'Data Source'!A9</f>
         <v/>
       </c>
@@ -3258,61 +3265,61 @@
         <f>'Data Source'!B9</f>
         <v/>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <f>IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=80,"A+",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=70,"A",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=60,"A-",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=50,"B",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=40,"C",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="7">
         <f>IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=80,"A+",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=70,"A",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=60,"A-",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=50,"B",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=40,"C",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <f>IF('Data Source'!G9&gt;=80,"A+",IF('Data Source'!G9&gt;=70,"A",IF('Data Source'!G9&gt;=60,"A-",IF('Data Source'!G9&gt;=50,"B",IF('Data Source'!G9&gt;=40,"C",IF('Data Source'!G9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="7">
         <f>IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=80,"A+",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=70,"A",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=60,"A-",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=50,"B",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=40,"C",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <f>IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=80,"A+",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=70,"A",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=60,"A-",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=50,"B",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=40,"C",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="7">
         <f>IF('Data Source'!L9&gt;=80,"A+",IF('Data Source'!L9&gt;=70,"A",IF('Data Source'!L9&gt;=60,"A-",IF('Data Source'!L9&gt;=50,"B",IF('Data Source'!L9&gt;=40,"C",IF('Data Source'!L9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="7">
         <f>IF('Data Source'!M9&gt;=80,"A+",IF('Data Source'!M9&gt;=70,"A",IF('Data Source'!M9&gt;=60,"A-",IF('Data Source'!M9&gt;=50,"B",IF('Data Source'!M9&gt;=40,"C",IF('Data Source'!M9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J10" s="6">
-        <f>IF('Data Source'!N9&gt;=80,"A+",IF('Data Source'!N9&gt;=70,"A",IF('Data Source'!N9&gt;=60,"A-",IF('Data Source'!N9&gt;=50,"B",IF('Data Source'!N9&gt;=40,"C",IF('Data Source'!N9&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K10" s="6">
+      <c r="J10" s="7">
+        <f>IF('Data Source'!N9/50*100&gt;=80,"A+",IF('Data Source'!N9/50*100&gt;=70,"A",IF('Data Source'!N9/50*100&gt;=60,"A-",IF('Data Source'!N9/50*100&gt;=50,"B",IF('Data Source'!N9/50*100&gt;=40,"C",IF('Data Source'!N9/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K10" s="7">
         <f>IF('Data Source'!O9&gt;=80,"A+",IF('Data Source'!O9&gt;=70,"A",IF('Data Source'!O9&gt;=60,"A-",IF('Data Source'!O9&gt;=50,"B",IF('Data Source'!O9&gt;=40,"C",IF('Data Source'!O9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="7">
         <f>IF('Data Source'!P9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="7">
         <f>IF('Data Source'!Q9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="6">
         <f>'Data Source'!T9</f>
         <v/>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="7">
         <f>'Data Source'!U9</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="7">
         <f>'Data Source'!A10</f>
         <v/>
       </c>
@@ -3320,61 +3327,61 @@
         <f>'Data Source'!B10</f>
         <v/>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <f>IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=80,"A+",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=70,"A",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=60,"A-",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=50,"B",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=40,"C",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <f>IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=80,"A+",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=70,"A",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=60,"A-",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=50,"B",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=40,"C",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <f>IF('Data Source'!G10&gt;=80,"A+",IF('Data Source'!G10&gt;=70,"A",IF('Data Source'!G10&gt;=60,"A-",IF('Data Source'!G10&gt;=50,"B",IF('Data Source'!G10&gt;=40,"C",IF('Data Source'!G10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="7">
         <f>IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=80,"A+",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=70,"A",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=60,"A-",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=50,"B",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=40,"C",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="7">
         <f>IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=80,"A+",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=70,"A",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=60,"A-",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=50,"B",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=40,"C",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="7">
         <f>IF('Data Source'!L10&gt;=80,"A+",IF('Data Source'!L10&gt;=70,"A",IF('Data Source'!L10&gt;=60,"A-",IF('Data Source'!L10&gt;=50,"B",IF('Data Source'!L10&gt;=40,"C",IF('Data Source'!L10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="7">
         <f>IF('Data Source'!M10&gt;=80,"A+",IF('Data Source'!M10&gt;=70,"A",IF('Data Source'!M10&gt;=60,"A-",IF('Data Source'!M10&gt;=50,"B",IF('Data Source'!M10&gt;=40,"C",IF('Data Source'!M10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J11" s="6">
-        <f>IF('Data Source'!N10&gt;=80,"A+",IF('Data Source'!N10&gt;=70,"A",IF('Data Source'!N10&gt;=60,"A-",IF('Data Source'!N10&gt;=50,"B",IF('Data Source'!N10&gt;=40,"C",IF('Data Source'!N10&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K11" s="6">
+      <c r="J11" s="7">
+        <f>IF('Data Source'!N10/50*100&gt;=80,"A+",IF('Data Source'!N10/50*100&gt;=70,"A",IF('Data Source'!N10/50*100&gt;=60,"A-",IF('Data Source'!N10/50*100&gt;=50,"B",IF('Data Source'!N10/50*100&gt;=40,"C",IF('Data Source'!N10/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K11" s="7">
         <f>IF('Data Source'!O10&gt;=80,"A+",IF('Data Source'!O10&gt;=70,"A",IF('Data Source'!O10&gt;=60,"A-",IF('Data Source'!O10&gt;=50,"B",IF('Data Source'!O10&gt;=40,"C",IF('Data Source'!O10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="7">
         <f>IF('Data Source'!P10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="7">
         <f>IF('Data Source'!Q10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="6">
         <f>'Data Source'!T10</f>
         <v/>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="7">
         <f>'Data Source'!U10</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <f>'Data Source'!A11</f>
         <v/>
       </c>
@@ -3382,61 +3389,61 @@
         <f>'Data Source'!B11</f>
         <v/>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <f>IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=80,"A+",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=70,"A",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=60,"A-",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=50,"B",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=40,"C",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="7">
         <f>IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=80,"A+",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=70,"A",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=60,"A-",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=50,"B",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=40,"C",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <f>IF('Data Source'!G11&gt;=80,"A+",IF('Data Source'!G11&gt;=70,"A",IF('Data Source'!G11&gt;=60,"A-",IF('Data Source'!G11&gt;=50,"B",IF('Data Source'!G11&gt;=40,"C",IF('Data Source'!G11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <f>IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=80,"A+",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=70,"A",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=60,"A-",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=50,"B",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=40,"C",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="7">
         <f>IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=80,"A+",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=70,"A",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=60,"A-",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=50,"B",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=40,"C",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="7">
         <f>IF('Data Source'!L11&gt;=80,"A+",IF('Data Source'!L11&gt;=70,"A",IF('Data Source'!L11&gt;=60,"A-",IF('Data Source'!L11&gt;=50,"B",IF('Data Source'!L11&gt;=40,"C",IF('Data Source'!L11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="7">
         <f>IF('Data Source'!M11&gt;=80,"A+",IF('Data Source'!M11&gt;=70,"A",IF('Data Source'!M11&gt;=60,"A-",IF('Data Source'!M11&gt;=50,"B",IF('Data Source'!M11&gt;=40,"C",IF('Data Source'!M11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J12" s="6">
-        <f>IF('Data Source'!N11&gt;=80,"A+",IF('Data Source'!N11&gt;=70,"A",IF('Data Source'!N11&gt;=60,"A-",IF('Data Source'!N11&gt;=50,"B",IF('Data Source'!N11&gt;=40,"C",IF('Data Source'!N11&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K12" s="6">
+      <c r="J12" s="7">
+        <f>IF('Data Source'!N11/50*100&gt;=80,"A+",IF('Data Source'!N11/50*100&gt;=70,"A",IF('Data Source'!N11/50*100&gt;=60,"A-",IF('Data Source'!N11/50*100&gt;=50,"B",IF('Data Source'!N11/50*100&gt;=40,"C",IF('Data Source'!N11/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K12" s="7">
         <f>IF('Data Source'!O11&gt;=80,"A+",IF('Data Source'!O11&gt;=70,"A",IF('Data Source'!O11&gt;=60,"A-",IF('Data Source'!O11&gt;=50,"B",IF('Data Source'!O11&gt;=40,"C",IF('Data Source'!O11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="7">
         <f>IF('Data Source'!P11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="7">
         <f>IF('Data Source'!Q11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="6">
         <f>'Data Source'!T11</f>
         <v/>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="7">
         <f>'Data Source'!U11</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <f>'Data Source'!A12</f>
         <v/>
       </c>
@@ -3444,61 +3451,61 @@
         <f>'Data Source'!B12</f>
         <v/>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <f>IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=80,"A+",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=70,"A",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=60,"A-",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=50,"B",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=40,"C",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="7">
         <f>IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=80,"A+",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=70,"A",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=60,"A-",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=50,"B",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=40,"C",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <f>IF('Data Source'!G12&gt;=80,"A+",IF('Data Source'!G12&gt;=70,"A",IF('Data Source'!G12&gt;=60,"A-",IF('Data Source'!G12&gt;=50,"B",IF('Data Source'!G12&gt;=40,"C",IF('Data Source'!G12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <f>IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=80,"A+",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=70,"A",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=60,"A-",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=50,"B",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=40,"C",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <f>IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=80,"A+",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=70,"A",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=60,"A-",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=50,"B",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=40,"C",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="7">
         <f>IF('Data Source'!L12&gt;=80,"A+",IF('Data Source'!L12&gt;=70,"A",IF('Data Source'!L12&gt;=60,"A-",IF('Data Source'!L12&gt;=50,"B",IF('Data Source'!L12&gt;=40,"C",IF('Data Source'!L12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="7">
         <f>IF('Data Source'!M12&gt;=80,"A+",IF('Data Source'!M12&gt;=70,"A",IF('Data Source'!M12&gt;=60,"A-",IF('Data Source'!M12&gt;=50,"B",IF('Data Source'!M12&gt;=40,"C",IF('Data Source'!M12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J13" s="6">
-        <f>IF('Data Source'!N12&gt;=80,"A+",IF('Data Source'!N12&gt;=70,"A",IF('Data Source'!N12&gt;=60,"A-",IF('Data Source'!N12&gt;=50,"B",IF('Data Source'!N12&gt;=40,"C",IF('Data Source'!N12&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K13" s="6">
+      <c r="J13" s="7">
+        <f>IF('Data Source'!N12/50*100&gt;=80,"A+",IF('Data Source'!N12/50*100&gt;=70,"A",IF('Data Source'!N12/50*100&gt;=60,"A-",IF('Data Source'!N12/50*100&gt;=50,"B",IF('Data Source'!N12/50*100&gt;=40,"C",IF('Data Source'!N12/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K13" s="7">
         <f>IF('Data Source'!O12&gt;=80,"A+",IF('Data Source'!O12&gt;=70,"A",IF('Data Source'!O12&gt;=60,"A-",IF('Data Source'!O12&gt;=50,"B",IF('Data Source'!O12&gt;=40,"C",IF('Data Source'!O12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="7">
         <f>IF('Data Source'!P12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <f>IF('Data Source'!Q12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="6">
         <f>'Data Source'!T12</f>
         <v/>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="7">
         <f>'Data Source'!U12</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <f>'Data Source'!A13</f>
         <v/>
       </c>
@@ -3506,61 +3513,61 @@
         <f>'Data Source'!B13</f>
         <v/>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="7">
         <f>IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=80,"A+",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=70,"A",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=60,"A-",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=50,"B",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=40,"C",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="7">
         <f>IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=80,"A+",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=70,"A",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=60,"A-",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=50,"B",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=40,"C",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <f>IF('Data Source'!G13&gt;=80,"A+",IF('Data Source'!G13&gt;=70,"A",IF('Data Source'!G13&gt;=60,"A-",IF('Data Source'!G13&gt;=50,"B",IF('Data Source'!G13&gt;=40,"C",IF('Data Source'!G13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="7">
         <f>IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=80,"A+",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=70,"A",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=60,"A-",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=50,"B",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=40,"C",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="7">
         <f>IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=80,"A+",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=70,"A",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=60,"A-",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=50,"B",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=40,"C",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="7">
         <f>IF('Data Source'!L13&gt;=80,"A+",IF('Data Source'!L13&gt;=70,"A",IF('Data Source'!L13&gt;=60,"A-",IF('Data Source'!L13&gt;=50,"B",IF('Data Source'!L13&gt;=40,"C",IF('Data Source'!L13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="7">
         <f>IF('Data Source'!M13&gt;=80,"A+",IF('Data Source'!M13&gt;=70,"A",IF('Data Source'!M13&gt;=60,"A-",IF('Data Source'!M13&gt;=50,"B",IF('Data Source'!M13&gt;=40,"C",IF('Data Source'!M13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J14" s="6">
-        <f>IF('Data Source'!N13&gt;=80,"A+",IF('Data Source'!N13&gt;=70,"A",IF('Data Source'!N13&gt;=60,"A-",IF('Data Source'!N13&gt;=50,"B",IF('Data Source'!N13&gt;=40,"C",IF('Data Source'!N13&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K14" s="6">
+      <c r="J14" s="7">
+        <f>IF('Data Source'!N13/50*100&gt;=80,"A+",IF('Data Source'!N13/50*100&gt;=70,"A",IF('Data Source'!N13/50*100&gt;=60,"A-",IF('Data Source'!N13/50*100&gt;=50,"B",IF('Data Source'!N13/50*100&gt;=40,"C",IF('Data Source'!N13/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K14" s="7">
         <f>IF('Data Source'!O13&gt;=80,"A+",IF('Data Source'!O13&gt;=70,"A",IF('Data Source'!O13&gt;=60,"A-",IF('Data Source'!O13&gt;=50,"B",IF('Data Source'!O13&gt;=40,"C",IF('Data Source'!O13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="7">
         <f>IF('Data Source'!P13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="7">
         <f>IF('Data Source'!Q13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="6">
         <f>'Data Source'!T13</f>
         <v/>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="7">
         <f>'Data Source'!U13</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <f>'Data Source'!A14</f>
         <v/>
       </c>
@@ -3568,61 +3575,61 @@
         <f>'Data Source'!B14</f>
         <v/>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="7">
         <f>IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=80,"A+",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=70,"A",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=60,"A-",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=50,"B",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=40,"C",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="7">
         <f>IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=80,"A+",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=70,"A",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=60,"A-",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=50,"B",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=40,"C",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <f>IF('Data Source'!G14&gt;=80,"A+",IF('Data Source'!G14&gt;=70,"A",IF('Data Source'!G14&gt;=60,"A-",IF('Data Source'!G14&gt;=50,"B",IF('Data Source'!G14&gt;=40,"C",IF('Data Source'!G14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="7">
         <f>IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=80,"A+",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=70,"A",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=60,"A-",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=50,"B",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=40,"C",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="7">
         <f>IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=80,"A+",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=70,"A",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=60,"A-",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=50,"B",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=40,"C",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="7">
         <f>IF('Data Source'!L14&gt;=80,"A+",IF('Data Source'!L14&gt;=70,"A",IF('Data Source'!L14&gt;=60,"A-",IF('Data Source'!L14&gt;=50,"B",IF('Data Source'!L14&gt;=40,"C",IF('Data Source'!L14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="7">
         <f>IF('Data Source'!M14&gt;=80,"A+",IF('Data Source'!M14&gt;=70,"A",IF('Data Source'!M14&gt;=60,"A-",IF('Data Source'!M14&gt;=50,"B",IF('Data Source'!M14&gt;=40,"C",IF('Data Source'!M14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J15" s="6">
-        <f>IF('Data Source'!N14&gt;=80,"A+",IF('Data Source'!N14&gt;=70,"A",IF('Data Source'!N14&gt;=60,"A-",IF('Data Source'!N14&gt;=50,"B",IF('Data Source'!N14&gt;=40,"C",IF('Data Source'!N14&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K15" s="6">
+      <c r="J15" s="7">
+        <f>IF('Data Source'!N14/50*100&gt;=80,"A+",IF('Data Source'!N14/50*100&gt;=70,"A",IF('Data Source'!N14/50*100&gt;=60,"A-",IF('Data Source'!N14/50*100&gt;=50,"B",IF('Data Source'!N14/50*100&gt;=40,"C",IF('Data Source'!N14/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K15" s="7">
         <f>IF('Data Source'!O14&gt;=80,"A+",IF('Data Source'!O14&gt;=70,"A",IF('Data Source'!O14&gt;=60,"A-",IF('Data Source'!O14&gt;=50,"B",IF('Data Source'!O14&gt;=40,"C",IF('Data Source'!O14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="7">
         <f>IF('Data Source'!P14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="7">
         <f>IF('Data Source'!Q14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="6">
         <f>'Data Source'!T14</f>
         <v/>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="7">
         <f>'Data Source'!U14</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <f>'Data Source'!A15</f>
         <v/>
       </c>
@@ -3630,61 +3637,61 @@
         <f>'Data Source'!B15</f>
         <v/>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
         <f>IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=80,"A+",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=70,"A",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=60,"A-",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=50,"B",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=40,"C",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="7">
         <f>IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=80,"A+",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=70,"A",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=60,"A-",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=50,"B",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=40,"C",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="7">
         <f>IF('Data Source'!G15&gt;=80,"A+",IF('Data Source'!G15&gt;=70,"A",IF('Data Source'!G15&gt;=60,"A-",IF('Data Source'!G15&gt;=50,"B",IF('Data Source'!G15&gt;=40,"C",IF('Data Source'!G15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="7">
         <f>IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=80,"A+",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=70,"A",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=60,"A-",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=50,"B",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=40,"C",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="7">
         <f>IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=80,"A+",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=70,"A",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=60,"A-",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=50,"B",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=40,"C",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="7">
         <f>IF('Data Source'!L15&gt;=80,"A+",IF('Data Source'!L15&gt;=70,"A",IF('Data Source'!L15&gt;=60,"A-",IF('Data Source'!L15&gt;=50,"B",IF('Data Source'!L15&gt;=40,"C",IF('Data Source'!L15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="7">
         <f>IF('Data Source'!M15&gt;=80,"A+",IF('Data Source'!M15&gt;=70,"A",IF('Data Source'!M15&gt;=60,"A-",IF('Data Source'!M15&gt;=50,"B",IF('Data Source'!M15&gt;=40,"C",IF('Data Source'!M15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J16" s="6">
-        <f>IF('Data Source'!N15&gt;=80,"A+",IF('Data Source'!N15&gt;=70,"A",IF('Data Source'!N15&gt;=60,"A-",IF('Data Source'!N15&gt;=50,"B",IF('Data Source'!N15&gt;=40,"C",IF('Data Source'!N15&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K16" s="6">
+      <c r="J16" s="7">
+        <f>IF('Data Source'!N15/50*100&gt;=80,"A+",IF('Data Source'!N15/50*100&gt;=70,"A",IF('Data Source'!N15/50*100&gt;=60,"A-",IF('Data Source'!N15/50*100&gt;=50,"B",IF('Data Source'!N15/50*100&gt;=40,"C",IF('Data Source'!N15/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K16" s="7">
         <f>IF('Data Source'!O15&gt;=80,"A+",IF('Data Source'!O15&gt;=70,"A",IF('Data Source'!O15&gt;=60,"A-",IF('Data Source'!O15&gt;=50,"B",IF('Data Source'!O15&gt;=40,"C",IF('Data Source'!O15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="7">
         <f>IF('Data Source'!P15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="7">
         <f>IF('Data Source'!Q15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="6">
         <f>'Data Source'!T15</f>
         <v/>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="7">
         <f>'Data Source'!U15</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="6">
+      <c r="A17" s="7">
         <f>'Data Source'!A16</f>
         <v/>
       </c>
@@ -3692,61 +3699,61 @@
         <f>'Data Source'!B16</f>
         <v/>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
         <f>IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=80,"A+",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=70,"A",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=60,"A-",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=50,"B",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=40,"C",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="7">
         <f>IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=80,"A+",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=70,"A",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=60,"A-",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=50,"B",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=40,"C",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="7">
         <f>IF('Data Source'!G16&gt;=80,"A+",IF('Data Source'!G16&gt;=70,"A",IF('Data Source'!G16&gt;=60,"A-",IF('Data Source'!G16&gt;=50,"B",IF('Data Source'!G16&gt;=40,"C",IF('Data Source'!G16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="7">
         <f>IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=80,"A+",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=70,"A",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=60,"A-",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=50,"B",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=40,"C",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="7">
         <f>IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=80,"A+",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=70,"A",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=60,"A-",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=50,"B",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=40,"C",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="7">
         <f>IF('Data Source'!L16&gt;=80,"A+",IF('Data Source'!L16&gt;=70,"A",IF('Data Source'!L16&gt;=60,"A-",IF('Data Source'!L16&gt;=50,"B",IF('Data Source'!L16&gt;=40,"C",IF('Data Source'!L16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="7">
         <f>IF('Data Source'!M16&gt;=80,"A+",IF('Data Source'!M16&gt;=70,"A",IF('Data Source'!M16&gt;=60,"A-",IF('Data Source'!M16&gt;=50,"B",IF('Data Source'!M16&gt;=40,"C",IF('Data Source'!M16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J17" s="6">
-        <f>IF('Data Source'!N16&gt;=80,"A+",IF('Data Source'!N16&gt;=70,"A",IF('Data Source'!N16&gt;=60,"A-",IF('Data Source'!N16&gt;=50,"B",IF('Data Source'!N16&gt;=40,"C",IF('Data Source'!N16&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K17" s="6">
+      <c r="J17" s="7">
+        <f>IF('Data Source'!N16/50*100&gt;=80,"A+",IF('Data Source'!N16/50*100&gt;=70,"A",IF('Data Source'!N16/50*100&gt;=60,"A-",IF('Data Source'!N16/50*100&gt;=50,"B",IF('Data Source'!N16/50*100&gt;=40,"C",IF('Data Source'!N16/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K17" s="7">
         <f>IF('Data Source'!O16&gt;=80,"A+",IF('Data Source'!O16&gt;=70,"A",IF('Data Source'!O16&gt;=60,"A-",IF('Data Source'!O16&gt;=50,"B",IF('Data Source'!O16&gt;=40,"C",IF('Data Source'!O16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="7">
         <f>IF('Data Source'!P16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="7">
         <f>IF('Data Source'!Q16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="6">
         <f>'Data Source'!T16</f>
         <v/>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="7">
         <f>'Data Source'!U16</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6">
+      <c r="A18" s="7">
         <f>'Data Source'!A17</f>
         <v/>
       </c>
@@ -3754,61 +3761,61 @@
         <f>'Data Source'!B17</f>
         <v/>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <f>IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=80,"A+",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=70,"A",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=60,"A-",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=50,"B",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=40,"C",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="7">
         <f>IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=80,"A+",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=70,"A",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=60,"A-",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=50,"B",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=40,"C",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <f>IF('Data Source'!G17&gt;=80,"A+",IF('Data Source'!G17&gt;=70,"A",IF('Data Source'!G17&gt;=60,"A-",IF('Data Source'!G17&gt;=50,"B",IF('Data Source'!G17&gt;=40,"C",IF('Data Source'!G17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="7">
         <f>IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=80,"A+",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=70,"A",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=60,"A-",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=50,"B",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=40,"C",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="7">
         <f>IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=80,"A+",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=70,"A",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=60,"A-",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=50,"B",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=40,"C",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="7">
         <f>IF('Data Source'!L17&gt;=80,"A+",IF('Data Source'!L17&gt;=70,"A",IF('Data Source'!L17&gt;=60,"A-",IF('Data Source'!L17&gt;=50,"B",IF('Data Source'!L17&gt;=40,"C",IF('Data Source'!L17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="7">
         <f>IF('Data Source'!M17&gt;=80,"A+",IF('Data Source'!M17&gt;=70,"A",IF('Data Source'!M17&gt;=60,"A-",IF('Data Source'!M17&gt;=50,"B",IF('Data Source'!M17&gt;=40,"C",IF('Data Source'!M17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J18" s="6">
-        <f>IF('Data Source'!N17&gt;=80,"A+",IF('Data Source'!N17&gt;=70,"A",IF('Data Source'!N17&gt;=60,"A-",IF('Data Source'!N17&gt;=50,"B",IF('Data Source'!N17&gt;=40,"C",IF('Data Source'!N17&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K18" s="6">
+      <c r="J18" s="7">
+        <f>IF('Data Source'!N17/50*100&gt;=80,"A+",IF('Data Source'!N17/50*100&gt;=70,"A",IF('Data Source'!N17/50*100&gt;=60,"A-",IF('Data Source'!N17/50*100&gt;=50,"B",IF('Data Source'!N17/50*100&gt;=40,"C",IF('Data Source'!N17/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K18" s="7">
         <f>IF('Data Source'!O17&gt;=80,"A+",IF('Data Source'!O17&gt;=70,"A",IF('Data Source'!O17&gt;=60,"A-",IF('Data Source'!O17&gt;=50,"B",IF('Data Source'!O17&gt;=40,"C",IF('Data Source'!O17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="7">
         <f>IF('Data Source'!P17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="7">
         <f>IF('Data Source'!Q17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="6">
         <f>'Data Source'!T17</f>
         <v/>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="7">
         <f>'Data Source'!U17</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6">
+      <c r="A19" s="7">
         <f>'Data Source'!A18</f>
         <v/>
       </c>
@@ -3816,61 +3823,61 @@
         <f>'Data Source'!B18</f>
         <v/>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <f>IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=80,"A+",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=70,"A",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=60,"A-",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=50,"B",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=40,"C",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <f>IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=80,"A+",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=70,"A",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=60,"A-",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=50,"B",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=40,"C",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="7">
         <f>IF('Data Source'!G18&gt;=80,"A+",IF('Data Source'!G18&gt;=70,"A",IF('Data Source'!G18&gt;=60,"A-",IF('Data Source'!G18&gt;=50,"B",IF('Data Source'!G18&gt;=40,"C",IF('Data Source'!G18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="7">
         <f>IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=80,"A+",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=70,"A",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=60,"A-",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=50,"B",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=40,"C",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="7">
         <f>IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=80,"A+",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=70,"A",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=60,"A-",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=50,"B",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=40,"C",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="7">
         <f>IF('Data Source'!L18&gt;=80,"A+",IF('Data Source'!L18&gt;=70,"A",IF('Data Source'!L18&gt;=60,"A-",IF('Data Source'!L18&gt;=50,"B",IF('Data Source'!L18&gt;=40,"C",IF('Data Source'!L18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="7">
         <f>IF('Data Source'!M18&gt;=80,"A+",IF('Data Source'!M18&gt;=70,"A",IF('Data Source'!M18&gt;=60,"A-",IF('Data Source'!M18&gt;=50,"B",IF('Data Source'!M18&gt;=40,"C",IF('Data Source'!M18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J19" s="6">
-        <f>IF('Data Source'!N18&gt;=80,"A+",IF('Data Source'!N18&gt;=70,"A",IF('Data Source'!N18&gt;=60,"A-",IF('Data Source'!N18&gt;=50,"B",IF('Data Source'!N18&gt;=40,"C",IF('Data Source'!N18&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K19" s="6">
+      <c r="J19" s="7">
+        <f>IF('Data Source'!N18/50*100&gt;=80,"A+",IF('Data Source'!N18/50*100&gt;=70,"A",IF('Data Source'!N18/50*100&gt;=60,"A-",IF('Data Source'!N18/50*100&gt;=50,"B",IF('Data Source'!N18/50*100&gt;=40,"C",IF('Data Source'!N18/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K19" s="7">
         <f>IF('Data Source'!O18&gt;=80,"A+",IF('Data Source'!O18&gt;=70,"A",IF('Data Source'!O18&gt;=60,"A-",IF('Data Source'!O18&gt;=50,"B",IF('Data Source'!O18&gt;=40,"C",IF('Data Source'!O18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="7">
         <f>IF('Data Source'!P18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="7">
         <f>IF('Data Source'!Q18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="6">
         <f>'Data Source'!T18</f>
         <v/>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="7">
         <f>'Data Source'!U18</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6">
+      <c r="A20" s="7">
         <f>'Data Source'!A19</f>
         <v/>
       </c>
@@ -3878,61 +3885,61 @@
         <f>'Data Source'!B19</f>
         <v/>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="7">
         <f>IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=80,"A+",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=70,"A",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=60,"A-",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=50,"B",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=40,"C",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="7">
         <f>IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=80,"A+",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=70,"A",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=60,"A-",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=50,"B",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=40,"C",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="7">
         <f>IF('Data Source'!G19&gt;=80,"A+",IF('Data Source'!G19&gt;=70,"A",IF('Data Source'!G19&gt;=60,"A-",IF('Data Source'!G19&gt;=50,"B",IF('Data Source'!G19&gt;=40,"C",IF('Data Source'!G19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="7">
         <f>IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=80,"A+",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=70,"A",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=60,"A-",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=50,"B",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=40,"C",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="7">
         <f>IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=80,"A+",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=70,"A",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=60,"A-",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=50,"B",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=40,"C",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="7">
         <f>IF('Data Source'!L19&gt;=80,"A+",IF('Data Source'!L19&gt;=70,"A",IF('Data Source'!L19&gt;=60,"A-",IF('Data Source'!L19&gt;=50,"B",IF('Data Source'!L19&gt;=40,"C",IF('Data Source'!L19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="7">
         <f>IF('Data Source'!M19&gt;=80,"A+",IF('Data Source'!M19&gt;=70,"A",IF('Data Source'!M19&gt;=60,"A-",IF('Data Source'!M19&gt;=50,"B",IF('Data Source'!M19&gt;=40,"C",IF('Data Source'!M19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J20" s="6">
-        <f>IF('Data Source'!N19&gt;=80,"A+",IF('Data Source'!N19&gt;=70,"A",IF('Data Source'!N19&gt;=60,"A-",IF('Data Source'!N19&gt;=50,"B",IF('Data Source'!N19&gt;=40,"C",IF('Data Source'!N19&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K20" s="6">
+      <c r="J20" s="7">
+        <f>IF('Data Source'!N19/50*100&gt;=80,"A+",IF('Data Source'!N19/50*100&gt;=70,"A",IF('Data Source'!N19/50*100&gt;=60,"A-",IF('Data Source'!N19/50*100&gt;=50,"B",IF('Data Source'!N19/50*100&gt;=40,"C",IF('Data Source'!N19/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K20" s="7">
         <f>IF('Data Source'!O19&gt;=80,"A+",IF('Data Source'!O19&gt;=70,"A",IF('Data Source'!O19&gt;=60,"A-",IF('Data Source'!O19&gt;=50,"B",IF('Data Source'!O19&gt;=40,"C",IF('Data Source'!O19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="7">
         <f>IF('Data Source'!P19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="7">
         <f>IF('Data Source'!Q19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="6">
         <f>'Data Source'!T19</f>
         <v/>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="7">
         <f>'Data Source'!U19</f>
         <v/>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <f>'Data Source'!A20</f>
         <v/>
       </c>
@@ -3940,61 +3947,61 @@
         <f>'Data Source'!B20</f>
         <v/>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="7">
         <f>IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=80,"A+",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=70,"A",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=60,"A-",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=50,"B",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=40,"C",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="7">
         <f>IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=80,"A+",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=70,"A",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=60,"A-",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=50,"B",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=40,"C",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="7">
         <f>IF('Data Source'!G20&gt;=80,"A+",IF('Data Source'!G20&gt;=70,"A",IF('Data Source'!G20&gt;=60,"A-",IF('Data Source'!G20&gt;=50,"B",IF('Data Source'!G20&gt;=40,"C",IF('Data Source'!G20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="7">
         <f>IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=80,"A+",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=70,"A",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=60,"A-",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=50,"B",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=40,"C",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="7">
         <f>IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=80,"A+",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=70,"A",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=60,"A-",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=50,"B",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=40,"C",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="7">
         <f>IF('Data Source'!L20&gt;=80,"A+",IF('Data Source'!L20&gt;=70,"A",IF('Data Source'!L20&gt;=60,"A-",IF('Data Source'!L20&gt;=50,"B",IF('Data Source'!L20&gt;=40,"C",IF('Data Source'!L20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="7">
         <f>IF('Data Source'!M20&gt;=80,"A+",IF('Data Source'!M20&gt;=70,"A",IF('Data Source'!M20&gt;=60,"A-",IF('Data Source'!M20&gt;=50,"B",IF('Data Source'!M20&gt;=40,"C",IF('Data Source'!M20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J21" s="6">
-        <f>IF('Data Source'!N20&gt;=80,"A+",IF('Data Source'!N20&gt;=70,"A",IF('Data Source'!N20&gt;=60,"A-",IF('Data Source'!N20&gt;=50,"B",IF('Data Source'!N20&gt;=40,"C",IF('Data Source'!N20&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K21" s="6">
+      <c r="J21" s="7">
+        <f>IF('Data Source'!N20/50*100&gt;=80,"A+",IF('Data Source'!N20/50*100&gt;=70,"A",IF('Data Source'!N20/50*100&gt;=60,"A-",IF('Data Source'!N20/50*100&gt;=50,"B",IF('Data Source'!N20/50*100&gt;=40,"C",IF('Data Source'!N20/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K21" s="7">
         <f>IF('Data Source'!O20&gt;=80,"A+",IF('Data Source'!O20&gt;=70,"A",IF('Data Source'!O20&gt;=60,"A-",IF('Data Source'!O20&gt;=50,"B",IF('Data Source'!O20&gt;=40,"C",IF('Data Source'!O20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="7">
         <f>IF('Data Source'!P20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="7">
         <f>IF('Data Source'!Q20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="6">
         <f>'Data Source'!T20</f>
         <v/>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="7">
         <f>'Data Source'!U20</f>
         <v/>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <f>'Data Source'!A21</f>
         <v/>
       </c>
@@ -4002,55 +4009,55 @@
         <f>'Data Source'!B21</f>
         <v/>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="7">
         <f>IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=80,"A+",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=70,"A",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=60,"A-",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=50,"B",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=40,"C",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="7">
         <f>IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=80,"A+",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=70,"A",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=60,"A-",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=50,"B",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=40,"C",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="7">
         <f>IF('Data Source'!G21&gt;=80,"A+",IF('Data Source'!G21&gt;=70,"A",IF('Data Source'!G21&gt;=60,"A-",IF('Data Source'!G21&gt;=50,"B",IF('Data Source'!G21&gt;=40,"C",IF('Data Source'!G21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="7">
         <f>IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=80,"A+",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=70,"A",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=60,"A-",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=50,"B",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=40,"C",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="7">
         <f>IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=80,"A+",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=70,"A",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=60,"A-",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=50,"B",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=40,"C",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="7">
         <f>IF('Data Source'!L21&gt;=80,"A+",IF('Data Source'!L21&gt;=70,"A",IF('Data Source'!L21&gt;=60,"A-",IF('Data Source'!L21&gt;=50,"B",IF('Data Source'!L21&gt;=40,"C",IF('Data Source'!L21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="7">
         <f>IF('Data Source'!M21&gt;=80,"A+",IF('Data Source'!M21&gt;=70,"A",IF('Data Source'!M21&gt;=60,"A-",IF('Data Source'!M21&gt;=50,"B",IF('Data Source'!M21&gt;=40,"C",IF('Data Source'!M21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J22" s="6">
-        <f>IF('Data Source'!N21&gt;=80,"A+",IF('Data Source'!N21&gt;=70,"A",IF('Data Source'!N21&gt;=60,"A-",IF('Data Source'!N21&gt;=50,"B",IF('Data Source'!N21&gt;=40,"C",IF('Data Source'!N21&gt;=33,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="K22" s="6">
+      <c r="J22" s="7">
+        <f>IF('Data Source'!N21/50*100&gt;=80,"A+",IF('Data Source'!N21/50*100&gt;=70,"A",IF('Data Source'!N21/50*100&gt;=60,"A-",IF('Data Source'!N21/50*100&gt;=50,"B",IF('Data Source'!N21/50*100&gt;=40,"C",IF('Data Source'!N21/50*100&gt;=33,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="K22" s="7">
         <f>IF('Data Source'!O21&gt;=80,"A+",IF('Data Source'!O21&gt;=70,"A",IF('Data Source'!O21&gt;=60,"A-",IF('Data Source'!O21&gt;=50,"B",IF('Data Source'!O21&gt;=40,"C",IF('Data Source'!O21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="7">
         <f>IF('Data Source'!P21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="7">
         <f>IF('Data Source'!Q21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="6">
         <f>'Data Source'!T21</f>
         <v/>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="7">
         <f>'Data Source'!U21</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Update Dakhil GPA calculation to accommodate new Bangla subject structure and adjust pass criteria
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -94,14 +94,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFE699"/>
-        <bgColor rgb="00FFE699"/>
+        <fgColor rgb="00FC9999"/>
+        <bgColor rgb="00FC9999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FC9999"/>
-        <bgColor rgb="00FC9999"/>
+        <fgColor rgb="00FFE699"/>
+        <bgColor rgb="00FFE699"/>
       </patternFill>
     </fill>
     <fill>
@@ -129,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -137,14 +137,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -155,6 +151,9 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -749,7 +748,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -828,60 +827,70 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Bangla_I</t>
+          <t>Bangla_I_MCQ</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Bangla_II</t>
+          <t>Bangla_I_Written</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Bangla_II_MCQ</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bangla_II_Written</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Mathematics</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Islamic_History</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ICT</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Career_Education</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Physical_Education</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Overall Grade</t>
         </is>
@@ -917,43 +926,41 @@
       <c r="I2" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="N2" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="P2" s="3" t="n">
-        <v>93</v>
+      <c r="J2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>52</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>33</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="R2">
-        <f>SUM(C2:N2)</f>
-        <v/>
-      </c>
-      <c r="S2" s="5">
-        <f>ROUND(R2/11.5,2)</f>
-        <v/>
+        <v>65</v>
+      </c>
+      <c r="R2" t="n">
+        <v>79</v>
+      </c>
+      <c r="S2" t="n">
+        <v>77</v>
       </c>
       <c r="T2" s="6">
-        <f>IF(OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,(J2+K2)&lt;66,L2&lt;33,M2&lt;33,N2&lt;8.25,P2&lt;33,Q2&lt;33),0,MIN(5,ROUND((IF((C2+D2)/200*100&gt;=80,5,IF((C2+D2)/200*100&gt;=70,4,IF((C2+D2)/200*100&gt;=60,3.5,IF((C2+D2)/200*100&gt;=50,3,IF((C2+D2)/200*100&gt;=40,2,IF((C2+D2)/200*100&gt;=33,1,0))))))+IF((E2+F2)/200*100&gt;=80,5,IF((E2+F2)/200*100&gt;=70,4,IF((E2+F2)/200*100&gt;=60,3.5,IF((E2+F2)/200*100&gt;=50,3,IF((E2+F2)/200*100&gt;=40,2,IF((E2+F2)/200*100&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF((H2+I2)/200*100&gt;=80,5,IF((H2+I2)/200*100&gt;=70,4,IF((H2+I2)/200*100&gt;=60,3.5,IF((H2+I2)/200*100&gt;=50,3,IF((H2+I2)/200*100&gt;=40,2,IF((H2+I2)/200*100&gt;=33,1,0))))))+IF((J2+K2)/200*100&gt;=80,5,IF((J2+K2)/200*100&gt;=70,4,IF((J2+K2)/200*100&gt;=60,3.5,IF((J2+K2)/200*100&gt;=50,3,IF((J2+K2)/200*100&gt;=40,2,IF((J2+K2)/200*100&gt;=33,1,0))))))+IF(L2&gt;=80,5,IF(L2&gt;=70,4,IF(L2&gt;=60,3.5,IF(L2&gt;=50,3,IF(L2&gt;=40,2,IF(L2&gt;=33,1,0))))))+IF(M2&gt;=80,5,IF(M2&gt;=70,4,IF(M2&gt;=60,3.5,IF(M2&gt;=50,3,IF(M2&gt;=40,2,IF(M2&gt;=33,1,0))))))+IF(N2/50*100&gt;=80,5,IF(N2/50*100&gt;=70,4,IF(N2/50*100&gt;=60,3.5,IF(N2/50*100&gt;=50,3,IF(N2/50*100&gt;=40,2,IF(N2/50*100&gt;=33,1,0)))))))/8+IF(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))&gt;=2,(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U2" s="7">
+        <f>IF(OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,NOT(OR(AND(J2&gt;=10,K2&gt;=23,L2&gt;=10,M2&gt;=23),AND((J2+L2)&gt;=20,(K2+M2)&gt;=46))),N2&lt;33,O2&lt;33,P2&lt;8.25,R2&lt;33,S2&lt;33),0,MIN(5,ROUND((IF((C2+D2)/200*100&gt;=80,5,IF((C2+D2)/200*100&gt;=70,4,IF((C2+D2)/200*100&gt;=60,3.5,IF((C2+D2)/200*100&gt;=50,3,IF((C2+D2)/200*100&gt;=40,2,IF((C2+D2)/200*100&gt;=33,1,0))))))+IF((E2+F2)/200*100&gt;=80,5,IF((E2+F2)/200*100&gt;=70,4,IF((E2+F2)/200*100&gt;=60,3.5,IF((E2+F2)/200*100&gt;=50,3,IF((E2+F2)/200*100&gt;=40,2,IF((E2+F2)/200*100&gt;=33,1,0))))))+IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))+IF((H2+I2)/200*100&gt;=80,5,IF((H2+I2)/200*100&gt;=70,4,IF((H2+I2)/200*100&gt;=60,3.5,IF((H2+I2)/200*100&gt;=50,3,IF((H2+I2)/200*100&gt;=40,2,IF((H2+I2)/200*100&gt;=33,1,0))))))+IF((J2+K2)/200*100&gt;=80,5,IF((J2+K2)/200*100&gt;=70,4,IF((J2+K2)/200*100&gt;=60,3.5,IF((J2+K2)/200*100&gt;=50,3,IF((J2+K2)/200*100&gt;=40,2,IF((J2+K2)/200*100&gt;=33,1,0))))))+IF(L2&gt;=80,5,IF(L2&gt;=70,4,IF(L2&gt;=60,3.5,IF(L2&gt;=50,3,IF(L2&gt;=40,2,IF(L2&gt;=33,1,0))))))+IF(M2&gt;=80,5,IF(M2&gt;=70,4,IF(M2&gt;=60,3.5,IF(M2&gt;=50,3,IF(M2&gt;=40,2,IF(M2&gt;=33,1,0))))))+IF(N2/50*100&gt;=80,5,IF(N2/50*100&gt;=70,4,IF(N2/50*100&gt;=60,3.5,IF(N2/50*100&gt;=50,3,IF(N2/50*100&gt;=40,2,IF(N2/50*100&gt;=33,1,0)))))))/8+IF(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))&gt;=2,(IF(O2&gt;=80,5,IF(O2&gt;=70,4,IF(O2&gt;=60,3.5,IF(O2&gt;=50,3,IF(O2&gt;=40,2,IF(O2&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U2" s="6">
         <f>IF(T2&gt;=5,"A+",IF(T2&gt;=4,"A",IF(T2&gt;=3.5,"A-",IF(T2&gt;=3,"B",IF(T2&gt;=2,"C",IF(T2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -988,43 +995,41 @@
       <c r="I3" s="3" t="n">
         <v>84</v>
       </c>
-      <c r="J3" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="K3" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="N3" s="8" t="n">
-        <v>30</v>
-      </c>
-      <c r="O3" s="4" t="n">
+      <c r="J3" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="5" t="n">
         <v>58</v>
       </c>
-      <c r="P3" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="R3">
-        <f>SUM(C3:N3)</f>
-        <v/>
-      </c>
-      <c r="S3" s="5">
-        <f>ROUND(R3/11.5,2)</f>
-        <v/>
+      <c r="L3" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="R3" t="n">
+        <v>76</v>
+      </c>
+      <c r="S3" t="n">
+        <v>94</v>
       </c>
       <c r="T3" s="6">
-        <f>IF(OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,(J3+K3)&lt;66,L3&lt;33,M3&lt;33,N3&lt;8.25,P3&lt;33,Q3&lt;33),0,MIN(5,ROUND((IF((C3+D3)/200*100&gt;=80,5,IF((C3+D3)/200*100&gt;=70,4,IF((C3+D3)/200*100&gt;=60,3.5,IF((C3+D3)/200*100&gt;=50,3,IF((C3+D3)/200*100&gt;=40,2,IF((C3+D3)/200*100&gt;=33,1,0))))))+IF((E3+F3)/200*100&gt;=80,5,IF((E3+F3)/200*100&gt;=70,4,IF((E3+F3)/200*100&gt;=60,3.5,IF((E3+F3)/200*100&gt;=50,3,IF((E3+F3)/200*100&gt;=40,2,IF((E3+F3)/200*100&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF((H3+I3)/200*100&gt;=80,5,IF((H3+I3)/200*100&gt;=70,4,IF((H3+I3)/200*100&gt;=60,3.5,IF((H3+I3)/200*100&gt;=50,3,IF((H3+I3)/200*100&gt;=40,2,IF((H3+I3)/200*100&gt;=33,1,0))))))+IF((J3+K3)/200*100&gt;=80,5,IF((J3+K3)/200*100&gt;=70,4,IF((J3+K3)/200*100&gt;=60,3.5,IF((J3+K3)/200*100&gt;=50,3,IF((J3+K3)/200*100&gt;=40,2,IF((J3+K3)/200*100&gt;=33,1,0))))))+IF(L3&gt;=80,5,IF(L3&gt;=70,4,IF(L3&gt;=60,3.5,IF(L3&gt;=50,3,IF(L3&gt;=40,2,IF(L3&gt;=33,1,0))))))+IF(M3&gt;=80,5,IF(M3&gt;=70,4,IF(M3&gt;=60,3.5,IF(M3&gt;=50,3,IF(M3&gt;=40,2,IF(M3&gt;=33,1,0))))))+IF(N3/50*100&gt;=80,5,IF(N3/50*100&gt;=70,4,IF(N3/50*100&gt;=60,3.5,IF(N3/50*100&gt;=50,3,IF(N3/50*100&gt;=40,2,IF(N3/50*100&gt;=33,1,0)))))))/8+IF(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))&gt;=2,(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U3" s="7">
+        <f>IF(OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,NOT(OR(AND(J3&gt;=10,K3&gt;=23,L3&gt;=10,M3&gt;=23),AND((J3+L3)&gt;=20,(K3+M3)&gt;=46))),N3&lt;33,O3&lt;33,P3&lt;8.25,R3&lt;33,S3&lt;33),0,MIN(5,ROUND((IF((C3+D3)/200*100&gt;=80,5,IF((C3+D3)/200*100&gt;=70,4,IF((C3+D3)/200*100&gt;=60,3.5,IF((C3+D3)/200*100&gt;=50,3,IF((C3+D3)/200*100&gt;=40,2,IF((C3+D3)/200*100&gt;=33,1,0))))))+IF((E3+F3)/200*100&gt;=80,5,IF((E3+F3)/200*100&gt;=70,4,IF((E3+F3)/200*100&gt;=60,3.5,IF((E3+F3)/200*100&gt;=50,3,IF((E3+F3)/200*100&gt;=40,2,IF((E3+F3)/200*100&gt;=33,1,0))))))+IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))+IF((H3+I3)/200*100&gt;=80,5,IF((H3+I3)/200*100&gt;=70,4,IF((H3+I3)/200*100&gt;=60,3.5,IF((H3+I3)/200*100&gt;=50,3,IF((H3+I3)/200*100&gt;=40,2,IF((H3+I3)/200*100&gt;=33,1,0))))))+IF((J3+K3)/200*100&gt;=80,5,IF((J3+K3)/200*100&gt;=70,4,IF((J3+K3)/200*100&gt;=60,3.5,IF((J3+K3)/200*100&gt;=50,3,IF((J3+K3)/200*100&gt;=40,2,IF((J3+K3)/200*100&gt;=33,1,0))))))+IF(L3&gt;=80,5,IF(L3&gt;=70,4,IF(L3&gt;=60,3.5,IF(L3&gt;=50,3,IF(L3&gt;=40,2,IF(L3&gt;=33,1,0))))))+IF(M3&gt;=80,5,IF(M3&gt;=70,4,IF(M3&gt;=60,3.5,IF(M3&gt;=50,3,IF(M3&gt;=40,2,IF(M3&gt;=33,1,0))))))+IF(N3/50*100&gt;=80,5,IF(N3/50*100&gt;=70,4,IF(N3/50*100&gt;=60,3.5,IF(N3/50*100&gt;=50,3,IF(N3/50*100&gt;=40,2,IF(N3/50*100&gt;=33,1,0)))))))/8+IF(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))&gt;=2,(IF(O3&gt;=80,5,IF(O3&gt;=70,4,IF(O3&gt;=60,3.5,IF(O3&gt;=50,3,IF(O3&gt;=40,2,IF(O3&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U3" s="6">
         <f>IF(T3&gt;=5,"A+",IF(T3&gt;=4,"A",IF(T3&gt;=3.5,"A-",IF(T3&gt;=3,"B",IF(T3&gt;=2,"C",IF(T3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1059,43 +1064,41 @@
       <c r="I4" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="J4" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>70</v>
+      <c r="J4" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>32</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>58</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="N4" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="P4" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="Q4" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="R4">
-        <f>SUM(C4:N4)</f>
-        <v/>
-      </c>
-      <c r="S4" s="5">
-        <f>ROUND(R4/11.5,2)</f>
-        <v/>
+        <v>23</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="R4" t="n">
+        <v>71</v>
+      </c>
+      <c r="S4" t="n">
+        <v>77</v>
       </c>
       <c r="T4" s="6">
-        <f>IF(OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,(J4+K4)&lt;66,L4&lt;33,M4&lt;33,N4&lt;8.25,P4&lt;33,Q4&lt;33),0,MIN(5,ROUND((IF((C4+D4)/200*100&gt;=80,5,IF((C4+D4)/200*100&gt;=70,4,IF((C4+D4)/200*100&gt;=60,3.5,IF((C4+D4)/200*100&gt;=50,3,IF((C4+D4)/200*100&gt;=40,2,IF((C4+D4)/200*100&gt;=33,1,0))))))+IF((E4+F4)/200*100&gt;=80,5,IF((E4+F4)/200*100&gt;=70,4,IF((E4+F4)/200*100&gt;=60,3.5,IF((E4+F4)/200*100&gt;=50,3,IF((E4+F4)/200*100&gt;=40,2,IF((E4+F4)/200*100&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF((H4+I4)/200*100&gt;=80,5,IF((H4+I4)/200*100&gt;=70,4,IF((H4+I4)/200*100&gt;=60,3.5,IF((H4+I4)/200*100&gt;=50,3,IF((H4+I4)/200*100&gt;=40,2,IF((H4+I4)/200*100&gt;=33,1,0))))))+IF((J4+K4)/200*100&gt;=80,5,IF((J4+K4)/200*100&gt;=70,4,IF((J4+K4)/200*100&gt;=60,3.5,IF((J4+K4)/200*100&gt;=50,3,IF((J4+K4)/200*100&gt;=40,2,IF((J4+K4)/200*100&gt;=33,1,0))))))+IF(L4&gt;=80,5,IF(L4&gt;=70,4,IF(L4&gt;=60,3.5,IF(L4&gt;=50,3,IF(L4&gt;=40,2,IF(L4&gt;=33,1,0))))))+IF(M4&gt;=80,5,IF(M4&gt;=70,4,IF(M4&gt;=60,3.5,IF(M4&gt;=50,3,IF(M4&gt;=40,2,IF(M4&gt;=33,1,0))))))+IF(N4/50*100&gt;=80,5,IF(N4/50*100&gt;=70,4,IF(N4/50*100&gt;=60,3.5,IF(N4/50*100&gt;=50,3,IF(N4/50*100&gt;=40,2,IF(N4/50*100&gt;=33,1,0)))))))/8+IF(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))&gt;=2,(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U4" s="7">
+        <f>IF(OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,NOT(OR(AND(J4&gt;=10,K4&gt;=23,L4&gt;=10,M4&gt;=23),AND((J4+L4)&gt;=20,(K4+M4)&gt;=46))),N4&lt;33,O4&lt;33,P4&lt;8.25,R4&lt;33,S4&lt;33),0,MIN(5,ROUND((IF((C4+D4)/200*100&gt;=80,5,IF((C4+D4)/200*100&gt;=70,4,IF((C4+D4)/200*100&gt;=60,3.5,IF((C4+D4)/200*100&gt;=50,3,IF((C4+D4)/200*100&gt;=40,2,IF((C4+D4)/200*100&gt;=33,1,0))))))+IF((E4+F4)/200*100&gt;=80,5,IF((E4+F4)/200*100&gt;=70,4,IF((E4+F4)/200*100&gt;=60,3.5,IF((E4+F4)/200*100&gt;=50,3,IF((E4+F4)/200*100&gt;=40,2,IF((E4+F4)/200*100&gt;=33,1,0))))))+IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))+IF((H4+I4)/200*100&gt;=80,5,IF((H4+I4)/200*100&gt;=70,4,IF((H4+I4)/200*100&gt;=60,3.5,IF((H4+I4)/200*100&gt;=50,3,IF((H4+I4)/200*100&gt;=40,2,IF((H4+I4)/200*100&gt;=33,1,0))))))+IF((J4+K4)/200*100&gt;=80,5,IF((J4+K4)/200*100&gt;=70,4,IF((J4+K4)/200*100&gt;=60,3.5,IF((J4+K4)/200*100&gt;=50,3,IF((J4+K4)/200*100&gt;=40,2,IF((J4+K4)/200*100&gt;=33,1,0))))))+IF(L4&gt;=80,5,IF(L4&gt;=70,4,IF(L4&gt;=60,3.5,IF(L4&gt;=50,3,IF(L4&gt;=40,2,IF(L4&gt;=33,1,0))))))+IF(M4&gt;=80,5,IF(M4&gt;=70,4,IF(M4&gt;=60,3.5,IF(M4&gt;=50,3,IF(M4&gt;=40,2,IF(M4&gt;=33,1,0))))))+IF(N4/50*100&gt;=80,5,IF(N4/50*100&gt;=70,4,IF(N4/50*100&gt;=60,3.5,IF(N4/50*100&gt;=50,3,IF(N4/50*100&gt;=40,2,IF(N4/50*100&gt;=33,1,0)))))))/8+IF(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))&gt;=2,(IF(O4&gt;=80,5,IF(O4&gt;=70,4,IF(O4&gt;=60,3.5,IF(O4&gt;=50,3,IF(O4&gt;=40,2,IF(O4&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U4" s="6">
         <f>IF(T4&gt;=5,"A+",IF(T4&gt;=4,"A",IF(T4&gt;=3.5,"A-",IF(T4&gt;=3,"B",IF(T4&gt;=2,"C",IF(T4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1130,43 +1133,41 @@
       <c r="I5" s="3" t="n">
         <v>87</v>
       </c>
-      <c r="J5" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="K5" s="3" t="n">
+      <c r="J5" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="P5" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="R5" t="n">
+        <v>88</v>
+      </c>
+      <c r="S5" t="n">
         <v>82</v>
       </c>
-      <c r="L5" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>83</v>
-      </c>
-      <c r="N5" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="R5">
-        <f>SUM(C5:N5)</f>
-        <v/>
-      </c>
-      <c r="S5" s="5">
-        <f>ROUND(R5/11.5,2)</f>
-        <v/>
-      </c>
       <c r="T5" s="6">
-        <f>IF(OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,(J5+K5)&lt;66,L5&lt;33,M5&lt;33,N5&lt;8.25,P5&lt;33,Q5&lt;33),0,MIN(5,ROUND((IF((C5+D5)/200*100&gt;=80,5,IF((C5+D5)/200*100&gt;=70,4,IF((C5+D5)/200*100&gt;=60,3.5,IF((C5+D5)/200*100&gt;=50,3,IF((C5+D5)/200*100&gt;=40,2,IF((C5+D5)/200*100&gt;=33,1,0))))))+IF((E5+F5)/200*100&gt;=80,5,IF((E5+F5)/200*100&gt;=70,4,IF((E5+F5)/200*100&gt;=60,3.5,IF((E5+F5)/200*100&gt;=50,3,IF((E5+F5)/200*100&gt;=40,2,IF((E5+F5)/200*100&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF((H5+I5)/200*100&gt;=80,5,IF((H5+I5)/200*100&gt;=70,4,IF((H5+I5)/200*100&gt;=60,3.5,IF((H5+I5)/200*100&gt;=50,3,IF((H5+I5)/200*100&gt;=40,2,IF((H5+I5)/200*100&gt;=33,1,0))))))+IF((J5+K5)/200*100&gt;=80,5,IF((J5+K5)/200*100&gt;=70,4,IF((J5+K5)/200*100&gt;=60,3.5,IF((J5+K5)/200*100&gt;=50,3,IF((J5+K5)/200*100&gt;=40,2,IF((J5+K5)/200*100&gt;=33,1,0))))))+IF(L5&gt;=80,5,IF(L5&gt;=70,4,IF(L5&gt;=60,3.5,IF(L5&gt;=50,3,IF(L5&gt;=40,2,IF(L5&gt;=33,1,0))))))+IF(M5&gt;=80,5,IF(M5&gt;=70,4,IF(M5&gt;=60,3.5,IF(M5&gt;=50,3,IF(M5&gt;=40,2,IF(M5&gt;=33,1,0))))))+IF(N5/50*100&gt;=80,5,IF(N5/50*100&gt;=70,4,IF(N5/50*100&gt;=60,3.5,IF(N5/50*100&gt;=50,3,IF(N5/50*100&gt;=40,2,IF(N5/50*100&gt;=33,1,0)))))))/8+IF(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))&gt;=2,(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U5" s="7">
+        <f>IF(OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,NOT(OR(AND(J5&gt;=10,K5&gt;=23,L5&gt;=10,M5&gt;=23),AND((J5+L5)&gt;=20,(K5+M5)&gt;=46))),N5&lt;33,O5&lt;33,P5&lt;8.25,R5&lt;33,S5&lt;33),0,MIN(5,ROUND((IF((C5+D5)/200*100&gt;=80,5,IF((C5+D5)/200*100&gt;=70,4,IF((C5+D5)/200*100&gt;=60,3.5,IF((C5+D5)/200*100&gt;=50,3,IF((C5+D5)/200*100&gt;=40,2,IF((C5+D5)/200*100&gt;=33,1,0))))))+IF((E5+F5)/200*100&gt;=80,5,IF((E5+F5)/200*100&gt;=70,4,IF((E5+F5)/200*100&gt;=60,3.5,IF((E5+F5)/200*100&gt;=50,3,IF((E5+F5)/200*100&gt;=40,2,IF((E5+F5)/200*100&gt;=33,1,0))))))+IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))+IF((H5+I5)/200*100&gt;=80,5,IF((H5+I5)/200*100&gt;=70,4,IF((H5+I5)/200*100&gt;=60,3.5,IF((H5+I5)/200*100&gt;=50,3,IF((H5+I5)/200*100&gt;=40,2,IF((H5+I5)/200*100&gt;=33,1,0))))))+IF((J5+K5)/200*100&gt;=80,5,IF((J5+K5)/200*100&gt;=70,4,IF((J5+K5)/200*100&gt;=60,3.5,IF((J5+K5)/200*100&gt;=50,3,IF((J5+K5)/200*100&gt;=40,2,IF((J5+K5)/200*100&gt;=33,1,0))))))+IF(L5&gt;=80,5,IF(L5&gt;=70,4,IF(L5&gt;=60,3.5,IF(L5&gt;=50,3,IF(L5&gt;=40,2,IF(L5&gt;=33,1,0))))))+IF(M5&gt;=80,5,IF(M5&gt;=70,4,IF(M5&gt;=60,3.5,IF(M5&gt;=50,3,IF(M5&gt;=40,2,IF(M5&gt;=33,1,0))))))+IF(N5/50*100&gt;=80,5,IF(N5/50*100&gt;=70,4,IF(N5/50*100&gt;=60,3.5,IF(N5/50*100&gt;=50,3,IF(N5/50*100&gt;=40,2,IF(N5/50*100&gt;=33,1,0)))))))/8+IF(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))&gt;=2,(IF(O5&gt;=80,5,IF(O5&gt;=70,4,IF(O5&gt;=60,3.5,IF(O5&gt;=50,3,IF(O5&gt;=40,2,IF(O5&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U5" s="6">
         <f>IF(T5&gt;=5,"A+",IF(T5&gt;=4,"A",IF(T5&gt;=3.5,"A-",IF(T5&gt;=3,"B",IF(T5&gt;=2,"C",IF(T5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1201,43 +1202,41 @@
       <c r="I6" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="J6" s="3" t="n">
-        <v>81</v>
-      </c>
-      <c r="K6" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="L6" s="3" t="n">
-        <v>91</v>
-      </c>
-      <c r="M6" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="N6" s="8" t="n">
-        <v>37</v>
-      </c>
-      <c r="O6" s="3" t="n">
+      <c r="J6" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="P6" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="R6">
-        <f>SUM(C6:N6)</f>
-        <v/>
-      </c>
-      <c r="S6" s="5">
-        <f>ROUND(R6/11.5,2)</f>
-        <v/>
+      <c r="R6" t="n">
+        <v>93</v>
+      </c>
+      <c r="S6" t="n">
+        <v>87</v>
       </c>
       <c r="T6" s="6">
-        <f>IF(OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,(J6+K6)&lt;66,L6&lt;33,M6&lt;33,N6&lt;8.25,P6&lt;33,Q6&lt;33),0,MIN(5,ROUND((IF((C6+D6)/200*100&gt;=80,5,IF((C6+D6)/200*100&gt;=70,4,IF((C6+D6)/200*100&gt;=60,3.5,IF((C6+D6)/200*100&gt;=50,3,IF((C6+D6)/200*100&gt;=40,2,IF((C6+D6)/200*100&gt;=33,1,0))))))+IF((E6+F6)/200*100&gt;=80,5,IF((E6+F6)/200*100&gt;=70,4,IF((E6+F6)/200*100&gt;=60,3.5,IF((E6+F6)/200*100&gt;=50,3,IF((E6+F6)/200*100&gt;=40,2,IF((E6+F6)/200*100&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF((H6+I6)/200*100&gt;=80,5,IF((H6+I6)/200*100&gt;=70,4,IF((H6+I6)/200*100&gt;=60,3.5,IF((H6+I6)/200*100&gt;=50,3,IF((H6+I6)/200*100&gt;=40,2,IF((H6+I6)/200*100&gt;=33,1,0))))))+IF((J6+K6)/200*100&gt;=80,5,IF((J6+K6)/200*100&gt;=70,4,IF((J6+K6)/200*100&gt;=60,3.5,IF((J6+K6)/200*100&gt;=50,3,IF((J6+K6)/200*100&gt;=40,2,IF((J6+K6)/200*100&gt;=33,1,0))))))+IF(L6&gt;=80,5,IF(L6&gt;=70,4,IF(L6&gt;=60,3.5,IF(L6&gt;=50,3,IF(L6&gt;=40,2,IF(L6&gt;=33,1,0))))))+IF(M6&gt;=80,5,IF(M6&gt;=70,4,IF(M6&gt;=60,3.5,IF(M6&gt;=50,3,IF(M6&gt;=40,2,IF(M6&gt;=33,1,0))))))+IF(N6/50*100&gt;=80,5,IF(N6/50*100&gt;=70,4,IF(N6/50*100&gt;=60,3.5,IF(N6/50*100&gt;=50,3,IF(N6/50*100&gt;=40,2,IF(N6/50*100&gt;=33,1,0)))))))/8+IF(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))&gt;=2,(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U6" s="7">
+        <f>IF(OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,NOT(OR(AND(J6&gt;=10,K6&gt;=23,L6&gt;=10,M6&gt;=23),AND((J6+L6)&gt;=20,(K6+M6)&gt;=46))),N6&lt;33,O6&lt;33,P6&lt;8.25,R6&lt;33,S6&lt;33),0,MIN(5,ROUND((IF((C6+D6)/200*100&gt;=80,5,IF((C6+D6)/200*100&gt;=70,4,IF((C6+D6)/200*100&gt;=60,3.5,IF((C6+D6)/200*100&gt;=50,3,IF((C6+D6)/200*100&gt;=40,2,IF((C6+D6)/200*100&gt;=33,1,0))))))+IF((E6+F6)/200*100&gt;=80,5,IF((E6+F6)/200*100&gt;=70,4,IF((E6+F6)/200*100&gt;=60,3.5,IF((E6+F6)/200*100&gt;=50,3,IF((E6+F6)/200*100&gt;=40,2,IF((E6+F6)/200*100&gt;=33,1,0))))))+IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))+IF((H6+I6)/200*100&gt;=80,5,IF((H6+I6)/200*100&gt;=70,4,IF((H6+I6)/200*100&gt;=60,3.5,IF((H6+I6)/200*100&gt;=50,3,IF((H6+I6)/200*100&gt;=40,2,IF((H6+I6)/200*100&gt;=33,1,0))))))+IF((J6+K6)/200*100&gt;=80,5,IF((J6+K6)/200*100&gt;=70,4,IF((J6+K6)/200*100&gt;=60,3.5,IF((J6+K6)/200*100&gt;=50,3,IF((J6+K6)/200*100&gt;=40,2,IF((J6+K6)/200*100&gt;=33,1,0))))))+IF(L6&gt;=80,5,IF(L6&gt;=70,4,IF(L6&gt;=60,3.5,IF(L6&gt;=50,3,IF(L6&gt;=40,2,IF(L6&gt;=33,1,0))))))+IF(M6&gt;=80,5,IF(M6&gt;=70,4,IF(M6&gt;=60,3.5,IF(M6&gt;=50,3,IF(M6&gt;=40,2,IF(M6&gt;=33,1,0))))))+IF(N6/50*100&gt;=80,5,IF(N6/50*100&gt;=70,4,IF(N6/50*100&gt;=60,3.5,IF(N6/50*100&gt;=50,3,IF(N6/50*100&gt;=40,2,IF(N6/50*100&gt;=33,1,0)))))))/8+IF(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))&gt;=2,(IF(O6&gt;=80,5,IF(O6&gt;=70,4,IF(O6&gt;=60,3.5,IF(O6&gt;=50,3,IF(O6&gt;=40,2,IF(O6&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U6" s="6">
         <f>IF(T6&gt;=5,"A+",IF(T6&gt;=4,"A",IF(T6&gt;=3.5,"A-",IF(T6&gt;=3,"B",IF(T6&gt;=2,"C",IF(T6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1272,43 +1271,41 @@
       <c r="I7" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="J7" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="K7" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>66</v>
-      </c>
-      <c r="N7" s="4" t="n">
-        <v>48</v>
+      <c r="J7" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>87</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="Q7" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="R7">
-        <f>SUM(C7:N7)</f>
-        <v/>
-      </c>
-      <c r="S7" s="5">
-        <f>ROUND(R7/11.5,2)</f>
-        <v/>
+        <v>73</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="R7" t="n">
+        <v>87</v>
+      </c>
+      <c r="S7" t="n">
+        <v>78</v>
       </c>
       <c r="T7" s="6">
-        <f>IF(OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,(J7+K7)&lt;66,L7&lt;33,M7&lt;33,N7&lt;8.25,P7&lt;33,Q7&lt;33),0,MIN(5,ROUND((IF((C7+D7)/200*100&gt;=80,5,IF((C7+D7)/200*100&gt;=70,4,IF((C7+D7)/200*100&gt;=60,3.5,IF((C7+D7)/200*100&gt;=50,3,IF((C7+D7)/200*100&gt;=40,2,IF((C7+D7)/200*100&gt;=33,1,0))))))+IF((E7+F7)/200*100&gt;=80,5,IF((E7+F7)/200*100&gt;=70,4,IF((E7+F7)/200*100&gt;=60,3.5,IF((E7+F7)/200*100&gt;=50,3,IF((E7+F7)/200*100&gt;=40,2,IF((E7+F7)/200*100&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF((H7+I7)/200*100&gt;=80,5,IF((H7+I7)/200*100&gt;=70,4,IF((H7+I7)/200*100&gt;=60,3.5,IF((H7+I7)/200*100&gt;=50,3,IF((H7+I7)/200*100&gt;=40,2,IF((H7+I7)/200*100&gt;=33,1,0))))))+IF((J7+K7)/200*100&gt;=80,5,IF((J7+K7)/200*100&gt;=70,4,IF((J7+K7)/200*100&gt;=60,3.5,IF((J7+K7)/200*100&gt;=50,3,IF((J7+K7)/200*100&gt;=40,2,IF((J7+K7)/200*100&gt;=33,1,0))))))+IF(L7&gt;=80,5,IF(L7&gt;=70,4,IF(L7&gt;=60,3.5,IF(L7&gt;=50,3,IF(L7&gt;=40,2,IF(L7&gt;=33,1,0))))))+IF(M7&gt;=80,5,IF(M7&gt;=70,4,IF(M7&gt;=60,3.5,IF(M7&gt;=50,3,IF(M7&gt;=40,2,IF(M7&gt;=33,1,0))))))+IF(N7/50*100&gt;=80,5,IF(N7/50*100&gt;=70,4,IF(N7/50*100&gt;=60,3.5,IF(N7/50*100&gt;=50,3,IF(N7/50*100&gt;=40,2,IF(N7/50*100&gt;=33,1,0)))))))/8+IF(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))&gt;=2,(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U7" s="7">
+        <f>IF(OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,NOT(OR(AND(J7&gt;=10,K7&gt;=23,L7&gt;=10,M7&gt;=23),AND((J7+L7)&gt;=20,(K7+M7)&gt;=46))),N7&lt;33,O7&lt;33,P7&lt;8.25,R7&lt;33,S7&lt;33),0,MIN(5,ROUND((IF((C7+D7)/200*100&gt;=80,5,IF((C7+D7)/200*100&gt;=70,4,IF((C7+D7)/200*100&gt;=60,3.5,IF((C7+D7)/200*100&gt;=50,3,IF((C7+D7)/200*100&gt;=40,2,IF((C7+D7)/200*100&gt;=33,1,0))))))+IF((E7+F7)/200*100&gt;=80,5,IF((E7+F7)/200*100&gt;=70,4,IF((E7+F7)/200*100&gt;=60,3.5,IF((E7+F7)/200*100&gt;=50,3,IF((E7+F7)/200*100&gt;=40,2,IF((E7+F7)/200*100&gt;=33,1,0))))))+IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))+IF((H7+I7)/200*100&gt;=80,5,IF((H7+I7)/200*100&gt;=70,4,IF((H7+I7)/200*100&gt;=60,3.5,IF((H7+I7)/200*100&gt;=50,3,IF((H7+I7)/200*100&gt;=40,2,IF((H7+I7)/200*100&gt;=33,1,0))))))+IF((J7+K7)/200*100&gt;=80,5,IF((J7+K7)/200*100&gt;=70,4,IF((J7+K7)/200*100&gt;=60,3.5,IF((J7+K7)/200*100&gt;=50,3,IF((J7+K7)/200*100&gt;=40,2,IF((J7+K7)/200*100&gt;=33,1,0))))))+IF(L7&gt;=80,5,IF(L7&gt;=70,4,IF(L7&gt;=60,3.5,IF(L7&gt;=50,3,IF(L7&gt;=40,2,IF(L7&gt;=33,1,0))))))+IF(M7&gt;=80,5,IF(M7&gt;=70,4,IF(M7&gt;=60,3.5,IF(M7&gt;=50,3,IF(M7&gt;=40,2,IF(M7&gt;=33,1,0))))))+IF(N7/50*100&gt;=80,5,IF(N7/50*100&gt;=70,4,IF(N7/50*100&gt;=60,3.5,IF(N7/50*100&gt;=50,3,IF(N7/50*100&gt;=40,2,IF(N7/50*100&gt;=33,1,0)))))))/8+IF(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))&gt;=2,(IF(O7&gt;=80,5,IF(O7&gt;=70,4,IF(O7&gt;=60,3.5,IF(O7&gt;=50,3,IF(O7&gt;=40,2,IF(O7&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U7" s="6">
         <f>IF(T7&gt;=5,"A+",IF(T7&gt;=4,"A",IF(T7&gt;=3.5,"A-",IF(T7&gt;=3,"B",IF(T7&gt;=2,"C",IF(T7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1343,43 +1340,41 @@
       <c r="I8" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="J8" s="2" t="n">
-        <v>78</v>
-      </c>
-      <c r="K8" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="M8" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="N8" s="8" t="n">
-        <v>37</v>
-      </c>
-      <c r="O8" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="R8">
-        <f>SUM(C8:N8)</f>
-        <v/>
-      </c>
-      <c r="S8" s="5">
-        <f>ROUND(R8/11.5,2)</f>
-        <v/>
+      <c r="J8" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="R8" t="n">
+        <v>71</v>
+      </c>
+      <c r="S8" t="n">
+        <v>93</v>
       </c>
       <c r="T8" s="6">
-        <f>IF(OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,(J8+K8)&lt;66,L8&lt;33,M8&lt;33,N8&lt;8.25,P8&lt;33,Q8&lt;33),0,MIN(5,ROUND((IF((C8+D8)/200*100&gt;=80,5,IF((C8+D8)/200*100&gt;=70,4,IF((C8+D8)/200*100&gt;=60,3.5,IF((C8+D8)/200*100&gt;=50,3,IF((C8+D8)/200*100&gt;=40,2,IF((C8+D8)/200*100&gt;=33,1,0))))))+IF((E8+F8)/200*100&gt;=80,5,IF((E8+F8)/200*100&gt;=70,4,IF((E8+F8)/200*100&gt;=60,3.5,IF((E8+F8)/200*100&gt;=50,3,IF((E8+F8)/200*100&gt;=40,2,IF((E8+F8)/200*100&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF((H8+I8)/200*100&gt;=80,5,IF((H8+I8)/200*100&gt;=70,4,IF((H8+I8)/200*100&gt;=60,3.5,IF((H8+I8)/200*100&gt;=50,3,IF((H8+I8)/200*100&gt;=40,2,IF((H8+I8)/200*100&gt;=33,1,0))))))+IF((J8+K8)/200*100&gt;=80,5,IF((J8+K8)/200*100&gt;=70,4,IF((J8+K8)/200*100&gt;=60,3.5,IF((J8+K8)/200*100&gt;=50,3,IF((J8+K8)/200*100&gt;=40,2,IF((J8+K8)/200*100&gt;=33,1,0))))))+IF(L8&gt;=80,5,IF(L8&gt;=70,4,IF(L8&gt;=60,3.5,IF(L8&gt;=50,3,IF(L8&gt;=40,2,IF(L8&gt;=33,1,0))))))+IF(M8&gt;=80,5,IF(M8&gt;=70,4,IF(M8&gt;=60,3.5,IF(M8&gt;=50,3,IF(M8&gt;=40,2,IF(M8&gt;=33,1,0))))))+IF(N8/50*100&gt;=80,5,IF(N8/50*100&gt;=70,4,IF(N8/50*100&gt;=60,3.5,IF(N8/50*100&gt;=50,3,IF(N8/50*100&gt;=40,2,IF(N8/50*100&gt;=33,1,0)))))))/8+IF(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))&gt;=2,(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U8" s="7">
+        <f>IF(OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,NOT(OR(AND(J8&gt;=10,K8&gt;=23,L8&gt;=10,M8&gt;=23),AND((J8+L8)&gt;=20,(K8+M8)&gt;=46))),N8&lt;33,O8&lt;33,P8&lt;8.25,R8&lt;33,S8&lt;33),0,MIN(5,ROUND((IF((C8+D8)/200*100&gt;=80,5,IF((C8+D8)/200*100&gt;=70,4,IF((C8+D8)/200*100&gt;=60,3.5,IF((C8+D8)/200*100&gt;=50,3,IF((C8+D8)/200*100&gt;=40,2,IF((C8+D8)/200*100&gt;=33,1,0))))))+IF((E8+F8)/200*100&gt;=80,5,IF((E8+F8)/200*100&gt;=70,4,IF((E8+F8)/200*100&gt;=60,3.5,IF((E8+F8)/200*100&gt;=50,3,IF((E8+F8)/200*100&gt;=40,2,IF((E8+F8)/200*100&gt;=33,1,0))))))+IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))+IF((H8+I8)/200*100&gt;=80,5,IF((H8+I8)/200*100&gt;=70,4,IF((H8+I8)/200*100&gt;=60,3.5,IF((H8+I8)/200*100&gt;=50,3,IF((H8+I8)/200*100&gt;=40,2,IF((H8+I8)/200*100&gt;=33,1,0))))))+IF((J8+K8)/200*100&gt;=80,5,IF((J8+K8)/200*100&gt;=70,4,IF((J8+K8)/200*100&gt;=60,3.5,IF((J8+K8)/200*100&gt;=50,3,IF((J8+K8)/200*100&gt;=40,2,IF((J8+K8)/200*100&gt;=33,1,0))))))+IF(L8&gt;=80,5,IF(L8&gt;=70,4,IF(L8&gt;=60,3.5,IF(L8&gt;=50,3,IF(L8&gt;=40,2,IF(L8&gt;=33,1,0))))))+IF(M8&gt;=80,5,IF(M8&gt;=70,4,IF(M8&gt;=60,3.5,IF(M8&gt;=50,3,IF(M8&gt;=40,2,IF(M8&gt;=33,1,0))))))+IF(N8/50*100&gt;=80,5,IF(N8/50*100&gt;=70,4,IF(N8/50*100&gt;=60,3.5,IF(N8/50*100&gt;=50,3,IF(N8/50*100&gt;=40,2,IF(N8/50*100&gt;=33,1,0)))))))/8+IF(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))&gt;=2,(IF(O8&gt;=80,5,IF(O8&gt;=70,4,IF(O8&gt;=60,3.5,IF(O8&gt;=50,3,IF(O8&gt;=40,2,IF(O8&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U8" s="6">
         <f>IF(T8&gt;=5,"A+",IF(T8&gt;=4,"A",IF(T8&gt;=3.5,"A-",IF(T8&gt;=3,"B",IF(T8&gt;=2,"C",IF(T8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1414,43 +1409,41 @@
       <c r="I9" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="O9" s="3" t="n">
         <v>87</v>
       </c>
-      <c r="K9" s="3" t="n">
-        <v>81</v>
-      </c>
-      <c r="L9" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>69</v>
-      </c>
-      <c r="N9" s="8" t="n">
-        <v>30</v>
-      </c>
-      <c r="O9" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="P9" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="Q9" s="3" t="n">
-        <v>88</v>
-      </c>
-      <c r="R9">
-        <f>SUM(C9:N9)</f>
-        <v/>
-      </c>
-      <c r="S9" s="5">
-        <f>ROUND(R9/11.5,2)</f>
-        <v/>
+      <c r="P9" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="R9" t="n">
+        <v>93</v>
+      </c>
+      <c r="S9" t="n">
+        <v>82</v>
       </c>
       <c r="T9" s="6">
-        <f>IF(OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,(J9+K9)&lt;66,L9&lt;33,M9&lt;33,N9&lt;8.25,P9&lt;33,Q9&lt;33),0,MIN(5,ROUND((IF((C9+D9)/200*100&gt;=80,5,IF((C9+D9)/200*100&gt;=70,4,IF((C9+D9)/200*100&gt;=60,3.5,IF((C9+D9)/200*100&gt;=50,3,IF((C9+D9)/200*100&gt;=40,2,IF((C9+D9)/200*100&gt;=33,1,0))))))+IF((E9+F9)/200*100&gt;=80,5,IF((E9+F9)/200*100&gt;=70,4,IF((E9+F9)/200*100&gt;=60,3.5,IF((E9+F9)/200*100&gt;=50,3,IF((E9+F9)/200*100&gt;=40,2,IF((E9+F9)/200*100&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF((H9+I9)/200*100&gt;=80,5,IF((H9+I9)/200*100&gt;=70,4,IF((H9+I9)/200*100&gt;=60,3.5,IF((H9+I9)/200*100&gt;=50,3,IF((H9+I9)/200*100&gt;=40,2,IF((H9+I9)/200*100&gt;=33,1,0))))))+IF((J9+K9)/200*100&gt;=80,5,IF((J9+K9)/200*100&gt;=70,4,IF((J9+K9)/200*100&gt;=60,3.5,IF((J9+K9)/200*100&gt;=50,3,IF((J9+K9)/200*100&gt;=40,2,IF((J9+K9)/200*100&gt;=33,1,0))))))+IF(L9&gt;=80,5,IF(L9&gt;=70,4,IF(L9&gt;=60,3.5,IF(L9&gt;=50,3,IF(L9&gt;=40,2,IF(L9&gt;=33,1,0))))))+IF(M9&gt;=80,5,IF(M9&gt;=70,4,IF(M9&gt;=60,3.5,IF(M9&gt;=50,3,IF(M9&gt;=40,2,IF(M9&gt;=33,1,0))))))+IF(N9/50*100&gt;=80,5,IF(N9/50*100&gt;=70,4,IF(N9/50*100&gt;=60,3.5,IF(N9/50*100&gt;=50,3,IF(N9/50*100&gt;=40,2,IF(N9/50*100&gt;=33,1,0)))))))/8+IF(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))&gt;=2,(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U9" s="7">
+        <f>IF(OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,NOT(OR(AND(J9&gt;=10,K9&gt;=23,L9&gt;=10,M9&gt;=23),AND((J9+L9)&gt;=20,(K9+M9)&gt;=46))),N9&lt;33,O9&lt;33,P9&lt;8.25,R9&lt;33,S9&lt;33),0,MIN(5,ROUND((IF((C9+D9)/200*100&gt;=80,5,IF((C9+D9)/200*100&gt;=70,4,IF((C9+D9)/200*100&gt;=60,3.5,IF((C9+D9)/200*100&gt;=50,3,IF((C9+D9)/200*100&gt;=40,2,IF((C9+D9)/200*100&gt;=33,1,0))))))+IF((E9+F9)/200*100&gt;=80,5,IF((E9+F9)/200*100&gt;=70,4,IF((E9+F9)/200*100&gt;=60,3.5,IF((E9+F9)/200*100&gt;=50,3,IF((E9+F9)/200*100&gt;=40,2,IF((E9+F9)/200*100&gt;=33,1,0))))))+IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))+IF((H9+I9)/200*100&gt;=80,5,IF((H9+I9)/200*100&gt;=70,4,IF((H9+I9)/200*100&gt;=60,3.5,IF((H9+I9)/200*100&gt;=50,3,IF((H9+I9)/200*100&gt;=40,2,IF((H9+I9)/200*100&gt;=33,1,0))))))+IF((J9+K9)/200*100&gt;=80,5,IF((J9+K9)/200*100&gt;=70,4,IF((J9+K9)/200*100&gt;=60,3.5,IF((J9+K9)/200*100&gt;=50,3,IF((J9+K9)/200*100&gt;=40,2,IF((J9+K9)/200*100&gt;=33,1,0))))))+IF(L9&gt;=80,5,IF(L9&gt;=70,4,IF(L9&gt;=60,3.5,IF(L9&gt;=50,3,IF(L9&gt;=40,2,IF(L9&gt;=33,1,0))))))+IF(M9&gt;=80,5,IF(M9&gt;=70,4,IF(M9&gt;=60,3.5,IF(M9&gt;=50,3,IF(M9&gt;=40,2,IF(M9&gt;=33,1,0))))))+IF(N9/50*100&gt;=80,5,IF(N9/50*100&gt;=70,4,IF(N9/50*100&gt;=60,3.5,IF(N9/50*100&gt;=50,3,IF(N9/50*100&gt;=40,2,IF(N9/50*100&gt;=33,1,0)))))))/8+IF(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))&gt;=2,(IF(O9&gt;=80,5,IF(O9&gt;=70,4,IF(O9&gt;=60,3.5,IF(O9&gt;=50,3,IF(O9&gt;=40,2,IF(O9&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U9" s="6">
         <f>IF(T9&gt;=5,"A+",IF(T9&gt;=4,"A",IF(T9&gt;=3.5,"A-",IF(T9&gt;=3,"B",IF(T9&gt;=2,"C",IF(T9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1485,43 +1478,41 @@
       <c r="I10" s="3" t="n">
         <v>85</v>
       </c>
-      <c r="J10" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="K10" s="3" t="n">
-        <v>94</v>
+      <c r="J10" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>59</v>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="N10" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="P10" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="Q10" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="R10">
-        <f>SUM(C10:N10)</f>
-        <v/>
-      </c>
-      <c r="S10" s="5">
-        <f>ROUND(R10/11.5,2)</f>
-        <v/>
+        <v>25</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="O10" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="P10" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="R10" t="n">
+        <v>80</v>
+      </c>
+      <c r="S10" t="n">
+        <v>93</v>
       </c>
       <c r="T10" s="6">
-        <f>IF(OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,(J10+K10)&lt;66,L10&lt;33,M10&lt;33,N10&lt;8.25,P10&lt;33,Q10&lt;33),0,MIN(5,ROUND((IF((C10+D10)/200*100&gt;=80,5,IF((C10+D10)/200*100&gt;=70,4,IF((C10+D10)/200*100&gt;=60,3.5,IF((C10+D10)/200*100&gt;=50,3,IF((C10+D10)/200*100&gt;=40,2,IF((C10+D10)/200*100&gt;=33,1,0))))))+IF((E10+F10)/200*100&gt;=80,5,IF((E10+F10)/200*100&gt;=70,4,IF((E10+F10)/200*100&gt;=60,3.5,IF((E10+F10)/200*100&gt;=50,3,IF((E10+F10)/200*100&gt;=40,2,IF((E10+F10)/200*100&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF((H10+I10)/200*100&gt;=80,5,IF((H10+I10)/200*100&gt;=70,4,IF((H10+I10)/200*100&gt;=60,3.5,IF((H10+I10)/200*100&gt;=50,3,IF((H10+I10)/200*100&gt;=40,2,IF((H10+I10)/200*100&gt;=33,1,0))))))+IF((J10+K10)/200*100&gt;=80,5,IF((J10+K10)/200*100&gt;=70,4,IF((J10+K10)/200*100&gt;=60,3.5,IF((J10+K10)/200*100&gt;=50,3,IF((J10+K10)/200*100&gt;=40,2,IF((J10+K10)/200*100&gt;=33,1,0))))))+IF(L10&gt;=80,5,IF(L10&gt;=70,4,IF(L10&gt;=60,3.5,IF(L10&gt;=50,3,IF(L10&gt;=40,2,IF(L10&gt;=33,1,0))))))+IF(M10&gt;=80,5,IF(M10&gt;=70,4,IF(M10&gt;=60,3.5,IF(M10&gt;=50,3,IF(M10&gt;=40,2,IF(M10&gt;=33,1,0))))))+IF(N10/50*100&gt;=80,5,IF(N10/50*100&gt;=70,4,IF(N10/50*100&gt;=60,3.5,IF(N10/50*100&gt;=50,3,IF(N10/50*100&gt;=40,2,IF(N10/50*100&gt;=33,1,0)))))))/8+IF(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))&gt;=2,(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U10" s="7">
+        <f>IF(OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,NOT(OR(AND(J10&gt;=10,K10&gt;=23,L10&gt;=10,M10&gt;=23),AND((J10+L10)&gt;=20,(K10+M10)&gt;=46))),N10&lt;33,O10&lt;33,P10&lt;8.25,R10&lt;33,S10&lt;33),0,MIN(5,ROUND((IF((C10+D10)/200*100&gt;=80,5,IF((C10+D10)/200*100&gt;=70,4,IF((C10+D10)/200*100&gt;=60,3.5,IF((C10+D10)/200*100&gt;=50,3,IF((C10+D10)/200*100&gt;=40,2,IF((C10+D10)/200*100&gt;=33,1,0))))))+IF((E10+F10)/200*100&gt;=80,5,IF((E10+F10)/200*100&gt;=70,4,IF((E10+F10)/200*100&gt;=60,3.5,IF((E10+F10)/200*100&gt;=50,3,IF((E10+F10)/200*100&gt;=40,2,IF((E10+F10)/200*100&gt;=33,1,0))))))+IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))+IF((H10+I10)/200*100&gt;=80,5,IF((H10+I10)/200*100&gt;=70,4,IF((H10+I10)/200*100&gt;=60,3.5,IF((H10+I10)/200*100&gt;=50,3,IF((H10+I10)/200*100&gt;=40,2,IF((H10+I10)/200*100&gt;=33,1,0))))))+IF((J10+K10)/200*100&gt;=80,5,IF((J10+K10)/200*100&gt;=70,4,IF((J10+K10)/200*100&gt;=60,3.5,IF((J10+K10)/200*100&gt;=50,3,IF((J10+K10)/200*100&gt;=40,2,IF((J10+K10)/200*100&gt;=33,1,0))))))+IF(L10&gt;=80,5,IF(L10&gt;=70,4,IF(L10&gt;=60,3.5,IF(L10&gt;=50,3,IF(L10&gt;=40,2,IF(L10&gt;=33,1,0))))))+IF(M10&gt;=80,5,IF(M10&gt;=70,4,IF(M10&gt;=60,3.5,IF(M10&gt;=50,3,IF(M10&gt;=40,2,IF(M10&gt;=33,1,0))))))+IF(N10/50*100&gt;=80,5,IF(N10/50*100&gt;=70,4,IF(N10/50*100&gt;=60,3.5,IF(N10/50*100&gt;=50,3,IF(N10/50*100&gt;=40,2,IF(N10/50*100&gt;=33,1,0)))))))/8+IF(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))&gt;=2,(IF(O10&gt;=80,5,IF(O10&gt;=70,4,IF(O10&gt;=60,3.5,IF(O10&gt;=50,3,IF(O10&gt;=40,2,IF(O10&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U10" s="6">
         <f>IF(T10&gt;=5,"A+",IF(T10&gt;=4,"A",IF(T10&gt;=3.5,"A-",IF(T10&gt;=3,"B",IF(T10&gt;=2,"C",IF(T10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1556,43 +1547,41 @@
       <c r="I11" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="J11" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="L11" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="M11" s="3" t="n">
-        <v>81</v>
-      </c>
-      <c r="N11" s="8" t="n">
-        <v>31</v>
-      </c>
-      <c r="O11" s="4" t="n">
-        <v>56</v>
-      </c>
-      <c r="P11" s="2" t="n">
+      <c r="J11" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>58</v>
+      </c>
+      <c r="L11" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="M11" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="P11" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="Q11" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="R11">
-        <f>SUM(C11:N11)</f>
-        <v/>
-      </c>
-      <c r="S11" s="5">
-        <f>ROUND(R11/11.5,2)</f>
-        <v/>
+      <c r="R11" t="n">
+        <v>71</v>
+      </c>
+      <c r="S11" t="n">
+        <v>94</v>
       </c>
       <c r="T11" s="6">
-        <f>IF(OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,(J11+K11)&lt;66,L11&lt;33,M11&lt;33,N11&lt;8.25,P11&lt;33,Q11&lt;33),0,MIN(5,ROUND((IF((C11+D11)/200*100&gt;=80,5,IF((C11+D11)/200*100&gt;=70,4,IF((C11+D11)/200*100&gt;=60,3.5,IF((C11+D11)/200*100&gt;=50,3,IF((C11+D11)/200*100&gt;=40,2,IF((C11+D11)/200*100&gt;=33,1,0))))))+IF((E11+F11)/200*100&gt;=80,5,IF((E11+F11)/200*100&gt;=70,4,IF((E11+F11)/200*100&gt;=60,3.5,IF((E11+F11)/200*100&gt;=50,3,IF((E11+F11)/200*100&gt;=40,2,IF((E11+F11)/200*100&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF((H11+I11)/200*100&gt;=80,5,IF((H11+I11)/200*100&gt;=70,4,IF((H11+I11)/200*100&gt;=60,3.5,IF((H11+I11)/200*100&gt;=50,3,IF((H11+I11)/200*100&gt;=40,2,IF((H11+I11)/200*100&gt;=33,1,0))))))+IF((J11+K11)/200*100&gt;=80,5,IF((J11+K11)/200*100&gt;=70,4,IF((J11+K11)/200*100&gt;=60,3.5,IF((J11+K11)/200*100&gt;=50,3,IF((J11+K11)/200*100&gt;=40,2,IF((J11+K11)/200*100&gt;=33,1,0))))))+IF(L11&gt;=80,5,IF(L11&gt;=70,4,IF(L11&gt;=60,3.5,IF(L11&gt;=50,3,IF(L11&gt;=40,2,IF(L11&gt;=33,1,0))))))+IF(M11&gt;=80,5,IF(M11&gt;=70,4,IF(M11&gt;=60,3.5,IF(M11&gt;=50,3,IF(M11&gt;=40,2,IF(M11&gt;=33,1,0))))))+IF(N11/50*100&gt;=80,5,IF(N11/50*100&gt;=70,4,IF(N11/50*100&gt;=60,3.5,IF(N11/50*100&gt;=50,3,IF(N11/50*100&gt;=40,2,IF(N11/50*100&gt;=33,1,0)))))))/8+IF(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))&gt;=2,(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U11" s="7">
+        <f>IF(OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,NOT(OR(AND(J11&gt;=10,K11&gt;=23,L11&gt;=10,M11&gt;=23),AND((J11+L11)&gt;=20,(K11+M11)&gt;=46))),N11&lt;33,O11&lt;33,P11&lt;8.25,R11&lt;33,S11&lt;33),0,MIN(5,ROUND((IF((C11+D11)/200*100&gt;=80,5,IF((C11+D11)/200*100&gt;=70,4,IF((C11+D11)/200*100&gt;=60,3.5,IF((C11+D11)/200*100&gt;=50,3,IF((C11+D11)/200*100&gt;=40,2,IF((C11+D11)/200*100&gt;=33,1,0))))))+IF((E11+F11)/200*100&gt;=80,5,IF((E11+F11)/200*100&gt;=70,4,IF((E11+F11)/200*100&gt;=60,3.5,IF((E11+F11)/200*100&gt;=50,3,IF((E11+F11)/200*100&gt;=40,2,IF((E11+F11)/200*100&gt;=33,1,0))))))+IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))+IF((H11+I11)/200*100&gt;=80,5,IF((H11+I11)/200*100&gt;=70,4,IF((H11+I11)/200*100&gt;=60,3.5,IF((H11+I11)/200*100&gt;=50,3,IF((H11+I11)/200*100&gt;=40,2,IF((H11+I11)/200*100&gt;=33,1,0))))))+IF((J11+K11)/200*100&gt;=80,5,IF((J11+K11)/200*100&gt;=70,4,IF((J11+K11)/200*100&gt;=60,3.5,IF((J11+K11)/200*100&gt;=50,3,IF((J11+K11)/200*100&gt;=40,2,IF((J11+K11)/200*100&gt;=33,1,0))))))+IF(L11&gt;=80,5,IF(L11&gt;=70,4,IF(L11&gt;=60,3.5,IF(L11&gt;=50,3,IF(L11&gt;=40,2,IF(L11&gt;=33,1,0))))))+IF(M11&gt;=80,5,IF(M11&gt;=70,4,IF(M11&gt;=60,3.5,IF(M11&gt;=50,3,IF(M11&gt;=40,2,IF(M11&gt;=33,1,0))))))+IF(N11/50*100&gt;=80,5,IF(N11/50*100&gt;=70,4,IF(N11/50*100&gt;=60,3.5,IF(N11/50*100&gt;=50,3,IF(N11/50*100&gt;=40,2,IF(N11/50*100&gt;=33,1,0)))))))/8+IF(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))&gt;=2,(IF(O11&gt;=80,5,IF(O11&gt;=70,4,IF(O11&gt;=60,3.5,IF(O11&gt;=50,3,IF(O11&gt;=40,2,IF(O11&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U11" s="6">
         <f>IF(T11&gt;=5,"A+",IF(T11&gt;=4,"A",IF(T11&gt;=3.5,"A-",IF(T11&gt;=3,"B",IF(T11&gt;=2,"C",IF(T11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1627,43 +1616,41 @@
       <c r="I12" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="J12" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="K12" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="L12" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="M12" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="N12" s="8" t="n">
-        <v>37</v>
-      </c>
-      <c r="O12" s="4" t="n">
-        <v>56</v>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>83</v>
-      </c>
-      <c r="Q12" s="3" t="n">
+      <c r="J12" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="L12" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="O12" s="3" t="n">
         <v>81</v>
       </c>
-      <c r="R12">
-        <f>SUM(C12:N12)</f>
-        <v/>
-      </c>
-      <c r="S12" s="5">
-        <f>ROUND(R12/11.5,2)</f>
-        <v/>
+      <c r="P12" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="R12" t="n">
+        <v>71</v>
+      </c>
+      <c r="S12" t="n">
+        <v>76</v>
       </c>
       <c r="T12" s="6">
-        <f>IF(OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,(J12+K12)&lt;66,L12&lt;33,M12&lt;33,N12&lt;8.25,P12&lt;33,Q12&lt;33),0,MIN(5,ROUND((IF((C12+D12)/200*100&gt;=80,5,IF((C12+D12)/200*100&gt;=70,4,IF((C12+D12)/200*100&gt;=60,3.5,IF((C12+D12)/200*100&gt;=50,3,IF((C12+D12)/200*100&gt;=40,2,IF((C12+D12)/200*100&gt;=33,1,0))))))+IF((E12+F12)/200*100&gt;=80,5,IF((E12+F12)/200*100&gt;=70,4,IF((E12+F12)/200*100&gt;=60,3.5,IF((E12+F12)/200*100&gt;=50,3,IF((E12+F12)/200*100&gt;=40,2,IF((E12+F12)/200*100&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF((H12+I12)/200*100&gt;=80,5,IF((H12+I12)/200*100&gt;=70,4,IF((H12+I12)/200*100&gt;=60,3.5,IF((H12+I12)/200*100&gt;=50,3,IF((H12+I12)/200*100&gt;=40,2,IF((H12+I12)/200*100&gt;=33,1,0))))))+IF((J12+K12)/200*100&gt;=80,5,IF((J12+K12)/200*100&gt;=70,4,IF((J12+K12)/200*100&gt;=60,3.5,IF((J12+K12)/200*100&gt;=50,3,IF((J12+K12)/200*100&gt;=40,2,IF((J12+K12)/200*100&gt;=33,1,0))))))+IF(L12&gt;=80,5,IF(L12&gt;=70,4,IF(L12&gt;=60,3.5,IF(L12&gt;=50,3,IF(L12&gt;=40,2,IF(L12&gt;=33,1,0))))))+IF(M12&gt;=80,5,IF(M12&gt;=70,4,IF(M12&gt;=60,3.5,IF(M12&gt;=50,3,IF(M12&gt;=40,2,IF(M12&gt;=33,1,0))))))+IF(N12/50*100&gt;=80,5,IF(N12/50*100&gt;=70,4,IF(N12/50*100&gt;=60,3.5,IF(N12/50*100&gt;=50,3,IF(N12/50*100&gt;=40,2,IF(N12/50*100&gt;=33,1,0)))))))/8+IF(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))&gt;=2,(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U12" s="7">
+        <f>IF(OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,NOT(OR(AND(J12&gt;=10,K12&gt;=23,L12&gt;=10,M12&gt;=23),AND((J12+L12)&gt;=20,(K12+M12)&gt;=46))),N12&lt;33,O12&lt;33,P12&lt;8.25,R12&lt;33,S12&lt;33),0,MIN(5,ROUND((IF((C12+D12)/200*100&gt;=80,5,IF((C12+D12)/200*100&gt;=70,4,IF((C12+D12)/200*100&gt;=60,3.5,IF((C12+D12)/200*100&gt;=50,3,IF((C12+D12)/200*100&gt;=40,2,IF((C12+D12)/200*100&gt;=33,1,0))))))+IF((E12+F12)/200*100&gt;=80,5,IF((E12+F12)/200*100&gt;=70,4,IF((E12+F12)/200*100&gt;=60,3.5,IF((E12+F12)/200*100&gt;=50,3,IF((E12+F12)/200*100&gt;=40,2,IF((E12+F12)/200*100&gt;=33,1,0))))))+IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))+IF((H12+I12)/200*100&gt;=80,5,IF((H12+I12)/200*100&gt;=70,4,IF((H12+I12)/200*100&gt;=60,3.5,IF((H12+I12)/200*100&gt;=50,3,IF((H12+I12)/200*100&gt;=40,2,IF((H12+I12)/200*100&gt;=33,1,0))))))+IF((J12+K12)/200*100&gt;=80,5,IF((J12+K12)/200*100&gt;=70,4,IF((J12+K12)/200*100&gt;=60,3.5,IF((J12+K12)/200*100&gt;=50,3,IF((J12+K12)/200*100&gt;=40,2,IF((J12+K12)/200*100&gt;=33,1,0))))))+IF(L12&gt;=80,5,IF(L12&gt;=70,4,IF(L12&gt;=60,3.5,IF(L12&gt;=50,3,IF(L12&gt;=40,2,IF(L12&gt;=33,1,0))))))+IF(M12&gt;=80,5,IF(M12&gt;=70,4,IF(M12&gt;=60,3.5,IF(M12&gt;=50,3,IF(M12&gt;=40,2,IF(M12&gt;=33,1,0))))))+IF(N12/50*100&gt;=80,5,IF(N12/50*100&gt;=70,4,IF(N12/50*100&gt;=60,3.5,IF(N12/50*100&gt;=50,3,IF(N12/50*100&gt;=40,2,IF(N12/50*100&gt;=33,1,0)))))))/8+IF(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))&gt;=2,(IF(O12&gt;=80,5,IF(O12&gt;=70,4,IF(O12&gt;=60,3.5,IF(O12&gt;=50,3,IF(O12&gt;=40,2,IF(O12&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U12" s="6">
         <f>IF(T12&gt;=5,"A+",IF(T12&gt;=4,"A",IF(T12&gt;=3.5,"A-",IF(T12&gt;=3,"B",IF(T12&gt;=2,"C",IF(T12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1698,43 +1685,41 @@
       <c r="I13" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="J13" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="L13" s="2" t="n">
+      <c r="J13" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="N13" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="M13" s="2" t="n">
-        <v>71</v>
-      </c>
-      <c r="N13" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="O13" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="P13" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="R13">
-        <f>SUM(C13:N13)</f>
-        <v/>
-      </c>
-      <c r="S13" s="5">
-        <f>ROUND(R13/11.5,2)</f>
-        <v/>
+      <c r="O13" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="R13" t="n">
+        <v>88</v>
+      </c>
+      <c r="S13" t="n">
+        <v>94</v>
       </c>
       <c r="T13" s="6">
-        <f>IF(OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,(J13+K13)&lt;66,L13&lt;33,M13&lt;33,N13&lt;8.25,P13&lt;33,Q13&lt;33),0,MIN(5,ROUND((IF((C13+D13)/200*100&gt;=80,5,IF((C13+D13)/200*100&gt;=70,4,IF((C13+D13)/200*100&gt;=60,3.5,IF((C13+D13)/200*100&gt;=50,3,IF((C13+D13)/200*100&gt;=40,2,IF((C13+D13)/200*100&gt;=33,1,0))))))+IF((E13+F13)/200*100&gt;=80,5,IF((E13+F13)/200*100&gt;=70,4,IF((E13+F13)/200*100&gt;=60,3.5,IF((E13+F13)/200*100&gt;=50,3,IF((E13+F13)/200*100&gt;=40,2,IF((E13+F13)/200*100&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF((H13+I13)/200*100&gt;=80,5,IF((H13+I13)/200*100&gt;=70,4,IF((H13+I13)/200*100&gt;=60,3.5,IF((H13+I13)/200*100&gt;=50,3,IF((H13+I13)/200*100&gt;=40,2,IF((H13+I13)/200*100&gt;=33,1,0))))))+IF((J13+K13)/200*100&gt;=80,5,IF((J13+K13)/200*100&gt;=70,4,IF((J13+K13)/200*100&gt;=60,3.5,IF((J13+K13)/200*100&gt;=50,3,IF((J13+K13)/200*100&gt;=40,2,IF((J13+K13)/200*100&gt;=33,1,0))))))+IF(L13&gt;=80,5,IF(L13&gt;=70,4,IF(L13&gt;=60,3.5,IF(L13&gt;=50,3,IF(L13&gt;=40,2,IF(L13&gt;=33,1,0))))))+IF(M13&gt;=80,5,IF(M13&gt;=70,4,IF(M13&gt;=60,3.5,IF(M13&gt;=50,3,IF(M13&gt;=40,2,IF(M13&gt;=33,1,0))))))+IF(N13/50*100&gt;=80,5,IF(N13/50*100&gt;=70,4,IF(N13/50*100&gt;=60,3.5,IF(N13/50*100&gt;=50,3,IF(N13/50*100&gt;=40,2,IF(N13/50*100&gt;=33,1,0)))))))/8+IF(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))&gt;=2,(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U13" s="7">
+        <f>IF(OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,NOT(OR(AND(J13&gt;=10,K13&gt;=23,L13&gt;=10,M13&gt;=23),AND((J13+L13)&gt;=20,(K13+M13)&gt;=46))),N13&lt;33,O13&lt;33,P13&lt;8.25,R13&lt;33,S13&lt;33),0,MIN(5,ROUND((IF((C13+D13)/200*100&gt;=80,5,IF((C13+D13)/200*100&gt;=70,4,IF((C13+D13)/200*100&gt;=60,3.5,IF((C13+D13)/200*100&gt;=50,3,IF((C13+D13)/200*100&gt;=40,2,IF((C13+D13)/200*100&gt;=33,1,0))))))+IF((E13+F13)/200*100&gt;=80,5,IF((E13+F13)/200*100&gt;=70,4,IF((E13+F13)/200*100&gt;=60,3.5,IF((E13+F13)/200*100&gt;=50,3,IF((E13+F13)/200*100&gt;=40,2,IF((E13+F13)/200*100&gt;=33,1,0))))))+IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))+IF((H13+I13)/200*100&gt;=80,5,IF((H13+I13)/200*100&gt;=70,4,IF((H13+I13)/200*100&gt;=60,3.5,IF((H13+I13)/200*100&gt;=50,3,IF((H13+I13)/200*100&gt;=40,2,IF((H13+I13)/200*100&gt;=33,1,0))))))+IF((J13+K13)/200*100&gt;=80,5,IF((J13+K13)/200*100&gt;=70,4,IF((J13+K13)/200*100&gt;=60,3.5,IF((J13+K13)/200*100&gt;=50,3,IF((J13+K13)/200*100&gt;=40,2,IF((J13+K13)/200*100&gt;=33,1,0))))))+IF(L13&gt;=80,5,IF(L13&gt;=70,4,IF(L13&gt;=60,3.5,IF(L13&gt;=50,3,IF(L13&gt;=40,2,IF(L13&gt;=33,1,0))))))+IF(M13&gt;=80,5,IF(M13&gt;=70,4,IF(M13&gt;=60,3.5,IF(M13&gt;=50,3,IF(M13&gt;=40,2,IF(M13&gt;=33,1,0))))))+IF(N13/50*100&gt;=80,5,IF(N13/50*100&gt;=70,4,IF(N13/50*100&gt;=60,3.5,IF(N13/50*100&gt;=50,3,IF(N13/50*100&gt;=40,2,IF(N13/50*100&gt;=33,1,0)))))))/8+IF(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))&gt;=2,(IF(O13&gt;=80,5,IF(O13&gt;=70,4,IF(O13&gt;=60,3.5,IF(O13&gt;=50,3,IF(O13&gt;=40,2,IF(O13&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U13" s="6">
         <f>IF(T13&gt;=5,"A+",IF(T13&gt;=4,"A",IF(T13&gt;=3.5,"A-",IF(T13&gt;=3,"B",IF(T13&gt;=2,"C",IF(T13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1769,43 +1754,41 @@
       <c r="I14" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="J14" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="K14" s="3" t="n">
+      <c r="J14" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="K14" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="L14" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="M14" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="O14" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="P14" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="R14" t="n">
         <v>85</v>
       </c>
-      <c r="M14" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="N14" s="8" t="n">
-        <v>31</v>
-      </c>
-      <c r="O14" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="P14" s="2" t="n">
-        <v>78</v>
-      </c>
-      <c r="Q14" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="R14">
-        <f>SUM(C14:N14)</f>
-        <v/>
-      </c>
-      <c r="S14" s="5">
-        <f>ROUND(R14/11.5,2)</f>
-        <v/>
+      <c r="S14" t="n">
+        <v>77</v>
       </c>
       <c r="T14" s="6">
-        <f>IF(OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,(J14+K14)&lt;66,L14&lt;33,M14&lt;33,N14&lt;8.25,P14&lt;33,Q14&lt;33),0,MIN(5,ROUND((IF((C14+D14)/200*100&gt;=80,5,IF((C14+D14)/200*100&gt;=70,4,IF((C14+D14)/200*100&gt;=60,3.5,IF((C14+D14)/200*100&gt;=50,3,IF((C14+D14)/200*100&gt;=40,2,IF((C14+D14)/200*100&gt;=33,1,0))))))+IF((E14+F14)/200*100&gt;=80,5,IF((E14+F14)/200*100&gt;=70,4,IF((E14+F14)/200*100&gt;=60,3.5,IF((E14+F14)/200*100&gt;=50,3,IF((E14+F14)/200*100&gt;=40,2,IF((E14+F14)/200*100&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF((H14+I14)/200*100&gt;=80,5,IF((H14+I14)/200*100&gt;=70,4,IF((H14+I14)/200*100&gt;=60,3.5,IF((H14+I14)/200*100&gt;=50,3,IF((H14+I14)/200*100&gt;=40,2,IF((H14+I14)/200*100&gt;=33,1,0))))))+IF((J14+K14)/200*100&gt;=80,5,IF((J14+K14)/200*100&gt;=70,4,IF((J14+K14)/200*100&gt;=60,3.5,IF((J14+K14)/200*100&gt;=50,3,IF((J14+K14)/200*100&gt;=40,2,IF((J14+K14)/200*100&gt;=33,1,0))))))+IF(L14&gt;=80,5,IF(L14&gt;=70,4,IF(L14&gt;=60,3.5,IF(L14&gt;=50,3,IF(L14&gt;=40,2,IF(L14&gt;=33,1,0))))))+IF(M14&gt;=80,5,IF(M14&gt;=70,4,IF(M14&gt;=60,3.5,IF(M14&gt;=50,3,IF(M14&gt;=40,2,IF(M14&gt;=33,1,0))))))+IF(N14/50*100&gt;=80,5,IF(N14/50*100&gt;=70,4,IF(N14/50*100&gt;=60,3.5,IF(N14/50*100&gt;=50,3,IF(N14/50*100&gt;=40,2,IF(N14/50*100&gt;=33,1,0)))))))/8+IF(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))&gt;=2,(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U14" s="7">
+        <f>IF(OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,NOT(OR(AND(J14&gt;=10,K14&gt;=23,L14&gt;=10,M14&gt;=23),AND((J14+L14)&gt;=20,(K14+M14)&gt;=46))),N14&lt;33,O14&lt;33,P14&lt;8.25,R14&lt;33,S14&lt;33),0,MIN(5,ROUND((IF((C14+D14)/200*100&gt;=80,5,IF((C14+D14)/200*100&gt;=70,4,IF((C14+D14)/200*100&gt;=60,3.5,IF((C14+D14)/200*100&gt;=50,3,IF((C14+D14)/200*100&gt;=40,2,IF((C14+D14)/200*100&gt;=33,1,0))))))+IF((E14+F14)/200*100&gt;=80,5,IF((E14+F14)/200*100&gt;=70,4,IF((E14+F14)/200*100&gt;=60,3.5,IF((E14+F14)/200*100&gt;=50,3,IF((E14+F14)/200*100&gt;=40,2,IF((E14+F14)/200*100&gt;=33,1,0))))))+IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))+IF((H14+I14)/200*100&gt;=80,5,IF((H14+I14)/200*100&gt;=70,4,IF((H14+I14)/200*100&gt;=60,3.5,IF((H14+I14)/200*100&gt;=50,3,IF((H14+I14)/200*100&gt;=40,2,IF((H14+I14)/200*100&gt;=33,1,0))))))+IF((J14+K14)/200*100&gt;=80,5,IF((J14+K14)/200*100&gt;=70,4,IF((J14+K14)/200*100&gt;=60,3.5,IF((J14+K14)/200*100&gt;=50,3,IF((J14+K14)/200*100&gt;=40,2,IF((J14+K14)/200*100&gt;=33,1,0))))))+IF(L14&gt;=80,5,IF(L14&gt;=70,4,IF(L14&gt;=60,3.5,IF(L14&gt;=50,3,IF(L14&gt;=40,2,IF(L14&gt;=33,1,0))))))+IF(M14&gt;=80,5,IF(M14&gt;=70,4,IF(M14&gt;=60,3.5,IF(M14&gt;=50,3,IF(M14&gt;=40,2,IF(M14&gt;=33,1,0))))))+IF(N14/50*100&gt;=80,5,IF(N14/50*100&gt;=70,4,IF(N14/50*100&gt;=60,3.5,IF(N14/50*100&gt;=50,3,IF(N14/50*100&gt;=40,2,IF(N14/50*100&gt;=33,1,0)))))))/8+IF(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))&gt;=2,(IF(O14&gt;=80,5,IF(O14&gt;=70,4,IF(O14&gt;=60,3.5,IF(O14&gt;=50,3,IF(O14&gt;=40,2,IF(O14&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U14" s="6">
         <f>IF(T14&gt;=5,"A+",IF(T14&gt;=4,"A",IF(T14&gt;=3.5,"A-",IF(T14&gt;=3,"B",IF(T14&gt;=2,"C",IF(T14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1840,43 +1823,41 @@
       <c r="I15" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="J15" s="2" t="n">
-        <v>71</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="L15" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="M15" s="3" t="n">
+      <c r="J15" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="L15" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="P15" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q15" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="R15" t="n">
+        <v>86</v>
+      </c>
+      <c r="S15" t="n">
         <v>88</v>
       </c>
-      <c r="N15" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="O15" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="P15" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="Q15" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="R15">
-        <f>SUM(C15:N15)</f>
-        <v/>
-      </c>
-      <c r="S15" s="5">
-        <f>ROUND(R15/11.5,2)</f>
-        <v/>
-      </c>
       <c r="T15" s="6">
-        <f>IF(OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,(J15+K15)&lt;66,L15&lt;33,M15&lt;33,N15&lt;8.25,P15&lt;33,Q15&lt;33),0,MIN(5,ROUND((IF((C15+D15)/200*100&gt;=80,5,IF((C15+D15)/200*100&gt;=70,4,IF((C15+D15)/200*100&gt;=60,3.5,IF((C15+D15)/200*100&gt;=50,3,IF((C15+D15)/200*100&gt;=40,2,IF((C15+D15)/200*100&gt;=33,1,0))))))+IF((E15+F15)/200*100&gt;=80,5,IF((E15+F15)/200*100&gt;=70,4,IF((E15+F15)/200*100&gt;=60,3.5,IF((E15+F15)/200*100&gt;=50,3,IF((E15+F15)/200*100&gt;=40,2,IF((E15+F15)/200*100&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF((H15+I15)/200*100&gt;=80,5,IF((H15+I15)/200*100&gt;=70,4,IF((H15+I15)/200*100&gt;=60,3.5,IF((H15+I15)/200*100&gt;=50,3,IF((H15+I15)/200*100&gt;=40,2,IF((H15+I15)/200*100&gt;=33,1,0))))))+IF((J15+K15)/200*100&gt;=80,5,IF((J15+K15)/200*100&gt;=70,4,IF((J15+K15)/200*100&gt;=60,3.5,IF((J15+K15)/200*100&gt;=50,3,IF((J15+K15)/200*100&gt;=40,2,IF((J15+K15)/200*100&gt;=33,1,0))))))+IF(L15&gt;=80,5,IF(L15&gt;=70,4,IF(L15&gt;=60,3.5,IF(L15&gt;=50,3,IF(L15&gt;=40,2,IF(L15&gt;=33,1,0))))))+IF(M15&gt;=80,5,IF(M15&gt;=70,4,IF(M15&gt;=60,3.5,IF(M15&gt;=50,3,IF(M15&gt;=40,2,IF(M15&gt;=33,1,0))))))+IF(N15/50*100&gt;=80,5,IF(N15/50*100&gt;=70,4,IF(N15/50*100&gt;=60,3.5,IF(N15/50*100&gt;=50,3,IF(N15/50*100&gt;=40,2,IF(N15/50*100&gt;=33,1,0)))))))/8+IF(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))&gt;=2,(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U15" s="7">
+        <f>IF(OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,NOT(OR(AND(J15&gt;=10,K15&gt;=23,L15&gt;=10,M15&gt;=23),AND((J15+L15)&gt;=20,(K15+M15)&gt;=46))),N15&lt;33,O15&lt;33,P15&lt;8.25,R15&lt;33,S15&lt;33),0,MIN(5,ROUND((IF((C15+D15)/200*100&gt;=80,5,IF((C15+D15)/200*100&gt;=70,4,IF((C15+D15)/200*100&gt;=60,3.5,IF((C15+D15)/200*100&gt;=50,3,IF((C15+D15)/200*100&gt;=40,2,IF((C15+D15)/200*100&gt;=33,1,0))))))+IF((E15+F15)/200*100&gt;=80,5,IF((E15+F15)/200*100&gt;=70,4,IF((E15+F15)/200*100&gt;=60,3.5,IF((E15+F15)/200*100&gt;=50,3,IF((E15+F15)/200*100&gt;=40,2,IF((E15+F15)/200*100&gt;=33,1,0))))))+IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))+IF((H15+I15)/200*100&gt;=80,5,IF((H15+I15)/200*100&gt;=70,4,IF((H15+I15)/200*100&gt;=60,3.5,IF((H15+I15)/200*100&gt;=50,3,IF((H15+I15)/200*100&gt;=40,2,IF((H15+I15)/200*100&gt;=33,1,0))))))+IF((J15+K15)/200*100&gt;=80,5,IF((J15+K15)/200*100&gt;=70,4,IF((J15+K15)/200*100&gt;=60,3.5,IF((J15+K15)/200*100&gt;=50,3,IF((J15+K15)/200*100&gt;=40,2,IF((J15+K15)/200*100&gt;=33,1,0))))))+IF(L15&gt;=80,5,IF(L15&gt;=70,4,IF(L15&gt;=60,3.5,IF(L15&gt;=50,3,IF(L15&gt;=40,2,IF(L15&gt;=33,1,0))))))+IF(M15&gt;=80,5,IF(M15&gt;=70,4,IF(M15&gt;=60,3.5,IF(M15&gt;=50,3,IF(M15&gt;=40,2,IF(M15&gt;=33,1,0))))))+IF(N15/50*100&gt;=80,5,IF(N15/50*100&gt;=70,4,IF(N15/50*100&gt;=60,3.5,IF(N15/50*100&gt;=50,3,IF(N15/50*100&gt;=40,2,IF(N15/50*100&gt;=33,1,0)))))))/8+IF(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))&gt;=2,(IF(O15&gt;=80,5,IF(O15&gt;=70,4,IF(O15&gt;=60,3.5,IF(O15&gt;=50,3,IF(O15&gt;=40,2,IF(O15&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U15" s="6">
         <f>IF(T15&gt;=5,"A+",IF(T15&gt;=4,"A",IF(T15&gt;=3.5,"A-",IF(T15&gt;=3,"B",IF(T15&gt;=2,"C",IF(T15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1911,43 +1892,41 @@
       <c r="I16" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="J16" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="K16" s="2" t="n">
+      <c r="J16" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="L16" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="M16" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q16" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="L16" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="M16" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="N16" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="O16" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="P16" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="Q16" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="R16">
-        <f>SUM(C16:N16)</f>
-        <v/>
-      </c>
-      <c r="S16" s="5">
-        <f>ROUND(R16/11.5,2)</f>
-        <v/>
+      <c r="R16" t="n">
+        <v>86</v>
+      </c>
+      <c r="S16" t="n">
+        <v>93</v>
       </c>
       <c r="T16" s="6">
-        <f>IF(OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,(J16+K16)&lt;66,L16&lt;33,M16&lt;33,N16&lt;8.25,P16&lt;33,Q16&lt;33),0,MIN(5,ROUND((IF((C16+D16)/200*100&gt;=80,5,IF((C16+D16)/200*100&gt;=70,4,IF((C16+D16)/200*100&gt;=60,3.5,IF((C16+D16)/200*100&gt;=50,3,IF((C16+D16)/200*100&gt;=40,2,IF((C16+D16)/200*100&gt;=33,1,0))))))+IF((E16+F16)/200*100&gt;=80,5,IF((E16+F16)/200*100&gt;=70,4,IF((E16+F16)/200*100&gt;=60,3.5,IF((E16+F16)/200*100&gt;=50,3,IF((E16+F16)/200*100&gt;=40,2,IF((E16+F16)/200*100&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF((H16+I16)/200*100&gt;=80,5,IF((H16+I16)/200*100&gt;=70,4,IF((H16+I16)/200*100&gt;=60,3.5,IF((H16+I16)/200*100&gt;=50,3,IF((H16+I16)/200*100&gt;=40,2,IF((H16+I16)/200*100&gt;=33,1,0))))))+IF((J16+K16)/200*100&gt;=80,5,IF((J16+K16)/200*100&gt;=70,4,IF((J16+K16)/200*100&gt;=60,3.5,IF((J16+K16)/200*100&gt;=50,3,IF((J16+K16)/200*100&gt;=40,2,IF((J16+K16)/200*100&gt;=33,1,0))))))+IF(L16&gt;=80,5,IF(L16&gt;=70,4,IF(L16&gt;=60,3.5,IF(L16&gt;=50,3,IF(L16&gt;=40,2,IF(L16&gt;=33,1,0))))))+IF(M16&gt;=80,5,IF(M16&gt;=70,4,IF(M16&gt;=60,3.5,IF(M16&gt;=50,3,IF(M16&gt;=40,2,IF(M16&gt;=33,1,0))))))+IF(N16/50*100&gt;=80,5,IF(N16/50*100&gt;=70,4,IF(N16/50*100&gt;=60,3.5,IF(N16/50*100&gt;=50,3,IF(N16/50*100&gt;=40,2,IF(N16/50*100&gt;=33,1,0)))))))/8+IF(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))&gt;=2,(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U16" s="7">
+        <f>IF(OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,NOT(OR(AND(J16&gt;=10,K16&gt;=23,L16&gt;=10,M16&gt;=23),AND((J16+L16)&gt;=20,(K16+M16)&gt;=46))),N16&lt;33,O16&lt;33,P16&lt;8.25,R16&lt;33,S16&lt;33),0,MIN(5,ROUND((IF((C16+D16)/200*100&gt;=80,5,IF((C16+D16)/200*100&gt;=70,4,IF((C16+D16)/200*100&gt;=60,3.5,IF((C16+D16)/200*100&gt;=50,3,IF((C16+D16)/200*100&gt;=40,2,IF((C16+D16)/200*100&gt;=33,1,0))))))+IF((E16+F16)/200*100&gt;=80,5,IF((E16+F16)/200*100&gt;=70,4,IF((E16+F16)/200*100&gt;=60,3.5,IF((E16+F16)/200*100&gt;=50,3,IF((E16+F16)/200*100&gt;=40,2,IF((E16+F16)/200*100&gt;=33,1,0))))))+IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))+IF((H16+I16)/200*100&gt;=80,5,IF((H16+I16)/200*100&gt;=70,4,IF((H16+I16)/200*100&gt;=60,3.5,IF((H16+I16)/200*100&gt;=50,3,IF((H16+I16)/200*100&gt;=40,2,IF((H16+I16)/200*100&gt;=33,1,0))))))+IF((J16+K16)/200*100&gt;=80,5,IF((J16+K16)/200*100&gt;=70,4,IF((J16+K16)/200*100&gt;=60,3.5,IF((J16+K16)/200*100&gt;=50,3,IF((J16+K16)/200*100&gt;=40,2,IF((J16+K16)/200*100&gt;=33,1,0))))))+IF(L16&gt;=80,5,IF(L16&gt;=70,4,IF(L16&gt;=60,3.5,IF(L16&gt;=50,3,IF(L16&gt;=40,2,IF(L16&gt;=33,1,0))))))+IF(M16&gt;=80,5,IF(M16&gt;=70,4,IF(M16&gt;=60,3.5,IF(M16&gt;=50,3,IF(M16&gt;=40,2,IF(M16&gt;=33,1,0))))))+IF(N16/50*100&gt;=80,5,IF(N16/50*100&gt;=70,4,IF(N16/50*100&gt;=60,3.5,IF(N16/50*100&gt;=50,3,IF(N16/50*100&gt;=40,2,IF(N16/50*100&gt;=33,1,0)))))))/8+IF(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))&gt;=2,(IF(O16&gt;=80,5,IF(O16&gt;=70,4,IF(O16&gt;=60,3.5,IF(O16&gt;=50,3,IF(O16&gt;=40,2,IF(O16&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U16" s="6">
         <f>IF(T16&gt;=5,"A+",IF(T16&gt;=4,"A",IF(T16&gt;=3.5,"A-",IF(T16&gt;=3,"B",IF(T16&gt;=2,"C",IF(T16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -1982,43 +1961,41 @@
       <c r="I17" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="J17" s="2" t="n">
-        <v>66</v>
-      </c>
-      <c r="K17" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="L17" s="2" t="n">
-        <v>71</v>
-      </c>
-      <c r="M17" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="N17" s="4" t="n">
-        <v>46</v>
+      <c r="J17" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="K17" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="L17" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="M17" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>70</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="P17" s="2" t="n">
         <v>72</v>
       </c>
+      <c r="P17" s="4" t="n">
+        <v>33</v>
+      </c>
       <c r="Q17" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="R17" t="n">
         <v>75</v>
       </c>
-      <c r="R17">
-        <f>SUM(C17:N17)</f>
-        <v/>
-      </c>
-      <c r="S17" s="5">
-        <f>ROUND(R17/11.5,2)</f>
-        <v/>
+      <c r="S17" t="n">
+        <v>93</v>
       </c>
       <c r="T17" s="6">
-        <f>IF(OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,(J17+K17)&lt;66,L17&lt;33,M17&lt;33,N17&lt;8.25,P17&lt;33,Q17&lt;33),0,MIN(5,ROUND((IF((C17+D17)/200*100&gt;=80,5,IF((C17+D17)/200*100&gt;=70,4,IF((C17+D17)/200*100&gt;=60,3.5,IF((C17+D17)/200*100&gt;=50,3,IF((C17+D17)/200*100&gt;=40,2,IF((C17+D17)/200*100&gt;=33,1,0))))))+IF((E17+F17)/200*100&gt;=80,5,IF((E17+F17)/200*100&gt;=70,4,IF((E17+F17)/200*100&gt;=60,3.5,IF((E17+F17)/200*100&gt;=50,3,IF((E17+F17)/200*100&gt;=40,2,IF((E17+F17)/200*100&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF((H17+I17)/200*100&gt;=80,5,IF((H17+I17)/200*100&gt;=70,4,IF((H17+I17)/200*100&gt;=60,3.5,IF((H17+I17)/200*100&gt;=50,3,IF((H17+I17)/200*100&gt;=40,2,IF((H17+I17)/200*100&gt;=33,1,0))))))+IF((J17+K17)/200*100&gt;=80,5,IF((J17+K17)/200*100&gt;=70,4,IF((J17+K17)/200*100&gt;=60,3.5,IF((J17+K17)/200*100&gt;=50,3,IF((J17+K17)/200*100&gt;=40,2,IF((J17+K17)/200*100&gt;=33,1,0))))))+IF(L17&gt;=80,5,IF(L17&gt;=70,4,IF(L17&gt;=60,3.5,IF(L17&gt;=50,3,IF(L17&gt;=40,2,IF(L17&gt;=33,1,0))))))+IF(M17&gt;=80,5,IF(M17&gt;=70,4,IF(M17&gt;=60,3.5,IF(M17&gt;=50,3,IF(M17&gt;=40,2,IF(M17&gt;=33,1,0))))))+IF(N17/50*100&gt;=80,5,IF(N17/50*100&gt;=70,4,IF(N17/50*100&gt;=60,3.5,IF(N17/50*100&gt;=50,3,IF(N17/50*100&gt;=40,2,IF(N17/50*100&gt;=33,1,0)))))))/8+IF(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))&gt;=2,(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U17" s="7">
+        <f>IF(OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,NOT(OR(AND(J17&gt;=10,K17&gt;=23,L17&gt;=10,M17&gt;=23),AND((J17+L17)&gt;=20,(K17+M17)&gt;=46))),N17&lt;33,O17&lt;33,P17&lt;8.25,R17&lt;33,S17&lt;33),0,MIN(5,ROUND((IF((C17+D17)/200*100&gt;=80,5,IF((C17+D17)/200*100&gt;=70,4,IF((C17+D17)/200*100&gt;=60,3.5,IF((C17+D17)/200*100&gt;=50,3,IF((C17+D17)/200*100&gt;=40,2,IF((C17+D17)/200*100&gt;=33,1,0))))))+IF((E17+F17)/200*100&gt;=80,5,IF((E17+F17)/200*100&gt;=70,4,IF((E17+F17)/200*100&gt;=60,3.5,IF((E17+F17)/200*100&gt;=50,3,IF((E17+F17)/200*100&gt;=40,2,IF((E17+F17)/200*100&gt;=33,1,0))))))+IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))+IF((H17+I17)/200*100&gt;=80,5,IF((H17+I17)/200*100&gt;=70,4,IF((H17+I17)/200*100&gt;=60,3.5,IF((H17+I17)/200*100&gt;=50,3,IF((H17+I17)/200*100&gt;=40,2,IF((H17+I17)/200*100&gt;=33,1,0))))))+IF((J17+K17)/200*100&gt;=80,5,IF((J17+K17)/200*100&gt;=70,4,IF((J17+K17)/200*100&gt;=60,3.5,IF((J17+K17)/200*100&gt;=50,3,IF((J17+K17)/200*100&gt;=40,2,IF((J17+K17)/200*100&gt;=33,1,0))))))+IF(L17&gt;=80,5,IF(L17&gt;=70,4,IF(L17&gt;=60,3.5,IF(L17&gt;=50,3,IF(L17&gt;=40,2,IF(L17&gt;=33,1,0))))))+IF(M17&gt;=80,5,IF(M17&gt;=70,4,IF(M17&gt;=60,3.5,IF(M17&gt;=50,3,IF(M17&gt;=40,2,IF(M17&gt;=33,1,0))))))+IF(N17/50*100&gt;=80,5,IF(N17/50*100&gt;=70,4,IF(N17/50*100&gt;=60,3.5,IF(N17/50*100&gt;=50,3,IF(N17/50*100&gt;=40,2,IF(N17/50*100&gt;=33,1,0)))))))/8+IF(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))&gt;=2,(IF(O17&gt;=80,5,IF(O17&gt;=70,4,IF(O17&gt;=60,3.5,IF(O17&gt;=50,3,IF(O17&gt;=40,2,IF(O17&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U17" s="6">
         <f>IF(T17&gt;=5,"A+",IF(T17&gt;=4,"A",IF(T17&gt;=3.5,"A-",IF(T17&gt;=3,"B",IF(T17&gt;=2,"C",IF(T17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2053,43 +2030,41 @@
       <c r="I18" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="J18" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="K18" s="2" t="n">
-        <v>76</v>
-      </c>
-      <c r="L18" s="3" t="n">
-        <v>88</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="N18" s="8" t="n">
-        <v>37</v>
-      </c>
-      <c r="O18" s="4" t="n">
-        <v>53</v>
-      </c>
-      <c r="P18" s="3" t="n">
-        <v>84</v>
+      <c r="J18" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="L18" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="M18" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="O18" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="P18" s="4" t="n">
+        <v>31</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="R18">
-        <f>SUM(C18:N18)</f>
-        <v/>
-      </c>
-      <c r="S18" s="5">
-        <f>ROUND(R18/11.5,2)</f>
-        <v/>
+        <v>85</v>
+      </c>
+      <c r="R18" t="n">
+        <v>71</v>
+      </c>
+      <c r="S18" t="n">
+        <v>91</v>
       </c>
       <c r="T18" s="6">
-        <f>IF(OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,(J18+K18)&lt;66,L18&lt;33,M18&lt;33,N18&lt;8.25,P18&lt;33,Q18&lt;33),0,MIN(5,ROUND((IF((C18+D18)/200*100&gt;=80,5,IF((C18+D18)/200*100&gt;=70,4,IF((C18+D18)/200*100&gt;=60,3.5,IF((C18+D18)/200*100&gt;=50,3,IF((C18+D18)/200*100&gt;=40,2,IF((C18+D18)/200*100&gt;=33,1,0))))))+IF((E18+F18)/200*100&gt;=80,5,IF((E18+F18)/200*100&gt;=70,4,IF((E18+F18)/200*100&gt;=60,3.5,IF((E18+F18)/200*100&gt;=50,3,IF((E18+F18)/200*100&gt;=40,2,IF((E18+F18)/200*100&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF((H18+I18)/200*100&gt;=80,5,IF((H18+I18)/200*100&gt;=70,4,IF((H18+I18)/200*100&gt;=60,3.5,IF((H18+I18)/200*100&gt;=50,3,IF((H18+I18)/200*100&gt;=40,2,IF((H18+I18)/200*100&gt;=33,1,0))))))+IF((J18+K18)/200*100&gt;=80,5,IF((J18+K18)/200*100&gt;=70,4,IF((J18+K18)/200*100&gt;=60,3.5,IF((J18+K18)/200*100&gt;=50,3,IF((J18+K18)/200*100&gt;=40,2,IF((J18+K18)/200*100&gt;=33,1,0))))))+IF(L18&gt;=80,5,IF(L18&gt;=70,4,IF(L18&gt;=60,3.5,IF(L18&gt;=50,3,IF(L18&gt;=40,2,IF(L18&gt;=33,1,0))))))+IF(M18&gt;=80,5,IF(M18&gt;=70,4,IF(M18&gt;=60,3.5,IF(M18&gt;=50,3,IF(M18&gt;=40,2,IF(M18&gt;=33,1,0))))))+IF(N18/50*100&gt;=80,5,IF(N18/50*100&gt;=70,4,IF(N18/50*100&gt;=60,3.5,IF(N18/50*100&gt;=50,3,IF(N18/50*100&gt;=40,2,IF(N18/50*100&gt;=33,1,0)))))))/8+IF(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))&gt;=2,(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U18" s="7">
+        <f>IF(OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,NOT(OR(AND(J18&gt;=10,K18&gt;=23,L18&gt;=10,M18&gt;=23),AND((J18+L18)&gt;=20,(K18+M18)&gt;=46))),N18&lt;33,O18&lt;33,P18&lt;8.25,R18&lt;33,S18&lt;33),0,MIN(5,ROUND((IF((C18+D18)/200*100&gt;=80,5,IF((C18+D18)/200*100&gt;=70,4,IF((C18+D18)/200*100&gt;=60,3.5,IF((C18+D18)/200*100&gt;=50,3,IF((C18+D18)/200*100&gt;=40,2,IF((C18+D18)/200*100&gt;=33,1,0))))))+IF((E18+F18)/200*100&gt;=80,5,IF((E18+F18)/200*100&gt;=70,4,IF((E18+F18)/200*100&gt;=60,3.5,IF((E18+F18)/200*100&gt;=50,3,IF((E18+F18)/200*100&gt;=40,2,IF((E18+F18)/200*100&gt;=33,1,0))))))+IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))+IF((H18+I18)/200*100&gt;=80,5,IF((H18+I18)/200*100&gt;=70,4,IF((H18+I18)/200*100&gt;=60,3.5,IF((H18+I18)/200*100&gt;=50,3,IF((H18+I18)/200*100&gt;=40,2,IF((H18+I18)/200*100&gt;=33,1,0))))))+IF((J18+K18)/200*100&gt;=80,5,IF((J18+K18)/200*100&gt;=70,4,IF((J18+K18)/200*100&gt;=60,3.5,IF((J18+K18)/200*100&gt;=50,3,IF((J18+K18)/200*100&gt;=40,2,IF((J18+K18)/200*100&gt;=33,1,0))))))+IF(L18&gt;=80,5,IF(L18&gt;=70,4,IF(L18&gt;=60,3.5,IF(L18&gt;=50,3,IF(L18&gt;=40,2,IF(L18&gt;=33,1,0))))))+IF(M18&gt;=80,5,IF(M18&gt;=70,4,IF(M18&gt;=60,3.5,IF(M18&gt;=50,3,IF(M18&gt;=40,2,IF(M18&gt;=33,1,0))))))+IF(N18/50*100&gt;=80,5,IF(N18/50*100&gt;=70,4,IF(N18/50*100&gt;=60,3.5,IF(N18/50*100&gt;=50,3,IF(N18/50*100&gt;=40,2,IF(N18/50*100&gt;=33,1,0)))))))/8+IF(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))&gt;=2,(IF(O18&gt;=80,5,IF(O18&gt;=70,4,IF(O18&gt;=60,3.5,IF(O18&gt;=50,3,IF(O18&gt;=40,2,IF(O18&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U18" s="6">
         <f>IF(T18&gt;=5,"A+",IF(T18&gt;=4,"A",IF(T18&gt;=3.5,"A-",IF(T18&gt;=3,"B",IF(T18&gt;=2,"C",IF(T18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2124,43 +2099,41 @@
       <c r="I19" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="J19" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="L19" s="3" t="n">
-        <v>93</v>
+      <c r="J19" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="K19" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="L19" s="4" t="n">
+        <v>17</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="N19" s="8" t="n">
-        <v>38</v>
-      </c>
-      <c r="O19" s="4" t="n">
-        <v>56</v>
-      </c>
-      <c r="P19" s="3" t="n">
-        <v>95</v>
+        <v>65</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <v>47</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>83</v>
-      </c>
-      <c r="R19">
-        <f>SUM(C19:N19)</f>
-        <v/>
-      </c>
-      <c r="S19" s="5">
-        <f>ROUND(R19/11.5,2)</f>
-        <v/>
+        <v>81</v>
+      </c>
+      <c r="R19" t="n">
+        <v>86</v>
+      </c>
+      <c r="S19" t="n">
+        <v>85</v>
       </c>
       <c r="T19" s="6">
-        <f>IF(OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,(J19+K19)&lt;66,L19&lt;33,M19&lt;33,N19&lt;8.25,P19&lt;33,Q19&lt;33),0,MIN(5,ROUND((IF((C19+D19)/200*100&gt;=80,5,IF((C19+D19)/200*100&gt;=70,4,IF((C19+D19)/200*100&gt;=60,3.5,IF((C19+D19)/200*100&gt;=50,3,IF((C19+D19)/200*100&gt;=40,2,IF((C19+D19)/200*100&gt;=33,1,0))))))+IF((E19+F19)/200*100&gt;=80,5,IF((E19+F19)/200*100&gt;=70,4,IF((E19+F19)/200*100&gt;=60,3.5,IF((E19+F19)/200*100&gt;=50,3,IF((E19+F19)/200*100&gt;=40,2,IF((E19+F19)/200*100&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF((H19+I19)/200*100&gt;=80,5,IF((H19+I19)/200*100&gt;=70,4,IF((H19+I19)/200*100&gt;=60,3.5,IF((H19+I19)/200*100&gt;=50,3,IF((H19+I19)/200*100&gt;=40,2,IF((H19+I19)/200*100&gt;=33,1,0))))))+IF((J19+K19)/200*100&gt;=80,5,IF((J19+K19)/200*100&gt;=70,4,IF((J19+K19)/200*100&gt;=60,3.5,IF((J19+K19)/200*100&gt;=50,3,IF((J19+K19)/200*100&gt;=40,2,IF((J19+K19)/200*100&gt;=33,1,0))))))+IF(L19&gt;=80,5,IF(L19&gt;=70,4,IF(L19&gt;=60,3.5,IF(L19&gt;=50,3,IF(L19&gt;=40,2,IF(L19&gt;=33,1,0))))))+IF(M19&gt;=80,5,IF(M19&gt;=70,4,IF(M19&gt;=60,3.5,IF(M19&gt;=50,3,IF(M19&gt;=40,2,IF(M19&gt;=33,1,0))))))+IF(N19/50*100&gt;=80,5,IF(N19/50*100&gt;=70,4,IF(N19/50*100&gt;=60,3.5,IF(N19/50*100&gt;=50,3,IF(N19/50*100&gt;=40,2,IF(N19/50*100&gt;=33,1,0)))))))/8+IF(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))&gt;=2,(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U19" s="7">
+        <f>IF(OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,NOT(OR(AND(J19&gt;=10,K19&gt;=23,L19&gt;=10,M19&gt;=23),AND((J19+L19)&gt;=20,(K19+M19)&gt;=46))),N19&lt;33,O19&lt;33,P19&lt;8.25,R19&lt;33,S19&lt;33),0,MIN(5,ROUND((IF((C19+D19)/200*100&gt;=80,5,IF((C19+D19)/200*100&gt;=70,4,IF((C19+D19)/200*100&gt;=60,3.5,IF((C19+D19)/200*100&gt;=50,3,IF((C19+D19)/200*100&gt;=40,2,IF((C19+D19)/200*100&gt;=33,1,0))))))+IF((E19+F19)/200*100&gt;=80,5,IF((E19+F19)/200*100&gt;=70,4,IF((E19+F19)/200*100&gt;=60,3.5,IF((E19+F19)/200*100&gt;=50,3,IF((E19+F19)/200*100&gt;=40,2,IF((E19+F19)/200*100&gt;=33,1,0))))))+IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))+IF((H19+I19)/200*100&gt;=80,5,IF((H19+I19)/200*100&gt;=70,4,IF((H19+I19)/200*100&gt;=60,3.5,IF((H19+I19)/200*100&gt;=50,3,IF((H19+I19)/200*100&gt;=40,2,IF((H19+I19)/200*100&gt;=33,1,0))))))+IF((J19+K19)/200*100&gt;=80,5,IF((J19+K19)/200*100&gt;=70,4,IF((J19+K19)/200*100&gt;=60,3.5,IF((J19+K19)/200*100&gt;=50,3,IF((J19+K19)/200*100&gt;=40,2,IF((J19+K19)/200*100&gt;=33,1,0))))))+IF(L19&gt;=80,5,IF(L19&gt;=70,4,IF(L19&gt;=60,3.5,IF(L19&gt;=50,3,IF(L19&gt;=40,2,IF(L19&gt;=33,1,0))))))+IF(M19&gt;=80,5,IF(M19&gt;=70,4,IF(M19&gt;=60,3.5,IF(M19&gt;=50,3,IF(M19&gt;=40,2,IF(M19&gt;=33,1,0))))))+IF(N19/50*100&gt;=80,5,IF(N19/50*100&gt;=70,4,IF(N19/50*100&gt;=60,3.5,IF(N19/50*100&gt;=50,3,IF(N19/50*100&gt;=40,2,IF(N19/50*100&gt;=33,1,0)))))))/8+IF(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))&gt;=2,(IF(O19&gt;=80,5,IF(O19&gt;=70,4,IF(O19&gt;=60,3.5,IF(O19&gt;=50,3,IF(O19&gt;=40,2,IF(O19&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U19" s="6">
         <f>IF(T19&gt;=5,"A+",IF(T19&gt;=4,"A",IF(T19&gt;=3.5,"A-",IF(T19&gt;=3,"B",IF(T19&gt;=2,"C",IF(T19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2195,43 +2168,41 @@
       <c r="I20" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="J20" s="2" t="n">
+      <c r="J20" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="K20" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="O20" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="P20" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="R20" t="n">
         <v>72</v>
       </c>
-      <c r="K20" s="3" t="n">
-        <v>91</v>
-      </c>
-      <c r="L20" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="M20" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="N20" s="4" t="n">
-        <v>45</v>
-      </c>
-      <c r="O20" s="4" t="n">
-        <v>53</v>
-      </c>
-      <c r="P20" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="Q20" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="R20">
-        <f>SUM(C20:N20)</f>
-        <v/>
-      </c>
-      <c r="S20" s="5">
-        <f>ROUND(R20/11.5,2)</f>
-        <v/>
+      <c r="S20" t="n">
+        <v>83</v>
       </c>
       <c r="T20" s="6">
-        <f>IF(OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,(J20+K20)&lt;66,L20&lt;33,M20&lt;33,N20&lt;8.25,P20&lt;33,Q20&lt;33),0,MIN(5,ROUND((IF((C20+D20)/200*100&gt;=80,5,IF((C20+D20)/200*100&gt;=70,4,IF((C20+D20)/200*100&gt;=60,3.5,IF((C20+D20)/200*100&gt;=50,3,IF((C20+D20)/200*100&gt;=40,2,IF((C20+D20)/200*100&gt;=33,1,0))))))+IF((E20+F20)/200*100&gt;=80,5,IF((E20+F20)/200*100&gt;=70,4,IF((E20+F20)/200*100&gt;=60,3.5,IF((E20+F20)/200*100&gt;=50,3,IF((E20+F20)/200*100&gt;=40,2,IF((E20+F20)/200*100&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF((H20+I20)/200*100&gt;=80,5,IF((H20+I20)/200*100&gt;=70,4,IF((H20+I20)/200*100&gt;=60,3.5,IF((H20+I20)/200*100&gt;=50,3,IF((H20+I20)/200*100&gt;=40,2,IF((H20+I20)/200*100&gt;=33,1,0))))))+IF((J20+K20)/200*100&gt;=80,5,IF((J20+K20)/200*100&gt;=70,4,IF((J20+K20)/200*100&gt;=60,3.5,IF((J20+K20)/200*100&gt;=50,3,IF((J20+K20)/200*100&gt;=40,2,IF((J20+K20)/200*100&gt;=33,1,0))))))+IF(L20&gt;=80,5,IF(L20&gt;=70,4,IF(L20&gt;=60,3.5,IF(L20&gt;=50,3,IF(L20&gt;=40,2,IF(L20&gt;=33,1,0))))))+IF(M20&gt;=80,5,IF(M20&gt;=70,4,IF(M20&gt;=60,3.5,IF(M20&gt;=50,3,IF(M20&gt;=40,2,IF(M20&gt;=33,1,0))))))+IF(N20/50*100&gt;=80,5,IF(N20/50*100&gt;=70,4,IF(N20/50*100&gt;=60,3.5,IF(N20/50*100&gt;=50,3,IF(N20/50*100&gt;=40,2,IF(N20/50*100&gt;=33,1,0)))))))/8+IF(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))&gt;=2,(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U20" s="7">
+        <f>IF(OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,NOT(OR(AND(J20&gt;=10,K20&gt;=23,L20&gt;=10,M20&gt;=23),AND((J20+L20)&gt;=20,(K20+M20)&gt;=46))),N20&lt;33,O20&lt;33,P20&lt;8.25,R20&lt;33,S20&lt;33),0,MIN(5,ROUND((IF((C20+D20)/200*100&gt;=80,5,IF((C20+D20)/200*100&gt;=70,4,IF((C20+D20)/200*100&gt;=60,3.5,IF((C20+D20)/200*100&gt;=50,3,IF((C20+D20)/200*100&gt;=40,2,IF((C20+D20)/200*100&gt;=33,1,0))))))+IF((E20+F20)/200*100&gt;=80,5,IF((E20+F20)/200*100&gt;=70,4,IF((E20+F20)/200*100&gt;=60,3.5,IF((E20+F20)/200*100&gt;=50,3,IF((E20+F20)/200*100&gt;=40,2,IF((E20+F20)/200*100&gt;=33,1,0))))))+IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))+IF((H20+I20)/200*100&gt;=80,5,IF((H20+I20)/200*100&gt;=70,4,IF((H20+I20)/200*100&gt;=60,3.5,IF((H20+I20)/200*100&gt;=50,3,IF((H20+I20)/200*100&gt;=40,2,IF((H20+I20)/200*100&gt;=33,1,0))))))+IF((J20+K20)/200*100&gt;=80,5,IF((J20+K20)/200*100&gt;=70,4,IF((J20+K20)/200*100&gt;=60,3.5,IF((J20+K20)/200*100&gt;=50,3,IF((J20+K20)/200*100&gt;=40,2,IF((J20+K20)/200*100&gt;=33,1,0))))))+IF(L20&gt;=80,5,IF(L20&gt;=70,4,IF(L20&gt;=60,3.5,IF(L20&gt;=50,3,IF(L20&gt;=40,2,IF(L20&gt;=33,1,0))))))+IF(M20&gt;=80,5,IF(M20&gt;=70,4,IF(M20&gt;=60,3.5,IF(M20&gt;=50,3,IF(M20&gt;=40,2,IF(M20&gt;=33,1,0))))))+IF(N20/50*100&gt;=80,5,IF(N20/50*100&gt;=70,4,IF(N20/50*100&gt;=60,3.5,IF(N20/50*100&gt;=50,3,IF(N20/50*100&gt;=40,2,IF(N20/50*100&gt;=33,1,0)))))))/8+IF(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))&gt;=2,(IF(O20&gt;=80,5,IF(O20&gt;=70,4,IF(O20&gt;=60,3.5,IF(O20&gt;=50,3,IF(O20&gt;=40,2,IF(O20&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U20" s="6">
         <f>IF(T20&gt;=5,"A+",IF(T20&gt;=4,"A",IF(T20&gt;=3.5,"A-",IF(T20&gt;=3,"B",IF(T20&gt;=2,"C",IF(T20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2266,43 +2237,41 @@
       <c r="I21" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="J21" s="2" t="n">
-        <v>69</v>
-      </c>
-      <c r="K21" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="L21" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="M21" s="2" t="n">
+      <c r="J21" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="L21" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="M21" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="O21" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="N21" s="8" t="n">
-        <v>36</v>
-      </c>
-      <c r="O21" s="2" t="n">
+      <c r="R21" t="n">
         <v>75</v>
       </c>
-      <c r="P21" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="Q21" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="R21">
-        <f>SUM(C21:N21)</f>
-        <v/>
-      </c>
-      <c r="S21" s="5">
-        <f>ROUND(R21/11.5,2)</f>
-        <v/>
+      <c r="S21" t="n">
+        <v>81</v>
       </c>
       <c r="T21" s="6">
-        <f>IF(OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,(J21+K21)&lt;66,L21&lt;33,M21&lt;33,N21&lt;8.25,P21&lt;33,Q21&lt;33),0,MIN(5,ROUND((IF((C21+D21)/200*100&gt;=80,5,IF((C21+D21)/200*100&gt;=70,4,IF((C21+D21)/200*100&gt;=60,3.5,IF((C21+D21)/200*100&gt;=50,3,IF((C21+D21)/200*100&gt;=40,2,IF((C21+D21)/200*100&gt;=33,1,0))))))+IF((E21+F21)/200*100&gt;=80,5,IF((E21+F21)/200*100&gt;=70,4,IF((E21+F21)/200*100&gt;=60,3.5,IF((E21+F21)/200*100&gt;=50,3,IF((E21+F21)/200*100&gt;=40,2,IF((E21+F21)/200*100&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF((H21+I21)/200*100&gt;=80,5,IF((H21+I21)/200*100&gt;=70,4,IF((H21+I21)/200*100&gt;=60,3.5,IF((H21+I21)/200*100&gt;=50,3,IF((H21+I21)/200*100&gt;=40,2,IF((H21+I21)/200*100&gt;=33,1,0))))))+IF((J21+K21)/200*100&gt;=80,5,IF((J21+K21)/200*100&gt;=70,4,IF((J21+K21)/200*100&gt;=60,3.5,IF((J21+K21)/200*100&gt;=50,3,IF((J21+K21)/200*100&gt;=40,2,IF((J21+K21)/200*100&gt;=33,1,0))))))+IF(L21&gt;=80,5,IF(L21&gt;=70,4,IF(L21&gt;=60,3.5,IF(L21&gt;=50,3,IF(L21&gt;=40,2,IF(L21&gt;=33,1,0))))))+IF(M21&gt;=80,5,IF(M21&gt;=70,4,IF(M21&gt;=60,3.5,IF(M21&gt;=50,3,IF(M21&gt;=40,2,IF(M21&gt;=33,1,0))))))+IF(N21/50*100&gt;=80,5,IF(N21/50*100&gt;=70,4,IF(N21/50*100&gt;=60,3.5,IF(N21/50*100&gt;=50,3,IF(N21/50*100&gt;=40,2,IF(N21/50*100&gt;=33,1,0)))))))/8+IF(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))&gt;=2,(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))-2)/8,0),2)))</f>
-        <v/>
-      </c>
-      <c r="U21" s="7">
+        <f>IF(OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,NOT(OR(AND(J21&gt;=10,K21&gt;=23,L21&gt;=10,M21&gt;=23),AND((J21+L21)&gt;=20,(K21+M21)&gt;=46))),N21&lt;33,O21&lt;33,P21&lt;8.25,R21&lt;33,S21&lt;33),0,MIN(5,ROUND((IF((C21+D21)/200*100&gt;=80,5,IF((C21+D21)/200*100&gt;=70,4,IF((C21+D21)/200*100&gt;=60,3.5,IF((C21+D21)/200*100&gt;=50,3,IF((C21+D21)/200*100&gt;=40,2,IF((C21+D21)/200*100&gt;=33,1,0))))))+IF((E21+F21)/200*100&gt;=80,5,IF((E21+F21)/200*100&gt;=70,4,IF((E21+F21)/200*100&gt;=60,3.5,IF((E21+F21)/200*100&gt;=50,3,IF((E21+F21)/200*100&gt;=40,2,IF((E21+F21)/200*100&gt;=33,1,0))))))+IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))+IF((H21+I21)/200*100&gt;=80,5,IF((H21+I21)/200*100&gt;=70,4,IF((H21+I21)/200*100&gt;=60,3.5,IF((H21+I21)/200*100&gt;=50,3,IF((H21+I21)/200*100&gt;=40,2,IF((H21+I21)/200*100&gt;=33,1,0))))))+IF((J21+K21)/200*100&gt;=80,5,IF((J21+K21)/200*100&gt;=70,4,IF((J21+K21)/200*100&gt;=60,3.5,IF((J21+K21)/200*100&gt;=50,3,IF((J21+K21)/200*100&gt;=40,2,IF((J21+K21)/200*100&gt;=33,1,0))))))+IF(L21&gt;=80,5,IF(L21&gt;=70,4,IF(L21&gt;=60,3.5,IF(L21&gt;=50,3,IF(L21&gt;=40,2,IF(L21&gt;=33,1,0))))))+IF(M21&gt;=80,5,IF(M21&gt;=70,4,IF(M21&gt;=60,3.5,IF(M21&gt;=50,3,IF(M21&gt;=40,2,IF(M21&gt;=33,1,0))))))+IF(N21/50*100&gt;=80,5,IF(N21/50*100&gt;=70,4,IF(N21/50*100&gt;=60,3.5,IF(N21/50*100&gt;=50,3,IF(N21/50*100&gt;=40,2,IF(N21/50*100&gt;=33,1,0)))))))/8+IF(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))&gt;=2,(IF(O21&gt;=80,5,IF(O21&gt;=70,4,IF(O21&gt;=60,3.5,IF(O21&gt;=50,3,IF(O21&gt;=40,2,IF(O21&gt;=33,1,0))))))-2)/8,0),2)))</f>
+        <v/>
+      </c>
+      <c r="U21" s="6">
         <f>IF(T21&gt;=5,"A+",IF(T21&gt;=4,"A",IF(T21&gt;=3.5,"A-",IF(T21&gt;=3,"B",IF(T21&gt;=2,"C",IF(T21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
@@ -2334,7 +2303,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>📊 ACADEMIC RESULTS DASHBOARD</t>
         </is>
@@ -2342,116 +2311,116 @@
     </row>
     <row r="2"/>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>SUMMARY STATISTICS</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="9" t="inlineStr">
         <is>
           <t>Total Students:</t>
         </is>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <f>COUNTA('Data Source'!B:B)-1</f>
         <v/>
       </c>
-      <c r="E5" s="11" t="inlineStr">
+      <c r="E5" s="9" t="inlineStr">
         <is>
           <t>Average GPA:</t>
         </is>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <f>IFERROR(ROUND(AVERAGE('Data Source'!T:T),2), 0)</f>
         <v/>
       </c>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="H5" s="9" t="inlineStr">
         <is>
           <t>Highest Total:</t>
         </is>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="10">
         <f>MAX('Data Source'!R:R)</f>
         <v/>
       </c>
-      <c r="K5" s="11" t="inlineStr">
+      <c r="K5" s="9" t="inlineStr">
         <is>
           <t>Pass Rate:</t>
         </is>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <f>IF(C5&gt;0,COUNTIF('Data Source'!T:T,"&gt;0")/C5,0)</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="inlineStr">
+      <c r="A7" s="13" t="inlineStr">
         <is>
           <t>GRADE DISTRIBUTION</t>
         </is>
       </c>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="D7" s="13" t="inlineStr">
         <is>
           <t>SUBJECT-WISE AVERAGE</t>
         </is>
       </c>
-      <c r="G7" s="15" t="inlineStr">
+      <c r="G7" s="13" t="inlineStr">
         <is>
           <t>TOP 5 STUDENTS</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="inlineStr">
+      <c r="A8" s="14" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="E8" s="16" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>Avg</t>
         </is>
       </c>
-      <c r="F8" s="16" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="G8" s="16" t="inlineStr">
+      <c r="G8" s="14" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
-      <c r="H8" s="11" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="I8" s="16" t="inlineStr">
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="15" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"A+")</f>
         <v/>
       </c>
@@ -2464,29 +2433,29 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!C:C),2),0)</f>
         <v/>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <f>IFERROR(ROUND(E9/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="15" t="n">
         <v>1</v>
       </c>
       <c r="H9">
-        <f>'Data Source'!B4</f>
+        <f>'Data Source'!B10</f>
         <v/>
       </c>
       <c r="I9" s="6">
-        <f>'Data Source'!T4</f>
+        <f>'Data Source'!T10</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="15" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"A")</f>
         <v/>
       </c>
@@ -2499,29 +2468,29 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!D:D),2),0)</f>
         <v/>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <f>IFERROR(ROUND(E10/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="15" t="n">
         <v>2</v>
       </c>
       <c r="H10">
-        <f>'Data Source'!B5</f>
+        <f>'Data Source'!B21</f>
         <v/>
       </c>
       <c r="I10" s="6">
-        <f>'Data Source'!T5</f>
+        <f>'Data Source'!T21</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="15" t="inlineStr">
         <is>
           <t>A-</t>
         </is>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"A-")</f>
         <v/>
       </c>
@@ -2534,11 +2503,11 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!E:E),2),0)</f>
         <v/>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <f>IFERROR(ROUND(E11/100*100,1),0)</f>
         <v/>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="15" t="n">
         <v>3</v>
       </c>
       <c r="H11">
@@ -2551,12 +2520,12 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="A12" s="15" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"B")</f>
         <v/>
       </c>
@@ -2569,29 +2538,29 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!F:F),2),0)</f>
         <v/>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <f>IFERROR(ROUND(E12/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="15" t="n">
         <v>4</v>
       </c>
       <c r="H12">
-        <f>'Data Source'!B17</f>
+        <f>'Data Source'!B19</f>
         <v/>
       </c>
       <c r="I12" s="6">
-        <f>'Data Source'!T17</f>
+        <f>'Data Source'!T19</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="15" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"C")</f>
         <v/>
       </c>
@@ -2604,29 +2573,29 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!G:G),2),0)</f>
         <v/>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <f>IFERROR(ROUND(E13/200*100,1),0)</f>
         <v/>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="15" t="n">
         <v>5</v>
       </c>
       <c r="H13">
-        <f>'Data Source'!B6</f>
+        <f>'Data Source'!B12</f>
         <v/>
       </c>
       <c r="I13" s="6">
-        <f>'Data Source'!T6</f>
+        <f>'Data Source'!T12</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="A14" s="15" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"D")</f>
         <v/>
       </c>
@@ -2639,18 +2608,18 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!H:H),2),0)</f>
         <v/>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="16">
         <f>IFERROR(ROUND(E14/100*100,1),0)</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="A15" s="15" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="15">
         <f>COUNTIF('Data Source'!Q:Q,"F")</f>
         <v/>
       </c>
@@ -2663,7 +2632,7 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!I:I),2),0)</f>
         <v/>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="16">
         <f>IFERROR(ROUND(E15/100*100,1),0)</f>
         <v/>
       </c>
@@ -2678,7 +2647,7 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!J:J),2),0)</f>
         <v/>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <f>IFERROR(ROUND(E16/100*100,1),0)</f>
         <v/>
       </c>
@@ -2693,7 +2662,7 @@
         <f>IFERROR(ROUND(AVERAGE('Data Source'!K:K),2),0)</f>
         <v/>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="16">
         <f>IFERROR(ROUND(E17/100*100,1),0)</f>
         <v/>
       </c>
@@ -2739,91 +2708,91 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="17" t="inlineStr">
         <is>
           <t>SUBJECT-WISE GRADES</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="inlineStr">
+      <c r="A2" s="18" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
       </c>
-      <c r="B2" s="19" t="inlineStr">
+      <c r="B2" s="18" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C2" s="19" t="inlineStr">
+      <c r="C2" s="18" t="inlineStr">
         <is>
           <t>Quran+Hadith</t>
         </is>
       </c>
-      <c r="D2" s="19" t="inlineStr">
+      <c r="D2" s="18" t="inlineStr">
         <is>
           <t>Arabic</t>
         </is>
       </c>
-      <c r="E2" s="19" t="inlineStr">
+      <c r="E2" s="18" t="inlineStr">
         <is>
           <t>Aqaid</t>
         </is>
       </c>
-      <c r="F2" s="19" t="inlineStr">
+      <c r="F2" s="18" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="G2" s="19" t="inlineStr">
+      <c r="G2" s="18" t="inlineStr">
         <is>
           <t>Bangla</t>
         </is>
       </c>
-      <c r="H2" s="19" t="inlineStr">
+      <c r="H2" s="18" t="inlineStr">
         <is>
           <t>Math</t>
         </is>
       </c>
-      <c r="I2" s="19" t="inlineStr">
+      <c r="I2" s="18" t="inlineStr">
         <is>
           <t>History</t>
         </is>
       </c>
-      <c r="J2" s="19" t="inlineStr">
+      <c r="J2" s="18" t="inlineStr">
         <is>
           <t>ICT</t>
         </is>
       </c>
-      <c r="K2" s="19" t="inlineStr">
+      <c r="K2" s="18" t="inlineStr">
         <is>
           <t>Mantiq</t>
         </is>
       </c>
-      <c r="L2" s="19" t="inlineStr">
+      <c r="L2" s="18" t="inlineStr">
         <is>
           <t>Career</t>
         </is>
       </c>
-      <c r="M2" s="19" t="inlineStr">
+      <c r="M2" s="18" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
-      <c r="N2" s="19" t="inlineStr">
+      <c r="N2" s="18" t="inlineStr">
         <is>
           <t>Overall GPA</t>
         </is>
       </c>
-      <c r="O2" s="19" t="inlineStr">
+      <c r="O2" s="18" t="inlineStr">
         <is>
           <t>Overall Grade</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7">
+      <c r="A3" s="15">
         <f>'Data Source'!A2</f>
         <v/>
       </c>
@@ -2831,47 +2800,47 @@
         <f>'Data Source'!B2</f>
         <v/>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="15">
         <f>IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=80,"A+",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=70,"A",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=60,"A-",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=50,"B",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=40,"C",IF(('Data Source'!C2+'Data Source'!D2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="15">
         <f>IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=80,"A+",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=70,"A",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=60,"A-",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=50,"B",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=40,"C",IF(('Data Source'!E2+'Data Source'!F2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="15">
         <f>IF('Data Source'!G2&gt;=80,"A+",IF('Data Source'!G2&gt;=70,"A",IF('Data Source'!G2&gt;=60,"A-",IF('Data Source'!G2&gt;=50,"B",IF('Data Source'!G2&gt;=40,"C",IF('Data Source'!G2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="15">
         <f>IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=80,"A+",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=70,"A",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=60,"A-",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=50,"B",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=40,"C",IF(('Data Source'!H2+'Data Source'!I2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="15">
         <f>IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=80,"A+",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=70,"A",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=60,"A-",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=50,"B",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=40,"C",IF(('Data Source'!J2+'Data Source'!K2)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="15">
         <f>IF('Data Source'!L2&gt;=80,"A+",IF('Data Source'!L2&gt;=70,"A",IF('Data Source'!L2&gt;=60,"A-",IF('Data Source'!L2&gt;=50,"B",IF('Data Source'!L2&gt;=40,"C",IF('Data Source'!L2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="15">
         <f>IF('Data Source'!M2&gt;=80,"A+",IF('Data Source'!M2&gt;=70,"A",IF('Data Source'!M2&gt;=60,"A-",IF('Data Source'!M2&gt;=50,"B",IF('Data Source'!M2&gt;=40,"C",IF('Data Source'!M2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="15">
         <f>IF('Data Source'!N2/50*100&gt;=80,"A+",IF('Data Source'!N2/50*100&gt;=70,"A",IF('Data Source'!N2/50*100&gt;=60,"A-",IF('Data Source'!N2/50*100&gt;=50,"B",IF('Data Source'!N2/50*100&gt;=40,"C",IF('Data Source'!N2/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="15">
         <f>IF('Data Source'!O2&gt;=80,"A+",IF('Data Source'!O2&gt;=70,"A",IF('Data Source'!O2&gt;=60,"A-",IF('Data Source'!O2&gt;=50,"B",IF('Data Source'!O2&gt;=40,"C",IF('Data Source'!O2&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="15">
         <f>IF('Data Source'!P2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="15">
         <f>IF('Data Source'!Q2&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -2879,13 +2848,13 @@
         <f>'Data Source'!T2</f>
         <v/>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="15">
         <f>'Data Source'!U2</f>
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7">
+      <c r="A4" s="15">
         <f>'Data Source'!A3</f>
         <v/>
       </c>
@@ -2893,47 +2862,47 @@
         <f>'Data Source'!B3</f>
         <v/>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="15">
         <f>IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=80,"A+",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=70,"A",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=60,"A-",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=50,"B",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=40,"C",IF(('Data Source'!C3+'Data Source'!D3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="15">
         <f>IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=80,"A+",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=70,"A",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=60,"A-",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=50,"B",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=40,"C",IF(('Data Source'!E3+'Data Source'!F3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="15">
         <f>IF('Data Source'!G3&gt;=80,"A+",IF('Data Source'!G3&gt;=70,"A",IF('Data Source'!G3&gt;=60,"A-",IF('Data Source'!G3&gt;=50,"B",IF('Data Source'!G3&gt;=40,"C",IF('Data Source'!G3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="15">
         <f>IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=80,"A+",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=70,"A",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=60,"A-",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=50,"B",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=40,"C",IF(('Data Source'!H3+'Data Source'!I3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="15">
         <f>IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=80,"A+",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=70,"A",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=60,"A-",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=50,"B",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=40,"C",IF(('Data Source'!J3+'Data Source'!K3)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="15">
         <f>IF('Data Source'!L3&gt;=80,"A+",IF('Data Source'!L3&gt;=70,"A",IF('Data Source'!L3&gt;=60,"A-",IF('Data Source'!L3&gt;=50,"B",IF('Data Source'!L3&gt;=40,"C",IF('Data Source'!L3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="15">
         <f>IF('Data Source'!M3&gt;=80,"A+",IF('Data Source'!M3&gt;=70,"A",IF('Data Source'!M3&gt;=60,"A-",IF('Data Source'!M3&gt;=50,"B",IF('Data Source'!M3&gt;=40,"C",IF('Data Source'!M3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="15">
         <f>IF('Data Source'!N3/50*100&gt;=80,"A+",IF('Data Source'!N3/50*100&gt;=70,"A",IF('Data Source'!N3/50*100&gt;=60,"A-",IF('Data Source'!N3/50*100&gt;=50,"B",IF('Data Source'!N3/50*100&gt;=40,"C",IF('Data Source'!N3/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="15">
         <f>IF('Data Source'!O3&gt;=80,"A+",IF('Data Source'!O3&gt;=70,"A",IF('Data Source'!O3&gt;=60,"A-",IF('Data Source'!O3&gt;=50,"B",IF('Data Source'!O3&gt;=40,"C",IF('Data Source'!O3&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="15">
         <f>IF('Data Source'!P3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="15">
         <f>IF('Data Source'!Q3&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -2941,13 +2910,13 @@
         <f>'Data Source'!T3</f>
         <v/>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="15">
         <f>'Data Source'!U3</f>
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7">
+      <c r="A5" s="15">
         <f>'Data Source'!A4</f>
         <v/>
       </c>
@@ -2955,47 +2924,47 @@
         <f>'Data Source'!B4</f>
         <v/>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="15">
         <f>IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=80,"A+",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=70,"A",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=60,"A-",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=50,"B",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=40,"C",IF(('Data Source'!C4+'Data Source'!D4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="15">
         <f>IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=80,"A+",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=70,"A",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=60,"A-",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=50,"B",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=40,"C",IF(('Data Source'!E4+'Data Source'!F4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="15">
         <f>IF('Data Source'!G4&gt;=80,"A+",IF('Data Source'!G4&gt;=70,"A",IF('Data Source'!G4&gt;=60,"A-",IF('Data Source'!G4&gt;=50,"B",IF('Data Source'!G4&gt;=40,"C",IF('Data Source'!G4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="15">
         <f>IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=80,"A+",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=70,"A",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=60,"A-",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=50,"B",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=40,"C",IF(('Data Source'!H4+'Data Source'!I4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="15">
         <f>IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=80,"A+",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=70,"A",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=60,"A-",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=50,"B",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=40,"C",IF(('Data Source'!J4+'Data Source'!K4)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="15">
         <f>IF('Data Source'!L4&gt;=80,"A+",IF('Data Source'!L4&gt;=70,"A",IF('Data Source'!L4&gt;=60,"A-",IF('Data Source'!L4&gt;=50,"B",IF('Data Source'!L4&gt;=40,"C",IF('Data Source'!L4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="15">
         <f>IF('Data Source'!M4&gt;=80,"A+",IF('Data Source'!M4&gt;=70,"A",IF('Data Source'!M4&gt;=60,"A-",IF('Data Source'!M4&gt;=50,"B",IF('Data Source'!M4&gt;=40,"C",IF('Data Source'!M4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="15">
         <f>IF('Data Source'!N4/50*100&gt;=80,"A+",IF('Data Source'!N4/50*100&gt;=70,"A",IF('Data Source'!N4/50*100&gt;=60,"A-",IF('Data Source'!N4/50*100&gt;=50,"B",IF('Data Source'!N4/50*100&gt;=40,"C",IF('Data Source'!N4/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="15">
         <f>IF('Data Source'!O4&gt;=80,"A+",IF('Data Source'!O4&gt;=70,"A",IF('Data Source'!O4&gt;=60,"A-",IF('Data Source'!O4&gt;=50,"B",IF('Data Source'!O4&gt;=40,"C",IF('Data Source'!O4&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="15">
         <f>IF('Data Source'!P4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="15">
         <f>IF('Data Source'!Q4&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3003,13 +2972,13 @@
         <f>'Data Source'!T4</f>
         <v/>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="15">
         <f>'Data Source'!U4</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7">
+      <c r="A6" s="15">
         <f>'Data Source'!A5</f>
         <v/>
       </c>
@@ -3017,47 +2986,47 @@
         <f>'Data Source'!B5</f>
         <v/>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="15">
         <f>IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=80,"A+",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=70,"A",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=60,"A-",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=50,"B",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=40,"C",IF(('Data Source'!C5+'Data Source'!D5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="15">
         <f>IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=80,"A+",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=70,"A",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=60,"A-",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=50,"B",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=40,"C",IF(('Data Source'!E5+'Data Source'!F5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="15">
         <f>IF('Data Source'!G5&gt;=80,"A+",IF('Data Source'!G5&gt;=70,"A",IF('Data Source'!G5&gt;=60,"A-",IF('Data Source'!G5&gt;=50,"B",IF('Data Source'!G5&gt;=40,"C",IF('Data Source'!G5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="15">
         <f>IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=80,"A+",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=70,"A",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=60,"A-",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=50,"B",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=40,"C",IF(('Data Source'!H5+'Data Source'!I5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="15">
         <f>IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=80,"A+",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=70,"A",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=60,"A-",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=50,"B",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=40,"C",IF(('Data Source'!J5+'Data Source'!K5)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="15">
         <f>IF('Data Source'!L5&gt;=80,"A+",IF('Data Source'!L5&gt;=70,"A",IF('Data Source'!L5&gt;=60,"A-",IF('Data Source'!L5&gt;=50,"B",IF('Data Source'!L5&gt;=40,"C",IF('Data Source'!L5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="15">
         <f>IF('Data Source'!M5&gt;=80,"A+",IF('Data Source'!M5&gt;=70,"A",IF('Data Source'!M5&gt;=60,"A-",IF('Data Source'!M5&gt;=50,"B",IF('Data Source'!M5&gt;=40,"C",IF('Data Source'!M5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="15">
         <f>IF('Data Source'!N5/50*100&gt;=80,"A+",IF('Data Source'!N5/50*100&gt;=70,"A",IF('Data Source'!N5/50*100&gt;=60,"A-",IF('Data Source'!N5/50*100&gt;=50,"B",IF('Data Source'!N5/50*100&gt;=40,"C",IF('Data Source'!N5/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="15">
         <f>IF('Data Source'!O5&gt;=80,"A+",IF('Data Source'!O5&gt;=70,"A",IF('Data Source'!O5&gt;=60,"A-",IF('Data Source'!O5&gt;=50,"B",IF('Data Source'!O5&gt;=40,"C",IF('Data Source'!O5&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="15">
         <f>IF('Data Source'!P5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="15">
         <f>IF('Data Source'!Q5&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3065,13 +3034,13 @@
         <f>'Data Source'!T5</f>
         <v/>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="15">
         <f>'Data Source'!U5</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7">
+      <c r="A7" s="15">
         <f>'Data Source'!A6</f>
         <v/>
       </c>
@@ -3079,47 +3048,47 @@
         <f>'Data Source'!B6</f>
         <v/>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="15">
         <f>IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=80,"A+",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=70,"A",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=60,"A-",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=50,"B",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=40,"C",IF(('Data Source'!C6+'Data Source'!D6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="15">
         <f>IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=80,"A+",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=70,"A",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=60,"A-",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=50,"B",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=40,"C",IF(('Data Source'!E6+'Data Source'!F6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="15">
         <f>IF('Data Source'!G6&gt;=80,"A+",IF('Data Source'!G6&gt;=70,"A",IF('Data Source'!G6&gt;=60,"A-",IF('Data Source'!G6&gt;=50,"B",IF('Data Source'!G6&gt;=40,"C",IF('Data Source'!G6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="15">
         <f>IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=80,"A+",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=70,"A",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=60,"A-",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=50,"B",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=40,"C",IF(('Data Source'!H6+'Data Source'!I6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="15">
         <f>IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=80,"A+",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=70,"A",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=60,"A-",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=50,"B",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=40,"C",IF(('Data Source'!J6+'Data Source'!K6)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="15">
         <f>IF('Data Source'!L6&gt;=80,"A+",IF('Data Source'!L6&gt;=70,"A",IF('Data Source'!L6&gt;=60,"A-",IF('Data Source'!L6&gt;=50,"B",IF('Data Source'!L6&gt;=40,"C",IF('Data Source'!L6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="15">
         <f>IF('Data Source'!M6&gt;=80,"A+",IF('Data Source'!M6&gt;=70,"A",IF('Data Source'!M6&gt;=60,"A-",IF('Data Source'!M6&gt;=50,"B",IF('Data Source'!M6&gt;=40,"C",IF('Data Source'!M6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="15">
         <f>IF('Data Source'!N6/50*100&gt;=80,"A+",IF('Data Source'!N6/50*100&gt;=70,"A",IF('Data Source'!N6/50*100&gt;=60,"A-",IF('Data Source'!N6/50*100&gt;=50,"B",IF('Data Source'!N6/50*100&gt;=40,"C",IF('Data Source'!N6/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="15">
         <f>IF('Data Source'!O6&gt;=80,"A+",IF('Data Source'!O6&gt;=70,"A",IF('Data Source'!O6&gt;=60,"A-",IF('Data Source'!O6&gt;=50,"B",IF('Data Source'!O6&gt;=40,"C",IF('Data Source'!O6&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="15">
         <f>IF('Data Source'!P6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="15">
         <f>IF('Data Source'!Q6&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3127,13 +3096,13 @@
         <f>'Data Source'!T6</f>
         <v/>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="15">
         <f>'Data Source'!U6</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7">
+      <c r="A8" s="15">
         <f>'Data Source'!A7</f>
         <v/>
       </c>
@@ -3141,47 +3110,47 @@
         <f>'Data Source'!B7</f>
         <v/>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="15">
         <f>IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=80,"A+",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=70,"A",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=60,"A-",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=50,"B",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=40,"C",IF(('Data Source'!C7+'Data Source'!D7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="15">
         <f>IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=80,"A+",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=70,"A",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=60,"A-",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=50,"B",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=40,"C",IF(('Data Source'!E7+'Data Source'!F7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="15">
         <f>IF('Data Source'!G7&gt;=80,"A+",IF('Data Source'!G7&gt;=70,"A",IF('Data Source'!G7&gt;=60,"A-",IF('Data Source'!G7&gt;=50,"B",IF('Data Source'!G7&gt;=40,"C",IF('Data Source'!G7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="15">
         <f>IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=80,"A+",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=70,"A",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=60,"A-",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=50,"B",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=40,"C",IF(('Data Source'!H7+'Data Source'!I7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="15">
         <f>IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=80,"A+",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=70,"A",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=60,"A-",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=50,"B",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=40,"C",IF(('Data Source'!J7+'Data Source'!K7)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="15">
         <f>IF('Data Source'!L7&gt;=80,"A+",IF('Data Source'!L7&gt;=70,"A",IF('Data Source'!L7&gt;=60,"A-",IF('Data Source'!L7&gt;=50,"B",IF('Data Source'!L7&gt;=40,"C",IF('Data Source'!L7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="15">
         <f>IF('Data Source'!M7&gt;=80,"A+",IF('Data Source'!M7&gt;=70,"A",IF('Data Source'!M7&gt;=60,"A-",IF('Data Source'!M7&gt;=50,"B",IF('Data Source'!M7&gt;=40,"C",IF('Data Source'!M7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="15">
         <f>IF('Data Source'!N7/50*100&gt;=80,"A+",IF('Data Source'!N7/50*100&gt;=70,"A",IF('Data Source'!N7/50*100&gt;=60,"A-",IF('Data Source'!N7/50*100&gt;=50,"B",IF('Data Source'!N7/50*100&gt;=40,"C",IF('Data Source'!N7/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="15">
         <f>IF('Data Source'!O7&gt;=80,"A+",IF('Data Source'!O7&gt;=70,"A",IF('Data Source'!O7&gt;=60,"A-",IF('Data Source'!O7&gt;=50,"B",IF('Data Source'!O7&gt;=40,"C",IF('Data Source'!O7&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="15">
         <f>IF('Data Source'!P7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="15">
         <f>IF('Data Source'!Q7&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3189,13 +3158,13 @@
         <f>'Data Source'!T7</f>
         <v/>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="15">
         <f>'Data Source'!U7</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7">
+      <c r="A9" s="15">
         <f>'Data Source'!A8</f>
         <v/>
       </c>
@@ -3203,47 +3172,47 @@
         <f>'Data Source'!B8</f>
         <v/>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="15">
         <f>IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=80,"A+",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=70,"A",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=60,"A-",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=50,"B",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=40,"C",IF(('Data Source'!C8+'Data Source'!D8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="15">
         <f>IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=80,"A+",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=70,"A",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=60,"A-",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=50,"B",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=40,"C",IF(('Data Source'!E8+'Data Source'!F8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="15">
         <f>IF('Data Source'!G8&gt;=80,"A+",IF('Data Source'!G8&gt;=70,"A",IF('Data Source'!G8&gt;=60,"A-",IF('Data Source'!G8&gt;=50,"B",IF('Data Source'!G8&gt;=40,"C",IF('Data Source'!G8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="15">
         <f>IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=80,"A+",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=70,"A",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=60,"A-",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=50,"B",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=40,"C",IF(('Data Source'!H8+'Data Source'!I8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="15">
         <f>IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=80,"A+",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=70,"A",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=60,"A-",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=50,"B",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=40,"C",IF(('Data Source'!J8+'Data Source'!K8)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="15">
         <f>IF('Data Source'!L8&gt;=80,"A+",IF('Data Source'!L8&gt;=70,"A",IF('Data Source'!L8&gt;=60,"A-",IF('Data Source'!L8&gt;=50,"B",IF('Data Source'!L8&gt;=40,"C",IF('Data Source'!L8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="15">
         <f>IF('Data Source'!M8&gt;=80,"A+",IF('Data Source'!M8&gt;=70,"A",IF('Data Source'!M8&gt;=60,"A-",IF('Data Source'!M8&gt;=50,"B",IF('Data Source'!M8&gt;=40,"C",IF('Data Source'!M8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="15">
         <f>IF('Data Source'!N8/50*100&gt;=80,"A+",IF('Data Source'!N8/50*100&gt;=70,"A",IF('Data Source'!N8/50*100&gt;=60,"A-",IF('Data Source'!N8/50*100&gt;=50,"B",IF('Data Source'!N8/50*100&gt;=40,"C",IF('Data Source'!N8/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="15">
         <f>IF('Data Source'!O8&gt;=80,"A+",IF('Data Source'!O8&gt;=70,"A",IF('Data Source'!O8&gt;=60,"A-",IF('Data Source'!O8&gt;=50,"B",IF('Data Source'!O8&gt;=40,"C",IF('Data Source'!O8&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="15">
         <f>IF('Data Source'!P8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="15">
         <f>IF('Data Source'!Q8&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3251,13 +3220,13 @@
         <f>'Data Source'!T8</f>
         <v/>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="15">
         <f>'Data Source'!U8</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7">
+      <c r="A10" s="15">
         <f>'Data Source'!A9</f>
         <v/>
       </c>
@@ -3265,47 +3234,47 @@
         <f>'Data Source'!B9</f>
         <v/>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="15">
         <f>IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=80,"A+",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=70,"A",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=60,"A-",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=50,"B",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=40,"C",IF(('Data Source'!C9+'Data Source'!D9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="15">
         <f>IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=80,"A+",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=70,"A",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=60,"A-",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=50,"B",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=40,"C",IF(('Data Source'!E9+'Data Source'!F9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="15">
         <f>IF('Data Source'!G9&gt;=80,"A+",IF('Data Source'!G9&gt;=70,"A",IF('Data Source'!G9&gt;=60,"A-",IF('Data Source'!G9&gt;=50,"B",IF('Data Source'!G9&gt;=40,"C",IF('Data Source'!G9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="15">
         <f>IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=80,"A+",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=70,"A",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=60,"A-",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=50,"B",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=40,"C",IF(('Data Source'!H9+'Data Source'!I9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="15">
         <f>IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=80,"A+",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=70,"A",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=60,"A-",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=50,"B",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=40,"C",IF(('Data Source'!J9+'Data Source'!K9)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="15">
         <f>IF('Data Source'!L9&gt;=80,"A+",IF('Data Source'!L9&gt;=70,"A",IF('Data Source'!L9&gt;=60,"A-",IF('Data Source'!L9&gt;=50,"B",IF('Data Source'!L9&gt;=40,"C",IF('Data Source'!L9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="15">
         <f>IF('Data Source'!M9&gt;=80,"A+",IF('Data Source'!M9&gt;=70,"A",IF('Data Source'!M9&gt;=60,"A-",IF('Data Source'!M9&gt;=50,"B",IF('Data Source'!M9&gt;=40,"C",IF('Data Source'!M9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="15">
         <f>IF('Data Source'!N9/50*100&gt;=80,"A+",IF('Data Source'!N9/50*100&gt;=70,"A",IF('Data Source'!N9/50*100&gt;=60,"A-",IF('Data Source'!N9/50*100&gt;=50,"B",IF('Data Source'!N9/50*100&gt;=40,"C",IF('Data Source'!N9/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="15">
         <f>IF('Data Source'!O9&gt;=80,"A+",IF('Data Source'!O9&gt;=70,"A",IF('Data Source'!O9&gt;=60,"A-",IF('Data Source'!O9&gt;=50,"B",IF('Data Source'!O9&gt;=40,"C",IF('Data Source'!O9&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="15">
         <f>IF('Data Source'!P9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="15">
         <f>IF('Data Source'!Q9&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3313,13 +3282,13 @@
         <f>'Data Source'!T9</f>
         <v/>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="15">
         <f>'Data Source'!U9</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7">
+      <c r="A11" s="15">
         <f>'Data Source'!A10</f>
         <v/>
       </c>
@@ -3327,47 +3296,47 @@
         <f>'Data Source'!B10</f>
         <v/>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="15">
         <f>IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=80,"A+",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=70,"A",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=60,"A-",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=50,"B",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=40,"C",IF(('Data Source'!C10+'Data Source'!D10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="15">
         <f>IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=80,"A+",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=70,"A",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=60,"A-",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=50,"B",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=40,"C",IF(('Data Source'!E10+'Data Source'!F10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="15">
         <f>IF('Data Source'!G10&gt;=80,"A+",IF('Data Source'!G10&gt;=70,"A",IF('Data Source'!G10&gt;=60,"A-",IF('Data Source'!G10&gt;=50,"B",IF('Data Source'!G10&gt;=40,"C",IF('Data Source'!G10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="15">
         <f>IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=80,"A+",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=70,"A",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=60,"A-",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=50,"B",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=40,"C",IF(('Data Source'!H10+'Data Source'!I10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="15">
         <f>IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=80,"A+",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=70,"A",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=60,"A-",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=50,"B",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=40,"C",IF(('Data Source'!J10+'Data Source'!K10)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="15">
         <f>IF('Data Source'!L10&gt;=80,"A+",IF('Data Source'!L10&gt;=70,"A",IF('Data Source'!L10&gt;=60,"A-",IF('Data Source'!L10&gt;=50,"B",IF('Data Source'!L10&gt;=40,"C",IF('Data Source'!L10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="15">
         <f>IF('Data Source'!M10&gt;=80,"A+",IF('Data Source'!M10&gt;=70,"A",IF('Data Source'!M10&gt;=60,"A-",IF('Data Source'!M10&gt;=50,"B",IF('Data Source'!M10&gt;=40,"C",IF('Data Source'!M10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="15">
         <f>IF('Data Source'!N10/50*100&gt;=80,"A+",IF('Data Source'!N10/50*100&gt;=70,"A",IF('Data Source'!N10/50*100&gt;=60,"A-",IF('Data Source'!N10/50*100&gt;=50,"B",IF('Data Source'!N10/50*100&gt;=40,"C",IF('Data Source'!N10/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="15">
         <f>IF('Data Source'!O10&gt;=80,"A+",IF('Data Source'!O10&gt;=70,"A",IF('Data Source'!O10&gt;=60,"A-",IF('Data Source'!O10&gt;=50,"B",IF('Data Source'!O10&gt;=40,"C",IF('Data Source'!O10&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="15">
         <f>IF('Data Source'!P10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="15">
         <f>IF('Data Source'!Q10&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3375,13 +3344,13 @@
         <f>'Data Source'!T10</f>
         <v/>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="15">
         <f>'Data Source'!U10</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7">
+      <c r="A12" s="15">
         <f>'Data Source'!A11</f>
         <v/>
       </c>
@@ -3389,47 +3358,47 @@
         <f>'Data Source'!B11</f>
         <v/>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="15">
         <f>IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=80,"A+",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=70,"A",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=60,"A-",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=50,"B",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=40,"C",IF(('Data Source'!C11+'Data Source'!D11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="15">
         <f>IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=80,"A+",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=70,"A",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=60,"A-",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=50,"B",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=40,"C",IF(('Data Source'!E11+'Data Source'!F11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="15">
         <f>IF('Data Source'!G11&gt;=80,"A+",IF('Data Source'!G11&gt;=70,"A",IF('Data Source'!G11&gt;=60,"A-",IF('Data Source'!G11&gt;=50,"B",IF('Data Source'!G11&gt;=40,"C",IF('Data Source'!G11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="15">
         <f>IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=80,"A+",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=70,"A",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=60,"A-",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=50,"B",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=40,"C",IF(('Data Source'!H11+'Data Source'!I11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="15">
         <f>IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=80,"A+",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=70,"A",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=60,"A-",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=50,"B",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=40,"C",IF(('Data Source'!J11+'Data Source'!K11)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="15">
         <f>IF('Data Source'!L11&gt;=80,"A+",IF('Data Source'!L11&gt;=70,"A",IF('Data Source'!L11&gt;=60,"A-",IF('Data Source'!L11&gt;=50,"B",IF('Data Source'!L11&gt;=40,"C",IF('Data Source'!L11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="15">
         <f>IF('Data Source'!M11&gt;=80,"A+",IF('Data Source'!M11&gt;=70,"A",IF('Data Source'!M11&gt;=60,"A-",IF('Data Source'!M11&gt;=50,"B",IF('Data Source'!M11&gt;=40,"C",IF('Data Source'!M11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="15">
         <f>IF('Data Source'!N11/50*100&gt;=80,"A+",IF('Data Source'!N11/50*100&gt;=70,"A",IF('Data Source'!N11/50*100&gt;=60,"A-",IF('Data Source'!N11/50*100&gt;=50,"B",IF('Data Source'!N11/50*100&gt;=40,"C",IF('Data Source'!N11/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="15">
         <f>IF('Data Source'!O11&gt;=80,"A+",IF('Data Source'!O11&gt;=70,"A",IF('Data Source'!O11&gt;=60,"A-",IF('Data Source'!O11&gt;=50,"B",IF('Data Source'!O11&gt;=40,"C",IF('Data Source'!O11&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="15">
         <f>IF('Data Source'!P11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="15">
         <f>IF('Data Source'!Q11&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3437,13 +3406,13 @@
         <f>'Data Source'!T11</f>
         <v/>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="15">
         <f>'Data Source'!U11</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7">
+      <c r="A13" s="15">
         <f>'Data Source'!A12</f>
         <v/>
       </c>
@@ -3451,47 +3420,47 @@
         <f>'Data Source'!B12</f>
         <v/>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="15">
         <f>IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=80,"A+",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=70,"A",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=60,"A-",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=50,"B",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=40,"C",IF(('Data Source'!C12+'Data Source'!D12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="15">
         <f>IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=80,"A+",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=70,"A",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=60,"A-",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=50,"B",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=40,"C",IF(('Data Source'!E12+'Data Source'!F12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="15">
         <f>IF('Data Source'!G12&gt;=80,"A+",IF('Data Source'!G12&gt;=70,"A",IF('Data Source'!G12&gt;=60,"A-",IF('Data Source'!G12&gt;=50,"B",IF('Data Source'!G12&gt;=40,"C",IF('Data Source'!G12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="15">
         <f>IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=80,"A+",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=70,"A",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=60,"A-",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=50,"B",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=40,"C",IF(('Data Source'!H12+'Data Source'!I12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="15">
         <f>IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=80,"A+",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=70,"A",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=60,"A-",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=50,"B",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=40,"C",IF(('Data Source'!J12+'Data Source'!K12)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="15">
         <f>IF('Data Source'!L12&gt;=80,"A+",IF('Data Source'!L12&gt;=70,"A",IF('Data Source'!L12&gt;=60,"A-",IF('Data Source'!L12&gt;=50,"B",IF('Data Source'!L12&gt;=40,"C",IF('Data Source'!L12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="15">
         <f>IF('Data Source'!M12&gt;=80,"A+",IF('Data Source'!M12&gt;=70,"A",IF('Data Source'!M12&gt;=60,"A-",IF('Data Source'!M12&gt;=50,"B",IF('Data Source'!M12&gt;=40,"C",IF('Data Source'!M12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="15">
         <f>IF('Data Source'!N12/50*100&gt;=80,"A+",IF('Data Source'!N12/50*100&gt;=70,"A",IF('Data Source'!N12/50*100&gt;=60,"A-",IF('Data Source'!N12/50*100&gt;=50,"B",IF('Data Source'!N12/50*100&gt;=40,"C",IF('Data Source'!N12/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="15">
         <f>IF('Data Source'!O12&gt;=80,"A+",IF('Data Source'!O12&gt;=70,"A",IF('Data Source'!O12&gt;=60,"A-",IF('Data Source'!O12&gt;=50,"B",IF('Data Source'!O12&gt;=40,"C",IF('Data Source'!O12&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="15">
         <f>IF('Data Source'!P12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="15">
         <f>IF('Data Source'!Q12&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3499,13 +3468,13 @@
         <f>'Data Source'!T12</f>
         <v/>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="15">
         <f>'Data Source'!U12</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7">
+      <c r="A14" s="15">
         <f>'Data Source'!A13</f>
         <v/>
       </c>
@@ -3513,47 +3482,47 @@
         <f>'Data Source'!B13</f>
         <v/>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="15">
         <f>IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=80,"A+",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=70,"A",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=60,"A-",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=50,"B",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=40,"C",IF(('Data Source'!C13+'Data Source'!D13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="15">
         <f>IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=80,"A+",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=70,"A",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=60,"A-",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=50,"B",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=40,"C",IF(('Data Source'!E13+'Data Source'!F13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="15">
         <f>IF('Data Source'!G13&gt;=80,"A+",IF('Data Source'!G13&gt;=70,"A",IF('Data Source'!G13&gt;=60,"A-",IF('Data Source'!G13&gt;=50,"B",IF('Data Source'!G13&gt;=40,"C",IF('Data Source'!G13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="15">
         <f>IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=80,"A+",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=70,"A",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=60,"A-",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=50,"B",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=40,"C",IF(('Data Source'!H13+'Data Source'!I13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="15">
         <f>IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=80,"A+",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=70,"A",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=60,"A-",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=50,"B",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=40,"C",IF(('Data Source'!J13+'Data Source'!K13)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="15">
         <f>IF('Data Source'!L13&gt;=80,"A+",IF('Data Source'!L13&gt;=70,"A",IF('Data Source'!L13&gt;=60,"A-",IF('Data Source'!L13&gt;=50,"B",IF('Data Source'!L13&gt;=40,"C",IF('Data Source'!L13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="15">
         <f>IF('Data Source'!M13&gt;=80,"A+",IF('Data Source'!M13&gt;=70,"A",IF('Data Source'!M13&gt;=60,"A-",IF('Data Source'!M13&gt;=50,"B",IF('Data Source'!M13&gt;=40,"C",IF('Data Source'!M13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="15">
         <f>IF('Data Source'!N13/50*100&gt;=80,"A+",IF('Data Source'!N13/50*100&gt;=70,"A",IF('Data Source'!N13/50*100&gt;=60,"A-",IF('Data Source'!N13/50*100&gt;=50,"B",IF('Data Source'!N13/50*100&gt;=40,"C",IF('Data Source'!N13/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="15">
         <f>IF('Data Source'!O13&gt;=80,"A+",IF('Data Source'!O13&gt;=70,"A",IF('Data Source'!O13&gt;=60,"A-",IF('Data Source'!O13&gt;=50,"B",IF('Data Source'!O13&gt;=40,"C",IF('Data Source'!O13&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="15">
         <f>IF('Data Source'!P13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="15">
         <f>IF('Data Source'!Q13&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3561,13 +3530,13 @@
         <f>'Data Source'!T13</f>
         <v/>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="15">
         <f>'Data Source'!U13</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7">
+      <c r="A15" s="15">
         <f>'Data Source'!A14</f>
         <v/>
       </c>
@@ -3575,47 +3544,47 @@
         <f>'Data Source'!B14</f>
         <v/>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="15">
         <f>IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=80,"A+",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=70,"A",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=60,"A-",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=50,"B",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=40,"C",IF(('Data Source'!C14+'Data Source'!D14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="15">
         <f>IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=80,"A+",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=70,"A",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=60,"A-",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=50,"B",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=40,"C",IF(('Data Source'!E14+'Data Source'!F14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="15">
         <f>IF('Data Source'!G14&gt;=80,"A+",IF('Data Source'!G14&gt;=70,"A",IF('Data Source'!G14&gt;=60,"A-",IF('Data Source'!G14&gt;=50,"B",IF('Data Source'!G14&gt;=40,"C",IF('Data Source'!G14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="15">
         <f>IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=80,"A+",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=70,"A",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=60,"A-",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=50,"B",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=40,"C",IF(('Data Source'!H14+'Data Source'!I14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="15">
         <f>IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=80,"A+",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=70,"A",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=60,"A-",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=50,"B",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=40,"C",IF(('Data Source'!J14+'Data Source'!K14)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="15">
         <f>IF('Data Source'!L14&gt;=80,"A+",IF('Data Source'!L14&gt;=70,"A",IF('Data Source'!L14&gt;=60,"A-",IF('Data Source'!L14&gt;=50,"B",IF('Data Source'!L14&gt;=40,"C",IF('Data Source'!L14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="15">
         <f>IF('Data Source'!M14&gt;=80,"A+",IF('Data Source'!M14&gt;=70,"A",IF('Data Source'!M14&gt;=60,"A-",IF('Data Source'!M14&gt;=50,"B",IF('Data Source'!M14&gt;=40,"C",IF('Data Source'!M14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="15">
         <f>IF('Data Source'!N14/50*100&gt;=80,"A+",IF('Data Source'!N14/50*100&gt;=70,"A",IF('Data Source'!N14/50*100&gt;=60,"A-",IF('Data Source'!N14/50*100&gt;=50,"B",IF('Data Source'!N14/50*100&gt;=40,"C",IF('Data Source'!N14/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="15">
         <f>IF('Data Source'!O14&gt;=80,"A+",IF('Data Source'!O14&gt;=70,"A",IF('Data Source'!O14&gt;=60,"A-",IF('Data Source'!O14&gt;=50,"B",IF('Data Source'!O14&gt;=40,"C",IF('Data Source'!O14&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="15">
         <f>IF('Data Source'!P14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="15">
         <f>IF('Data Source'!Q14&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3623,13 +3592,13 @@
         <f>'Data Source'!T14</f>
         <v/>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="15">
         <f>'Data Source'!U14</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7">
+      <c r="A16" s="15">
         <f>'Data Source'!A15</f>
         <v/>
       </c>
@@ -3637,47 +3606,47 @@
         <f>'Data Source'!B15</f>
         <v/>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="15">
         <f>IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=80,"A+",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=70,"A",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=60,"A-",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=50,"B",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=40,"C",IF(('Data Source'!C15+'Data Source'!D15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="15">
         <f>IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=80,"A+",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=70,"A",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=60,"A-",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=50,"B",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=40,"C",IF(('Data Source'!E15+'Data Source'!F15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="15">
         <f>IF('Data Source'!G15&gt;=80,"A+",IF('Data Source'!G15&gt;=70,"A",IF('Data Source'!G15&gt;=60,"A-",IF('Data Source'!G15&gt;=50,"B",IF('Data Source'!G15&gt;=40,"C",IF('Data Source'!G15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="15">
         <f>IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=80,"A+",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=70,"A",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=60,"A-",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=50,"B",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=40,"C",IF(('Data Source'!H15+'Data Source'!I15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="15">
         <f>IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=80,"A+",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=70,"A",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=60,"A-",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=50,"B",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=40,"C",IF(('Data Source'!J15+'Data Source'!K15)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="15">
         <f>IF('Data Source'!L15&gt;=80,"A+",IF('Data Source'!L15&gt;=70,"A",IF('Data Source'!L15&gt;=60,"A-",IF('Data Source'!L15&gt;=50,"B",IF('Data Source'!L15&gt;=40,"C",IF('Data Source'!L15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="15">
         <f>IF('Data Source'!M15&gt;=80,"A+",IF('Data Source'!M15&gt;=70,"A",IF('Data Source'!M15&gt;=60,"A-",IF('Data Source'!M15&gt;=50,"B",IF('Data Source'!M15&gt;=40,"C",IF('Data Source'!M15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="15">
         <f>IF('Data Source'!N15/50*100&gt;=80,"A+",IF('Data Source'!N15/50*100&gt;=70,"A",IF('Data Source'!N15/50*100&gt;=60,"A-",IF('Data Source'!N15/50*100&gt;=50,"B",IF('Data Source'!N15/50*100&gt;=40,"C",IF('Data Source'!N15/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="15">
         <f>IF('Data Source'!O15&gt;=80,"A+",IF('Data Source'!O15&gt;=70,"A",IF('Data Source'!O15&gt;=60,"A-",IF('Data Source'!O15&gt;=50,"B",IF('Data Source'!O15&gt;=40,"C",IF('Data Source'!O15&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="15">
         <f>IF('Data Source'!P15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="15">
         <f>IF('Data Source'!Q15&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3685,13 +3654,13 @@
         <f>'Data Source'!T15</f>
         <v/>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="15">
         <f>'Data Source'!U15</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7">
+      <c r="A17" s="15">
         <f>'Data Source'!A16</f>
         <v/>
       </c>
@@ -3699,47 +3668,47 @@
         <f>'Data Source'!B16</f>
         <v/>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="15">
         <f>IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=80,"A+",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=70,"A",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=60,"A-",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=50,"B",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=40,"C",IF(('Data Source'!C16+'Data Source'!D16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="15">
         <f>IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=80,"A+",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=70,"A",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=60,"A-",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=50,"B",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=40,"C",IF(('Data Source'!E16+'Data Source'!F16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="15">
         <f>IF('Data Source'!G16&gt;=80,"A+",IF('Data Source'!G16&gt;=70,"A",IF('Data Source'!G16&gt;=60,"A-",IF('Data Source'!G16&gt;=50,"B",IF('Data Source'!G16&gt;=40,"C",IF('Data Source'!G16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="15">
         <f>IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=80,"A+",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=70,"A",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=60,"A-",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=50,"B",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=40,"C",IF(('Data Source'!H16+'Data Source'!I16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="15">
         <f>IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=80,"A+",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=70,"A",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=60,"A-",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=50,"B",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=40,"C",IF(('Data Source'!J16+'Data Source'!K16)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="15">
         <f>IF('Data Source'!L16&gt;=80,"A+",IF('Data Source'!L16&gt;=70,"A",IF('Data Source'!L16&gt;=60,"A-",IF('Data Source'!L16&gt;=50,"B",IF('Data Source'!L16&gt;=40,"C",IF('Data Source'!L16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="15">
         <f>IF('Data Source'!M16&gt;=80,"A+",IF('Data Source'!M16&gt;=70,"A",IF('Data Source'!M16&gt;=60,"A-",IF('Data Source'!M16&gt;=50,"B",IF('Data Source'!M16&gt;=40,"C",IF('Data Source'!M16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="15">
         <f>IF('Data Source'!N16/50*100&gt;=80,"A+",IF('Data Source'!N16/50*100&gt;=70,"A",IF('Data Source'!N16/50*100&gt;=60,"A-",IF('Data Source'!N16/50*100&gt;=50,"B",IF('Data Source'!N16/50*100&gt;=40,"C",IF('Data Source'!N16/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="15">
         <f>IF('Data Source'!O16&gt;=80,"A+",IF('Data Source'!O16&gt;=70,"A",IF('Data Source'!O16&gt;=60,"A-",IF('Data Source'!O16&gt;=50,"B",IF('Data Source'!O16&gt;=40,"C",IF('Data Source'!O16&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="15">
         <f>IF('Data Source'!P16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="15">
         <f>IF('Data Source'!Q16&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3747,13 +3716,13 @@
         <f>'Data Source'!T16</f>
         <v/>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="15">
         <f>'Data Source'!U16</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7">
+      <c r="A18" s="15">
         <f>'Data Source'!A17</f>
         <v/>
       </c>
@@ -3761,47 +3730,47 @@
         <f>'Data Source'!B17</f>
         <v/>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="15">
         <f>IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=80,"A+",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=70,"A",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=60,"A-",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=50,"B",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=40,"C",IF(('Data Source'!C17+'Data Source'!D17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="15">
         <f>IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=80,"A+",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=70,"A",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=60,"A-",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=50,"B",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=40,"C",IF(('Data Source'!E17+'Data Source'!F17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="15">
         <f>IF('Data Source'!G17&gt;=80,"A+",IF('Data Source'!G17&gt;=70,"A",IF('Data Source'!G17&gt;=60,"A-",IF('Data Source'!G17&gt;=50,"B",IF('Data Source'!G17&gt;=40,"C",IF('Data Source'!G17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="15">
         <f>IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=80,"A+",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=70,"A",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=60,"A-",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=50,"B",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=40,"C",IF(('Data Source'!H17+'Data Source'!I17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="15">
         <f>IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=80,"A+",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=70,"A",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=60,"A-",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=50,"B",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=40,"C",IF(('Data Source'!J17+'Data Source'!K17)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="15">
         <f>IF('Data Source'!L17&gt;=80,"A+",IF('Data Source'!L17&gt;=70,"A",IF('Data Source'!L17&gt;=60,"A-",IF('Data Source'!L17&gt;=50,"B",IF('Data Source'!L17&gt;=40,"C",IF('Data Source'!L17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="15">
         <f>IF('Data Source'!M17&gt;=80,"A+",IF('Data Source'!M17&gt;=70,"A",IF('Data Source'!M17&gt;=60,"A-",IF('Data Source'!M17&gt;=50,"B",IF('Data Source'!M17&gt;=40,"C",IF('Data Source'!M17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="15">
         <f>IF('Data Source'!N17/50*100&gt;=80,"A+",IF('Data Source'!N17/50*100&gt;=70,"A",IF('Data Source'!N17/50*100&gt;=60,"A-",IF('Data Source'!N17/50*100&gt;=50,"B",IF('Data Source'!N17/50*100&gt;=40,"C",IF('Data Source'!N17/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="15">
         <f>IF('Data Source'!O17&gt;=80,"A+",IF('Data Source'!O17&gt;=70,"A",IF('Data Source'!O17&gt;=60,"A-",IF('Data Source'!O17&gt;=50,"B",IF('Data Source'!O17&gt;=40,"C",IF('Data Source'!O17&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="15">
         <f>IF('Data Source'!P17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="15">
         <f>IF('Data Source'!Q17&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3809,13 +3778,13 @@
         <f>'Data Source'!T17</f>
         <v/>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="15">
         <f>'Data Source'!U17</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7">
+      <c r="A19" s="15">
         <f>'Data Source'!A18</f>
         <v/>
       </c>
@@ -3823,47 +3792,47 @@
         <f>'Data Source'!B18</f>
         <v/>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="15">
         <f>IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=80,"A+",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=70,"A",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=60,"A-",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=50,"B",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=40,"C",IF(('Data Source'!C18+'Data Source'!D18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="15">
         <f>IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=80,"A+",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=70,"A",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=60,"A-",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=50,"B",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=40,"C",IF(('Data Source'!E18+'Data Source'!F18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="15">
         <f>IF('Data Source'!G18&gt;=80,"A+",IF('Data Source'!G18&gt;=70,"A",IF('Data Source'!G18&gt;=60,"A-",IF('Data Source'!G18&gt;=50,"B",IF('Data Source'!G18&gt;=40,"C",IF('Data Source'!G18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="15">
         <f>IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=80,"A+",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=70,"A",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=60,"A-",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=50,"B",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=40,"C",IF(('Data Source'!H18+'Data Source'!I18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="15">
         <f>IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=80,"A+",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=70,"A",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=60,"A-",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=50,"B",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=40,"C",IF(('Data Source'!J18+'Data Source'!K18)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="15">
         <f>IF('Data Source'!L18&gt;=80,"A+",IF('Data Source'!L18&gt;=70,"A",IF('Data Source'!L18&gt;=60,"A-",IF('Data Source'!L18&gt;=50,"B",IF('Data Source'!L18&gt;=40,"C",IF('Data Source'!L18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="15">
         <f>IF('Data Source'!M18&gt;=80,"A+",IF('Data Source'!M18&gt;=70,"A",IF('Data Source'!M18&gt;=60,"A-",IF('Data Source'!M18&gt;=50,"B",IF('Data Source'!M18&gt;=40,"C",IF('Data Source'!M18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="15">
         <f>IF('Data Source'!N18/50*100&gt;=80,"A+",IF('Data Source'!N18/50*100&gt;=70,"A",IF('Data Source'!N18/50*100&gt;=60,"A-",IF('Data Source'!N18/50*100&gt;=50,"B",IF('Data Source'!N18/50*100&gt;=40,"C",IF('Data Source'!N18/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="15">
         <f>IF('Data Source'!O18&gt;=80,"A+",IF('Data Source'!O18&gt;=70,"A",IF('Data Source'!O18&gt;=60,"A-",IF('Data Source'!O18&gt;=50,"B",IF('Data Source'!O18&gt;=40,"C",IF('Data Source'!O18&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="15">
         <f>IF('Data Source'!P18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="15">
         <f>IF('Data Source'!Q18&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3871,13 +3840,13 @@
         <f>'Data Source'!T18</f>
         <v/>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="15">
         <f>'Data Source'!U18</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7">
+      <c r="A20" s="15">
         <f>'Data Source'!A19</f>
         <v/>
       </c>
@@ -3885,47 +3854,47 @@
         <f>'Data Source'!B19</f>
         <v/>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="15">
         <f>IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=80,"A+",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=70,"A",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=60,"A-",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=50,"B",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=40,"C",IF(('Data Source'!C19+'Data Source'!D19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="15">
         <f>IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=80,"A+",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=70,"A",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=60,"A-",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=50,"B",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=40,"C",IF(('Data Source'!E19+'Data Source'!F19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="15">
         <f>IF('Data Source'!G19&gt;=80,"A+",IF('Data Source'!G19&gt;=70,"A",IF('Data Source'!G19&gt;=60,"A-",IF('Data Source'!G19&gt;=50,"B",IF('Data Source'!G19&gt;=40,"C",IF('Data Source'!G19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="15">
         <f>IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=80,"A+",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=70,"A",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=60,"A-",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=50,"B",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=40,"C",IF(('Data Source'!H19+'Data Source'!I19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="15">
         <f>IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=80,"A+",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=70,"A",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=60,"A-",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=50,"B",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=40,"C",IF(('Data Source'!J19+'Data Source'!K19)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="15">
         <f>IF('Data Source'!L19&gt;=80,"A+",IF('Data Source'!L19&gt;=70,"A",IF('Data Source'!L19&gt;=60,"A-",IF('Data Source'!L19&gt;=50,"B",IF('Data Source'!L19&gt;=40,"C",IF('Data Source'!L19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="15">
         <f>IF('Data Source'!M19&gt;=80,"A+",IF('Data Source'!M19&gt;=70,"A",IF('Data Source'!M19&gt;=60,"A-",IF('Data Source'!M19&gt;=50,"B",IF('Data Source'!M19&gt;=40,"C",IF('Data Source'!M19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="15">
         <f>IF('Data Source'!N19/50*100&gt;=80,"A+",IF('Data Source'!N19/50*100&gt;=70,"A",IF('Data Source'!N19/50*100&gt;=60,"A-",IF('Data Source'!N19/50*100&gt;=50,"B",IF('Data Source'!N19/50*100&gt;=40,"C",IF('Data Source'!N19/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="15">
         <f>IF('Data Source'!O19&gt;=80,"A+",IF('Data Source'!O19&gt;=70,"A",IF('Data Source'!O19&gt;=60,"A-",IF('Data Source'!O19&gt;=50,"B",IF('Data Source'!O19&gt;=40,"C",IF('Data Source'!O19&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="15">
         <f>IF('Data Source'!P19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="15">
         <f>IF('Data Source'!Q19&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3933,13 +3902,13 @@
         <f>'Data Source'!T19</f>
         <v/>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="15">
         <f>'Data Source'!U19</f>
         <v/>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7">
+      <c r="A21" s="15">
         <f>'Data Source'!A20</f>
         <v/>
       </c>
@@ -3947,47 +3916,47 @@
         <f>'Data Source'!B20</f>
         <v/>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="15">
         <f>IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=80,"A+",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=70,"A",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=60,"A-",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=50,"B",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=40,"C",IF(('Data Source'!C20+'Data Source'!D20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="15">
         <f>IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=80,"A+",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=70,"A",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=60,"A-",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=50,"B",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=40,"C",IF(('Data Source'!E20+'Data Source'!F20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="15">
         <f>IF('Data Source'!G20&gt;=80,"A+",IF('Data Source'!G20&gt;=70,"A",IF('Data Source'!G20&gt;=60,"A-",IF('Data Source'!G20&gt;=50,"B",IF('Data Source'!G20&gt;=40,"C",IF('Data Source'!G20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="15">
         <f>IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=80,"A+",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=70,"A",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=60,"A-",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=50,"B",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=40,"C",IF(('Data Source'!H20+'Data Source'!I20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="15">
         <f>IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=80,"A+",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=70,"A",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=60,"A-",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=50,"B",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=40,"C",IF(('Data Source'!J20+'Data Source'!K20)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="15">
         <f>IF('Data Source'!L20&gt;=80,"A+",IF('Data Source'!L20&gt;=70,"A",IF('Data Source'!L20&gt;=60,"A-",IF('Data Source'!L20&gt;=50,"B",IF('Data Source'!L20&gt;=40,"C",IF('Data Source'!L20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="15">
         <f>IF('Data Source'!M20&gt;=80,"A+",IF('Data Source'!M20&gt;=70,"A",IF('Data Source'!M20&gt;=60,"A-",IF('Data Source'!M20&gt;=50,"B",IF('Data Source'!M20&gt;=40,"C",IF('Data Source'!M20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="15">
         <f>IF('Data Source'!N20/50*100&gt;=80,"A+",IF('Data Source'!N20/50*100&gt;=70,"A",IF('Data Source'!N20/50*100&gt;=60,"A-",IF('Data Source'!N20/50*100&gt;=50,"B",IF('Data Source'!N20/50*100&gt;=40,"C",IF('Data Source'!N20/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="15">
         <f>IF('Data Source'!O20&gt;=80,"A+",IF('Data Source'!O20&gt;=70,"A",IF('Data Source'!O20&gt;=60,"A-",IF('Data Source'!O20&gt;=50,"B",IF('Data Source'!O20&gt;=40,"C",IF('Data Source'!O20&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="15">
         <f>IF('Data Source'!P20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="15">
         <f>IF('Data Source'!Q20&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -3995,13 +3964,13 @@
         <f>'Data Source'!T20</f>
         <v/>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="15">
         <f>'Data Source'!U20</f>
         <v/>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7">
+      <c r="A22" s="15">
         <f>'Data Source'!A21</f>
         <v/>
       </c>
@@ -4009,47 +3978,47 @@
         <f>'Data Source'!B21</f>
         <v/>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="15">
         <f>IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=80,"A+",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=70,"A",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=60,"A-",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=50,"B",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=40,"C",IF(('Data Source'!C21+'Data Source'!D21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="15">
         <f>IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=80,"A+",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=70,"A",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=60,"A-",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=50,"B",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=40,"C",IF(('Data Source'!E21+'Data Source'!F21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="15">
         <f>IF('Data Source'!G21&gt;=80,"A+",IF('Data Source'!G21&gt;=70,"A",IF('Data Source'!G21&gt;=60,"A-",IF('Data Source'!G21&gt;=50,"B",IF('Data Source'!G21&gt;=40,"C",IF('Data Source'!G21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="15">
         <f>IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=80,"A+",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=70,"A",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=60,"A-",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=50,"B",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=40,"C",IF(('Data Source'!H21+'Data Source'!I21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="15">
         <f>IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=80,"A+",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=70,"A",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=60,"A-",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=50,"B",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=40,"C",IF(('Data Source'!J21+'Data Source'!K21)/200*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="15">
         <f>IF('Data Source'!L21&gt;=80,"A+",IF('Data Source'!L21&gt;=70,"A",IF('Data Source'!L21&gt;=60,"A-",IF('Data Source'!L21&gt;=50,"B",IF('Data Source'!L21&gt;=40,"C",IF('Data Source'!L21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="15">
         <f>IF('Data Source'!M21&gt;=80,"A+",IF('Data Source'!M21&gt;=70,"A",IF('Data Source'!M21&gt;=60,"A-",IF('Data Source'!M21&gt;=50,"B",IF('Data Source'!M21&gt;=40,"C",IF('Data Source'!M21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="15">
         <f>IF('Data Source'!N21/50*100&gt;=80,"A+",IF('Data Source'!N21/50*100&gt;=70,"A",IF('Data Source'!N21/50*100&gt;=60,"A-",IF('Data Source'!N21/50*100&gt;=50,"B",IF('Data Source'!N21/50*100&gt;=40,"C",IF('Data Source'!N21/50*100&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="15">
         <f>IF('Data Source'!O21&gt;=80,"A+",IF('Data Source'!O21&gt;=70,"A",IF('Data Source'!O21&gt;=60,"A-",IF('Data Source'!O21&gt;=50,"B",IF('Data Source'!O21&gt;=40,"C",IF('Data Source'!O21&gt;=33,"D","F"))))))</f>
         <v/>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="15">
         <f>IF('Data Source'!P21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="15">
         <f>IF('Data Source'!Q21&gt;=33,"Pass","Fail")</f>
         <v/>
       </c>
@@ -4057,7 +4026,7 @@
         <f>'Data Source'!T21</f>
         <v/>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="15">
         <f>'Data Source'!U21</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Add Subject-wise GPA sheet and update GPA calculations in Excel generation
</commit_message>
<xml_diff>
--- a/Academic_Results_Dashboard.xlsx
+++ b/Academic_Results_Dashboard.xlsx
@@ -10,7 +10,8 @@
     <sheet name="Data Source" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Subject Grades" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Pivot" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Subject-wise GPA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Pivot" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -749,7 +750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN21"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,9 +781,9 @@
     <col width="12" customWidth="1" min="21" max="21"/>
     <col width="10" customWidth="1" min="22" max="22"/>
     <col width="10" customWidth="1" min="23" max="23"/>
-    <col width="8" customWidth="1" min="24" max="24"/>
+    <col width="14" customWidth="1" min="24" max="24"/>
     <col width="12" customWidth="1" min="25" max="25"/>
-    <col hidden="1" width="13" customWidth="1" min="26" max="26"/>
+    <col width="12" customWidth="1" min="26" max="26"/>
     <col hidden="1" width="13" customWidth="1" min="27" max="27"/>
     <col hidden="1" width="13" customWidth="1" min="28" max="28"/>
     <col hidden="1" width="13" customWidth="1" min="29" max="29"/>
@@ -797,6 +798,7 @@
     <col hidden="1" width="13" customWidth="1" min="38" max="38"/>
     <col hidden="1" width="13" customWidth="1" min="39" max="39"/>
     <col hidden="1" width="13" customWidth="1" min="40" max="40"/>
+    <col hidden="1" width="13" customWidth="1" min="41" max="41"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -917,15 +919,19 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>GPA</t>
+          <t>GPA (Compulsory)</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
+          <t>GPA (Final)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>Overall Grade</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="n"/>
       <c r="AA1" s="1" t="n"/>
       <c r="AB1" s="1" t="n"/>
       <c r="AC1" s="1" t="n"/>
@@ -940,6 +946,7 @@
       <c r="AL1" s="1" t="n"/>
       <c r="AM1" s="1" t="n"/>
       <c r="AN1" s="1" t="n"/>
+      <c r="AO1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1016,71 +1023,75 @@
         <v/>
       </c>
       <c r="X2" s="7">
-        <f>IF(AC2,0,MIN(5,ROUND(AM2+AN2,2)))</f>
-        <v/>
-      </c>
-      <c r="Y2" s="8">
-        <f>IF(X2&gt;=5,"A+",IF(X2&gt;=4,"A",IF(X2&gt;=3.5,"A-",IF(X2&gt;=3,"B",IF(X2&gt;=2,"C",IF(X2&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z2">
+        <f>IF(AD2,0,ROUND(AN2,2))</f>
+        <v/>
+      </c>
+      <c r="Y2" s="7">
+        <f>IF(AD2,0,MIN(5,ROUND(AN2+AO2,2)))</f>
+        <v/>
+      </c>
+      <c r="Z2" s="8">
+        <f>IF(Y2&gt;=5,"A+",IF(Y2&gt;=4,"A",IF(Y2&gt;=3.5,"A-",IF(Y2&gt;=3,"B",IF(Y2&gt;=2,"C",IF(Y2&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA2">
         <f>NOT(OR(AND(J2&gt;=10,K2&gt;=23,L2&gt;=10,M2&gt;=23),AND(J2+L2&gt;=20,K2+M2&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <f>OR(N2&lt;10,O2&lt;23)</f>
         <v/>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <f>OR(P2&lt;10,Q2&lt;23)</f>
         <v/>
       </c>
-      <c r="AC2">
-        <f>OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,Z2,AA2,AB2,R2&lt;8.25,T2&lt;33,U2&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD2">
-        <f>IF((C2+D2)/2&gt;=80,5,IF((C2+D2)/2&gt;=70,4,IF((C2+D2)/2&gt;=60,3.5,IF((C2+D2)/2&gt;=50,3,IF((C2+D2)/2&gt;=40,2,IF((C2+D2)/2&gt;=33,1,0))))))</f>
+        <f>OR((C2+D2)&lt;66,(E2+F2)&lt;66,G2&lt;33,(H2+I2)&lt;66,AA2,AB2,AC2,R2&lt;8.25,T2&lt;33,U2&lt;33)</f>
         <v/>
       </c>
       <c r="AE2">
-        <f>IF((E2+F2)/2&gt;=80,5,IF((E2+F2)/2&gt;=70,4,IF((E2+F2)/2&gt;=60,3.5,IF((E2+F2)/2&gt;=50,3,IF((E2+F2)/2&gt;=40,2,IF((E2+F2)/2&gt;=33,1,0))))))</f>
+        <f>IF(C2+D2&lt;66,0,IF((C2+D2)/2&gt;=80,5,IF((C2+D2)/2&gt;=70,4,IF((C2+D2)/2&gt;=60,3.5,IF((C2+D2)/2&gt;=50,3,IF((C2+D2)/2&gt;=40,2,IF((C2+D2)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF2">
-        <f>IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0))))))</f>
+        <f>IF(E2+F2&lt;66,0,IF((E2+F2)/2&gt;=80,5,IF((E2+F2)/2&gt;=70,4,IF((E2+F2)/2&gt;=60,3.5,IF((E2+F2)/2&gt;=50,3,IF((E2+F2)/2&gt;=40,2,IF((E2+F2)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG2">
-        <f>IF((H2+I2)/2&gt;=80,5,IF((H2+I2)/2&gt;=70,4,IF((H2+I2)/2&gt;=60,3.5,IF((H2+I2)/2&gt;=50,3,IF((H2+I2)/2&gt;=40,2,IF((H2+I2)/2&gt;=33,1,0))))))</f>
+        <f>IF(G2&lt;33,0,IF(G2&gt;=80,5,IF(G2&gt;=70,4,IF(G2&gt;=60,3.5,IF(G2&gt;=50,3,IF(G2&gt;=40,2,IF(G2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH2">
-        <f>IF((J2+K2+L2+M2)/2&gt;=80,5,IF((J2+K2+L2+M2)/2&gt;=70,4,IF((J2+K2+L2+M2)/2&gt;=60,3.5,IF((J2+K2+L2+M2)/2&gt;=50,3,IF((J2+K2+L2+M2)/2&gt;=40,2,IF((J2+K2+L2+M2)/2&gt;=33,1,0))))))</f>
+        <f>IF(H2+I2&lt;66,0,IF((H2+I2)/2&gt;=80,5,IF((H2+I2)/2&gt;=70,4,IF((H2+I2)/2&gt;=60,3.5,IF((H2+I2)/2&gt;=50,3,IF((H2+I2)/2&gt;=40,2,IF((H2+I2)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI2">
-        <f>IF(N2+O2&gt;=80,5,IF(N2+O2&gt;=70,4,IF(N2+O2&gt;=60,3.5,IF(N2+O2&gt;=50,3,IF(N2+O2&gt;=40,2,IF(N2+O2&gt;=33,1,0))))))</f>
+        <f>IF(AA2,0,IF((J2+K2+L2+M2)/2&gt;=80,5,IF((J2+K2+L2+M2)/2&gt;=70,4,IF((J2+K2+L2+M2)/2&gt;=60,3.5,IF((J2+K2+L2+M2)/2&gt;=50,3,IF((J2+K2+L2+M2)/2&gt;=40,2,IF((J2+K2+L2+M2)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ2">
-        <f>IF(P2+Q2&gt;=80,5,IF(P2+Q2&gt;=70,4,IF(P2+Q2&gt;=60,3.5,IF(P2+Q2&gt;=50,3,IF(P2+Q2&gt;=40,2,IF(P2+Q2&gt;=33,1,0))))))</f>
+        <f>IF(AB2,0,IF(N2+O2&gt;=80,5,IF(N2+O2&gt;=70,4,IF(N2+O2&gt;=60,3.5,IF(N2+O2&gt;=50,3,IF(N2+O2&gt;=40,2,IF(N2+O2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK2">
-        <f>IF(R2*2&gt;=80,5,IF(R2*2&gt;=70,4,IF(R2*2&gt;=60,3.5,IF(R2*2&gt;=50,3,IF(R2*2&gt;=40,2,IF(R2*2&gt;=33,1,0))))))</f>
+        <f>IF(AC2,0,IF(P2+Q2&gt;=80,5,IF(P2+Q2&gt;=70,4,IF(P2+Q2&gt;=60,3.5,IF(P2+Q2&gt;=50,3,IF(P2+Q2&gt;=40,2,IF(P2+Q2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL2">
-        <f>IF(S2&gt;=80,5,IF(S2&gt;=70,4,IF(S2&gt;=60,3.5,IF(S2&gt;=50,3,IF(S2&gt;=40,2,IF(S2&gt;=33,1,0))))))</f>
+        <f>IF(R2&lt;8.25,0,IF(R2*2&gt;=80,5,IF(R2*2&gt;=70,4,IF(R2*2&gt;=60,3.5,IF(R2*2&gt;=50,3,IF(R2*2&gt;=40,2,IF(R2*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM2">
-        <f>(AD2+AE2+AF2+AG2+AH2+AI2+AJ2+AK2)/8</f>
+        <f>IF(S2&lt;33,0,IF(S2&gt;=80,5,IF(S2&gt;=70,4,IF(S2&gt;=60,3.5,IF(S2&gt;=50,3,IF(S2&gt;=40,2,IF(S2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN2">
-        <f>IF(AL2&gt;=2,(AL2-2)/8,0)</f>
+        <f>(AE2+AF2+AG2+AH2+AI2+AJ2+AK2+AL2)/8</f>
+        <v/>
+      </c>
+      <c r="AO2">
+        <f>IF(AM2&gt;=2,(AM2-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1159,71 +1170,75 @@
         <v/>
       </c>
       <c r="X3" s="7">
-        <f>IF(AC3,0,MIN(5,ROUND(AM3+AN3,2)))</f>
-        <v/>
-      </c>
-      <c r="Y3" s="8">
-        <f>IF(X3&gt;=5,"A+",IF(X3&gt;=4,"A",IF(X3&gt;=3.5,"A-",IF(X3&gt;=3,"B",IF(X3&gt;=2,"C",IF(X3&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z3">
+        <f>IF(AD3,0,ROUND(AN3,2))</f>
+        <v/>
+      </c>
+      <c r="Y3" s="7">
+        <f>IF(AD3,0,MIN(5,ROUND(AN3+AO3,2)))</f>
+        <v/>
+      </c>
+      <c r="Z3" s="8">
+        <f>IF(Y3&gt;=5,"A+",IF(Y3&gt;=4,"A",IF(Y3&gt;=3.5,"A-",IF(Y3&gt;=3,"B",IF(Y3&gt;=2,"C",IF(Y3&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA3">
         <f>NOT(OR(AND(J3&gt;=10,K3&gt;=23,L3&gt;=10,M3&gt;=23),AND(J3+L3&gt;=20,K3+M3&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <f>OR(N3&lt;10,O3&lt;23)</f>
         <v/>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <f>OR(P3&lt;10,Q3&lt;23)</f>
         <v/>
       </c>
-      <c r="AC3">
-        <f>OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,Z3,AA3,AB3,R3&lt;8.25,T3&lt;33,U3&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD3">
-        <f>IF((C3+D3)/2&gt;=80,5,IF((C3+D3)/2&gt;=70,4,IF((C3+D3)/2&gt;=60,3.5,IF((C3+D3)/2&gt;=50,3,IF((C3+D3)/2&gt;=40,2,IF((C3+D3)/2&gt;=33,1,0))))))</f>
+        <f>OR((C3+D3)&lt;66,(E3+F3)&lt;66,G3&lt;33,(H3+I3)&lt;66,AA3,AB3,AC3,R3&lt;8.25,T3&lt;33,U3&lt;33)</f>
         <v/>
       </c>
       <c r="AE3">
-        <f>IF((E3+F3)/2&gt;=80,5,IF((E3+F3)/2&gt;=70,4,IF((E3+F3)/2&gt;=60,3.5,IF((E3+F3)/2&gt;=50,3,IF((E3+F3)/2&gt;=40,2,IF((E3+F3)/2&gt;=33,1,0))))))</f>
+        <f>IF(C3+D3&lt;66,0,IF((C3+D3)/2&gt;=80,5,IF((C3+D3)/2&gt;=70,4,IF((C3+D3)/2&gt;=60,3.5,IF((C3+D3)/2&gt;=50,3,IF((C3+D3)/2&gt;=40,2,IF((C3+D3)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF3">
-        <f>IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0))))))</f>
+        <f>IF(E3+F3&lt;66,0,IF((E3+F3)/2&gt;=80,5,IF((E3+F3)/2&gt;=70,4,IF((E3+F3)/2&gt;=60,3.5,IF((E3+F3)/2&gt;=50,3,IF((E3+F3)/2&gt;=40,2,IF((E3+F3)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG3">
-        <f>IF((H3+I3)/2&gt;=80,5,IF((H3+I3)/2&gt;=70,4,IF((H3+I3)/2&gt;=60,3.5,IF((H3+I3)/2&gt;=50,3,IF((H3+I3)/2&gt;=40,2,IF((H3+I3)/2&gt;=33,1,0))))))</f>
+        <f>IF(G3&lt;33,0,IF(G3&gt;=80,5,IF(G3&gt;=70,4,IF(G3&gt;=60,3.5,IF(G3&gt;=50,3,IF(G3&gt;=40,2,IF(G3&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH3">
-        <f>IF((J3+K3+L3+M3)/2&gt;=80,5,IF((J3+K3+L3+M3)/2&gt;=70,4,IF((J3+K3+L3+M3)/2&gt;=60,3.5,IF((J3+K3+L3+M3)/2&gt;=50,3,IF((J3+K3+L3+M3)/2&gt;=40,2,IF((J3+K3+L3+M3)/2&gt;=33,1,0))))))</f>
+        <f>IF(H3+I3&lt;66,0,IF((H3+I3)/2&gt;=80,5,IF((H3+I3)/2&gt;=70,4,IF((H3+I3)/2&gt;=60,3.5,IF((H3+I3)/2&gt;=50,3,IF((H3+I3)/2&gt;=40,2,IF((H3+I3)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI3">
-        <f>IF(N3+O3&gt;=80,5,IF(N3+O3&gt;=70,4,IF(N3+O3&gt;=60,3.5,IF(N3+O3&gt;=50,3,IF(N3+O3&gt;=40,2,IF(N3+O3&gt;=33,1,0))))))</f>
+        <f>IF(AA3,0,IF((J3+K3+L3+M3)/2&gt;=80,5,IF((J3+K3+L3+M3)/2&gt;=70,4,IF((J3+K3+L3+M3)/2&gt;=60,3.5,IF((J3+K3+L3+M3)/2&gt;=50,3,IF((J3+K3+L3+M3)/2&gt;=40,2,IF((J3+K3+L3+M3)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ3">
-        <f>IF(P3+Q3&gt;=80,5,IF(P3+Q3&gt;=70,4,IF(P3+Q3&gt;=60,3.5,IF(P3+Q3&gt;=50,3,IF(P3+Q3&gt;=40,2,IF(P3+Q3&gt;=33,1,0))))))</f>
+        <f>IF(AB3,0,IF(N3+O3&gt;=80,5,IF(N3+O3&gt;=70,4,IF(N3+O3&gt;=60,3.5,IF(N3+O3&gt;=50,3,IF(N3+O3&gt;=40,2,IF(N3+O3&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK3">
-        <f>IF(R3*2&gt;=80,5,IF(R3*2&gt;=70,4,IF(R3*2&gt;=60,3.5,IF(R3*2&gt;=50,3,IF(R3*2&gt;=40,2,IF(R3*2&gt;=33,1,0))))))</f>
+        <f>IF(AC3,0,IF(P3+Q3&gt;=80,5,IF(P3+Q3&gt;=70,4,IF(P3+Q3&gt;=60,3.5,IF(P3+Q3&gt;=50,3,IF(P3+Q3&gt;=40,2,IF(P3+Q3&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL3">
-        <f>IF(S3&gt;=80,5,IF(S3&gt;=70,4,IF(S3&gt;=60,3.5,IF(S3&gt;=50,3,IF(S3&gt;=40,2,IF(S3&gt;=33,1,0))))))</f>
+        <f>IF(R3&lt;8.25,0,IF(R3*2&gt;=80,5,IF(R3*2&gt;=70,4,IF(R3*2&gt;=60,3.5,IF(R3*2&gt;=50,3,IF(R3*2&gt;=40,2,IF(R3*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM3">
-        <f>(AD3+AE3+AF3+AG3+AH3+AI3+AJ3+AK3)/8</f>
+        <f>IF(S3&lt;33,0,IF(S3&gt;=80,5,IF(S3&gt;=70,4,IF(S3&gt;=60,3.5,IF(S3&gt;=50,3,IF(S3&gt;=40,2,IF(S3&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN3">
-        <f>IF(AL3&gt;=2,(AL3-2)/8,0)</f>
+        <f>(AE3+AF3+AG3+AH3+AI3+AJ3+AK3+AL3)/8</f>
+        <v/>
+      </c>
+      <c r="AO3">
+        <f>IF(AM3&gt;=2,(AM3-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1302,71 +1317,75 @@
         <v/>
       </c>
       <c r="X4" s="7">
-        <f>IF(AC4,0,MIN(5,ROUND(AM4+AN4,2)))</f>
-        <v/>
-      </c>
-      <c r="Y4" s="8">
-        <f>IF(X4&gt;=5,"A+",IF(X4&gt;=4,"A",IF(X4&gt;=3.5,"A-",IF(X4&gt;=3,"B",IF(X4&gt;=2,"C",IF(X4&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z4">
+        <f>IF(AD4,0,ROUND(AN4,2))</f>
+        <v/>
+      </c>
+      <c r="Y4" s="7">
+        <f>IF(AD4,0,MIN(5,ROUND(AN4+AO4,2)))</f>
+        <v/>
+      </c>
+      <c r="Z4" s="8">
+        <f>IF(Y4&gt;=5,"A+",IF(Y4&gt;=4,"A",IF(Y4&gt;=3.5,"A-",IF(Y4&gt;=3,"B",IF(Y4&gt;=2,"C",IF(Y4&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA4">
         <f>NOT(OR(AND(J4&gt;=10,K4&gt;=23,L4&gt;=10,M4&gt;=23),AND(J4+L4&gt;=20,K4+M4&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <f>OR(N4&lt;10,O4&lt;23)</f>
         <v/>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <f>OR(P4&lt;10,Q4&lt;23)</f>
         <v/>
       </c>
-      <c r="AC4">
-        <f>OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,Z4,AA4,AB4,R4&lt;8.25,T4&lt;33,U4&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD4">
-        <f>IF((C4+D4)/2&gt;=80,5,IF((C4+D4)/2&gt;=70,4,IF((C4+D4)/2&gt;=60,3.5,IF((C4+D4)/2&gt;=50,3,IF((C4+D4)/2&gt;=40,2,IF((C4+D4)/2&gt;=33,1,0))))))</f>
+        <f>OR((C4+D4)&lt;66,(E4+F4)&lt;66,G4&lt;33,(H4+I4)&lt;66,AA4,AB4,AC4,R4&lt;8.25,T4&lt;33,U4&lt;33)</f>
         <v/>
       </c>
       <c r="AE4">
-        <f>IF((E4+F4)/2&gt;=80,5,IF((E4+F4)/2&gt;=70,4,IF((E4+F4)/2&gt;=60,3.5,IF((E4+F4)/2&gt;=50,3,IF((E4+F4)/2&gt;=40,2,IF((E4+F4)/2&gt;=33,1,0))))))</f>
+        <f>IF(C4+D4&lt;66,0,IF((C4+D4)/2&gt;=80,5,IF((C4+D4)/2&gt;=70,4,IF((C4+D4)/2&gt;=60,3.5,IF((C4+D4)/2&gt;=50,3,IF((C4+D4)/2&gt;=40,2,IF((C4+D4)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF4">
-        <f>IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0))))))</f>
+        <f>IF(E4+F4&lt;66,0,IF((E4+F4)/2&gt;=80,5,IF((E4+F4)/2&gt;=70,4,IF((E4+F4)/2&gt;=60,3.5,IF((E4+F4)/2&gt;=50,3,IF((E4+F4)/2&gt;=40,2,IF((E4+F4)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG4">
-        <f>IF((H4+I4)/2&gt;=80,5,IF((H4+I4)/2&gt;=70,4,IF((H4+I4)/2&gt;=60,3.5,IF((H4+I4)/2&gt;=50,3,IF((H4+I4)/2&gt;=40,2,IF((H4+I4)/2&gt;=33,1,0))))))</f>
+        <f>IF(G4&lt;33,0,IF(G4&gt;=80,5,IF(G4&gt;=70,4,IF(G4&gt;=60,3.5,IF(G4&gt;=50,3,IF(G4&gt;=40,2,IF(G4&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH4">
-        <f>IF((J4+K4+L4+M4)/2&gt;=80,5,IF((J4+K4+L4+M4)/2&gt;=70,4,IF((J4+K4+L4+M4)/2&gt;=60,3.5,IF((J4+K4+L4+M4)/2&gt;=50,3,IF((J4+K4+L4+M4)/2&gt;=40,2,IF((J4+K4+L4+M4)/2&gt;=33,1,0))))))</f>
+        <f>IF(H4+I4&lt;66,0,IF((H4+I4)/2&gt;=80,5,IF((H4+I4)/2&gt;=70,4,IF((H4+I4)/2&gt;=60,3.5,IF((H4+I4)/2&gt;=50,3,IF((H4+I4)/2&gt;=40,2,IF((H4+I4)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI4">
-        <f>IF(N4+O4&gt;=80,5,IF(N4+O4&gt;=70,4,IF(N4+O4&gt;=60,3.5,IF(N4+O4&gt;=50,3,IF(N4+O4&gt;=40,2,IF(N4+O4&gt;=33,1,0))))))</f>
+        <f>IF(AA4,0,IF((J4+K4+L4+M4)/2&gt;=80,5,IF((J4+K4+L4+M4)/2&gt;=70,4,IF((J4+K4+L4+M4)/2&gt;=60,3.5,IF((J4+K4+L4+M4)/2&gt;=50,3,IF((J4+K4+L4+M4)/2&gt;=40,2,IF((J4+K4+L4+M4)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ4">
-        <f>IF(P4+Q4&gt;=80,5,IF(P4+Q4&gt;=70,4,IF(P4+Q4&gt;=60,3.5,IF(P4+Q4&gt;=50,3,IF(P4+Q4&gt;=40,2,IF(P4+Q4&gt;=33,1,0))))))</f>
+        <f>IF(AB4,0,IF(N4+O4&gt;=80,5,IF(N4+O4&gt;=70,4,IF(N4+O4&gt;=60,3.5,IF(N4+O4&gt;=50,3,IF(N4+O4&gt;=40,2,IF(N4+O4&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK4">
-        <f>IF(R4*2&gt;=80,5,IF(R4*2&gt;=70,4,IF(R4*2&gt;=60,3.5,IF(R4*2&gt;=50,3,IF(R4*2&gt;=40,2,IF(R4*2&gt;=33,1,0))))))</f>
+        <f>IF(AC4,0,IF(P4+Q4&gt;=80,5,IF(P4+Q4&gt;=70,4,IF(P4+Q4&gt;=60,3.5,IF(P4+Q4&gt;=50,3,IF(P4+Q4&gt;=40,2,IF(P4+Q4&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL4">
-        <f>IF(S4&gt;=80,5,IF(S4&gt;=70,4,IF(S4&gt;=60,3.5,IF(S4&gt;=50,3,IF(S4&gt;=40,2,IF(S4&gt;=33,1,0))))))</f>
+        <f>IF(R4&lt;8.25,0,IF(R4*2&gt;=80,5,IF(R4*2&gt;=70,4,IF(R4*2&gt;=60,3.5,IF(R4*2&gt;=50,3,IF(R4*2&gt;=40,2,IF(R4*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM4">
-        <f>(AD4+AE4+AF4+AG4+AH4+AI4+AJ4+AK4)/8</f>
+        <f>IF(S4&lt;33,0,IF(S4&gt;=80,5,IF(S4&gt;=70,4,IF(S4&gt;=60,3.5,IF(S4&gt;=50,3,IF(S4&gt;=40,2,IF(S4&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN4">
-        <f>IF(AL4&gt;=2,(AL4-2)/8,0)</f>
+        <f>(AE4+AF4+AG4+AH4+AI4+AJ4+AK4+AL4)/8</f>
+        <v/>
+      </c>
+      <c r="AO4">
+        <f>IF(AM4&gt;=2,(AM4-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1445,71 +1464,75 @@
         <v/>
       </c>
       <c r="X5" s="7">
-        <f>IF(AC5,0,MIN(5,ROUND(AM5+AN5,2)))</f>
-        <v/>
-      </c>
-      <c r="Y5" s="8">
-        <f>IF(X5&gt;=5,"A+",IF(X5&gt;=4,"A",IF(X5&gt;=3.5,"A-",IF(X5&gt;=3,"B",IF(X5&gt;=2,"C",IF(X5&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z5">
+        <f>IF(AD5,0,ROUND(AN5,2))</f>
+        <v/>
+      </c>
+      <c r="Y5" s="7">
+        <f>IF(AD5,0,MIN(5,ROUND(AN5+AO5,2)))</f>
+        <v/>
+      </c>
+      <c r="Z5" s="8">
+        <f>IF(Y5&gt;=5,"A+",IF(Y5&gt;=4,"A",IF(Y5&gt;=3.5,"A-",IF(Y5&gt;=3,"B",IF(Y5&gt;=2,"C",IF(Y5&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA5">
         <f>NOT(OR(AND(J5&gt;=10,K5&gt;=23,L5&gt;=10,M5&gt;=23),AND(J5+L5&gt;=20,K5+M5&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <f>OR(N5&lt;10,O5&lt;23)</f>
         <v/>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <f>OR(P5&lt;10,Q5&lt;23)</f>
         <v/>
       </c>
-      <c r="AC5">
-        <f>OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,Z5,AA5,AB5,R5&lt;8.25,T5&lt;33,U5&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD5">
-        <f>IF((C5+D5)/2&gt;=80,5,IF((C5+D5)/2&gt;=70,4,IF((C5+D5)/2&gt;=60,3.5,IF((C5+D5)/2&gt;=50,3,IF((C5+D5)/2&gt;=40,2,IF((C5+D5)/2&gt;=33,1,0))))))</f>
+        <f>OR((C5+D5)&lt;66,(E5+F5)&lt;66,G5&lt;33,(H5+I5)&lt;66,AA5,AB5,AC5,R5&lt;8.25,T5&lt;33,U5&lt;33)</f>
         <v/>
       </c>
       <c r="AE5">
-        <f>IF((E5+F5)/2&gt;=80,5,IF((E5+F5)/2&gt;=70,4,IF((E5+F5)/2&gt;=60,3.5,IF((E5+F5)/2&gt;=50,3,IF((E5+F5)/2&gt;=40,2,IF((E5+F5)/2&gt;=33,1,0))))))</f>
+        <f>IF(C5+D5&lt;66,0,IF((C5+D5)/2&gt;=80,5,IF((C5+D5)/2&gt;=70,4,IF((C5+D5)/2&gt;=60,3.5,IF((C5+D5)/2&gt;=50,3,IF((C5+D5)/2&gt;=40,2,IF((C5+D5)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF5">
-        <f>IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0))))))</f>
+        <f>IF(E5+F5&lt;66,0,IF((E5+F5)/2&gt;=80,5,IF((E5+F5)/2&gt;=70,4,IF((E5+F5)/2&gt;=60,3.5,IF((E5+F5)/2&gt;=50,3,IF((E5+F5)/2&gt;=40,2,IF((E5+F5)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG5">
-        <f>IF((H5+I5)/2&gt;=80,5,IF((H5+I5)/2&gt;=70,4,IF((H5+I5)/2&gt;=60,3.5,IF((H5+I5)/2&gt;=50,3,IF((H5+I5)/2&gt;=40,2,IF((H5+I5)/2&gt;=33,1,0))))))</f>
+        <f>IF(G5&lt;33,0,IF(G5&gt;=80,5,IF(G5&gt;=70,4,IF(G5&gt;=60,3.5,IF(G5&gt;=50,3,IF(G5&gt;=40,2,IF(G5&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH5">
-        <f>IF((J5+K5+L5+M5)/2&gt;=80,5,IF((J5+K5+L5+M5)/2&gt;=70,4,IF((J5+K5+L5+M5)/2&gt;=60,3.5,IF((J5+K5+L5+M5)/2&gt;=50,3,IF((J5+K5+L5+M5)/2&gt;=40,2,IF((J5+K5+L5+M5)/2&gt;=33,1,0))))))</f>
+        <f>IF(H5+I5&lt;66,0,IF((H5+I5)/2&gt;=80,5,IF((H5+I5)/2&gt;=70,4,IF((H5+I5)/2&gt;=60,3.5,IF((H5+I5)/2&gt;=50,3,IF((H5+I5)/2&gt;=40,2,IF((H5+I5)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI5">
-        <f>IF(N5+O5&gt;=80,5,IF(N5+O5&gt;=70,4,IF(N5+O5&gt;=60,3.5,IF(N5+O5&gt;=50,3,IF(N5+O5&gt;=40,2,IF(N5+O5&gt;=33,1,0))))))</f>
+        <f>IF(AA5,0,IF((J5+K5+L5+M5)/2&gt;=80,5,IF((J5+K5+L5+M5)/2&gt;=70,4,IF((J5+K5+L5+M5)/2&gt;=60,3.5,IF((J5+K5+L5+M5)/2&gt;=50,3,IF((J5+K5+L5+M5)/2&gt;=40,2,IF((J5+K5+L5+M5)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ5">
-        <f>IF(P5+Q5&gt;=80,5,IF(P5+Q5&gt;=70,4,IF(P5+Q5&gt;=60,3.5,IF(P5+Q5&gt;=50,3,IF(P5+Q5&gt;=40,2,IF(P5+Q5&gt;=33,1,0))))))</f>
+        <f>IF(AB5,0,IF(N5+O5&gt;=80,5,IF(N5+O5&gt;=70,4,IF(N5+O5&gt;=60,3.5,IF(N5+O5&gt;=50,3,IF(N5+O5&gt;=40,2,IF(N5+O5&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK5">
-        <f>IF(R5*2&gt;=80,5,IF(R5*2&gt;=70,4,IF(R5*2&gt;=60,3.5,IF(R5*2&gt;=50,3,IF(R5*2&gt;=40,2,IF(R5*2&gt;=33,1,0))))))</f>
+        <f>IF(AC5,0,IF(P5+Q5&gt;=80,5,IF(P5+Q5&gt;=70,4,IF(P5+Q5&gt;=60,3.5,IF(P5+Q5&gt;=50,3,IF(P5+Q5&gt;=40,2,IF(P5+Q5&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL5">
-        <f>IF(S5&gt;=80,5,IF(S5&gt;=70,4,IF(S5&gt;=60,3.5,IF(S5&gt;=50,3,IF(S5&gt;=40,2,IF(S5&gt;=33,1,0))))))</f>
+        <f>IF(R5&lt;8.25,0,IF(R5*2&gt;=80,5,IF(R5*2&gt;=70,4,IF(R5*2&gt;=60,3.5,IF(R5*2&gt;=50,3,IF(R5*2&gt;=40,2,IF(R5*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM5">
-        <f>(AD5+AE5+AF5+AG5+AH5+AI5+AJ5+AK5)/8</f>
+        <f>IF(S5&lt;33,0,IF(S5&gt;=80,5,IF(S5&gt;=70,4,IF(S5&gt;=60,3.5,IF(S5&gt;=50,3,IF(S5&gt;=40,2,IF(S5&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN5">
-        <f>IF(AL5&gt;=2,(AL5-2)/8,0)</f>
+        <f>(AE5+AF5+AG5+AH5+AI5+AJ5+AK5+AL5)/8</f>
+        <v/>
+      </c>
+      <c r="AO5">
+        <f>IF(AM5&gt;=2,(AM5-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1588,71 +1611,75 @@
         <v/>
       </c>
       <c r="X6" s="7">
-        <f>IF(AC6,0,MIN(5,ROUND(AM6+AN6,2)))</f>
-        <v/>
-      </c>
-      <c r="Y6" s="8">
-        <f>IF(X6&gt;=5,"A+",IF(X6&gt;=4,"A",IF(X6&gt;=3.5,"A-",IF(X6&gt;=3,"B",IF(X6&gt;=2,"C",IF(X6&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z6">
+        <f>IF(AD6,0,ROUND(AN6,2))</f>
+        <v/>
+      </c>
+      <c r="Y6" s="7">
+        <f>IF(AD6,0,MIN(5,ROUND(AN6+AO6,2)))</f>
+        <v/>
+      </c>
+      <c r="Z6" s="8">
+        <f>IF(Y6&gt;=5,"A+",IF(Y6&gt;=4,"A",IF(Y6&gt;=3.5,"A-",IF(Y6&gt;=3,"B",IF(Y6&gt;=2,"C",IF(Y6&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA6">
         <f>NOT(OR(AND(J6&gt;=10,K6&gt;=23,L6&gt;=10,M6&gt;=23),AND(J6+L6&gt;=20,K6+M6&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <f>OR(N6&lt;10,O6&lt;23)</f>
         <v/>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <f>OR(P6&lt;10,Q6&lt;23)</f>
         <v/>
       </c>
-      <c r="AC6">
-        <f>OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,Z6,AA6,AB6,R6&lt;8.25,T6&lt;33,U6&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD6">
-        <f>IF((C6+D6)/2&gt;=80,5,IF((C6+D6)/2&gt;=70,4,IF((C6+D6)/2&gt;=60,3.5,IF((C6+D6)/2&gt;=50,3,IF((C6+D6)/2&gt;=40,2,IF((C6+D6)/2&gt;=33,1,0))))))</f>
+        <f>OR((C6+D6)&lt;66,(E6+F6)&lt;66,G6&lt;33,(H6+I6)&lt;66,AA6,AB6,AC6,R6&lt;8.25,T6&lt;33,U6&lt;33)</f>
         <v/>
       </c>
       <c r="AE6">
-        <f>IF((E6+F6)/2&gt;=80,5,IF((E6+F6)/2&gt;=70,4,IF((E6+F6)/2&gt;=60,3.5,IF((E6+F6)/2&gt;=50,3,IF((E6+F6)/2&gt;=40,2,IF((E6+F6)/2&gt;=33,1,0))))))</f>
+        <f>IF(C6+D6&lt;66,0,IF((C6+D6)/2&gt;=80,5,IF((C6+D6)/2&gt;=70,4,IF((C6+D6)/2&gt;=60,3.5,IF((C6+D6)/2&gt;=50,3,IF((C6+D6)/2&gt;=40,2,IF((C6+D6)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF6">
-        <f>IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0))))))</f>
+        <f>IF(E6+F6&lt;66,0,IF((E6+F6)/2&gt;=80,5,IF((E6+F6)/2&gt;=70,4,IF((E6+F6)/2&gt;=60,3.5,IF((E6+F6)/2&gt;=50,3,IF((E6+F6)/2&gt;=40,2,IF((E6+F6)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG6">
-        <f>IF((H6+I6)/2&gt;=80,5,IF((H6+I6)/2&gt;=70,4,IF((H6+I6)/2&gt;=60,3.5,IF((H6+I6)/2&gt;=50,3,IF((H6+I6)/2&gt;=40,2,IF((H6+I6)/2&gt;=33,1,0))))))</f>
+        <f>IF(G6&lt;33,0,IF(G6&gt;=80,5,IF(G6&gt;=70,4,IF(G6&gt;=60,3.5,IF(G6&gt;=50,3,IF(G6&gt;=40,2,IF(G6&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH6">
-        <f>IF((J6+K6+L6+M6)/2&gt;=80,5,IF((J6+K6+L6+M6)/2&gt;=70,4,IF((J6+K6+L6+M6)/2&gt;=60,3.5,IF((J6+K6+L6+M6)/2&gt;=50,3,IF((J6+K6+L6+M6)/2&gt;=40,2,IF((J6+K6+L6+M6)/2&gt;=33,1,0))))))</f>
+        <f>IF(H6+I6&lt;66,0,IF((H6+I6)/2&gt;=80,5,IF((H6+I6)/2&gt;=70,4,IF((H6+I6)/2&gt;=60,3.5,IF((H6+I6)/2&gt;=50,3,IF((H6+I6)/2&gt;=40,2,IF((H6+I6)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI6">
-        <f>IF(N6+O6&gt;=80,5,IF(N6+O6&gt;=70,4,IF(N6+O6&gt;=60,3.5,IF(N6+O6&gt;=50,3,IF(N6+O6&gt;=40,2,IF(N6+O6&gt;=33,1,0))))))</f>
+        <f>IF(AA6,0,IF((J6+K6+L6+M6)/2&gt;=80,5,IF((J6+K6+L6+M6)/2&gt;=70,4,IF((J6+K6+L6+M6)/2&gt;=60,3.5,IF((J6+K6+L6+M6)/2&gt;=50,3,IF((J6+K6+L6+M6)/2&gt;=40,2,IF((J6+K6+L6+M6)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ6">
-        <f>IF(P6+Q6&gt;=80,5,IF(P6+Q6&gt;=70,4,IF(P6+Q6&gt;=60,3.5,IF(P6+Q6&gt;=50,3,IF(P6+Q6&gt;=40,2,IF(P6+Q6&gt;=33,1,0))))))</f>
+        <f>IF(AB6,0,IF(N6+O6&gt;=80,5,IF(N6+O6&gt;=70,4,IF(N6+O6&gt;=60,3.5,IF(N6+O6&gt;=50,3,IF(N6+O6&gt;=40,2,IF(N6+O6&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK6">
-        <f>IF(R6*2&gt;=80,5,IF(R6*2&gt;=70,4,IF(R6*2&gt;=60,3.5,IF(R6*2&gt;=50,3,IF(R6*2&gt;=40,2,IF(R6*2&gt;=33,1,0))))))</f>
+        <f>IF(AC6,0,IF(P6+Q6&gt;=80,5,IF(P6+Q6&gt;=70,4,IF(P6+Q6&gt;=60,3.5,IF(P6+Q6&gt;=50,3,IF(P6+Q6&gt;=40,2,IF(P6+Q6&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL6">
-        <f>IF(S6&gt;=80,5,IF(S6&gt;=70,4,IF(S6&gt;=60,3.5,IF(S6&gt;=50,3,IF(S6&gt;=40,2,IF(S6&gt;=33,1,0))))))</f>
+        <f>IF(R6&lt;8.25,0,IF(R6*2&gt;=80,5,IF(R6*2&gt;=70,4,IF(R6*2&gt;=60,3.5,IF(R6*2&gt;=50,3,IF(R6*2&gt;=40,2,IF(R6*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM6">
-        <f>(AD6+AE6+AF6+AG6+AH6+AI6+AJ6+AK6)/8</f>
+        <f>IF(S6&lt;33,0,IF(S6&gt;=80,5,IF(S6&gt;=70,4,IF(S6&gt;=60,3.5,IF(S6&gt;=50,3,IF(S6&gt;=40,2,IF(S6&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN6">
-        <f>IF(AL6&gt;=2,(AL6-2)/8,0)</f>
+        <f>(AE6+AF6+AG6+AH6+AI6+AJ6+AK6+AL6)/8</f>
+        <v/>
+      </c>
+      <c r="AO6">
+        <f>IF(AM6&gt;=2,(AM6-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1731,71 +1758,75 @@
         <v/>
       </c>
       <c r="X7" s="7">
-        <f>IF(AC7,0,MIN(5,ROUND(AM7+AN7,2)))</f>
-        <v/>
-      </c>
-      <c r="Y7" s="8">
-        <f>IF(X7&gt;=5,"A+",IF(X7&gt;=4,"A",IF(X7&gt;=3.5,"A-",IF(X7&gt;=3,"B",IF(X7&gt;=2,"C",IF(X7&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z7">
+        <f>IF(AD7,0,ROUND(AN7,2))</f>
+        <v/>
+      </c>
+      <c r="Y7" s="7">
+        <f>IF(AD7,0,MIN(5,ROUND(AN7+AO7,2)))</f>
+        <v/>
+      </c>
+      <c r="Z7" s="8">
+        <f>IF(Y7&gt;=5,"A+",IF(Y7&gt;=4,"A",IF(Y7&gt;=3.5,"A-",IF(Y7&gt;=3,"B",IF(Y7&gt;=2,"C",IF(Y7&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA7">
         <f>NOT(OR(AND(J7&gt;=10,K7&gt;=23,L7&gt;=10,M7&gt;=23),AND(J7+L7&gt;=20,K7+M7&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <f>OR(N7&lt;10,O7&lt;23)</f>
         <v/>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <f>OR(P7&lt;10,Q7&lt;23)</f>
         <v/>
       </c>
-      <c r="AC7">
-        <f>OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,Z7,AA7,AB7,R7&lt;8.25,T7&lt;33,U7&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD7">
-        <f>IF((C7+D7)/2&gt;=80,5,IF((C7+D7)/2&gt;=70,4,IF((C7+D7)/2&gt;=60,3.5,IF((C7+D7)/2&gt;=50,3,IF((C7+D7)/2&gt;=40,2,IF((C7+D7)/2&gt;=33,1,0))))))</f>
+        <f>OR((C7+D7)&lt;66,(E7+F7)&lt;66,G7&lt;33,(H7+I7)&lt;66,AA7,AB7,AC7,R7&lt;8.25,T7&lt;33,U7&lt;33)</f>
         <v/>
       </c>
       <c r="AE7">
-        <f>IF((E7+F7)/2&gt;=80,5,IF((E7+F7)/2&gt;=70,4,IF((E7+F7)/2&gt;=60,3.5,IF((E7+F7)/2&gt;=50,3,IF((E7+F7)/2&gt;=40,2,IF((E7+F7)/2&gt;=33,1,0))))))</f>
+        <f>IF(C7+D7&lt;66,0,IF((C7+D7)/2&gt;=80,5,IF((C7+D7)/2&gt;=70,4,IF((C7+D7)/2&gt;=60,3.5,IF((C7+D7)/2&gt;=50,3,IF((C7+D7)/2&gt;=40,2,IF((C7+D7)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF7">
-        <f>IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0))))))</f>
+        <f>IF(E7+F7&lt;66,0,IF((E7+F7)/2&gt;=80,5,IF((E7+F7)/2&gt;=70,4,IF((E7+F7)/2&gt;=60,3.5,IF((E7+F7)/2&gt;=50,3,IF((E7+F7)/2&gt;=40,2,IF((E7+F7)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG7">
-        <f>IF((H7+I7)/2&gt;=80,5,IF((H7+I7)/2&gt;=70,4,IF((H7+I7)/2&gt;=60,3.5,IF((H7+I7)/2&gt;=50,3,IF((H7+I7)/2&gt;=40,2,IF((H7+I7)/2&gt;=33,1,0))))))</f>
+        <f>IF(G7&lt;33,0,IF(G7&gt;=80,5,IF(G7&gt;=70,4,IF(G7&gt;=60,3.5,IF(G7&gt;=50,3,IF(G7&gt;=40,2,IF(G7&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH7">
-        <f>IF((J7+K7+L7+M7)/2&gt;=80,5,IF((J7+K7+L7+M7)/2&gt;=70,4,IF((J7+K7+L7+M7)/2&gt;=60,3.5,IF((J7+K7+L7+M7)/2&gt;=50,3,IF((J7+K7+L7+M7)/2&gt;=40,2,IF((J7+K7+L7+M7)/2&gt;=33,1,0))))))</f>
+        <f>IF(H7+I7&lt;66,0,IF((H7+I7)/2&gt;=80,5,IF((H7+I7)/2&gt;=70,4,IF((H7+I7)/2&gt;=60,3.5,IF((H7+I7)/2&gt;=50,3,IF((H7+I7)/2&gt;=40,2,IF((H7+I7)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI7">
-        <f>IF(N7+O7&gt;=80,5,IF(N7+O7&gt;=70,4,IF(N7+O7&gt;=60,3.5,IF(N7+O7&gt;=50,3,IF(N7+O7&gt;=40,2,IF(N7+O7&gt;=33,1,0))))))</f>
+        <f>IF(AA7,0,IF((J7+K7+L7+M7)/2&gt;=80,5,IF((J7+K7+L7+M7)/2&gt;=70,4,IF((J7+K7+L7+M7)/2&gt;=60,3.5,IF((J7+K7+L7+M7)/2&gt;=50,3,IF((J7+K7+L7+M7)/2&gt;=40,2,IF((J7+K7+L7+M7)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ7">
-        <f>IF(P7+Q7&gt;=80,5,IF(P7+Q7&gt;=70,4,IF(P7+Q7&gt;=60,3.5,IF(P7+Q7&gt;=50,3,IF(P7+Q7&gt;=40,2,IF(P7+Q7&gt;=33,1,0))))))</f>
+        <f>IF(AB7,0,IF(N7+O7&gt;=80,5,IF(N7+O7&gt;=70,4,IF(N7+O7&gt;=60,3.5,IF(N7+O7&gt;=50,3,IF(N7+O7&gt;=40,2,IF(N7+O7&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK7">
-        <f>IF(R7*2&gt;=80,5,IF(R7*2&gt;=70,4,IF(R7*2&gt;=60,3.5,IF(R7*2&gt;=50,3,IF(R7*2&gt;=40,2,IF(R7*2&gt;=33,1,0))))))</f>
+        <f>IF(AC7,0,IF(P7+Q7&gt;=80,5,IF(P7+Q7&gt;=70,4,IF(P7+Q7&gt;=60,3.5,IF(P7+Q7&gt;=50,3,IF(P7+Q7&gt;=40,2,IF(P7+Q7&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL7">
-        <f>IF(S7&gt;=80,5,IF(S7&gt;=70,4,IF(S7&gt;=60,3.5,IF(S7&gt;=50,3,IF(S7&gt;=40,2,IF(S7&gt;=33,1,0))))))</f>
+        <f>IF(R7&lt;8.25,0,IF(R7*2&gt;=80,5,IF(R7*2&gt;=70,4,IF(R7*2&gt;=60,3.5,IF(R7*2&gt;=50,3,IF(R7*2&gt;=40,2,IF(R7*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM7">
-        <f>(AD7+AE7+AF7+AG7+AH7+AI7+AJ7+AK7)/8</f>
+        <f>IF(S7&lt;33,0,IF(S7&gt;=80,5,IF(S7&gt;=70,4,IF(S7&gt;=60,3.5,IF(S7&gt;=50,3,IF(S7&gt;=40,2,IF(S7&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN7">
-        <f>IF(AL7&gt;=2,(AL7-2)/8,0)</f>
+        <f>(AE7+AF7+AG7+AH7+AI7+AJ7+AK7+AL7)/8</f>
+        <v/>
+      </c>
+      <c r="AO7">
+        <f>IF(AM7&gt;=2,(AM7-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -1874,71 +1905,75 @@
         <v/>
       </c>
       <c r="X8" s="7">
-        <f>IF(AC8,0,MIN(5,ROUND(AM8+AN8,2)))</f>
-        <v/>
-      </c>
-      <c r="Y8" s="8">
-        <f>IF(X8&gt;=5,"A+",IF(X8&gt;=4,"A",IF(X8&gt;=3.5,"A-",IF(X8&gt;=3,"B",IF(X8&gt;=2,"C",IF(X8&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z8">
+        <f>IF(AD8,0,ROUND(AN8,2))</f>
+        <v/>
+      </c>
+      <c r="Y8" s="7">
+        <f>IF(AD8,0,MIN(5,ROUND(AN8+AO8,2)))</f>
+        <v/>
+      </c>
+      <c r="Z8" s="8">
+        <f>IF(Y8&gt;=5,"A+",IF(Y8&gt;=4,"A",IF(Y8&gt;=3.5,"A-",IF(Y8&gt;=3,"B",IF(Y8&gt;=2,"C",IF(Y8&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA8">
         <f>NOT(OR(AND(J8&gt;=10,K8&gt;=23,L8&gt;=10,M8&gt;=23),AND(J8+L8&gt;=20,K8+M8&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <f>OR(N8&lt;10,O8&lt;23)</f>
         <v/>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <f>OR(P8&lt;10,Q8&lt;23)</f>
         <v/>
       </c>
-      <c r="AC8">
-        <f>OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,Z8,AA8,AB8,R8&lt;8.25,T8&lt;33,U8&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD8">
-        <f>IF((C8+D8)/2&gt;=80,5,IF((C8+D8)/2&gt;=70,4,IF((C8+D8)/2&gt;=60,3.5,IF((C8+D8)/2&gt;=50,3,IF((C8+D8)/2&gt;=40,2,IF((C8+D8)/2&gt;=33,1,0))))))</f>
+        <f>OR((C8+D8)&lt;66,(E8+F8)&lt;66,G8&lt;33,(H8+I8)&lt;66,AA8,AB8,AC8,R8&lt;8.25,T8&lt;33,U8&lt;33)</f>
         <v/>
       </c>
       <c r="AE8">
-        <f>IF((E8+F8)/2&gt;=80,5,IF((E8+F8)/2&gt;=70,4,IF((E8+F8)/2&gt;=60,3.5,IF((E8+F8)/2&gt;=50,3,IF((E8+F8)/2&gt;=40,2,IF((E8+F8)/2&gt;=33,1,0))))))</f>
+        <f>IF(C8+D8&lt;66,0,IF((C8+D8)/2&gt;=80,5,IF((C8+D8)/2&gt;=70,4,IF((C8+D8)/2&gt;=60,3.5,IF((C8+D8)/2&gt;=50,3,IF((C8+D8)/2&gt;=40,2,IF((C8+D8)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF8">
-        <f>IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0))))))</f>
+        <f>IF(E8+F8&lt;66,0,IF((E8+F8)/2&gt;=80,5,IF((E8+F8)/2&gt;=70,4,IF((E8+F8)/2&gt;=60,3.5,IF((E8+F8)/2&gt;=50,3,IF((E8+F8)/2&gt;=40,2,IF((E8+F8)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG8">
-        <f>IF((H8+I8)/2&gt;=80,5,IF((H8+I8)/2&gt;=70,4,IF((H8+I8)/2&gt;=60,3.5,IF((H8+I8)/2&gt;=50,3,IF((H8+I8)/2&gt;=40,2,IF((H8+I8)/2&gt;=33,1,0))))))</f>
+        <f>IF(G8&lt;33,0,IF(G8&gt;=80,5,IF(G8&gt;=70,4,IF(G8&gt;=60,3.5,IF(G8&gt;=50,3,IF(G8&gt;=40,2,IF(G8&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH8">
-        <f>IF((J8+K8+L8+M8)/2&gt;=80,5,IF((J8+K8+L8+M8)/2&gt;=70,4,IF((J8+K8+L8+M8)/2&gt;=60,3.5,IF((J8+K8+L8+M8)/2&gt;=50,3,IF((J8+K8+L8+M8)/2&gt;=40,2,IF((J8+K8+L8+M8)/2&gt;=33,1,0))))))</f>
+        <f>IF(H8+I8&lt;66,0,IF((H8+I8)/2&gt;=80,5,IF((H8+I8)/2&gt;=70,4,IF((H8+I8)/2&gt;=60,3.5,IF((H8+I8)/2&gt;=50,3,IF((H8+I8)/2&gt;=40,2,IF((H8+I8)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI8">
-        <f>IF(N8+O8&gt;=80,5,IF(N8+O8&gt;=70,4,IF(N8+O8&gt;=60,3.5,IF(N8+O8&gt;=50,3,IF(N8+O8&gt;=40,2,IF(N8+O8&gt;=33,1,0))))))</f>
+        <f>IF(AA8,0,IF((J8+K8+L8+M8)/2&gt;=80,5,IF((J8+K8+L8+M8)/2&gt;=70,4,IF((J8+K8+L8+M8)/2&gt;=60,3.5,IF((J8+K8+L8+M8)/2&gt;=50,3,IF((J8+K8+L8+M8)/2&gt;=40,2,IF((J8+K8+L8+M8)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ8">
-        <f>IF(P8+Q8&gt;=80,5,IF(P8+Q8&gt;=70,4,IF(P8+Q8&gt;=60,3.5,IF(P8+Q8&gt;=50,3,IF(P8+Q8&gt;=40,2,IF(P8+Q8&gt;=33,1,0))))))</f>
+        <f>IF(AB8,0,IF(N8+O8&gt;=80,5,IF(N8+O8&gt;=70,4,IF(N8+O8&gt;=60,3.5,IF(N8+O8&gt;=50,3,IF(N8+O8&gt;=40,2,IF(N8+O8&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK8">
-        <f>IF(R8*2&gt;=80,5,IF(R8*2&gt;=70,4,IF(R8*2&gt;=60,3.5,IF(R8*2&gt;=50,3,IF(R8*2&gt;=40,2,IF(R8*2&gt;=33,1,0))))))</f>
+        <f>IF(AC8,0,IF(P8+Q8&gt;=80,5,IF(P8+Q8&gt;=70,4,IF(P8+Q8&gt;=60,3.5,IF(P8+Q8&gt;=50,3,IF(P8+Q8&gt;=40,2,IF(P8+Q8&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL8">
-        <f>IF(S8&gt;=80,5,IF(S8&gt;=70,4,IF(S8&gt;=60,3.5,IF(S8&gt;=50,3,IF(S8&gt;=40,2,IF(S8&gt;=33,1,0))))))</f>
+        <f>IF(R8&lt;8.25,0,IF(R8*2&gt;=80,5,IF(R8*2&gt;=70,4,IF(R8*2&gt;=60,3.5,IF(R8*2&gt;=50,3,IF(R8*2&gt;=40,2,IF(R8*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM8">
-        <f>(AD8+AE8+AF8+AG8+AH8+AI8+AJ8+AK8)/8</f>
+        <f>IF(S8&lt;33,0,IF(S8&gt;=80,5,IF(S8&gt;=70,4,IF(S8&gt;=60,3.5,IF(S8&gt;=50,3,IF(S8&gt;=40,2,IF(S8&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN8">
-        <f>IF(AL8&gt;=2,(AL8-2)/8,0)</f>
+        <f>(AE8+AF8+AG8+AH8+AI8+AJ8+AK8+AL8)/8</f>
+        <v/>
+      </c>
+      <c r="AO8">
+        <f>IF(AM8&gt;=2,(AM8-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2017,71 +2052,75 @@
         <v/>
       </c>
       <c r="X9" s="7">
-        <f>IF(AC9,0,MIN(5,ROUND(AM9+AN9,2)))</f>
-        <v/>
-      </c>
-      <c r="Y9" s="8">
-        <f>IF(X9&gt;=5,"A+",IF(X9&gt;=4,"A",IF(X9&gt;=3.5,"A-",IF(X9&gt;=3,"B",IF(X9&gt;=2,"C",IF(X9&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z9">
+        <f>IF(AD9,0,ROUND(AN9,2))</f>
+        <v/>
+      </c>
+      <c r="Y9" s="7">
+        <f>IF(AD9,0,MIN(5,ROUND(AN9+AO9,2)))</f>
+        <v/>
+      </c>
+      <c r="Z9" s="8">
+        <f>IF(Y9&gt;=5,"A+",IF(Y9&gt;=4,"A",IF(Y9&gt;=3.5,"A-",IF(Y9&gt;=3,"B",IF(Y9&gt;=2,"C",IF(Y9&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA9">
         <f>NOT(OR(AND(J9&gt;=10,K9&gt;=23,L9&gt;=10,M9&gt;=23),AND(J9+L9&gt;=20,K9+M9&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <f>OR(N9&lt;10,O9&lt;23)</f>
         <v/>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <f>OR(P9&lt;10,Q9&lt;23)</f>
         <v/>
       </c>
-      <c r="AC9">
-        <f>OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,Z9,AA9,AB9,R9&lt;8.25,T9&lt;33,U9&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD9">
-        <f>IF((C9+D9)/2&gt;=80,5,IF((C9+D9)/2&gt;=70,4,IF((C9+D9)/2&gt;=60,3.5,IF((C9+D9)/2&gt;=50,3,IF((C9+D9)/2&gt;=40,2,IF((C9+D9)/2&gt;=33,1,0))))))</f>
+        <f>OR((C9+D9)&lt;66,(E9+F9)&lt;66,G9&lt;33,(H9+I9)&lt;66,AA9,AB9,AC9,R9&lt;8.25,T9&lt;33,U9&lt;33)</f>
         <v/>
       </c>
       <c r="AE9">
-        <f>IF((E9+F9)/2&gt;=80,5,IF((E9+F9)/2&gt;=70,4,IF((E9+F9)/2&gt;=60,3.5,IF((E9+F9)/2&gt;=50,3,IF((E9+F9)/2&gt;=40,2,IF((E9+F9)/2&gt;=33,1,0))))))</f>
+        <f>IF(C9+D9&lt;66,0,IF((C9+D9)/2&gt;=80,5,IF((C9+D9)/2&gt;=70,4,IF((C9+D9)/2&gt;=60,3.5,IF((C9+D9)/2&gt;=50,3,IF((C9+D9)/2&gt;=40,2,IF((C9+D9)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF9">
-        <f>IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0))))))</f>
+        <f>IF(E9+F9&lt;66,0,IF((E9+F9)/2&gt;=80,5,IF((E9+F9)/2&gt;=70,4,IF((E9+F9)/2&gt;=60,3.5,IF((E9+F9)/2&gt;=50,3,IF((E9+F9)/2&gt;=40,2,IF((E9+F9)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG9">
-        <f>IF((H9+I9)/2&gt;=80,5,IF((H9+I9)/2&gt;=70,4,IF((H9+I9)/2&gt;=60,3.5,IF((H9+I9)/2&gt;=50,3,IF((H9+I9)/2&gt;=40,2,IF((H9+I9)/2&gt;=33,1,0))))))</f>
+        <f>IF(G9&lt;33,0,IF(G9&gt;=80,5,IF(G9&gt;=70,4,IF(G9&gt;=60,3.5,IF(G9&gt;=50,3,IF(G9&gt;=40,2,IF(G9&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH9">
-        <f>IF((J9+K9+L9+M9)/2&gt;=80,5,IF((J9+K9+L9+M9)/2&gt;=70,4,IF((J9+K9+L9+M9)/2&gt;=60,3.5,IF((J9+K9+L9+M9)/2&gt;=50,3,IF((J9+K9+L9+M9)/2&gt;=40,2,IF((J9+K9+L9+M9)/2&gt;=33,1,0))))))</f>
+        <f>IF(H9+I9&lt;66,0,IF((H9+I9)/2&gt;=80,5,IF((H9+I9)/2&gt;=70,4,IF((H9+I9)/2&gt;=60,3.5,IF((H9+I9)/2&gt;=50,3,IF((H9+I9)/2&gt;=40,2,IF((H9+I9)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI9">
-        <f>IF(N9+O9&gt;=80,5,IF(N9+O9&gt;=70,4,IF(N9+O9&gt;=60,3.5,IF(N9+O9&gt;=50,3,IF(N9+O9&gt;=40,2,IF(N9+O9&gt;=33,1,0))))))</f>
+        <f>IF(AA9,0,IF((J9+K9+L9+M9)/2&gt;=80,5,IF((J9+K9+L9+M9)/2&gt;=70,4,IF((J9+K9+L9+M9)/2&gt;=60,3.5,IF((J9+K9+L9+M9)/2&gt;=50,3,IF((J9+K9+L9+M9)/2&gt;=40,2,IF((J9+K9+L9+M9)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ9">
-        <f>IF(P9+Q9&gt;=80,5,IF(P9+Q9&gt;=70,4,IF(P9+Q9&gt;=60,3.5,IF(P9+Q9&gt;=50,3,IF(P9+Q9&gt;=40,2,IF(P9+Q9&gt;=33,1,0))))))</f>
+        <f>IF(AB9,0,IF(N9+O9&gt;=80,5,IF(N9+O9&gt;=70,4,IF(N9+O9&gt;=60,3.5,IF(N9+O9&gt;=50,3,IF(N9+O9&gt;=40,2,IF(N9+O9&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK9">
-        <f>IF(R9*2&gt;=80,5,IF(R9*2&gt;=70,4,IF(R9*2&gt;=60,3.5,IF(R9*2&gt;=50,3,IF(R9*2&gt;=40,2,IF(R9*2&gt;=33,1,0))))))</f>
+        <f>IF(AC9,0,IF(P9+Q9&gt;=80,5,IF(P9+Q9&gt;=70,4,IF(P9+Q9&gt;=60,3.5,IF(P9+Q9&gt;=50,3,IF(P9+Q9&gt;=40,2,IF(P9+Q9&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL9">
-        <f>IF(S9&gt;=80,5,IF(S9&gt;=70,4,IF(S9&gt;=60,3.5,IF(S9&gt;=50,3,IF(S9&gt;=40,2,IF(S9&gt;=33,1,0))))))</f>
+        <f>IF(R9&lt;8.25,0,IF(R9*2&gt;=80,5,IF(R9*2&gt;=70,4,IF(R9*2&gt;=60,3.5,IF(R9*2&gt;=50,3,IF(R9*2&gt;=40,2,IF(R9*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM9">
-        <f>(AD9+AE9+AF9+AG9+AH9+AI9+AJ9+AK9)/8</f>
+        <f>IF(S9&lt;33,0,IF(S9&gt;=80,5,IF(S9&gt;=70,4,IF(S9&gt;=60,3.5,IF(S9&gt;=50,3,IF(S9&gt;=40,2,IF(S9&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN9">
-        <f>IF(AL9&gt;=2,(AL9-2)/8,0)</f>
+        <f>(AE9+AF9+AG9+AH9+AI9+AJ9+AK9+AL9)/8</f>
+        <v/>
+      </c>
+      <c r="AO9">
+        <f>IF(AM9&gt;=2,(AM9-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2160,71 +2199,75 @@
         <v/>
       </c>
       <c r="X10" s="7">
-        <f>IF(AC10,0,MIN(5,ROUND(AM10+AN10,2)))</f>
-        <v/>
-      </c>
-      <c r="Y10" s="8">
-        <f>IF(X10&gt;=5,"A+",IF(X10&gt;=4,"A",IF(X10&gt;=3.5,"A-",IF(X10&gt;=3,"B",IF(X10&gt;=2,"C",IF(X10&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z10">
+        <f>IF(AD10,0,ROUND(AN10,2))</f>
+        <v/>
+      </c>
+      <c r="Y10" s="7">
+        <f>IF(AD10,0,MIN(5,ROUND(AN10+AO10,2)))</f>
+        <v/>
+      </c>
+      <c r="Z10" s="8">
+        <f>IF(Y10&gt;=5,"A+",IF(Y10&gt;=4,"A",IF(Y10&gt;=3.5,"A-",IF(Y10&gt;=3,"B",IF(Y10&gt;=2,"C",IF(Y10&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA10">
         <f>NOT(OR(AND(J10&gt;=10,K10&gt;=23,L10&gt;=10,M10&gt;=23),AND(J10+L10&gt;=20,K10+M10&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <f>OR(N10&lt;10,O10&lt;23)</f>
         <v/>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <f>OR(P10&lt;10,Q10&lt;23)</f>
         <v/>
       </c>
-      <c r="AC10">
-        <f>OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,Z10,AA10,AB10,R10&lt;8.25,T10&lt;33,U10&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD10">
-        <f>IF((C10+D10)/2&gt;=80,5,IF((C10+D10)/2&gt;=70,4,IF((C10+D10)/2&gt;=60,3.5,IF((C10+D10)/2&gt;=50,3,IF((C10+D10)/2&gt;=40,2,IF((C10+D10)/2&gt;=33,1,0))))))</f>
+        <f>OR((C10+D10)&lt;66,(E10+F10)&lt;66,G10&lt;33,(H10+I10)&lt;66,AA10,AB10,AC10,R10&lt;8.25,T10&lt;33,U10&lt;33)</f>
         <v/>
       </c>
       <c r="AE10">
-        <f>IF((E10+F10)/2&gt;=80,5,IF((E10+F10)/2&gt;=70,4,IF((E10+F10)/2&gt;=60,3.5,IF((E10+F10)/2&gt;=50,3,IF((E10+F10)/2&gt;=40,2,IF((E10+F10)/2&gt;=33,1,0))))))</f>
+        <f>IF(C10+D10&lt;66,0,IF((C10+D10)/2&gt;=80,5,IF((C10+D10)/2&gt;=70,4,IF((C10+D10)/2&gt;=60,3.5,IF((C10+D10)/2&gt;=50,3,IF((C10+D10)/2&gt;=40,2,IF((C10+D10)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF10">
-        <f>IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0))))))</f>
+        <f>IF(E10+F10&lt;66,0,IF((E10+F10)/2&gt;=80,5,IF((E10+F10)/2&gt;=70,4,IF((E10+F10)/2&gt;=60,3.5,IF((E10+F10)/2&gt;=50,3,IF((E10+F10)/2&gt;=40,2,IF((E10+F10)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG10">
-        <f>IF((H10+I10)/2&gt;=80,5,IF((H10+I10)/2&gt;=70,4,IF((H10+I10)/2&gt;=60,3.5,IF((H10+I10)/2&gt;=50,3,IF((H10+I10)/2&gt;=40,2,IF((H10+I10)/2&gt;=33,1,0))))))</f>
+        <f>IF(G10&lt;33,0,IF(G10&gt;=80,5,IF(G10&gt;=70,4,IF(G10&gt;=60,3.5,IF(G10&gt;=50,3,IF(G10&gt;=40,2,IF(G10&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH10">
-        <f>IF((J10+K10+L10+M10)/2&gt;=80,5,IF((J10+K10+L10+M10)/2&gt;=70,4,IF((J10+K10+L10+M10)/2&gt;=60,3.5,IF((J10+K10+L10+M10)/2&gt;=50,3,IF((J10+K10+L10+M10)/2&gt;=40,2,IF((J10+K10+L10+M10)/2&gt;=33,1,0))))))</f>
+        <f>IF(H10+I10&lt;66,0,IF((H10+I10)/2&gt;=80,5,IF((H10+I10)/2&gt;=70,4,IF((H10+I10)/2&gt;=60,3.5,IF((H10+I10)/2&gt;=50,3,IF((H10+I10)/2&gt;=40,2,IF((H10+I10)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI10">
-        <f>IF(N10+O10&gt;=80,5,IF(N10+O10&gt;=70,4,IF(N10+O10&gt;=60,3.5,IF(N10+O10&gt;=50,3,IF(N10+O10&gt;=40,2,IF(N10+O10&gt;=33,1,0))))))</f>
+        <f>IF(AA10,0,IF((J10+K10+L10+M10)/2&gt;=80,5,IF((J10+K10+L10+M10)/2&gt;=70,4,IF((J10+K10+L10+M10)/2&gt;=60,3.5,IF((J10+K10+L10+M10)/2&gt;=50,3,IF((J10+K10+L10+M10)/2&gt;=40,2,IF((J10+K10+L10+M10)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ10">
-        <f>IF(P10+Q10&gt;=80,5,IF(P10+Q10&gt;=70,4,IF(P10+Q10&gt;=60,3.5,IF(P10+Q10&gt;=50,3,IF(P10+Q10&gt;=40,2,IF(P10+Q10&gt;=33,1,0))))))</f>
+        <f>IF(AB10,0,IF(N10+O10&gt;=80,5,IF(N10+O10&gt;=70,4,IF(N10+O10&gt;=60,3.5,IF(N10+O10&gt;=50,3,IF(N10+O10&gt;=40,2,IF(N10+O10&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK10">
-        <f>IF(R10*2&gt;=80,5,IF(R10*2&gt;=70,4,IF(R10*2&gt;=60,3.5,IF(R10*2&gt;=50,3,IF(R10*2&gt;=40,2,IF(R10*2&gt;=33,1,0))))))</f>
+        <f>IF(AC10,0,IF(P10+Q10&gt;=80,5,IF(P10+Q10&gt;=70,4,IF(P10+Q10&gt;=60,3.5,IF(P10+Q10&gt;=50,3,IF(P10+Q10&gt;=40,2,IF(P10+Q10&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL10">
-        <f>IF(S10&gt;=80,5,IF(S10&gt;=70,4,IF(S10&gt;=60,3.5,IF(S10&gt;=50,3,IF(S10&gt;=40,2,IF(S10&gt;=33,1,0))))))</f>
+        <f>IF(R10&lt;8.25,0,IF(R10*2&gt;=80,5,IF(R10*2&gt;=70,4,IF(R10*2&gt;=60,3.5,IF(R10*2&gt;=50,3,IF(R10*2&gt;=40,2,IF(R10*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM10">
-        <f>(AD10+AE10+AF10+AG10+AH10+AI10+AJ10+AK10)/8</f>
+        <f>IF(S10&lt;33,0,IF(S10&gt;=80,5,IF(S10&gt;=70,4,IF(S10&gt;=60,3.5,IF(S10&gt;=50,3,IF(S10&gt;=40,2,IF(S10&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN10">
-        <f>IF(AL10&gt;=2,(AL10-2)/8,0)</f>
+        <f>(AE10+AF10+AG10+AH10+AI10+AJ10+AK10+AL10)/8</f>
+        <v/>
+      </c>
+      <c r="AO10">
+        <f>IF(AM10&gt;=2,(AM10-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2303,71 +2346,75 @@
         <v/>
       </c>
       <c r="X11" s="7">
-        <f>IF(AC11,0,MIN(5,ROUND(AM11+AN11,2)))</f>
-        <v/>
-      </c>
-      <c r="Y11" s="8">
-        <f>IF(X11&gt;=5,"A+",IF(X11&gt;=4,"A",IF(X11&gt;=3.5,"A-",IF(X11&gt;=3,"B",IF(X11&gt;=2,"C",IF(X11&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z11">
+        <f>IF(AD11,0,ROUND(AN11,2))</f>
+        <v/>
+      </c>
+      <c r="Y11" s="7">
+        <f>IF(AD11,0,MIN(5,ROUND(AN11+AO11,2)))</f>
+        <v/>
+      </c>
+      <c r="Z11" s="8">
+        <f>IF(Y11&gt;=5,"A+",IF(Y11&gt;=4,"A",IF(Y11&gt;=3.5,"A-",IF(Y11&gt;=3,"B",IF(Y11&gt;=2,"C",IF(Y11&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA11">
         <f>NOT(OR(AND(J11&gt;=10,K11&gt;=23,L11&gt;=10,M11&gt;=23),AND(J11+L11&gt;=20,K11+M11&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <f>OR(N11&lt;10,O11&lt;23)</f>
         <v/>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <f>OR(P11&lt;10,Q11&lt;23)</f>
         <v/>
       </c>
-      <c r="AC11">
-        <f>OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,Z11,AA11,AB11,R11&lt;8.25,T11&lt;33,U11&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD11">
-        <f>IF((C11+D11)/2&gt;=80,5,IF((C11+D11)/2&gt;=70,4,IF((C11+D11)/2&gt;=60,3.5,IF((C11+D11)/2&gt;=50,3,IF((C11+D11)/2&gt;=40,2,IF((C11+D11)/2&gt;=33,1,0))))))</f>
+        <f>OR((C11+D11)&lt;66,(E11+F11)&lt;66,G11&lt;33,(H11+I11)&lt;66,AA11,AB11,AC11,R11&lt;8.25,T11&lt;33,U11&lt;33)</f>
         <v/>
       </c>
       <c r="AE11">
-        <f>IF((E11+F11)/2&gt;=80,5,IF((E11+F11)/2&gt;=70,4,IF((E11+F11)/2&gt;=60,3.5,IF((E11+F11)/2&gt;=50,3,IF((E11+F11)/2&gt;=40,2,IF((E11+F11)/2&gt;=33,1,0))))))</f>
+        <f>IF(C11+D11&lt;66,0,IF((C11+D11)/2&gt;=80,5,IF((C11+D11)/2&gt;=70,4,IF((C11+D11)/2&gt;=60,3.5,IF((C11+D11)/2&gt;=50,3,IF((C11+D11)/2&gt;=40,2,IF((C11+D11)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF11">
-        <f>IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0))))))</f>
+        <f>IF(E11+F11&lt;66,0,IF((E11+F11)/2&gt;=80,5,IF((E11+F11)/2&gt;=70,4,IF((E11+F11)/2&gt;=60,3.5,IF((E11+F11)/2&gt;=50,3,IF((E11+F11)/2&gt;=40,2,IF((E11+F11)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG11">
-        <f>IF((H11+I11)/2&gt;=80,5,IF((H11+I11)/2&gt;=70,4,IF((H11+I11)/2&gt;=60,3.5,IF((H11+I11)/2&gt;=50,3,IF((H11+I11)/2&gt;=40,2,IF((H11+I11)/2&gt;=33,1,0))))))</f>
+        <f>IF(G11&lt;33,0,IF(G11&gt;=80,5,IF(G11&gt;=70,4,IF(G11&gt;=60,3.5,IF(G11&gt;=50,3,IF(G11&gt;=40,2,IF(G11&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH11">
-        <f>IF((J11+K11+L11+M11)/2&gt;=80,5,IF((J11+K11+L11+M11)/2&gt;=70,4,IF((J11+K11+L11+M11)/2&gt;=60,3.5,IF((J11+K11+L11+M11)/2&gt;=50,3,IF((J11+K11+L11+M11)/2&gt;=40,2,IF((J11+K11+L11+M11)/2&gt;=33,1,0))))))</f>
+        <f>IF(H11+I11&lt;66,0,IF((H11+I11)/2&gt;=80,5,IF((H11+I11)/2&gt;=70,4,IF((H11+I11)/2&gt;=60,3.5,IF((H11+I11)/2&gt;=50,3,IF((H11+I11)/2&gt;=40,2,IF((H11+I11)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI11">
-        <f>IF(N11+O11&gt;=80,5,IF(N11+O11&gt;=70,4,IF(N11+O11&gt;=60,3.5,IF(N11+O11&gt;=50,3,IF(N11+O11&gt;=40,2,IF(N11+O11&gt;=33,1,0))))))</f>
+        <f>IF(AA11,0,IF((J11+K11+L11+M11)/2&gt;=80,5,IF((J11+K11+L11+M11)/2&gt;=70,4,IF((J11+K11+L11+M11)/2&gt;=60,3.5,IF((J11+K11+L11+M11)/2&gt;=50,3,IF((J11+K11+L11+M11)/2&gt;=40,2,IF((J11+K11+L11+M11)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ11">
-        <f>IF(P11+Q11&gt;=80,5,IF(P11+Q11&gt;=70,4,IF(P11+Q11&gt;=60,3.5,IF(P11+Q11&gt;=50,3,IF(P11+Q11&gt;=40,2,IF(P11+Q11&gt;=33,1,0))))))</f>
+        <f>IF(AB11,0,IF(N11+O11&gt;=80,5,IF(N11+O11&gt;=70,4,IF(N11+O11&gt;=60,3.5,IF(N11+O11&gt;=50,3,IF(N11+O11&gt;=40,2,IF(N11+O11&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK11">
-        <f>IF(R11*2&gt;=80,5,IF(R11*2&gt;=70,4,IF(R11*2&gt;=60,3.5,IF(R11*2&gt;=50,3,IF(R11*2&gt;=40,2,IF(R11*2&gt;=33,1,0))))))</f>
+        <f>IF(AC11,0,IF(P11+Q11&gt;=80,5,IF(P11+Q11&gt;=70,4,IF(P11+Q11&gt;=60,3.5,IF(P11+Q11&gt;=50,3,IF(P11+Q11&gt;=40,2,IF(P11+Q11&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL11">
-        <f>IF(S11&gt;=80,5,IF(S11&gt;=70,4,IF(S11&gt;=60,3.5,IF(S11&gt;=50,3,IF(S11&gt;=40,2,IF(S11&gt;=33,1,0))))))</f>
+        <f>IF(R11&lt;8.25,0,IF(R11*2&gt;=80,5,IF(R11*2&gt;=70,4,IF(R11*2&gt;=60,3.5,IF(R11*2&gt;=50,3,IF(R11*2&gt;=40,2,IF(R11*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM11">
-        <f>(AD11+AE11+AF11+AG11+AH11+AI11+AJ11+AK11)/8</f>
+        <f>IF(S11&lt;33,0,IF(S11&gt;=80,5,IF(S11&gt;=70,4,IF(S11&gt;=60,3.5,IF(S11&gt;=50,3,IF(S11&gt;=40,2,IF(S11&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN11">
-        <f>IF(AL11&gt;=2,(AL11-2)/8,0)</f>
+        <f>(AE11+AF11+AG11+AH11+AI11+AJ11+AK11+AL11)/8</f>
+        <v/>
+      </c>
+      <c r="AO11">
+        <f>IF(AM11&gt;=2,(AM11-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2446,71 +2493,75 @@
         <v/>
       </c>
       <c r="X12" s="7">
-        <f>IF(AC12,0,MIN(5,ROUND(AM12+AN12,2)))</f>
-        <v/>
-      </c>
-      <c r="Y12" s="8">
-        <f>IF(X12&gt;=5,"A+",IF(X12&gt;=4,"A",IF(X12&gt;=3.5,"A-",IF(X12&gt;=3,"B",IF(X12&gt;=2,"C",IF(X12&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z12">
+        <f>IF(AD12,0,ROUND(AN12,2))</f>
+        <v/>
+      </c>
+      <c r="Y12" s="7">
+        <f>IF(AD12,0,MIN(5,ROUND(AN12+AO12,2)))</f>
+        <v/>
+      </c>
+      <c r="Z12" s="8">
+        <f>IF(Y12&gt;=5,"A+",IF(Y12&gt;=4,"A",IF(Y12&gt;=3.5,"A-",IF(Y12&gt;=3,"B",IF(Y12&gt;=2,"C",IF(Y12&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA12">
         <f>NOT(OR(AND(J12&gt;=10,K12&gt;=23,L12&gt;=10,M12&gt;=23),AND(J12+L12&gt;=20,K12+M12&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <f>OR(N12&lt;10,O12&lt;23)</f>
         <v/>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <f>OR(P12&lt;10,Q12&lt;23)</f>
         <v/>
       </c>
-      <c r="AC12">
-        <f>OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,Z12,AA12,AB12,R12&lt;8.25,T12&lt;33,U12&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD12">
-        <f>IF((C12+D12)/2&gt;=80,5,IF((C12+D12)/2&gt;=70,4,IF((C12+D12)/2&gt;=60,3.5,IF((C12+D12)/2&gt;=50,3,IF((C12+D12)/2&gt;=40,2,IF((C12+D12)/2&gt;=33,1,0))))))</f>
+        <f>OR((C12+D12)&lt;66,(E12+F12)&lt;66,G12&lt;33,(H12+I12)&lt;66,AA12,AB12,AC12,R12&lt;8.25,T12&lt;33,U12&lt;33)</f>
         <v/>
       </c>
       <c r="AE12">
-        <f>IF((E12+F12)/2&gt;=80,5,IF((E12+F12)/2&gt;=70,4,IF((E12+F12)/2&gt;=60,3.5,IF((E12+F12)/2&gt;=50,3,IF((E12+F12)/2&gt;=40,2,IF((E12+F12)/2&gt;=33,1,0))))))</f>
+        <f>IF(C12+D12&lt;66,0,IF((C12+D12)/2&gt;=80,5,IF((C12+D12)/2&gt;=70,4,IF((C12+D12)/2&gt;=60,3.5,IF((C12+D12)/2&gt;=50,3,IF((C12+D12)/2&gt;=40,2,IF((C12+D12)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF12">
-        <f>IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0))))))</f>
+        <f>IF(E12+F12&lt;66,0,IF((E12+F12)/2&gt;=80,5,IF((E12+F12)/2&gt;=70,4,IF((E12+F12)/2&gt;=60,3.5,IF((E12+F12)/2&gt;=50,3,IF((E12+F12)/2&gt;=40,2,IF((E12+F12)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG12">
-        <f>IF((H12+I12)/2&gt;=80,5,IF((H12+I12)/2&gt;=70,4,IF((H12+I12)/2&gt;=60,3.5,IF((H12+I12)/2&gt;=50,3,IF((H12+I12)/2&gt;=40,2,IF((H12+I12)/2&gt;=33,1,0))))))</f>
+        <f>IF(G12&lt;33,0,IF(G12&gt;=80,5,IF(G12&gt;=70,4,IF(G12&gt;=60,3.5,IF(G12&gt;=50,3,IF(G12&gt;=40,2,IF(G12&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH12">
-        <f>IF((J12+K12+L12+M12)/2&gt;=80,5,IF((J12+K12+L12+M12)/2&gt;=70,4,IF((J12+K12+L12+M12)/2&gt;=60,3.5,IF((J12+K12+L12+M12)/2&gt;=50,3,IF((J12+K12+L12+M12)/2&gt;=40,2,IF((J12+K12+L12+M12)/2&gt;=33,1,0))))))</f>
+        <f>IF(H12+I12&lt;66,0,IF((H12+I12)/2&gt;=80,5,IF((H12+I12)/2&gt;=70,4,IF((H12+I12)/2&gt;=60,3.5,IF((H12+I12)/2&gt;=50,3,IF((H12+I12)/2&gt;=40,2,IF((H12+I12)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI12">
-        <f>IF(N12+O12&gt;=80,5,IF(N12+O12&gt;=70,4,IF(N12+O12&gt;=60,3.5,IF(N12+O12&gt;=50,3,IF(N12+O12&gt;=40,2,IF(N12+O12&gt;=33,1,0))))))</f>
+        <f>IF(AA12,0,IF((J12+K12+L12+M12)/2&gt;=80,5,IF((J12+K12+L12+M12)/2&gt;=70,4,IF((J12+K12+L12+M12)/2&gt;=60,3.5,IF((J12+K12+L12+M12)/2&gt;=50,3,IF((J12+K12+L12+M12)/2&gt;=40,2,IF((J12+K12+L12+M12)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ12">
-        <f>IF(P12+Q12&gt;=80,5,IF(P12+Q12&gt;=70,4,IF(P12+Q12&gt;=60,3.5,IF(P12+Q12&gt;=50,3,IF(P12+Q12&gt;=40,2,IF(P12+Q12&gt;=33,1,0))))))</f>
+        <f>IF(AB12,0,IF(N12+O12&gt;=80,5,IF(N12+O12&gt;=70,4,IF(N12+O12&gt;=60,3.5,IF(N12+O12&gt;=50,3,IF(N12+O12&gt;=40,2,IF(N12+O12&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK12">
-        <f>IF(R12*2&gt;=80,5,IF(R12*2&gt;=70,4,IF(R12*2&gt;=60,3.5,IF(R12*2&gt;=50,3,IF(R12*2&gt;=40,2,IF(R12*2&gt;=33,1,0))))))</f>
+        <f>IF(AC12,0,IF(P12+Q12&gt;=80,5,IF(P12+Q12&gt;=70,4,IF(P12+Q12&gt;=60,3.5,IF(P12+Q12&gt;=50,3,IF(P12+Q12&gt;=40,2,IF(P12+Q12&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL12">
-        <f>IF(S12&gt;=80,5,IF(S12&gt;=70,4,IF(S12&gt;=60,3.5,IF(S12&gt;=50,3,IF(S12&gt;=40,2,IF(S12&gt;=33,1,0))))))</f>
+        <f>IF(R12&lt;8.25,0,IF(R12*2&gt;=80,5,IF(R12*2&gt;=70,4,IF(R12*2&gt;=60,3.5,IF(R12*2&gt;=50,3,IF(R12*2&gt;=40,2,IF(R12*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM12">
-        <f>(AD12+AE12+AF12+AG12+AH12+AI12+AJ12+AK12)/8</f>
+        <f>IF(S12&lt;33,0,IF(S12&gt;=80,5,IF(S12&gt;=70,4,IF(S12&gt;=60,3.5,IF(S12&gt;=50,3,IF(S12&gt;=40,2,IF(S12&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN12">
-        <f>IF(AL12&gt;=2,(AL12-2)/8,0)</f>
+        <f>(AE12+AF12+AG12+AH12+AI12+AJ12+AK12+AL12)/8</f>
+        <v/>
+      </c>
+      <c r="AO12">
+        <f>IF(AM12&gt;=2,(AM12-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2589,71 +2640,75 @@
         <v/>
       </c>
       <c r="X13" s="7">
-        <f>IF(AC13,0,MIN(5,ROUND(AM13+AN13,2)))</f>
-        <v/>
-      </c>
-      <c r="Y13" s="8">
-        <f>IF(X13&gt;=5,"A+",IF(X13&gt;=4,"A",IF(X13&gt;=3.5,"A-",IF(X13&gt;=3,"B",IF(X13&gt;=2,"C",IF(X13&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z13">
+        <f>IF(AD13,0,ROUND(AN13,2))</f>
+        <v/>
+      </c>
+      <c r="Y13" s="7">
+        <f>IF(AD13,0,MIN(5,ROUND(AN13+AO13,2)))</f>
+        <v/>
+      </c>
+      <c r="Z13" s="8">
+        <f>IF(Y13&gt;=5,"A+",IF(Y13&gt;=4,"A",IF(Y13&gt;=3.5,"A-",IF(Y13&gt;=3,"B",IF(Y13&gt;=2,"C",IF(Y13&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA13">
         <f>NOT(OR(AND(J13&gt;=10,K13&gt;=23,L13&gt;=10,M13&gt;=23),AND(J13+L13&gt;=20,K13+M13&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <f>OR(N13&lt;10,O13&lt;23)</f>
         <v/>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <f>OR(P13&lt;10,Q13&lt;23)</f>
         <v/>
       </c>
-      <c r="AC13">
-        <f>OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,Z13,AA13,AB13,R13&lt;8.25,T13&lt;33,U13&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD13">
-        <f>IF((C13+D13)/2&gt;=80,5,IF((C13+D13)/2&gt;=70,4,IF((C13+D13)/2&gt;=60,3.5,IF((C13+D13)/2&gt;=50,3,IF((C13+D13)/2&gt;=40,2,IF((C13+D13)/2&gt;=33,1,0))))))</f>
+        <f>OR((C13+D13)&lt;66,(E13+F13)&lt;66,G13&lt;33,(H13+I13)&lt;66,AA13,AB13,AC13,R13&lt;8.25,T13&lt;33,U13&lt;33)</f>
         <v/>
       </c>
       <c r="AE13">
-        <f>IF((E13+F13)/2&gt;=80,5,IF((E13+F13)/2&gt;=70,4,IF((E13+F13)/2&gt;=60,3.5,IF((E13+F13)/2&gt;=50,3,IF((E13+F13)/2&gt;=40,2,IF((E13+F13)/2&gt;=33,1,0))))))</f>
+        <f>IF(C13+D13&lt;66,0,IF((C13+D13)/2&gt;=80,5,IF((C13+D13)/2&gt;=70,4,IF((C13+D13)/2&gt;=60,3.5,IF((C13+D13)/2&gt;=50,3,IF((C13+D13)/2&gt;=40,2,IF((C13+D13)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF13">
-        <f>IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0))))))</f>
+        <f>IF(E13+F13&lt;66,0,IF((E13+F13)/2&gt;=80,5,IF((E13+F13)/2&gt;=70,4,IF((E13+F13)/2&gt;=60,3.5,IF((E13+F13)/2&gt;=50,3,IF((E13+F13)/2&gt;=40,2,IF((E13+F13)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG13">
-        <f>IF((H13+I13)/2&gt;=80,5,IF((H13+I13)/2&gt;=70,4,IF((H13+I13)/2&gt;=60,3.5,IF((H13+I13)/2&gt;=50,3,IF((H13+I13)/2&gt;=40,2,IF((H13+I13)/2&gt;=33,1,0))))))</f>
+        <f>IF(G13&lt;33,0,IF(G13&gt;=80,5,IF(G13&gt;=70,4,IF(G13&gt;=60,3.5,IF(G13&gt;=50,3,IF(G13&gt;=40,2,IF(G13&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH13">
-        <f>IF((J13+K13+L13+M13)/2&gt;=80,5,IF((J13+K13+L13+M13)/2&gt;=70,4,IF((J13+K13+L13+M13)/2&gt;=60,3.5,IF((J13+K13+L13+M13)/2&gt;=50,3,IF((J13+K13+L13+M13)/2&gt;=40,2,IF((J13+K13+L13+M13)/2&gt;=33,1,0))))))</f>
+        <f>IF(H13+I13&lt;66,0,IF((H13+I13)/2&gt;=80,5,IF((H13+I13)/2&gt;=70,4,IF((H13+I13)/2&gt;=60,3.5,IF((H13+I13)/2&gt;=50,3,IF((H13+I13)/2&gt;=40,2,IF((H13+I13)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI13">
-        <f>IF(N13+O13&gt;=80,5,IF(N13+O13&gt;=70,4,IF(N13+O13&gt;=60,3.5,IF(N13+O13&gt;=50,3,IF(N13+O13&gt;=40,2,IF(N13+O13&gt;=33,1,0))))))</f>
+        <f>IF(AA13,0,IF((J13+K13+L13+M13)/2&gt;=80,5,IF((J13+K13+L13+M13)/2&gt;=70,4,IF((J13+K13+L13+M13)/2&gt;=60,3.5,IF((J13+K13+L13+M13)/2&gt;=50,3,IF((J13+K13+L13+M13)/2&gt;=40,2,IF((J13+K13+L13+M13)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ13">
-        <f>IF(P13+Q13&gt;=80,5,IF(P13+Q13&gt;=70,4,IF(P13+Q13&gt;=60,3.5,IF(P13+Q13&gt;=50,3,IF(P13+Q13&gt;=40,2,IF(P13+Q13&gt;=33,1,0))))))</f>
+        <f>IF(AB13,0,IF(N13+O13&gt;=80,5,IF(N13+O13&gt;=70,4,IF(N13+O13&gt;=60,3.5,IF(N13+O13&gt;=50,3,IF(N13+O13&gt;=40,2,IF(N13+O13&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK13">
-        <f>IF(R13*2&gt;=80,5,IF(R13*2&gt;=70,4,IF(R13*2&gt;=60,3.5,IF(R13*2&gt;=50,3,IF(R13*2&gt;=40,2,IF(R13*2&gt;=33,1,0))))))</f>
+        <f>IF(AC13,0,IF(P13+Q13&gt;=80,5,IF(P13+Q13&gt;=70,4,IF(P13+Q13&gt;=60,3.5,IF(P13+Q13&gt;=50,3,IF(P13+Q13&gt;=40,2,IF(P13+Q13&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL13">
-        <f>IF(S13&gt;=80,5,IF(S13&gt;=70,4,IF(S13&gt;=60,3.5,IF(S13&gt;=50,3,IF(S13&gt;=40,2,IF(S13&gt;=33,1,0))))))</f>
+        <f>IF(R13&lt;8.25,0,IF(R13*2&gt;=80,5,IF(R13*2&gt;=70,4,IF(R13*2&gt;=60,3.5,IF(R13*2&gt;=50,3,IF(R13*2&gt;=40,2,IF(R13*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM13">
-        <f>(AD13+AE13+AF13+AG13+AH13+AI13+AJ13+AK13)/8</f>
+        <f>IF(S13&lt;33,0,IF(S13&gt;=80,5,IF(S13&gt;=70,4,IF(S13&gt;=60,3.5,IF(S13&gt;=50,3,IF(S13&gt;=40,2,IF(S13&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN13">
-        <f>IF(AL13&gt;=2,(AL13-2)/8,0)</f>
+        <f>(AE13+AF13+AG13+AH13+AI13+AJ13+AK13+AL13)/8</f>
+        <v/>
+      </c>
+      <c r="AO13">
+        <f>IF(AM13&gt;=2,(AM13-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2732,71 +2787,75 @@
         <v/>
       </c>
       <c r="X14" s="7">
-        <f>IF(AC14,0,MIN(5,ROUND(AM14+AN14,2)))</f>
-        <v/>
-      </c>
-      <c r="Y14" s="8">
-        <f>IF(X14&gt;=5,"A+",IF(X14&gt;=4,"A",IF(X14&gt;=3.5,"A-",IF(X14&gt;=3,"B",IF(X14&gt;=2,"C",IF(X14&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z14">
+        <f>IF(AD14,0,ROUND(AN14,2))</f>
+        <v/>
+      </c>
+      <c r="Y14" s="7">
+        <f>IF(AD14,0,MIN(5,ROUND(AN14+AO14,2)))</f>
+        <v/>
+      </c>
+      <c r="Z14" s="8">
+        <f>IF(Y14&gt;=5,"A+",IF(Y14&gt;=4,"A",IF(Y14&gt;=3.5,"A-",IF(Y14&gt;=3,"B",IF(Y14&gt;=2,"C",IF(Y14&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA14">
         <f>NOT(OR(AND(J14&gt;=10,K14&gt;=23,L14&gt;=10,M14&gt;=23),AND(J14+L14&gt;=20,K14+M14&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <f>OR(N14&lt;10,O14&lt;23)</f>
         <v/>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <f>OR(P14&lt;10,Q14&lt;23)</f>
         <v/>
       </c>
-      <c r="AC14">
-        <f>OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,Z14,AA14,AB14,R14&lt;8.25,T14&lt;33,U14&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD14">
-        <f>IF((C14+D14)/2&gt;=80,5,IF((C14+D14)/2&gt;=70,4,IF((C14+D14)/2&gt;=60,3.5,IF((C14+D14)/2&gt;=50,3,IF((C14+D14)/2&gt;=40,2,IF((C14+D14)/2&gt;=33,1,0))))))</f>
+        <f>OR((C14+D14)&lt;66,(E14+F14)&lt;66,G14&lt;33,(H14+I14)&lt;66,AA14,AB14,AC14,R14&lt;8.25,T14&lt;33,U14&lt;33)</f>
         <v/>
       </c>
       <c r="AE14">
-        <f>IF((E14+F14)/2&gt;=80,5,IF((E14+F14)/2&gt;=70,4,IF((E14+F14)/2&gt;=60,3.5,IF((E14+F14)/2&gt;=50,3,IF((E14+F14)/2&gt;=40,2,IF((E14+F14)/2&gt;=33,1,0))))))</f>
+        <f>IF(C14+D14&lt;66,0,IF((C14+D14)/2&gt;=80,5,IF((C14+D14)/2&gt;=70,4,IF((C14+D14)/2&gt;=60,3.5,IF((C14+D14)/2&gt;=50,3,IF((C14+D14)/2&gt;=40,2,IF((C14+D14)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF14">
-        <f>IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0))))))</f>
+        <f>IF(E14+F14&lt;66,0,IF((E14+F14)/2&gt;=80,5,IF((E14+F14)/2&gt;=70,4,IF((E14+F14)/2&gt;=60,3.5,IF((E14+F14)/2&gt;=50,3,IF((E14+F14)/2&gt;=40,2,IF((E14+F14)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG14">
-        <f>IF((H14+I14)/2&gt;=80,5,IF((H14+I14)/2&gt;=70,4,IF((H14+I14)/2&gt;=60,3.5,IF((H14+I14)/2&gt;=50,3,IF((H14+I14)/2&gt;=40,2,IF((H14+I14)/2&gt;=33,1,0))))))</f>
+        <f>IF(G14&lt;33,0,IF(G14&gt;=80,5,IF(G14&gt;=70,4,IF(G14&gt;=60,3.5,IF(G14&gt;=50,3,IF(G14&gt;=40,2,IF(G14&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH14">
-        <f>IF((J14+K14+L14+M14)/2&gt;=80,5,IF((J14+K14+L14+M14)/2&gt;=70,4,IF((J14+K14+L14+M14)/2&gt;=60,3.5,IF((J14+K14+L14+M14)/2&gt;=50,3,IF((J14+K14+L14+M14)/2&gt;=40,2,IF((J14+K14+L14+M14)/2&gt;=33,1,0))))))</f>
+        <f>IF(H14+I14&lt;66,0,IF((H14+I14)/2&gt;=80,5,IF((H14+I14)/2&gt;=70,4,IF((H14+I14)/2&gt;=60,3.5,IF((H14+I14)/2&gt;=50,3,IF((H14+I14)/2&gt;=40,2,IF((H14+I14)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI14">
-        <f>IF(N14+O14&gt;=80,5,IF(N14+O14&gt;=70,4,IF(N14+O14&gt;=60,3.5,IF(N14+O14&gt;=50,3,IF(N14+O14&gt;=40,2,IF(N14+O14&gt;=33,1,0))))))</f>
+        <f>IF(AA14,0,IF((J14+K14+L14+M14)/2&gt;=80,5,IF((J14+K14+L14+M14)/2&gt;=70,4,IF((J14+K14+L14+M14)/2&gt;=60,3.5,IF((J14+K14+L14+M14)/2&gt;=50,3,IF((J14+K14+L14+M14)/2&gt;=40,2,IF((J14+K14+L14+M14)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ14">
-        <f>IF(P14+Q14&gt;=80,5,IF(P14+Q14&gt;=70,4,IF(P14+Q14&gt;=60,3.5,IF(P14+Q14&gt;=50,3,IF(P14+Q14&gt;=40,2,IF(P14+Q14&gt;=33,1,0))))))</f>
+        <f>IF(AB14,0,IF(N14+O14&gt;=80,5,IF(N14+O14&gt;=70,4,IF(N14+O14&gt;=60,3.5,IF(N14+O14&gt;=50,3,IF(N14+O14&gt;=40,2,IF(N14+O14&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK14">
-        <f>IF(R14*2&gt;=80,5,IF(R14*2&gt;=70,4,IF(R14*2&gt;=60,3.5,IF(R14*2&gt;=50,3,IF(R14*2&gt;=40,2,IF(R14*2&gt;=33,1,0))))))</f>
+        <f>IF(AC14,0,IF(P14+Q14&gt;=80,5,IF(P14+Q14&gt;=70,4,IF(P14+Q14&gt;=60,3.5,IF(P14+Q14&gt;=50,3,IF(P14+Q14&gt;=40,2,IF(P14+Q14&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL14">
-        <f>IF(S14&gt;=80,5,IF(S14&gt;=70,4,IF(S14&gt;=60,3.5,IF(S14&gt;=50,3,IF(S14&gt;=40,2,IF(S14&gt;=33,1,0))))))</f>
+        <f>IF(R14&lt;8.25,0,IF(R14*2&gt;=80,5,IF(R14*2&gt;=70,4,IF(R14*2&gt;=60,3.5,IF(R14*2&gt;=50,3,IF(R14*2&gt;=40,2,IF(R14*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM14">
-        <f>(AD14+AE14+AF14+AG14+AH14+AI14+AJ14+AK14)/8</f>
+        <f>IF(S14&lt;33,0,IF(S14&gt;=80,5,IF(S14&gt;=70,4,IF(S14&gt;=60,3.5,IF(S14&gt;=50,3,IF(S14&gt;=40,2,IF(S14&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN14">
-        <f>IF(AL14&gt;=2,(AL14-2)/8,0)</f>
+        <f>(AE14+AF14+AG14+AH14+AI14+AJ14+AK14+AL14)/8</f>
+        <v/>
+      </c>
+      <c r="AO14">
+        <f>IF(AM14&gt;=2,(AM14-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -2875,71 +2934,75 @@
         <v/>
       </c>
       <c r="X15" s="7">
-        <f>IF(AC15,0,MIN(5,ROUND(AM15+AN15,2)))</f>
-        <v/>
-      </c>
-      <c r="Y15" s="8">
-        <f>IF(X15&gt;=5,"A+",IF(X15&gt;=4,"A",IF(X15&gt;=3.5,"A-",IF(X15&gt;=3,"B",IF(X15&gt;=2,"C",IF(X15&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z15">
+        <f>IF(AD15,0,ROUND(AN15,2))</f>
+        <v/>
+      </c>
+      <c r="Y15" s="7">
+        <f>IF(AD15,0,MIN(5,ROUND(AN15+AO15,2)))</f>
+        <v/>
+      </c>
+      <c r="Z15" s="8">
+        <f>IF(Y15&gt;=5,"A+",IF(Y15&gt;=4,"A",IF(Y15&gt;=3.5,"A-",IF(Y15&gt;=3,"B",IF(Y15&gt;=2,"C",IF(Y15&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA15">
         <f>NOT(OR(AND(J15&gt;=10,K15&gt;=23,L15&gt;=10,M15&gt;=23),AND(J15+L15&gt;=20,K15+M15&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <f>OR(N15&lt;10,O15&lt;23)</f>
         <v/>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <f>OR(P15&lt;10,Q15&lt;23)</f>
         <v/>
       </c>
-      <c r="AC15">
-        <f>OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,Z15,AA15,AB15,R15&lt;8.25,T15&lt;33,U15&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD15">
-        <f>IF((C15+D15)/2&gt;=80,5,IF((C15+D15)/2&gt;=70,4,IF((C15+D15)/2&gt;=60,3.5,IF((C15+D15)/2&gt;=50,3,IF((C15+D15)/2&gt;=40,2,IF((C15+D15)/2&gt;=33,1,0))))))</f>
+        <f>OR((C15+D15)&lt;66,(E15+F15)&lt;66,G15&lt;33,(H15+I15)&lt;66,AA15,AB15,AC15,R15&lt;8.25,T15&lt;33,U15&lt;33)</f>
         <v/>
       </c>
       <c r="AE15">
-        <f>IF((E15+F15)/2&gt;=80,5,IF((E15+F15)/2&gt;=70,4,IF((E15+F15)/2&gt;=60,3.5,IF((E15+F15)/2&gt;=50,3,IF((E15+F15)/2&gt;=40,2,IF((E15+F15)/2&gt;=33,1,0))))))</f>
+        <f>IF(C15+D15&lt;66,0,IF((C15+D15)/2&gt;=80,5,IF((C15+D15)/2&gt;=70,4,IF((C15+D15)/2&gt;=60,3.5,IF((C15+D15)/2&gt;=50,3,IF((C15+D15)/2&gt;=40,2,IF((C15+D15)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF15">
-        <f>IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0))))))</f>
+        <f>IF(E15+F15&lt;66,0,IF((E15+F15)/2&gt;=80,5,IF((E15+F15)/2&gt;=70,4,IF((E15+F15)/2&gt;=60,3.5,IF((E15+F15)/2&gt;=50,3,IF((E15+F15)/2&gt;=40,2,IF((E15+F15)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG15">
-        <f>IF((H15+I15)/2&gt;=80,5,IF((H15+I15)/2&gt;=70,4,IF((H15+I15)/2&gt;=60,3.5,IF((H15+I15)/2&gt;=50,3,IF((H15+I15)/2&gt;=40,2,IF((H15+I15)/2&gt;=33,1,0))))))</f>
+        <f>IF(G15&lt;33,0,IF(G15&gt;=80,5,IF(G15&gt;=70,4,IF(G15&gt;=60,3.5,IF(G15&gt;=50,3,IF(G15&gt;=40,2,IF(G15&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH15">
-        <f>IF((J15+K15+L15+M15)/2&gt;=80,5,IF((J15+K15+L15+M15)/2&gt;=70,4,IF((J15+K15+L15+M15)/2&gt;=60,3.5,IF((J15+K15+L15+M15)/2&gt;=50,3,IF((J15+K15+L15+M15)/2&gt;=40,2,IF((J15+K15+L15+M15)/2&gt;=33,1,0))))))</f>
+        <f>IF(H15+I15&lt;66,0,IF((H15+I15)/2&gt;=80,5,IF((H15+I15)/2&gt;=70,4,IF((H15+I15)/2&gt;=60,3.5,IF((H15+I15)/2&gt;=50,3,IF((H15+I15)/2&gt;=40,2,IF((H15+I15)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI15">
-        <f>IF(N15+O15&gt;=80,5,IF(N15+O15&gt;=70,4,IF(N15+O15&gt;=60,3.5,IF(N15+O15&gt;=50,3,IF(N15+O15&gt;=40,2,IF(N15+O15&gt;=33,1,0))))))</f>
+        <f>IF(AA15,0,IF((J15+K15+L15+M15)/2&gt;=80,5,IF((J15+K15+L15+M15)/2&gt;=70,4,IF((J15+K15+L15+M15)/2&gt;=60,3.5,IF((J15+K15+L15+M15)/2&gt;=50,3,IF((J15+K15+L15+M15)/2&gt;=40,2,IF((J15+K15+L15+M15)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ15">
-        <f>IF(P15+Q15&gt;=80,5,IF(P15+Q15&gt;=70,4,IF(P15+Q15&gt;=60,3.5,IF(P15+Q15&gt;=50,3,IF(P15+Q15&gt;=40,2,IF(P15+Q15&gt;=33,1,0))))))</f>
+        <f>IF(AB15,0,IF(N15+O15&gt;=80,5,IF(N15+O15&gt;=70,4,IF(N15+O15&gt;=60,3.5,IF(N15+O15&gt;=50,3,IF(N15+O15&gt;=40,2,IF(N15+O15&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK15">
-        <f>IF(R15*2&gt;=80,5,IF(R15*2&gt;=70,4,IF(R15*2&gt;=60,3.5,IF(R15*2&gt;=50,3,IF(R15*2&gt;=40,2,IF(R15*2&gt;=33,1,0))))))</f>
+        <f>IF(AC15,0,IF(P15+Q15&gt;=80,5,IF(P15+Q15&gt;=70,4,IF(P15+Q15&gt;=60,3.5,IF(P15+Q15&gt;=50,3,IF(P15+Q15&gt;=40,2,IF(P15+Q15&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL15">
-        <f>IF(S15&gt;=80,5,IF(S15&gt;=70,4,IF(S15&gt;=60,3.5,IF(S15&gt;=50,3,IF(S15&gt;=40,2,IF(S15&gt;=33,1,0))))))</f>
+        <f>IF(R15&lt;8.25,0,IF(R15*2&gt;=80,5,IF(R15*2&gt;=70,4,IF(R15*2&gt;=60,3.5,IF(R15*2&gt;=50,3,IF(R15*2&gt;=40,2,IF(R15*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM15">
-        <f>(AD15+AE15+AF15+AG15+AH15+AI15+AJ15+AK15)/8</f>
+        <f>IF(S15&lt;33,0,IF(S15&gt;=80,5,IF(S15&gt;=70,4,IF(S15&gt;=60,3.5,IF(S15&gt;=50,3,IF(S15&gt;=40,2,IF(S15&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN15">
-        <f>IF(AL15&gt;=2,(AL15-2)/8,0)</f>
+        <f>(AE15+AF15+AG15+AH15+AI15+AJ15+AK15+AL15)/8</f>
+        <v/>
+      </c>
+      <c r="AO15">
+        <f>IF(AM15&gt;=2,(AM15-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3018,71 +3081,75 @@
         <v/>
       </c>
       <c r="X16" s="7">
-        <f>IF(AC16,0,MIN(5,ROUND(AM16+AN16,2)))</f>
-        <v/>
-      </c>
-      <c r="Y16" s="8">
-        <f>IF(X16&gt;=5,"A+",IF(X16&gt;=4,"A",IF(X16&gt;=3.5,"A-",IF(X16&gt;=3,"B",IF(X16&gt;=2,"C",IF(X16&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z16">
+        <f>IF(AD16,0,ROUND(AN16,2))</f>
+        <v/>
+      </c>
+      <c r="Y16" s="7">
+        <f>IF(AD16,0,MIN(5,ROUND(AN16+AO16,2)))</f>
+        <v/>
+      </c>
+      <c r="Z16" s="8">
+        <f>IF(Y16&gt;=5,"A+",IF(Y16&gt;=4,"A",IF(Y16&gt;=3.5,"A-",IF(Y16&gt;=3,"B",IF(Y16&gt;=2,"C",IF(Y16&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA16">
         <f>NOT(OR(AND(J16&gt;=10,K16&gt;=23,L16&gt;=10,M16&gt;=23),AND(J16+L16&gt;=20,K16+M16&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <f>OR(N16&lt;10,O16&lt;23)</f>
         <v/>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <f>OR(P16&lt;10,Q16&lt;23)</f>
         <v/>
       </c>
-      <c r="AC16">
-        <f>OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,Z16,AA16,AB16,R16&lt;8.25,T16&lt;33,U16&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD16">
-        <f>IF((C16+D16)/2&gt;=80,5,IF((C16+D16)/2&gt;=70,4,IF((C16+D16)/2&gt;=60,3.5,IF((C16+D16)/2&gt;=50,3,IF((C16+D16)/2&gt;=40,2,IF((C16+D16)/2&gt;=33,1,0))))))</f>
+        <f>OR((C16+D16)&lt;66,(E16+F16)&lt;66,G16&lt;33,(H16+I16)&lt;66,AA16,AB16,AC16,R16&lt;8.25,T16&lt;33,U16&lt;33)</f>
         <v/>
       </c>
       <c r="AE16">
-        <f>IF((E16+F16)/2&gt;=80,5,IF((E16+F16)/2&gt;=70,4,IF((E16+F16)/2&gt;=60,3.5,IF((E16+F16)/2&gt;=50,3,IF((E16+F16)/2&gt;=40,2,IF((E16+F16)/2&gt;=33,1,0))))))</f>
+        <f>IF(C16+D16&lt;66,0,IF((C16+D16)/2&gt;=80,5,IF((C16+D16)/2&gt;=70,4,IF((C16+D16)/2&gt;=60,3.5,IF((C16+D16)/2&gt;=50,3,IF((C16+D16)/2&gt;=40,2,IF((C16+D16)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF16">
-        <f>IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0))))))</f>
+        <f>IF(E16+F16&lt;66,0,IF((E16+F16)/2&gt;=80,5,IF((E16+F16)/2&gt;=70,4,IF((E16+F16)/2&gt;=60,3.5,IF((E16+F16)/2&gt;=50,3,IF((E16+F16)/2&gt;=40,2,IF((E16+F16)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG16">
-        <f>IF((H16+I16)/2&gt;=80,5,IF((H16+I16)/2&gt;=70,4,IF((H16+I16)/2&gt;=60,3.5,IF((H16+I16)/2&gt;=50,3,IF((H16+I16)/2&gt;=40,2,IF((H16+I16)/2&gt;=33,1,0))))))</f>
+        <f>IF(G16&lt;33,0,IF(G16&gt;=80,5,IF(G16&gt;=70,4,IF(G16&gt;=60,3.5,IF(G16&gt;=50,3,IF(G16&gt;=40,2,IF(G16&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH16">
-        <f>IF((J16+K16+L16+M16)/2&gt;=80,5,IF((J16+K16+L16+M16)/2&gt;=70,4,IF((J16+K16+L16+M16)/2&gt;=60,3.5,IF((J16+K16+L16+M16)/2&gt;=50,3,IF((J16+K16+L16+M16)/2&gt;=40,2,IF((J16+K16+L16+M16)/2&gt;=33,1,0))))))</f>
+        <f>IF(H16+I16&lt;66,0,IF((H16+I16)/2&gt;=80,5,IF((H16+I16)/2&gt;=70,4,IF((H16+I16)/2&gt;=60,3.5,IF((H16+I16)/2&gt;=50,3,IF((H16+I16)/2&gt;=40,2,IF((H16+I16)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI16">
-        <f>IF(N16+O16&gt;=80,5,IF(N16+O16&gt;=70,4,IF(N16+O16&gt;=60,3.5,IF(N16+O16&gt;=50,3,IF(N16+O16&gt;=40,2,IF(N16+O16&gt;=33,1,0))))))</f>
+        <f>IF(AA16,0,IF((J16+K16+L16+M16)/2&gt;=80,5,IF((J16+K16+L16+M16)/2&gt;=70,4,IF((J16+K16+L16+M16)/2&gt;=60,3.5,IF((J16+K16+L16+M16)/2&gt;=50,3,IF((J16+K16+L16+M16)/2&gt;=40,2,IF((J16+K16+L16+M16)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ16">
-        <f>IF(P16+Q16&gt;=80,5,IF(P16+Q16&gt;=70,4,IF(P16+Q16&gt;=60,3.5,IF(P16+Q16&gt;=50,3,IF(P16+Q16&gt;=40,2,IF(P16+Q16&gt;=33,1,0))))))</f>
+        <f>IF(AB16,0,IF(N16+O16&gt;=80,5,IF(N16+O16&gt;=70,4,IF(N16+O16&gt;=60,3.5,IF(N16+O16&gt;=50,3,IF(N16+O16&gt;=40,2,IF(N16+O16&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK16">
-        <f>IF(R16*2&gt;=80,5,IF(R16*2&gt;=70,4,IF(R16*2&gt;=60,3.5,IF(R16*2&gt;=50,3,IF(R16*2&gt;=40,2,IF(R16*2&gt;=33,1,0))))))</f>
+        <f>IF(AC16,0,IF(P16+Q16&gt;=80,5,IF(P16+Q16&gt;=70,4,IF(P16+Q16&gt;=60,3.5,IF(P16+Q16&gt;=50,3,IF(P16+Q16&gt;=40,2,IF(P16+Q16&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL16">
-        <f>IF(S16&gt;=80,5,IF(S16&gt;=70,4,IF(S16&gt;=60,3.5,IF(S16&gt;=50,3,IF(S16&gt;=40,2,IF(S16&gt;=33,1,0))))))</f>
+        <f>IF(R16&lt;8.25,0,IF(R16*2&gt;=80,5,IF(R16*2&gt;=70,4,IF(R16*2&gt;=60,3.5,IF(R16*2&gt;=50,3,IF(R16*2&gt;=40,2,IF(R16*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM16">
-        <f>(AD16+AE16+AF16+AG16+AH16+AI16+AJ16+AK16)/8</f>
+        <f>IF(S16&lt;33,0,IF(S16&gt;=80,5,IF(S16&gt;=70,4,IF(S16&gt;=60,3.5,IF(S16&gt;=50,3,IF(S16&gt;=40,2,IF(S16&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN16">
-        <f>IF(AL16&gt;=2,(AL16-2)/8,0)</f>
+        <f>(AE16+AF16+AG16+AH16+AI16+AJ16+AK16+AL16)/8</f>
+        <v/>
+      </c>
+      <c r="AO16">
+        <f>IF(AM16&gt;=2,(AM16-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3161,71 +3228,75 @@
         <v/>
       </c>
       <c r="X17" s="7">
-        <f>IF(AC17,0,MIN(5,ROUND(AM17+AN17,2)))</f>
-        <v/>
-      </c>
-      <c r="Y17" s="8">
-        <f>IF(X17&gt;=5,"A+",IF(X17&gt;=4,"A",IF(X17&gt;=3.5,"A-",IF(X17&gt;=3,"B",IF(X17&gt;=2,"C",IF(X17&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z17">
+        <f>IF(AD17,0,ROUND(AN17,2))</f>
+        <v/>
+      </c>
+      <c r="Y17" s="7">
+        <f>IF(AD17,0,MIN(5,ROUND(AN17+AO17,2)))</f>
+        <v/>
+      </c>
+      <c r="Z17" s="8">
+        <f>IF(Y17&gt;=5,"A+",IF(Y17&gt;=4,"A",IF(Y17&gt;=3.5,"A-",IF(Y17&gt;=3,"B",IF(Y17&gt;=2,"C",IF(Y17&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA17">
         <f>NOT(OR(AND(J17&gt;=10,K17&gt;=23,L17&gt;=10,M17&gt;=23),AND(J17+L17&gt;=20,K17+M17&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <f>OR(N17&lt;10,O17&lt;23)</f>
         <v/>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <f>OR(P17&lt;10,Q17&lt;23)</f>
         <v/>
       </c>
-      <c r="AC17">
-        <f>OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,Z17,AA17,AB17,R17&lt;8.25,T17&lt;33,U17&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD17">
-        <f>IF((C17+D17)/2&gt;=80,5,IF((C17+D17)/2&gt;=70,4,IF((C17+D17)/2&gt;=60,3.5,IF((C17+D17)/2&gt;=50,3,IF((C17+D17)/2&gt;=40,2,IF((C17+D17)/2&gt;=33,1,0))))))</f>
+        <f>OR((C17+D17)&lt;66,(E17+F17)&lt;66,G17&lt;33,(H17+I17)&lt;66,AA17,AB17,AC17,R17&lt;8.25,T17&lt;33,U17&lt;33)</f>
         <v/>
       </c>
       <c r="AE17">
-        <f>IF((E17+F17)/2&gt;=80,5,IF((E17+F17)/2&gt;=70,4,IF((E17+F17)/2&gt;=60,3.5,IF((E17+F17)/2&gt;=50,3,IF((E17+F17)/2&gt;=40,2,IF((E17+F17)/2&gt;=33,1,0))))))</f>
+        <f>IF(C17+D17&lt;66,0,IF((C17+D17)/2&gt;=80,5,IF((C17+D17)/2&gt;=70,4,IF((C17+D17)/2&gt;=60,3.5,IF((C17+D17)/2&gt;=50,3,IF((C17+D17)/2&gt;=40,2,IF((C17+D17)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF17">
-        <f>IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0))))))</f>
+        <f>IF(E17+F17&lt;66,0,IF((E17+F17)/2&gt;=80,5,IF((E17+F17)/2&gt;=70,4,IF((E17+F17)/2&gt;=60,3.5,IF((E17+F17)/2&gt;=50,3,IF((E17+F17)/2&gt;=40,2,IF((E17+F17)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG17">
-        <f>IF((H17+I17)/2&gt;=80,5,IF((H17+I17)/2&gt;=70,4,IF((H17+I17)/2&gt;=60,3.5,IF((H17+I17)/2&gt;=50,3,IF((H17+I17)/2&gt;=40,2,IF((H17+I17)/2&gt;=33,1,0))))))</f>
+        <f>IF(G17&lt;33,0,IF(G17&gt;=80,5,IF(G17&gt;=70,4,IF(G17&gt;=60,3.5,IF(G17&gt;=50,3,IF(G17&gt;=40,2,IF(G17&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH17">
-        <f>IF((J17+K17+L17+M17)/2&gt;=80,5,IF((J17+K17+L17+M17)/2&gt;=70,4,IF((J17+K17+L17+M17)/2&gt;=60,3.5,IF((J17+K17+L17+M17)/2&gt;=50,3,IF((J17+K17+L17+M17)/2&gt;=40,2,IF((J17+K17+L17+M17)/2&gt;=33,1,0))))))</f>
+        <f>IF(H17+I17&lt;66,0,IF((H17+I17)/2&gt;=80,5,IF((H17+I17)/2&gt;=70,4,IF((H17+I17)/2&gt;=60,3.5,IF((H17+I17)/2&gt;=50,3,IF((H17+I17)/2&gt;=40,2,IF((H17+I17)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI17">
-        <f>IF(N17+O17&gt;=80,5,IF(N17+O17&gt;=70,4,IF(N17+O17&gt;=60,3.5,IF(N17+O17&gt;=50,3,IF(N17+O17&gt;=40,2,IF(N17+O17&gt;=33,1,0))))))</f>
+        <f>IF(AA17,0,IF((J17+K17+L17+M17)/2&gt;=80,5,IF((J17+K17+L17+M17)/2&gt;=70,4,IF((J17+K17+L17+M17)/2&gt;=60,3.5,IF((J17+K17+L17+M17)/2&gt;=50,3,IF((J17+K17+L17+M17)/2&gt;=40,2,IF((J17+K17+L17+M17)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ17">
-        <f>IF(P17+Q17&gt;=80,5,IF(P17+Q17&gt;=70,4,IF(P17+Q17&gt;=60,3.5,IF(P17+Q17&gt;=50,3,IF(P17+Q17&gt;=40,2,IF(P17+Q17&gt;=33,1,0))))))</f>
+        <f>IF(AB17,0,IF(N17+O17&gt;=80,5,IF(N17+O17&gt;=70,4,IF(N17+O17&gt;=60,3.5,IF(N17+O17&gt;=50,3,IF(N17+O17&gt;=40,2,IF(N17+O17&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK17">
-        <f>IF(R17*2&gt;=80,5,IF(R17*2&gt;=70,4,IF(R17*2&gt;=60,3.5,IF(R17*2&gt;=50,3,IF(R17*2&gt;=40,2,IF(R17*2&gt;=33,1,0))))))</f>
+        <f>IF(AC17,0,IF(P17+Q17&gt;=80,5,IF(P17+Q17&gt;=70,4,IF(P17+Q17&gt;=60,3.5,IF(P17+Q17&gt;=50,3,IF(P17+Q17&gt;=40,2,IF(P17+Q17&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL17">
-        <f>IF(S17&gt;=80,5,IF(S17&gt;=70,4,IF(S17&gt;=60,3.5,IF(S17&gt;=50,3,IF(S17&gt;=40,2,IF(S17&gt;=33,1,0))))))</f>
+        <f>IF(R17&lt;8.25,0,IF(R17*2&gt;=80,5,IF(R17*2&gt;=70,4,IF(R17*2&gt;=60,3.5,IF(R17*2&gt;=50,3,IF(R17*2&gt;=40,2,IF(R17*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM17">
-        <f>(AD17+AE17+AF17+AG17+AH17+AI17+AJ17+AK17)/8</f>
+        <f>IF(S17&lt;33,0,IF(S17&gt;=80,5,IF(S17&gt;=70,4,IF(S17&gt;=60,3.5,IF(S17&gt;=50,3,IF(S17&gt;=40,2,IF(S17&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN17">
-        <f>IF(AL17&gt;=2,(AL17-2)/8,0)</f>
+        <f>(AE17+AF17+AG17+AH17+AI17+AJ17+AK17+AL17)/8</f>
+        <v/>
+      </c>
+      <c r="AO17">
+        <f>IF(AM17&gt;=2,(AM17-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3304,71 +3375,75 @@
         <v/>
       </c>
       <c r="X18" s="7">
-        <f>IF(AC18,0,MIN(5,ROUND(AM18+AN18,2)))</f>
-        <v/>
-      </c>
-      <c r="Y18" s="8">
-        <f>IF(X18&gt;=5,"A+",IF(X18&gt;=4,"A",IF(X18&gt;=3.5,"A-",IF(X18&gt;=3,"B",IF(X18&gt;=2,"C",IF(X18&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z18">
+        <f>IF(AD18,0,ROUND(AN18,2))</f>
+        <v/>
+      </c>
+      <c r="Y18" s="7">
+        <f>IF(AD18,0,MIN(5,ROUND(AN18+AO18,2)))</f>
+        <v/>
+      </c>
+      <c r="Z18" s="8">
+        <f>IF(Y18&gt;=5,"A+",IF(Y18&gt;=4,"A",IF(Y18&gt;=3.5,"A-",IF(Y18&gt;=3,"B",IF(Y18&gt;=2,"C",IF(Y18&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA18">
         <f>NOT(OR(AND(J18&gt;=10,K18&gt;=23,L18&gt;=10,M18&gt;=23),AND(J18+L18&gt;=20,K18+M18&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <f>OR(N18&lt;10,O18&lt;23)</f>
         <v/>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <f>OR(P18&lt;10,Q18&lt;23)</f>
         <v/>
       </c>
-      <c r="AC18">
-        <f>OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,Z18,AA18,AB18,R18&lt;8.25,T18&lt;33,U18&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD18">
-        <f>IF((C18+D18)/2&gt;=80,5,IF((C18+D18)/2&gt;=70,4,IF((C18+D18)/2&gt;=60,3.5,IF((C18+D18)/2&gt;=50,3,IF((C18+D18)/2&gt;=40,2,IF((C18+D18)/2&gt;=33,1,0))))))</f>
+        <f>OR((C18+D18)&lt;66,(E18+F18)&lt;66,G18&lt;33,(H18+I18)&lt;66,AA18,AB18,AC18,R18&lt;8.25,T18&lt;33,U18&lt;33)</f>
         <v/>
       </c>
       <c r="AE18">
-        <f>IF((E18+F18)/2&gt;=80,5,IF((E18+F18)/2&gt;=70,4,IF((E18+F18)/2&gt;=60,3.5,IF((E18+F18)/2&gt;=50,3,IF((E18+F18)/2&gt;=40,2,IF((E18+F18)/2&gt;=33,1,0))))))</f>
+        <f>IF(C18+D18&lt;66,0,IF((C18+D18)/2&gt;=80,5,IF((C18+D18)/2&gt;=70,4,IF((C18+D18)/2&gt;=60,3.5,IF((C18+D18)/2&gt;=50,3,IF((C18+D18)/2&gt;=40,2,IF((C18+D18)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF18">
-        <f>IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0))))))</f>
+        <f>IF(E18+F18&lt;66,0,IF((E18+F18)/2&gt;=80,5,IF((E18+F18)/2&gt;=70,4,IF((E18+F18)/2&gt;=60,3.5,IF((E18+F18)/2&gt;=50,3,IF((E18+F18)/2&gt;=40,2,IF((E18+F18)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG18">
-        <f>IF((H18+I18)/2&gt;=80,5,IF((H18+I18)/2&gt;=70,4,IF((H18+I18)/2&gt;=60,3.5,IF((H18+I18)/2&gt;=50,3,IF((H18+I18)/2&gt;=40,2,IF((H18+I18)/2&gt;=33,1,0))))))</f>
+        <f>IF(G18&lt;33,0,IF(G18&gt;=80,5,IF(G18&gt;=70,4,IF(G18&gt;=60,3.5,IF(G18&gt;=50,3,IF(G18&gt;=40,2,IF(G18&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH18">
-        <f>IF((J18+K18+L18+M18)/2&gt;=80,5,IF((J18+K18+L18+M18)/2&gt;=70,4,IF((J18+K18+L18+M18)/2&gt;=60,3.5,IF((J18+K18+L18+M18)/2&gt;=50,3,IF((J18+K18+L18+M18)/2&gt;=40,2,IF((J18+K18+L18+M18)/2&gt;=33,1,0))))))</f>
+        <f>IF(H18+I18&lt;66,0,IF((H18+I18)/2&gt;=80,5,IF((H18+I18)/2&gt;=70,4,IF((H18+I18)/2&gt;=60,3.5,IF((H18+I18)/2&gt;=50,3,IF((H18+I18)/2&gt;=40,2,IF((H18+I18)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI18">
-        <f>IF(N18+O18&gt;=80,5,IF(N18+O18&gt;=70,4,IF(N18+O18&gt;=60,3.5,IF(N18+O18&gt;=50,3,IF(N18+O18&gt;=40,2,IF(N18+O18&gt;=33,1,0))))))</f>
+        <f>IF(AA18,0,IF((J18+K18+L18+M18)/2&gt;=80,5,IF((J18+K18+L18+M18)/2&gt;=70,4,IF((J18+K18+L18+M18)/2&gt;=60,3.5,IF((J18+K18+L18+M18)/2&gt;=50,3,IF((J18+K18+L18+M18)/2&gt;=40,2,IF((J18+K18+L18+M18)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ18">
-        <f>IF(P18+Q18&gt;=80,5,IF(P18+Q18&gt;=70,4,IF(P18+Q18&gt;=60,3.5,IF(P18+Q18&gt;=50,3,IF(P18+Q18&gt;=40,2,IF(P18+Q18&gt;=33,1,0))))))</f>
+        <f>IF(AB18,0,IF(N18+O18&gt;=80,5,IF(N18+O18&gt;=70,4,IF(N18+O18&gt;=60,3.5,IF(N18+O18&gt;=50,3,IF(N18+O18&gt;=40,2,IF(N18+O18&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK18">
-        <f>IF(R18*2&gt;=80,5,IF(R18*2&gt;=70,4,IF(R18*2&gt;=60,3.5,IF(R18*2&gt;=50,3,IF(R18*2&gt;=40,2,IF(R18*2&gt;=33,1,0))))))</f>
+        <f>IF(AC18,0,IF(P18+Q18&gt;=80,5,IF(P18+Q18&gt;=70,4,IF(P18+Q18&gt;=60,3.5,IF(P18+Q18&gt;=50,3,IF(P18+Q18&gt;=40,2,IF(P18+Q18&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL18">
-        <f>IF(S18&gt;=80,5,IF(S18&gt;=70,4,IF(S18&gt;=60,3.5,IF(S18&gt;=50,3,IF(S18&gt;=40,2,IF(S18&gt;=33,1,0))))))</f>
+        <f>IF(R18&lt;8.25,0,IF(R18*2&gt;=80,5,IF(R18*2&gt;=70,4,IF(R18*2&gt;=60,3.5,IF(R18*2&gt;=50,3,IF(R18*2&gt;=40,2,IF(R18*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM18">
-        <f>(AD18+AE18+AF18+AG18+AH18+AI18+AJ18+AK18)/8</f>
+        <f>IF(S18&lt;33,0,IF(S18&gt;=80,5,IF(S18&gt;=70,4,IF(S18&gt;=60,3.5,IF(S18&gt;=50,3,IF(S18&gt;=40,2,IF(S18&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN18">
-        <f>IF(AL18&gt;=2,(AL18-2)/8,0)</f>
+        <f>(AE18+AF18+AG18+AH18+AI18+AJ18+AK18+AL18)/8</f>
+        <v/>
+      </c>
+      <c r="AO18">
+        <f>IF(AM18&gt;=2,(AM18-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3447,71 +3522,75 @@
         <v/>
       </c>
       <c r="X19" s="7">
-        <f>IF(AC19,0,MIN(5,ROUND(AM19+AN19,2)))</f>
-        <v/>
-      </c>
-      <c r="Y19" s="8">
-        <f>IF(X19&gt;=5,"A+",IF(X19&gt;=4,"A",IF(X19&gt;=3.5,"A-",IF(X19&gt;=3,"B",IF(X19&gt;=2,"C",IF(X19&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z19">
+        <f>IF(AD19,0,ROUND(AN19,2))</f>
+        <v/>
+      </c>
+      <c r="Y19" s="7">
+        <f>IF(AD19,0,MIN(5,ROUND(AN19+AO19,2)))</f>
+        <v/>
+      </c>
+      <c r="Z19" s="8">
+        <f>IF(Y19&gt;=5,"A+",IF(Y19&gt;=4,"A",IF(Y19&gt;=3.5,"A-",IF(Y19&gt;=3,"B",IF(Y19&gt;=2,"C",IF(Y19&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA19">
         <f>NOT(OR(AND(J19&gt;=10,K19&gt;=23,L19&gt;=10,M19&gt;=23),AND(J19+L19&gt;=20,K19+M19&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <f>OR(N19&lt;10,O19&lt;23)</f>
         <v/>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <f>OR(P19&lt;10,Q19&lt;23)</f>
         <v/>
       </c>
-      <c r="AC19">
-        <f>OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,Z19,AA19,AB19,R19&lt;8.25,T19&lt;33,U19&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD19">
-        <f>IF((C19+D19)/2&gt;=80,5,IF((C19+D19)/2&gt;=70,4,IF((C19+D19)/2&gt;=60,3.5,IF((C19+D19)/2&gt;=50,3,IF((C19+D19)/2&gt;=40,2,IF((C19+D19)/2&gt;=33,1,0))))))</f>
+        <f>OR((C19+D19)&lt;66,(E19+F19)&lt;66,G19&lt;33,(H19+I19)&lt;66,AA19,AB19,AC19,R19&lt;8.25,T19&lt;33,U19&lt;33)</f>
         <v/>
       </c>
       <c r="AE19">
-        <f>IF((E19+F19)/2&gt;=80,5,IF((E19+F19)/2&gt;=70,4,IF((E19+F19)/2&gt;=60,3.5,IF((E19+F19)/2&gt;=50,3,IF((E19+F19)/2&gt;=40,2,IF((E19+F19)/2&gt;=33,1,0))))))</f>
+        <f>IF(C19+D19&lt;66,0,IF((C19+D19)/2&gt;=80,5,IF((C19+D19)/2&gt;=70,4,IF((C19+D19)/2&gt;=60,3.5,IF((C19+D19)/2&gt;=50,3,IF((C19+D19)/2&gt;=40,2,IF((C19+D19)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF19">
-        <f>IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0))))))</f>
+        <f>IF(E19+F19&lt;66,0,IF((E19+F19)/2&gt;=80,5,IF((E19+F19)/2&gt;=70,4,IF((E19+F19)/2&gt;=60,3.5,IF((E19+F19)/2&gt;=50,3,IF((E19+F19)/2&gt;=40,2,IF((E19+F19)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG19">
-        <f>IF((H19+I19)/2&gt;=80,5,IF((H19+I19)/2&gt;=70,4,IF((H19+I19)/2&gt;=60,3.5,IF((H19+I19)/2&gt;=50,3,IF((H19+I19)/2&gt;=40,2,IF((H19+I19)/2&gt;=33,1,0))))))</f>
+        <f>IF(G19&lt;33,0,IF(G19&gt;=80,5,IF(G19&gt;=70,4,IF(G19&gt;=60,3.5,IF(G19&gt;=50,3,IF(G19&gt;=40,2,IF(G19&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH19">
-        <f>IF((J19+K19+L19+M19)/2&gt;=80,5,IF((J19+K19+L19+M19)/2&gt;=70,4,IF((J19+K19+L19+M19)/2&gt;=60,3.5,IF((J19+K19+L19+M19)/2&gt;=50,3,IF((J19+K19+L19+M19)/2&gt;=40,2,IF((J19+K19+L19+M19)/2&gt;=33,1,0))))))</f>
+        <f>IF(H19+I19&lt;66,0,IF((H19+I19)/2&gt;=80,5,IF((H19+I19)/2&gt;=70,4,IF((H19+I19)/2&gt;=60,3.5,IF((H19+I19)/2&gt;=50,3,IF((H19+I19)/2&gt;=40,2,IF((H19+I19)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI19">
-        <f>IF(N19+O19&gt;=80,5,IF(N19+O19&gt;=70,4,IF(N19+O19&gt;=60,3.5,IF(N19+O19&gt;=50,3,IF(N19+O19&gt;=40,2,IF(N19+O19&gt;=33,1,0))))))</f>
+        <f>IF(AA19,0,IF((J19+K19+L19+M19)/2&gt;=80,5,IF((J19+K19+L19+M19)/2&gt;=70,4,IF((J19+K19+L19+M19)/2&gt;=60,3.5,IF((J19+K19+L19+M19)/2&gt;=50,3,IF((J19+K19+L19+M19)/2&gt;=40,2,IF((J19+K19+L19+M19)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ19">
-        <f>IF(P19+Q19&gt;=80,5,IF(P19+Q19&gt;=70,4,IF(P19+Q19&gt;=60,3.5,IF(P19+Q19&gt;=50,3,IF(P19+Q19&gt;=40,2,IF(P19+Q19&gt;=33,1,0))))))</f>
+        <f>IF(AB19,0,IF(N19+O19&gt;=80,5,IF(N19+O19&gt;=70,4,IF(N19+O19&gt;=60,3.5,IF(N19+O19&gt;=50,3,IF(N19+O19&gt;=40,2,IF(N19+O19&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK19">
-        <f>IF(R19*2&gt;=80,5,IF(R19*2&gt;=70,4,IF(R19*2&gt;=60,3.5,IF(R19*2&gt;=50,3,IF(R19*2&gt;=40,2,IF(R19*2&gt;=33,1,0))))))</f>
+        <f>IF(AC19,0,IF(P19+Q19&gt;=80,5,IF(P19+Q19&gt;=70,4,IF(P19+Q19&gt;=60,3.5,IF(P19+Q19&gt;=50,3,IF(P19+Q19&gt;=40,2,IF(P19+Q19&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL19">
-        <f>IF(S19&gt;=80,5,IF(S19&gt;=70,4,IF(S19&gt;=60,3.5,IF(S19&gt;=50,3,IF(S19&gt;=40,2,IF(S19&gt;=33,1,0))))))</f>
+        <f>IF(R19&lt;8.25,0,IF(R19*2&gt;=80,5,IF(R19*2&gt;=70,4,IF(R19*2&gt;=60,3.5,IF(R19*2&gt;=50,3,IF(R19*2&gt;=40,2,IF(R19*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM19">
-        <f>(AD19+AE19+AF19+AG19+AH19+AI19+AJ19+AK19)/8</f>
+        <f>IF(S19&lt;33,0,IF(S19&gt;=80,5,IF(S19&gt;=70,4,IF(S19&gt;=60,3.5,IF(S19&gt;=50,3,IF(S19&gt;=40,2,IF(S19&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN19">
-        <f>IF(AL19&gt;=2,(AL19-2)/8,0)</f>
+        <f>(AE19+AF19+AG19+AH19+AI19+AJ19+AK19+AL19)/8</f>
+        <v/>
+      </c>
+      <c r="AO19">
+        <f>IF(AM19&gt;=2,(AM19-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3590,71 +3669,75 @@
         <v/>
       </c>
       <c r="X20" s="7">
-        <f>IF(AC20,0,MIN(5,ROUND(AM20+AN20,2)))</f>
-        <v/>
-      </c>
-      <c r="Y20" s="8">
-        <f>IF(X20&gt;=5,"A+",IF(X20&gt;=4,"A",IF(X20&gt;=3.5,"A-",IF(X20&gt;=3,"B",IF(X20&gt;=2,"C",IF(X20&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z20">
+        <f>IF(AD20,0,ROUND(AN20,2))</f>
+        <v/>
+      </c>
+      <c r="Y20" s="7">
+        <f>IF(AD20,0,MIN(5,ROUND(AN20+AO20,2)))</f>
+        <v/>
+      </c>
+      <c r="Z20" s="8">
+        <f>IF(Y20&gt;=5,"A+",IF(Y20&gt;=4,"A",IF(Y20&gt;=3.5,"A-",IF(Y20&gt;=3,"B",IF(Y20&gt;=2,"C",IF(Y20&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA20">
         <f>NOT(OR(AND(J20&gt;=10,K20&gt;=23,L20&gt;=10,M20&gt;=23),AND(J20+L20&gt;=20,K20+M20&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <f>OR(N20&lt;10,O20&lt;23)</f>
         <v/>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <f>OR(P20&lt;10,Q20&lt;23)</f>
         <v/>
       </c>
-      <c r="AC20">
-        <f>OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,Z20,AA20,AB20,R20&lt;8.25,T20&lt;33,U20&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD20">
-        <f>IF((C20+D20)/2&gt;=80,5,IF((C20+D20)/2&gt;=70,4,IF((C20+D20)/2&gt;=60,3.5,IF((C20+D20)/2&gt;=50,3,IF((C20+D20)/2&gt;=40,2,IF((C20+D20)/2&gt;=33,1,0))))))</f>
+        <f>OR((C20+D20)&lt;66,(E20+F20)&lt;66,G20&lt;33,(H20+I20)&lt;66,AA20,AB20,AC20,R20&lt;8.25,T20&lt;33,U20&lt;33)</f>
         <v/>
       </c>
       <c r="AE20">
-        <f>IF((E20+F20)/2&gt;=80,5,IF((E20+F20)/2&gt;=70,4,IF((E20+F20)/2&gt;=60,3.5,IF((E20+F20)/2&gt;=50,3,IF((E20+F20)/2&gt;=40,2,IF((E20+F20)/2&gt;=33,1,0))))))</f>
+        <f>IF(C20+D20&lt;66,0,IF((C20+D20)/2&gt;=80,5,IF((C20+D20)/2&gt;=70,4,IF((C20+D20)/2&gt;=60,3.5,IF((C20+D20)/2&gt;=50,3,IF((C20+D20)/2&gt;=40,2,IF((C20+D20)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF20">
-        <f>IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0))))))</f>
+        <f>IF(E20+F20&lt;66,0,IF((E20+F20)/2&gt;=80,5,IF((E20+F20)/2&gt;=70,4,IF((E20+F20)/2&gt;=60,3.5,IF((E20+F20)/2&gt;=50,3,IF((E20+F20)/2&gt;=40,2,IF((E20+F20)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG20">
-        <f>IF((H20+I20)/2&gt;=80,5,IF((H20+I20)/2&gt;=70,4,IF((H20+I20)/2&gt;=60,3.5,IF((H20+I20)/2&gt;=50,3,IF((H20+I20)/2&gt;=40,2,IF((H20+I20)/2&gt;=33,1,0))))))</f>
+        <f>IF(G20&lt;33,0,IF(G20&gt;=80,5,IF(G20&gt;=70,4,IF(G20&gt;=60,3.5,IF(G20&gt;=50,3,IF(G20&gt;=40,2,IF(G20&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH20">
-        <f>IF((J20+K20+L20+M20)/2&gt;=80,5,IF((J20+K20+L20+M20)/2&gt;=70,4,IF((J20+K20+L20+M20)/2&gt;=60,3.5,IF((J20+K20+L20+M20)/2&gt;=50,3,IF((J20+K20+L20+M20)/2&gt;=40,2,IF((J20+K20+L20+M20)/2&gt;=33,1,0))))))</f>
+        <f>IF(H20+I20&lt;66,0,IF((H20+I20)/2&gt;=80,5,IF((H20+I20)/2&gt;=70,4,IF((H20+I20)/2&gt;=60,3.5,IF((H20+I20)/2&gt;=50,3,IF((H20+I20)/2&gt;=40,2,IF((H20+I20)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI20">
-        <f>IF(N20+O20&gt;=80,5,IF(N20+O20&gt;=70,4,IF(N20+O20&gt;=60,3.5,IF(N20+O20&gt;=50,3,IF(N20+O20&gt;=40,2,IF(N20+O20&gt;=33,1,0))))))</f>
+        <f>IF(AA20,0,IF((J20+K20+L20+M20)/2&gt;=80,5,IF((J20+K20+L20+M20)/2&gt;=70,4,IF((J20+K20+L20+M20)/2&gt;=60,3.5,IF((J20+K20+L20+M20)/2&gt;=50,3,IF((J20+K20+L20+M20)/2&gt;=40,2,IF((J20+K20+L20+M20)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ20">
-        <f>IF(P20+Q20&gt;=80,5,IF(P20+Q20&gt;=70,4,IF(P20+Q20&gt;=60,3.5,IF(P20+Q20&gt;=50,3,IF(P20+Q20&gt;=40,2,IF(P20+Q20&gt;=33,1,0))))))</f>
+        <f>IF(AB20,0,IF(N20+O20&gt;=80,5,IF(N20+O20&gt;=70,4,IF(N20+O20&gt;=60,3.5,IF(N20+O20&gt;=50,3,IF(N20+O20&gt;=40,2,IF(N20+O20&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK20">
-        <f>IF(R20*2&gt;=80,5,IF(R20*2&gt;=70,4,IF(R20*2&gt;=60,3.5,IF(R20*2&gt;=50,3,IF(R20*2&gt;=40,2,IF(R20*2&gt;=33,1,0))))))</f>
+        <f>IF(AC20,0,IF(P20+Q20&gt;=80,5,IF(P20+Q20&gt;=70,4,IF(P20+Q20&gt;=60,3.5,IF(P20+Q20&gt;=50,3,IF(P20+Q20&gt;=40,2,IF(P20+Q20&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL20">
-        <f>IF(S20&gt;=80,5,IF(S20&gt;=70,4,IF(S20&gt;=60,3.5,IF(S20&gt;=50,3,IF(S20&gt;=40,2,IF(S20&gt;=33,1,0))))))</f>
+        <f>IF(R20&lt;8.25,0,IF(R20*2&gt;=80,5,IF(R20*2&gt;=70,4,IF(R20*2&gt;=60,3.5,IF(R20*2&gt;=50,3,IF(R20*2&gt;=40,2,IF(R20*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM20">
-        <f>(AD20+AE20+AF20+AG20+AH20+AI20+AJ20+AK20)/8</f>
+        <f>IF(S20&lt;33,0,IF(S20&gt;=80,5,IF(S20&gt;=70,4,IF(S20&gt;=60,3.5,IF(S20&gt;=50,3,IF(S20&gt;=40,2,IF(S20&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN20">
-        <f>IF(AL20&gt;=2,(AL20-2)/8,0)</f>
+        <f>(AE20+AF20+AG20+AH20+AI20+AJ20+AK20+AL20)/8</f>
+        <v/>
+      </c>
+      <c r="AO20">
+        <f>IF(AM20&gt;=2,(AM20-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3733,71 +3816,75 @@
         <v/>
       </c>
       <c r="X21" s="7">
-        <f>IF(AC21,0,MIN(5,ROUND(AM21+AN21,2)))</f>
-        <v/>
-      </c>
-      <c r="Y21" s="8">
-        <f>IF(X21&gt;=5,"A+",IF(X21&gt;=4,"A",IF(X21&gt;=3.5,"A-",IF(X21&gt;=3,"B",IF(X21&gt;=2,"C",IF(X21&gt;=1,"D","F"))))))</f>
-        <v/>
-      </c>
-      <c r="Z21">
+        <f>IF(AD21,0,ROUND(AN21,2))</f>
+        <v/>
+      </c>
+      <c r="Y21" s="7">
+        <f>IF(AD21,0,MIN(5,ROUND(AN21+AO21,2)))</f>
+        <v/>
+      </c>
+      <c r="Z21" s="8">
+        <f>IF(Y21&gt;=5,"A+",IF(Y21&gt;=4,"A",IF(Y21&gt;=3.5,"A-",IF(Y21&gt;=3,"B",IF(Y21&gt;=2,"C",IF(Y21&gt;=1,"D","F"))))))</f>
+        <v/>
+      </c>
+      <c r="AA21">
         <f>NOT(OR(AND(J21&gt;=10,K21&gt;=23,L21&gt;=10,M21&gt;=23),AND(J21+L21&gt;=20,K21+M21&gt;=46)))</f>
         <v/>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <f>OR(N21&lt;10,O21&lt;23)</f>
         <v/>
       </c>
-      <c r="AB21">
+      <c r="AC21">
         <f>OR(P21&lt;10,Q21&lt;23)</f>
         <v/>
       </c>
-      <c r="AC21">
-        <f>OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,Z21,AA21,AB21,R21&lt;8.25,T21&lt;33,U21&lt;33)</f>
-        <v/>
-      </c>
       <c r="AD21">
-        <f>IF((C21+D21)/2&gt;=80,5,IF((C21+D21)/2&gt;=70,4,IF((C21+D21)/2&gt;=60,3.5,IF((C21+D21)/2&gt;=50,3,IF((C21+D21)/2&gt;=40,2,IF((C21+D21)/2&gt;=33,1,0))))))</f>
+        <f>OR((C21+D21)&lt;66,(E21+F21)&lt;66,G21&lt;33,(H21+I21)&lt;66,AA21,AB21,AC21,R21&lt;8.25,T21&lt;33,U21&lt;33)</f>
         <v/>
       </c>
       <c r="AE21">
-        <f>IF((E21+F21)/2&gt;=80,5,IF((E21+F21)/2&gt;=70,4,IF((E21+F21)/2&gt;=60,3.5,IF((E21+F21)/2&gt;=50,3,IF((E21+F21)/2&gt;=40,2,IF((E21+F21)/2&gt;=33,1,0))))))</f>
+        <f>IF(C21+D21&lt;66,0,IF((C21+D21)/2&gt;=80,5,IF((C21+D21)/2&gt;=70,4,IF((C21+D21)/2&gt;=60,3.5,IF((C21+D21)/2&gt;=50,3,IF((C21+D21)/2&gt;=40,2,IF((C21+D21)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AF21">
-        <f>IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0))))))</f>
+        <f>IF(E21+F21&lt;66,0,IF((E21+F21)/2&gt;=80,5,IF((E21+F21)/2&gt;=70,4,IF((E21+F21)/2&gt;=60,3.5,IF((E21+F21)/2&gt;=50,3,IF((E21+F21)/2&gt;=40,2,IF((E21+F21)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AG21">
-        <f>IF((H21+I21)/2&gt;=80,5,IF((H21+I21)/2&gt;=70,4,IF((H21+I21)/2&gt;=60,3.5,IF((H21+I21)/2&gt;=50,3,IF((H21+I21)/2&gt;=40,2,IF((H21+I21)/2&gt;=33,1,0))))))</f>
+        <f>IF(G21&lt;33,0,IF(G21&gt;=80,5,IF(G21&gt;=70,4,IF(G21&gt;=60,3.5,IF(G21&gt;=50,3,IF(G21&gt;=40,2,IF(G21&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AH21">
-        <f>IF((J21+K21+L21+M21)/2&gt;=80,5,IF((J21+K21+L21+M21)/2&gt;=70,4,IF((J21+K21+L21+M21)/2&gt;=60,3.5,IF((J21+K21+L21+M21)/2&gt;=50,3,IF((J21+K21+L21+M21)/2&gt;=40,2,IF((J21+K21+L21+M21)/2&gt;=33,1,0))))))</f>
+        <f>IF(H21+I21&lt;66,0,IF((H21+I21)/2&gt;=80,5,IF((H21+I21)/2&gt;=70,4,IF((H21+I21)/2&gt;=60,3.5,IF((H21+I21)/2&gt;=50,3,IF((H21+I21)/2&gt;=40,2,IF((H21+I21)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AI21">
-        <f>IF(N21+O21&gt;=80,5,IF(N21+O21&gt;=70,4,IF(N21+O21&gt;=60,3.5,IF(N21+O21&gt;=50,3,IF(N21+O21&gt;=40,2,IF(N21+O21&gt;=33,1,0))))))</f>
+        <f>IF(AA21,0,IF((J21+K21+L21+M21)/2&gt;=80,5,IF((J21+K21+L21+M21)/2&gt;=70,4,IF((J21+K21+L21+M21)/2&gt;=60,3.5,IF((J21+K21+L21+M21)/2&gt;=50,3,IF((J21+K21+L21+M21)/2&gt;=40,2,IF((J21+K21+L21+M21)/2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AJ21">
-        <f>IF(P21+Q21&gt;=80,5,IF(P21+Q21&gt;=70,4,IF(P21+Q21&gt;=60,3.5,IF(P21+Q21&gt;=50,3,IF(P21+Q21&gt;=40,2,IF(P21+Q21&gt;=33,1,0))))))</f>
+        <f>IF(AB21,0,IF(N21+O21&gt;=80,5,IF(N21+O21&gt;=70,4,IF(N21+O21&gt;=60,3.5,IF(N21+O21&gt;=50,3,IF(N21+O21&gt;=40,2,IF(N21+O21&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AK21">
-        <f>IF(R21*2&gt;=80,5,IF(R21*2&gt;=70,4,IF(R21*2&gt;=60,3.5,IF(R21*2&gt;=50,3,IF(R21*2&gt;=40,2,IF(R21*2&gt;=33,1,0))))))</f>
+        <f>IF(AC21,0,IF(P21+Q21&gt;=80,5,IF(P21+Q21&gt;=70,4,IF(P21+Q21&gt;=60,3.5,IF(P21+Q21&gt;=50,3,IF(P21+Q21&gt;=40,2,IF(P21+Q21&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AL21">
-        <f>IF(S21&gt;=80,5,IF(S21&gt;=70,4,IF(S21&gt;=60,3.5,IF(S21&gt;=50,3,IF(S21&gt;=40,2,IF(S21&gt;=33,1,0))))))</f>
+        <f>IF(R21&lt;8.25,0,IF(R21*2&gt;=80,5,IF(R21*2&gt;=70,4,IF(R21*2&gt;=60,3.5,IF(R21*2&gt;=50,3,IF(R21*2&gt;=40,2,IF(R21*2&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AM21">
-        <f>(AD21+AE21+AF21+AG21+AH21+AI21+AJ21+AK21)/8</f>
+        <f>IF(S21&lt;33,0,IF(S21&gt;=80,5,IF(S21&gt;=70,4,IF(S21&gt;=60,3.5,IF(S21&gt;=50,3,IF(S21&gt;=40,2,IF(S21&gt;=33,1,0)))))))</f>
         <v/>
       </c>
       <c r="AN21">
-        <f>IF(AL21&gt;=2,(AL21-2)/8,0)</f>
+        <f>(AE21+AF21+AG21+AH21+AI21+AJ21+AK21+AL21)/8</f>
+        <v/>
+      </c>
+      <c r="AO21">
+        <f>IF(AM21&gt;=2,(AM21-2)/8,0)</f>
         <v/>
       </c>
     </row>
@@ -3858,7 +3945,7 @@
         </is>
       </c>
       <c r="F5" s="13">
-        <f>IFERROR(ROUND(AVERAGE('Data Source'!X:X),2), 0)</f>
+        <f>IFERROR(ROUND(AVERAGE('Data Source'!Y:Y),2), 0)</f>
         <v/>
       </c>
       <c r="H5" s="11" t="inlineStr">
@@ -3876,7 +3963,7 @@
         </is>
       </c>
       <c r="L5" s="14">
-        <f>IF(C5&gt;0,COUNTIF('Data Source'!X:X,"&gt;0")/C5,0)</f>
+        <f>IF(C5&gt;0,COUNTIF('Data Source'!Y:Y,"&gt;0")/C5,0)</f>
         <v/>
       </c>
     </row>
@@ -3946,7 +4033,7 @@
         </is>
       </c>
       <c r="B9" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"A+")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"A+")</f>
         <v/>
       </c>
       <c r="D9" t="inlineStr">
@@ -3970,7 +4057,7 @@
         <v/>
       </c>
       <c r="I9" s="7">
-        <f>'Data Source'!T11</f>
+        <f>'Data Source'!Y11</f>
         <v/>
       </c>
     </row>
@@ -3981,7 +4068,7 @@
         </is>
       </c>
       <c r="B10" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"A")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"A")</f>
         <v/>
       </c>
       <c r="D10" t="inlineStr">
@@ -4005,7 +4092,7 @@
         <v/>
       </c>
       <c r="I10" s="7">
-        <f>'Data Source'!T21</f>
+        <f>'Data Source'!Y21</f>
         <v/>
       </c>
     </row>
@@ -4016,7 +4103,7 @@
         </is>
       </c>
       <c r="B11" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"A-")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"A-")</f>
         <v/>
       </c>
       <c r="D11" t="inlineStr">
@@ -4040,7 +4127,7 @@
         <v/>
       </c>
       <c r="I11" s="7">
-        <f>'Data Source'!T10</f>
+        <f>'Data Source'!Y10</f>
         <v/>
       </c>
     </row>
@@ -4051,7 +4138,7 @@
         </is>
       </c>
       <c r="B12" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"B")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"B")</f>
         <v/>
       </c>
       <c r="D12" t="inlineStr">
@@ -4075,7 +4162,7 @@
         <v/>
       </c>
       <c r="I12" s="7">
-        <f>'Data Source'!T15</f>
+        <f>'Data Source'!Y15</f>
         <v/>
       </c>
     </row>
@@ -4086,7 +4173,7 @@
         </is>
       </c>
       <c r="B13" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"C")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"C")</f>
         <v/>
       </c>
       <c r="D13" t="inlineStr">
@@ -4110,7 +4197,7 @@
         <v/>
       </c>
       <c r="I13" s="7">
-        <f>'Data Source'!T7</f>
+        <f>'Data Source'!Y7</f>
         <v/>
       </c>
     </row>
@@ -4121,7 +4208,7 @@
         </is>
       </c>
       <c r="B14" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"D")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"D")</f>
         <v/>
       </c>
       <c r="D14" t="inlineStr">
@@ -4145,7 +4232,7 @@
         </is>
       </c>
       <c r="B15" s="8">
-        <f>COUNTIF('Data Source'!Y:Y,"F")</f>
+        <f>COUNTIF('Data Source'!Z:Z,"F")</f>
         <v/>
       </c>
       <c r="D15" t="inlineStr">
@@ -4326,39 +4413,39 @@
         <v/>
       </c>
       <c r="C3" s="8">
-        <f>IF('Data Source'!AD2&gt;=5,"A+",IF('Data Source'!AD2&gt;=4,"A",IF('Data Source'!AD2&gt;=3.5,"A-",IF('Data Source'!AD2&gt;=3,"B",IF('Data Source'!AD2&gt;=2,"C",IF('Data Source'!AD2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE2&gt;=5,"A+",IF('Data Source'!AE2&gt;=4,"A",IF('Data Source'!AE2&gt;=3.5,"A-",IF('Data Source'!AE2&gt;=3,"B",IF('Data Source'!AE2&gt;=2,"C",IF('Data Source'!AE2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D3" s="8">
-        <f>IF('Data Source'!AE2&gt;=5,"A+",IF('Data Source'!AE2&gt;=4,"A",IF('Data Source'!AE2&gt;=3.5,"A-",IF('Data Source'!AE2&gt;=3,"B",IF('Data Source'!AE2&gt;=2,"C",IF('Data Source'!AE2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF2&gt;=5,"A+",IF('Data Source'!AF2&gt;=4,"A",IF('Data Source'!AF2&gt;=3.5,"A-",IF('Data Source'!AF2&gt;=3,"B",IF('Data Source'!AF2&gt;=2,"C",IF('Data Source'!AF2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E3" s="8">
-        <f>IF('Data Source'!AF2&gt;=5,"A+",IF('Data Source'!AF2&gt;=4,"A",IF('Data Source'!AF2&gt;=3.5,"A-",IF('Data Source'!AF2&gt;=3,"B",IF('Data Source'!AF2&gt;=2,"C",IF('Data Source'!AF2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG2&gt;=5,"A+",IF('Data Source'!AG2&gt;=4,"A",IF('Data Source'!AG2&gt;=3.5,"A-",IF('Data Source'!AG2&gt;=3,"B",IF('Data Source'!AG2&gt;=2,"C",IF('Data Source'!AG2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F3" s="8">
-        <f>IF('Data Source'!AG2&gt;=5,"A+",IF('Data Source'!AG2&gt;=4,"A",IF('Data Source'!AG2&gt;=3.5,"A-",IF('Data Source'!AG2&gt;=3,"B",IF('Data Source'!AG2&gt;=2,"C",IF('Data Source'!AG2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH2&gt;=5,"A+",IF('Data Source'!AH2&gt;=4,"A",IF('Data Source'!AH2&gt;=3.5,"A-",IF('Data Source'!AH2&gt;=3,"B",IF('Data Source'!AH2&gt;=2,"C",IF('Data Source'!AH2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G3" s="8">
-        <f>IF('Data Source'!AH2&gt;=5,"A+",IF('Data Source'!AH2&gt;=4,"A",IF('Data Source'!AH2&gt;=3.5,"A-",IF('Data Source'!AH2&gt;=3,"B",IF('Data Source'!AH2&gt;=2,"C",IF('Data Source'!AH2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI2&gt;=5,"A+",IF('Data Source'!AI2&gt;=4,"A",IF('Data Source'!AI2&gt;=3.5,"A-",IF('Data Source'!AI2&gt;=3,"B",IF('Data Source'!AI2&gt;=2,"C",IF('Data Source'!AI2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H3" s="8">
-        <f>IF('Data Source'!AI2&gt;=5,"A+",IF('Data Source'!AI2&gt;=4,"A",IF('Data Source'!AI2&gt;=3.5,"A-",IF('Data Source'!AI2&gt;=3,"B",IF('Data Source'!AI2&gt;=2,"C",IF('Data Source'!AI2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ2&gt;=5,"A+",IF('Data Source'!AJ2&gt;=4,"A",IF('Data Source'!AJ2&gt;=3.5,"A-",IF('Data Source'!AJ2&gt;=3,"B",IF('Data Source'!AJ2&gt;=2,"C",IF('Data Source'!AJ2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I3" s="8">
-        <f>IF('Data Source'!AJ2&gt;=5,"A+",IF('Data Source'!AJ2&gt;=4,"A",IF('Data Source'!AJ2&gt;=3.5,"A-",IF('Data Source'!AJ2&gt;=3,"B",IF('Data Source'!AJ2&gt;=2,"C",IF('Data Source'!AJ2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK2&gt;=5,"A+",IF('Data Source'!AK2&gt;=4,"A",IF('Data Source'!AK2&gt;=3.5,"A-",IF('Data Source'!AK2&gt;=3,"B",IF('Data Source'!AK2&gt;=2,"C",IF('Data Source'!AK2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J3" s="8">
-        <f>IF('Data Source'!AK2&gt;=5,"A+",IF('Data Source'!AK2&gt;=4,"A",IF('Data Source'!AK2&gt;=3.5,"A-",IF('Data Source'!AK2&gt;=3,"B",IF('Data Source'!AK2&gt;=2,"C",IF('Data Source'!AK2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL2&gt;=5,"A+",IF('Data Source'!AL2&gt;=4,"A",IF('Data Source'!AL2&gt;=3.5,"A-",IF('Data Source'!AL2&gt;=3,"B",IF('Data Source'!AL2&gt;=2,"C",IF('Data Source'!AL2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K3" s="8">
-        <f>IF('Data Source'!AL2&gt;=5,"A+",IF('Data Source'!AL2&gt;=4,"A",IF('Data Source'!AL2&gt;=3.5,"A-",IF('Data Source'!AL2&gt;=3,"B",IF('Data Source'!AL2&gt;=2,"C",IF('Data Source'!AL2&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM2&gt;=5,"A+",IF('Data Source'!AM2&gt;=4,"A",IF('Data Source'!AM2&gt;=3.5,"A-",IF('Data Source'!AM2&gt;=3,"B",IF('Data Source'!AM2&gt;=2,"C",IF('Data Source'!AM2&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L3" s="8">
@@ -4370,11 +4457,11 @@
         <v/>
       </c>
       <c r="N3" s="7">
-        <f>'Data Source'!X2</f>
+        <f>'Data Source'!Y2</f>
         <v/>
       </c>
       <c r="O3" s="8">
-        <f>'Data Source'!Y2</f>
+        <f>'Data Source'!Z2</f>
         <v/>
       </c>
     </row>
@@ -4388,39 +4475,39 @@
         <v/>
       </c>
       <c r="C4" s="8">
-        <f>IF('Data Source'!AD3&gt;=5,"A+",IF('Data Source'!AD3&gt;=4,"A",IF('Data Source'!AD3&gt;=3.5,"A-",IF('Data Source'!AD3&gt;=3,"B",IF('Data Source'!AD3&gt;=2,"C",IF('Data Source'!AD3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE3&gt;=5,"A+",IF('Data Source'!AE3&gt;=4,"A",IF('Data Source'!AE3&gt;=3.5,"A-",IF('Data Source'!AE3&gt;=3,"B",IF('Data Source'!AE3&gt;=2,"C",IF('Data Source'!AE3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D4" s="8">
-        <f>IF('Data Source'!AE3&gt;=5,"A+",IF('Data Source'!AE3&gt;=4,"A",IF('Data Source'!AE3&gt;=3.5,"A-",IF('Data Source'!AE3&gt;=3,"B",IF('Data Source'!AE3&gt;=2,"C",IF('Data Source'!AE3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF3&gt;=5,"A+",IF('Data Source'!AF3&gt;=4,"A",IF('Data Source'!AF3&gt;=3.5,"A-",IF('Data Source'!AF3&gt;=3,"B",IF('Data Source'!AF3&gt;=2,"C",IF('Data Source'!AF3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E4" s="8">
-        <f>IF('Data Source'!AF3&gt;=5,"A+",IF('Data Source'!AF3&gt;=4,"A",IF('Data Source'!AF3&gt;=3.5,"A-",IF('Data Source'!AF3&gt;=3,"B",IF('Data Source'!AF3&gt;=2,"C",IF('Data Source'!AF3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG3&gt;=5,"A+",IF('Data Source'!AG3&gt;=4,"A",IF('Data Source'!AG3&gt;=3.5,"A-",IF('Data Source'!AG3&gt;=3,"B",IF('Data Source'!AG3&gt;=2,"C",IF('Data Source'!AG3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F4" s="8">
-        <f>IF('Data Source'!AG3&gt;=5,"A+",IF('Data Source'!AG3&gt;=4,"A",IF('Data Source'!AG3&gt;=3.5,"A-",IF('Data Source'!AG3&gt;=3,"B",IF('Data Source'!AG3&gt;=2,"C",IF('Data Source'!AG3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH3&gt;=5,"A+",IF('Data Source'!AH3&gt;=4,"A",IF('Data Source'!AH3&gt;=3.5,"A-",IF('Data Source'!AH3&gt;=3,"B",IF('Data Source'!AH3&gt;=2,"C",IF('Data Source'!AH3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G4" s="8">
-        <f>IF('Data Source'!AH3&gt;=5,"A+",IF('Data Source'!AH3&gt;=4,"A",IF('Data Source'!AH3&gt;=3.5,"A-",IF('Data Source'!AH3&gt;=3,"B",IF('Data Source'!AH3&gt;=2,"C",IF('Data Source'!AH3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI3&gt;=5,"A+",IF('Data Source'!AI3&gt;=4,"A",IF('Data Source'!AI3&gt;=3.5,"A-",IF('Data Source'!AI3&gt;=3,"B",IF('Data Source'!AI3&gt;=2,"C",IF('Data Source'!AI3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H4" s="8">
-        <f>IF('Data Source'!AI3&gt;=5,"A+",IF('Data Source'!AI3&gt;=4,"A",IF('Data Source'!AI3&gt;=3.5,"A-",IF('Data Source'!AI3&gt;=3,"B",IF('Data Source'!AI3&gt;=2,"C",IF('Data Source'!AI3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ3&gt;=5,"A+",IF('Data Source'!AJ3&gt;=4,"A",IF('Data Source'!AJ3&gt;=3.5,"A-",IF('Data Source'!AJ3&gt;=3,"B",IF('Data Source'!AJ3&gt;=2,"C",IF('Data Source'!AJ3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I4" s="8">
-        <f>IF('Data Source'!AJ3&gt;=5,"A+",IF('Data Source'!AJ3&gt;=4,"A",IF('Data Source'!AJ3&gt;=3.5,"A-",IF('Data Source'!AJ3&gt;=3,"B",IF('Data Source'!AJ3&gt;=2,"C",IF('Data Source'!AJ3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK3&gt;=5,"A+",IF('Data Source'!AK3&gt;=4,"A",IF('Data Source'!AK3&gt;=3.5,"A-",IF('Data Source'!AK3&gt;=3,"B",IF('Data Source'!AK3&gt;=2,"C",IF('Data Source'!AK3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J4" s="8">
-        <f>IF('Data Source'!AK3&gt;=5,"A+",IF('Data Source'!AK3&gt;=4,"A",IF('Data Source'!AK3&gt;=3.5,"A-",IF('Data Source'!AK3&gt;=3,"B",IF('Data Source'!AK3&gt;=2,"C",IF('Data Source'!AK3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL3&gt;=5,"A+",IF('Data Source'!AL3&gt;=4,"A",IF('Data Source'!AL3&gt;=3.5,"A-",IF('Data Source'!AL3&gt;=3,"B",IF('Data Source'!AL3&gt;=2,"C",IF('Data Source'!AL3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K4" s="8">
-        <f>IF('Data Source'!AL3&gt;=5,"A+",IF('Data Source'!AL3&gt;=4,"A",IF('Data Source'!AL3&gt;=3.5,"A-",IF('Data Source'!AL3&gt;=3,"B",IF('Data Source'!AL3&gt;=2,"C",IF('Data Source'!AL3&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM3&gt;=5,"A+",IF('Data Source'!AM3&gt;=4,"A",IF('Data Source'!AM3&gt;=3.5,"A-",IF('Data Source'!AM3&gt;=3,"B",IF('Data Source'!AM3&gt;=2,"C",IF('Data Source'!AM3&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L4" s="8">
@@ -4432,11 +4519,11 @@
         <v/>
       </c>
       <c r="N4" s="7">
-        <f>'Data Source'!X3</f>
+        <f>'Data Source'!Y3</f>
         <v/>
       </c>
       <c r="O4" s="8">
-        <f>'Data Source'!Y3</f>
+        <f>'Data Source'!Z3</f>
         <v/>
       </c>
     </row>
@@ -4450,39 +4537,39 @@
         <v/>
       </c>
       <c r="C5" s="8">
-        <f>IF('Data Source'!AD4&gt;=5,"A+",IF('Data Source'!AD4&gt;=4,"A",IF('Data Source'!AD4&gt;=3.5,"A-",IF('Data Source'!AD4&gt;=3,"B",IF('Data Source'!AD4&gt;=2,"C",IF('Data Source'!AD4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE4&gt;=5,"A+",IF('Data Source'!AE4&gt;=4,"A",IF('Data Source'!AE4&gt;=3.5,"A-",IF('Data Source'!AE4&gt;=3,"B",IF('Data Source'!AE4&gt;=2,"C",IF('Data Source'!AE4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D5" s="8">
-        <f>IF('Data Source'!AE4&gt;=5,"A+",IF('Data Source'!AE4&gt;=4,"A",IF('Data Source'!AE4&gt;=3.5,"A-",IF('Data Source'!AE4&gt;=3,"B",IF('Data Source'!AE4&gt;=2,"C",IF('Data Source'!AE4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF4&gt;=5,"A+",IF('Data Source'!AF4&gt;=4,"A",IF('Data Source'!AF4&gt;=3.5,"A-",IF('Data Source'!AF4&gt;=3,"B",IF('Data Source'!AF4&gt;=2,"C",IF('Data Source'!AF4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E5" s="8">
-        <f>IF('Data Source'!AF4&gt;=5,"A+",IF('Data Source'!AF4&gt;=4,"A",IF('Data Source'!AF4&gt;=3.5,"A-",IF('Data Source'!AF4&gt;=3,"B",IF('Data Source'!AF4&gt;=2,"C",IF('Data Source'!AF4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG4&gt;=5,"A+",IF('Data Source'!AG4&gt;=4,"A",IF('Data Source'!AG4&gt;=3.5,"A-",IF('Data Source'!AG4&gt;=3,"B",IF('Data Source'!AG4&gt;=2,"C",IF('Data Source'!AG4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F5" s="8">
-        <f>IF('Data Source'!AG4&gt;=5,"A+",IF('Data Source'!AG4&gt;=4,"A",IF('Data Source'!AG4&gt;=3.5,"A-",IF('Data Source'!AG4&gt;=3,"B",IF('Data Source'!AG4&gt;=2,"C",IF('Data Source'!AG4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH4&gt;=5,"A+",IF('Data Source'!AH4&gt;=4,"A",IF('Data Source'!AH4&gt;=3.5,"A-",IF('Data Source'!AH4&gt;=3,"B",IF('Data Source'!AH4&gt;=2,"C",IF('Data Source'!AH4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G5" s="8">
-        <f>IF('Data Source'!AH4&gt;=5,"A+",IF('Data Source'!AH4&gt;=4,"A",IF('Data Source'!AH4&gt;=3.5,"A-",IF('Data Source'!AH4&gt;=3,"B",IF('Data Source'!AH4&gt;=2,"C",IF('Data Source'!AH4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI4&gt;=5,"A+",IF('Data Source'!AI4&gt;=4,"A",IF('Data Source'!AI4&gt;=3.5,"A-",IF('Data Source'!AI4&gt;=3,"B",IF('Data Source'!AI4&gt;=2,"C",IF('Data Source'!AI4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H5" s="8">
-        <f>IF('Data Source'!AI4&gt;=5,"A+",IF('Data Source'!AI4&gt;=4,"A",IF('Data Source'!AI4&gt;=3.5,"A-",IF('Data Source'!AI4&gt;=3,"B",IF('Data Source'!AI4&gt;=2,"C",IF('Data Source'!AI4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ4&gt;=5,"A+",IF('Data Source'!AJ4&gt;=4,"A",IF('Data Source'!AJ4&gt;=3.5,"A-",IF('Data Source'!AJ4&gt;=3,"B",IF('Data Source'!AJ4&gt;=2,"C",IF('Data Source'!AJ4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I5" s="8">
-        <f>IF('Data Source'!AJ4&gt;=5,"A+",IF('Data Source'!AJ4&gt;=4,"A",IF('Data Source'!AJ4&gt;=3.5,"A-",IF('Data Source'!AJ4&gt;=3,"B",IF('Data Source'!AJ4&gt;=2,"C",IF('Data Source'!AJ4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK4&gt;=5,"A+",IF('Data Source'!AK4&gt;=4,"A",IF('Data Source'!AK4&gt;=3.5,"A-",IF('Data Source'!AK4&gt;=3,"B",IF('Data Source'!AK4&gt;=2,"C",IF('Data Source'!AK4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J5" s="8">
-        <f>IF('Data Source'!AK4&gt;=5,"A+",IF('Data Source'!AK4&gt;=4,"A",IF('Data Source'!AK4&gt;=3.5,"A-",IF('Data Source'!AK4&gt;=3,"B",IF('Data Source'!AK4&gt;=2,"C",IF('Data Source'!AK4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL4&gt;=5,"A+",IF('Data Source'!AL4&gt;=4,"A",IF('Data Source'!AL4&gt;=3.5,"A-",IF('Data Source'!AL4&gt;=3,"B",IF('Data Source'!AL4&gt;=2,"C",IF('Data Source'!AL4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K5" s="8">
-        <f>IF('Data Source'!AL4&gt;=5,"A+",IF('Data Source'!AL4&gt;=4,"A",IF('Data Source'!AL4&gt;=3.5,"A-",IF('Data Source'!AL4&gt;=3,"B",IF('Data Source'!AL4&gt;=2,"C",IF('Data Source'!AL4&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM4&gt;=5,"A+",IF('Data Source'!AM4&gt;=4,"A",IF('Data Source'!AM4&gt;=3.5,"A-",IF('Data Source'!AM4&gt;=3,"B",IF('Data Source'!AM4&gt;=2,"C",IF('Data Source'!AM4&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L5" s="8">
@@ -4494,11 +4581,11 @@
         <v/>
       </c>
       <c r="N5" s="7">
-        <f>'Data Source'!X4</f>
+        <f>'Data Source'!Y4</f>
         <v/>
       </c>
       <c r="O5" s="8">
-        <f>'Data Source'!Y4</f>
+        <f>'Data Source'!Z4</f>
         <v/>
       </c>
     </row>
@@ -4512,39 +4599,39 @@
         <v/>
       </c>
       <c r="C6" s="8">
-        <f>IF('Data Source'!AD5&gt;=5,"A+",IF('Data Source'!AD5&gt;=4,"A",IF('Data Source'!AD5&gt;=3.5,"A-",IF('Data Source'!AD5&gt;=3,"B",IF('Data Source'!AD5&gt;=2,"C",IF('Data Source'!AD5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE5&gt;=5,"A+",IF('Data Source'!AE5&gt;=4,"A",IF('Data Source'!AE5&gt;=3.5,"A-",IF('Data Source'!AE5&gt;=3,"B",IF('Data Source'!AE5&gt;=2,"C",IF('Data Source'!AE5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D6" s="8">
-        <f>IF('Data Source'!AE5&gt;=5,"A+",IF('Data Source'!AE5&gt;=4,"A",IF('Data Source'!AE5&gt;=3.5,"A-",IF('Data Source'!AE5&gt;=3,"B",IF('Data Source'!AE5&gt;=2,"C",IF('Data Source'!AE5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF5&gt;=5,"A+",IF('Data Source'!AF5&gt;=4,"A",IF('Data Source'!AF5&gt;=3.5,"A-",IF('Data Source'!AF5&gt;=3,"B",IF('Data Source'!AF5&gt;=2,"C",IF('Data Source'!AF5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E6" s="8">
-        <f>IF('Data Source'!AF5&gt;=5,"A+",IF('Data Source'!AF5&gt;=4,"A",IF('Data Source'!AF5&gt;=3.5,"A-",IF('Data Source'!AF5&gt;=3,"B",IF('Data Source'!AF5&gt;=2,"C",IF('Data Source'!AF5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG5&gt;=5,"A+",IF('Data Source'!AG5&gt;=4,"A",IF('Data Source'!AG5&gt;=3.5,"A-",IF('Data Source'!AG5&gt;=3,"B",IF('Data Source'!AG5&gt;=2,"C",IF('Data Source'!AG5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F6" s="8">
-        <f>IF('Data Source'!AG5&gt;=5,"A+",IF('Data Source'!AG5&gt;=4,"A",IF('Data Source'!AG5&gt;=3.5,"A-",IF('Data Source'!AG5&gt;=3,"B",IF('Data Source'!AG5&gt;=2,"C",IF('Data Source'!AG5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH5&gt;=5,"A+",IF('Data Source'!AH5&gt;=4,"A",IF('Data Source'!AH5&gt;=3.5,"A-",IF('Data Source'!AH5&gt;=3,"B",IF('Data Source'!AH5&gt;=2,"C",IF('Data Source'!AH5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G6" s="8">
-        <f>IF('Data Source'!AH5&gt;=5,"A+",IF('Data Source'!AH5&gt;=4,"A",IF('Data Source'!AH5&gt;=3.5,"A-",IF('Data Source'!AH5&gt;=3,"B",IF('Data Source'!AH5&gt;=2,"C",IF('Data Source'!AH5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI5&gt;=5,"A+",IF('Data Source'!AI5&gt;=4,"A",IF('Data Source'!AI5&gt;=3.5,"A-",IF('Data Source'!AI5&gt;=3,"B",IF('Data Source'!AI5&gt;=2,"C",IF('Data Source'!AI5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H6" s="8">
-        <f>IF('Data Source'!AI5&gt;=5,"A+",IF('Data Source'!AI5&gt;=4,"A",IF('Data Source'!AI5&gt;=3.5,"A-",IF('Data Source'!AI5&gt;=3,"B",IF('Data Source'!AI5&gt;=2,"C",IF('Data Source'!AI5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ5&gt;=5,"A+",IF('Data Source'!AJ5&gt;=4,"A",IF('Data Source'!AJ5&gt;=3.5,"A-",IF('Data Source'!AJ5&gt;=3,"B",IF('Data Source'!AJ5&gt;=2,"C",IF('Data Source'!AJ5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I6" s="8">
-        <f>IF('Data Source'!AJ5&gt;=5,"A+",IF('Data Source'!AJ5&gt;=4,"A",IF('Data Source'!AJ5&gt;=3.5,"A-",IF('Data Source'!AJ5&gt;=3,"B",IF('Data Source'!AJ5&gt;=2,"C",IF('Data Source'!AJ5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK5&gt;=5,"A+",IF('Data Source'!AK5&gt;=4,"A",IF('Data Source'!AK5&gt;=3.5,"A-",IF('Data Source'!AK5&gt;=3,"B",IF('Data Source'!AK5&gt;=2,"C",IF('Data Source'!AK5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J6" s="8">
-        <f>IF('Data Source'!AK5&gt;=5,"A+",IF('Data Source'!AK5&gt;=4,"A",IF('Data Source'!AK5&gt;=3.5,"A-",IF('Data Source'!AK5&gt;=3,"B",IF('Data Source'!AK5&gt;=2,"C",IF('Data Source'!AK5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL5&gt;=5,"A+",IF('Data Source'!AL5&gt;=4,"A",IF('Data Source'!AL5&gt;=3.5,"A-",IF('Data Source'!AL5&gt;=3,"B",IF('Data Source'!AL5&gt;=2,"C",IF('Data Source'!AL5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K6" s="8">
-        <f>IF('Data Source'!AL5&gt;=5,"A+",IF('Data Source'!AL5&gt;=4,"A",IF('Data Source'!AL5&gt;=3.5,"A-",IF('Data Source'!AL5&gt;=3,"B",IF('Data Source'!AL5&gt;=2,"C",IF('Data Source'!AL5&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM5&gt;=5,"A+",IF('Data Source'!AM5&gt;=4,"A",IF('Data Source'!AM5&gt;=3.5,"A-",IF('Data Source'!AM5&gt;=3,"B",IF('Data Source'!AM5&gt;=2,"C",IF('Data Source'!AM5&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L6" s="8">
@@ -4556,11 +4643,11 @@
         <v/>
       </c>
       <c r="N6" s="7">
-        <f>'Data Source'!X5</f>
+        <f>'Data Source'!Y5</f>
         <v/>
       </c>
       <c r="O6" s="8">
-        <f>'Data Source'!Y5</f>
+        <f>'Data Source'!Z5</f>
         <v/>
       </c>
     </row>
@@ -4574,39 +4661,39 @@
         <v/>
       </c>
       <c r="C7" s="8">
-        <f>IF('Data Source'!AD6&gt;=5,"A+",IF('Data Source'!AD6&gt;=4,"A",IF('Data Source'!AD6&gt;=3.5,"A-",IF('Data Source'!AD6&gt;=3,"B",IF('Data Source'!AD6&gt;=2,"C",IF('Data Source'!AD6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE6&gt;=5,"A+",IF('Data Source'!AE6&gt;=4,"A",IF('Data Source'!AE6&gt;=3.5,"A-",IF('Data Source'!AE6&gt;=3,"B",IF('Data Source'!AE6&gt;=2,"C",IF('Data Source'!AE6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D7" s="8">
-        <f>IF('Data Source'!AE6&gt;=5,"A+",IF('Data Source'!AE6&gt;=4,"A",IF('Data Source'!AE6&gt;=3.5,"A-",IF('Data Source'!AE6&gt;=3,"B",IF('Data Source'!AE6&gt;=2,"C",IF('Data Source'!AE6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF6&gt;=5,"A+",IF('Data Source'!AF6&gt;=4,"A",IF('Data Source'!AF6&gt;=3.5,"A-",IF('Data Source'!AF6&gt;=3,"B",IF('Data Source'!AF6&gt;=2,"C",IF('Data Source'!AF6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E7" s="8">
-        <f>IF('Data Source'!AF6&gt;=5,"A+",IF('Data Source'!AF6&gt;=4,"A",IF('Data Source'!AF6&gt;=3.5,"A-",IF('Data Source'!AF6&gt;=3,"B",IF('Data Source'!AF6&gt;=2,"C",IF('Data Source'!AF6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG6&gt;=5,"A+",IF('Data Source'!AG6&gt;=4,"A",IF('Data Source'!AG6&gt;=3.5,"A-",IF('Data Source'!AG6&gt;=3,"B",IF('Data Source'!AG6&gt;=2,"C",IF('Data Source'!AG6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F7" s="8">
-        <f>IF('Data Source'!AG6&gt;=5,"A+",IF('Data Source'!AG6&gt;=4,"A",IF('Data Source'!AG6&gt;=3.5,"A-",IF('Data Source'!AG6&gt;=3,"B",IF('Data Source'!AG6&gt;=2,"C",IF('Data Source'!AG6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH6&gt;=5,"A+",IF('Data Source'!AH6&gt;=4,"A",IF('Data Source'!AH6&gt;=3.5,"A-",IF('Data Source'!AH6&gt;=3,"B",IF('Data Source'!AH6&gt;=2,"C",IF('Data Source'!AH6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G7" s="8">
-        <f>IF('Data Source'!AH6&gt;=5,"A+",IF('Data Source'!AH6&gt;=4,"A",IF('Data Source'!AH6&gt;=3.5,"A-",IF('Data Source'!AH6&gt;=3,"B",IF('Data Source'!AH6&gt;=2,"C",IF('Data Source'!AH6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI6&gt;=5,"A+",IF('Data Source'!AI6&gt;=4,"A",IF('Data Source'!AI6&gt;=3.5,"A-",IF('Data Source'!AI6&gt;=3,"B",IF('Data Source'!AI6&gt;=2,"C",IF('Data Source'!AI6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H7" s="8">
-        <f>IF('Data Source'!AI6&gt;=5,"A+",IF('Data Source'!AI6&gt;=4,"A",IF('Data Source'!AI6&gt;=3.5,"A-",IF('Data Source'!AI6&gt;=3,"B",IF('Data Source'!AI6&gt;=2,"C",IF('Data Source'!AI6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ6&gt;=5,"A+",IF('Data Source'!AJ6&gt;=4,"A",IF('Data Source'!AJ6&gt;=3.5,"A-",IF('Data Source'!AJ6&gt;=3,"B",IF('Data Source'!AJ6&gt;=2,"C",IF('Data Source'!AJ6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I7" s="8">
-        <f>IF('Data Source'!AJ6&gt;=5,"A+",IF('Data Source'!AJ6&gt;=4,"A",IF('Data Source'!AJ6&gt;=3.5,"A-",IF('Data Source'!AJ6&gt;=3,"B",IF('Data Source'!AJ6&gt;=2,"C",IF('Data Source'!AJ6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK6&gt;=5,"A+",IF('Data Source'!AK6&gt;=4,"A",IF('Data Source'!AK6&gt;=3.5,"A-",IF('Data Source'!AK6&gt;=3,"B",IF('Data Source'!AK6&gt;=2,"C",IF('Data Source'!AK6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J7" s="8">
-        <f>IF('Data Source'!AK6&gt;=5,"A+",IF('Data Source'!AK6&gt;=4,"A",IF('Data Source'!AK6&gt;=3.5,"A-",IF('Data Source'!AK6&gt;=3,"B",IF('Data Source'!AK6&gt;=2,"C",IF('Data Source'!AK6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL6&gt;=5,"A+",IF('Data Source'!AL6&gt;=4,"A",IF('Data Source'!AL6&gt;=3.5,"A-",IF('Data Source'!AL6&gt;=3,"B",IF('Data Source'!AL6&gt;=2,"C",IF('Data Source'!AL6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K7" s="8">
-        <f>IF('Data Source'!AL6&gt;=5,"A+",IF('Data Source'!AL6&gt;=4,"A",IF('Data Source'!AL6&gt;=3.5,"A-",IF('Data Source'!AL6&gt;=3,"B",IF('Data Source'!AL6&gt;=2,"C",IF('Data Source'!AL6&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM6&gt;=5,"A+",IF('Data Source'!AM6&gt;=4,"A",IF('Data Source'!AM6&gt;=3.5,"A-",IF('Data Source'!AM6&gt;=3,"B",IF('Data Source'!AM6&gt;=2,"C",IF('Data Source'!AM6&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L7" s="8">
@@ -4618,11 +4705,11 @@
         <v/>
       </c>
       <c r="N7" s="7">
-        <f>'Data Source'!X6</f>
+        <f>'Data Source'!Y6</f>
         <v/>
       </c>
       <c r="O7" s="8">
-        <f>'Data Source'!Y6</f>
+        <f>'Data Source'!Z6</f>
         <v/>
       </c>
     </row>
@@ -4636,39 +4723,39 @@
         <v/>
       </c>
       <c r="C8" s="8">
-        <f>IF('Data Source'!AD7&gt;=5,"A+",IF('Data Source'!AD7&gt;=4,"A",IF('Data Source'!AD7&gt;=3.5,"A-",IF('Data Source'!AD7&gt;=3,"B",IF('Data Source'!AD7&gt;=2,"C",IF('Data Source'!AD7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE7&gt;=5,"A+",IF('Data Source'!AE7&gt;=4,"A",IF('Data Source'!AE7&gt;=3.5,"A-",IF('Data Source'!AE7&gt;=3,"B",IF('Data Source'!AE7&gt;=2,"C",IF('Data Source'!AE7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D8" s="8">
-        <f>IF('Data Source'!AE7&gt;=5,"A+",IF('Data Source'!AE7&gt;=4,"A",IF('Data Source'!AE7&gt;=3.5,"A-",IF('Data Source'!AE7&gt;=3,"B",IF('Data Source'!AE7&gt;=2,"C",IF('Data Source'!AE7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF7&gt;=5,"A+",IF('Data Source'!AF7&gt;=4,"A",IF('Data Source'!AF7&gt;=3.5,"A-",IF('Data Source'!AF7&gt;=3,"B",IF('Data Source'!AF7&gt;=2,"C",IF('Data Source'!AF7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E8" s="8">
-        <f>IF('Data Source'!AF7&gt;=5,"A+",IF('Data Source'!AF7&gt;=4,"A",IF('Data Source'!AF7&gt;=3.5,"A-",IF('Data Source'!AF7&gt;=3,"B",IF('Data Source'!AF7&gt;=2,"C",IF('Data Source'!AF7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG7&gt;=5,"A+",IF('Data Source'!AG7&gt;=4,"A",IF('Data Source'!AG7&gt;=3.5,"A-",IF('Data Source'!AG7&gt;=3,"B",IF('Data Source'!AG7&gt;=2,"C",IF('Data Source'!AG7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F8" s="8">
-        <f>IF('Data Source'!AG7&gt;=5,"A+",IF('Data Source'!AG7&gt;=4,"A",IF('Data Source'!AG7&gt;=3.5,"A-",IF('Data Source'!AG7&gt;=3,"B",IF('Data Source'!AG7&gt;=2,"C",IF('Data Source'!AG7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH7&gt;=5,"A+",IF('Data Source'!AH7&gt;=4,"A",IF('Data Source'!AH7&gt;=3.5,"A-",IF('Data Source'!AH7&gt;=3,"B",IF('Data Source'!AH7&gt;=2,"C",IF('Data Source'!AH7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G8" s="8">
-        <f>IF('Data Source'!AH7&gt;=5,"A+",IF('Data Source'!AH7&gt;=4,"A",IF('Data Source'!AH7&gt;=3.5,"A-",IF('Data Source'!AH7&gt;=3,"B",IF('Data Source'!AH7&gt;=2,"C",IF('Data Source'!AH7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI7&gt;=5,"A+",IF('Data Source'!AI7&gt;=4,"A",IF('Data Source'!AI7&gt;=3.5,"A-",IF('Data Source'!AI7&gt;=3,"B",IF('Data Source'!AI7&gt;=2,"C",IF('Data Source'!AI7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H8" s="8">
-        <f>IF('Data Source'!AI7&gt;=5,"A+",IF('Data Source'!AI7&gt;=4,"A",IF('Data Source'!AI7&gt;=3.5,"A-",IF('Data Source'!AI7&gt;=3,"B",IF('Data Source'!AI7&gt;=2,"C",IF('Data Source'!AI7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ7&gt;=5,"A+",IF('Data Source'!AJ7&gt;=4,"A",IF('Data Source'!AJ7&gt;=3.5,"A-",IF('Data Source'!AJ7&gt;=3,"B",IF('Data Source'!AJ7&gt;=2,"C",IF('Data Source'!AJ7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I8" s="8">
-        <f>IF('Data Source'!AJ7&gt;=5,"A+",IF('Data Source'!AJ7&gt;=4,"A",IF('Data Source'!AJ7&gt;=3.5,"A-",IF('Data Source'!AJ7&gt;=3,"B",IF('Data Source'!AJ7&gt;=2,"C",IF('Data Source'!AJ7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK7&gt;=5,"A+",IF('Data Source'!AK7&gt;=4,"A",IF('Data Source'!AK7&gt;=3.5,"A-",IF('Data Source'!AK7&gt;=3,"B",IF('Data Source'!AK7&gt;=2,"C",IF('Data Source'!AK7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J8" s="8">
-        <f>IF('Data Source'!AK7&gt;=5,"A+",IF('Data Source'!AK7&gt;=4,"A",IF('Data Source'!AK7&gt;=3.5,"A-",IF('Data Source'!AK7&gt;=3,"B",IF('Data Source'!AK7&gt;=2,"C",IF('Data Source'!AK7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL7&gt;=5,"A+",IF('Data Source'!AL7&gt;=4,"A",IF('Data Source'!AL7&gt;=3.5,"A-",IF('Data Source'!AL7&gt;=3,"B",IF('Data Source'!AL7&gt;=2,"C",IF('Data Source'!AL7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K8" s="8">
-        <f>IF('Data Source'!AL7&gt;=5,"A+",IF('Data Source'!AL7&gt;=4,"A",IF('Data Source'!AL7&gt;=3.5,"A-",IF('Data Source'!AL7&gt;=3,"B",IF('Data Source'!AL7&gt;=2,"C",IF('Data Source'!AL7&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM7&gt;=5,"A+",IF('Data Source'!AM7&gt;=4,"A",IF('Data Source'!AM7&gt;=3.5,"A-",IF('Data Source'!AM7&gt;=3,"B",IF('Data Source'!AM7&gt;=2,"C",IF('Data Source'!AM7&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L8" s="8">
@@ -4680,11 +4767,11 @@
         <v/>
       </c>
       <c r="N8" s="7">
-        <f>'Data Source'!X7</f>
+        <f>'Data Source'!Y7</f>
         <v/>
       </c>
       <c r="O8" s="8">
-        <f>'Data Source'!Y7</f>
+        <f>'Data Source'!Z7</f>
         <v/>
       </c>
     </row>
@@ -4698,39 +4785,39 @@
         <v/>
       </c>
       <c r="C9" s="8">
-        <f>IF('Data Source'!AD8&gt;=5,"A+",IF('Data Source'!AD8&gt;=4,"A",IF('Data Source'!AD8&gt;=3.5,"A-",IF('Data Source'!AD8&gt;=3,"B",IF('Data Source'!AD8&gt;=2,"C",IF('Data Source'!AD8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE8&gt;=5,"A+",IF('Data Source'!AE8&gt;=4,"A",IF('Data Source'!AE8&gt;=3.5,"A-",IF('Data Source'!AE8&gt;=3,"B",IF('Data Source'!AE8&gt;=2,"C",IF('Data Source'!AE8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D9" s="8">
-        <f>IF('Data Source'!AE8&gt;=5,"A+",IF('Data Source'!AE8&gt;=4,"A",IF('Data Source'!AE8&gt;=3.5,"A-",IF('Data Source'!AE8&gt;=3,"B",IF('Data Source'!AE8&gt;=2,"C",IF('Data Source'!AE8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF8&gt;=5,"A+",IF('Data Source'!AF8&gt;=4,"A",IF('Data Source'!AF8&gt;=3.5,"A-",IF('Data Source'!AF8&gt;=3,"B",IF('Data Source'!AF8&gt;=2,"C",IF('Data Source'!AF8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E9" s="8">
-        <f>IF('Data Source'!AF8&gt;=5,"A+",IF('Data Source'!AF8&gt;=4,"A",IF('Data Source'!AF8&gt;=3.5,"A-",IF('Data Source'!AF8&gt;=3,"B",IF('Data Source'!AF8&gt;=2,"C",IF('Data Source'!AF8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG8&gt;=5,"A+",IF('Data Source'!AG8&gt;=4,"A",IF('Data Source'!AG8&gt;=3.5,"A-",IF('Data Source'!AG8&gt;=3,"B",IF('Data Source'!AG8&gt;=2,"C",IF('Data Source'!AG8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F9" s="8">
-        <f>IF('Data Source'!AG8&gt;=5,"A+",IF('Data Source'!AG8&gt;=4,"A",IF('Data Source'!AG8&gt;=3.5,"A-",IF('Data Source'!AG8&gt;=3,"B",IF('Data Source'!AG8&gt;=2,"C",IF('Data Source'!AG8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH8&gt;=5,"A+",IF('Data Source'!AH8&gt;=4,"A",IF('Data Source'!AH8&gt;=3.5,"A-",IF('Data Source'!AH8&gt;=3,"B",IF('Data Source'!AH8&gt;=2,"C",IF('Data Source'!AH8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G9" s="8">
-        <f>IF('Data Source'!AH8&gt;=5,"A+",IF('Data Source'!AH8&gt;=4,"A",IF('Data Source'!AH8&gt;=3.5,"A-",IF('Data Source'!AH8&gt;=3,"B",IF('Data Source'!AH8&gt;=2,"C",IF('Data Source'!AH8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI8&gt;=5,"A+",IF('Data Source'!AI8&gt;=4,"A",IF('Data Source'!AI8&gt;=3.5,"A-",IF('Data Source'!AI8&gt;=3,"B",IF('Data Source'!AI8&gt;=2,"C",IF('Data Source'!AI8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H9" s="8">
-        <f>IF('Data Source'!AI8&gt;=5,"A+",IF('Data Source'!AI8&gt;=4,"A",IF('Data Source'!AI8&gt;=3.5,"A-",IF('Data Source'!AI8&gt;=3,"B",IF('Data Source'!AI8&gt;=2,"C",IF('Data Source'!AI8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ8&gt;=5,"A+",IF('Data Source'!AJ8&gt;=4,"A",IF('Data Source'!AJ8&gt;=3.5,"A-",IF('Data Source'!AJ8&gt;=3,"B",IF('Data Source'!AJ8&gt;=2,"C",IF('Data Source'!AJ8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I9" s="8">
-        <f>IF('Data Source'!AJ8&gt;=5,"A+",IF('Data Source'!AJ8&gt;=4,"A",IF('Data Source'!AJ8&gt;=3.5,"A-",IF('Data Source'!AJ8&gt;=3,"B",IF('Data Source'!AJ8&gt;=2,"C",IF('Data Source'!AJ8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK8&gt;=5,"A+",IF('Data Source'!AK8&gt;=4,"A",IF('Data Source'!AK8&gt;=3.5,"A-",IF('Data Source'!AK8&gt;=3,"B",IF('Data Source'!AK8&gt;=2,"C",IF('Data Source'!AK8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J9" s="8">
-        <f>IF('Data Source'!AK8&gt;=5,"A+",IF('Data Source'!AK8&gt;=4,"A",IF('Data Source'!AK8&gt;=3.5,"A-",IF('Data Source'!AK8&gt;=3,"B",IF('Data Source'!AK8&gt;=2,"C",IF('Data Source'!AK8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL8&gt;=5,"A+",IF('Data Source'!AL8&gt;=4,"A",IF('Data Source'!AL8&gt;=3.5,"A-",IF('Data Source'!AL8&gt;=3,"B",IF('Data Source'!AL8&gt;=2,"C",IF('Data Source'!AL8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K9" s="8">
-        <f>IF('Data Source'!AL8&gt;=5,"A+",IF('Data Source'!AL8&gt;=4,"A",IF('Data Source'!AL8&gt;=3.5,"A-",IF('Data Source'!AL8&gt;=3,"B",IF('Data Source'!AL8&gt;=2,"C",IF('Data Source'!AL8&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM8&gt;=5,"A+",IF('Data Source'!AM8&gt;=4,"A",IF('Data Source'!AM8&gt;=3.5,"A-",IF('Data Source'!AM8&gt;=3,"B",IF('Data Source'!AM8&gt;=2,"C",IF('Data Source'!AM8&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L9" s="8">
@@ -4742,11 +4829,11 @@
         <v/>
       </c>
       <c r="N9" s="7">
-        <f>'Data Source'!X8</f>
+        <f>'Data Source'!Y8</f>
         <v/>
       </c>
       <c r="O9" s="8">
-        <f>'Data Source'!Y8</f>
+        <f>'Data Source'!Z8</f>
         <v/>
       </c>
     </row>
@@ -4760,39 +4847,39 @@
         <v/>
       </c>
       <c r="C10" s="8">
-        <f>IF('Data Source'!AD9&gt;=5,"A+",IF('Data Source'!AD9&gt;=4,"A",IF('Data Source'!AD9&gt;=3.5,"A-",IF('Data Source'!AD9&gt;=3,"B",IF('Data Source'!AD9&gt;=2,"C",IF('Data Source'!AD9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE9&gt;=5,"A+",IF('Data Source'!AE9&gt;=4,"A",IF('Data Source'!AE9&gt;=3.5,"A-",IF('Data Source'!AE9&gt;=3,"B",IF('Data Source'!AE9&gt;=2,"C",IF('Data Source'!AE9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D10" s="8">
-        <f>IF('Data Source'!AE9&gt;=5,"A+",IF('Data Source'!AE9&gt;=4,"A",IF('Data Source'!AE9&gt;=3.5,"A-",IF('Data Source'!AE9&gt;=3,"B",IF('Data Source'!AE9&gt;=2,"C",IF('Data Source'!AE9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF9&gt;=5,"A+",IF('Data Source'!AF9&gt;=4,"A",IF('Data Source'!AF9&gt;=3.5,"A-",IF('Data Source'!AF9&gt;=3,"B",IF('Data Source'!AF9&gt;=2,"C",IF('Data Source'!AF9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E10" s="8">
-        <f>IF('Data Source'!AF9&gt;=5,"A+",IF('Data Source'!AF9&gt;=4,"A",IF('Data Source'!AF9&gt;=3.5,"A-",IF('Data Source'!AF9&gt;=3,"B",IF('Data Source'!AF9&gt;=2,"C",IF('Data Source'!AF9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG9&gt;=5,"A+",IF('Data Source'!AG9&gt;=4,"A",IF('Data Source'!AG9&gt;=3.5,"A-",IF('Data Source'!AG9&gt;=3,"B",IF('Data Source'!AG9&gt;=2,"C",IF('Data Source'!AG9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F10" s="8">
-        <f>IF('Data Source'!AG9&gt;=5,"A+",IF('Data Source'!AG9&gt;=4,"A",IF('Data Source'!AG9&gt;=3.5,"A-",IF('Data Source'!AG9&gt;=3,"B",IF('Data Source'!AG9&gt;=2,"C",IF('Data Source'!AG9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH9&gt;=5,"A+",IF('Data Source'!AH9&gt;=4,"A",IF('Data Source'!AH9&gt;=3.5,"A-",IF('Data Source'!AH9&gt;=3,"B",IF('Data Source'!AH9&gt;=2,"C",IF('Data Source'!AH9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G10" s="8">
-        <f>IF('Data Source'!AH9&gt;=5,"A+",IF('Data Source'!AH9&gt;=4,"A",IF('Data Source'!AH9&gt;=3.5,"A-",IF('Data Source'!AH9&gt;=3,"B",IF('Data Source'!AH9&gt;=2,"C",IF('Data Source'!AH9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI9&gt;=5,"A+",IF('Data Source'!AI9&gt;=4,"A",IF('Data Source'!AI9&gt;=3.5,"A-",IF('Data Source'!AI9&gt;=3,"B",IF('Data Source'!AI9&gt;=2,"C",IF('Data Source'!AI9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H10" s="8">
-        <f>IF('Data Source'!AI9&gt;=5,"A+",IF('Data Source'!AI9&gt;=4,"A",IF('Data Source'!AI9&gt;=3.5,"A-",IF('Data Source'!AI9&gt;=3,"B",IF('Data Source'!AI9&gt;=2,"C",IF('Data Source'!AI9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ9&gt;=5,"A+",IF('Data Source'!AJ9&gt;=4,"A",IF('Data Source'!AJ9&gt;=3.5,"A-",IF('Data Source'!AJ9&gt;=3,"B",IF('Data Source'!AJ9&gt;=2,"C",IF('Data Source'!AJ9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I10" s="8">
-        <f>IF('Data Source'!AJ9&gt;=5,"A+",IF('Data Source'!AJ9&gt;=4,"A",IF('Data Source'!AJ9&gt;=3.5,"A-",IF('Data Source'!AJ9&gt;=3,"B",IF('Data Source'!AJ9&gt;=2,"C",IF('Data Source'!AJ9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK9&gt;=5,"A+",IF('Data Source'!AK9&gt;=4,"A",IF('Data Source'!AK9&gt;=3.5,"A-",IF('Data Source'!AK9&gt;=3,"B",IF('Data Source'!AK9&gt;=2,"C",IF('Data Source'!AK9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J10" s="8">
-        <f>IF('Data Source'!AK9&gt;=5,"A+",IF('Data Source'!AK9&gt;=4,"A",IF('Data Source'!AK9&gt;=3.5,"A-",IF('Data Source'!AK9&gt;=3,"B",IF('Data Source'!AK9&gt;=2,"C",IF('Data Source'!AK9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL9&gt;=5,"A+",IF('Data Source'!AL9&gt;=4,"A",IF('Data Source'!AL9&gt;=3.5,"A-",IF('Data Source'!AL9&gt;=3,"B",IF('Data Source'!AL9&gt;=2,"C",IF('Data Source'!AL9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K10" s="8">
-        <f>IF('Data Source'!AL9&gt;=5,"A+",IF('Data Source'!AL9&gt;=4,"A",IF('Data Source'!AL9&gt;=3.5,"A-",IF('Data Source'!AL9&gt;=3,"B",IF('Data Source'!AL9&gt;=2,"C",IF('Data Source'!AL9&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM9&gt;=5,"A+",IF('Data Source'!AM9&gt;=4,"A",IF('Data Source'!AM9&gt;=3.5,"A-",IF('Data Source'!AM9&gt;=3,"B",IF('Data Source'!AM9&gt;=2,"C",IF('Data Source'!AM9&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L10" s="8">
@@ -4804,11 +4891,11 @@
         <v/>
       </c>
       <c r="N10" s="7">
-        <f>'Data Source'!X9</f>
+        <f>'Data Source'!Y9</f>
         <v/>
       </c>
       <c r="O10" s="8">
-        <f>'Data Source'!Y9</f>
+        <f>'Data Source'!Z9</f>
         <v/>
       </c>
     </row>
@@ -4822,39 +4909,39 @@
         <v/>
       </c>
       <c r="C11" s="8">
-        <f>IF('Data Source'!AD10&gt;=5,"A+",IF('Data Source'!AD10&gt;=4,"A",IF('Data Source'!AD10&gt;=3.5,"A-",IF('Data Source'!AD10&gt;=3,"B",IF('Data Source'!AD10&gt;=2,"C",IF('Data Source'!AD10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE10&gt;=5,"A+",IF('Data Source'!AE10&gt;=4,"A",IF('Data Source'!AE10&gt;=3.5,"A-",IF('Data Source'!AE10&gt;=3,"B",IF('Data Source'!AE10&gt;=2,"C",IF('Data Source'!AE10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D11" s="8">
-        <f>IF('Data Source'!AE10&gt;=5,"A+",IF('Data Source'!AE10&gt;=4,"A",IF('Data Source'!AE10&gt;=3.5,"A-",IF('Data Source'!AE10&gt;=3,"B",IF('Data Source'!AE10&gt;=2,"C",IF('Data Source'!AE10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF10&gt;=5,"A+",IF('Data Source'!AF10&gt;=4,"A",IF('Data Source'!AF10&gt;=3.5,"A-",IF('Data Source'!AF10&gt;=3,"B",IF('Data Source'!AF10&gt;=2,"C",IF('Data Source'!AF10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E11" s="8">
-        <f>IF('Data Source'!AF10&gt;=5,"A+",IF('Data Source'!AF10&gt;=4,"A",IF('Data Source'!AF10&gt;=3.5,"A-",IF('Data Source'!AF10&gt;=3,"B",IF('Data Source'!AF10&gt;=2,"C",IF('Data Source'!AF10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG10&gt;=5,"A+",IF('Data Source'!AG10&gt;=4,"A",IF('Data Source'!AG10&gt;=3.5,"A-",IF('Data Source'!AG10&gt;=3,"B",IF('Data Source'!AG10&gt;=2,"C",IF('Data Source'!AG10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F11" s="8">
-        <f>IF('Data Source'!AG10&gt;=5,"A+",IF('Data Source'!AG10&gt;=4,"A",IF('Data Source'!AG10&gt;=3.5,"A-",IF('Data Source'!AG10&gt;=3,"B",IF('Data Source'!AG10&gt;=2,"C",IF('Data Source'!AG10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH10&gt;=5,"A+",IF('Data Source'!AH10&gt;=4,"A",IF('Data Source'!AH10&gt;=3.5,"A-",IF('Data Source'!AH10&gt;=3,"B",IF('Data Source'!AH10&gt;=2,"C",IF('Data Source'!AH10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G11" s="8">
-        <f>IF('Data Source'!AH10&gt;=5,"A+",IF('Data Source'!AH10&gt;=4,"A",IF('Data Source'!AH10&gt;=3.5,"A-",IF('Data Source'!AH10&gt;=3,"B",IF('Data Source'!AH10&gt;=2,"C",IF('Data Source'!AH10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI10&gt;=5,"A+",IF('Data Source'!AI10&gt;=4,"A",IF('Data Source'!AI10&gt;=3.5,"A-",IF('Data Source'!AI10&gt;=3,"B",IF('Data Source'!AI10&gt;=2,"C",IF('Data Source'!AI10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H11" s="8">
-        <f>IF('Data Source'!AI10&gt;=5,"A+",IF('Data Source'!AI10&gt;=4,"A",IF('Data Source'!AI10&gt;=3.5,"A-",IF('Data Source'!AI10&gt;=3,"B",IF('Data Source'!AI10&gt;=2,"C",IF('Data Source'!AI10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ10&gt;=5,"A+",IF('Data Source'!AJ10&gt;=4,"A",IF('Data Source'!AJ10&gt;=3.5,"A-",IF('Data Source'!AJ10&gt;=3,"B",IF('Data Source'!AJ10&gt;=2,"C",IF('Data Source'!AJ10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I11" s="8">
-        <f>IF('Data Source'!AJ10&gt;=5,"A+",IF('Data Source'!AJ10&gt;=4,"A",IF('Data Source'!AJ10&gt;=3.5,"A-",IF('Data Source'!AJ10&gt;=3,"B",IF('Data Source'!AJ10&gt;=2,"C",IF('Data Source'!AJ10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK10&gt;=5,"A+",IF('Data Source'!AK10&gt;=4,"A",IF('Data Source'!AK10&gt;=3.5,"A-",IF('Data Source'!AK10&gt;=3,"B",IF('Data Source'!AK10&gt;=2,"C",IF('Data Source'!AK10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J11" s="8">
-        <f>IF('Data Source'!AK10&gt;=5,"A+",IF('Data Source'!AK10&gt;=4,"A",IF('Data Source'!AK10&gt;=3.5,"A-",IF('Data Source'!AK10&gt;=3,"B",IF('Data Source'!AK10&gt;=2,"C",IF('Data Source'!AK10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL10&gt;=5,"A+",IF('Data Source'!AL10&gt;=4,"A",IF('Data Source'!AL10&gt;=3.5,"A-",IF('Data Source'!AL10&gt;=3,"B",IF('Data Source'!AL10&gt;=2,"C",IF('Data Source'!AL10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K11" s="8">
-        <f>IF('Data Source'!AL10&gt;=5,"A+",IF('Data Source'!AL10&gt;=4,"A",IF('Data Source'!AL10&gt;=3.5,"A-",IF('Data Source'!AL10&gt;=3,"B",IF('Data Source'!AL10&gt;=2,"C",IF('Data Source'!AL10&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM10&gt;=5,"A+",IF('Data Source'!AM10&gt;=4,"A",IF('Data Source'!AM10&gt;=3.5,"A-",IF('Data Source'!AM10&gt;=3,"B",IF('Data Source'!AM10&gt;=2,"C",IF('Data Source'!AM10&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L11" s="8">
@@ -4866,11 +4953,11 @@
         <v/>
       </c>
       <c r="N11" s="7">
-        <f>'Data Source'!X10</f>
+        <f>'Data Source'!Y10</f>
         <v/>
       </c>
       <c r="O11" s="8">
-        <f>'Data Source'!Y10</f>
+        <f>'Data Source'!Z10</f>
         <v/>
       </c>
     </row>
@@ -4884,39 +4971,39 @@
         <v/>
       </c>
       <c r="C12" s="8">
-        <f>IF('Data Source'!AD11&gt;=5,"A+",IF('Data Source'!AD11&gt;=4,"A",IF('Data Source'!AD11&gt;=3.5,"A-",IF('Data Source'!AD11&gt;=3,"B",IF('Data Source'!AD11&gt;=2,"C",IF('Data Source'!AD11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE11&gt;=5,"A+",IF('Data Source'!AE11&gt;=4,"A",IF('Data Source'!AE11&gt;=3.5,"A-",IF('Data Source'!AE11&gt;=3,"B",IF('Data Source'!AE11&gt;=2,"C",IF('Data Source'!AE11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D12" s="8">
-        <f>IF('Data Source'!AE11&gt;=5,"A+",IF('Data Source'!AE11&gt;=4,"A",IF('Data Source'!AE11&gt;=3.5,"A-",IF('Data Source'!AE11&gt;=3,"B",IF('Data Source'!AE11&gt;=2,"C",IF('Data Source'!AE11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF11&gt;=5,"A+",IF('Data Source'!AF11&gt;=4,"A",IF('Data Source'!AF11&gt;=3.5,"A-",IF('Data Source'!AF11&gt;=3,"B",IF('Data Source'!AF11&gt;=2,"C",IF('Data Source'!AF11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E12" s="8">
-        <f>IF('Data Source'!AF11&gt;=5,"A+",IF('Data Source'!AF11&gt;=4,"A",IF('Data Source'!AF11&gt;=3.5,"A-",IF('Data Source'!AF11&gt;=3,"B",IF('Data Source'!AF11&gt;=2,"C",IF('Data Source'!AF11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG11&gt;=5,"A+",IF('Data Source'!AG11&gt;=4,"A",IF('Data Source'!AG11&gt;=3.5,"A-",IF('Data Source'!AG11&gt;=3,"B",IF('Data Source'!AG11&gt;=2,"C",IF('Data Source'!AG11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F12" s="8">
-        <f>IF('Data Source'!AG11&gt;=5,"A+",IF('Data Source'!AG11&gt;=4,"A",IF('Data Source'!AG11&gt;=3.5,"A-",IF('Data Source'!AG11&gt;=3,"B",IF('Data Source'!AG11&gt;=2,"C",IF('Data Source'!AG11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH11&gt;=5,"A+",IF('Data Source'!AH11&gt;=4,"A",IF('Data Source'!AH11&gt;=3.5,"A-",IF('Data Source'!AH11&gt;=3,"B",IF('Data Source'!AH11&gt;=2,"C",IF('Data Source'!AH11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G12" s="8">
-        <f>IF('Data Source'!AH11&gt;=5,"A+",IF('Data Source'!AH11&gt;=4,"A",IF('Data Source'!AH11&gt;=3.5,"A-",IF('Data Source'!AH11&gt;=3,"B",IF('Data Source'!AH11&gt;=2,"C",IF('Data Source'!AH11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI11&gt;=5,"A+",IF('Data Source'!AI11&gt;=4,"A",IF('Data Source'!AI11&gt;=3.5,"A-",IF('Data Source'!AI11&gt;=3,"B",IF('Data Source'!AI11&gt;=2,"C",IF('Data Source'!AI11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H12" s="8">
-        <f>IF('Data Source'!AI11&gt;=5,"A+",IF('Data Source'!AI11&gt;=4,"A",IF('Data Source'!AI11&gt;=3.5,"A-",IF('Data Source'!AI11&gt;=3,"B",IF('Data Source'!AI11&gt;=2,"C",IF('Data Source'!AI11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ11&gt;=5,"A+",IF('Data Source'!AJ11&gt;=4,"A",IF('Data Source'!AJ11&gt;=3.5,"A-",IF('Data Source'!AJ11&gt;=3,"B",IF('Data Source'!AJ11&gt;=2,"C",IF('Data Source'!AJ11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I12" s="8">
-        <f>IF('Data Source'!AJ11&gt;=5,"A+",IF('Data Source'!AJ11&gt;=4,"A",IF('Data Source'!AJ11&gt;=3.5,"A-",IF('Data Source'!AJ11&gt;=3,"B",IF('Data Source'!AJ11&gt;=2,"C",IF('Data Source'!AJ11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK11&gt;=5,"A+",IF('Data Source'!AK11&gt;=4,"A",IF('Data Source'!AK11&gt;=3.5,"A-",IF('Data Source'!AK11&gt;=3,"B",IF('Data Source'!AK11&gt;=2,"C",IF('Data Source'!AK11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J12" s="8">
-        <f>IF('Data Source'!AK11&gt;=5,"A+",IF('Data Source'!AK11&gt;=4,"A",IF('Data Source'!AK11&gt;=3.5,"A-",IF('Data Source'!AK11&gt;=3,"B",IF('Data Source'!AK11&gt;=2,"C",IF('Data Source'!AK11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL11&gt;=5,"A+",IF('Data Source'!AL11&gt;=4,"A",IF('Data Source'!AL11&gt;=3.5,"A-",IF('Data Source'!AL11&gt;=3,"B",IF('Data Source'!AL11&gt;=2,"C",IF('Data Source'!AL11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K12" s="8">
-        <f>IF('Data Source'!AL11&gt;=5,"A+",IF('Data Source'!AL11&gt;=4,"A",IF('Data Source'!AL11&gt;=3.5,"A-",IF('Data Source'!AL11&gt;=3,"B",IF('Data Source'!AL11&gt;=2,"C",IF('Data Source'!AL11&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM11&gt;=5,"A+",IF('Data Source'!AM11&gt;=4,"A",IF('Data Source'!AM11&gt;=3.5,"A-",IF('Data Source'!AM11&gt;=3,"B",IF('Data Source'!AM11&gt;=2,"C",IF('Data Source'!AM11&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L12" s="8">
@@ -4928,11 +5015,11 @@
         <v/>
       </c>
       <c r="N12" s="7">
-        <f>'Data Source'!X11</f>
+        <f>'Data Source'!Y11</f>
         <v/>
       </c>
       <c r="O12" s="8">
-        <f>'Data Source'!Y11</f>
+        <f>'Data Source'!Z11</f>
         <v/>
       </c>
     </row>
@@ -4946,39 +5033,39 @@
         <v/>
       </c>
       <c r="C13" s="8">
-        <f>IF('Data Source'!AD12&gt;=5,"A+",IF('Data Source'!AD12&gt;=4,"A",IF('Data Source'!AD12&gt;=3.5,"A-",IF('Data Source'!AD12&gt;=3,"B",IF('Data Source'!AD12&gt;=2,"C",IF('Data Source'!AD12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE12&gt;=5,"A+",IF('Data Source'!AE12&gt;=4,"A",IF('Data Source'!AE12&gt;=3.5,"A-",IF('Data Source'!AE12&gt;=3,"B",IF('Data Source'!AE12&gt;=2,"C",IF('Data Source'!AE12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D13" s="8">
-        <f>IF('Data Source'!AE12&gt;=5,"A+",IF('Data Source'!AE12&gt;=4,"A",IF('Data Source'!AE12&gt;=3.5,"A-",IF('Data Source'!AE12&gt;=3,"B",IF('Data Source'!AE12&gt;=2,"C",IF('Data Source'!AE12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF12&gt;=5,"A+",IF('Data Source'!AF12&gt;=4,"A",IF('Data Source'!AF12&gt;=3.5,"A-",IF('Data Source'!AF12&gt;=3,"B",IF('Data Source'!AF12&gt;=2,"C",IF('Data Source'!AF12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E13" s="8">
-        <f>IF('Data Source'!AF12&gt;=5,"A+",IF('Data Source'!AF12&gt;=4,"A",IF('Data Source'!AF12&gt;=3.5,"A-",IF('Data Source'!AF12&gt;=3,"B",IF('Data Source'!AF12&gt;=2,"C",IF('Data Source'!AF12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG12&gt;=5,"A+",IF('Data Source'!AG12&gt;=4,"A",IF('Data Source'!AG12&gt;=3.5,"A-",IF('Data Source'!AG12&gt;=3,"B",IF('Data Source'!AG12&gt;=2,"C",IF('Data Source'!AG12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F13" s="8">
-        <f>IF('Data Source'!AG12&gt;=5,"A+",IF('Data Source'!AG12&gt;=4,"A",IF('Data Source'!AG12&gt;=3.5,"A-",IF('Data Source'!AG12&gt;=3,"B",IF('Data Source'!AG12&gt;=2,"C",IF('Data Source'!AG12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH12&gt;=5,"A+",IF('Data Source'!AH12&gt;=4,"A",IF('Data Source'!AH12&gt;=3.5,"A-",IF('Data Source'!AH12&gt;=3,"B",IF('Data Source'!AH12&gt;=2,"C",IF('Data Source'!AH12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G13" s="8">
-        <f>IF('Data Source'!AH12&gt;=5,"A+",IF('Data Source'!AH12&gt;=4,"A",IF('Data Source'!AH12&gt;=3.5,"A-",IF('Data Source'!AH12&gt;=3,"B",IF('Data Source'!AH12&gt;=2,"C",IF('Data Source'!AH12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI12&gt;=5,"A+",IF('Data Source'!AI12&gt;=4,"A",IF('Data Source'!AI12&gt;=3.5,"A-",IF('Data Source'!AI12&gt;=3,"B",IF('Data Source'!AI12&gt;=2,"C",IF('Data Source'!AI12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H13" s="8">
-        <f>IF('Data Source'!AI12&gt;=5,"A+",IF('Data Source'!AI12&gt;=4,"A",IF('Data Source'!AI12&gt;=3.5,"A-",IF('Data Source'!AI12&gt;=3,"B",IF('Data Source'!AI12&gt;=2,"C",IF('Data Source'!AI12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ12&gt;=5,"A+",IF('Data Source'!AJ12&gt;=4,"A",IF('Data Source'!AJ12&gt;=3.5,"A-",IF('Data Source'!AJ12&gt;=3,"B",IF('Data Source'!AJ12&gt;=2,"C",IF('Data Source'!AJ12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I13" s="8">
-        <f>IF('Data Source'!AJ12&gt;=5,"A+",IF('Data Source'!AJ12&gt;=4,"A",IF('Data Source'!AJ12&gt;=3.5,"A-",IF('Data Source'!AJ12&gt;=3,"B",IF('Data Source'!AJ12&gt;=2,"C",IF('Data Source'!AJ12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK12&gt;=5,"A+",IF('Data Source'!AK12&gt;=4,"A",IF('Data Source'!AK12&gt;=3.5,"A-",IF('Data Source'!AK12&gt;=3,"B",IF('Data Source'!AK12&gt;=2,"C",IF('Data Source'!AK12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J13" s="8">
-        <f>IF('Data Source'!AK12&gt;=5,"A+",IF('Data Source'!AK12&gt;=4,"A",IF('Data Source'!AK12&gt;=3.5,"A-",IF('Data Source'!AK12&gt;=3,"B",IF('Data Source'!AK12&gt;=2,"C",IF('Data Source'!AK12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL12&gt;=5,"A+",IF('Data Source'!AL12&gt;=4,"A",IF('Data Source'!AL12&gt;=3.5,"A-",IF('Data Source'!AL12&gt;=3,"B",IF('Data Source'!AL12&gt;=2,"C",IF('Data Source'!AL12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K13" s="8">
-        <f>IF('Data Source'!AL12&gt;=5,"A+",IF('Data Source'!AL12&gt;=4,"A",IF('Data Source'!AL12&gt;=3.5,"A-",IF('Data Source'!AL12&gt;=3,"B",IF('Data Source'!AL12&gt;=2,"C",IF('Data Source'!AL12&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM12&gt;=5,"A+",IF('Data Source'!AM12&gt;=4,"A",IF('Data Source'!AM12&gt;=3.5,"A-",IF('Data Source'!AM12&gt;=3,"B",IF('Data Source'!AM12&gt;=2,"C",IF('Data Source'!AM12&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L13" s="8">
@@ -4990,11 +5077,11 @@
         <v/>
       </c>
       <c r="N13" s="7">
-        <f>'Data Source'!X12</f>
+        <f>'Data Source'!Y12</f>
         <v/>
       </c>
       <c r="O13" s="8">
-        <f>'Data Source'!Y12</f>
+        <f>'Data Source'!Z12</f>
         <v/>
       </c>
     </row>
@@ -5008,39 +5095,39 @@
         <v/>
       </c>
       <c r="C14" s="8">
-        <f>IF('Data Source'!AD13&gt;=5,"A+",IF('Data Source'!AD13&gt;=4,"A",IF('Data Source'!AD13&gt;=3.5,"A-",IF('Data Source'!AD13&gt;=3,"B",IF('Data Source'!AD13&gt;=2,"C",IF('Data Source'!AD13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE13&gt;=5,"A+",IF('Data Source'!AE13&gt;=4,"A",IF('Data Source'!AE13&gt;=3.5,"A-",IF('Data Source'!AE13&gt;=3,"B",IF('Data Source'!AE13&gt;=2,"C",IF('Data Source'!AE13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D14" s="8">
-        <f>IF('Data Source'!AE13&gt;=5,"A+",IF('Data Source'!AE13&gt;=4,"A",IF('Data Source'!AE13&gt;=3.5,"A-",IF('Data Source'!AE13&gt;=3,"B",IF('Data Source'!AE13&gt;=2,"C",IF('Data Source'!AE13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF13&gt;=5,"A+",IF('Data Source'!AF13&gt;=4,"A",IF('Data Source'!AF13&gt;=3.5,"A-",IF('Data Source'!AF13&gt;=3,"B",IF('Data Source'!AF13&gt;=2,"C",IF('Data Source'!AF13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E14" s="8">
-        <f>IF('Data Source'!AF13&gt;=5,"A+",IF('Data Source'!AF13&gt;=4,"A",IF('Data Source'!AF13&gt;=3.5,"A-",IF('Data Source'!AF13&gt;=3,"B",IF('Data Source'!AF13&gt;=2,"C",IF('Data Source'!AF13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG13&gt;=5,"A+",IF('Data Source'!AG13&gt;=4,"A",IF('Data Source'!AG13&gt;=3.5,"A-",IF('Data Source'!AG13&gt;=3,"B",IF('Data Source'!AG13&gt;=2,"C",IF('Data Source'!AG13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F14" s="8">
-        <f>IF('Data Source'!AG13&gt;=5,"A+",IF('Data Source'!AG13&gt;=4,"A",IF('Data Source'!AG13&gt;=3.5,"A-",IF('Data Source'!AG13&gt;=3,"B",IF('Data Source'!AG13&gt;=2,"C",IF('Data Source'!AG13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH13&gt;=5,"A+",IF('Data Source'!AH13&gt;=4,"A",IF('Data Source'!AH13&gt;=3.5,"A-",IF('Data Source'!AH13&gt;=3,"B",IF('Data Source'!AH13&gt;=2,"C",IF('Data Source'!AH13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G14" s="8">
-        <f>IF('Data Source'!AH13&gt;=5,"A+",IF('Data Source'!AH13&gt;=4,"A",IF('Data Source'!AH13&gt;=3.5,"A-",IF('Data Source'!AH13&gt;=3,"B",IF('Data Source'!AH13&gt;=2,"C",IF('Data Source'!AH13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI13&gt;=5,"A+",IF('Data Source'!AI13&gt;=4,"A",IF('Data Source'!AI13&gt;=3.5,"A-",IF('Data Source'!AI13&gt;=3,"B",IF('Data Source'!AI13&gt;=2,"C",IF('Data Source'!AI13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H14" s="8">
-        <f>IF('Data Source'!AI13&gt;=5,"A+",IF('Data Source'!AI13&gt;=4,"A",IF('Data Source'!AI13&gt;=3.5,"A-",IF('Data Source'!AI13&gt;=3,"B",IF('Data Source'!AI13&gt;=2,"C",IF('Data Source'!AI13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ13&gt;=5,"A+",IF('Data Source'!AJ13&gt;=4,"A",IF('Data Source'!AJ13&gt;=3.5,"A-",IF('Data Source'!AJ13&gt;=3,"B",IF('Data Source'!AJ13&gt;=2,"C",IF('Data Source'!AJ13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I14" s="8">
-        <f>IF('Data Source'!AJ13&gt;=5,"A+",IF('Data Source'!AJ13&gt;=4,"A",IF('Data Source'!AJ13&gt;=3.5,"A-",IF('Data Source'!AJ13&gt;=3,"B",IF('Data Source'!AJ13&gt;=2,"C",IF('Data Source'!AJ13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK13&gt;=5,"A+",IF('Data Source'!AK13&gt;=4,"A",IF('Data Source'!AK13&gt;=3.5,"A-",IF('Data Source'!AK13&gt;=3,"B",IF('Data Source'!AK13&gt;=2,"C",IF('Data Source'!AK13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J14" s="8">
-        <f>IF('Data Source'!AK13&gt;=5,"A+",IF('Data Source'!AK13&gt;=4,"A",IF('Data Source'!AK13&gt;=3.5,"A-",IF('Data Source'!AK13&gt;=3,"B",IF('Data Source'!AK13&gt;=2,"C",IF('Data Source'!AK13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL13&gt;=5,"A+",IF('Data Source'!AL13&gt;=4,"A",IF('Data Source'!AL13&gt;=3.5,"A-",IF('Data Source'!AL13&gt;=3,"B",IF('Data Source'!AL13&gt;=2,"C",IF('Data Source'!AL13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K14" s="8">
-        <f>IF('Data Source'!AL13&gt;=5,"A+",IF('Data Source'!AL13&gt;=4,"A",IF('Data Source'!AL13&gt;=3.5,"A-",IF('Data Source'!AL13&gt;=3,"B",IF('Data Source'!AL13&gt;=2,"C",IF('Data Source'!AL13&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM13&gt;=5,"A+",IF('Data Source'!AM13&gt;=4,"A",IF('Data Source'!AM13&gt;=3.5,"A-",IF('Data Source'!AM13&gt;=3,"B",IF('Data Source'!AM13&gt;=2,"C",IF('Data Source'!AM13&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L14" s="8">
@@ -5052,11 +5139,11 @@
         <v/>
       </c>
       <c r="N14" s="7">
-        <f>'Data Source'!X13</f>
+        <f>'Data Source'!Y13</f>
         <v/>
       </c>
       <c r="O14" s="8">
-        <f>'Data Source'!Y13</f>
+        <f>'Data Source'!Z13</f>
         <v/>
       </c>
     </row>
@@ -5070,39 +5157,39 @@
         <v/>
       </c>
       <c r="C15" s="8">
-        <f>IF('Data Source'!AD14&gt;=5,"A+",IF('Data Source'!AD14&gt;=4,"A",IF('Data Source'!AD14&gt;=3.5,"A-",IF('Data Source'!AD14&gt;=3,"B",IF('Data Source'!AD14&gt;=2,"C",IF('Data Source'!AD14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE14&gt;=5,"A+",IF('Data Source'!AE14&gt;=4,"A",IF('Data Source'!AE14&gt;=3.5,"A-",IF('Data Source'!AE14&gt;=3,"B",IF('Data Source'!AE14&gt;=2,"C",IF('Data Source'!AE14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D15" s="8">
-        <f>IF('Data Source'!AE14&gt;=5,"A+",IF('Data Source'!AE14&gt;=4,"A",IF('Data Source'!AE14&gt;=3.5,"A-",IF('Data Source'!AE14&gt;=3,"B",IF('Data Source'!AE14&gt;=2,"C",IF('Data Source'!AE14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF14&gt;=5,"A+",IF('Data Source'!AF14&gt;=4,"A",IF('Data Source'!AF14&gt;=3.5,"A-",IF('Data Source'!AF14&gt;=3,"B",IF('Data Source'!AF14&gt;=2,"C",IF('Data Source'!AF14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E15" s="8">
-        <f>IF('Data Source'!AF14&gt;=5,"A+",IF('Data Source'!AF14&gt;=4,"A",IF('Data Source'!AF14&gt;=3.5,"A-",IF('Data Source'!AF14&gt;=3,"B",IF('Data Source'!AF14&gt;=2,"C",IF('Data Source'!AF14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG14&gt;=5,"A+",IF('Data Source'!AG14&gt;=4,"A",IF('Data Source'!AG14&gt;=3.5,"A-",IF('Data Source'!AG14&gt;=3,"B",IF('Data Source'!AG14&gt;=2,"C",IF('Data Source'!AG14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F15" s="8">
-        <f>IF('Data Source'!AG14&gt;=5,"A+",IF('Data Source'!AG14&gt;=4,"A",IF('Data Source'!AG14&gt;=3.5,"A-",IF('Data Source'!AG14&gt;=3,"B",IF('Data Source'!AG14&gt;=2,"C",IF('Data Source'!AG14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH14&gt;=5,"A+",IF('Data Source'!AH14&gt;=4,"A",IF('Data Source'!AH14&gt;=3.5,"A-",IF('Data Source'!AH14&gt;=3,"B",IF('Data Source'!AH14&gt;=2,"C",IF('Data Source'!AH14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G15" s="8">
-        <f>IF('Data Source'!AH14&gt;=5,"A+",IF('Data Source'!AH14&gt;=4,"A",IF('Data Source'!AH14&gt;=3.5,"A-",IF('Data Source'!AH14&gt;=3,"B",IF('Data Source'!AH14&gt;=2,"C",IF('Data Source'!AH14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI14&gt;=5,"A+",IF('Data Source'!AI14&gt;=4,"A",IF('Data Source'!AI14&gt;=3.5,"A-",IF('Data Source'!AI14&gt;=3,"B",IF('Data Source'!AI14&gt;=2,"C",IF('Data Source'!AI14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H15" s="8">
-        <f>IF('Data Source'!AI14&gt;=5,"A+",IF('Data Source'!AI14&gt;=4,"A",IF('Data Source'!AI14&gt;=3.5,"A-",IF('Data Source'!AI14&gt;=3,"B",IF('Data Source'!AI14&gt;=2,"C",IF('Data Source'!AI14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ14&gt;=5,"A+",IF('Data Source'!AJ14&gt;=4,"A",IF('Data Source'!AJ14&gt;=3.5,"A-",IF('Data Source'!AJ14&gt;=3,"B",IF('Data Source'!AJ14&gt;=2,"C",IF('Data Source'!AJ14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I15" s="8">
-        <f>IF('Data Source'!AJ14&gt;=5,"A+",IF('Data Source'!AJ14&gt;=4,"A",IF('Data Source'!AJ14&gt;=3.5,"A-",IF('Data Source'!AJ14&gt;=3,"B",IF('Data Source'!AJ14&gt;=2,"C",IF('Data Source'!AJ14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK14&gt;=5,"A+",IF('Data Source'!AK14&gt;=4,"A",IF('Data Source'!AK14&gt;=3.5,"A-",IF('Data Source'!AK14&gt;=3,"B",IF('Data Source'!AK14&gt;=2,"C",IF('Data Source'!AK14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J15" s="8">
-        <f>IF('Data Source'!AK14&gt;=5,"A+",IF('Data Source'!AK14&gt;=4,"A",IF('Data Source'!AK14&gt;=3.5,"A-",IF('Data Source'!AK14&gt;=3,"B",IF('Data Source'!AK14&gt;=2,"C",IF('Data Source'!AK14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL14&gt;=5,"A+",IF('Data Source'!AL14&gt;=4,"A",IF('Data Source'!AL14&gt;=3.5,"A-",IF('Data Source'!AL14&gt;=3,"B",IF('Data Source'!AL14&gt;=2,"C",IF('Data Source'!AL14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K15" s="8">
-        <f>IF('Data Source'!AL14&gt;=5,"A+",IF('Data Source'!AL14&gt;=4,"A",IF('Data Source'!AL14&gt;=3.5,"A-",IF('Data Source'!AL14&gt;=3,"B",IF('Data Source'!AL14&gt;=2,"C",IF('Data Source'!AL14&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM14&gt;=5,"A+",IF('Data Source'!AM14&gt;=4,"A",IF('Data Source'!AM14&gt;=3.5,"A-",IF('Data Source'!AM14&gt;=3,"B",IF('Data Source'!AM14&gt;=2,"C",IF('Data Source'!AM14&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L15" s="8">
@@ -5114,11 +5201,11 @@
         <v/>
       </c>
       <c r="N15" s="7">
-        <f>'Data Source'!X14</f>
+        <f>'Data Source'!Y14</f>
         <v/>
       </c>
       <c r="O15" s="8">
-        <f>'Data Source'!Y14</f>
+        <f>'Data Source'!Z14</f>
         <v/>
       </c>
     </row>
@@ -5132,39 +5219,39 @@
         <v/>
       </c>
       <c r="C16" s="8">
-        <f>IF('Data Source'!AD15&gt;=5,"A+",IF('Data Source'!AD15&gt;=4,"A",IF('Data Source'!AD15&gt;=3.5,"A-",IF('Data Source'!AD15&gt;=3,"B",IF('Data Source'!AD15&gt;=2,"C",IF('Data Source'!AD15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE15&gt;=5,"A+",IF('Data Source'!AE15&gt;=4,"A",IF('Data Source'!AE15&gt;=3.5,"A-",IF('Data Source'!AE15&gt;=3,"B",IF('Data Source'!AE15&gt;=2,"C",IF('Data Source'!AE15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D16" s="8">
-        <f>IF('Data Source'!AE15&gt;=5,"A+",IF('Data Source'!AE15&gt;=4,"A",IF('Data Source'!AE15&gt;=3.5,"A-",IF('Data Source'!AE15&gt;=3,"B",IF('Data Source'!AE15&gt;=2,"C",IF('Data Source'!AE15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF15&gt;=5,"A+",IF('Data Source'!AF15&gt;=4,"A",IF('Data Source'!AF15&gt;=3.5,"A-",IF('Data Source'!AF15&gt;=3,"B",IF('Data Source'!AF15&gt;=2,"C",IF('Data Source'!AF15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E16" s="8">
-        <f>IF('Data Source'!AF15&gt;=5,"A+",IF('Data Source'!AF15&gt;=4,"A",IF('Data Source'!AF15&gt;=3.5,"A-",IF('Data Source'!AF15&gt;=3,"B",IF('Data Source'!AF15&gt;=2,"C",IF('Data Source'!AF15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG15&gt;=5,"A+",IF('Data Source'!AG15&gt;=4,"A",IF('Data Source'!AG15&gt;=3.5,"A-",IF('Data Source'!AG15&gt;=3,"B",IF('Data Source'!AG15&gt;=2,"C",IF('Data Source'!AG15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F16" s="8">
-        <f>IF('Data Source'!AG15&gt;=5,"A+",IF('Data Source'!AG15&gt;=4,"A",IF('Data Source'!AG15&gt;=3.5,"A-",IF('Data Source'!AG15&gt;=3,"B",IF('Data Source'!AG15&gt;=2,"C",IF('Data Source'!AG15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH15&gt;=5,"A+",IF('Data Source'!AH15&gt;=4,"A",IF('Data Source'!AH15&gt;=3.5,"A-",IF('Data Source'!AH15&gt;=3,"B",IF('Data Source'!AH15&gt;=2,"C",IF('Data Source'!AH15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G16" s="8">
-        <f>IF('Data Source'!AH15&gt;=5,"A+",IF('Data Source'!AH15&gt;=4,"A",IF('Data Source'!AH15&gt;=3.5,"A-",IF('Data Source'!AH15&gt;=3,"B",IF('Data Source'!AH15&gt;=2,"C",IF('Data Source'!AH15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI15&gt;=5,"A+",IF('Data Source'!AI15&gt;=4,"A",IF('Data Source'!AI15&gt;=3.5,"A-",IF('Data Source'!AI15&gt;=3,"B",IF('Data Source'!AI15&gt;=2,"C",IF('Data Source'!AI15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H16" s="8">
-        <f>IF('Data Source'!AI15&gt;=5,"A+",IF('Data Source'!AI15&gt;=4,"A",IF('Data Source'!AI15&gt;=3.5,"A-",IF('Data Source'!AI15&gt;=3,"B",IF('Data Source'!AI15&gt;=2,"C",IF('Data Source'!AI15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ15&gt;=5,"A+",IF('Data Source'!AJ15&gt;=4,"A",IF('Data Source'!AJ15&gt;=3.5,"A-",IF('Data Source'!AJ15&gt;=3,"B",IF('Data Source'!AJ15&gt;=2,"C",IF('Data Source'!AJ15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I16" s="8">
-        <f>IF('Data Source'!AJ15&gt;=5,"A+",IF('Data Source'!AJ15&gt;=4,"A",IF('Data Source'!AJ15&gt;=3.5,"A-",IF('Data Source'!AJ15&gt;=3,"B",IF('Data Source'!AJ15&gt;=2,"C",IF('Data Source'!AJ15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK15&gt;=5,"A+",IF('Data Source'!AK15&gt;=4,"A",IF('Data Source'!AK15&gt;=3.5,"A-",IF('Data Source'!AK15&gt;=3,"B",IF('Data Source'!AK15&gt;=2,"C",IF('Data Source'!AK15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J16" s="8">
-        <f>IF('Data Source'!AK15&gt;=5,"A+",IF('Data Source'!AK15&gt;=4,"A",IF('Data Source'!AK15&gt;=3.5,"A-",IF('Data Source'!AK15&gt;=3,"B",IF('Data Source'!AK15&gt;=2,"C",IF('Data Source'!AK15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL15&gt;=5,"A+",IF('Data Source'!AL15&gt;=4,"A",IF('Data Source'!AL15&gt;=3.5,"A-",IF('Data Source'!AL15&gt;=3,"B",IF('Data Source'!AL15&gt;=2,"C",IF('Data Source'!AL15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K16" s="8">
-        <f>IF('Data Source'!AL15&gt;=5,"A+",IF('Data Source'!AL15&gt;=4,"A",IF('Data Source'!AL15&gt;=3.5,"A-",IF('Data Source'!AL15&gt;=3,"B",IF('Data Source'!AL15&gt;=2,"C",IF('Data Source'!AL15&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM15&gt;=5,"A+",IF('Data Source'!AM15&gt;=4,"A",IF('Data Source'!AM15&gt;=3.5,"A-",IF('Data Source'!AM15&gt;=3,"B",IF('Data Source'!AM15&gt;=2,"C",IF('Data Source'!AM15&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L16" s="8">
@@ -5176,11 +5263,11 @@
         <v/>
       </c>
       <c r="N16" s="7">
-        <f>'Data Source'!X15</f>
+        <f>'Data Source'!Y15</f>
         <v/>
       </c>
       <c r="O16" s="8">
-        <f>'Data Source'!Y15</f>
+        <f>'Data Source'!Z15</f>
         <v/>
       </c>
     </row>
@@ -5194,39 +5281,39 @@
         <v/>
       </c>
       <c r="C17" s="8">
-        <f>IF('Data Source'!AD16&gt;=5,"A+",IF('Data Source'!AD16&gt;=4,"A",IF('Data Source'!AD16&gt;=3.5,"A-",IF('Data Source'!AD16&gt;=3,"B",IF('Data Source'!AD16&gt;=2,"C",IF('Data Source'!AD16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE16&gt;=5,"A+",IF('Data Source'!AE16&gt;=4,"A",IF('Data Source'!AE16&gt;=3.5,"A-",IF('Data Source'!AE16&gt;=3,"B",IF('Data Source'!AE16&gt;=2,"C",IF('Data Source'!AE16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D17" s="8">
-        <f>IF('Data Source'!AE16&gt;=5,"A+",IF('Data Source'!AE16&gt;=4,"A",IF('Data Source'!AE16&gt;=3.5,"A-",IF('Data Source'!AE16&gt;=3,"B",IF('Data Source'!AE16&gt;=2,"C",IF('Data Source'!AE16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF16&gt;=5,"A+",IF('Data Source'!AF16&gt;=4,"A",IF('Data Source'!AF16&gt;=3.5,"A-",IF('Data Source'!AF16&gt;=3,"B",IF('Data Source'!AF16&gt;=2,"C",IF('Data Source'!AF16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E17" s="8">
-        <f>IF('Data Source'!AF16&gt;=5,"A+",IF('Data Source'!AF16&gt;=4,"A",IF('Data Source'!AF16&gt;=3.5,"A-",IF('Data Source'!AF16&gt;=3,"B",IF('Data Source'!AF16&gt;=2,"C",IF('Data Source'!AF16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG16&gt;=5,"A+",IF('Data Source'!AG16&gt;=4,"A",IF('Data Source'!AG16&gt;=3.5,"A-",IF('Data Source'!AG16&gt;=3,"B",IF('Data Source'!AG16&gt;=2,"C",IF('Data Source'!AG16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F17" s="8">
-        <f>IF('Data Source'!AG16&gt;=5,"A+",IF('Data Source'!AG16&gt;=4,"A",IF('Data Source'!AG16&gt;=3.5,"A-",IF('Data Source'!AG16&gt;=3,"B",IF('Data Source'!AG16&gt;=2,"C",IF('Data Source'!AG16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH16&gt;=5,"A+",IF('Data Source'!AH16&gt;=4,"A",IF('Data Source'!AH16&gt;=3.5,"A-",IF('Data Source'!AH16&gt;=3,"B",IF('Data Source'!AH16&gt;=2,"C",IF('Data Source'!AH16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G17" s="8">
-        <f>IF('Data Source'!AH16&gt;=5,"A+",IF('Data Source'!AH16&gt;=4,"A",IF('Data Source'!AH16&gt;=3.5,"A-",IF('Data Source'!AH16&gt;=3,"B",IF('Data Source'!AH16&gt;=2,"C",IF('Data Source'!AH16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI16&gt;=5,"A+",IF('Data Source'!AI16&gt;=4,"A",IF('Data Source'!AI16&gt;=3.5,"A-",IF('Data Source'!AI16&gt;=3,"B",IF('Data Source'!AI16&gt;=2,"C",IF('Data Source'!AI16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H17" s="8">
-        <f>IF('Data Source'!AI16&gt;=5,"A+",IF('Data Source'!AI16&gt;=4,"A",IF('Data Source'!AI16&gt;=3.5,"A-",IF('Data Source'!AI16&gt;=3,"B",IF('Data Source'!AI16&gt;=2,"C",IF('Data Source'!AI16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ16&gt;=5,"A+",IF('Data Source'!AJ16&gt;=4,"A",IF('Data Source'!AJ16&gt;=3.5,"A-",IF('Data Source'!AJ16&gt;=3,"B",IF('Data Source'!AJ16&gt;=2,"C",IF('Data Source'!AJ16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I17" s="8">
-        <f>IF('Data Source'!AJ16&gt;=5,"A+",IF('Data Source'!AJ16&gt;=4,"A",IF('Data Source'!AJ16&gt;=3.5,"A-",IF('Data Source'!AJ16&gt;=3,"B",IF('Data Source'!AJ16&gt;=2,"C",IF('Data Source'!AJ16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK16&gt;=5,"A+",IF('Data Source'!AK16&gt;=4,"A",IF('Data Source'!AK16&gt;=3.5,"A-",IF('Data Source'!AK16&gt;=3,"B",IF('Data Source'!AK16&gt;=2,"C",IF('Data Source'!AK16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J17" s="8">
-        <f>IF('Data Source'!AK16&gt;=5,"A+",IF('Data Source'!AK16&gt;=4,"A",IF('Data Source'!AK16&gt;=3.5,"A-",IF('Data Source'!AK16&gt;=3,"B",IF('Data Source'!AK16&gt;=2,"C",IF('Data Source'!AK16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL16&gt;=5,"A+",IF('Data Source'!AL16&gt;=4,"A",IF('Data Source'!AL16&gt;=3.5,"A-",IF('Data Source'!AL16&gt;=3,"B",IF('Data Source'!AL16&gt;=2,"C",IF('Data Source'!AL16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K17" s="8">
-        <f>IF('Data Source'!AL16&gt;=5,"A+",IF('Data Source'!AL16&gt;=4,"A",IF('Data Source'!AL16&gt;=3.5,"A-",IF('Data Source'!AL16&gt;=3,"B",IF('Data Source'!AL16&gt;=2,"C",IF('Data Source'!AL16&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM16&gt;=5,"A+",IF('Data Source'!AM16&gt;=4,"A",IF('Data Source'!AM16&gt;=3.5,"A-",IF('Data Source'!AM16&gt;=3,"B",IF('Data Source'!AM16&gt;=2,"C",IF('Data Source'!AM16&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L17" s="8">
@@ -5238,11 +5325,11 @@
         <v/>
       </c>
       <c r="N17" s="7">
-        <f>'Data Source'!X16</f>
+        <f>'Data Source'!Y16</f>
         <v/>
       </c>
       <c r="O17" s="8">
-        <f>'Data Source'!Y16</f>
+        <f>'Data Source'!Z16</f>
         <v/>
       </c>
     </row>
@@ -5256,39 +5343,39 @@
         <v/>
       </c>
       <c r="C18" s="8">
-        <f>IF('Data Source'!AD17&gt;=5,"A+",IF('Data Source'!AD17&gt;=4,"A",IF('Data Source'!AD17&gt;=3.5,"A-",IF('Data Source'!AD17&gt;=3,"B",IF('Data Source'!AD17&gt;=2,"C",IF('Data Source'!AD17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE17&gt;=5,"A+",IF('Data Source'!AE17&gt;=4,"A",IF('Data Source'!AE17&gt;=3.5,"A-",IF('Data Source'!AE17&gt;=3,"B",IF('Data Source'!AE17&gt;=2,"C",IF('Data Source'!AE17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D18" s="8">
-        <f>IF('Data Source'!AE17&gt;=5,"A+",IF('Data Source'!AE17&gt;=4,"A",IF('Data Source'!AE17&gt;=3.5,"A-",IF('Data Source'!AE17&gt;=3,"B",IF('Data Source'!AE17&gt;=2,"C",IF('Data Source'!AE17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF17&gt;=5,"A+",IF('Data Source'!AF17&gt;=4,"A",IF('Data Source'!AF17&gt;=3.5,"A-",IF('Data Source'!AF17&gt;=3,"B",IF('Data Source'!AF17&gt;=2,"C",IF('Data Source'!AF17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E18" s="8">
-        <f>IF('Data Source'!AF17&gt;=5,"A+",IF('Data Source'!AF17&gt;=4,"A",IF('Data Source'!AF17&gt;=3.5,"A-",IF('Data Source'!AF17&gt;=3,"B",IF('Data Source'!AF17&gt;=2,"C",IF('Data Source'!AF17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG17&gt;=5,"A+",IF('Data Source'!AG17&gt;=4,"A",IF('Data Source'!AG17&gt;=3.5,"A-",IF('Data Source'!AG17&gt;=3,"B",IF('Data Source'!AG17&gt;=2,"C",IF('Data Source'!AG17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F18" s="8">
-        <f>IF('Data Source'!AG17&gt;=5,"A+",IF('Data Source'!AG17&gt;=4,"A",IF('Data Source'!AG17&gt;=3.5,"A-",IF('Data Source'!AG17&gt;=3,"B",IF('Data Source'!AG17&gt;=2,"C",IF('Data Source'!AG17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH17&gt;=5,"A+",IF('Data Source'!AH17&gt;=4,"A",IF('Data Source'!AH17&gt;=3.5,"A-",IF('Data Source'!AH17&gt;=3,"B",IF('Data Source'!AH17&gt;=2,"C",IF('Data Source'!AH17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G18" s="8">
-        <f>IF('Data Source'!AH17&gt;=5,"A+",IF('Data Source'!AH17&gt;=4,"A",IF('Data Source'!AH17&gt;=3.5,"A-",IF('Data Source'!AH17&gt;=3,"B",IF('Data Source'!AH17&gt;=2,"C",IF('Data Source'!AH17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI17&gt;=5,"A+",IF('Data Source'!AI17&gt;=4,"A",IF('Data Source'!AI17&gt;=3.5,"A-",IF('Data Source'!AI17&gt;=3,"B",IF('Data Source'!AI17&gt;=2,"C",IF('Data Source'!AI17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H18" s="8">
-        <f>IF('Data Source'!AI17&gt;=5,"A+",IF('Data Source'!AI17&gt;=4,"A",IF('Data Source'!AI17&gt;=3.5,"A-",IF('Data Source'!AI17&gt;=3,"B",IF('Data Source'!AI17&gt;=2,"C",IF('Data Source'!AI17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ17&gt;=5,"A+",IF('Data Source'!AJ17&gt;=4,"A",IF('Data Source'!AJ17&gt;=3.5,"A-",IF('Data Source'!AJ17&gt;=3,"B",IF('Data Source'!AJ17&gt;=2,"C",IF('Data Source'!AJ17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I18" s="8">
-        <f>IF('Data Source'!AJ17&gt;=5,"A+",IF('Data Source'!AJ17&gt;=4,"A",IF('Data Source'!AJ17&gt;=3.5,"A-",IF('Data Source'!AJ17&gt;=3,"B",IF('Data Source'!AJ17&gt;=2,"C",IF('Data Source'!AJ17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK17&gt;=5,"A+",IF('Data Source'!AK17&gt;=4,"A",IF('Data Source'!AK17&gt;=3.5,"A-",IF('Data Source'!AK17&gt;=3,"B",IF('Data Source'!AK17&gt;=2,"C",IF('Data Source'!AK17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J18" s="8">
-        <f>IF('Data Source'!AK17&gt;=5,"A+",IF('Data Source'!AK17&gt;=4,"A",IF('Data Source'!AK17&gt;=3.5,"A-",IF('Data Source'!AK17&gt;=3,"B",IF('Data Source'!AK17&gt;=2,"C",IF('Data Source'!AK17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL17&gt;=5,"A+",IF('Data Source'!AL17&gt;=4,"A",IF('Data Source'!AL17&gt;=3.5,"A-",IF('Data Source'!AL17&gt;=3,"B",IF('Data Source'!AL17&gt;=2,"C",IF('Data Source'!AL17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K18" s="8">
-        <f>IF('Data Source'!AL17&gt;=5,"A+",IF('Data Source'!AL17&gt;=4,"A",IF('Data Source'!AL17&gt;=3.5,"A-",IF('Data Source'!AL17&gt;=3,"B",IF('Data Source'!AL17&gt;=2,"C",IF('Data Source'!AL17&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM17&gt;=5,"A+",IF('Data Source'!AM17&gt;=4,"A",IF('Data Source'!AM17&gt;=3.5,"A-",IF('Data Source'!AM17&gt;=3,"B",IF('Data Source'!AM17&gt;=2,"C",IF('Data Source'!AM17&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L18" s="8">
@@ -5300,11 +5387,11 @@
         <v/>
       </c>
       <c r="N18" s="7">
-        <f>'Data Source'!X17</f>
+        <f>'Data Source'!Y17</f>
         <v/>
       </c>
       <c r="O18" s="8">
-        <f>'Data Source'!Y17</f>
+        <f>'Data Source'!Z17</f>
         <v/>
       </c>
     </row>
@@ -5318,39 +5405,39 @@
         <v/>
       </c>
       <c r="C19" s="8">
-        <f>IF('Data Source'!AD18&gt;=5,"A+",IF('Data Source'!AD18&gt;=4,"A",IF('Data Source'!AD18&gt;=3.5,"A-",IF('Data Source'!AD18&gt;=3,"B",IF('Data Source'!AD18&gt;=2,"C",IF('Data Source'!AD18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE18&gt;=5,"A+",IF('Data Source'!AE18&gt;=4,"A",IF('Data Source'!AE18&gt;=3.5,"A-",IF('Data Source'!AE18&gt;=3,"B",IF('Data Source'!AE18&gt;=2,"C",IF('Data Source'!AE18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D19" s="8">
-        <f>IF('Data Source'!AE18&gt;=5,"A+",IF('Data Source'!AE18&gt;=4,"A",IF('Data Source'!AE18&gt;=3.5,"A-",IF('Data Source'!AE18&gt;=3,"B",IF('Data Source'!AE18&gt;=2,"C",IF('Data Source'!AE18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF18&gt;=5,"A+",IF('Data Source'!AF18&gt;=4,"A",IF('Data Source'!AF18&gt;=3.5,"A-",IF('Data Source'!AF18&gt;=3,"B",IF('Data Source'!AF18&gt;=2,"C",IF('Data Source'!AF18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E19" s="8">
-        <f>IF('Data Source'!AF18&gt;=5,"A+",IF('Data Source'!AF18&gt;=4,"A",IF('Data Source'!AF18&gt;=3.5,"A-",IF('Data Source'!AF18&gt;=3,"B",IF('Data Source'!AF18&gt;=2,"C",IF('Data Source'!AF18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG18&gt;=5,"A+",IF('Data Source'!AG18&gt;=4,"A",IF('Data Source'!AG18&gt;=3.5,"A-",IF('Data Source'!AG18&gt;=3,"B",IF('Data Source'!AG18&gt;=2,"C",IF('Data Source'!AG18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F19" s="8">
-        <f>IF('Data Source'!AG18&gt;=5,"A+",IF('Data Source'!AG18&gt;=4,"A",IF('Data Source'!AG18&gt;=3.5,"A-",IF('Data Source'!AG18&gt;=3,"B",IF('Data Source'!AG18&gt;=2,"C",IF('Data Source'!AG18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH18&gt;=5,"A+",IF('Data Source'!AH18&gt;=4,"A",IF('Data Source'!AH18&gt;=3.5,"A-",IF('Data Source'!AH18&gt;=3,"B",IF('Data Source'!AH18&gt;=2,"C",IF('Data Source'!AH18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G19" s="8">
-        <f>IF('Data Source'!AH18&gt;=5,"A+",IF('Data Source'!AH18&gt;=4,"A",IF('Data Source'!AH18&gt;=3.5,"A-",IF('Data Source'!AH18&gt;=3,"B",IF('Data Source'!AH18&gt;=2,"C",IF('Data Source'!AH18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI18&gt;=5,"A+",IF('Data Source'!AI18&gt;=4,"A",IF('Data Source'!AI18&gt;=3.5,"A-",IF('Data Source'!AI18&gt;=3,"B",IF('Data Source'!AI18&gt;=2,"C",IF('Data Source'!AI18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H19" s="8">
-        <f>IF('Data Source'!AI18&gt;=5,"A+",IF('Data Source'!AI18&gt;=4,"A",IF('Data Source'!AI18&gt;=3.5,"A-",IF('Data Source'!AI18&gt;=3,"B",IF('Data Source'!AI18&gt;=2,"C",IF('Data Source'!AI18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ18&gt;=5,"A+",IF('Data Source'!AJ18&gt;=4,"A",IF('Data Source'!AJ18&gt;=3.5,"A-",IF('Data Source'!AJ18&gt;=3,"B",IF('Data Source'!AJ18&gt;=2,"C",IF('Data Source'!AJ18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I19" s="8">
-        <f>IF('Data Source'!AJ18&gt;=5,"A+",IF('Data Source'!AJ18&gt;=4,"A",IF('Data Source'!AJ18&gt;=3.5,"A-",IF('Data Source'!AJ18&gt;=3,"B",IF('Data Source'!AJ18&gt;=2,"C",IF('Data Source'!AJ18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK18&gt;=5,"A+",IF('Data Source'!AK18&gt;=4,"A",IF('Data Source'!AK18&gt;=3.5,"A-",IF('Data Source'!AK18&gt;=3,"B",IF('Data Source'!AK18&gt;=2,"C",IF('Data Source'!AK18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J19" s="8">
-        <f>IF('Data Source'!AK18&gt;=5,"A+",IF('Data Source'!AK18&gt;=4,"A",IF('Data Source'!AK18&gt;=3.5,"A-",IF('Data Source'!AK18&gt;=3,"B",IF('Data Source'!AK18&gt;=2,"C",IF('Data Source'!AK18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL18&gt;=5,"A+",IF('Data Source'!AL18&gt;=4,"A",IF('Data Source'!AL18&gt;=3.5,"A-",IF('Data Source'!AL18&gt;=3,"B",IF('Data Source'!AL18&gt;=2,"C",IF('Data Source'!AL18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K19" s="8">
-        <f>IF('Data Source'!AL18&gt;=5,"A+",IF('Data Source'!AL18&gt;=4,"A",IF('Data Source'!AL18&gt;=3.5,"A-",IF('Data Source'!AL18&gt;=3,"B",IF('Data Source'!AL18&gt;=2,"C",IF('Data Source'!AL18&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM18&gt;=5,"A+",IF('Data Source'!AM18&gt;=4,"A",IF('Data Source'!AM18&gt;=3.5,"A-",IF('Data Source'!AM18&gt;=3,"B",IF('Data Source'!AM18&gt;=2,"C",IF('Data Source'!AM18&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L19" s="8">
@@ -5362,11 +5449,11 @@
         <v/>
       </c>
       <c r="N19" s="7">
-        <f>'Data Source'!X18</f>
+        <f>'Data Source'!Y18</f>
         <v/>
       </c>
       <c r="O19" s="8">
-        <f>'Data Source'!Y18</f>
+        <f>'Data Source'!Z18</f>
         <v/>
       </c>
     </row>
@@ -5380,39 +5467,39 @@
         <v/>
       </c>
       <c r="C20" s="8">
-        <f>IF('Data Source'!AD19&gt;=5,"A+",IF('Data Source'!AD19&gt;=4,"A",IF('Data Source'!AD19&gt;=3.5,"A-",IF('Data Source'!AD19&gt;=3,"B",IF('Data Source'!AD19&gt;=2,"C",IF('Data Source'!AD19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE19&gt;=5,"A+",IF('Data Source'!AE19&gt;=4,"A",IF('Data Source'!AE19&gt;=3.5,"A-",IF('Data Source'!AE19&gt;=3,"B",IF('Data Source'!AE19&gt;=2,"C",IF('Data Source'!AE19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D20" s="8">
-        <f>IF('Data Source'!AE19&gt;=5,"A+",IF('Data Source'!AE19&gt;=4,"A",IF('Data Source'!AE19&gt;=3.5,"A-",IF('Data Source'!AE19&gt;=3,"B",IF('Data Source'!AE19&gt;=2,"C",IF('Data Source'!AE19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF19&gt;=5,"A+",IF('Data Source'!AF19&gt;=4,"A",IF('Data Source'!AF19&gt;=3.5,"A-",IF('Data Source'!AF19&gt;=3,"B",IF('Data Source'!AF19&gt;=2,"C",IF('Data Source'!AF19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E20" s="8">
-        <f>IF('Data Source'!AF19&gt;=5,"A+",IF('Data Source'!AF19&gt;=4,"A",IF('Data Source'!AF19&gt;=3.5,"A-",IF('Data Source'!AF19&gt;=3,"B",IF('Data Source'!AF19&gt;=2,"C",IF('Data Source'!AF19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG19&gt;=5,"A+",IF('Data Source'!AG19&gt;=4,"A",IF('Data Source'!AG19&gt;=3.5,"A-",IF('Data Source'!AG19&gt;=3,"B",IF('Data Source'!AG19&gt;=2,"C",IF('Data Source'!AG19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F20" s="8">
-        <f>IF('Data Source'!AG19&gt;=5,"A+",IF('Data Source'!AG19&gt;=4,"A",IF('Data Source'!AG19&gt;=3.5,"A-",IF('Data Source'!AG19&gt;=3,"B",IF('Data Source'!AG19&gt;=2,"C",IF('Data Source'!AG19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH19&gt;=5,"A+",IF('Data Source'!AH19&gt;=4,"A",IF('Data Source'!AH19&gt;=3.5,"A-",IF('Data Source'!AH19&gt;=3,"B",IF('Data Source'!AH19&gt;=2,"C",IF('Data Source'!AH19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G20" s="8">
-        <f>IF('Data Source'!AH19&gt;=5,"A+",IF('Data Source'!AH19&gt;=4,"A",IF('Data Source'!AH19&gt;=3.5,"A-",IF('Data Source'!AH19&gt;=3,"B",IF('Data Source'!AH19&gt;=2,"C",IF('Data Source'!AH19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI19&gt;=5,"A+",IF('Data Source'!AI19&gt;=4,"A",IF('Data Source'!AI19&gt;=3.5,"A-",IF('Data Source'!AI19&gt;=3,"B",IF('Data Source'!AI19&gt;=2,"C",IF('Data Source'!AI19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H20" s="8">
-        <f>IF('Data Source'!AI19&gt;=5,"A+",IF('Data Source'!AI19&gt;=4,"A",IF('Data Source'!AI19&gt;=3.5,"A-",IF('Data Source'!AI19&gt;=3,"B",IF('Data Source'!AI19&gt;=2,"C",IF('Data Source'!AI19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ19&gt;=5,"A+",IF('Data Source'!AJ19&gt;=4,"A",IF('Data Source'!AJ19&gt;=3.5,"A-",IF('Data Source'!AJ19&gt;=3,"B",IF('Data Source'!AJ19&gt;=2,"C",IF('Data Source'!AJ19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I20" s="8">
-        <f>IF('Data Source'!AJ19&gt;=5,"A+",IF('Data Source'!AJ19&gt;=4,"A",IF('Data Source'!AJ19&gt;=3.5,"A-",IF('Data Source'!AJ19&gt;=3,"B",IF('Data Source'!AJ19&gt;=2,"C",IF('Data Source'!AJ19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK19&gt;=5,"A+",IF('Data Source'!AK19&gt;=4,"A",IF('Data Source'!AK19&gt;=3.5,"A-",IF('Data Source'!AK19&gt;=3,"B",IF('Data Source'!AK19&gt;=2,"C",IF('Data Source'!AK19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J20" s="8">
-        <f>IF('Data Source'!AK19&gt;=5,"A+",IF('Data Source'!AK19&gt;=4,"A",IF('Data Source'!AK19&gt;=3.5,"A-",IF('Data Source'!AK19&gt;=3,"B",IF('Data Source'!AK19&gt;=2,"C",IF('Data Source'!AK19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL19&gt;=5,"A+",IF('Data Source'!AL19&gt;=4,"A",IF('Data Source'!AL19&gt;=3.5,"A-",IF('Data Source'!AL19&gt;=3,"B",IF('Data Source'!AL19&gt;=2,"C",IF('Data Source'!AL19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K20" s="8">
-        <f>IF('Data Source'!AL19&gt;=5,"A+",IF('Data Source'!AL19&gt;=4,"A",IF('Data Source'!AL19&gt;=3.5,"A-",IF('Data Source'!AL19&gt;=3,"B",IF('Data Source'!AL19&gt;=2,"C",IF('Data Source'!AL19&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM19&gt;=5,"A+",IF('Data Source'!AM19&gt;=4,"A",IF('Data Source'!AM19&gt;=3.5,"A-",IF('Data Source'!AM19&gt;=3,"B",IF('Data Source'!AM19&gt;=2,"C",IF('Data Source'!AM19&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L20" s="8">
@@ -5424,11 +5511,11 @@
         <v/>
       </c>
       <c r="N20" s="7">
-        <f>'Data Source'!X19</f>
+        <f>'Data Source'!Y19</f>
         <v/>
       </c>
       <c r="O20" s="8">
-        <f>'Data Source'!Y19</f>
+        <f>'Data Source'!Z19</f>
         <v/>
       </c>
     </row>
@@ -5442,39 +5529,39 @@
         <v/>
       </c>
       <c r="C21" s="8">
-        <f>IF('Data Source'!AD20&gt;=5,"A+",IF('Data Source'!AD20&gt;=4,"A",IF('Data Source'!AD20&gt;=3.5,"A-",IF('Data Source'!AD20&gt;=3,"B",IF('Data Source'!AD20&gt;=2,"C",IF('Data Source'!AD20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE20&gt;=5,"A+",IF('Data Source'!AE20&gt;=4,"A",IF('Data Source'!AE20&gt;=3.5,"A-",IF('Data Source'!AE20&gt;=3,"B",IF('Data Source'!AE20&gt;=2,"C",IF('Data Source'!AE20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D21" s="8">
-        <f>IF('Data Source'!AE20&gt;=5,"A+",IF('Data Source'!AE20&gt;=4,"A",IF('Data Source'!AE20&gt;=3.5,"A-",IF('Data Source'!AE20&gt;=3,"B",IF('Data Source'!AE20&gt;=2,"C",IF('Data Source'!AE20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF20&gt;=5,"A+",IF('Data Source'!AF20&gt;=4,"A",IF('Data Source'!AF20&gt;=3.5,"A-",IF('Data Source'!AF20&gt;=3,"B",IF('Data Source'!AF20&gt;=2,"C",IF('Data Source'!AF20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E21" s="8">
-        <f>IF('Data Source'!AF20&gt;=5,"A+",IF('Data Source'!AF20&gt;=4,"A",IF('Data Source'!AF20&gt;=3.5,"A-",IF('Data Source'!AF20&gt;=3,"B",IF('Data Source'!AF20&gt;=2,"C",IF('Data Source'!AF20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG20&gt;=5,"A+",IF('Data Source'!AG20&gt;=4,"A",IF('Data Source'!AG20&gt;=3.5,"A-",IF('Data Source'!AG20&gt;=3,"B",IF('Data Source'!AG20&gt;=2,"C",IF('Data Source'!AG20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F21" s="8">
-        <f>IF('Data Source'!AG20&gt;=5,"A+",IF('Data Source'!AG20&gt;=4,"A",IF('Data Source'!AG20&gt;=3.5,"A-",IF('Data Source'!AG20&gt;=3,"B",IF('Data Source'!AG20&gt;=2,"C",IF('Data Source'!AG20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH20&gt;=5,"A+",IF('Data Source'!AH20&gt;=4,"A",IF('Data Source'!AH20&gt;=3.5,"A-",IF('Data Source'!AH20&gt;=3,"B",IF('Data Source'!AH20&gt;=2,"C",IF('Data Source'!AH20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G21" s="8">
-        <f>IF('Data Source'!AH20&gt;=5,"A+",IF('Data Source'!AH20&gt;=4,"A",IF('Data Source'!AH20&gt;=3.5,"A-",IF('Data Source'!AH20&gt;=3,"B",IF('Data Source'!AH20&gt;=2,"C",IF('Data Source'!AH20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI20&gt;=5,"A+",IF('Data Source'!AI20&gt;=4,"A",IF('Data Source'!AI20&gt;=3.5,"A-",IF('Data Source'!AI20&gt;=3,"B",IF('Data Source'!AI20&gt;=2,"C",IF('Data Source'!AI20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H21" s="8">
-        <f>IF('Data Source'!AI20&gt;=5,"A+",IF('Data Source'!AI20&gt;=4,"A",IF('Data Source'!AI20&gt;=3.5,"A-",IF('Data Source'!AI20&gt;=3,"B",IF('Data Source'!AI20&gt;=2,"C",IF('Data Source'!AI20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ20&gt;=5,"A+",IF('Data Source'!AJ20&gt;=4,"A",IF('Data Source'!AJ20&gt;=3.5,"A-",IF('Data Source'!AJ20&gt;=3,"B",IF('Data Source'!AJ20&gt;=2,"C",IF('Data Source'!AJ20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I21" s="8">
-        <f>IF('Data Source'!AJ20&gt;=5,"A+",IF('Data Source'!AJ20&gt;=4,"A",IF('Data Source'!AJ20&gt;=3.5,"A-",IF('Data Source'!AJ20&gt;=3,"B",IF('Data Source'!AJ20&gt;=2,"C",IF('Data Source'!AJ20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK20&gt;=5,"A+",IF('Data Source'!AK20&gt;=4,"A",IF('Data Source'!AK20&gt;=3.5,"A-",IF('Data Source'!AK20&gt;=3,"B",IF('Data Source'!AK20&gt;=2,"C",IF('Data Source'!AK20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J21" s="8">
-        <f>IF('Data Source'!AK20&gt;=5,"A+",IF('Data Source'!AK20&gt;=4,"A",IF('Data Source'!AK20&gt;=3.5,"A-",IF('Data Source'!AK20&gt;=3,"B",IF('Data Source'!AK20&gt;=2,"C",IF('Data Source'!AK20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL20&gt;=5,"A+",IF('Data Source'!AL20&gt;=4,"A",IF('Data Source'!AL20&gt;=3.5,"A-",IF('Data Source'!AL20&gt;=3,"B",IF('Data Source'!AL20&gt;=2,"C",IF('Data Source'!AL20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K21" s="8">
-        <f>IF('Data Source'!AL20&gt;=5,"A+",IF('Data Source'!AL20&gt;=4,"A",IF('Data Source'!AL20&gt;=3.5,"A-",IF('Data Source'!AL20&gt;=3,"B",IF('Data Source'!AL20&gt;=2,"C",IF('Data Source'!AL20&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM20&gt;=5,"A+",IF('Data Source'!AM20&gt;=4,"A",IF('Data Source'!AM20&gt;=3.5,"A-",IF('Data Source'!AM20&gt;=3,"B",IF('Data Source'!AM20&gt;=2,"C",IF('Data Source'!AM20&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L21" s="8">
@@ -5486,11 +5573,11 @@
         <v/>
       </c>
       <c r="N21" s="7">
-        <f>'Data Source'!X20</f>
+        <f>'Data Source'!Y20</f>
         <v/>
       </c>
       <c r="O21" s="8">
-        <f>'Data Source'!Y20</f>
+        <f>'Data Source'!Z20</f>
         <v/>
       </c>
     </row>
@@ -5504,39 +5591,39 @@
         <v/>
       </c>
       <c r="C22" s="8">
-        <f>IF('Data Source'!AD21&gt;=5,"A+",IF('Data Source'!AD21&gt;=4,"A",IF('Data Source'!AD21&gt;=3.5,"A-",IF('Data Source'!AD21&gt;=3,"B",IF('Data Source'!AD21&gt;=2,"C",IF('Data Source'!AD21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AE21&gt;=5,"A+",IF('Data Source'!AE21&gt;=4,"A",IF('Data Source'!AE21&gt;=3.5,"A-",IF('Data Source'!AE21&gt;=3,"B",IF('Data Source'!AE21&gt;=2,"C",IF('Data Source'!AE21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="D22" s="8">
-        <f>IF('Data Source'!AE21&gt;=5,"A+",IF('Data Source'!AE21&gt;=4,"A",IF('Data Source'!AE21&gt;=3.5,"A-",IF('Data Source'!AE21&gt;=3,"B",IF('Data Source'!AE21&gt;=2,"C",IF('Data Source'!AE21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AF21&gt;=5,"A+",IF('Data Source'!AF21&gt;=4,"A",IF('Data Source'!AF21&gt;=3.5,"A-",IF('Data Source'!AF21&gt;=3,"B",IF('Data Source'!AF21&gt;=2,"C",IF('Data Source'!AF21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="E22" s="8">
-        <f>IF('Data Source'!AF21&gt;=5,"A+",IF('Data Source'!AF21&gt;=4,"A",IF('Data Source'!AF21&gt;=3.5,"A-",IF('Data Source'!AF21&gt;=3,"B",IF('Data Source'!AF21&gt;=2,"C",IF('Data Source'!AF21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AG21&gt;=5,"A+",IF('Data Source'!AG21&gt;=4,"A",IF('Data Source'!AG21&gt;=3.5,"A-",IF('Data Source'!AG21&gt;=3,"B",IF('Data Source'!AG21&gt;=2,"C",IF('Data Source'!AG21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="F22" s="8">
-        <f>IF('Data Source'!AG21&gt;=5,"A+",IF('Data Source'!AG21&gt;=4,"A",IF('Data Source'!AG21&gt;=3.5,"A-",IF('Data Source'!AG21&gt;=3,"B",IF('Data Source'!AG21&gt;=2,"C",IF('Data Source'!AG21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AH21&gt;=5,"A+",IF('Data Source'!AH21&gt;=4,"A",IF('Data Source'!AH21&gt;=3.5,"A-",IF('Data Source'!AH21&gt;=3,"B",IF('Data Source'!AH21&gt;=2,"C",IF('Data Source'!AH21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="G22" s="8">
-        <f>IF('Data Source'!AH21&gt;=5,"A+",IF('Data Source'!AH21&gt;=4,"A",IF('Data Source'!AH21&gt;=3.5,"A-",IF('Data Source'!AH21&gt;=3,"B",IF('Data Source'!AH21&gt;=2,"C",IF('Data Source'!AH21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AI21&gt;=5,"A+",IF('Data Source'!AI21&gt;=4,"A",IF('Data Source'!AI21&gt;=3.5,"A-",IF('Data Source'!AI21&gt;=3,"B",IF('Data Source'!AI21&gt;=2,"C",IF('Data Source'!AI21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="H22" s="8">
-        <f>IF('Data Source'!AI21&gt;=5,"A+",IF('Data Source'!AI21&gt;=4,"A",IF('Data Source'!AI21&gt;=3.5,"A-",IF('Data Source'!AI21&gt;=3,"B",IF('Data Source'!AI21&gt;=2,"C",IF('Data Source'!AI21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AJ21&gt;=5,"A+",IF('Data Source'!AJ21&gt;=4,"A",IF('Data Source'!AJ21&gt;=3.5,"A-",IF('Data Source'!AJ21&gt;=3,"B",IF('Data Source'!AJ21&gt;=2,"C",IF('Data Source'!AJ21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="I22" s="8">
-        <f>IF('Data Source'!AJ21&gt;=5,"A+",IF('Data Source'!AJ21&gt;=4,"A",IF('Data Source'!AJ21&gt;=3.5,"A-",IF('Data Source'!AJ21&gt;=3,"B",IF('Data Source'!AJ21&gt;=2,"C",IF('Data Source'!AJ21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AK21&gt;=5,"A+",IF('Data Source'!AK21&gt;=4,"A",IF('Data Source'!AK21&gt;=3.5,"A-",IF('Data Source'!AK21&gt;=3,"B",IF('Data Source'!AK21&gt;=2,"C",IF('Data Source'!AK21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="J22" s="8">
-        <f>IF('Data Source'!AK21&gt;=5,"A+",IF('Data Source'!AK21&gt;=4,"A",IF('Data Source'!AK21&gt;=3.5,"A-",IF('Data Source'!AK21&gt;=3,"B",IF('Data Source'!AK21&gt;=2,"C",IF('Data Source'!AK21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AL21&gt;=5,"A+",IF('Data Source'!AL21&gt;=4,"A",IF('Data Source'!AL21&gt;=3.5,"A-",IF('Data Source'!AL21&gt;=3,"B",IF('Data Source'!AL21&gt;=2,"C",IF('Data Source'!AL21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="K22" s="8">
-        <f>IF('Data Source'!AL21&gt;=5,"A+",IF('Data Source'!AL21&gt;=4,"A",IF('Data Source'!AL21&gt;=3.5,"A-",IF('Data Source'!AL21&gt;=3,"B",IF('Data Source'!AL21&gt;=2,"C",IF('Data Source'!AL21&gt;=1,"D","F"))))))</f>
+        <f>IF('Data Source'!AM21&gt;=5,"A+",IF('Data Source'!AM21&gt;=4,"A",IF('Data Source'!AM21&gt;=3.5,"A-",IF('Data Source'!AM21&gt;=3,"B",IF('Data Source'!AM21&gt;=2,"C",IF('Data Source'!AM21&gt;=1,"D","F"))))))</f>
         <v/>
       </c>
       <c r="L22" s="8">
@@ -5548,11 +5635,11 @@
         <v/>
       </c>
       <c r="N22" s="7">
-        <f>'Data Source'!X21</f>
+        <f>'Data Source'!Y21</f>
         <v/>
       </c>
       <c r="O22" s="8">
-        <f>'Data Source'!Y21</f>
+        <f>'Data Source'!Z21</f>
         <v/>
       </c>
     </row>
@@ -5565,6 +5652,1283 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="18" t="inlineStr">
+        <is>
+          <t>SUBJECT-WISE GPA (GRADE POINTS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="B2" s="19" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" s="19" t="inlineStr">
+        <is>
+          <t>Quran+Hadith GP</t>
+        </is>
+      </c>
+      <c r="D2" s="19" t="inlineStr">
+        <is>
+          <t>Arabic GP</t>
+        </is>
+      </c>
+      <c r="E2" s="19" t="inlineStr">
+        <is>
+          <t>Aqaid GP</t>
+        </is>
+      </c>
+      <c r="F2" s="19" t="inlineStr">
+        <is>
+          <t>English GP</t>
+        </is>
+      </c>
+      <c r="G2" s="19" t="inlineStr">
+        <is>
+          <t>Bangla GP</t>
+        </is>
+      </c>
+      <c r="H2" s="19" t="inlineStr">
+        <is>
+          <t>Math GP</t>
+        </is>
+      </c>
+      <c r="I2" s="19" t="inlineStr">
+        <is>
+          <t>History GP</t>
+        </is>
+      </c>
+      <c r="J2" s="19" t="inlineStr">
+        <is>
+          <t>ICT GP</t>
+        </is>
+      </c>
+      <c r="K2" s="19" t="inlineStr">
+        <is>
+          <t>Mantiq GP</t>
+        </is>
+      </c>
+      <c r="L2" s="19" t="inlineStr">
+        <is>
+          <t>Base GPA</t>
+        </is>
+      </c>
+      <c r="M2" s="19" t="inlineStr">
+        <is>
+          <t>Final GPA</t>
+        </is>
+      </c>
+      <c r="N2" s="19" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8">
+        <f>'Data Source'!A2</f>
+        <v/>
+      </c>
+      <c r="B3">
+        <f>'Data Source'!B2</f>
+        <v/>
+      </c>
+      <c r="C3" s="7">
+        <f>'Data Source'!AE2</f>
+        <v/>
+      </c>
+      <c r="D3" s="7">
+        <f>'Data Source'!AF2</f>
+        <v/>
+      </c>
+      <c r="E3" s="7">
+        <f>'Data Source'!AG2</f>
+        <v/>
+      </c>
+      <c r="F3" s="7">
+        <f>'Data Source'!AH2</f>
+        <v/>
+      </c>
+      <c r="G3" s="7">
+        <f>'Data Source'!AI2</f>
+        <v/>
+      </c>
+      <c r="H3" s="7">
+        <f>'Data Source'!AJ2</f>
+        <v/>
+      </c>
+      <c r="I3" s="7">
+        <f>'Data Source'!AK2</f>
+        <v/>
+      </c>
+      <c r="J3" s="7">
+        <f>'Data Source'!AL2</f>
+        <v/>
+      </c>
+      <c r="K3" s="7">
+        <f>'Data Source'!AM2</f>
+        <v/>
+      </c>
+      <c r="L3" s="7">
+        <f>'Data Source'!AN2</f>
+        <v/>
+      </c>
+      <c r="M3" s="7">
+        <f>'Data Source'!Y2</f>
+        <v/>
+      </c>
+      <c r="N3" s="8">
+        <f>'Data Source'!Z2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <f>'Data Source'!A3</f>
+        <v/>
+      </c>
+      <c r="B4">
+        <f>'Data Source'!B3</f>
+        <v/>
+      </c>
+      <c r="C4" s="7">
+        <f>'Data Source'!AE3</f>
+        <v/>
+      </c>
+      <c r="D4" s="7">
+        <f>'Data Source'!AF3</f>
+        <v/>
+      </c>
+      <c r="E4" s="7">
+        <f>'Data Source'!AG3</f>
+        <v/>
+      </c>
+      <c r="F4" s="7">
+        <f>'Data Source'!AH3</f>
+        <v/>
+      </c>
+      <c r="G4" s="7">
+        <f>'Data Source'!AI3</f>
+        <v/>
+      </c>
+      <c r="H4" s="7">
+        <f>'Data Source'!AJ3</f>
+        <v/>
+      </c>
+      <c r="I4" s="7">
+        <f>'Data Source'!AK3</f>
+        <v/>
+      </c>
+      <c r="J4" s="7">
+        <f>'Data Source'!AL3</f>
+        <v/>
+      </c>
+      <c r="K4" s="7">
+        <f>'Data Source'!AM3</f>
+        <v/>
+      </c>
+      <c r="L4" s="7">
+        <f>'Data Source'!AN3</f>
+        <v/>
+      </c>
+      <c r="M4" s="7">
+        <f>'Data Source'!Y3</f>
+        <v/>
+      </c>
+      <c r="N4" s="8">
+        <f>'Data Source'!Z3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <f>'Data Source'!A4</f>
+        <v/>
+      </c>
+      <c r="B5">
+        <f>'Data Source'!B4</f>
+        <v/>
+      </c>
+      <c r="C5" s="7">
+        <f>'Data Source'!AE4</f>
+        <v/>
+      </c>
+      <c r="D5" s="7">
+        <f>'Data Source'!AF4</f>
+        <v/>
+      </c>
+      <c r="E5" s="7">
+        <f>'Data Source'!AG4</f>
+        <v/>
+      </c>
+      <c r="F5" s="7">
+        <f>'Data Source'!AH4</f>
+        <v/>
+      </c>
+      <c r="G5" s="7">
+        <f>'Data Source'!AI4</f>
+        <v/>
+      </c>
+      <c r="H5" s="7">
+        <f>'Data Source'!AJ4</f>
+        <v/>
+      </c>
+      <c r="I5" s="7">
+        <f>'Data Source'!AK4</f>
+        <v/>
+      </c>
+      <c r="J5" s="7">
+        <f>'Data Source'!AL4</f>
+        <v/>
+      </c>
+      <c r="K5" s="7">
+        <f>'Data Source'!AM4</f>
+        <v/>
+      </c>
+      <c r="L5" s="7">
+        <f>'Data Source'!AN4</f>
+        <v/>
+      </c>
+      <c r="M5" s="7">
+        <f>'Data Source'!Y4</f>
+        <v/>
+      </c>
+      <c r="N5" s="8">
+        <f>'Data Source'!Z4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8">
+        <f>'Data Source'!A5</f>
+        <v/>
+      </c>
+      <c r="B6">
+        <f>'Data Source'!B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="7">
+        <f>'Data Source'!AE5</f>
+        <v/>
+      </c>
+      <c r="D6" s="7">
+        <f>'Data Source'!AF5</f>
+        <v/>
+      </c>
+      <c r="E6" s="7">
+        <f>'Data Source'!AG5</f>
+        <v/>
+      </c>
+      <c r="F6" s="7">
+        <f>'Data Source'!AH5</f>
+        <v/>
+      </c>
+      <c r="G6" s="7">
+        <f>'Data Source'!AI5</f>
+        <v/>
+      </c>
+      <c r="H6" s="7">
+        <f>'Data Source'!AJ5</f>
+        <v/>
+      </c>
+      <c r="I6" s="7">
+        <f>'Data Source'!AK5</f>
+        <v/>
+      </c>
+      <c r="J6" s="7">
+        <f>'Data Source'!AL5</f>
+        <v/>
+      </c>
+      <c r="K6" s="7">
+        <f>'Data Source'!AM5</f>
+        <v/>
+      </c>
+      <c r="L6" s="7">
+        <f>'Data Source'!AN5</f>
+        <v/>
+      </c>
+      <c r="M6" s="7">
+        <f>'Data Source'!Y5</f>
+        <v/>
+      </c>
+      <c r="N6" s="8">
+        <f>'Data Source'!Z5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8">
+        <f>'Data Source'!A6</f>
+        <v/>
+      </c>
+      <c r="B7">
+        <f>'Data Source'!B6</f>
+        <v/>
+      </c>
+      <c r="C7" s="7">
+        <f>'Data Source'!AE6</f>
+        <v/>
+      </c>
+      <c r="D7" s="7">
+        <f>'Data Source'!AF6</f>
+        <v/>
+      </c>
+      <c r="E7" s="7">
+        <f>'Data Source'!AG6</f>
+        <v/>
+      </c>
+      <c r="F7" s="7">
+        <f>'Data Source'!AH6</f>
+        <v/>
+      </c>
+      <c r="G7" s="7">
+        <f>'Data Source'!AI6</f>
+        <v/>
+      </c>
+      <c r="H7" s="7">
+        <f>'Data Source'!AJ6</f>
+        <v/>
+      </c>
+      <c r="I7" s="7">
+        <f>'Data Source'!AK6</f>
+        <v/>
+      </c>
+      <c r="J7" s="7">
+        <f>'Data Source'!AL6</f>
+        <v/>
+      </c>
+      <c r="K7" s="7">
+        <f>'Data Source'!AM6</f>
+        <v/>
+      </c>
+      <c r="L7" s="7">
+        <f>'Data Source'!AN6</f>
+        <v/>
+      </c>
+      <c r="M7" s="7">
+        <f>'Data Source'!Y6</f>
+        <v/>
+      </c>
+      <c r="N7" s="8">
+        <f>'Data Source'!Z6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8">
+        <f>'Data Source'!A7</f>
+        <v/>
+      </c>
+      <c r="B8">
+        <f>'Data Source'!B7</f>
+        <v/>
+      </c>
+      <c r="C8" s="7">
+        <f>'Data Source'!AE7</f>
+        <v/>
+      </c>
+      <c r="D8" s="7">
+        <f>'Data Source'!AF7</f>
+        <v/>
+      </c>
+      <c r="E8" s="7">
+        <f>'Data Source'!AG7</f>
+        <v/>
+      </c>
+      <c r="F8" s="7">
+        <f>'Data Source'!AH7</f>
+        <v/>
+      </c>
+      <c r="G8" s="7">
+        <f>'Data Source'!AI7</f>
+        <v/>
+      </c>
+      <c r="H8" s="7">
+        <f>'Data Source'!AJ7</f>
+        <v/>
+      </c>
+      <c r="I8" s="7">
+        <f>'Data Source'!AK7</f>
+        <v/>
+      </c>
+      <c r="J8" s="7">
+        <f>'Data Source'!AL7</f>
+        <v/>
+      </c>
+      <c r="K8" s="7">
+        <f>'Data Source'!AM7</f>
+        <v/>
+      </c>
+      <c r="L8" s="7">
+        <f>'Data Source'!AN7</f>
+        <v/>
+      </c>
+      <c r="M8" s="7">
+        <f>'Data Source'!Y7</f>
+        <v/>
+      </c>
+      <c r="N8" s="8">
+        <f>'Data Source'!Z7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
+        <f>'Data Source'!A8</f>
+        <v/>
+      </c>
+      <c r="B9">
+        <f>'Data Source'!B8</f>
+        <v/>
+      </c>
+      <c r="C9" s="7">
+        <f>'Data Source'!AE8</f>
+        <v/>
+      </c>
+      <c r="D9" s="7">
+        <f>'Data Source'!AF8</f>
+        <v/>
+      </c>
+      <c r="E9" s="7">
+        <f>'Data Source'!AG8</f>
+        <v/>
+      </c>
+      <c r="F9" s="7">
+        <f>'Data Source'!AH8</f>
+        <v/>
+      </c>
+      <c r="G9" s="7">
+        <f>'Data Source'!AI8</f>
+        <v/>
+      </c>
+      <c r="H9" s="7">
+        <f>'Data Source'!AJ8</f>
+        <v/>
+      </c>
+      <c r="I9" s="7">
+        <f>'Data Source'!AK8</f>
+        <v/>
+      </c>
+      <c r="J9" s="7">
+        <f>'Data Source'!AL8</f>
+        <v/>
+      </c>
+      <c r="K9" s="7">
+        <f>'Data Source'!AM8</f>
+        <v/>
+      </c>
+      <c r="L9" s="7">
+        <f>'Data Source'!AN8</f>
+        <v/>
+      </c>
+      <c r="M9" s="7">
+        <f>'Data Source'!Y8</f>
+        <v/>
+      </c>
+      <c r="N9" s="8">
+        <f>'Data Source'!Z8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8">
+        <f>'Data Source'!A9</f>
+        <v/>
+      </c>
+      <c r="B10">
+        <f>'Data Source'!B9</f>
+        <v/>
+      </c>
+      <c r="C10" s="7">
+        <f>'Data Source'!AE9</f>
+        <v/>
+      </c>
+      <c r="D10" s="7">
+        <f>'Data Source'!AF9</f>
+        <v/>
+      </c>
+      <c r="E10" s="7">
+        <f>'Data Source'!AG9</f>
+        <v/>
+      </c>
+      <c r="F10" s="7">
+        <f>'Data Source'!AH9</f>
+        <v/>
+      </c>
+      <c r="G10" s="7">
+        <f>'Data Source'!AI9</f>
+        <v/>
+      </c>
+      <c r="H10" s="7">
+        <f>'Data Source'!AJ9</f>
+        <v/>
+      </c>
+      <c r="I10" s="7">
+        <f>'Data Source'!AK9</f>
+        <v/>
+      </c>
+      <c r="J10" s="7">
+        <f>'Data Source'!AL9</f>
+        <v/>
+      </c>
+      <c r="K10" s="7">
+        <f>'Data Source'!AM9</f>
+        <v/>
+      </c>
+      <c r="L10" s="7">
+        <f>'Data Source'!AN9</f>
+        <v/>
+      </c>
+      <c r="M10" s="7">
+        <f>'Data Source'!Y9</f>
+        <v/>
+      </c>
+      <c r="N10" s="8">
+        <f>'Data Source'!Z9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <f>'Data Source'!A10</f>
+        <v/>
+      </c>
+      <c r="B11">
+        <f>'Data Source'!B10</f>
+        <v/>
+      </c>
+      <c r="C11" s="7">
+        <f>'Data Source'!AE10</f>
+        <v/>
+      </c>
+      <c r="D11" s="7">
+        <f>'Data Source'!AF10</f>
+        <v/>
+      </c>
+      <c r="E11" s="7">
+        <f>'Data Source'!AG10</f>
+        <v/>
+      </c>
+      <c r="F11" s="7">
+        <f>'Data Source'!AH10</f>
+        <v/>
+      </c>
+      <c r="G11" s="7">
+        <f>'Data Source'!AI10</f>
+        <v/>
+      </c>
+      <c r="H11" s="7">
+        <f>'Data Source'!AJ10</f>
+        <v/>
+      </c>
+      <c r="I11" s="7">
+        <f>'Data Source'!AK10</f>
+        <v/>
+      </c>
+      <c r="J11" s="7">
+        <f>'Data Source'!AL10</f>
+        <v/>
+      </c>
+      <c r="K11" s="7">
+        <f>'Data Source'!AM10</f>
+        <v/>
+      </c>
+      <c r="L11" s="7">
+        <f>'Data Source'!AN10</f>
+        <v/>
+      </c>
+      <c r="M11" s="7">
+        <f>'Data Source'!Y10</f>
+        <v/>
+      </c>
+      <c r="N11" s="8">
+        <f>'Data Source'!Z10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8">
+        <f>'Data Source'!A11</f>
+        <v/>
+      </c>
+      <c r="B12">
+        <f>'Data Source'!B11</f>
+        <v/>
+      </c>
+      <c r="C12" s="7">
+        <f>'Data Source'!AE11</f>
+        <v/>
+      </c>
+      <c r="D12" s="7">
+        <f>'Data Source'!AF11</f>
+        <v/>
+      </c>
+      <c r="E12" s="7">
+        <f>'Data Source'!AG11</f>
+        <v/>
+      </c>
+      <c r="F12" s="7">
+        <f>'Data Source'!AH11</f>
+        <v/>
+      </c>
+      <c r="G12" s="7">
+        <f>'Data Source'!AI11</f>
+        <v/>
+      </c>
+      <c r="H12" s="7">
+        <f>'Data Source'!AJ11</f>
+        <v/>
+      </c>
+      <c r="I12" s="7">
+        <f>'Data Source'!AK11</f>
+        <v/>
+      </c>
+      <c r="J12" s="7">
+        <f>'Data Source'!AL11</f>
+        <v/>
+      </c>
+      <c r="K12" s="7">
+        <f>'Data Source'!AM11</f>
+        <v/>
+      </c>
+      <c r="L12" s="7">
+        <f>'Data Source'!AN11</f>
+        <v/>
+      </c>
+      <c r="M12" s="7">
+        <f>'Data Source'!Y11</f>
+        <v/>
+      </c>
+      <c r="N12" s="8">
+        <f>'Data Source'!Z11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <f>'Data Source'!A12</f>
+        <v/>
+      </c>
+      <c r="B13">
+        <f>'Data Source'!B12</f>
+        <v/>
+      </c>
+      <c r="C13" s="7">
+        <f>'Data Source'!AE12</f>
+        <v/>
+      </c>
+      <c r="D13" s="7">
+        <f>'Data Source'!AF12</f>
+        <v/>
+      </c>
+      <c r="E13" s="7">
+        <f>'Data Source'!AG12</f>
+        <v/>
+      </c>
+      <c r="F13" s="7">
+        <f>'Data Source'!AH12</f>
+        <v/>
+      </c>
+      <c r="G13" s="7">
+        <f>'Data Source'!AI12</f>
+        <v/>
+      </c>
+      <c r="H13" s="7">
+        <f>'Data Source'!AJ12</f>
+        <v/>
+      </c>
+      <c r="I13" s="7">
+        <f>'Data Source'!AK12</f>
+        <v/>
+      </c>
+      <c r="J13" s="7">
+        <f>'Data Source'!AL12</f>
+        <v/>
+      </c>
+      <c r="K13" s="7">
+        <f>'Data Source'!AM12</f>
+        <v/>
+      </c>
+      <c r="L13" s="7">
+        <f>'Data Source'!AN12</f>
+        <v/>
+      </c>
+      <c r="M13" s="7">
+        <f>'Data Source'!Y12</f>
+        <v/>
+      </c>
+      <c r="N13" s="8">
+        <f>'Data Source'!Z12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <f>'Data Source'!A13</f>
+        <v/>
+      </c>
+      <c r="B14">
+        <f>'Data Source'!B13</f>
+        <v/>
+      </c>
+      <c r="C14" s="7">
+        <f>'Data Source'!AE13</f>
+        <v/>
+      </c>
+      <c r="D14" s="7">
+        <f>'Data Source'!AF13</f>
+        <v/>
+      </c>
+      <c r="E14" s="7">
+        <f>'Data Source'!AG13</f>
+        <v/>
+      </c>
+      <c r="F14" s="7">
+        <f>'Data Source'!AH13</f>
+        <v/>
+      </c>
+      <c r="G14" s="7">
+        <f>'Data Source'!AI13</f>
+        <v/>
+      </c>
+      <c r="H14" s="7">
+        <f>'Data Source'!AJ13</f>
+        <v/>
+      </c>
+      <c r="I14" s="7">
+        <f>'Data Source'!AK13</f>
+        <v/>
+      </c>
+      <c r="J14" s="7">
+        <f>'Data Source'!AL13</f>
+        <v/>
+      </c>
+      <c r="K14" s="7">
+        <f>'Data Source'!AM13</f>
+        <v/>
+      </c>
+      <c r="L14" s="7">
+        <f>'Data Source'!AN13</f>
+        <v/>
+      </c>
+      <c r="M14" s="7">
+        <f>'Data Source'!Y13</f>
+        <v/>
+      </c>
+      <c r="N14" s="8">
+        <f>'Data Source'!Z13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <f>'Data Source'!A14</f>
+        <v/>
+      </c>
+      <c r="B15">
+        <f>'Data Source'!B14</f>
+        <v/>
+      </c>
+      <c r="C15" s="7">
+        <f>'Data Source'!AE14</f>
+        <v/>
+      </c>
+      <c r="D15" s="7">
+        <f>'Data Source'!AF14</f>
+        <v/>
+      </c>
+      <c r="E15" s="7">
+        <f>'Data Source'!AG14</f>
+        <v/>
+      </c>
+      <c r="F15" s="7">
+        <f>'Data Source'!AH14</f>
+        <v/>
+      </c>
+      <c r="G15" s="7">
+        <f>'Data Source'!AI14</f>
+        <v/>
+      </c>
+      <c r="H15" s="7">
+        <f>'Data Source'!AJ14</f>
+        <v/>
+      </c>
+      <c r="I15" s="7">
+        <f>'Data Source'!AK14</f>
+        <v/>
+      </c>
+      <c r="J15" s="7">
+        <f>'Data Source'!AL14</f>
+        <v/>
+      </c>
+      <c r="K15" s="7">
+        <f>'Data Source'!AM14</f>
+        <v/>
+      </c>
+      <c r="L15" s="7">
+        <f>'Data Source'!AN14</f>
+        <v/>
+      </c>
+      <c r="M15" s="7">
+        <f>'Data Source'!Y14</f>
+        <v/>
+      </c>
+      <c r="N15" s="8">
+        <f>'Data Source'!Z14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <f>'Data Source'!A15</f>
+        <v/>
+      </c>
+      <c r="B16">
+        <f>'Data Source'!B15</f>
+        <v/>
+      </c>
+      <c r="C16" s="7">
+        <f>'Data Source'!AE15</f>
+        <v/>
+      </c>
+      <c r="D16" s="7">
+        <f>'Data Source'!AF15</f>
+        <v/>
+      </c>
+      <c r="E16" s="7">
+        <f>'Data Source'!AG15</f>
+        <v/>
+      </c>
+      <c r="F16" s="7">
+        <f>'Data Source'!AH15</f>
+        <v/>
+      </c>
+      <c r="G16" s="7">
+        <f>'Data Source'!AI15</f>
+        <v/>
+      </c>
+      <c r="H16" s="7">
+        <f>'Data Source'!AJ15</f>
+        <v/>
+      </c>
+      <c r="I16" s="7">
+        <f>'Data Source'!AK15</f>
+        <v/>
+      </c>
+      <c r="J16" s="7">
+        <f>'Data Source'!AL15</f>
+        <v/>
+      </c>
+      <c r="K16" s="7">
+        <f>'Data Source'!AM15</f>
+        <v/>
+      </c>
+      <c r="L16" s="7">
+        <f>'Data Source'!AN15</f>
+        <v/>
+      </c>
+      <c r="M16" s="7">
+        <f>'Data Source'!Y15</f>
+        <v/>
+      </c>
+      <c r="N16" s="8">
+        <f>'Data Source'!Z15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <f>'Data Source'!A16</f>
+        <v/>
+      </c>
+      <c r="B17">
+        <f>'Data Source'!B16</f>
+        <v/>
+      </c>
+      <c r="C17" s="7">
+        <f>'Data Source'!AE16</f>
+        <v/>
+      </c>
+      <c r="D17" s="7">
+        <f>'Data Source'!AF16</f>
+        <v/>
+      </c>
+      <c r="E17" s="7">
+        <f>'Data Source'!AG16</f>
+        <v/>
+      </c>
+      <c r="F17" s="7">
+        <f>'Data Source'!AH16</f>
+        <v/>
+      </c>
+      <c r="G17" s="7">
+        <f>'Data Source'!AI16</f>
+        <v/>
+      </c>
+      <c r="H17" s="7">
+        <f>'Data Source'!AJ16</f>
+        <v/>
+      </c>
+      <c r="I17" s="7">
+        <f>'Data Source'!AK16</f>
+        <v/>
+      </c>
+      <c r="J17" s="7">
+        <f>'Data Source'!AL16</f>
+        <v/>
+      </c>
+      <c r="K17" s="7">
+        <f>'Data Source'!AM16</f>
+        <v/>
+      </c>
+      <c r="L17" s="7">
+        <f>'Data Source'!AN16</f>
+        <v/>
+      </c>
+      <c r="M17" s="7">
+        <f>'Data Source'!Y16</f>
+        <v/>
+      </c>
+      <c r="N17" s="8">
+        <f>'Data Source'!Z16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <f>'Data Source'!A17</f>
+        <v/>
+      </c>
+      <c r="B18">
+        <f>'Data Source'!B17</f>
+        <v/>
+      </c>
+      <c r="C18" s="7">
+        <f>'Data Source'!AE17</f>
+        <v/>
+      </c>
+      <c r="D18" s="7">
+        <f>'Data Source'!AF17</f>
+        <v/>
+      </c>
+      <c r="E18" s="7">
+        <f>'Data Source'!AG17</f>
+        <v/>
+      </c>
+      <c r="F18" s="7">
+        <f>'Data Source'!AH17</f>
+        <v/>
+      </c>
+      <c r="G18" s="7">
+        <f>'Data Source'!AI17</f>
+        <v/>
+      </c>
+      <c r="H18" s="7">
+        <f>'Data Source'!AJ17</f>
+        <v/>
+      </c>
+      <c r="I18" s="7">
+        <f>'Data Source'!AK17</f>
+        <v/>
+      </c>
+      <c r="J18" s="7">
+        <f>'Data Source'!AL17</f>
+        <v/>
+      </c>
+      <c r="K18" s="7">
+        <f>'Data Source'!AM17</f>
+        <v/>
+      </c>
+      <c r="L18" s="7">
+        <f>'Data Source'!AN17</f>
+        <v/>
+      </c>
+      <c r="M18" s="7">
+        <f>'Data Source'!Y17</f>
+        <v/>
+      </c>
+      <c r="N18" s="8">
+        <f>'Data Source'!Z17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <f>'Data Source'!A18</f>
+        <v/>
+      </c>
+      <c r="B19">
+        <f>'Data Source'!B18</f>
+        <v/>
+      </c>
+      <c r="C19" s="7">
+        <f>'Data Source'!AE18</f>
+        <v/>
+      </c>
+      <c r="D19" s="7">
+        <f>'Data Source'!AF18</f>
+        <v/>
+      </c>
+      <c r="E19" s="7">
+        <f>'Data Source'!AG18</f>
+        <v/>
+      </c>
+      <c r="F19" s="7">
+        <f>'Data Source'!AH18</f>
+        <v/>
+      </c>
+      <c r="G19" s="7">
+        <f>'Data Source'!AI18</f>
+        <v/>
+      </c>
+      <c r="H19" s="7">
+        <f>'Data Source'!AJ18</f>
+        <v/>
+      </c>
+      <c r="I19" s="7">
+        <f>'Data Source'!AK18</f>
+        <v/>
+      </c>
+      <c r="J19" s="7">
+        <f>'Data Source'!AL18</f>
+        <v/>
+      </c>
+      <c r="K19" s="7">
+        <f>'Data Source'!AM18</f>
+        <v/>
+      </c>
+      <c r="L19" s="7">
+        <f>'Data Source'!AN18</f>
+        <v/>
+      </c>
+      <c r="M19" s="7">
+        <f>'Data Source'!Y18</f>
+        <v/>
+      </c>
+      <c r="N19" s="8">
+        <f>'Data Source'!Z18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8">
+        <f>'Data Source'!A19</f>
+        <v/>
+      </c>
+      <c r="B20">
+        <f>'Data Source'!B19</f>
+        <v/>
+      </c>
+      <c r="C20" s="7">
+        <f>'Data Source'!AE19</f>
+        <v/>
+      </c>
+      <c r="D20" s="7">
+        <f>'Data Source'!AF19</f>
+        <v/>
+      </c>
+      <c r="E20" s="7">
+        <f>'Data Source'!AG19</f>
+        <v/>
+      </c>
+      <c r="F20" s="7">
+        <f>'Data Source'!AH19</f>
+        <v/>
+      </c>
+      <c r="G20" s="7">
+        <f>'Data Source'!AI19</f>
+        <v/>
+      </c>
+      <c r="H20" s="7">
+        <f>'Data Source'!AJ19</f>
+        <v/>
+      </c>
+      <c r="I20" s="7">
+        <f>'Data Source'!AK19</f>
+        <v/>
+      </c>
+      <c r="J20" s="7">
+        <f>'Data Source'!AL19</f>
+        <v/>
+      </c>
+      <c r="K20" s="7">
+        <f>'Data Source'!AM19</f>
+        <v/>
+      </c>
+      <c r="L20" s="7">
+        <f>'Data Source'!AN19</f>
+        <v/>
+      </c>
+      <c r="M20" s="7">
+        <f>'Data Source'!Y19</f>
+        <v/>
+      </c>
+      <c r="N20" s="8">
+        <f>'Data Source'!Z19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8">
+        <f>'Data Source'!A20</f>
+        <v/>
+      </c>
+      <c r="B21">
+        <f>'Data Source'!B20</f>
+        <v/>
+      </c>
+      <c r="C21" s="7">
+        <f>'Data Source'!AE20</f>
+        <v/>
+      </c>
+      <c r="D21" s="7">
+        <f>'Data Source'!AF20</f>
+        <v/>
+      </c>
+      <c r="E21" s="7">
+        <f>'Data Source'!AG20</f>
+        <v/>
+      </c>
+      <c r="F21" s="7">
+        <f>'Data Source'!AH20</f>
+        <v/>
+      </c>
+      <c r="G21" s="7">
+        <f>'Data Source'!AI20</f>
+        <v/>
+      </c>
+      <c r="H21" s="7">
+        <f>'Data Source'!AJ20</f>
+        <v/>
+      </c>
+      <c r="I21" s="7">
+        <f>'Data Source'!AK20</f>
+        <v/>
+      </c>
+      <c r="J21" s="7">
+        <f>'Data Source'!AL20</f>
+        <v/>
+      </c>
+      <c r="K21" s="7">
+        <f>'Data Source'!AM20</f>
+        <v/>
+      </c>
+      <c r="L21" s="7">
+        <f>'Data Source'!AN20</f>
+        <v/>
+      </c>
+      <c r="M21" s="7">
+        <f>'Data Source'!Y20</f>
+        <v/>
+      </c>
+      <c r="N21" s="8">
+        <f>'Data Source'!Z20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8">
+        <f>'Data Source'!A21</f>
+        <v/>
+      </c>
+      <c r="B22">
+        <f>'Data Source'!B21</f>
+        <v/>
+      </c>
+      <c r="C22" s="7">
+        <f>'Data Source'!AE21</f>
+        <v/>
+      </c>
+      <c r="D22" s="7">
+        <f>'Data Source'!AF21</f>
+        <v/>
+      </c>
+      <c r="E22" s="7">
+        <f>'Data Source'!AG21</f>
+        <v/>
+      </c>
+      <c r="F22" s="7">
+        <f>'Data Source'!AH21</f>
+        <v/>
+      </c>
+      <c r="G22" s="7">
+        <f>'Data Source'!AI21</f>
+        <v/>
+      </c>
+      <c r="H22" s="7">
+        <f>'Data Source'!AJ21</f>
+        <v/>
+      </c>
+      <c r="I22" s="7">
+        <f>'Data Source'!AK21</f>
+        <v/>
+      </c>
+      <c r="J22" s="7">
+        <f>'Data Source'!AL21</f>
+        <v/>
+      </c>
+      <c r="K22" s="7">
+        <f>'Data Source'!AM21</f>
+        <v/>
+      </c>
+      <c r="L22" s="7">
+        <f>'Data Source'!AN21</f>
+        <v/>
+      </c>
+      <c r="M22" s="7">
+        <f>'Data Source'!Y21</f>
+        <v/>
+      </c>
+      <c r="N22" s="8">
+        <f>'Data Source'!Z21</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>